<commit_message>
Restore point before implementing the JV
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE891E1F-152E-436C-8B31-1ECC56634DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A5E0B9-914D-4A6D-8AD8-23D665FB7F99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -4758,9 +4758,6 @@
     <t>连</t>
   </si>
   <si>
-    <t>版权所有？保留{{一年}}巴南IT有限公司保留所有权利。</t>
-  </si>
-  <si>
     <t>由我创建</t>
   </si>
   <si>
@@ -4809,9 +4806,6 @@
     <t>不活动的项目无法进行编辑，请先激活它。</t>
   </si>
   <si>
-    <t>您选择的文件超过{{MAXSIZE}} MB的最大允许大小</t>
-  </si>
-  <si>
     <t>错误加载公司设置</t>
   </si>
   <si>
@@ -4884,9 +4878,6 @@
     <t>导入的文件没有通过验证，见下文</t>
   </si>
   <si>
-    <t>成功插入{{插入的}}记录（S），并在{{秒}}秒更新{{更新}}结果</t>
-  </si>
-  <si>
     <t>下载模板文件，并填写您的数据：</t>
   </si>
   <si>
@@ -4920,15 +4911,9 @@
     <t>加载系统设置</t>
   </si>
   <si>
-    <t>只有{{最大值}}项目可以同时输出</t>
-  </si>
-  <si>
     <t>模式</t>
   </si>
   <si>
-    <t>我{{占位符}}帐户</t>
-  </si>
-  <si>
     <t>我的公司</t>
   </si>
   <si>
@@ -4950,9 +4935,6 @@
     <t>不公开</t>
   </si>
   <si>
-    <t>{{计数}}选择项目</t>
-  </si>
-  <si>
     <t>以前</t>
   </si>
   <si>
@@ -5091,9 +5073,6 @@
     <t>你未保存的更改都将被丢弃，你确定你想继续吗？</t>
   </si>
   <si>
-    <t>注：邀请电子邮件将被发送到“{{EMAIL}}”一旦你保存这个文件。</t>
-  </si>
-  <si>
     <t>欢迎页面</t>
   </si>
   <si>
@@ -5158,6 +5137,27 @@
   </si>
   <si>
     <t>获取更多与{{appName}}</t>
+  </si>
+  <si>
+    <t>版权所有？保留{{year}}巴南IT有限公司保留所有权利。</t>
+  </si>
+  <si>
+    <t>您选择的文件超过{{maxSize}} MB的最大允许大小</t>
+  </si>
+  <si>
+    <t>成功插入{{Inserted}}记录，并在{{Updated}}秒更新{{Seconds}}结果</t>
+  </si>
+  <si>
+    <t>只有{{max}}项目可以同时输出</t>
+  </si>
+  <si>
+    <t>我{{placeholder}}帐户</t>
+  </si>
+  <si>
+    <t>注：邀请电子邮件将被发送到“{{email}}”一旦你保存这个文件。</t>
+  </si>
+  <si>
+    <t>{{count}}选择项目</t>
   </si>
 </sst>
 </file>
@@ -5545,9 +5545,9 @@
   <dimension ref="A1:G464"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5861,7 +5861,7 @@
         <v>827</v>
       </c>
       <c r="G15" t="s">
-        <v>1703</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -6081,7 +6081,7 @@
         <v>52</v>
       </c>
       <c r="G26" t="s">
-        <v>1702</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6581,7 +6581,7 @@
         <v>899</v>
       </c>
       <c r="G51" t="s">
-        <v>1574</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -6681,7 +6681,7 @@
         <v>900</v>
       </c>
       <c r="G56" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -6701,7 +6701,7 @@
         <v>901</v>
       </c>
       <c r="G57" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -6721,7 +6721,7 @@
         <v>902</v>
       </c>
       <c r="G58" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -6741,7 +6741,7 @@
         <v>1021</v>
       </c>
       <c r="G59" t="s">
-        <v>1691</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -6941,7 +6941,7 @@
         <v>904</v>
       </c>
       <c r="G69" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -6981,7 +6981,7 @@
         <v>905</v>
       </c>
       <c r="G71" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -7041,7 +7041,7 @@
         <v>906</v>
       </c>
       <c r="G74" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -7081,7 +7081,7 @@
         <v>908</v>
       </c>
       <c r="G76" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -7101,7 +7101,7 @@
         <v>909</v>
       </c>
       <c r="G77" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -7141,7 +7141,7 @@
         <v>910</v>
       </c>
       <c r="G79" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -7221,7 +7221,7 @@
         <v>911</v>
       </c>
       <c r="G83" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -7241,7 +7241,7 @@
         <v>912</v>
       </c>
       <c r="G84" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -7321,7 +7321,7 @@
         <v>913</v>
       </c>
       <c r="G88" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -7341,7 +7341,7 @@
         <v>914</v>
       </c>
       <c r="G89" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -7441,7 +7441,7 @@
         <v>915</v>
       </c>
       <c r="G94" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -7501,7 +7501,7 @@
         <v>916</v>
       </c>
       <c r="G97" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -7681,7 +7681,7 @@
         <v>917</v>
       </c>
       <c r="G106" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -7901,7 +7901,7 @@
         <v>918</v>
       </c>
       <c r="G117" t="s">
-        <v>1591</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -7961,7 +7961,7 @@
         <v>919</v>
       </c>
       <c r="G120" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -8001,7 +8001,7 @@
         <v>920</v>
       </c>
       <c r="G122" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -8021,7 +8021,7 @@
         <v>921</v>
       </c>
       <c r="G123" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -8101,7 +8101,7 @@
         <v>922</v>
       </c>
       <c r="G127" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -8121,7 +8121,7 @@
         <v>923</v>
       </c>
       <c r="G128" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -8201,7 +8201,7 @@
         <v>924</v>
       </c>
       <c r="G132" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -8641,7 +8641,7 @@
         <v>925</v>
       </c>
       <c r="G154" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -8661,7 +8661,7 @@
         <v>926</v>
       </c>
       <c r="G155" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -8681,7 +8681,7 @@
         <v>927</v>
       </c>
       <c r="G156" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -8701,7 +8701,7 @@
         <v>928</v>
       </c>
       <c r="G157" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -8741,7 +8741,7 @@
         <v>929</v>
       </c>
       <c r="G159" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -8761,7 +8761,7 @@
         <v>930</v>
       </c>
       <c r="G160" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -8821,7 +8821,7 @@
         <v>931</v>
       </c>
       <c r="G163" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -8841,7 +8841,7 @@
         <v>932</v>
       </c>
       <c r="G164" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -8861,7 +8861,7 @@
         <v>933</v>
       </c>
       <c r="G165" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -8901,7 +8901,7 @@
         <v>934</v>
       </c>
       <c r="G167" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -8921,7 +8921,7 @@
         <v>935</v>
       </c>
       <c r="G168" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -8941,7 +8941,7 @@
         <v>936</v>
       </c>
       <c r="G169" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -9041,7 +9041,7 @@
         <v>937</v>
       </c>
       <c r="G174" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -9061,7 +9061,7 @@
         <v>938</v>
       </c>
       <c r="G175" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -9121,7 +9121,7 @@
         <v>939</v>
       </c>
       <c r="G178" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -9181,7 +9181,7 @@
         <v>940</v>
       </c>
       <c r="G181" t="s">
-        <v>1705</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -9221,7 +9221,7 @@
         <v>1024</v>
       </c>
       <c r="G183" t="s">
-        <v>1694</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -9261,7 +9261,7 @@
         <v>941</v>
       </c>
       <c r="G185" t="s">
-        <v>1706</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -9441,7 +9441,7 @@
         <v>942</v>
       </c>
       <c r="G194" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -9461,7 +9461,7 @@
         <v>943</v>
       </c>
       <c r="G195" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -9481,7 +9481,7 @@
         <v>944</v>
       </c>
       <c r="G196" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -9501,7 +9501,7 @@
         <v>945</v>
       </c>
       <c r="G197" t="s">
-        <v>1616</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -9521,7 +9521,7 @@
         <v>946</v>
       </c>
       <c r="G198" t="s">
-        <v>1617</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -9541,7 +9541,7 @@
         <v>947</v>
       </c>
       <c r="G199" t="s">
-        <v>1618</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -9581,7 +9581,7 @@
         <v>948</v>
       </c>
       <c r="G201" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -9621,7 +9621,7 @@
         <v>949</v>
       </c>
       <c r="G203" t="s">
-        <v>1620</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -9641,7 +9641,7 @@
         <v>950</v>
       </c>
       <c r="G204" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -9821,7 +9821,7 @@
         <v>951</v>
       </c>
       <c r="G213" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -9921,7 +9921,7 @@
         <v>952</v>
       </c>
       <c r="G218" t="s">
-        <v>1623</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -9941,7 +9941,7 @@
         <v>953</v>
       </c>
       <c r="G219" t="s">
-        <v>1707</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -9961,7 +9961,7 @@
         <v>954</v>
       </c>
       <c r="G220" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -9981,7 +9981,7 @@
         <v>955</v>
       </c>
       <c r="G221" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -10001,7 +10001,7 @@
         <v>956</v>
       </c>
       <c r="G222" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -10021,7 +10021,7 @@
         <v>957</v>
       </c>
       <c r="G223" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -10101,7 +10101,7 @@
         <v>958</v>
       </c>
       <c r="G227" t="s">
-        <v>1628</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -10301,7 +10301,7 @@
         <v>1022</v>
       </c>
       <c r="G237" t="s">
-        <v>1692</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -10321,7 +10321,7 @@
         <v>959</v>
       </c>
       <c r="G238" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -10621,7 +10621,7 @@
         <v>960</v>
       </c>
       <c r="G253" t="s">
-        <v>1630</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -10641,7 +10641,7 @@
         <v>961</v>
       </c>
       <c r="G254" t="s">
-        <v>1631</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -10681,7 +10681,7 @@
         <v>962</v>
       </c>
       <c r="G256" t="s">
-        <v>1632</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -10701,7 +10701,7 @@
         <v>963</v>
       </c>
       <c r="G257" t="s">
-        <v>1633</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -10741,7 +10741,7 @@
         <v>964</v>
       </c>
       <c r="G259" t="s">
-        <v>1634</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -10761,7 +10761,7 @@
         <v>965</v>
       </c>
       <c r="G260" t="s">
-        <v>1635</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -10801,7 +10801,7 @@
         <v>966</v>
       </c>
       <c r="G262" t="s">
-        <v>1636</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
@@ -10821,7 +10821,7 @@
         <v>1020</v>
       </c>
       <c r="G263" t="s">
-        <v>1690</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
@@ -10841,7 +10841,7 @@
         <v>967</v>
       </c>
       <c r="G264" t="s">
-        <v>1637</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
@@ -10861,7 +10861,7 @@
         <v>968</v>
       </c>
       <c r="G265" t="s">
-        <v>1638</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
@@ -11401,7 +11401,7 @@
         <v>969</v>
       </c>
       <c r="G292" t="s">
-        <v>1639</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
@@ -11441,7 +11441,7 @@
         <v>970</v>
       </c>
       <c r="G294" t="s">
-        <v>1640</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
@@ -11501,7 +11501,7 @@
         <v>971</v>
       </c>
       <c r="G297" t="s">
-        <v>1641</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
@@ -11521,7 +11521,7 @@
         <v>972</v>
       </c>
       <c r="G298" t="s">
-        <v>1642</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.25">
@@ -11541,7 +11541,7 @@
         <v>973</v>
       </c>
       <c r="G299" s="4" t="s">
-        <v>1643</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.25">
@@ -11721,7 +11721,7 @@
         <v>974</v>
       </c>
       <c r="G308" t="s">
-        <v>1644</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
@@ -11741,7 +11741,7 @@
         <v>975</v>
       </c>
       <c r="G309" t="s">
-        <v>1645</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.25">
@@ -11761,7 +11761,7 @@
         <v>976</v>
       </c>
       <c r="G310" t="s">
-        <v>1646</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.25">
@@ -11881,7 +11881,7 @@
         <v>977</v>
       </c>
       <c r="G316" t="s">
-        <v>1647</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.25">
@@ -11901,7 +11901,7 @@
         <v>978</v>
       </c>
       <c r="G317" t="s">
-        <v>1648</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
@@ -12361,7 +12361,7 @@
         <v>979</v>
       </c>
       <c r="G340" t="s">
-        <v>1649</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="341" spans="1:7" x14ac:dyDescent="0.25">
@@ -12521,7 +12521,7 @@
         <v>980</v>
       </c>
       <c r="G348" t="s">
-        <v>1650</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -12541,7 +12541,7 @@
         <v>1025</v>
       </c>
       <c r="G349" t="s">
-        <v>1695</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
@@ -12561,7 +12561,7 @@
         <v>1026</v>
       </c>
       <c r="G350" t="s">
-        <v>1696</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
@@ -12661,7 +12661,7 @@
         <v>981</v>
       </c>
       <c r="G355" t="s">
-        <v>1651</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.25">
@@ -12681,7 +12681,7 @@
         <v>982</v>
       </c>
       <c r="G356" t="s">
-        <v>1652</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
@@ -12721,7 +12721,7 @@
         <v>983</v>
       </c>
       <c r="G358" t="s">
-        <v>1653</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="359" spans="1:7" x14ac:dyDescent="0.25">
@@ -12778,10 +12778,10 @@
         <v>642</v>
       </c>
       <c r="F361" t="s">
-        <v>1698</v>
+        <v>1691</v>
       </c>
       <c r="G361" t="s">
-        <v>1704</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
@@ -12861,7 +12861,7 @@
         <v>984</v>
       </c>
       <c r="G365" t="s">
-        <v>1654</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="366" spans="1:7" x14ac:dyDescent="0.25">
@@ -12906,7 +12906,7 @@
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>1697</v>
+        <v>1690</v>
       </c>
       <c r="B368" t="b">
         <v>0</v>
@@ -12915,13 +12915,13 @@
         <v>1</v>
       </c>
       <c r="E368" t="s">
-        <v>1700</v>
+        <v>1693</v>
       </c>
       <c r="F368" t="s">
-        <v>1699</v>
+        <v>1692</v>
       </c>
       <c r="G368" t="s">
-        <v>1701</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.25">
@@ -12981,7 +12981,7 @@
         <v>985</v>
       </c>
       <c r="G371" t="s">
-        <v>1655</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
@@ -13001,7 +13001,7 @@
         <v>986</v>
       </c>
       <c r="G372" t="s">
-        <v>1656</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.25">
@@ -13021,7 +13021,7 @@
         <v>987</v>
       </c>
       <c r="G373" t="s">
-        <v>1657</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.25">
@@ -13041,7 +13041,7 @@
         <v>988</v>
       </c>
       <c r="G374" t="s">
-        <v>1658</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.25">
@@ -13061,7 +13061,7 @@
         <v>989</v>
       </c>
       <c r="G375" t="s">
-        <v>1659</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
@@ -13081,7 +13081,7 @@
         <v>990</v>
       </c>
       <c r="G376" t="s">
-        <v>1660</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.25">
@@ -13101,7 +13101,7 @@
         <v>991</v>
       </c>
       <c r="G377" t="s">
-        <v>1661</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.25">
@@ -13121,7 +13121,7 @@
         <v>992</v>
       </c>
       <c r="G378" t="s">
-        <v>1662</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
@@ -13141,7 +13141,7 @@
         <v>993</v>
       </c>
       <c r="G379" t="s">
-        <v>1663</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.25">
@@ -13161,7 +13161,7 @@
         <v>994</v>
       </c>
       <c r="G380" t="s">
-        <v>1664</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.25">
@@ -13181,7 +13181,7 @@
         <v>995</v>
       </c>
       <c r="G381" t="s">
-        <v>1665</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.25">
@@ -13201,7 +13201,7 @@
         <v>996</v>
       </c>
       <c r="G382" t="s">
-        <v>1666</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.25">
@@ -13221,7 +13221,7 @@
         <v>997</v>
       </c>
       <c r="G383" t="s">
-        <v>1667</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.25">
@@ -13241,7 +13241,7 @@
         <v>998</v>
       </c>
       <c r="G384" t="s">
-        <v>1668</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.25">
@@ -13261,7 +13261,7 @@
         <v>999</v>
       </c>
       <c r="G385" t="s">
-        <v>1669</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.25">
@@ -13281,7 +13281,7 @@
         <v>1000</v>
       </c>
       <c r="G386" t="s">
-        <v>1670</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.25">
@@ -13301,7 +13301,7 @@
         <v>1001</v>
       </c>
       <c r="G387" t="s">
-        <v>1671</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.25">
@@ -13321,7 +13321,7 @@
         <v>1002</v>
       </c>
       <c r="G388" t="s">
-        <v>1672</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.25">
@@ -13341,7 +13341,7 @@
         <v>1003</v>
       </c>
       <c r="G389" t="s">
-        <v>1673</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="390" spans="1:7" x14ac:dyDescent="0.25">
@@ -13641,7 +13641,7 @@
         <v>1004</v>
       </c>
       <c r="G404" t="s">
-        <v>1674</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="405" spans="1:7" x14ac:dyDescent="0.25">
@@ -13661,7 +13661,7 @@
         <v>1005</v>
       </c>
       <c r="G405" t="s">
-        <v>1675</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="406" spans="1:7" x14ac:dyDescent="0.25">
@@ -13721,7 +13721,7 @@
         <v>1006</v>
       </c>
       <c r="G408" t="s">
-        <v>1676</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.25">
@@ -13821,7 +13821,7 @@
         <v>1007</v>
       </c>
       <c r="G413" t="s">
-        <v>1677</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="414" spans="1:7" x14ac:dyDescent="0.25">
@@ -13841,7 +13841,7 @@
         <v>1008</v>
       </c>
       <c r="G414" t="s">
-        <v>1678</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.25">
@@ -13941,7 +13941,7 @@
         <v>1009</v>
       </c>
       <c r="G419" t="s">
-        <v>1679</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="420" spans="1:7" x14ac:dyDescent="0.25">
@@ -13961,7 +13961,7 @@
         <v>1010</v>
       </c>
       <c r="G420" t="s">
-        <v>1680</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="421" spans="1:7" x14ac:dyDescent="0.25">
@@ -14001,7 +14001,7 @@
         <v>1011</v>
       </c>
       <c r="G422" t="s">
-        <v>1681</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.25">
@@ -14121,7 +14121,7 @@
         <v>1012</v>
       </c>
       <c r="G428" t="s">
-        <v>1682</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.25">
@@ -14141,7 +14141,7 @@
         <v>1013</v>
       </c>
       <c r="G429" t="s">
-        <v>1683</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="430" spans="1:7" x14ac:dyDescent="0.25">
@@ -14161,7 +14161,7 @@
         <v>1014</v>
       </c>
       <c r="G430" t="s">
-        <v>1684</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="431" spans="1:7" x14ac:dyDescent="0.25">
@@ -14181,7 +14181,7 @@
         <v>1023</v>
       </c>
       <c r="G431" t="s">
-        <v>1693</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="432" spans="1:7" x14ac:dyDescent="0.25">
@@ -14401,7 +14401,7 @@
         <v>1015</v>
       </c>
       <c r="G442" t="s">
-        <v>1685</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.25">
@@ -14621,7 +14621,7 @@
         <v>1016</v>
       </c>
       <c r="G453" t="s">
-        <v>1686</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="454" spans="1:7" x14ac:dyDescent="0.25">
@@ -14641,7 +14641,7 @@
         <v>1017</v>
       </c>
       <c r="G454" t="s">
-        <v>1687</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="455" spans="1:7" x14ac:dyDescent="0.25">
@@ -14661,7 +14661,7 @@
         <v>1018</v>
       </c>
       <c r="G455" t="s">
-        <v>1688</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="456" spans="1:7" x14ac:dyDescent="0.25">
@@ -14681,7 +14681,7 @@
         <v>1019</v>
       </c>
       <c r="G456" t="s">
-        <v>1689</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="457" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added auto expand and collapse buttons to tree screens
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341A1B2E-E75F-4865-B113-AFF2A7E2DDFD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE33284-4267-4BF8-A4FE-146573E507BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="1887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="1895">
   <si>
     <t>Key</t>
   </si>
@@ -5695,13 +5695,37 @@
   </si>
   <si>
     <t>可分配</t>
+  </si>
+  <si>
+    <t>CollapseAll</t>
+  </si>
+  <si>
+    <t>Collapse All</t>
+  </si>
+  <si>
+    <t>طوي الكل</t>
+  </si>
+  <si>
+    <t>全部收缩</t>
+  </si>
+  <si>
+    <t>展开级别{{level}}</t>
+  </si>
+  <si>
+    <t>AutoExpandLevel0</t>
+  </si>
+  <si>
+    <t>Auto Expand Level {{level}}</t>
+  </si>
+  <si>
+    <t>توسيع الدرجة {{level}} تلقائيا</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5728,6 +5752,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -5765,13 +5795,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6086,12 +6119,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G517"/>
+  <dimension ref="A1:G521"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A496" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F506" sqref="F506"/>
+      <selection pane="bottomLeft" activeCell="E521" sqref="E521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16451,6 +16484,52 @@
         <v>1886</v>
       </c>
     </row>
+    <row r="518" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A518" s="6" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B518" t="b">
+        <v>0</v>
+      </c>
+      <c r="C518" t="b">
+        <v>1</v>
+      </c>
+      <c r="E518" t="s">
+        <v>1893</v>
+      </c>
+      <c r="F518" t="s">
+        <v>1894</v>
+      </c>
+      <c r="G518" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="519" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A519" s="5" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B519" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C519" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E519" t="s">
+        <v>1888</v>
+      </c>
+      <c r="F519" t="s">
+        <v>1889</v>
+      </c>
+      <c r="G519" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="520" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A520" s="6"/>
+    </row>
+    <row r="521" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E521" s="5"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Implemented the Account API
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE33284-4267-4BF8-A4FE-146573E507BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291E2458-12AF-4749-A41F-43A51389AB71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="1895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="1928">
   <si>
     <t>Key</t>
   </si>
@@ -5709,16 +5709,115 @@
     <t>全部收缩</t>
   </si>
   <si>
+    <t>ExpandLevel0</t>
+  </si>
+  <si>
+    <t>Expand Level {{level}}</t>
+  </si>
+  <si>
+    <t>توسيع الدرجة {{level}}</t>
+  </si>
+  <si>
     <t>展开级别{{level}}</t>
   </si>
   <si>
-    <t>AutoExpandLevel0</t>
-  </si>
-  <si>
-    <t>Auto Expand Level {{level}}</t>
-  </si>
-  <si>
-    <t>توسيع الدرجة {{level}} تلقائيا</t>
+    <t>Error_TernaryLanguageCannotBeTheSameAsPrimaryLanguage</t>
+  </si>
+  <si>
+    <t>Ternary language cannot be the same as the primary language.</t>
+  </si>
+  <si>
+    <t>اللغة الثالثة هي نفسها اللغة الرئيسية</t>
+  </si>
+  <si>
+    <t>Error_TernaryLanguageCannotBeTheSameAsSecondaryLanguage</t>
+  </si>
+  <si>
+    <t>Ternary language cannot be the same as the secondary language.</t>
+  </si>
+  <si>
+    <t>اللغة الثالثة هي نفسها اللغة الثانية</t>
+  </si>
+  <si>
+    <t>三元语言不能与主要语言相同。</t>
+  </si>
+  <si>
+    <t>三元语言不能与第二语言相同。</t>
+  </si>
+  <si>
+    <t>Account_ResponsibilityCenter</t>
+  </si>
+  <si>
+    <t>Account_PartyReference</t>
+  </si>
+  <si>
+    <t>Account_Custodian</t>
+  </si>
+  <si>
+    <t>Account_Resource</t>
+  </si>
+  <si>
+    <t>Account_Location</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Party Reference</t>
+  </si>
+  <si>
+    <t>Custodian</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>حساب</t>
+  </si>
+  <si>
+    <t>حسابات</t>
+  </si>
+  <si>
+    <t>الذمة</t>
+  </si>
+  <si>
+    <t>الموقع</t>
+  </si>
+  <si>
+    <t>الرقم الخارجي</t>
+  </si>
+  <si>
+    <t>帐号</t>
+  </si>
+  <si>
+    <t>党的文献</t>
+  </si>
+  <si>
+    <t>保管人</t>
+  </si>
+  <si>
+    <t>位置</t>
+  </si>
+  <si>
+    <t>Account_IsDeprecated</t>
+  </si>
+  <si>
+    <t>Account_Type</t>
+  </si>
+  <si>
+    <t>Account_Classification</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>النوع</t>
+  </si>
+  <si>
+    <t>Resource_Type</t>
+  </si>
+  <si>
+    <t>类型</t>
   </si>
 </sst>
 </file>
@@ -6119,17 +6218,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G521"/>
+  <dimension ref="A1:G530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A496" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A500" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E521" sqref="E521"/>
+      <selection pane="bottomLeft" activeCell="F533" sqref="F533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" hidden="1" customWidth="1"/>
@@ -13423,87 +13522,87 @@
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>810</v>
+        <v>1673</v>
       </c>
       <c r="B365" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C365" t="b">
         <v>1</v>
       </c>
       <c r="E365" t="s">
-        <v>812</v>
+        <v>1675</v>
       </c>
       <c r="F365" t="s">
-        <v>811</v>
+        <v>1676</v>
       </c>
       <c r="G365" t="s">
-        <v>1527</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="366" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>1673</v>
+        <v>813</v>
       </c>
       <c r="B366" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C366" t="b">
         <v>1</v>
       </c>
       <c r="E366" t="s">
-        <v>1675</v>
+        <v>815</v>
       </c>
       <c r="F366" t="s">
-        <v>1676</v>
+        <v>814</v>
       </c>
       <c r="G366" t="s">
-        <v>1677</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>813</v>
+        <v>1080</v>
       </c>
       <c r="B367" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C367" t="b">
         <v>1</v>
       </c>
       <c r="E367" t="s">
-        <v>815</v>
+        <v>971</v>
       </c>
       <c r="F367" t="s">
-        <v>814</v>
+        <v>1208</v>
       </c>
       <c r="G367" t="s">
-        <v>1528</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>813</v>
+        <v>1081</v>
       </c>
       <c r="B368" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C368" t="b">
         <v>1</v>
       </c>
       <c r="E368" t="s">
-        <v>815</v>
+        <v>972</v>
       </c>
       <c r="F368" t="s">
-        <v>814</v>
+        <v>1209</v>
       </c>
       <c r="G368" t="s">
-        <v>1528</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="B369" t="b">
         <v>0</v>
@@ -13512,18 +13611,18 @@
         <v>1</v>
       </c>
       <c r="E369" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="F369" t="s">
-        <v>1208</v>
+        <v>1210</v>
       </c>
       <c r="G369" t="s">
-        <v>1632</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="B370" t="b">
         <v>0</v>
@@ -13532,18 +13631,18 @@
         <v>1</v>
       </c>
       <c r="E370" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="F370" t="s">
-        <v>1209</v>
+        <v>1211</v>
       </c>
       <c r="G370" t="s">
-        <v>1633</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="B371" t="b">
         <v>0</v>
@@ -13552,18 +13651,18 @@
         <v>1</v>
       </c>
       <c r="E371" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="F371" t="s">
-        <v>1210</v>
+        <v>1212</v>
       </c>
       <c r="G371" t="s">
-        <v>1634</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="B372" t="b">
         <v>0</v>
@@ -13572,18 +13671,18 @@
         <v>1</v>
       </c>
       <c r="E372" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="F372" t="s">
-        <v>1211</v>
+        <v>1213</v>
       </c>
       <c r="G372" t="s">
-        <v>1635</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="B373" t="b">
         <v>0</v>
@@ -13592,18 +13691,18 @@
         <v>1</v>
       </c>
       <c r="E373" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="F373" t="s">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="G373" t="s">
-        <v>1636</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="B374" t="b">
         <v>0</v>
@@ -13612,18 +13711,18 @@
         <v>1</v>
       </c>
       <c r="E374" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="F374" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
       <c r="G374" t="s">
-        <v>1637</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="B375" t="b">
         <v>0</v>
@@ -13632,18 +13731,18 @@
         <v>1</v>
       </c>
       <c r="E375" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="F375" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="G375" t="s">
-        <v>1638</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="B376" t="b">
         <v>0</v>
@@ -13652,18 +13751,18 @@
         <v>1</v>
       </c>
       <c r="E376" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="F376" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="G376" t="s">
-        <v>1639</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="B377" t="b">
         <v>0</v>
@@ -13672,18 +13771,18 @@
         <v>1</v>
       </c>
       <c r="E377" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="F377" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="G377" t="s">
-        <v>1640</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="B378" t="b">
         <v>0</v>
@@ -13692,18 +13791,18 @@
         <v>1</v>
       </c>
       <c r="E378" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="F378" t="s">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="G378" t="s">
-        <v>1641</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="B379" t="b">
         <v>0</v>
@@ -13712,18 +13811,18 @@
         <v>1</v>
       </c>
       <c r="E379" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="F379" t="s">
-        <v>1218</v>
+        <v>1220</v>
       </c>
       <c r="G379" t="s">
-        <v>1642</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="B380" t="b">
         <v>0</v>
@@ -13732,18 +13831,18 @@
         <v>1</v>
       </c>
       <c r="E380" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="F380" t="s">
-        <v>1219</v>
+        <v>1221</v>
       </c>
       <c r="G380" t="s">
-        <v>1643</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="B381" t="b">
         <v>0</v>
@@ -13752,18 +13851,18 @@
         <v>1</v>
       </c>
       <c r="E381" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="F381" t="s">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="G381" t="s">
-        <v>1644</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="B382" t="b">
         <v>0</v>
@@ -13772,18 +13871,18 @@
         <v>1</v>
       </c>
       <c r="E382" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="F382" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="G382" t="s">
-        <v>1645</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="B383" t="b">
         <v>0</v>
@@ -13792,18 +13891,18 @@
         <v>1</v>
       </c>
       <c r="E383" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="F383" t="s">
-        <v>1222</v>
+        <v>1224</v>
       </c>
       <c r="G383" t="s">
-        <v>1646</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="B384" t="b">
         <v>0</v>
@@ -13812,18 +13911,18 @@
         <v>1</v>
       </c>
       <c r="E384" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="F384" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
       <c r="G384" t="s">
-        <v>1647</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="B385" t="b">
         <v>0</v>
@@ -13832,118 +13931,118 @@
         <v>1</v>
       </c>
       <c r="E385" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="F385" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="G385" t="s">
-        <v>1648</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>1097</v>
+        <v>643</v>
       </c>
       <c r="B386" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C386" t="b">
         <v>1</v>
       </c>
       <c r="E386" t="s">
-        <v>988</v>
+        <v>643</v>
       </c>
       <c r="F386" t="s">
-        <v>1225</v>
+        <v>644</v>
       </c>
       <c r="G386" t="s">
-        <v>1649</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>1098</v>
+        <v>645</v>
       </c>
       <c r="B387" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C387" t="b">
         <v>1</v>
       </c>
       <c r="E387" t="s">
-        <v>989</v>
+        <v>647</v>
       </c>
       <c r="F387" t="s">
-        <v>1226</v>
+        <v>646</v>
       </c>
       <c r="G387" t="s">
-        <v>1650</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="B388" t="b">
         <v>1</v>
       </c>
       <c r="C388" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E388" t="s">
-        <v>643</v>
+        <v>650</v>
       </c>
       <c r="F388" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="G388" t="s">
-        <v>1473</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="B389" t="b">
         <v>1</v>
       </c>
       <c r="C389" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E389" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="F389" t="s">
-        <v>646</v>
+        <v>652</v>
       </c>
       <c r="G389" t="s">
-        <v>1474</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="390" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="B390" t="b">
         <v>1</v>
       </c>
       <c r="C390" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E390" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="F390" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="G390" t="s">
-        <v>1475</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="391" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="B391" t="b">
         <v>1</v>
@@ -13952,38 +14051,38 @@
         <v>0</v>
       </c>
       <c r="E391" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="F391" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="G391" t="s">
-        <v>1476</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="B392" t="b">
         <v>1</v>
       </c>
       <c r="C392" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E392" t="s">
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="F392" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="G392" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="393" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="B393" t="b">
         <v>1</v>
@@ -13992,58 +14091,58 @@
         <v>0</v>
       </c>
       <c r="E393" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="F393" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="G393" t="s">
-        <v>1478</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>660</v>
+        <v>798</v>
       </c>
       <c r="B394" t="b">
         <v>1</v>
       </c>
       <c r="C394" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E394" t="s">
-        <v>662</v>
+        <v>800</v>
       </c>
       <c r="F394" t="s">
-        <v>661</v>
+        <v>799</v>
       </c>
       <c r="G394" t="s">
-        <v>1479</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>663</v>
+        <v>801</v>
       </c>
       <c r="B395" t="b">
         <v>1</v>
       </c>
       <c r="C395" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E395" t="s">
-        <v>665</v>
+        <v>2</v>
       </c>
       <c r="F395" t="s">
-        <v>664</v>
+        <v>802</v>
       </c>
       <c r="G395" t="s">
-        <v>1480</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="B396" t="b">
         <v>1</v>
@@ -14052,18 +14151,18 @@
         <v>1</v>
       </c>
       <c r="E396" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="F396" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="G396" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="397" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>801</v>
+        <v>790</v>
       </c>
       <c r="B397" t="b">
         <v>1</v>
@@ -14072,18 +14171,18 @@
         <v>1</v>
       </c>
       <c r="E397" t="s">
-        <v>2</v>
+        <v>792</v>
       </c>
       <c r="F397" t="s">
-        <v>802</v>
+        <v>791</v>
       </c>
       <c r="G397" t="s">
-        <v>1524</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B398" t="b">
         <v>1</v>
@@ -14092,18 +14191,18 @@
         <v>1</v>
       </c>
       <c r="E398" t="s">
-        <v>797</v>
+        <v>741</v>
       </c>
       <c r="F398" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G398" t="s">
-        <v>1522</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="399" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>790</v>
+        <v>666</v>
       </c>
       <c r="B399" t="b">
         <v>1</v>
@@ -14112,158 +14211,158 @@
         <v>1</v>
       </c>
       <c r="E399" t="s">
-        <v>792</v>
+        <v>666</v>
       </c>
       <c r="F399" t="s">
-        <v>791</v>
+        <v>667</v>
       </c>
       <c r="G399" t="s">
-        <v>1521</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="400" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>793</v>
+        <v>1099</v>
       </c>
       <c r="B400" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C400" t="b">
         <v>1</v>
       </c>
       <c r="E400" t="s">
-        <v>741</v>
+        <v>990</v>
       </c>
       <c r="F400" t="s">
-        <v>794</v>
+        <v>1227</v>
       </c>
       <c r="G400" t="s">
-        <v>1504</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>666</v>
+        <v>1100</v>
       </c>
       <c r="B401" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C401" t="b">
         <v>1</v>
       </c>
       <c r="E401" t="s">
-        <v>666</v>
+        <v>991</v>
       </c>
       <c r="F401" t="s">
-        <v>667</v>
+        <v>1228</v>
       </c>
       <c r="G401" t="s">
-        <v>1481</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>1099</v>
+        <v>668</v>
       </c>
       <c r="B402" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C402" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E402" t="s">
-        <v>990</v>
+        <v>670</v>
       </c>
       <c r="F402" t="s">
-        <v>1227</v>
+        <v>669</v>
       </c>
       <c r="G402" t="s">
-        <v>1651</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>1100</v>
+        <v>671</v>
       </c>
       <c r="B403" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C403" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E403" t="s">
-        <v>991</v>
+        <v>673</v>
       </c>
       <c r="F403" t="s">
-        <v>1228</v>
+        <v>672</v>
       </c>
       <c r="G403" t="s">
-        <v>1652</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="404" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>668</v>
+        <v>992</v>
       </c>
       <c r="B404" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C404" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E404" t="s">
-        <v>670</v>
+        <v>992</v>
       </c>
       <c r="F404" t="s">
-        <v>669</v>
+        <v>1229</v>
       </c>
       <c r="G404" t="s">
-        <v>1482</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="405" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="B405" t="b">
         <v>1</v>
       </c>
       <c r="C405" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E405" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="F405" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="G405" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="406" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>992</v>
+        <v>677</v>
       </c>
       <c r="B406" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C406" t="b">
         <v>1</v>
       </c>
       <c r="E406" t="s">
-        <v>992</v>
+        <v>8</v>
       </c>
       <c r="F406" t="s">
-        <v>1229</v>
+        <v>331</v>
       </c>
       <c r="G406" t="s">
-        <v>1653</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="407" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="B407" t="b">
         <v>1</v>
@@ -14272,18 +14371,18 @@
         <v>1</v>
       </c>
       <c r="E407" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="F407" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="G407" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="408" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="B408" t="b">
         <v>1</v>
@@ -14292,98 +14391,98 @@
         <v>1</v>
       </c>
       <c r="E408" t="s">
-        <v>8</v>
+        <v>683</v>
       </c>
       <c r="F408" t="s">
-        <v>331</v>
+        <v>682</v>
       </c>
       <c r="G408" t="s">
-        <v>1409</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>678</v>
+        <v>993</v>
       </c>
       <c r="B409" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C409" t="b">
         <v>1</v>
       </c>
       <c r="E409" t="s">
-        <v>680</v>
+        <v>993</v>
       </c>
       <c r="F409" t="s">
-        <v>679</v>
+        <v>1230</v>
       </c>
       <c r="G409" t="s">
-        <v>1485</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>681</v>
+        <v>994</v>
       </c>
       <c r="B410" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C410" t="b">
         <v>1</v>
       </c>
       <c r="E410" t="s">
-        <v>683</v>
+        <v>994</v>
       </c>
       <c r="F410" t="s">
-        <v>682</v>
+        <v>1231</v>
       </c>
       <c r="G410" t="s">
-        <v>1486</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>993</v>
+        <v>684</v>
       </c>
       <c r="B411" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C411" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E411" t="s">
-        <v>993</v>
+        <v>686</v>
       </c>
       <c r="F411" t="s">
-        <v>1230</v>
+        <v>685</v>
       </c>
       <c r="G411" t="s">
-        <v>1654</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>994</v>
+        <v>687</v>
       </c>
       <c r="B412" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C412" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E412" t="s">
-        <v>994</v>
+        <v>689</v>
       </c>
       <c r="F412" t="s">
-        <v>1231</v>
+        <v>688</v>
       </c>
       <c r="G412" t="s">
-        <v>1655</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="B413" t="b">
         <v>1</v>
@@ -14392,18 +14491,18 @@
         <v>0</v>
       </c>
       <c r="E413" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
       <c r="F413" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="G413" t="s">
-        <v>1487</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="414" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
       <c r="B414" t="b">
         <v>1</v>
@@ -14412,78 +14511,78 @@
         <v>0</v>
       </c>
       <c r="E414" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="F414" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
       <c r="G414" t="s">
-        <v>1488</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>690</v>
+        <v>995</v>
       </c>
       <c r="B415" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C415" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E415" t="s">
-        <v>692</v>
+        <v>995</v>
       </c>
       <c r="F415" t="s">
-        <v>691</v>
+        <v>1232</v>
       </c>
       <c r="G415" t="s">
-        <v>1489</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>693</v>
+        <v>996</v>
       </c>
       <c r="B416" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C416" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E416" t="s">
-        <v>695</v>
+        <v>996</v>
       </c>
       <c r="F416" t="s">
-        <v>694</v>
+        <v>1233</v>
       </c>
       <c r="G416" t="s">
-        <v>1490</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="417" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>995</v>
+        <v>696</v>
       </c>
       <c r="B417" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C417" t="b">
         <v>1</v>
       </c>
       <c r="E417" t="s">
-        <v>995</v>
+        <v>698</v>
       </c>
       <c r="F417" t="s">
-        <v>1232</v>
+        <v>697</v>
       </c>
       <c r="G417" t="s">
-        <v>1656</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="418" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>996</v>
+        <v>1101</v>
       </c>
       <c r="B418" t="b">
         <v>0</v>
@@ -14492,58 +14591,58 @@
         <v>1</v>
       </c>
       <c r="E418" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F418" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="G418" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="419" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="B419" t="b">
         <v>1</v>
       </c>
       <c r="C419" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E419" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="F419" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="G419" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>1101</v>
+        <v>701</v>
       </c>
       <c r="B420" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C420" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E420" t="s">
-        <v>997</v>
+        <v>703</v>
       </c>
       <c r="F420" t="s">
-        <v>1234</v>
+        <v>702</v>
       </c>
       <c r="G420" t="s">
-        <v>1658</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="421" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="B421" t="b">
         <v>1</v>
@@ -14552,18 +14651,18 @@
         <v>0</v>
       </c>
       <c r="E421" t="s">
-        <v>699</v>
+        <v>706</v>
       </c>
       <c r="F421" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
       <c r="G421" t="s">
-        <v>1492</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="B422" t="b">
         <v>1</v>
@@ -14572,18 +14671,18 @@
         <v>0</v>
       </c>
       <c r="E422" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="F422" t="s">
-        <v>702</v>
+        <v>1252</v>
       </c>
       <c r="G422" t="s">
-        <v>1493</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
       <c r="B423" t="b">
         <v>1</v>
@@ -14592,58 +14691,58 @@
         <v>0</v>
       </c>
       <c r="E423" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="F423" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="G423" t="s">
-        <v>1494</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="424" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>707</v>
+        <v>998</v>
       </c>
       <c r="B424" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C424" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E424" t="s">
-        <v>708</v>
+        <v>998</v>
       </c>
       <c r="F424" t="s">
-        <v>1252</v>
+        <v>1235</v>
       </c>
       <c r="G424" t="s">
-        <v>1495</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="425" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>709</v>
+        <v>1102</v>
       </c>
       <c r="B425" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C425" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E425" t="s">
-        <v>711</v>
+        <v>999</v>
       </c>
       <c r="F425" t="s">
-        <v>710</v>
+        <v>1236</v>
       </c>
       <c r="G425" t="s">
-        <v>1496</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="426" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>998</v>
+        <v>1103</v>
       </c>
       <c r="B426" t="b">
         <v>0</v>
@@ -14652,18 +14751,18 @@
         <v>1</v>
       </c>
       <c r="E426" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="F426" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="G426" t="s">
-        <v>1659</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="427" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>1102</v>
+        <v>1009</v>
       </c>
       <c r="B427" t="b">
         <v>0</v>
@@ -14672,58 +14771,58 @@
         <v>1</v>
       </c>
       <c r="E427" t="s">
-        <v>999</v>
+        <v>1009</v>
       </c>
       <c r="F427" t="s">
-        <v>1236</v>
+        <v>1246</v>
       </c>
       <c r="G427" t="s">
-        <v>1660</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="428" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>1103</v>
+        <v>608</v>
       </c>
       <c r="B428" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C428" t="b">
         <v>1</v>
       </c>
       <c r="E428" t="s">
-        <v>1000</v>
+        <v>608</v>
       </c>
       <c r="F428" t="s">
-        <v>1237</v>
+        <v>712</v>
       </c>
       <c r="G428" t="s">
-        <v>1661</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>1009</v>
+        <v>713</v>
       </c>
       <c r="B429" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C429" t="b">
         <v>1</v>
       </c>
       <c r="E429" t="s">
-        <v>1009</v>
+        <v>23</v>
       </c>
       <c r="F429" t="s">
-        <v>1246</v>
+        <v>714</v>
       </c>
       <c r="G429" t="s">
-        <v>1669</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="430" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>608</v>
+        <v>715</v>
       </c>
       <c r="B430" t="b">
         <v>1</v>
@@ -14732,18 +14831,18 @@
         <v>1</v>
       </c>
       <c r="E430" t="s">
-        <v>608</v>
+        <v>717</v>
       </c>
       <c r="F430" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="G430" t="s">
-        <v>1460</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="431" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c r="B431" t="b">
         <v>1</v>
@@ -14752,18 +14851,18 @@
         <v>1</v>
       </c>
       <c r="E431" t="s">
-        <v>23</v>
+        <v>720</v>
       </c>
       <c r="F431" t="s">
-        <v>714</v>
+        <v>719</v>
       </c>
       <c r="G431" t="s">
-        <v>1260</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="432" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>715</v>
+        <v>721</v>
       </c>
       <c r="B432" t="b">
         <v>1</v>
@@ -14772,18 +14871,18 @@
         <v>1</v>
       </c>
       <c r="E432" t="s">
-        <v>717</v>
+        <v>146</v>
       </c>
       <c r="F432" t="s">
-        <v>716</v>
+        <v>147</v>
       </c>
       <c r="G432" t="s">
-        <v>1497</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="433" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="B433" t="b">
         <v>1</v>
@@ -14792,18 +14891,18 @@
         <v>1</v>
       </c>
       <c r="E433" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="F433" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="G433" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="434" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="B434" t="b">
         <v>1</v>
@@ -14812,18 +14911,18 @@
         <v>1</v>
       </c>
       <c r="E434" t="s">
-        <v>146</v>
+        <v>727</v>
       </c>
       <c r="F434" t="s">
-        <v>147</v>
+        <v>726</v>
       </c>
       <c r="G434" t="s">
-        <v>1302</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="435" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>722</v>
+        <v>728</v>
       </c>
       <c r="B435" t="b">
         <v>1</v>
@@ -14832,78 +14931,78 @@
         <v>1</v>
       </c>
       <c r="E435" t="s">
-        <v>724</v>
+        <v>609</v>
       </c>
       <c r="F435" t="s">
-        <v>723</v>
+        <v>729</v>
       </c>
       <c r="G435" t="s">
-        <v>1499</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="436" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="B436" t="b">
         <v>1</v>
       </c>
       <c r="C436" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E436" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="F436" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="G436" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="437" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="B437" t="b">
         <v>1</v>
       </c>
       <c r="C437" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E437" t="s">
-        <v>609</v>
+        <v>735</v>
       </c>
       <c r="F437" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="G437" t="s">
-        <v>1430</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="438" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>730</v>
+        <v>1104</v>
       </c>
       <c r="B438" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C438" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E438" t="s">
-        <v>732</v>
+        <v>1001</v>
       </c>
       <c r="F438" t="s">
-        <v>731</v>
+        <v>1238</v>
       </c>
       <c r="G438" t="s">
-        <v>1501</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="439" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="B439" t="b">
         <v>1</v>
@@ -14912,38 +15011,38 @@
         <v>0</v>
       </c>
       <c r="E439" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="F439" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="G439" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="440" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>1104</v>
+        <v>739</v>
       </c>
       <c r="B440" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C440" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E440" t="s">
-        <v>1001</v>
+        <v>741</v>
       </c>
       <c r="F440" t="s">
-        <v>1238</v>
+        <v>740</v>
       </c>
       <c r="G440" t="s">
-        <v>1690</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="441" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="B441" t="b">
         <v>1</v>
@@ -14952,38 +15051,38 @@
         <v>0</v>
       </c>
       <c r="E441" t="s">
-        <v>738</v>
+        <v>744</v>
       </c>
       <c r="F441" t="s">
-        <v>737</v>
+        <v>743</v>
       </c>
       <c r="G441" t="s">
-        <v>1503</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="442" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>739</v>
+        <v>745</v>
       </c>
       <c r="B442" t="b">
         <v>1</v>
       </c>
       <c r="C442" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E442" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="F442" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="G442" t="s">
-        <v>1504</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="B443" t="b">
         <v>1</v>
@@ -14992,38 +15091,38 @@
         <v>0</v>
       </c>
       <c r="E443" t="s">
-        <v>744</v>
+        <v>749</v>
       </c>
       <c r="F443" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
       <c r="G443" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="444" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>745</v>
+        <v>750</v>
       </c>
       <c r="B444" t="b">
         <v>1</v>
       </c>
       <c r="C444" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E444" t="s">
-        <v>745</v>
+        <v>752</v>
       </c>
       <c r="F444" t="s">
-        <v>746</v>
+        <v>751</v>
       </c>
       <c r="G444" t="s">
-        <v>1460</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="445" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="B445" t="b">
         <v>1</v>
@@ -15032,58 +15131,58 @@
         <v>0</v>
       </c>
       <c r="E445" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="F445" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
       <c r="G445" t="s">
-        <v>1506</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>750</v>
+        <v>524</v>
       </c>
       <c r="B446" t="b">
         <v>1</v>
       </c>
       <c r="C446" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E446" t="s">
-        <v>752</v>
+        <v>524</v>
       </c>
       <c r="F446" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="G446" t="s">
-        <v>1507</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="447" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="B447" t="b">
         <v>1</v>
       </c>
       <c r="C447" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E447" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
       <c r="F447" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="G447" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="448" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>524</v>
+        <v>759</v>
       </c>
       <c r="B448" t="b">
         <v>1</v>
@@ -15092,58 +15191,58 @@
         <v>1</v>
       </c>
       <c r="E448" t="s">
-        <v>524</v>
+        <v>759</v>
       </c>
       <c r="F448" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
       <c r="G448" t="s">
-        <v>1432</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="449" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>756</v>
+        <v>1105</v>
       </c>
       <c r="B449" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C449" t="b">
         <v>1</v>
       </c>
       <c r="E449" t="s">
-        <v>758</v>
+        <v>1002</v>
       </c>
       <c r="F449" t="s">
-        <v>757</v>
+        <v>1239</v>
       </c>
       <c r="G449" t="s">
-        <v>1509</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="450" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>759</v>
+        <v>1106</v>
       </c>
       <c r="B450" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C450" t="b">
         <v>1</v>
       </c>
       <c r="E450" t="s">
-        <v>759</v>
+        <v>1003</v>
       </c>
       <c r="F450" t="s">
-        <v>760</v>
+        <v>1240</v>
       </c>
       <c r="G450" t="s">
-        <v>1510</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="451" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
       <c r="B451" t="b">
         <v>0</v>
@@ -15152,18 +15251,18 @@
         <v>1</v>
       </c>
       <c r="E451" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="F451" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="G451" t="s">
-        <v>1662</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="452" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="B452" t="b">
         <v>0</v>
@@ -15172,78 +15271,78 @@
         <v>1</v>
       </c>
       <c r="E452" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="F452" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="G452" t="s">
-        <v>1663</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="453" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>1107</v>
+        <v>761</v>
       </c>
       <c r="B453" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C453" t="b">
         <v>1</v>
       </c>
       <c r="E453" t="s">
-        <v>1004</v>
+        <v>761</v>
       </c>
       <c r="F453" t="s">
-        <v>1241</v>
+        <v>762</v>
       </c>
       <c r="G453" t="s">
-        <v>1664</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="454" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>1108</v>
+        <v>763</v>
       </c>
       <c r="B454" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C454" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E454" t="s">
-        <v>1005</v>
+        <v>765</v>
       </c>
       <c r="F454" t="s">
-        <v>1242</v>
+        <v>764</v>
       </c>
       <c r="G454" t="s">
-        <v>1665</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="455" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>761</v>
+        <v>766</v>
       </c>
       <c r="B455" t="b">
         <v>1</v>
       </c>
       <c r="C455" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E455" t="s">
-        <v>761</v>
+        <v>768</v>
       </c>
       <c r="F455" t="s">
-        <v>762</v>
+        <v>767</v>
       </c>
       <c r="G455" t="s">
-        <v>1511</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="456" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="B456" t="b">
         <v>1</v>
@@ -15252,18 +15351,18 @@
         <v>0</v>
       </c>
       <c r="E456" t="s">
-        <v>765</v>
+        <v>771</v>
       </c>
       <c r="F456" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
       <c r="G456" t="s">
-        <v>1512</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c r="B457" t="b">
         <v>1</v>
@@ -15272,18 +15371,18 @@
         <v>0</v>
       </c>
       <c r="E457" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="F457" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="G457" t="s">
-        <v>1513</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="B458" t="b">
         <v>1</v>
@@ -15292,18 +15391,18 @@
         <v>0</v>
       </c>
       <c r="E458" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
       <c r="F458" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c r="G458" t="s">
-        <v>1514</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="459" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c r="B459" t="b">
         <v>1</v>
@@ -15312,18 +15411,18 @@
         <v>0</v>
       </c>
       <c r="E459" t="s">
-        <v>774</v>
+        <v>780</v>
       </c>
       <c r="F459" t="s">
-        <v>773</v>
+        <v>779</v>
       </c>
       <c r="G459" t="s">
-        <v>1515</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="B460" t="b">
         <v>1</v>
@@ -15332,58 +15431,58 @@
         <v>0</v>
       </c>
       <c r="E460" t="s">
-        <v>777</v>
+        <v>783</v>
       </c>
       <c r="F460" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="G460" t="s">
-        <v>1516</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="461" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>778</v>
+        <v>1692</v>
       </c>
       <c r="B461" t="b">
         <v>1</v>
       </c>
       <c r="C461" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E461" t="s">
-        <v>780</v>
+        <v>1693</v>
       </c>
       <c r="F461" t="s">
-        <v>779</v>
+        <v>1694</v>
       </c>
       <c r="G461" t="s">
-        <v>1517</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="462" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>781</v>
+        <v>1695</v>
       </c>
       <c r="B462" t="b">
         <v>1</v>
       </c>
       <c r="C462" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E462" t="s">
-        <v>783</v>
+        <v>1697</v>
       </c>
       <c r="F462" t="s">
-        <v>782</v>
+        <v>1696</v>
       </c>
       <c r="G462" t="s">
-        <v>1518</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>1692</v>
+        <v>1698</v>
       </c>
       <c r="B463" t="b">
         <v>1</v>
@@ -15392,18 +15491,18 @@
         <v>1</v>
       </c>
       <c r="E463" t="s">
-        <v>1693</v>
+        <v>666</v>
       </c>
       <c r="F463" t="s">
-        <v>1694</v>
+        <v>1724</v>
       </c>
       <c r="G463" t="s">
-        <v>1810</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>1695</v>
+        <v>1708</v>
       </c>
       <c r="B464" t="b">
         <v>1</v>
@@ -15412,18 +15511,18 @@
         <v>1</v>
       </c>
       <c r="E464" t="s">
-        <v>1697</v>
+        <v>1699</v>
       </c>
       <c r="F464" t="s">
-        <v>1696</v>
+        <v>1185</v>
       </c>
       <c r="G464" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="465" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>1698</v>
+        <v>1709</v>
       </c>
       <c r="B465" t="b">
         <v>1</v>
@@ -15432,18 +15531,18 @@
         <v>1</v>
       </c>
       <c r="E465" t="s">
-        <v>666</v>
+        <v>1700</v>
       </c>
       <c r="F465" t="s">
-        <v>1724</v>
+        <v>1717</v>
       </c>
       <c r="G465" t="s">
-        <v>1481</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="466" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>1708</v>
+        <v>1710</v>
       </c>
       <c r="B466" t="b">
         <v>1</v>
@@ -15452,18 +15551,18 @@
         <v>1</v>
       </c>
       <c r="E466" t="s">
-        <v>1699</v>
+        <v>1701</v>
       </c>
       <c r="F466" t="s">
-        <v>1185</v>
+        <v>1725</v>
       </c>
       <c r="G466" t="s">
-        <v>1812</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="467" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>1709</v>
+        <v>1711</v>
       </c>
       <c r="B467" t="b">
         <v>1</v>
@@ -15472,18 +15571,18 @@
         <v>1</v>
       </c>
       <c r="E467" t="s">
-        <v>1700</v>
+        <v>1702</v>
       </c>
       <c r="F467" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="G467" t="s">
-        <v>1813</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="468" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>1710</v>
+        <v>1712</v>
       </c>
       <c r="B468" t="b">
         <v>1</v>
@@ -15492,18 +15591,18 @@
         <v>1</v>
       </c>
       <c r="E468" t="s">
-        <v>1701</v>
+        <v>1703</v>
       </c>
       <c r="F468" t="s">
-        <v>1725</v>
+        <v>1719</v>
       </c>
       <c r="G468" t="s">
-        <v>1814</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>1711</v>
+        <v>1713</v>
       </c>
       <c r="B469" t="b">
         <v>1</v>
@@ -15512,18 +15611,18 @@
         <v>1</v>
       </c>
       <c r="E469" t="s">
-        <v>1702</v>
+        <v>1704</v>
       </c>
       <c r="F469" t="s">
-        <v>1718</v>
+        <v>1720</v>
       </c>
       <c r="G469" t="s">
-        <v>1815</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="470" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>1712</v>
+        <v>1714</v>
       </c>
       <c r="B470" t="b">
         <v>1</v>
@@ -15532,18 +15631,18 @@
         <v>1</v>
       </c>
       <c r="E470" t="s">
-        <v>1703</v>
+        <v>1705</v>
       </c>
       <c r="F470" t="s">
-        <v>1719</v>
+        <v>1721</v>
       </c>
       <c r="G470" t="s">
-        <v>1816</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="471" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>1713</v>
+        <v>1715</v>
       </c>
       <c r="B471" t="b">
         <v>1</v>
@@ -15552,18 +15651,18 @@
         <v>1</v>
       </c>
       <c r="E471" t="s">
-        <v>1704</v>
+        <v>1706</v>
       </c>
       <c r="F471" t="s">
-        <v>1720</v>
+        <v>1722</v>
       </c>
       <c r="G471" t="s">
-        <v>1817</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="472" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>1714</v>
+        <v>1716</v>
       </c>
       <c r="B472" t="b">
         <v>1</v>
@@ -15572,18 +15671,18 @@
         <v>1</v>
       </c>
       <c r="E472" t="s">
-        <v>1705</v>
+        <v>1707</v>
       </c>
       <c r="F472" t="s">
-        <v>1721</v>
+        <v>1723</v>
       </c>
       <c r="G472" t="s">
-        <v>1818</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="473" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>1715</v>
+        <v>1726</v>
       </c>
       <c r="B473" t="b">
         <v>1</v>
@@ -15592,18 +15691,18 @@
         <v>1</v>
       </c>
       <c r="E473" t="s">
-        <v>1706</v>
+        <v>1727</v>
       </c>
       <c r="F473" t="s">
-        <v>1722</v>
+        <v>1728</v>
       </c>
       <c r="G473" t="s">
-        <v>1819</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="474" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>1716</v>
+        <v>1729</v>
       </c>
       <c r="B474" t="b">
         <v>1</v>
@@ -15612,18 +15711,18 @@
         <v>1</v>
       </c>
       <c r="E474" t="s">
-        <v>1707</v>
+        <v>1731</v>
       </c>
       <c r="F474" t="s">
-        <v>1723</v>
+        <v>1730</v>
       </c>
       <c r="G474" t="s">
-        <v>1820</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="475" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>1726</v>
+        <v>1732</v>
       </c>
       <c r="B475" t="b">
         <v>1</v>
@@ -15632,18 +15731,18 @@
         <v>1</v>
       </c>
       <c r="E475" t="s">
-        <v>1727</v>
+        <v>1735</v>
       </c>
       <c r="F475" t="s">
-        <v>1728</v>
+        <v>867</v>
       </c>
       <c r="G475" t="s">
-        <v>1821</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="476" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>1729</v>
+        <v>1733</v>
       </c>
       <c r="B476" t="b">
         <v>1</v>
@@ -15652,18 +15751,18 @@
         <v>1</v>
       </c>
       <c r="E476" t="s">
-        <v>1731</v>
+        <v>1736</v>
       </c>
       <c r="F476" t="s">
-        <v>1730</v>
+        <v>869</v>
       </c>
       <c r="G476" t="s">
-        <v>1822</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="477" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>1732</v>
+        <v>1734</v>
       </c>
       <c r="B477" t="b">
         <v>1</v>
@@ -15672,18 +15771,18 @@
         <v>1</v>
       </c>
       <c r="E477" t="s">
-        <v>1735</v>
+        <v>1737</v>
       </c>
       <c r="F477" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="G477" t="s">
-        <v>1823</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="478" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>1733</v>
+        <v>1739</v>
       </c>
       <c r="B478" t="b">
         <v>1</v>
@@ -15692,18 +15791,18 @@
         <v>1</v>
       </c>
       <c r="E478" t="s">
-        <v>1736</v>
+        <v>1741</v>
       </c>
       <c r="F478" t="s">
-        <v>869</v>
+        <v>1743</v>
       </c>
       <c r="G478" t="s">
-        <v>1824</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="479" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>1734</v>
+        <v>1740</v>
       </c>
       <c r="B479" t="b">
         <v>1</v>
@@ -15712,18 +15811,18 @@
         <v>1</v>
       </c>
       <c r="E479" t="s">
-        <v>1737</v>
+        <v>1742</v>
       </c>
       <c r="F479" t="s">
-        <v>871</v>
+        <v>1744</v>
       </c>
       <c r="G479" t="s">
-        <v>1825</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="480" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>1739</v>
+        <v>1745</v>
       </c>
       <c r="B480" t="b">
         <v>1</v>
@@ -15732,18 +15831,18 @@
         <v>1</v>
       </c>
       <c r="E480" t="s">
-        <v>1741</v>
+        <v>1746</v>
       </c>
       <c r="F480" t="s">
-        <v>1743</v>
+        <v>1747</v>
       </c>
       <c r="G480" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="481" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>1740</v>
+        <v>1749</v>
       </c>
       <c r="B481" t="b">
         <v>1</v>
@@ -15752,18 +15851,18 @@
         <v>1</v>
       </c>
       <c r="E481" t="s">
-        <v>1742</v>
+        <v>1751</v>
       </c>
       <c r="F481" t="s">
-        <v>1744</v>
+        <v>1754</v>
       </c>
       <c r="G481" t="s">
-        <v>1827</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="482" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>1745</v>
+        <v>1748</v>
       </c>
       <c r="B482" t="b">
         <v>1</v>
@@ -15772,18 +15871,18 @@
         <v>1</v>
       </c>
       <c r="E482" t="s">
-        <v>1746</v>
+        <v>1752</v>
       </c>
       <c r="F482" t="s">
-        <v>1747</v>
+        <v>1755</v>
       </c>
       <c r="G482" t="s">
-        <v>1828</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="483" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="B483" t="b">
         <v>1</v>
@@ -15792,18 +15891,18 @@
         <v>1</v>
       </c>
       <c r="E483" t="s">
-        <v>1751</v>
+        <v>1753</v>
       </c>
       <c r="F483" t="s">
-        <v>1754</v>
+        <v>1756</v>
       </c>
       <c r="G483" t="s">
-        <v>1829</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="484" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>1748</v>
+        <v>1757</v>
       </c>
       <c r="B484" t="b">
         <v>1</v>
@@ -15812,18 +15911,18 @@
         <v>1</v>
       </c>
       <c r="E484" t="s">
-        <v>1752</v>
+        <v>1761</v>
       </c>
       <c r="F484" t="s">
-        <v>1755</v>
+        <v>1765</v>
       </c>
       <c r="G484" t="s">
-        <v>1830</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="485" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>1750</v>
+        <v>1758</v>
       </c>
       <c r="B485" t="b">
         <v>1</v>
@@ -15832,18 +15931,18 @@
         <v>1</v>
       </c>
       <c r="E485" t="s">
-        <v>1753</v>
+        <v>1762</v>
       </c>
       <c r="F485" t="s">
-        <v>1756</v>
+        <v>1766</v>
       </c>
       <c r="G485" t="s">
-        <v>1831</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="486" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>1757</v>
+        <v>1759</v>
       </c>
       <c r="B486" t="b">
         <v>1</v>
@@ -15852,18 +15951,18 @@
         <v>1</v>
       </c>
       <c r="E486" t="s">
-        <v>1761</v>
+        <v>1763</v>
       </c>
       <c r="F486" t="s">
-        <v>1765</v>
+        <v>1767</v>
       </c>
       <c r="G486" t="s">
-        <v>1832</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="487" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>1758</v>
+        <v>1760</v>
       </c>
       <c r="B487" t="b">
         <v>1</v>
@@ -15872,18 +15971,18 @@
         <v>1</v>
       </c>
       <c r="E487" t="s">
-        <v>1762</v>
+        <v>1764</v>
       </c>
       <c r="F487" t="s">
-        <v>1766</v>
+        <v>1768</v>
       </c>
       <c r="G487" t="s">
-        <v>1833</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>1759</v>
+        <v>1769</v>
       </c>
       <c r="B488" t="b">
         <v>1</v>
@@ -15892,18 +15991,18 @@
         <v>1</v>
       </c>
       <c r="E488" t="s">
-        <v>1763</v>
+        <v>1679</v>
       </c>
       <c r="F488" t="s">
-        <v>1767</v>
+        <v>1792</v>
       </c>
       <c r="G488" t="s">
-        <v>1834</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="489" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>1760</v>
+        <v>1770</v>
       </c>
       <c r="B489" t="b">
         <v>1</v>
@@ -15912,18 +16011,18 @@
         <v>1</v>
       </c>
       <c r="E489" t="s">
-        <v>1764</v>
+        <v>1787</v>
       </c>
       <c r="F489" t="s">
-        <v>1768</v>
+        <v>1793</v>
       </c>
       <c r="G489" t="s">
-        <v>1835</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="490" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>1769</v>
+        <v>1771</v>
       </c>
       <c r="B490" t="b">
         <v>1</v>
@@ -15932,18 +16031,18 @@
         <v>1</v>
       </c>
       <c r="E490" t="s">
-        <v>1679</v>
+        <v>23</v>
       </c>
       <c r="F490" t="s">
-        <v>1792</v>
+        <v>714</v>
       </c>
       <c r="G490" t="s">
-        <v>1836</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="491" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>1770</v>
+        <v>1772</v>
       </c>
       <c r="B491" t="b">
         <v>1</v>
@@ -15952,18 +16051,18 @@
         <v>1</v>
       </c>
       <c r="E491" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="F491" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="G491" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="492" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>1771</v>
+        <v>1773</v>
       </c>
       <c r="B492" t="b">
         <v>1</v>
@@ -15972,18 +16071,18 @@
         <v>1</v>
       </c>
       <c r="E492" t="s">
-        <v>23</v>
+        <v>1784</v>
       </c>
       <c r="F492" t="s">
-        <v>714</v>
+        <v>1795</v>
       </c>
       <c r="G492" t="s">
-        <v>1260</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="493" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>1772</v>
+        <v>1774</v>
       </c>
       <c r="B493" t="b">
         <v>1</v>
@@ -15992,18 +16091,18 @@
         <v>1</v>
       </c>
       <c r="E493" t="s">
-        <v>1788</v>
+        <v>1789</v>
       </c>
       <c r="F493" t="s">
-        <v>1794</v>
+        <v>1804</v>
       </c>
       <c r="G493" t="s">
-        <v>1838</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>1773</v>
+        <v>1775</v>
       </c>
       <c r="B494" t="b">
         <v>1</v>
@@ -16012,18 +16111,18 @@
         <v>1</v>
       </c>
       <c r="E494" t="s">
-        <v>1784</v>
+        <v>1790</v>
       </c>
       <c r="F494" t="s">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="G494" t="s">
-        <v>1839</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>1774</v>
+        <v>1776</v>
       </c>
       <c r="B495" t="b">
         <v>1</v>
@@ -16032,18 +16131,18 @@
         <v>1</v>
       </c>
       <c r="E495" t="s">
-        <v>1789</v>
+        <v>1791</v>
       </c>
       <c r="F495" t="s">
-        <v>1804</v>
+        <v>1797</v>
       </c>
       <c r="G495" t="s">
-        <v>1840</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="496" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>1775</v>
+        <v>1777</v>
       </c>
       <c r="B496" t="b">
         <v>1</v>
@@ -16052,18 +16151,18 @@
         <v>1</v>
       </c>
       <c r="E496" t="s">
-        <v>1790</v>
+        <v>443</v>
       </c>
       <c r="F496" t="s">
-        <v>1796</v>
+        <v>1798</v>
       </c>
       <c r="G496" t="s">
-        <v>1841</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="497" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>1776</v>
+        <v>1778</v>
       </c>
       <c r="B497" t="b">
         <v>1</v>
@@ -16072,18 +16171,18 @@
         <v>1</v>
       </c>
       <c r="E497" t="s">
-        <v>1791</v>
+        <v>458</v>
       </c>
       <c r="F497" t="s">
-        <v>1797</v>
+        <v>1799</v>
       </c>
       <c r="G497" t="s">
-        <v>1842</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="498" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>1777</v>
+        <v>1779</v>
       </c>
       <c r="B498" t="b">
         <v>1</v>
@@ -16092,18 +16191,18 @@
         <v>1</v>
       </c>
       <c r="E498" t="s">
-        <v>443</v>
+        <v>1785</v>
       </c>
       <c r="F498" t="s">
-        <v>1798</v>
+        <v>1800</v>
       </c>
       <c r="G498" t="s">
-        <v>1403</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="499" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>1778</v>
+        <v>1780</v>
       </c>
       <c r="B499" t="b">
         <v>1</v>
@@ -16112,18 +16211,18 @@
         <v>1</v>
       </c>
       <c r="E499" t="s">
-        <v>458</v>
+        <v>1786</v>
       </c>
       <c r="F499" t="s">
-        <v>1799</v>
+        <v>1801</v>
       </c>
       <c r="G499" t="s">
-        <v>1408</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="500" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>1779</v>
+        <v>1781</v>
       </c>
       <c r="B500" t="b">
         <v>1</v>
@@ -16132,18 +16231,18 @@
         <v>1</v>
       </c>
       <c r="E500" t="s">
-        <v>1785</v>
+        <v>449</v>
       </c>
       <c r="F500" t="s">
-        <v>1800</v>
+        <v>1802</v>
       </c>
       <c r="G500" t="s">
-        <v>1843</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="501" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>1780</v>
+        <v>1782</v>
       </c>
       <c r="B501" t="b">
         <v>1</v>
@@ -16152,18 +16251,18 @@
         <v>1</v>
       </c>
       <c r="E501" t="s">
-        <v>1786</v>
+        <v>437</v>
       </c>
       <c r="F501" t="s">
-        <v>1801</v>
+        <v>1803</v>
       </c>
       <c r="G501" t="s">
-        <v>1844</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="502" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1781</v>
+        <v>1783</v>
       </c>
       <c r="B502" t="b">
         <v>1</v>
@@ -16172,18 +16271,18 @@
         <v>1</v>
       </c>
       <c r="E502" t="s">
-        <v>449</v>
+        <v>683</v>
       </c>
       <c r="F502" t="s">
-        <v>1802</v>
+        <v>682</v>
       </c>
       <c r="G502" t="s">
-        <v>1405</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="503" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>1782</v>
+        <v>842</v>
       </c>
       <c r="B503" t="b">
         <v>1</v>
@@ -16192,18 +16291,18 @@
         <v>1</v>
       </c>
       <c r="E503" t="s">
-        <v>437</v>
+        <v>842</v>
       </c>
       <c r="F503" t="s">
-        <v>1803</v>
+        <v>1807</v>
       </c>
       <c r="G503" t="s">
-        <v>1401</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>1783</v>
+        <v>1805</v>
       </c>
       <c r="B504" t="b">
         <v>1</v>
@@ -16212,18 +16311,18 @@
         <v>1</v>
       </c>
       <c r="E504" t="s">
-        <v>683</v>
+        <v>1805</v>
       </c>
       <c r="F504" t="s">
-        <v>682</v>
+        <v>1806</v>
       </c>
       <c r="G504" t="s">
-        <v>1486</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="505" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>842</v>
+        <v>1808</v>
       </c>
       <c r="B505" t="b">
         <v>1</v>
@@ -16232,18 +16331,18 @@
         <v>1</v>
       </c>
       <c r="E505" t="s">
-        <v>842</v>
+        <v>830</v>
       </c>
       <c r="F505" t="s">
-        <v>1807</v>
+        <v>829</v>
       </c>
       <c r="G505" t="s">
-        <v>1536</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>1805</v>
+        <v>1849</v>
       </c>
       <c r="B506" t="b">
         <v>1</v>
@@ -16252,18 +16351,18 @@
         <v>1</v>
       </c>
       <c r="E506" t="s">
-        <v>1805</v>
+        <v>1854</v>
       </c>
       <c r="F506" t="s">
-        <v>1806</v>
+        <v>1855</v>
       </c>
       <c r="G506" t="s">
-        <v>1536</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="507" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>1808</v>
+        <v>1850</v>
       </c>
       <c r="B507" t="b">
         <v>1</v>
@@ -16272,18 +16371,18 @@
         <v>1</v>
       </c>
       <c r="E507" t="s">
-        <v>830</v>
+        <v>1853</v>
       </c>
       <c r="F507" t="s">
-        <v>829</v>
+        <v>1856</v>
       </c>
       <c r="G507" t="s">
-        <v>1532</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="508" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>1849</v>
+        <v>1851</v>
       </c>
       <c r="B508" t="b">
         <v>1</v>
@@ -16292,38 +16391,38 @@
         <v>1</v>
       </c>
       <c r="E508" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
       <c r="F508" t="s">
-        <v>1855</v>
+        <v>1857</v>
       </c>
       <c r="G508" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="509" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>1850</v>
+        <v>1860</v>
       </c>
       <c r="B509" t="b">
         <v>1</v>
       </c>
       <c r="C509" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E509" t="s">
-        <v>1853</v>
+        <v>1861</v>
       </c>
       <c r="F509" t="s">
-        <v>1856</v>
+        <v>1862</v>
       </c>
       <c r="G509" t="s">
-        <v>1858</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="510" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>1851</v>
+        <v>1864</v>
       </c>
       <c r="B510" t="b">
         <v>1</v>
@@ -16332,98 +16431,100 @@
         <v>1</v>
       </c>
       <c r="E510" t="s">
-        <v>1852</v>
+        <v>1865</v>
       </c>
       <c r="F510" t="s">
-        <v>1857</v>
+        <v>1866</v>
       </c>
       <c r="G510" t="s">
-        <v>1859</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="511" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>1860</v>
+        <v>1868</v>
       </c>
       <c r="B511" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C511" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E511" t="s">
-        <v>1861</v>
+        <v>1868</v>
       </c>
       <c r="F511" t="s">
-        <v>1862</v>
+        <v>1869</v>
       </c>
       <c r="G511" t="s">
-        <v>1863</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>1864</v>
+        <v>1871</v>
       </c>
       <c r="B512" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C512" t="b">
         <v>1</v>
       </c>
       <c r="E512" t="s">
-        <v>1865</v>
+        <v>1872</v>
       </c>
       <c r="F512" t="s">
-        <v>1866</v>
+        <v>1873</v>
       </c>
       <c r="G512" t="s">
-        <v>1867</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="513" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A513" t="s">
-        <v>1868</v>
-      </c>
-      <c r="B513" t="b">
-        <v>0</v>
-      </c>
-      <c r="C513" t="b">
-        <v>1</v>
-      </c>
-      <c r="E513" t="s">
-        <v>1868</v>
-      </c>
-      <c r="F513" t="s">
-        <v>1869</v>
-      </c>
-      <c r="G513" t="s">
-        <v>1870</v>
+      <c r="A513" s="5" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B513" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C513" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D513" s="5"/>
+      <c r="E513" s="5" t="s">
+        <v>1876</v>
+      </c>
+      <c r="F513" s="5" t="s">
+        <v>1877</v>
+      </c>
+      <c r="G513" s="5" t="s">
+        <v>1878</v>
       </c>
     </row>
     <row r="514" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A514" t="s">
-        <v>1871</v>
-      </c>
-      <c r="B514" t="b">
-        <v>0</v>
-      </c>
-      <c r="C514" t="b">
-        <v>1</v>
-      </c>
-      <c r="E514" t="s">
-        <v>1872</v>
-      </c>
-      <c r="F514" t="s">
-        <v>1873</v>
-      </c>
-      <c r="G514" t="s">
-        <v>1874</v>
+      <c r="A514" s="5" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B514" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C514" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D514" s="5"/>
+      <c r="E514" s="5" t="s">
+        <v>1880</v>
+      </c>
+      <c r="F514" s="5" t="s">
+        <v>1881</v>
+      </c>
+      <c r="G514" s="5" t="s">
+        <v>1882</v>
       </c>
     </row>
     <row r="515" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A515" s="5" t="s">
-        <v>1875</v>
+        <v>1883</v>
       </c>
       <c r="B515" s="5" t="b">
         <v>1</v>
@@ -16433,102 +16534,315 @@
       </c>
       <c r="D515" s="5"/>
       <c r="E515" s="5" t="s">
-        <v>1876</v>
+        <v>1884</v>
       </c>
       <c r="F515" s="5" t="s">
-        <v>1877</v>
+        <v>1885</v>
       </c>
       <c r="G515" s="5" t="s">
-        <v>1878</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="516" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A516" s="5" t="s">
-        <v>1879</v>
-      </c>
-      <c r="B516" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C516" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D516" s="5"/>
-      <c r="E516" s="5" t="s">
-        <v>1880</v>
-      </c>
-      <c r="F516" s="5" t="s">
-        <v>1881</v>
-      </c>
-      <c r="G516" s="5" t="s">
-        <v>1882</v>
+      <c r="A516" s="6" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B516" t="b">
+        <v>0</v>
+      </c>
+      <c r="C516" t="b">
+        <v>1</v>
+      </c>
+      <c r="E516" t="s">
+        <v>1892</v>
+      </c>
+      <c r="F516" t="s">
+        <v>1893</v>
+      </c>
+      <c r="G516" t="s">
+        <v>1894</v>
       </c>
     </row>
     <row r="517" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A517" s="5" t="s">
-        <v>1883</v>
+        <v>1887</v>
       </c>
       <c r="B517" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C517" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D517" s="5"/>
-      <c r="E517" s="5" t="s">
-        <v>1884</v>
-      </c>
-      <c r="F517" s="5" t="s">
-        <v>1885</v>
-      </c>
-      <c r="G517" s="5" t="s">
-        <v>1886</v>
-      </c>
-    </row>
-    <row r="518" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A518" s="6" t="s">
-        <v>1892</v>
-      </c>
-      <c r="B518" t="b">
-        <v>0</v>
-      </c>
-      <c r="C518" t="b">
-        <v>1</v>
-      </c>
-      <c r="E518" t="s">
-        <v>1893</v>
-      </c>
-      <c r="F518" t="s">
-        <v>1894</v>
-      </c>
-      <c r="G518" t="s">
-        <v>1891</v>
+      <c r="E517" t="s">
+        <v>1888</v>
+      </c>
+      <c r="F517" t="s">
+        <v>1889</v>
+      </c>
+      <c r="G517" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="518" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A518" s="5" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B518" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C518" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E518" s="5" t="s">
+        <v>1896</v>
+      </c>
+      <c r="F518" s="5" t="s">
+        <v>1897</v>
+      </c>
+      <c r="G518" s="5" t="s">
+        <v>1901</v>
       </c>
     </row>
     <row r="519" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A519" s="5" t="s">
-        <v>1887</v>
+        <v>1898</v>
       </c>
       <c r="B519" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C519" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E519" t="s">
-        <v>1888</v>
-      </c>
-      <c r="F519" t="s">
-        <v>1889</v>
-      </c>
-      <c r="G519" t="s">
-        <v>1890</v>
+        <v>0</v>
+      </c>
+      <c r="D519" s="5"/>
+      <c r="E519" s="5" t="s">
+        <v>1899</v>
+      </c>
+      <c r="F519" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="G519" s="5" t="s">
+        <v>1902</v>
       </c>
     </row>
     <row r="520" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A520" s="6"/>
+      <c r="A520" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B520" t="b">
+        <v>1</v>
+      </c>
+      <c r="C520" t="b">
+        <v>1</v>
+      </c>
+      <c r="E520" t="s">
+        <v>1679</v>
+      </c>
+      <c r="F520" t="s">
+        <v>1912</v>
+      </c>
+      <c r="G520" t="s">
+        <v>1836</v>
+      </c>
     </row>
     <row r="521" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E521" s="5"/>
+      <c r="A521" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B521" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C521" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E521" t="s">
+        <v>1908</v>
+      </c>
+      <c r="F521" t="s">
+        <v>1913</v>
+      </c>
+      <c r="G521" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="522" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B522" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C522" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E522" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F522" t="s">
+        <v>1925</v>
+      </c>
+      <c r="G522" s="5" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="523" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B523" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C523" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E523" t="s">
+        <v>842</v>
+      </c>
+      <c r="F523" t="s">
+        <v>454</v>
+      </c>
+      <c r="G523" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="524" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B524" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C524" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E524" t="s">
+        <v>1909</v>
+      </c>
+      <c r="F524" t="s">
+        <v>1916</v>
+      </c>
+      <c r="G524" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="525" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B525" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C525" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E525" t="s">
+        <v>1788</v>
+      </c>
+      <c r="F525" t="s">
+        <v>1794</v>
+      </c>
+      <c r="G525" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="526" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B526" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C526" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E526" t="s">
+        <v>1910</v>
+      </c>
+      <c r="F526" t="s">
+        <v>1914</v>
+      </c>
+      <c r="G526" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="527" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B527" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C527" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E527" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F527" t="s">
+        <v>1795</v>
+      </c>
+      <c r="G527" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="528" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B528" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C528" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E528" t="s">
+        <v>1911</v>
+      </c>
+      <c r="F528" t="s">
+        <v>1915</v>
+      </c>
+      <c r="G528" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="529" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B529" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C529" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E529" t="s">
+        <v>1852</v>
+      </c>
+      <c r="F529" t="s">
+        <v>1857</v>
+      </c>
+      <c r="G529" s="5" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="530" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B530" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C530" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E530" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F530" t="s">
+        <v>1925</v>
+      </c>
+      <c r="G530" s="5" t="s">
+        <v>1927</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>

</xml_diff>

<commit_message>
Tree framework now it remembers the expansion state of the tree upon refresh
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291E2458-12AF-4749-A41F-43A51389AB71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFE458C-667F-4EB5-AE8B-C5DA5168B7A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -6221,9 +6221,9 @@
   <dimension ref="A1:G530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A500" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A509" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F533" sqref="F533"/>
+      <selection pane="bottomLeft" activeCell="E518" sqref="E518"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on the lookup definitions API
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFE458C-667F-4EB5-AE8B-C5DA5168B7A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5266DFEC-B28A-41C2-9CA1-71199F05A867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="1928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="1961">
   <si>
     <t>Key</t>
   </si>
@@ -5818,6 +5818,105 @@
   </si>
   <si>
     <t>类型</t>
+  </si>
+  <si>
+    <t>TitleSingular</t>
+  </si>
+  <si>
+    <t>الاسم المفرد</t>
+  </si>
+  <si>
+    <t>اسم الجمع</t>
+  </si>
+  <si>
+    <t>Singular Name</t>
+  </si>
+  <si>
+    <t>Plural Name</t>
+  </si>
+  <si>
+    <t>PluralName</t>
+  </si>
+  <si>
+    <t>MainMenuIcon</t>
+  </si>
+  <si>
+    <t>MainMenuSection</t>
+  </si>
+  <si>
+    <t>MainMenuSortKey</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>الترتيب في القائمة الرئيسية</t>
+  </si>
+  <si>
+    <t>القسم من القائمة الرئيسية</t>
+  </si>
+  <si>
+    <t>الأيقونة</t>
+  </si>
+  <si>
+    <t>Menu Section</t>
+  </si>
+  <si>
+    <t>Menu Sort Key</t>
+  </si>
+  <si>
+    <t>UpdateState</t>
+  </si>
+  <si>
+    <t>Update State</t>
+  </si>
+  <si>
+    <t>تعديل الحالة</t>
+  </si>
+  <si>
+    <t>奇异名称</t>
+  </si>
+  <si>
+    <t>复数名称</t>
+  </si>
+  <si>
+    <t>图标</t>
+  </si>
+  <si>
+    <t>菜单部分</t>
+  </si>
+  <si>
+    <t>菜单排序关键字</t>
+  </si>
+  <si>
+    <t>更新状态</t>
+  </si>
+  <si>
+    <t>Definition_State</t>
+  </si>
+  <si>
+    <t>Definition_State_Draft</t>
+  </si>
+  <si>
+    <t>Definition_State_Deployed</t>
+  </si>
+  <si>
+    <t>Definition_State_Archived</t>
+  </si>
+  <si>
+    <t>Deployed</t>
+  </si>
+  <si>
+    <t>Archived</t>
+  </si>
+  <si>
+    <t>مفعل</t>
+  </si>
+  <si>
+    <t>部署</t>
+  </si>
+  <si>
+    <t>存档</t>
   </si>
 </sst>
 </file>
@@ -6218,12 +6317,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G530"/>
+  <dimension ref="A1:G540"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A509" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A513" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E518" sqref="E518"/>
+      <selection pane="bottomLeft" activeCell="E529" sqref="E529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16844,6 +16943,206 @@
         <v>1927</v>
       </c>
     </row>
+    <row r="531" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B531" t="b">
+        <v>1</v>
+      </c>
+      <c r="C531" t="b">
+        <v>1</v>
+      </c>
+      <c r="E531" t="s">
+        <v>1931</v>
+      </c>
+      <c r="F531" t="s">
+        <v>1929</v>
+      </c>
+      <c r="G531" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="532" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B532" t="b">
+        <v>1</v>
+      </c>
+      <c r="C532" t="b">
+        <v>1</v>
+      </c>
+      <c r="E532" t="s">
+        <v>1932</v>
+      </c>
+      <c r="F532" t="s">
+        <v>1930</v>
+      </c>
+      <c r="G532" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="533" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B533" t="b">
+        <v>1</v>
+      </c>
+      <c r="C533" t="b">
+        <v>1</v>
+      </c>
+      <c r="E533" t="s">
+        <v>1937</v>
+      </c>
+      <c r="F533" t="s">
+        <v>1940</v>
+      </c>
+      <c r="G533" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="534" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B534" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C534" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E534" t="s">
+        <v>1941</v>
+      </c>
+      <c r="F534" t="s">
+        <v>1939</v>
+      </c>
+      <c r="G534" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="535" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B535" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C535" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E535" t="s">
+        <v>1942</v>
+      </c>
+      <c r="F535" t="s">
+        <v>1938</v>
+      </c>
+      <c r="G535" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="536" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>1943</v>
+      </c>
+      <c r="B536" t="b">
+        <v>1</v>
+      </c>
+      <c r="C536" t="b">
+        <v>1</v>
+      </c>
+      <c r="E536" t="s">
+        <v>1944</v>
+      </c>
+      <c r="F536" t="s">
+        <v>1945</v>
+      </c>
+      <c r="G536" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="537" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B537" t="b">
+        <v>1</v>
+      </c>
+      <c r="C537" t="b">
+        <v>1</v>
+      </c>
+      <c r="E537" t="s">
+        <v>666</v>
+      </c>
+      <c r="F537" t="s">
+        <v>667</v>
+      </c>
+      <c r="G537" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="538" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A538" s="5" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B538" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C538" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E538" t="s">
+        <v>1699</v>
+      </c>
+      <c r="F538" t="s">
+        <v>1185</v>
+      </c>
+      <c r="G538" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="539" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A539" s="5" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B539" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C539" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E539" t="s">
+        <v>1956</v>
+      </c>
+      <c r="F539" t="s">
+        <v>1958</v>
+      </c>
+      <c r="G539" t="s">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="540" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A540" s="5" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B540" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C540" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E540" t="s">
+        <v>1957</v>
+      </c>
+      <c r="F540" t="s">
+        <v>1857</v>
+      </c>
+      <c r="G540" t="s">
+        <v>1960</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Changed multiple charts to one specified in the report definition
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E15F2A7-B18D-4CED-951D-CEB5BA9E139E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA80FE74-B848-485F-9D7F-389DE0E28BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="660" windowWidth="28770" windowHeight="15570" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
+    <workbookView xWindow="6240" yWindow="6240" windowWidth="43200" windowHeight="23535" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$555</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$551</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2241" uniqueCount="2030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2225" uniqueCount="2014">
   <si>
     <t>Key</t>
   </si>
@@ -5919,54 +5919,6 @@
     <t>Permission_UpdateState</t>
   </si>
   <si>
-    <t>PieChart</t>
-  </si>
-  <si>
-    <t>BarChart</t>
-  </si>
-  <si>
-    <t>LineChart</t>
-  </si>
-  <si>
-    <t>AreaChart</t>
-  </si>
-  <si>
-    <t>Bar Chart</t>
-  </si>
-  <si>
-    <t>Line Chart</t>
-  </si>
-  <si>
-    <t>Area Chart</t>
-  </si>
-  <si>
-    <t>Pie Chart</t>
-  </si>
-  <si>
-    <t>مخطط أعمدة</t>
-  </si>
-  <si>
-    <t>مخطط مساحة</t>
-  </si>
-  <si>
-    <t>مخطط دائري</t>
-  </si>
-  <si>
-    <t>خط بياني</t>
-  </si>
-  <si>
-    <t>条图</t>
-  </si>
-  <si>
-    <t>折线图</t>
-  </si>
-  <si>
-    <t>面积图</t>
-  </si>
-  <si>
-    <t>饼形图</t>
-  </si>
-  <si>
     <t>Please fill the required fields above.</t>
   </si>
   <si>
@@ -6093,15 +6045,6 @@
     <t>(undefined)</t>
   </si>
   <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>بطاقة</t>
-  </si>
-  <si>
-    <t>卡</t>
-  </si>
-  <si>
     <t>ChartTypeDoesNotSupportNDimensions</t>
   </si>
   <si>
@@ -6124,6 +6067,15 @@
   </si>
   <si>
     <t>显示名称</t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>مخطط</t>
+  </si>
+  <si>
+    <t>图表</t>
   </si>
 </sst>
 </file>
@@ -6523,12 +6475,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G559"/>
+  <dimension ref="A1:G555"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A529" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G559" sqref="G559"/>
+      <selection pane="bottomLeft" activeCell="G564" sqref="G564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17883,52 +17835,52 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="541" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A541" t="s">
+    <row r="541" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A541" s="3" t="s">
+        <v>1963</v>
+      </c>
+      <c r="B541" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C541" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E541" s="3" t="s">
+        <v>1961</v>
+      </c>
+      <c r="F541" s="3" t="s">
+        <v>1964</v>
+      </c>
+      <c r="G541" s="3" t="s">
         <v>1962</v>
-      </c>
-      <c r="B541" t="b">
-        <v>0</v>
-      </c>
-      <c r="C541" t="b">
-        <v>1</v>
-      </c>
-      <c r="E541" s="3" t="s">
-        <v>1965</v>
-      </c>
-      <c r="F541" t="s">
-        <v>1969</v>
-      </c>
-      <c r="G541" t="s">
-        <v>1973</v>
       </c>
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>1963</v>
+        <v>1965</v>
       </c>
       <c r="B542" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C542" t="b">
         <v>1</v>
       </c>
-      <c r="E542" t="s">
-        <v>1966</v>
+      <c r="E542" s="3" t="s">
+        <v>1965</v>
       </c>
       <c r="F542" t="s">
-        <v>1972</v>
+        <v>1968</v>
       </c>
       <c r="G542" t="s">
-        <v>1974</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="543" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>1964</v>
+        <v>1966</v>
       </c>
       <c r="B543" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C543" t="b">
         <v>1</v>
@@ -17937,340 +17889,260 @@
         <v>1967</v>
       </c>
       <c r="F543" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="G543" t="s">
-        <v>1975</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="544" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>1961</v>
+        <v>1972</v>
       </c>
       <c r="B544" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C544" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D544" t="s">
+        <v>1975</v>
       </c>
       <c r="E544" s="3" t="s">
-        <v>1968</v>
+        <v>1973</v>
       </c>
       <c r="F544" t="s">
-        <v>1971</v>
-      </c>
-      <c r="G544" t="s">
+        <v>1974</v>
+      </c>
+      <c r="G544" s="3" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="545" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A545" s="3" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B545" t="b">
+        <v>0</v>
+      </c>
+      <c r="C545" t="b">
+        <v>1</v>
+      </c>
+      <c r="D545" s="3" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E545" s="3" t="s">
         <v>1976</v>
       </c>
-    </row>
-    <row r="545" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A545" s="3" t="s">
-        <v>1979</v>
-      </c>
-      <c r="B545" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C545" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E545" s="3" t="s">
+      <c r="F545" s="3" t="s">
         <v>1977</v>
       </c>
-      <c r="F545" s="3" t="s">
-        <v>1980</v>
-      </c>
       <c r="G545" s="3" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="546" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="B546" t="b">
         <v>1</v>
       </c>
-      <c r="C546" t="b">
+      <c r="C546" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E546" s="3" t="s">
-        <v>1981</v>
+        <v>1984</v>
       </c>
       <c r="F546" t="s">
-        <v>1984</v>
+        <v>1989</v>
       </c>
       <c r="G546" t="s">
-        <v>1986</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="547" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>1982</v>
-      </c>
-      <c r="B547" t="b">
-        <v>1</v>
-      </c>
-      <c r="C547" t="b">
+        <v>1979</v>
+      </c>
+      <c r="B547" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C547" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E547" s="3" t="s">
-        <v>1983</v>
+        <v>1985</v>
       </c>
       <c r="F547" t="s">
-        <v>1985</v>
+        <v>1990</v>
       </c>
       <c r="G547" t="s">
-        <v>1987</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="548" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A548" t="s">
-        <v>1988</v>
-      </c>
-      <c r="B548" t="b">
-        <v>1</v>
-      </c>
-      <c r="C548" t="b">
-        <v>0</v>
-      </c>
-      <c r="D548" t="s">
-        <v>1991</v>
+      <c r="A548" s="3" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B548" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C548" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="E548" s="3" t="s">
-        <v>1989</v>
+        <v>437</v>
       </c>
       <c r="F548" t="s">
-        <v>1990</v>
-      </c>
-      <c r="G548" s="3" t="s">
-        <v>1990</v>
+        <v>436</v>
+      </c>
+      <c r="G548" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="549" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A549" s="3" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B549" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C549" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E549" s="3" t="s">
+        <v>1986</v>
+      </c>
+      <c r="F549" t="s">
+        <v>1993</v>
+      </c>
+      <c r="G549" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="550" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A550" s="3" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B550" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C550" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E550" t="s">
+        <v>1987</v>
+      </c>
+      <c r="F550" t="s">
+        <v>1991</v>
+      </c>
+      <c r="G550" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="551" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A551" s="3" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B551" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C551" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E551" t="s">
         <v>1988</v>
       </c>
-      <c r="B549" t="b">
-        <v>0</v>
-      </c>
-      <c r="C549" t="b">
-        <v>1</v>
-      </c>
-      <c r="D549" s="3" t="s">
-        <v>1991</v>
-      </c>
-      <c r="E549" s="3" t="s">
+      <c r="F551" t="s">
         <v>1992</v>
       </c>
-      <c r="F549" s="3" t="s">
-        <v>1993</v>
-      </c>
-      <c r="G549" s="3" t="s">
-        <v>1993</v>
-      </c>
-    </row>
-    <row r="550" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A550" t="s">
-        <v>1994</v>
-      </c>
-      <c r="B550" t="b">
-        <v>1</v>
-      </c>
-      <c r="C550" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E550" s="3" t="s">
+      <c r="G551" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>1999</v>
+      </c>
+      <c r="B552" t="b">
+        <v>0</v>
+      </c>
+      <c r="C552" t="b">
+        <v>1</v>
+      </c>
+      <c r="E552" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F552" t="s">
         <v>2000</v>
       </c>
-      <c r="F550" t="s">
+      <c r="G552" s="3" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="553" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>2011</v>
+      </c>
+      <c r="B553" t="b">
+        <v>0</v>
+      </c>
+      <c r="C553" t="b">
+        <v>1</v>
+      </c>
+      <c r="E553" t="s">
+        <v>2011</v>
+      </c>
+      <c r="F553" t="s">
+        <v>2012</v>
+      </c>
+      <c r="G553" s="3" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="554" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B554" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C554" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E554" t="s">
+        <v>2004</v>
+      </c>
+      <c r="F554" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G554" t="s">
         <v>2005</v>
       </c>
-      <c r="G550" t="s">
+    </row>
+    <row r="555" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B555" t="b">
+        <v>0</v>
+      </c>
+      <c r="C555" t="b">
+        <v>1</v>
+      </c>
+      <c r="E555" t="s">
+        <v>2008</v>
+      </c>
+      <c r="F555" t="s">
+        <v>2009</v>
+      </c>
+      <c r="G555" t="s">
         <v>2010</v>
       </c>
     </row>
-    <row r="551" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A551" t="s">
-        <v>1995</v>
-      </c>
-      <c r="B551" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C551" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E551" s="3" t="s">
-        <v>2001</v>
-      </c>
-      <c r="F551" t="s">
-        <v>2006</v>
-      </c>
-      <c r="G551" t="s">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="552" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A552" s="3" t="s">
-        <v>1996</v>
-      </c>
-      <c r="B552" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C552" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E552" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="F552" t="s">
-        <v>436</v>
-      </c>
-      <c r="G552" t="s">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="553" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A553" s="3" t="s">
-        <v>1997</v>
-      </c>
-      <c r="B553" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C553" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E553" s="3" t="s">
-        <v>2002</v>
-      </c>
-      <c r="F553" t="s">
-        <v>2009</v>
-      </c>
-      <c r="G553" t="s">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="554" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A554" s="3" t="s">
-        <v>1998</v>
-      </c>
-      <c r="B554" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C554" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E554" t="s">
-        <v>2003</v>
-      </c>
-      <c r="F554" t="s">
-        <v>2007</v>
-      </c>
-      <c r="G554" t="s">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="555" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A555" s="3" t="s">
-        <v>1999</v>
-      </c>
-      <c r="B555" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C555" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E555" t="s">
-        <v>2004</v>
-      </c>
-      <c r="F555" t="s">
-        <v>2008</v>
-      </c>
-      <c r="G555" t="s">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="556" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A556" t="s">
-        <v>2015</v>
-      </c>
-      <c r="B556" t="b">
-        <v>0</v>
-      </c>
-      <c r="C556" t="b">
-        <v>1</v>
-      </c>
-      <c r="E556" t="s">
-        <v>2018</v>
-      </c>
-      <c r="F556" t="s">
-        <v>2016</v>
-      </c>
-      <c r="G556" s="3" t="s">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="557" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A557" t="s">
-        <v>2019</v>
-      </c>
-      <c r="B557" t="b">
-        <v>0</v>
-      </c>
-      <c r="C557" t="b">
-        <v>1</v>
-      </c>
-      <c r="E557" t="s">
-        <v>2019</v>
-      </c>
-      <c r="F557" t="s">
-        <v>2020</v>
-      </c>
-      <c r="G557" s="3" t="s">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="558" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A558" t="s">
-        <v>2022</v>
-      </c>
-      <c r="B558" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C558" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E558" t="s">
-        <v>2023</v>
-      </c>
-      <c r="F558" t="s">
-        <v>2025</v>
-      </c>
-      <c r="G558" t="s">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="559" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A559" t="s">
-        <v>2026</v>
-      </c>
-      <c r="B559" t="b">
-        <v>0</v>
-      </c>
-      <c r="C559" t="b">
-        <v>1</v>
-      </c>
-      <c r="E559" t="s">
-        <v>2027</v>
-      </c>
-      <c r="F559" t="s">
-        <v>2028</v>
-      </c>
-      <c r="G559" t="s">
-        <v>2029</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G555" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G551" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished the report definition screen (without a working BE)
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EBA7CC-5B19-407E-8137-59AEE8DB719B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABC752C-4FC6-4779-ABF1-7B7BCDCC440F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="0" windowWidth="26370" windowHeight="15600" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
+    <workbookView xWindow="26400" yWindow="4140" windowWidth="26370" windowHeight="15600" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2485" uniqueCount="2234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2501" uniqueCount="2250">
   <si>
     <t>Key</t>
   </si>
@@ -6736,6 +6736,54 @@
   </si>
   <si>
     <t>雷达图</t>
+  </si>
+  <si>
+    <t>DragDimensionsOrMeasures</t>
+  </si>
+  <si>
+    <t>Try adding rows, columns or measures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">قم بإضافة أسطر أو أعمدة أو قيم </t>
+  </si>
+  <si>
+    <t>DragSelect</t>
+  </si>
+  <si>
+    <t>قم بإضافة بعض الأعمدة</t>
+  </si>
+  <si>
+    <t>Try adding some columns</t>
+  </si>
+  <si>
+    <t>尝试添加的行，列或措施</t>
+  </si>
+  <si>
+    <t>尝试添加一些列</t>
+  </si>
+  <si>
+    <t>SpecifyNumericMeasure</t>
+  </si>
+  <si>
+    <t>Add at least one numeric measure</t>
+  </si>
+  <si>
+    <t>قم بتحديد قيمة واحدة على الأقل ذات طبيعة عددية</t>
+  </si>
+  <si>
+    <t>添加至少一个数字量度</t>
+  </si>
+  <si>
+    <t>Error_TheFollowingKeyWordsAreReserved0</t>
+  </si>
+  <si>
+    <t>المفاتيح التالية يحتكرها النظام: {0}</t>
+  </si>
+  <si>
+    <t>系统保留了以下密钥:{0}</t>
+  </si>
+  <si>
+    <t>The following IDs are reserved by the system: {0}</t>
   </si>
 </sst>
 </file>
@@ -7138,12 +7186,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G620"/>
+  <dimension ref="A1:G624"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A599" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E612" sqref="E612"/>
+      <selection pane="bottomLeft" activeCell="E625" sqref="E625"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20104,6 +20152,86 @@
         <v>1669</v>
       </c>
     </row>
+    <row r="621" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B621" t="b">
+        <v>0</v>
+      </c>
+      <c r="C621" t="b">
+        <v>1</v>
+      </c>
+      <c r="E621" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F621" t="s">
+        <v>2236</v>
+      </c>
+      <c r="G621" t="s">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="622" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>2237</v>
+      </c>
+      <c r="B622" t="b">
+        <v>0</v>
+      </c>
+      <c r="C622" t="b">
+        <v>1</v>
+      </c>
+      <c r="E622" t="s">
+        <v>2239</v>
+      </c>
+      <c r="F622" t="s">
+        <v>2238</v>
+      </c>
+      <c r="G622" t="s">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="623" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B623" t="b">
+        <v>0</v>
+      </c>
+      <c r="C623" t="b">
+        <v>1</v>
+      </c>
+      <c r="E623" t="s">
+        <v>2243</v>
+      </c>
+      <c r="F623" t="s">
+        <v>2244</v>
+      </c>
+      <c r="G623" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="624" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>2246</v>
+      </c>
+      <c r="B624" t="b">
+        <v>1</v>
+      </c>
+      <c r="C624" t="b">
+        <v>0</v>
+      </c>
+      <c r="E624" t="s">
+        <v>2249</v>
+      </c>
+      <c r="F624" t="s">
+        <v>2247</v>
+      </c>
+      <c r="G624" t="s">
+        <v>2248</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G549" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Implemented responsibility centers screens
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4251B6D5-71B2-4E37-BCED-70C09C506BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2292BB85-98C0-4A17-852F-98FD293AB8C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26400" yWindow="4140" windowWidth="26370" windowHeight="15600" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="2255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2533" uniqueCount="2277">
   <si>
     <t>Key</t>
   </si>
@@ -6799,6 +6799,72 @@
   </si>
   <si>
     <t>قطاع تشغيل</t>
+  </si>
+  <si>
+    <t>ResponsibilityCenter_Manager</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>المدير</t>
+  </si>
+  <si>
+    <t>ResponsibilityCenter_ResponsibilityType_Investment</t>
+  </si>
+  <si>
+    <t>ResponsibilityCenter_ResponsibilityType_Profit</t>
+  </si>
+  <si>
+    <t>ResponsibilityCenter_ResponsibilityType_Revenue</t>
+  </si>
+  <si>
+    <t>ResponsibilityCenter_ResponsibilityType_Cost</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>استثمار</t>
+  </si>
+  <si>
+    <t>ربح</t>
+  </si>
+  <si>
+    <t>إيراد</t>
+  </si>
+  <si>
+    <t>تكلفة</t>
+  </si>
+  <si>
+    <t>责任类型</t>
+  </si>
+  <si>
+    <t>投资</t>
+  </si>
+  <si>
+    <t>利润</t>
+  </si>
+  <si>
+    <t>收入</t>
+  </si>
+  <si>
+    <t>成本</t>
+  </si>
+  <si>
+    <t>是一家以经营分部</t>
+  </si>
+  <si>
+    <t>经理</t>
   </si>
 </sst>
 </file>
@@ -7201,12 +7267,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G627"/>
+  <dimension ref="A1:G632"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A597" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A610" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F621" sqref="F621"/>
+      <selection pane="bottomLeft" activeCell="F633" sqref="F633"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20220,6 +20286,9 @@
       <c r="F623" t="s">
         <v>2234</v>
       </c>
+      <c r="G623" t="s">
+        <v>1256</v>
+      </c>
     </row>
     <row r="624" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A624" s="3" t="s">
@@ -20237,8 +20306,11 @@
       <c r="F624" s="3" t="s">
         <v>2252</v>
       </c>
-    </row>
-    <row r="625" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G624" s="3" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="625" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A625" s="3" t="s">
         <v>2250</v>
       </c>
@@ -20254,8 +20326,11 @@
       <c r="F625" s="3" t="s">
         <v>2253</v>
       </c>
-    </row>
-    <row r="626" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G625" s="3" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="626" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
         <v>2243</v>
       </c>
@@ -20271,22 +20346,128 @@
       <c r="F626" t="s">
         <v>2248</v>
       </c>
-    </row>
-    <row r="627" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A627" t="s">
+      <c r="G626" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="627" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A627" s="3" t="s">
+        <v>2258</v>
+      </c>
+      <c r="B627" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C627" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E627" s="3" t="s">
+        <v>2262</v>
+      </c>
+      <c r="F627" s="3" t="s">
+        <v>2266</v>
+      </c>
+      <c r="G627" s="3" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="628" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A628" s="3" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B628" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C628" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E628" s="3" t="s">
+        <v>2263</v>
+      </c>
+      <c r="F628" s="3" t="s">
+        <v>2267</v>
+      </c>
+      <c r="G628" s="3" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="629" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A629" s="3" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B629" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C629" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E629" s="3" t="s">
+        <v>2264</v>
+      </c>
+      <c r="F629" s="3" t="s">
+        <v>2268</v>
+      </c>
+      <c r="G629" s="3" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="630" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A630" s="3" t="s">
+        <v>2261</v>
+      </c>
+      <c r="B630" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C630" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E630" s="3" t="s">
+        <v>2265</v>
+      </c>
+      <c r="F630" s="3" t="s">
+        <v>2269</v>
+      </c>
+      <c r="G630" s="3" t="s">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="631" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
         <v>2245</v>
       </c>
-      <c r="B627" t="b">
-        <v>1</v>
-      </c>
-      <c r="C627" t="b">
-        <v>1</v>
-      </c>
-      <c r="E627" t="s">
+      <c r="B631" t="b">
+        <v>1</v>
+      </c>
+      <c r="C631" t="b">
+        <v>1</v>
+      </c>
+      <c r="E631" t="s">
         <v>2246</v>
       </c>
-      <c r="F627" t="s">
+      <c r="F631" t="s">
         <v>2254</v>
+      </c>
+      <c r="G631" t="s">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="632" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>2255</v>
+      </c>
+      <c r="B632" t="b">
+        <v>1</v>
+      </c>
+      <c r="C632" t="b">
+        <v>1</v>
+      </c>
+      <c r="E632" t="s">
+        <v>2256</v>
+      </c>
+      <c r="F632" t="s">
+        <v>2257</v>
+      </c>
+      <c r="G632" t="s">
+        <v>2276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed FromSql now allowing for custom SQL queries
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2292BB85-98C0-4A17-852F-98FD293AB8C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E145584B-6964-47A9-8A4C-5AE9F81EE063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26400" yWindow="4140" windowWidth="26370" windowHeight="15600" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2533" uniqueCount="2277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="2289">
   <si>
     <t>Key</t>
   </si>
@@ -6865,6 +6865,42 @@
   </si>
   <si>
     <t>经理</t>
+  </si>
+  <si>
+    <t>TreeLevel</t>
+  </si>
+  <si>
+    <t>TreeChildCount</t>
+  </si>
+  <si>
+    <t>TreeActiveChildCount</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Child Count</t>
+  </si>
+  <si>
+    <t>Active Child Count</t>
+  </si>
+  <si>
+    <t>الدرجة</t>
+  </si>
+  <si>
+    <t>عدد الفروع</t>
+  </si>
+  <si>
+    <t>عدد الفروع المنشطة</t>
+  </si>
+  <si>
+    <t>水平</t>
+  </si>
+  <si>
+    <t>儿童计数</t>
+  </si>
+  <si>
+    <t>运动儿童计数</t>
   </si>
 </sst>
 </file>
@@ -7267,12 +7303,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G632"/>
+  <dimension ref="A1:G635"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A610" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A546" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F633" sqref="F633"/>
+      <selection pane="bottomLeft" activeCell="F609" sqref="F609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20470,6 +20506,66 @@
         <v>2276</v>
       </c>
     </row>
+    <row r="633" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A633" t="s">
+        <v>2277</v>
+      </c>
+      <c r="B633" t="b">
+        <v>1</v>
+      </c>
+      <c r="C633" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E633" t="s">
+        <v>2280</v>
+      </c>
+      <c r="F633" t="s">
+        <v>2283</v>
+      </c>
+      <c r="G633" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="634" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B634" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C634" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E634" t="s">
+        <v>2281</v>
+      </c>
+      <c r="F634" t="s">
+        <v>2284</v>
+      </c>
+      <c r="G634" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="635" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>2279</v>
+      </c>
+      <c r="B635" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C635" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E635" t="s">
+        <v>2282</v>
+      </c>
+      <c r="F635" t="s">
+        <v>2285</v>
+      </c>
+      <c r="G635" t="s">
+        <v>2288</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G547" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Finished the raw Agents screens, will incorporate definitions next
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B093EF26-BCE2-4A65-8937-43C35C595978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C9A65E-C0D0-4B1B-81D3-32C3E8BBC381}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="7065" windowWidth="18150" windowHeight="12585" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2533" uniqueCount="2277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="2305">
   <si>
     <t>Key</t>
   </si>
@@ -6865,6 +6865,90 @@
   </si>
   <si>
     <t>资源定义</t>
+  </si>
+  <si>
+    <t>OperatingSegment</t>
+  </si>
+  <si>
+    <t>Operating Segment</t>
+  </si>
+  <si>
+    <t>قطاع التشغيل</t>
+  </si>
+  <si>
+    <t>Agent_StartDate</t>
+  </si>
+  <si>
+    <t>Agent_Job</t>
+  </si>
+  <si>
+    <t>Agent_BasicSalary</t>
+  </si>
+  <si>
+    <t>Agent_TransportationAllowance</t>
+  </si>
+  <si>
+    <t>Agent_OvertimeRate</t>
+  </si>
+  <si>
+    <t>Agent_BankAccountNumber</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Basic Salary</t>
+  </si>
+  <si>
+    <t>Transportation Allowance</t>
+  </si>
+  <si>
+    <t>Overtime Rate</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Bank Account Number</t>
+  </si>
+  <si>
+    <t>تاريخ البدأ</t>
+  </si>
+  <si>
+    <t>الوظيفة</t>
+  </si>
+  <si>
+    <t>الراتب الأساسي</t>
+  </si>
+  <si>
+    <t>علاوة الترحيل</t>
+  </si>
+  <si>
+    <t>أجر العمل الإضافي</t>
+  </si>
+  <si>
+    <t>رقم حساب البنك</t>
+  </si>
+  <si>
+    <t>经营分部</t>
+  </si>
+  <si>
+    <t>开始日期</t>
+  </si>
+  <si>
+    <t>工作</t>
+  </si>
+  <si>
+    <t>基础工资</t>
+  </si>
+  <si>
+    <t>交通补贴</t>
+  </si>
+  <si>
+    <t>加班费</t>
+  </si>
+  <si>
+    <t>银行帐号</t>
   </si>
 </sst>
 </file>
@@ -7267,12 +7351,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G632"/>
+  <dimension ref="A1:G639"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A609" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A624" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A632" sqref="A632:XFD632"/>
+      <selection pane="bottomLeft" activeCell="G633" sqref="G633:G639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20465,6 +20549,146 @@
         <v>2276</v>
       </c>
     </row>
+    <row r="633" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A633" t="s">
+        <v>2277</v>
+      </c>
+      <c r="B633" t="b">
+        <v>1</v>
+      </c>
+      <c r="C633" t="b">
+        <v>1</v>
+      </c>
+      <c r="E633" t="s">
+        <v>2278</v>
+      </c>
+      <c r="F633" t="s">
+        <v>2279</v>
+      </c>
+      <c r="G633" t="s">
+        <v>2298</v>
+      </c>
+    </row>
+    <row r="634" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>2280</v>
+      </c>
+      <c r="B634" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C634" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E634" t="s">
+        <v>2286</v>
+      </c>
+      <c r="F634" t="s">
+        <v>2292</v>
+      </c>
+      <c r="G634" t="s">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="635" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>2281</v>
+      </c>
+      <c r="B635" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C635" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E635" t="s">
+        <v>2290</v>
+      </c>
+      <c r="F635" t="s">
+        <v>2293</v>
+      </c>
+      <c r="G635" t="s">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="636" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
+        <v>2282</v>
+      </c>
+      <c r="B636" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C636" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E636" s="3" t="s">
+        <v>2287</v>
+      </c>
+      <c r="F636" t="s">
+        <v>2294</v>
+      </c>
+      <c r="G636" t="s">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="637" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A637" t="s">
+        <v>2283</v>
+      </c>
+      <c r="B637" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C637" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E637" s="3" t="s">
+        <v>2288</v>
+      </c>
+      <c r="F637" t="s">
+        <v>2295</v>
+      </c>
+      <c r="G637" t="s">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="638" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A638" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B638" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C638" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E638" s="3" t="s">
+        <v>2289</v>
+      </c>
+      <c r="F638" t="s">
+        <v>2296</v>
+      </c>
+      <c r="G638" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="639" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
+        <v>2285</v>
+      </c>
+      <c r="B639" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C639" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E639" s="3" t="s">
+        <v>2291</v>
+      </c>
+      <c r="F639" t="s">
+        <v>2297</v>
+      </c>
+      <c r="G639" t="s">
+        <v>2304</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G543" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Implemented Entry Classifications screens
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3E69D2-84E3-4E0F-9CAE-BBB40641C0F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A239595D-C9A4-4D43-82D3-5262F394050D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31995" yWindow="0" windowWidth="17790" windowHeight="14805" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="2309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="2318">
   <si>
     <t>Key</t>
   </si>
@@ -6961,6 +6961,33 @@
   </si>
   <si>
     <t>定期</t>
+  </si>
+  <si>
+    <t>EntryClassifications</t>
+  </si>
+  <si>
+    <t>EntryClassifications_ForCredit</t>
+  </si>
+  <si>
+    <t>EntryClassifications_ForDebit</t>
+  </si>
+  <si>
+    <t>Entry Classification</t>
+  </si>
+  <si>
+    <t>Entry Classifications</t>
+  </si>
+  <si>
+    <t>EntryClassification</t>
+  </si>
+  <si>
+    <t>تصنيفات الأسطر</t>
+  </si>
+  <si>
+    <t>تصنيف السطر</t>
+  </si>
+  <si>
+    <t>进入分类</t>
   </si>
 </sst>
 </file>
@@ -7366,12 +7393,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G641"/>
+  <dimension ref="A1:G645"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A560" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B637" sqref="B637"/>
+      <selection pane="bottomLeft" activeCell="E634" sqref="E634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20737,6 +20764,86 @@
         <v>2308</v>
       </c>
     </row>
+    <row r="642" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A642" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B642" t="b">
+        <v>1</v>
+      </c>
+      <c r="C642" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E642" t="s">
+        <v>2312</v>
+      </c>
+      <c r="F642" s="6" t="s">
+        <v>2316</v>
+      </c>
+      <c r="G642" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="643" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A643" s="3" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B643" t="b">
+        <v>1</v>
+      </c>
+      <c r="C643" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E643" t="s">
+        <v>2313</v>
+      </c>
+      <c r="F643" s="6" t="s">
+        <v>2315</v>
+      </c>
+      <c r="G643" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="644" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A644" s="3" t="s">
+        <v>2310</v>
+      </c>
+      <c r="B644" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C644" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E644" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F644" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="G644" s="3" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="645" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A645" s="3" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B645" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C645" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E645" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F645" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="G645" s="3" t="s">
+        <v>1325</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G521" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Working on Documents and related entities
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A239595D-C9A4-4D43-82D3-5262F394050D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB327047-9304-4B43-889A-0F3C45B38535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31995" yWindow="0" windowWidth="17790" windowHeight="14805" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="2318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="2317">
   <si>
     <t>Key</t>
   </si>
@@ -5007,9 +5007,6 @@
     <t>Invalid</t>
   </si>
   <si>
-    <t>Posted</t>
-  </si>
-  <si>
     <t>Document_State_Draft</t>
   </si>
   <si>
@@ -5034,9 +5031,6 @@
     <t>Document_State_Invalid</t>
   </si>
   <si>
-    <t>Document_State_Posted</t>
-  </si>
-  <si>
     <t>ملغى</t>
   </si>
   <si>
@@ -5055,9 +5049,6 @@
     <t>خطأ</t>
   </si>
   <si>
-    <t>مرحل</t>
-  </si>
-  <si>
     <t>حالة القيد</t>
   </si>
   <si>
@@ -5130,45 +5121,18 @@
     <t>الملاحظات مشتركة</t>
   </si>
   <si>
-    <t>DocumentLine_ExternalReference</t>
-  </si>
-  <si>
-    <t>DocumentLine_LineType</t>
-  </si>
-  <si>
-    <t>DocumentLine_AdditionalReference</t>
-  </si>
-  <si>
-    <t>Line Type</t>
-  </si>
-  <si>
     <t>External Reference</t>
   </si>
   <si>
     <t>Additional Reference</t>
   </si>
   <si>
-    <t>نوع السطر</t>
-  </si>
-  <si>
     <t>رقم المرجع الخارجي</t>
   </si>
   <si>
     <t>مرجع إضافي</t>
   </si>
   <si>
-    <t>DocumentLine_RelatedResource</t>
-  </si>
-  <si>
-    <t>DocumentLine_RelatedAccount</t>
-  </si>
-  <si>
-    <t>DocumentLine_RelatedQuantity</t>
-  </si>
-  <si>
-    <t>DocumentLine_RelatedMoneyAmount</t>
-  </si>
-  <si>
     <t>Related Resource</t>
   </si>
   <si>
@@ -5193,48 +5157,6 @@
     <t>مبلغ نقدي ذو صلة</t>
   </si>
   <si>
-    <t>DocumentLineEntry_Account</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_IfrsEntryClassification</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Agent</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_ResponsibilityCenter</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Resource</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_BatchCode</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_MonetaryValue</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Mass</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Volume</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Area</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Length</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Time</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Count</t>
-  </si>
-  <si>
-    <t>DocumentLineEntry_Value</t>
-  </si>
-  <si>
     <t>Resource</t>
   </si>
   <si>
@@ -5361,9 +5283,6 @@
     <t>备注是常有的事</t>
   </si>
   <si>
-    <t>线路类型</t>
-  </si>
-  <si>
     <t>外部参考</t>
   </si>
   <si>
@@ -6988,6 +6907,84 @@
   </si>
   <si>
     <t>进入分类</t>
+  </si>
+  <si>
+    <t>Line_ExternalReference</t>
+  </si>
+  <si>
+    <t>Line_AdditionalReference</t>
+  </si>
+  <si>
+    <t>Line_RelatedResource</t>
+  </si>
+  <si>
+    <t>Line_RelatedAccount</t>
+  </si>
+  <si>
+    <t>Line_RelatedQuantity</t>
+  </si>
+  <si>
+    <t>Line_RelatedMoneyAmount</t>
+  </si>
+  <si>
+    <t>Entry_Account</t>
+  </si>
+  <si>
+    <t>Entry_IfrsEntryClassification</t>
+  </si>
+  <si>
+    <t>Entry_Agent</t>
+  </si>
+  <si>
+    <t>Entry_ResponsibilityCenter</t>
+  </si>
+  <si>
+    <t>Entry_Resource</t>
+  </si>
+  <si>
+    <t>Entry_BatchCode</t>
+  </si>
+  <si>
+    <t>Entry_MonetaryValue</t>
+  </si>
+  <si>
+    <t>Entry_Mass</t>
+  </si>
+  <si>
+    <t>Entry_Volume</t>
+  </si>
+  <si>
+    <t>Entry_Area</t>
+  </si>
+  <si>
+    <t>Entry_Length</t>
+  </si>
+  <si>
+    <t>Entry_Time</t>
+  </si>
+  <si>
+    <t>Entry_Count</t>
+  </si>
+  <si>
+    <t>Entry_Value</t>
+  </si>
+  <si>
+    <t>Document_State_Reviewed</t>
+  </si>
+  <si>
+    <t>Reviewed</t>
+  </si>
+  <si>
+    <t>مراجع</t>
+  </si>
+  <si>
+    <t>Document_State_Closed</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>مقفل</t>
   </si>
 </sst>
 </file>
@@ -7396,9 +7393,9 @@
   <dimension ref="A1:G645"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A560" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E634" sqref="E634"/>
+      <selection pane="bottomLeft" activeCell="A452" sqref="A452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9361,7 +9358,7 @@
         <v>162</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>1755</v>
+        <v>1729</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>1268</v>
@@ -10020,7 +10017,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>1790</v>
+        <v>1763</v>
       </c>
       <c r="B125" s="3" t="b">
         <v>1</v>
@@ -10030,13 +10027,13 @@
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3" t="s">
-        <v>1791</v>
+        <v>1764</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>1792</v>
+        <v>1765</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>1793</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -10104,7 +10101,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>2235</v>
+        <v>2208</v>
       </c>
       <c r="B129" s="3" t="b">
         <v>1</v>
@@ -10114,13 +10111,13 @@
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3" t="s">
-        <v>2236</v>
+        <v>2209</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>2238</v>
+        <v>2211</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>2237</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -14640,7 +14637,7 @@
     </row>
     <row r="345" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
-        <v>2293</v>
+        <v>2266</v>
       </c>
       <c r="B345" s="3" t="b">
         <v>1</v>
@@ -14649,13 +14646,13 @@
         <v>1</v>
       </c>
       <c r="E345" s="3" t="s">
-        <v>2294</v>
+        <v>2267</v>
       </c>
       <c r="F345" s="6" t="s">
-        <v>2296</v>
+        <v>2269</v>
       </c>
       <c r="G345" s="3" t="s">
-        <v>2295</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="346" spans="1:7" x14ac:dyDescent="0.25">
@@ -15909,7 +15906,7 @@
       </c>
       <c r="D405" s="3"/>
       <c r="E405" s="3" t="s">
-        <v>2292</v>
+        <v>2265</v>
       </c>
       <c r="F405" s="6" t="s">
         <v>1198</v>
@@ -16046,7 +16043,7 @@
     </row>
     <row r="412" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A412" s="3" t="s">
-        <v>2239</v>
+        <v>2212</v>
       </c>
       <c r="B412" s="3" t="b">
         <v>1</v>
@@ -16670,7 +16667,7 @@
         <v>1644</v>
       </c>
       <c r="G441" s="3" t="s">
-        <v>1756</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="442" spans="1:7" x14ac:dyDescent="0.25">
@@ -16691,7 +16688,7 @@
         <v>1646</v>
       </c>
       <c r="G442" s="3" t="s">
-        <v>1757</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.25">
@@ -16709,7 +16706,7 @@
         <v>648</v>
       </c>
       <c r="F443" s="6" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="G443" s="3" t="s">
         <v>1436</v>
@@ -16717,7 +16714,7 @@
     </row>
     <row r="444" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A444" s="3" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B444" s="3" t="b">
         <v>1</v>
@@ -16733,12 +16730,12 @@
         <v>1146</v>
       </c>
       <c r="G444" s="3" t="s">
-        <v>1758</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="445" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A445" s="3" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B445" s="3" t="b">
         <v>1</v>
@@ -16751,15 +16748,15 @@
         <v>1650</v>
       </c>
       <c r="F445" s="6" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="G445" s="3" t="s">
-        <v>1759</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A446" s="3" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="B446" s="3" t="b">
         <v>1</v>
@@ -16772,15 +16769,15 @@
         <v>1651</v>
       </c>
       <c r="F446" s="6" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
       <c r="G446" s="3" t="s">
-        <v>1760</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="447" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A447" s="3" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="B447" s="3" t="b">
         <v>1</v>
@@ -16793,15 +16790,15 @@
         <v>1652</v>
       </c>
       <c r="F447" s="6" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="G447" s="3" t="s">
-        <v>1761</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="448" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A448" s="3" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="B448" s="3" t="b">
         <v>1</v>
@@ -16814,15 +16811,15 @@
         <v>1653</v>
       </c>
       <c r="F448" s="6" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
       <c r="G448" s="3" t="s">
-        <v>1762</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="449" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A449" s="3" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B449" s="3" t="b">
         <v>1</v>
@@ -16835,15 +16832,15 @@
         <v>1654</v>
       </c>
       <c r="F449" s="6" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="G449" s="3" t="s">
-        <v>1763</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="450" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A450" s="3" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B450" s="3" t="b">
         <v>1</v>
@@ -16856,15 +16853,15 @@
         <v>1655</v>
       </c>
       <c r="F450" s="6" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="G450" s="3" t="s">
-        <v>1764</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="451" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A451" s="3" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="B451" s="3" t="b">
         <v>1</v>
@@ -16877,15 +16874,15 @@
         <v>1656</v>
       </c>
       <c r="F451" s="6" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="G451" s="3" t="s">
-        <v>1765</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="452" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A452" s="3" t="s">
-        <v>1666</v>
+        <v>2311</v>
       </c>
       <c r="B452" s="3" t="b">
         <v>1</v>
@@ -16895,18 +16892,18 @@
       </c>
       <c r="D452" s="3"/>
       <c r="E452" s="3" t="s">
-        <v>1657</v>
+        <v>2312</v>
       </c>
       <c r="F452" s="6" t="s">
-        <v>1673</v>
+        <v>2313</v>
       </c>
       <c r="G452" s="3" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A453" s="3" t="s">
-        <v>1676</v>
+        <v>2314</v>
       </c>
       <c r="B453" s="3" t="b">
         <v>1</v>
@@ -16914,20 +16911,19 @@
       <c r="C453" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D453" s="3"/>
       <c r="E453" s="3" t="s">
-        <v>1677</v>
+        <v>2315</v>
       </c>
       <c r="F453" s="6" t="s">
-        <v>1678</v>
+        <v>2316</v>
       </c>
       <c r="G453" s="3" t="s">
-        <v>1767</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="454" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A454" s="3" t="s">
-        <v>1679</v>
+        <v>1673</v>
       </c>
       <c r="B454" s="3" t="b">
         <v>1</v>
@@ -16937,18 +16933,18 @@
       </c>
       <c r="D454" s="3"/>
       <c r="E454" s="3" t="s">
-        <v>1681</v>
+        <v>1674</v>
       </c>
       <c r="F454" s="6" t="s">
-        <v>1680</v>
+        <v>1675</v>
       </c>
       <c r="G454" s="3" t="s">
-        <v>1768</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="455" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A455" s="3" t="s">
-        <v>1682</v>
+        <v>1676</v>
       </c>
       <c r="B455" s="3" t="b">
         <v>1</v>
@@ -16958,18 +16954,18 @@
       </c>
       <c r="D455" s="3"/>
       <c r="E455" s="3" t="s">
-        <v>1685</v>
+        <v>1678</v>
       </c>
       <c r="F455" s="6" t="s">
-        <v>832</v>
+        <v>1677</v>
       </c>
       <c r="G455" s="3" t="s">
-        <v>1769</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="456" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A456" s="3" t="s">
-        <v>1683</v>
+        <v>1679</v>
       </c>
       <c r="B456" s="3" t="b">
         <v>1</v>
@@ -16979,18 +16975,18 @@
       </c>
       <c r="D456" s="3"/>
       <c r="E456" s="3" t="s">
-        <v>1686</v>
+        <v>1682</v>
       </c>
       <c r="F456" s="6" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="G456" s="3" t="s">
-        <v>1770</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" s="3" t="s">
-        <v>1684</v>
+        <v>1680</v>
       </c>
       <c r="B457" s="3" t="b">
         <v>1</v>
@@ -17000,18 +16996,18 @@
       </c>
       <c r="D457" s="3"/>
       <c r="E457" s="3" t="s">
-        <v>1687</v>
+        <v>1683</v>
       </c>
       <c r="F457" s="6" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G457" s="3" t="s">
-        <v>1771</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">
-        <v>1689</v>
+        <v>1681</v>
       </c>
       <c r="B458" s="3" t="b">
         <v>1</v>
@@ -17021,18 +17017,18 @@
       </c>
       <c r="D458" s="3"/>
       <c r="E458" s="3" t="s">
-        <v>1691</v>
+        <v>1684</v>
       </c>
       <c r="F458" s="6" t="s">
-        <v>1693</v>
+        <v>834</v>
       </c>
       <c r="G458" s="3" t="s">
-        <v>1772</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="459" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A459" s="3" t="s">
-        <v>1690</v>
+        <v>1686</v>
       </c>
       <c r="B459" s="3" t="b">
         <v>1</v>
@@ -17042,18 +17038,18 @@
       </c>
       <c r="D459" s="3"/>
       <c r="E459" s="3" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
       <c r="F459" s="6" t="s">
-        <v>1694</v>
+        <v>1690</v>
       </c>
       <c r="G459" s="3" t="s">
-        <v>1773</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460" s="3" t="s">
-        <v>1695</v>
+        <v>1687</v>
       </c>
       <c r="B460" s="3" t="b">
         <v>1</v>
@@ -17063,18 +17059,18 @@
       </c>
       <c r="D460" s="3"/>
       <c r="E460" s="3" t="s">
-        <v>1696</v>
+        <v>1689</v>
       </c>
       <c r="F460" s="6" t="s">
-        <v>1697</v>
+        <v>1691</v>
       </c>
       <c r="G460" s="3" t="s">
-        <v>1774</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="461" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A461" s="3" t="s">
-        <v>1699</v>
+        <v>1692</v>
       </c>
       <c r="B461" s="3" t="b">
         <v>1</v>
@@ -17084,18 +17080,18 @@
       </c>
       <c r="D461" s="3"/>
       <c r="E461" s="3" t="s">
-        <v>1701</v>
+        <v>1693</v>
       </c>
       <c r="F461" s="6" t="s">
-        <v>1704</v>
+        <v>1694</v>
       </c>
       <c r="G461" s="3" t="s">
-        <v>1775</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="462" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A462" s="3" t="s">
-        <v>1698</v>
+        <v>2291</v>
       </c>
       <c r="B462" s="3" t="b">
         <v>1</v>
@@ -17105,18 +17101,18 @@
       </c>
       <c r="D462" s="3"/>
       <c r="E462" s="3" t="s">
-        <v>1702</v>
+        <v>1695</v>
       </c>
       <c r="F462" s="6" t="s">
-        <v>1705</v>
+        <v>1697</v>
       </c>
       <c r="G462" s="3" t="s">
-        <v>1776</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A463" s="3" t="s">
-        <v>1700</v>
+        <v>2292</v>
       </c>
       <c r="B463" s="3" t="b">
         <v>1</v>
@@ -17126,18 +17122,18 @@
       </c>
       <c r="D463" s="3"/>
       <c r="E463" s="3" t="s">
-        <v>1703</v>
+        <v>1696</v>
       </c>
       <c r="F463" s="6" t="s">
-        <v>1706</v>
+        <v>1698</v>
       </c>
       <c r="G463" s="3" t="s">
-        <v>1777</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A464" s="3" t="s">
-        <v>1707</v>
+        <v>2293</v>
       </c>
       <c r="B464" s="3" t="b">
         <v>1</v>
@@ -17147,18 +17143,18 @@
       </c>
       <c r="D464" s="3"/>
       <c r="E464" s="3" t="s">
-        <v>1711</v>
+        <v>1699</v>
       </c>
       <c r="F464" s="6" t="s">
-        <v>1715</v>
+        <v>1703</v>
       </c>
       <c r="G464" s="3" t="s">
-        <v>1778</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="465" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A465" s="3" t="s">
-        <v>1708</v>
+        <v>2294</v>
       </c>
       <c r="B465" s="3" t="b">
         <v>1</v>
@@ -17168,18 +17164,18 @@
       </c>
       <c r="D465" s="3"/>
       <c r="E465" s="3" t="s">
-        <v>1712</v>
+        <v>1700</v>
       </c>
       <c r="F465" s="6" t="s">
-        <v>1716</v>
+        <v>1704</v>
       </c>
       <c r="G465" s="3" t="s">
-        <v>1779</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="466" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A466" s="3" t="s">
-        <v>1709</v>
+        <v>2295</v>
       </c>
       <c r="B466" s="3" t="b">
         <v>1</v>
@@ -17189,18 +17185,18 @@
       </c>
       <c r="D466" s="3"/>
       <c r="E466" s="3" t="s">
-        <v>1713</v>
+        <v>1701</v>
       </c>
       <c r="F466" s="6" t="s">
-        <v>1717</v>
+        <v>1705</v>
       </c>
       <c r="G466" s="3" t="s">
-        <v>1780</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="467" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A467" s="3" t="s">
-        <v>1710</v>
+        <v>2296</v>
       </c>
       <c r="B467" s="3" t="b">
         <v>1</v>
@@ -17210,18 +17206,18 @@
       </c>
       <c r="D467" s="3"/>
       <c r="E467" s="3" t="s">
-        <v>1714</v>
+        <v>1702</v>
       </c>
       <c r="F467" s="6" t="s">
-        <v>1718</v>
+        <v>1706</v>
       </c>
       <c r="G467" s="3" t="s">
-        <v>1781</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="468" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A468" s="3" t="s">
-        <v>1719</v>
+        <v>2297</v>
       </c>
       <c r="B468" s="3" t="b">
         <v>1</v>
@@ -17234,15 +17230,15 @@
         <v>1630</v>
       </c>
       <c r="F468" s="6" t="s">
-        <v>1740</v>
+        <v>1714</v>
       </c>
       <c r="G468" s="3" t="s">
-        <v>1782</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A469" s="3" t="s">
-        <v>1720</v>
+        <v>2298</v>
       </c>
       <c r="B469" s="3" t="b">
         <v>1</v>
@@ -17252,18 +17248,18 @@
       </c>
       <c r="D469" s="3"/>
       <c r="E469" s="3" t="s">
-        <v>1736</v>
+        <v>1710</v>
       </c>
       <c r="F469" s="6" t="s">
-        <v>1741</v>
+        <v>1715</v>
       </c>
       <c r="G469" s="3" t="s">
-        <v>1783</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="470" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A470" s="3" t="s">
-        <v>1721</v>
+        <v>2299</v>
       </c>
       <c r="B470" s="3" t="b">
         <v>1</v>
@@ -17284,7 +17280,7 @@
     </row>
     <row r="471" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A471" s="3" t="s">
-        <v>1722</v>
+        <v>2300</v>
       </c>
       <c r="B471" s="3" t="b">
         <v>1</v>
@@ -17294,18 +17290,18 @@
       </c>
       <c r="D471" s="3"/>
       <c r="E471" s="3" t="s">
-        <v>1737</v>
+        <v>1711</v>
       </c>
       <c r="F471" s="6" t="s">
-        <v>1742</v>
+        <v>1716</v>
       </c>
       <c r="G471" s="3" t="s">
-        <v>1784</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="472" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A472" s="3" t="s">
-        <v>1723</v>
+        <v>2301</v>
       </c>
       <c r="B472" s="3" t="b">
         <v>1</v>
@@ -17315,18 +17311,18 @@
       </c>
       <c r="D472" s="3"/>
       <c r="E472" s="3" t="s">
-        <v>1733</v>
+        <v>1707</v>
       </c>
       <c r="F472" s="6" t="s">
-        <v>1743</v>
+        <v>1717</v>
       </c>
       <c r="G472" s="3" t="s">
-        <v>1785</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="473" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A473" s="3" t="s">
-        <v>1724</v>
+        <v>2302</v>
       </c>
       <c r="B473" s="3" t="b">
         <v>1</v>
@@ -17336,18 +17332,18 @@
       </c>
       <c r="D473" s="3"/>
       <c r="E473" s="3" t="s">
-        <v>1738</v>
+        <v>1712</v>
       </c>
       <c r="F473" s="6" t="s">
-        <v>1744</v>
+        <v>1718</v>
       </c>
       <c r="G473" s="3" t="s">
-        <v>1786</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="474" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A474" s="3" t="s">
-        <v>1725</v>
+        <v>2303</v>
       </c>
       <c r="B474" s="3" t="b">
         <v>1</v>
@@ -17357,18 +17353,18 @@
       </c>
       <c r="D474" s="3"/>
       <c r="E474" s="3" t="s">
-        <v>1739</v>
+        <v>1713</v>
       </c>
       <c r="F474" s="6" t="s">
-        <v>1745</v>
+        <v>1719</v>
       </c>
       <c r="G474" s="3" t="s">
-        <v>1787</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="475" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A475" s="3" t="s">
-        <v>1726</v>
+        <v>2304</v>
       </c>
       <c r="B475" s="3" t="b">
         <v>1</v>
@@ -17381,7 +17377,7 @@
         <v>428</v>
       </c>
       <c r="F475" s="6" t="s">
-        <v>1746</v>
+        <v>1720</v>
       </c>
       <c r="G475" s="3" t="s">
         <v>1359</v>
@@ -17389,7 +17385,7 @@
     </row>
     <row r="476" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A476" s="3" t="s">
-        <v>1727</v>
+        <v>2305</v>
       </c>
       <c r="B476" s="3" t="b">
         <v>1</v>
@@ -17402,7 +17398,7 @@
         <v>443</v>
       </c>
       <c r="F476" s="6" t="s">
-        <v>1747</v>
+        <v>1721</v>
       </c>
       <c r="G476" s="3" t="s">
         <v>1364</v>
@@ -17410,7 +17406,7 @@
     </row>
     <row r="477" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A477" s="3" t="s">
-        <v>1728</v>
+        <v>2306</v>
       </c>
       <c r="B477" s="3" t="b">
         <v>1</v>
@@ -17420,18 +17416,18 @@
       </c>
       <c r="D477" s="3"/>
       <c r="E477" s="3" t="s">
-        <v>1734</v>
+        <v>1708</v>
       </c>
       <c r="F477" s="6" t="s">
-        <v>1748</v>
+        <v>1722</v>
       </c>
       <c r="G477" s="3" t="s">
-        <v>1788</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="478" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A478" s="3" t="s">
-        <v>1729</v>
+        <v>2307</v>
       </c>
       <c r="B478" s="3" t="b">
         <v>1</v>
@@ -17441,18 +17437,18 @@
       </c>
       <c r="D478" s="3"/>
       <c r="E478" s="3" t="s">
-        <v>1735</v>
+        <v>1709</v>
       </c>
       <c r="F478" s="6" t="s">
-        <v>1749</v>
+        <v>1723</v>
       </c>
       <c r="G478" s="3" t="s">
-        <v>1789</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="479" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
-        <v>1730</v>
+        <v>2308</v>
       </c>
       <c r="B479" s="3" t="b">
         <v>1</v>
@@ -17465,7 +17461,7 @@
         <v>434</v>
       </c>
       <c r="F479" s="6" t="s">
-        <v>1750</v>
+        <v>1724</v>
       </c>
       <c r="G479" s="3" t="s">
         <v>1361</v>
@@ -17473,7 +17469,7 @@
     </row>
     <row r="480" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A480" s="3" t="s">
-        <v>1731</v>
+        <v>2309</v>
       </c>
       <c r="B480" s="3" t="b">
         <v>1</v>
@@ -17486,7 +17482,7 @@
         <v>422</v>
       </c>
       <c r="F480" s="6" t="s">
-        <v>1751</v>
+        <v>1725</v>
       </c>
       <c r="G480" s="3" t="s">
         <v>1357</v>
@@ -17494,7 +17490,7 @@
     </row>
     <row r="481" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
-        <v>1732</v>
+        <v>2310</v>
       </c>
       <c r="B481" s="3" t="b">
         <v>1</v>
@@ -17528,7 +17524,7 @@
         <v>817</v>
       </c>
       <c r="F482" s="6" t="s">
-        <v>1754</v>
+        <v>1728</v>
       </c>
       <c r="G482" s="3" t="s">
         <v>1490</v>
@@ -17536,7 +17532,7 @@
     </row>
     <row r="483" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A483" s="3" t="s">
-        <v>1752</v>
+        <v>1726</v>
       </c>
       <c r="B483" s="3" t="b">
         <v>1</v>
@@ -17546,10 +17542,10 @@
       </c>
       <c r="D483" s="3"/>
       <c r="E483" s="3" t="s">
-        <v>1752</v>
+        <v>1726</v>
       </c>
       <c r="F483" s="6" t="s">
-        <v>1753</v>
+        <v>1727</v>
       </c>
       <c r="G483" s="3" t="s">
         <v>1490</v>
@@ -17557,7 +17553,7 @@
     </row>
     <row r="484" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A484" s="3" t="s">
-        <v>2062</v>
+        <v>2035</v>
       </c>
       <c r="B484" s="3" t="b">
         <v>1</v>
@@ -17566,18 +17562,18 @@
         <v>1</v>
       </c>
       <c r="E484" s="3" t="s">
-        <v>2064</v>
+        <v>2037</v>
       </c>
       <c r="F484" s="6" t="s">
-        <v>2066</v>
+        <v>2039</v>
       </c>
       <c r="G484" s="3" t="s">
-        <v>2068</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="485" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A485" s="3" t="s">
-        <v>2063</v>
+        <v>2036</v>
       </c>
       <c r="B485" s="3" t="b">
         <v>1</v>
@@ -17586,18 +17582,18 @@
         <v>1</v>
       </c>
       <c r="E485" s="3" t="s">
-        <v>2065</v>
+        <v>2038</v>
       </c>
       <c r="F485" s="6" t="s">
-        <v>2067</v>
+        <v>2040</v>
       </c>
       <c r="G485" s="3" t="s">
-        <v>2068</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="486" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A486" s="3" t="s">
-        <v>2190</v>
+        <v>2163</v>
       </c>
       <c r="B486" s="3" t="b">
         <v>1</v>
@@ -17618,7 +17614,7 @@
     </row>
     <row r="487" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A487" s="3" t="s">
-        <v>1794</v>
+        <v>1767</v>
       </c>
       <c r="B487" s="3" t="b">
         <v>1</v>
@@ -17628,18 +17624,18 @@
       </c>
       <c r="D487" s="3"/>
       <c r="E487" s="3" t="s">
-        <v>1799</v>
+        <v>1772</v>
       </c>
       <c r="F487" s="6" t="s">
-        <v>1800</v>
+        <v>1773</v>
       </c>
       <c r="G487" s="3" t="s">
-        <v>1803</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A488" s="3" t="s">
-        <v>1795</v>
+        <v>1768</v>
       </c>
       <c r="B488" s="3" t="b">
         <v>1</v>
@@ -17649,18 +17645,18 @@
       </c>
       <c r="D488" s="3"/>
       <c r="E488" s="3" t="s">
-        <v>1798</v>
+        <v>1771</v>
       </c>
       <c r="F488" s="6" t="s">
-        <v>1801</v>
+        <v>1774</v>
       </c>
       <c r="G488" s="3" t="s">
-        <v>1803</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="489" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A489" s="3" t="s">
-        <v>1796</v>
+        <v>1769</v>
       </c>
       <c r="B489" s="3" t="b">
         <v>1</v>
@@ -17670,18 +17666,18 @@
       </c>
       <c r="D489" s="3"/>
       <c r="E489" s="3" t="s">
-        <v>1797</v>
+        <v>1770</v>
       </c>
       <c r="F489" s="6" t="s">
-        <v>1802</v>
+        <v>1775</v>
       </c>
       <c r="G489" s="3" t="s">
-        <v>1804</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="490" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
-        <v>1805</v>
+        <v>1778</v>
       </c>
       <c r="B490" s="3" t="b">
         <v>1</v>
@@ -17691,18 +17687,18 @@
       </c>
       <c r="D490" s="3"/>
       <c r="E490" s="3" t="s">
-        <v>1806</v>
+        <v>1779</v>
       </c>
       <c r="F490" s="6" t="s">
-        <v>1807</v>
+        <v>1780</v>
       </c>
       <c r="G490" s="3" t="s">
-        <v>1808</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="491" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A491" s="3" t="s">
-        <v>1809</v>
+        <v>1782</v>
       </c>
       <c r="B491" s="3" t="b">
         <v>1</v>
@@ -17712,18 +17708,18 @@
       </c>
       <c r="D491" s="3"/>
       <c r="E491" s="3" t="s">
-        <v>1810</v>
+        <v>1783</v>
       </c>
       <c r="F491" s="6" t="s">
-        <v>1811</v>
+        <v>1784</v>
       </c>
       <c r="G491" s="3" t="s">
-        <v>1812</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="492" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A492" s="3" t="s">
-        <v>1813</v>
+        <v>1786</v>
       </c>
       <c r="B492" s="3" t="b">
         <v>0</v>
@@ -17733,18 +17729,18 @@
       </c>
       <c r="D492" s="3"/>
       <c r="E492" s="3" t="s">
-        <v>1813</v>
+        <v>1786</v>
       </c>
       <c r="F492" s="6" t="s">
-        <v>1814</v>
+        <v>1787</v>
       </c>
       <c r="G492" s="3" t="s">
-        <v>1815</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="493" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A493" s="3" t="s">
-        <v>1816</v>
+        <v>1789</v>
       </c>
       <c r="B493" s="3" t="b">
         <v>0</v>
@@ -17754,18 +17750,18 @@
       </c>
       <c r="D493" s="3"/>
       <c r="E493" s="3" t="s">
-        <v>1817</v>
+        <v>1790</v>
       </c>
       <c r="F493" s="6" t="s">
-        <v>1818</v>
+        <v>1791</v>
       </c>
       <c r="G493" s="3" t="s">
-        <v>1819</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A494" s="3" t="s">
-        <v>1820</v>
+        <v>1793</v>
       </c>
       <c r="B494" s="3" t="b">
         <v>1</v>
@@ -17775,18 +17771,18 @@
       </c>
       <c r="D494" s="3"/>
       <c r="E494" s="3" t="s">
-        <v>1821</v>
+        <v>1794</v>
       </c>
       <c r="F494" s="6" t="s">
-        <v>1822</v>
+        <v>1795</v>
       </c>
       <c r="G494" s="3" t="s">
-        <v>1823</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A495" s="3" t="s">
-        <v>1824</v>
+        <v>1797</v>
       </c>
       <c r="B495" s="3" t="b">
         <v>1</v>
@@ -17796,18 +17792,18 @@
       </c>
       <c r="D495" s="3"/>
       <c r="E495" s="3" t="s">
-        <v>1825</v>
+        <v>1798</v>
       </c>
       <c r="F495" s="6" t="s">
-        <v>1826</v>
+        <v>1799</v>
       </c>
       <c r="G495" s="3" t="s">
-        <v>1827</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="496" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
-        <v>2240</v>
+        <v>2213</v>
       </c>
       <c r="B496" s="3" t="b">
         <v>1</v>
@@ -17817,18 +17813,18 @@
       </c>
       <c r="D496" s="3"/>
       <c r="E496" s="3" t="s">
-        <v>1828</v>
+        <v>1801</v>
       </c>
       <c r="F496" s="6" t="s">
-        <v>1829</v>
+        <v>1802</v>
       </c>
       <c r="G496" s="3" t="s">
-        <v>1830</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="497" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A497" s="4" t="s">
-        <v>1835</v>
+        <v>1808</v>
       </c>
       <c r="B497" s="3" t="b">
         <v>0</v>
@@ -17838,18 +17834,18 @@
       </c>
       <c r="D497" s="3"/>
       <c r="E497" s="3" t="s">
-        <v>1836</v>
+        <v>1809</v>
       </c>
       <c r="F497" s="6" t="s">
-        <v>1837</v>
+        <v>1810</v>
       </c>
       <c r="G497" s="3" t="s">
-        <v>1838</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="498" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
-        <v>1831</v>
+        <v>1804</v>
       </c>
       <c r="B498" s="3" t="b">
         <v>0</v>
@@ -17859,18 +17855,18 @@
       </c>
       <c r="D498" s="3"/>
       <c r="E498" s="3" t="s">
-        <v>1832</v>
+        <v>1805</v>
       </c>
       <c r="F498" s="6" t="s">
-        <v>1833</v>
+        <v>1806</v>
       </c>
       <c r="G498" s="3" t="s">
-        <v>1834</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="499" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
-        <v>1839</v>
+        <v>1812</v>
       </c>
       <c r="B499" s="3" t="b">
         <v>1</v>
@@ -17879,18 +17875,18 @@
         <v>0</v>
       </c>
       <c r="E499" s="3" t="s">
-        <v>1840</v>
+        <v>1813</v>
       </c>
       <c r="F499" s="6" t="s">
-        <v>1841</v>
+        <v>1814</v>
       </c>
       <c r="G499" s="3" t="s">
-        <v>1845</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="500" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
-        <v>1842</v>
+        <v>1815</v>
       </c>
       <c r="B500" s="3" t="b">
         <v>1</v>
@@ -17900,13 +17896,13 @@
       </c>
       <c r="D500" s="3"/>
       <c r="E500" s="3" t="s">
-        <v>1843</v>
+        <v>1816</v>
       </c>
       <c r="F500" s="6" t="s">
-        <v>1844</v>
+        <v>1817</v>
       </c>
       <c r="G500" s="3" t="s">
-        <v>1846</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="501" spans="1:7" x14ac:dyDescent="0.25">
@@ -17924,15 +17920,15 @@
         <v>1630</v>
       </c>
       <c r="F501" s="6" t="s">
-        <v>1848</v>
+        <v>1821</v>
       </c>
       <c r="G501" s="3" t="s">
-        <v>1782</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="502" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A502" s="3" t="s">
-        <v>1847</v>
+        <v>1820</v>
       </c>
       <c r="B502" s="3" t="b">
         <v>1</v>
@@ -17942,18 +17938,18 @@
       </c>
       <c r="D502" s="3"/>
       <c r="E502" s="3" t="s">
-        <v>1847</v>
+        <v>1820</v>
       </c>
       <c r="F502" s="6" t="s">
-        <v>1849</v>
+        <v>1822</v>
       </c>
       <c r="G502" s="3" t="s">
-        <v>1850</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="503" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A503" s="3" t="s">
-        <v>1852</v>
+        <v>1825</v>
       </c>
       <c r="B503" s="3" t="b">
         <v>1</v>
@@ -17963,18 +17959,18 @@
       </c>
       <c r="D503" s="3"/>
       <c r="E503" s="3" t="s">
-        <v>1854</v>
+        <v>1827</v>
       </c>
       <c r="F503" s="6" t="s">
-        <v>1855</v>
+        <v>1828</v>
       </c>
       <c r="G503" s="3" t="s">
-        <v>1856</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A504" s="3" t="s">
-        <v>1853</v>
+        <v>1826</v>
       </c>
       <c r="B504" s="3" t="b">
         <v>1</v>
@@ -17995,7 +17991,7 @@
     </row>
     <row r="505" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A505" s="3" t="s">
-        <v>2297</v>
+        <v>2270</v>
       </c>
       <c r="B505" s="3" t="b">
         <v>1</v>
@@ -18004,18 +18000,18 @@
         <v>1</v>
       </c>
       <c r="E505" s="3" t="s">
-        <v>2298</v>
+        <v>2271</v>
       </c>
       <c r="F505" s="6" t="s">
-        <v>2299</v>
+        <v>2272</v>
       </c>
       <c r="G505" s="3" t="s">
-        <v>2300</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A506" s="3" t="s">
-        <v>1851</v>
+        <v>1824</v>
       </c>
       <c r="B506" s="3" t="b">
         <v>1</v>
@@ -18025,18 +18021,18 @@
       </c>
       <c r="D506" s="3"/>
       <c r="E506" s="3" t="s">
-        <v>1797</v>
+        <v>1770</v>
       </c>
       <c r="F506" s="6" t="s">
-        <v>1802</v>
+        <v>1775</v>
       </c>
       <c r="G506" s="3" t="s">
-        <v>1804</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="507" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A507" s="3" t="s">
-        <v>1857</v>
+        <v>1830</v>
       </c>
       <c r="B507" s="3" t="b">
         <v>1</v>
@@ -18046,18 +18042,18 @@
       </c>
       <c r="D507" s="3"/>
       <c r="E507" s="3" t="s">
-        <v>1860</v>
+        <v>1833</v>
       </c>
       <c r="F507" s="6" t="s">
-        <v>1858</v>
+        <v>1831</v>
       </c>
       <c r="G507" s="3" t="s">
-        <v>1874</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="508" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A508" s="3" t="s">
-        <v>1862</v>
+        <v>1835</v>
       </c>
       <c r="B508" s="3" t="b">
         <v>1</v>
@@ -18067,18 +18063,18 @@
       </c>
       <c r="D508" s="3"/>
       <c r="E508" s="3" t="s">
-        <v>1861</v>
+        <v>1834</v>
       </c>
       <c r="F508" s="6" t="s">
-        <v>1859</v>
+        <v>1832</v>
       </c>
       <c r="G508" s="3" t="s">
-        <v>1875</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="509" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A509" s="3" t="s">
-        <v>1863</v>
+        <v>1836</v>
       </c>
       <c r="B509" s="3" t="b">
         <v>1</v>
@@ -18088,18 +18084,18 @@
       </c>
       <c r="D509" s="3"/>
       <c r="E509" s="3" t="s">
-        <v>1866</v>
+        <v>1839</v>
       </c>
       <c r="F509" s="6" t="s">
-        <v>1869</v>
+        <v>1842</v>
       </c>
       <c r="G509" s="3" t="s">
-        <v>1876</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="510" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A510" s="3" t="s">
-        <v>1864</v>
+        <v>1837</v>
       </c>
       <c r="B510" s="3" t="b">
         <v>1</v>
@@ -18109,18 +18105,18 @@
       </c>
       <c r="D510" s="3"/>
       <c r="E510" s="3" t="s">
-        <v>1870</v>
+        <v>1843</v>
       </c>
       <c r="F510" s="6" t="s">
-        <v>1868</v>
+        <v>1841</v>
       </c>
       <c r="G510" s="3" t="s">
-        <v>1877</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="511" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A511" s="3" t="s">
-        <v>1865</v>
+        <v>1838</v>
       </c>
       <c r="B511" s="3" t="b">
         <v>1</v>
@@ -18130,18 +18126,18 @@
       </c>
       <c r="D511" s="3"/>
       <c r="E511" s="3" t="s">
-        <v>1871</v>
+        <v>1844</v>
       </c>
       <c r="F511" s="6" t="s">
-        <v>1867</v>
+        <v>1840</v>
       </c>
       <c r="G511" s="3" t="s">
-        <v>1878</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A512" s="3" t="s">
-        <v>1889</v>
+        <v>1862</v>
       </c>
       <c r="B512" s="3" t="b">
         <v>1</v>
@@ -18151,18 +18147,18 @@
       </c>
       <c r="D512" s="3"/>
       <c r="E512" s="3" t="s">
-        <v>1872</v>
+        <v>1845</v>
       </c>
       <c r="F512" s="6" t="s">
-        <v>1873</v>
+        <v>1846</v>
       </c>
       <c r="G512" s="3" t="s">
-        <v>1879</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="513" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A513" s="3" t="s">
-        <v>1880</v>
+        <v>1853</v>
       </c>
       <c r="B513" s="3" t="b">
         <v>1</v>
@@ -18183,7 +18179,7 @@
     </row>
     <row r="514" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A514" s="3" t="s">
-        <v>1881</v>
+        <v>1854</v>
       </c>
       <c r="B514" s="3" t="b">
         <v>1</v>
@@ -18199,12 +18195,12 @@
         <v>1146</v>
       </c>
       <c r="G514" s="3" t="s">
-        <v>1758</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="515" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A515" s="3" t="s">
-        <v>1882</v>
+        <v>1855</v>
       </c>
       <c r="B515" s="3" t="b">
         <v>1</v>
@@ -18214,18 +18210,18 @@
       </c>
       <c r="D515" s="3"/>
       <c r="E515" s="3" t="s">
-        <v>1884</v>
+        <v>1857</v>
       </c>
       <c r="F515" s="6" t="s">
-        <v>1886</v>
+        <v>1859</v>
       </c>
       <c r="G515" s="3" t="s">
-        <v>1887</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="516" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A516" s="3" t="s">
-        <v>1883</v>
+        <v>1856</v>
       </c>
       <c r="B516" s="3" t="b">
         <v>1</v>
@@ -18235,18 +18231,18 @@
       </c>
       <c r="D516" s="3"/>
       <c r="E516" s="3" t="s">
-        <v>1885</v>
+        <v>1858</v>
       </c>
       <c r="F516" s="6" t="s">
-        <v>1802</v>
+        <v>1775</v>
       </c>
       <c r="G516" s="3" t="s">
-        <v>1888</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="517" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A517" s="3" t="s">
-        <v>1892</v>
+        <v>1865</v>
       </c>
       <c r="B517" s="3" t="b">
         <v>0</v>
@@ -18255,18 +18251,18 @@
         <v>1</v>
       </c>
       <c r="E517" s="3" t="s">
-        <v>1890</v>
+        <v>1863</v>
       </c>
       <c r="F517" s="6" t="s">
-        <v>1893</v>
+        <v>1866</v>
       </c>
       <c r="G517" s="3" t="s">
-        <v>1891</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="518" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>1894</v>
+        <v>1867</v>
       </c>
       <c r="B518" t="b">
         <v>1</v>
@@ -18275,18 +18271,18 @@
         <v>1</v>
       </c>
       <c r="E518" s="3" t="s">
-        <v>1894</v>
+        <v>1867</v>
       </c>
       <c r="F518" s="6" t="s">
-        <v>1897</v>
+        <v>1870</v>
       </c>
       <c r="G518" t="s">
-        <v>1899</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="519" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>1895</v>
+        <v>1868</v>
       </c>
       <c r="B519" t="b">
         <v>1</v>
@@ -18295,18 +18291,18 @@
         <v>1</v>
       </c>
       <c r="E519" s="3" t="s">
-        <v>1896</v>
+        <v>1869</v>
       </c>
       <c r="F519" s="6" t="s">
-        <v>1898</v>
+        <v>1871</v>
       </c>
       <c r="G519" t="s">
-        <v>1900</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="520" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>1901</v>
+        <v>1874</v>
       </c>
       <c r="B520" t="b">
         <v>1</v>
@@ -18315,21 +18311,21 @@
         <v>0</v>
       </c>
       <c r="D520" t="s">
-        <v>1904</v>
+        <v>1877</v>
       </c>
       <c r="E520" s="3" t="s">
-        <v>1902</v>
+        <v>1875</v>
       </c>
       <c r="F520" s="6" t="s">
-        <v>1903</v>
+        <v>1876</v>
       </c>
       <c r="G520" s="3" t="s">
-        <v>1903</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="521" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A521" s="3" t="s">
-        <v>1901</v>
+        <v>1874</v>
       </c>
       <c r="B521" t="b">
         <v>0</v>
@@ -18338,21 +18334,21 @@
         <v>1</v>
       </c>
       <c r="D521" s="3" t="s">
-        <v>1904</v>
+        <v>1877</v>
       </c>
       <c r="E521" s="3" t="s">
-        <v>1905</v>
+        <v>1878</v>
       </c>
       <c r="F521" s="6" t="s">
-        <v>1906</v>
+        <v>1879</v>
       </c>
       <c r="G521" s="3" t="s">
-        <v>1906</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="522" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>1919</v>
+        <v>1892</v>
       </c>
       <c r="B522" t="b">
         <v>0</v>
@@ -18361,18 +18357,18 @@
         <v>1</v>
       </c>
       <c r="E522" t="s">
-        <v>1922</v>
+        <v>1895</v>
       </c>
       <c r="F522" s="6" t="s">
-        <v>1920</v>
+        <v>1893</v>
       </c>
       <c r="G522" s="3" t="s">
-        <v>1921</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="523" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>1931</v>
+        <v>1904</v>
       </c>
       <c r="B523" t="b">
         <v>0</v>
@@ -18381,18 +18377,18 @@
         <v>1</v>
       </c>
       <c r="E523" t="s">
-        <v>1931</v>
+        <v>1904</v>
       </c>
       <c r="F523" s="6" t="s">
-        <v>1932</v>
+        <v>1905</v>
       </c>
       <c r="G523" s="3" t="s">
-        <v>1933</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="524" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>1923</v>
+        <v>1896</v>
       </c>
       <c r="B524" s="3" t="b">
         <v>0</v>
@@ -18401,18 +18397,18 @@
         <v>1</v>
       </c>
       <c r="E524" t="s">
-        <v>1924</v>
+        <v>1897</v>
       </c>
       <c r="F524" s="6" t="s">
-        <v>1926</v>
+        <v>1899</v>
       </c>
       <c r="G524" t="s">
-        <v>1925</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="525" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1927</v>
+        <v>1900</v>
       </c>
       <c r="B525" t="b">
         <v>0</v>
@@ -18421,18 +18417,18 @@
         <v>1</v>
       </c>
       <c r="E525" t="s">
-        <v>1928</v>
+        <v>1901</v>
       </c>
       <c r="F525" s="6" t="s">
-        <v>1929</v>
+        <v>1902</v>
       </c>
       <c r="G525" t="s">
-        <v>1930</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="526" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>1934</v>
+        <v>1907</v>
       </c>
       <c r="B526" s="3" t="b">
         <v>1</v>
@@ -18441,18 +18437,18 @@
         <v>1</v>
       </c>
       <c r="E526" t="s">
-        <v>1936</v>
+        <v>1909</v>
       </c>
       <c r="F526" s="6" t="s">
-        <v>1938</v>
+        <v>1911</v>
       </c>
       <c r="G526" t="s">
-        <v>2027</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="527" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>1935</v>
+        <v>1908</v>
       </c>
       <c r="B527" s="3" t="b">
         <v>1</v>
@@ -18461,13 +18457,13 @@
         <v>1</v>
       </c>
       <c r="E527" t="s">
-        <v>1937</v>
+        <v>1910</v>
       </c>
       <c r="F527" s="6" t="s">
-        <v>1939</v>
+        <v>1912</v>
       </c>
       <c r="G527" t="s">
-        <v>2027</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="528" spans="1:7" x14ac:dyDescent="0.25">
@@ -18492,7 +18488,7 @@
     </row>
     <row r="529" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1946</v>
+        <v>1919</v>
       </c>
       <c r="B529" s="3" t="b">
         <v>1</v>
@@ -18501,18 +18497,18 @@
         <v>1</v>
       </c>
       <c r="E529" t="s">
-        <v>1854</v>
+        <v>1827</v>
       </c>
       <c r="F529" s="6" t="s">
-        <v>1855</v>
+        <v>1828</v>
       </c>
       <c r="G529" t="s">
-        <v>1856</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="530" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1947</v>
+        <v>1920</v>
       </c>
       <c r="B530" s="3" t="b">
         <v>1</v>
@@ -18521,18 +18517,18 @@
         <v>1</v>
       </c>
       <c r="E530" t="s">
-        <v>1949</v>
+        <v>1922</v>
       </c>
       <c r="F530" s="6" t="s">
-        <v>1954</v>
+        <v>1927</v>
       </c>
       <c r="G530" t="s">
-        <v>2028</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="531" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1948</v>
+        <v>1921</v>
       </c>
       <c r="B531" s="3" t="b">
         <v>1</v>
@@ -18541,18 +18537,18 @@
         <v>1</v>
       </c>
       <c r="E531" t="s">
-        <v>1950</v>
+        <v>1923</v>
       </c>
       <c r="F531" s="6" t="s">
-        <v>1955</v>
+        <v>1928</v>
       </c>
       <c r="G531" t="s">
-        <v>2029</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="532" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1940</v>
+        <v>1913</v>
       </c>
       <c r="B532" s="3" t="b">
         <v>1</v>
@@ -18561,18 +18557,18 @@
         <v>1</v>
       </c>
       <c r="E532" t="s">
-        <v>1931</v>
+        <v>1904</v>
       </c>
       <c r="F532" s="6" t="s">
-        <v>1956</v>
+        <v>1929</v>
       </c>
       <c r="G532" t="s">
-        <v>1933</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="533" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1941</v>
+        <v>1914</v>
       </c>
       <c r="B533" s="3" t="b">
         <v>1</v>
@@ -18581,18 +18577,18 @@
         <v>1</v>
       </c>
       <c r="E533" t="s">
-        <v>1951</v>
+        <v>1924</v>
       </c>
       <c r="F533" s="6" t="s">
-        <v>1957</v>
+        <v>1930</v>
       </c>
       <c r="G533" t="s">
-        <v>2030</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="534" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1942</v>
+        <v>1915</v>
       </c>
       <c r="B534" s="3" t="b">
         <v>1</v>
@@ -18601,78 +18597,78 @@
         <v>1</v>
       </c>
       <c r="E534" t="s">
-        <v>2144</v>
+        <v>2117</v>
       </c>
       <c r="F534" s="6" t="s">
-        <v>2150</v>
+        <v>2123</v>
       </c>
       <c r="G534" t="s">
-        <v>2031</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="535" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A535" s="3" t="s">
+        <v>2071</v>
+      </c>
+      <c r="B535" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C535" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E535" s="3" t="s">
+        <v>2118</v>
+      </c>
+      <c r="F535" s="6" t="s">
+        <v>2124</v>
+      </c>
+      <c r="G535" s="3" t="s">
         <v>2098</v>
-      </c>
-      <c r="B535" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C535" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E535" s="3" t="s">
-        <v>2145</v>
-      </c>
-      <c r="F535" s="6" t="s">
-        <v>2151</v>
-      </c>
-      <c r="G535" s="3" t="s">
-        <v>2125</v>
       </c>
     </row>
     <row r="536" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A536" s="3" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B536" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C536" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E536" s="3" t="s">
+        <v>2119</v>
+      </c>
+      <c r="F536" s="6" t="s">
+        <v>2125</v>
+      </c>
+      <c r="G536" s="3" t="s">
         <v>2099</v>
-      </c>
-      <c r="B536" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C536" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E536" s="3" t="s">
-        <v>2146</v>
-      </c>
-      <c r="F536" s="6" t="s">
-        <v>2152</v>
-      </c>
-      <c r="G536" s="3" t="s">
-        <v>2126</v>
       </c>
     </row>
     <row r="537" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A537" s="3" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B537" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C537" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E537" s="3" t="s">
+        <v>2120</v>
+      </c>
+      <c r="F537" s="6" t="s">
+        <v>2126</v>
+      </c>
+      <c r="G537" s="3" t="s">
         <v>2100</v>
-      </c>
-      <c r="B537" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C537" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E537" s="3" t="s">
-        <v>2147</v>
-      </c>
-      <c r="F537" s="6" t="s">
-        <v>2153</v>
-      </c>
-      <c r="G537" s="3" t="s">
-        <v>2127</v>
       </c>
     </row>
     <row r="538" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>1943</v>
+        <v>1916</v>
       </c>
       <c r="B538" s="3" t="b">
         <v>1</v>
@@ -18681,78 +18677,78 @@
         <v>1</v>
       </c>
       <c r="E538" t="s">
-        <v>2143</v>
+        <v>2116</v>
       </c>
       <c r="F538" s="6" t="s">
-        <v>2154</v>
+        <v>2127</v>
       </c>
       <c r="G538" t="s">
-        <v>2032</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="539" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A539" s="3" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B539" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C539" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E539" s="3" t="s">
+        <v>2115</v>
+      </c>
+      <c r="F539" s="6" t="s">
+        <v>2128</v>
+      </c>
+      <c r="G539" s="3" t="s">
         <v>2101</v>
-      </c>
-      <c r="B539" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C539" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E539" s="3" t="s">
-        <v>2142</v>
-      </c>
-      <c r="F539" s="6" t="s">
-        <v>2155</v>
-      </c>
-      <c r="G539" s="3" t="s">
-        <v>2128</v>
       </c>
     </row>
     <row r="540" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A540" s="3" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B540" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C540" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E540" s="3" t="s">
+        <v>2114</v>
+      </c>
+      <c r="F540" s="6" t="s">
+        <v>2129</v>
+      </c>
+      <c r="G540" s="3" t="s">
         <v>2102</v>
-      </c>
-      <c r="B540" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C540" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E540" s="3" t="s">
-        <v>2141</v>
-      </c>
-      <c r="F540" s="6" t="s">
-        <v>2156</v>
-      </c>
-      <c r="G540" s="3" t="s">
-        <v>2129</v>
       </c>
     </row>
     <row r="541" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A541" s="3" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B541" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C541" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E541" s="3" t="s">
+        <v>2113</v>
+      </c>
+      <c r="F541" s="6" t="s">
+        <v>2130</v>
+      </c>
+      <c r="G541" s="3" t="s">
         <v>2103</v>
-      </c>
-      <c r="B541" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C541" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E541" s="3" t="s">
-        <v>2140</v>
-      </c>
-      <c r="F541" s="6" t="s">
-        <v>2157</v>
-      </c>
-      <c r="G541" s="3" t="s">
-        <v>2130</v>
       </c>
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>1944</v>
+        <v>1917</v>
       </c>
       <c r="B542" s="3" t="b">
         <v>1</v>
@@ -18761,78 +18757,78 @@
         <v>1</v>
       </c>
       <c r="E542" t="s">
-        <v>1952</v>
+        <v>1925</v>
       </c>
       <c r="F542" s="6" t="s">
-        <v>1959</v>
+        <v>1932</v>
       </c>
       <c r="G542" t="s">
-        <v>2033</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="543" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A543" s="3" t="s">
+        <v>2077</v>
+      </c>
+      <c r="B543" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C543" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E543" s="3" t="s">
+        <v>2085</v>
+      </c>
+      <c r="F543" s="6" t="s">
+        <v>2091</v>
+      </c>
+      <c r="G543" s="3" t="s">
         <v>2104</v>
-      </c>
-      <c r="B543" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C543" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E543" s="3" t="s">
-        <v>2112</v>
-      </c>
-      <c r="F543" s="6" t="s">
-        <v>2118</v>
-      </c>
-      <c r="G543" s="3" t="s">
-        <v>2131</v>
       </c>
     </row>
     <row r="544" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A544" s="3" t="s">
+        <v>2078</v>
+      </c>
+      <c r="B544" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C544" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E544" s="3" t="s">
+        <v>2121</v>
+      </c>
+      <c r="F544" s="6" t="s">
+        <v>2093</v>
+      </c>
+      <c r="G544" s="3" t="s">
         <v>2105</v>
-      </c>
-      <c r="B544" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C544" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E544" s="3" t="s">
-        <v>2148</v>
-      </c>
-      <c r="F544" s="6" t="s">
-        <v>2120</v>
-      </c>
-      <c r="G544" s="3" t="s">
-        <v>2132</v>
       </c>
     </row>
     <row r="545" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A545" s="3" t="s">
+        <v>2079</v>
+      </c>
+      <c r="B545" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C545" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E545" s="3" t="s">
+        <v>2122</v>
+      </c>
+      <c r="F545" s="6" t="s">
+        <v>2092</v>
+      </c>
+      <c r="G545" s="3" t="s">
         <v>2106</v>
-      </c>
-      <c r="B545" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C545" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E545" s="3" t="s">
-        <v>2149</v>
-      </c>
-      <c r="F545" s="6" t="s">
-        <v>2119</v>
-      </c>
-      <c r="G545" s="3" t="s">
-        <v>2133</v>
       </c>
     </row>
     <row r="546" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1945</v>
+        <v>1918</v>
       </c>
       <c r="B546" s="3" t="b">
         <v>1</v>
@@ -18841,118 +18837,118 @@
         <v>1</v>
       </c>
       <c r="E546" t="s">
-        <v>1953</v>
+        <v>1926</v>
       </c>
       <c r="F546" s="6" t="s">
-        <v>1958</v>
+        <v>1931</v>
       </c>
       <c r="G546" t="s">
-        <v>2034</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="547" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A547" s="3" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B547" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C547" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E547" s="3" t="s">
+        <v>2086</v>
+      </c>
+      <c r="F547" s="6" t="s">
+        <v>2094</v>
+      </c>
+      <c r="G547" s="3" t="s">
         <v>2107</v>
-      </c>
-      <c r="B547" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C547" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E547" s="3" t="s">
-        <v>2113</v>
-      </c>
-      <c r="F547" s="6" t="s">
-        <v>2121</v>
-      </c>
-      <c r="G547" s="3" t="s">
-        <v>2134</v>
       </c>
     </row>
     <row r="548" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A548" s="3" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B548" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C548" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E548" s="3" t="s">
+        <v>2087</v>
+      </c>
+      <c r="F548" s="6" t="s">
+        <v>2095</v>
+      </c>
+      <c r="G548" s="3" t="s">
         <v>2108</v>
-      </c>
-      <c r="B548" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C548" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E548" s="3" t="s">
-        <v>2114</v>
-      </c>
-      <c r="F548" s="6" t="s">
-        <v>2122</v>
-      </c>
-      <c r="G548" s="3" t="s">
-        <v>2135</v>
       </c>
     </row>
     <row r="549" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A549" s="3" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B549" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C549" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E549" s="3" t="s">
+        <v>2088</v>
+      </c>
+      <c r="F549" s="6" t="s">
+        <v>2112</v>
+      </c>
+      <c r="G549" s="3" t="s">
         <v>2109</v>
-      </c>
-      <c r="B549" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C549" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E549" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="F549" s="6" t="s">
-        <v>2139</v>
-      </c>
-      <c r="G549" s="3" t="s">
-        <v>2136</v>
       </c>
     </row>
     <row r="550" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A550" s="3" t="s">
+        <v>2083</v>
+      </c>
+      <c r="B550" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C550" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E550" s="3" t="s">
+        <v>2089</v>
+      </c>
+      <c r="F550" s="6" t="s">
+        <v>2096</v>
+      </c>
+      <c r="G550" s="3" t="s">
         <v>2110</v>
-      </c>
-      <c r="B550" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C550" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E550" s="3" t="s">
-        <v>2116</v>
-      </c>
-      <c r="F550" s="6" t="s">
-        <v>2123</v>
-      </c>
-      <c r="G550" s="3" t="s">
-        <v>2137</v>
       </c>
     </row>
     <row r="551" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A551" s="3" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B551" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C551" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E551" s="3" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F551" s="6" t="s">
+        <v>2097</v>
+      </c>
+      <c r="G551" s="3" t="s">
         <v>2111</v>
-      </c>
-      <c r="B551" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C551" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E551" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="F551" s="6" t="s">
-        <v>2124</v>
-      </c>
-      <c r="G551" s="3" t="s">
-        <v>2138</v>
       </c>
     </row>
     <row r="552" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A552" s="3" t="s">
-        <v>2159</v>
+        <v>2132</v>
       </c>
       <c r="B552" s="3" t="b">
         <v>1</v>
@@ -18961,18 +18957,18 @@
         <v>1</v>
       </c>
       <c r="E552" s="3" t="s">
-        <v>2160</v>
+        <v>2133</v>
       </c>
       <c r="F552" s="6" t="s">
-        <v>2161</v>
+        <v>2134</v>
       </c>
       <c r="G552" s="3" t="s">
-        <v>2162</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="553" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>1960</v>
+        <v>1933</v>
       </c>
       <c r="B553" s="3" t="b">
         <v>1</v>
@@ -18981,18 +18977,18 @@
         <v>1</v>
       </c>
       <c r="E553" t="s">
-        <v>1973</v>
+        <v>1946</v>
       </c>
       <c r="F553" s="6" t="s">
-        <v>2007</v>
+        <v>1980</v>
       </c>
       <c r="G553" t="s">
-        <v>2035</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="554" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>1961</v>
+        <v>1934</v>
       </c>
       <c r="B554" s="3" t="b">
         <v>1</v>
@@ -19001,18 +18997,18 @@
         <v>1</v>
       </c>
       <c r="E554" t="s">
-        <v>1977</v>
+        <v>1950</v>
       </c>
       <c r="F554" s="6" t="s">
-        <v>2008</v>
+        <v>1981</v>
       </c>
       <c r="G554" t="s">
-        <v>2036</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="555" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>1962</v>
+        <v>1935</v>
       </c>
       <c r="B555" s="3" t="b">
         <v>1</v>
@@ -19021,13 +19017,13 @@
         <v>1</v>
       </c>
       <c r="E555" t="s">
-        <v>2056</v>
+        <v>2029</v>
       </c>
       <c r="F555" s="6" t="s">
-        <v>2057</v>
+        <v>2030</v>
       </c>
       <c r="G555" t="s">
-        <v>2058</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.25">
@@ -19052,7 +19048,7 @@
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>1963</v>
+        <v>1936</v>
       </c>
       <c r="B557" s="3" t="b">
         <v>1</v>
@@ -19061,18 +19057,18 @@
         <v>1</v>
       </c>
       <c r="E557" t="s">
-        <v>1978</v>
+        <v>1951</v>
       </c>
       <c r="F557" s="6" t="s">
-        <v>2009</v>
+        <v>1982</v>
       </c>
       <c r="G557" t="s">
-        <v>2037</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="558" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>1964</v>
+        <v>1937</v>
       </c>
       <c r="B558" s="3" t="b">
         <v>1</v>
@@ -19081,18 +19077,18 @@
         <v>1</v>
       </c>
       <c r="E558" t="s">
-        <v>1979</v>
+        <v>1952</v>
       </c>
       <c r="F558" s="6" t="s">
-        <v>2010</v>
+        <v>1983</v>
       </c>
       <c r="G558" t="s">
-        <v>2038</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="559" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>1965</v>
+        <v>1938</v>
       </c>
       <c r="B559" s="3" t="b">
         <v>1</v>
@@ -19101,18 +19097,18 @@
         <v>1</v>
       </c>
       <c r="E559" t="s">
-        <v>1980</v>
+        <v>1953</v>
       </c>
       <c r="F559" s="6" t="s">
-        <v>2011</v>
+        <v>1984</v>
       </c>
       <c r="G559" t="s">
-        <v>2039</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="560" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>1966</v>
+        <v>1939</v>
       </c>
       <c r="B560" s="3" t="b">
         <v>1</v>
@@ -19121,18 +19117,18 @@
         <v>1</v>
       </c>
       <c r="E560" t="s">
-        <v>1981</v>
+        <v>1954</v>
       </c>
       <c r="F560" s="6" t="s">
-        <v>2012</v>
+        <v>1985</v>
       </c>
       <c r="G560" t="s">
-        <v>2040</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="561" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>1967</v>
+        <v>1940</v>
       </c>
       <c r="B561" s="3" t="b">
         <v>1</v>
@@ -19141,18 +19137,18 @@
         <v>1</v>
       </c>
       <c r="E561" t="s">
-        <v>1982</v>
+        <v>1955</v>
       </c>
       <c r="F561" s="6" t="s">
-        <v>2013</v>
+        <v>1986</v>
       </c>
       <c r="G561" t="s">
-        <v>2041</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="562" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>1968</v>
+        <v>1941</v>
       </c>
       <c r="B562" s="3" t="b">
         <v>1</v>
@@ -19164,7 +19160,7 @@
         <v>882</v>
       </c>
       <c r="F562" s="6" t="s">
-        <v>2014</v>
+        <v>1987</v>
       </c>
       <c r="G562" t="s">
         <v>1539</v>
@@ -19172,7 +19168,7 @@
     </row>
     <row r="563" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>1969</v>
+        <v>1942</v>
       </c>
       <c r="B563" s="3" t="b">
         <v>1</v>
@@ -19181,18 +19177,18 @@
         <v>1</v>
       </c>
       <c r="E563" t="s">
-        <v>1974</v>
+        <v>1947</v>
       </c>
       <c r="F563" s="6" t="s">
-        <v>2015</v>
+        <v>1988</v>
       </c>
       <c r="G563" t="s">
-        <v>2055</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="564" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>1970</v>
+        <v>1943</v>
       </c>
       <c r="B564" s="3" t="b">
         <v>1</v>
@@ -19201,18 +19197,18 @@
         <v>1</v>
       </c>
       <c r="E564" t="s">
-        <v>1983</v>
+        <v>1956</v>
       </c>
       <c r="F564" s="6" t="s">
-        <v>2016</v>
+        <v>1989</v>
       </c>
       <c r="G564" t="s">
-        <v>2042</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="565" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>1971</v>
+        <v>1944</v>
       </c>
       <c r="B565" s="3" t="b">
         <v>1</v>
@@ -19221,18 +19217,18 @@
         <v>1</v>
       </c>
       <c r="E565" t="s">
-        <v>1975</v>
+        <v>1948</v>
       </c>
       <c r="F565" s="6" t="s">
-        <v>2158</v>
+        <v>2131</v>
       </c>
       <c r="G565" t="s">
-        <v>2043</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="566" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>1972</v>
+        <v>1945</v>
       </c>
       <c r="B566" s="3" t="b">
         <v>1</v>
@@ -19241,18 +19237,18 @@
         <v>1</v>
       </c>
       <c r="E566" t="s">
-        <v>1976</v>
+        <v>1949</v>
       </c>
       <c r="F566" s="6" t="s">
+        <v>1990</v>
+      </c>
+      <c r="G566" t="s">
         <v>2017</v>
-      </c>
-      <c r="G566" t="s">
-        <v>2044</v>
       </c>
     </row>
     <row r="567" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>1988</v>
+        <v>1961</v>
       </c>
       <c r="B567" t="b">
         <v>1</v>
@@ -19267,12 +19263,12 @@
         <v>1208</v>
       </c>
       <c r="G567" t="s">
-        <v>2045</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="568" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>1984</v>
+        <v>1957</v>
       </c>
       <c r="B568" t="b">
         <v>1</v>
@@ -19281,18 +19277,18 @@
         <v>1</v>
       </c>
       <c r="E568" t="s">
-        <v>1985</v>
+        <v>1958</v>
       </c>
       <c r="F568" s="6" t="s">
-        <v>2018</v>
+        <v>1991</v>
       </c>
       <c r="G568" t="s">
-        <v>2046</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>1986</v>
+        <v>1959</v>
       </c>
       <c r="B569" t="b">
         <v>1</v>
@@ -19301,18 +19297,18 @@
         <v>1</v>
       </c>
       <c r="E569" t="s">
-        <v>1987</v>
+        <v>1960</v>
       </c>
       <c r="F569" s="6" t="s">
-        <v>2019</v>
+        <v>1992</v>
       </c>
       <c r="G569" t="s">
-        <v>2047</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="570" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>1994</v>
+        <v>1967</v>
       </c>
       <c r="B570" s="3" t="b">
         <v>1</v>
@@ -19321,18 +19317,18 @@
         <v>1</v>
       </c>
       <c r="E570" t="s">
-        <v>1989</v>
+        <v>1962</v>
       </c>
       <c r="F570" s="6" t="s">
-        <v>2020</v>
+        <v>1993</v>
       </c>
       <c r="G570" t="s">
-        <v>2048</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>1995</v>
+        <v>1968</v>
       </c>
       <c r="B571" s="3" t="b">
         <v>1</v>
@@ -19341,18 +19337,18 @@
         <v>1</v>
       </c>
       <c r="E571" t="s">
-        <v>1990</v>
+        <v>1963</v>
       </c>
       <c r="F571" s="6" t="s">
-        <v>2021</v>
+        <v>1994</v>
       </c>
       <c r="G571" t="s">
-        <v>2049</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="572" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>1991</v>
+        <v>1964</v>
       </c>
       <c r="B572" s="3" t="b">
         <v>1</v>
@@ -19361,18 +19357,18 @@
         <v>1</v>
       </c>
       <c r="E572" t="s">
-        <v>1992</v>
+        <v>1965</v>
       </c>
       <c r="F572" s="6" t="s">
-        <v>2022</v>
+        <v>1995</v>
       </c>
       <c r="G572" t="s">
-        <v>2050</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>1993</v>
+        <v>1966</v>
       </c>
       <c r="B573" s="3" t="b">
         <v>1</v>
@@ -19381,18 +19377,18 @@
         <v>1</v>
       </c>
       <c r="E573" t="s">
+        <v>1997</v>
+      </c>
+      <c r="F573" s="6" t="s">
+        <v>1996</v>
+      </c>
+      <c r="G573" t="s">
         <v>2024</v>
-      </c>
-      <c r="F573" s="6" t="s">
-        <v>2023</v>
-      </c>
-      <c r="G573" t="s">
-        <v>2051</v>
       </c>
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>1996</v>
+        <v>1969</v>
       </c>
       <c r="B574" s="3" t="b">
         <v>1</v>
@@ -19412,7 +19408,7 @@
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>1997</v>
+        <v>1970</v>
       </c>
       <c r="B575" s="3" t="b">
         <v>1</v>
@@ -19421,18 +19417,18 @@
         <v>1</v>
       </c>
       <c r="E575" t="s">
-        <v>1908</v>
+        <v>1881</v>
       </c>
       <c r="F575" s="6" t="s">
-        <v>1912</v>
+        <v>1885</v>
       </c>
       <c r="G575" t="s">
-        <v>1916</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="576" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>1998</v>
+        <v>1971</v>
       </c>
       <c r="B576" s="3" t="b">
         <v>1</v>
@@ -19441,18 +19437,18 @@
         <v>1</v>
       </c>
       <c r="E576" t="s">
-        <v>1907</v>
+        <v>1880</v>
       </c>
       <c r="F576" s="6" t="s">
-        <v>1911</v>
+        <v>1884</v>
       </c>
       <c r="G576" t="s">
-        <v>1915</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>1999</v>
+        <v>1972</v>
       </c>
       <c r="B577" s="3" t="b">
         <v>1</v>
@@ -19461,18 +19457,18 @@
         <v>1</v>
       </c>
       <c r="E577" t="s">
-        <v>1910</v>
+        <v>1883</v>
       </c>
       <c r="F577" s="6" t="s">
-        <v>1914</v>
+        <v>1887</v>
       </c>
       <c r="G577" t="s">
-        <v>1918</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="578" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>2000</v>
+        <v>1973</v>
       </c>
       <c r="B578" s="3" t="b">
         <v>1</v>
@@ -19481,18 +19477,18 @@
         <v>1</v>
       </c>
       <c r="E578" t="s">
-        <v>1909</v>
+        <v>1882</v>
       </c>
       <c r="F578" s="6" t="s">
-        <v>1913</v>
+        <v>1886</v>
       </c>
       <c r="G578" t="s">
-        <v>1917</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="579" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>2001</v>
+        <v>1974</v>
       </c>
       <c r="B579" s="3" t="b">
         <v>1</v>
@@ -19501,18 +19497,18 @@
         <v>1</v>
       </c>
       <c r="E579" t="s">
-        <v>2002</v>
+        <v>1975</v>
       </c>
       <c r="F579" s="6" t="s">
+        <v>1998</v>
+      </c>
+      <c r="G579" t="s">
         <v>2025</v>
-      </c>
-      <c r="G579" t="s">
-        <v>2052</v>
       </c>
     </row>
     <row r="580" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>2003</v>
+        <v>1976</v>
       </c>
       <c r="B580" s="3" t="b">
         <v>1</v>
@@ -19521,18 +19517,18 @@
         <v>1</v>
       </c>
       <c r="E580" t="s">
-        <v>2005</v>
+        <v>1978</v>
       </c>
       <c r="F580" s="6" t="s">
+        <v>1999</v>
+      </c>
+      <c r="G580" t="s">
         <v>2026</v>
-      </c>
-      <c r="G580" t="s">
-        <v>2053</v>
       </c>
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>2004</v>
+        <v>1977</v>
       </c>
       <c r="B581" s="3" t="b">
         <v>1</v>
@@ -19541,18 +19537,18 @@
         <v>1</v>
       </c>
       <c r="E581" t="s">
-        <v>2006</v>
+        <v>1979</v>
       </c>
       <c r="F581" s="6" t="s">
-        <v>1958</v>
+        <v>1931</v>
       </c>
       <c r="G581" t="s">
-        <v>2054</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="582" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>2056</v>
+        <v>2029</v>
       </c>
       <c r="B582" t="b">
         <v>0</v>
@@ -19561,18 +19557,18 @@
         <v>1</v>
       </c>
       <c r="E582" t="s">
-        <v>2056</v>
+        <v>2029</v>
       </c>
       <c r="F582" s="6" t="s">
-        <v>2057</v>
+        <v>2030</v>
       </c>
       <c r="G582" t="s">
-        <v>2058</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="583" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>2059</v>
+        <v>2032</v>
       </c>
       <c r="B583" t="b">
         <v>0</v>
@@ -19581,18 +19577,18 @@
         <v>1</v>
       </c>
       <c r="E583" t="s">
-        <v>2059</v>
+        <v>2032</v>
       </c>
       <c r="F583" s="6" t="s">
-        <v>2060</v>
+        <v>2033</v>
       </c>
       <c r="G583" t="s">
-        <v>2061</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>2069</v>
+        <v>2042</v>
       </c>
       <c r="B584" t="b">
         <v>1</v>
@@ -19601,18 +19597,18 @@
         <v>1</v>
       </c>
       <c r="E584" t="s">
-        <v>2069</v>
+        <v>2042</v>
       </c>
       <c r="F584" s="6" t="s">
-        <v>2072</v>
+        <v>2045</v>
       </c>
       <c r="G584" t="s">
-        <v>2073</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>2070</v>
+        <v>2043</v>
       </c>
       <c r="B585" s="3" t="b">
         <v>1</v>
@@ -19621,18 +19617,18 @@
         <v>1</v>
       </c>
       <c r="E585" t="s">
-        <v>2070</v>
+        <v>2043</v>
       </c>
       <c r="F585" s="6" t="s">
-        <v>2071</v>
+        <v>2044</v>
       </c>
       <c r="G585" t="s">
-        <v>2074</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>2081</v>
+        <v>2054</v>
       </c>
       <c r="B586" t="b">
         <v>0</v>
@@ -19641,18 +19637,18 @@
         <v>1</v>
       </c>
       <c r="E586" t="s">
-        <v>2081</v>
+        <v>2054</v>
       </c>
       <c r="F586" s="6" t="s">
-        <v>2013</v>
+        <v>1986</v>
       </c>
       <c r="G586" t="s">
-        <v>2088</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>2078</v>
+        <v>2051</v>
       </c>
       <c r="B587" t="b">
         <v>1</v>
@@ -19661,18 +19657,18 @@
         <v>1</v>
       </c>
       <c r="E587" t="s">
-        <v>2079</v>
+        <v>2052</v>
       </c>
       <c r="F587" s="6" t="s">
-        <v>2080</v>
+        <v>2053</v>
       </c>
       <c r="G587" t="s">
-        <v>2089</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="588" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A588" s="3" t="s">
-        <v>2082</v>
+        <v>2055</v>
       </c>
       <c r="B588" t="b">
         <v>0</v>
@@ -19681,18 +19677,18 @@
         <v>1</v>
       </c>
       <c r="E588" t="s">
-        <v>2083</v>
+        <v>2056</v>
       </c>
       <c r="F588" s="6" t="s">
-        <v>2084</v>
+        <v>2057</v>
       </c>
       <c r="G588" t="s">
-        <v>2090</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="589" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>2085</v>
+        <v>2058</v>
       </c>
       <c r="B589" t="b">
         <v>0</v>
@@ -19701,18 +19697,18 @@
         <v>1</v>
       </c>
       <c r="E589" t="s">
-        <v>2086</v>
+        <v>2059</v>
       </c>
       <c r="F589" s="6" t="s">
-        <v>2087</v>
+        <v>2060</v>
       </c>
       <c r="G589" t="s">
-        <v>2091</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>2092</v>
+        <v>2065</v>
       </c>
       <c r="B590" t="b">
         <v>0</v>
@@ -19721,18 +19717,18 @@
         <v>1</v>
       </c>
       <c r="E590" t="s">
-        <v>2092</v>
+        <v>2065</v>
       </c>
       <c r="F590" s="6" t="s">
-        <v>2095</v>
+        <v>2068</v>
       </c>
       <c r="G590" t="s">
-        <v>2096</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="591" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>2093</v>
+        <v>2066</v>
       </c>
       <c r="B591" t="b">
         <v>0</v>
@@ -19741,13 +19737,13 @@
         <v>1</v>
       </c>
       <c r="E591" t="s">
-        <v>2093</v>
+        <v>2066</v>
       </c>
       <c r="F591" s="6" t="s">
-        <v>2094</v>
+        <v>2067</v>
       </c>
       <c r="G591" t="s">
-        <v>2097</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="592" spans="1:7" x14ac:dyDescent="0.25">
@@ -19772,7 +19768,7 @@
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>2163</v>
+        <v>2136</v>
       </c>
       <c r="B593" t="b">
         <v>0</v>
@@ -19781,18 +19777,18 @@
         <v>1</v>
       </c>
       <c r="E593" t="s">
-        <v>2164</v>
+        <v>2137</v>
       </c>
       <c r="F593" s="6" t="s">
-        <v>2165</v>
+        <v>2138</v>
       </c>
       <c r="G593" t="s">
-        <v>2169</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="594" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>2166</v>
+        <v>2139</v>
       </c>
       <c r="B594" t="b">
         <v>0</v>
@@ -19801,18 +19797,18 @@
         <v>1</v>
       </c>
       <c r="E594" t="s">
-        <v>2168</v>
+        <v>2141</v>
       </c>
       <c r="F594" s="6" t="s">
-        <v>2167</v>
+        <v>2140</v>
       </c>
       <c r="G594" t="s">
-        <v>2170</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="595" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>2171</v>
+        <v>2144</v>
       </c>
       <c r="B595" t="b">
         <v>0</v>
@@ -19821,18 +19817,18 @@
         <v>1</v>
       </c>
       <c r="E595" t="s">
-        <v>2172</v>
+        <v>2145</v>
       </c>
       <c r="F595" s="6" t="s">
-        <v>2173</v>
+        <v>2146</v>
       </c>
       <c r="G595" t="s">
-        <v>2174</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>2175</v>
+        <v>2148</v>
       </c>
       <c r="B596" t="b">
         <v>1</v>
@@ -19841,13 +19837,13 @@
         <v>0</v>
       </c>
       <c r="E596" t="s">
-        <v>2178</v>
+        <v>2151</v>
       </c>
       <c r="F596" s="6" t="s">
-        <v>2176</v>
+        <v>2149</v>
       </c>
       <c r="G596" t="s">
-        <v>2177</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="597" spans="1:7" x14ac:dyDescent="0.25">
@@ -19861,10 +19857,10 @@
         <v>1</v>
       </c>
       <c r="E597" t="s">
-        <v>2179</v>
+        <v>2152</v>
       </c>
       <c r="F597" s="6" t="s">
-        <v>2180</v>
+        <v>2153</v>
       </c>
       <c r="G597" t="s">
         <v>1226</v>
@@ -19872,7 +19868,7 @@
     </row>
     <row r="598" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A598" s="3" t="s">
-        <v>2195</v>
+        <v>2168</v>
       </c>
       <c r="B598" s="3" t="b">
         <v>1</v>
@@ -19881,18 +19877,18 @@
         <v>1</v>
       </c>
       <c r="E598" s="3" t="s">
-        <v>1737</v>
+        <v>1711</v>
       </c>
       <c r="F598" s="6" t="s">
-        <v>2198</v>
+        <v>2171</v>
       </c>
       <c r="G598" s="3" t="s">
-        <v>1784</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="599" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A599" s="3" t="s">
-        <v>2196</v>
+        <v>2169</v>
       </c>
       <c r="B599" s="3" t="b">
         <v>1</v>
@@ -19901,38 +19897,38 @@
         <v>1</v>
       </c>
       <c r="E599" s="3" t="s">
-        <v>2197</v>
+        <v>2170</v>
       </c>
       <c r="F599" s="6" t="s">
-        <v>2199</v>
+        <v>2172</v>
       </c>
       <c r="G599" s="3" t="s">
-        <v>1784</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="600" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
+        <v>2162</v>
+      </c>
+      <c r="B600" t="b">
+        <v>1</v>
+      </c>
+      <c r="C600" t="b">
+        <v>1</v>
+      </c>
+      <c r="E600" t="s">
+        <v>2166</v>
+      </c>
+      <c r="F600" s="6" t="s">
+        <v>2167</v>
+      </c>
+      <c r="G600" t="s">
         <v>2189</v>
-      </c>
-      <c r="B600" t="b">
-        <v>1</v>
-      </c>
-      <c r="C600" t="b">
-        <v>1</v>
-      </c>
-      <c r="E600" t="s">
-        <v>2193</v>
-      </c>
-      <c r="F600" s="6" t="s">
-        <v>2194</v>
-      </c>
-      <c r="G600" t="s">
-        <v>2216</v>
       </c>
     </row>
     <row r="601" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A601" s="3" t="s">
-        <v>2204</v>
+        <v>2177</v>
       </c>
       <c r="B601" s="3" t="b">
         <v>1</v>
@@ -19941,18 +19937,18 @@
         <v>1</v>
       </c>
       <c r="E601" s="3" t="s">
-        <v>2208</v>
+        <v>2181</v>
       </c>
       <c r="F601" s="6" t="s">
-        <v>2212</v>
+        <v>2185</v>
       </c>
       <c r="G601" s="3" t="s">
-        <v>2217</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="602" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A602" s="3" t="s">
-        <v>2205</v>
+        <v>2178</v>
       </c>
       <c r="B602" s="3" t="b">
         <v>1</v>
@@ -19961,18 +19957,18 @@
         <v>1</v>
       </c>
       <c r="E602" s="3" t="s">
-        <v>2209</v>
+        <v>2182</v>
       </c>
       <c r="F602" s="6" t="s">
-        <v>2213</v>
+        <v>2186</v>
       </c>
       <c r="G602" s="3" t="s">
-        <v>2218</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="603" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A603" s="3" t="s">
-        <v>2206</v>
+        <v>2179</v>
       </c>
       <c r="B603" s="3" t="b">
         <v>1</v>
@@ -19981,18 +19977,18 @@
         <v>1</v>
       </c>
       <c r="E603" s="3" t="s">
-        <v>2210</v>
+        <v>2183</v>
       </c>
       <c r="F603" s="6" t="s">
-        <v>2214</v>
+        <v>2187</v>
       </c>
       <c r="G603" s="3" t="s">
-        <v>2219</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="604" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A604" s="3" t="s">
-        <v>2207</v>
+        <v>2180</v>
       </c>
       <c r="B604" s="3" t="b">
         <v>1</v>
@@ -20001,18 +19997,18 @@
         <v>1</v>
       </c>
       <c r="E604" s="3" t="s">
-        <v>2211</v>
+        <v>2184</v>
       </c>
       <c r="F604" s="6" t="s">
-        <v>2215</v>
+        <v>2188</v>
       </c>
       <c r="G604" s="3" t="s">
-        <v>2220</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>2191</v>
+        <v>2164</v>
       </c>
       <c r="B605" t="b">
         <v>1</v>
@@ -20021,18 +20017,18 @@
         <v>1</v>
       </c>
       <c r="E605" t="s">
-        <v>2192</v>
+        <v>2165</v>
       </c>
       <c r="F605" s="6" t="s">
-        <v>2200</v>
+        <v>2173</v>
       </c>
       <c r="G605" t="s">
-        <v>2221</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="606" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>2201</v>
+        <v>2174</v>
       </c>
       <c r="B606" t="b">
         <v>1</v>
@@ -20041,18 +20037,18 @@
         <v>1</v>
       </c>
       <c r="E606" t="s">
-        <v>2202</v>
+        <v>2175</v>
       </c>
       <c r="F606" s="6" t="s">
-        <v>2203</v>
+        <v>2176</v>
       </c>
       <c r="G606" t="s">
-        <v>2222</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="607" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>2223</v>
+        <v>2196</v>
       </c>
       <c r="B607" t="b">
         <v>1</v>
@@ -20061,18 +20057,18 @@
         <v>1</v>
       </c>
       <c r="E607" t="s">
-        <v>2226</v>
+        <v>2199</v>
       </c>
       <c r="F607" s="6" t="s">
-        <v>2229</v>
+        <v>2202</v>
       </c>
       <c r="G607" t="s">
-        <v>2232</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="608" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>2224</v>
+        <v>2197</v>
       </c>
       <c r="B608" s="3" t="b">
         <v>1</v>
@@ -20081,18 +20077,18 @@
         <v>1</v>
       </c>
       <c r="E608" t="s">
-        <v>2227</v>
+        <v>2200</v>
       </c>
       <c r="F608" s="6" t="s">
-        <v>2230</v>
+        <v>2203</v>
       </c>
       <c r="G608" t="s">
-        <v>2233</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="609" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>2225</v>
+        <v>2198</v>
       </c>
       <c r="B609" s="3" t="b">
         <v>1</v>
@@ -20101,18 +20097,18 @@
         <v>1</v>
       </c>
       <c r="E609" t="s">
-        <v>2228</v>
+        <v>2201</v>
       </c>
       <c r="F609" s="6" t="s">
-        <v>2231</v>
+        <v>2204</v>
       </c>
       <c r="G609" t="s">
-        <v>2234</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="610" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>2241</v>
+        <v>2214</v>
       </c>
       <c r="B610" s="3" t="b">
         <v>1</v>
@@ -20121,18 +20117,18 @@
         <v>1</v>
       </c>
       <c r="E610" t="s">
-        <v>2242</v>
+        <v>2215</v>
       </c>
       <c r="F610" s="6" t="s">
-        <v>2243</v>
+        <v>2216</v>
       </c>
       <c r="G610" t="s">
-        <v>2244</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="611" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>2245</v>
+        <v>2218</v>
       </c>
       <c r="B611" t="b">
         <v>1</v>
@@ -20141,18 +20137,18 @@
         <v>1</v>
       </c>
       <c r="E611" t="s">
-        <v>2246</v>
+        <v>2219</v>
       </c>
       <c r="F611" s="6" t="s">
-        <v>2247</v>
+        <v>2220</v>
       </c>
       <c r="G611" t="s">
-        <v>2266</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="612" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>2248</v>
+        <v>2221</v>
       </c>
       <c r="B612" s="3" t="b">
         <v>1</v>
@@ -20161,18 +20157,18 @@
         <v>1</v>
       </c>
       <c r="E612" t="s">
-        <v>2254</v>
+        <v>2227</v>
       </c>
       <c r="F612" s="6" t="s">
-        <v>2260</v>
+        <v>2233</v>
       </c>
       <c r="G612" t="s">
-        <v>2267</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="613" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>2249</v>
+        <v>2222</v>
       </c>
       <c r="B613" s="3" t="b">
         <v>1</v>
@@ -20181,18 +20177,18 @@
         <v>1</v>
       </c>
       <c r="E613" t="s">
-        <v>2258</v>
+        <v>2231</v>
       </c>
       <c r="F613" s="6" t="s">
-        <v>2261</v>
+        <v>2234</v>
       </c>
       <c r="G613" t="s">
-        <v>2268</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="614" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>2250</v>
+        <v>2223</v>
       </c>
       <c r="B614" s="3" t="b">
         <v>1</v>
@@ -20201,18 +20197,18 @@
         <v>1</v>
       </c>
       <c r="E614" s="3" t="s">
-        <v>2255</v>
+        <v>2228</v>
       </c>
       <c r="F614" s="6" t="s">
-        <v>2262</v>
+        <v>2235</v>
       </c>
       <c r="G614" t="s">
-        <v>2269</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="615" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>2251</v>
+        <v>2224</v>
       </c>
       <c r="B615" s="3" t="b">
         <v>1</v>
@@ -20221,18 +20217,18 @@
         <v>1</v>
       </c>
       <c r="E615" s="3" t="s">
-        <v>2256</v>
+        <v>2229</v>
       </c>
       <c r="F615" s="6" t="s">
-        <v>2263</v>
+        <v>2236</v>
       </c>
       <c r="G615" t="s">
-        <v>2270</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="616" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>2252</v>
+        <v>2225</v>
       </c>
       <c r="B616" s="3" t="b">
         <v>1</v>
@@ -20241,18 +20237,18 @@
         <v>1</v>
       </c>
       <c r="E616" s="3" t="s">
-        <v>2257</v>
+        <v>2230</v>
       </c>
       <c r="F616" s="6" t="s">
-        <v>2264</v>
+        <v>2237</v>
       </c>
       <c r="G616" t="s">
-        <v>2271</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="617" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>2253</v>
+        <v>2226</v>
       </c>
       <c r="B617" s="3" t="b">
         <v>1</v>
@@ -20261,18 +20257,18 @@
         <v>1</v>
       </c>
       <c r="E617" s="3" t="s">
-        <v>2259</v>
+        <v>2232</v>
       </c>
       <c r="F617" s="6" t="s">
-        <v>2265</v>
+        <v>2238</v>
       </c>
       <c r="G617" t="s">
-        <v>2272</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="618" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A618" s="3" t="s">
-        <v>1733</v>
+        <v>1707</v>
       </c>
       <c r="B618" s="3" t="b">
         <v>1</v>
@@ -20282,18 +20278,18 @@
       </c>
       <c r="D618" s="3"/>
       <c r="E618" s="3" t="s">
-        <v>1733</v>
+        <v>1707</v>
       </c>
       <c r="F618" s="6" t="s">
-        <v>2077</v>
+        <v>2050</v>
       </c>
       <c r="G618" s="3" t="s">
-        <v>1785</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="619" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A619" s="3" t="s">
-        <v>2075</v>
+        <v>2048</v>
       </c>
       <c r="B619" s="3" t="b">
         <v>1</v>
@@ -20303,13 +20299,13 @@
       </c>
       <c r="D619" s="3"/>
       <c r="E619" s="3" t="s">
-        <v>2075</v>
+        <v>2048</v>
       </c>
       <c r="F619" s="6" t="s">
-        <v>2076</v>
+        <v>2049</v>
       </c>
       <c r="G619" s="3" t="s">
-        <v>1785</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="620" spans="1:7" x14ac:dyDescent="0.25">
@@ -20397,7 +20393,7 @@
     </row>
     <row r="624" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A624" s="3" t="s">
-        <v>2181</v>
+        <v>2154</v>
       </c>
       <c r="B624" s="3" t="b">
         <v>1</v>
@@ -20406,7 +20402,7 @@
         <v>1</v>
       </c>
       <c r="E624" s="3" t="s">
-        <v>1685</v>
+        <v>1682</v>
       </c>
       <c r="F624" s="6" t="s">
         <v>832</v>
@@ -20417,7 +20413,7 @@
     </row>
     <row r="625" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A625" s="3" t="s">
-        <v>2182</v>
+        <v>2155</v>
       </c>
       <c r="B625" s="3" t="b">
         <v>1</v>
@@ -20427,7 +20423,7 @@
       </c>
       <c r="D625" s="3"/>
       <c r="E625" s="3" t="s">
-        <v>1686</v>
+        <v>1683</v>
       </c>
       <c r="F625" s="6" t="s">
         <v>833</v>
@@ -20438,7 +20434,7 @@
     </row>
     <row r="626" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A626" s="3" t="s">
-        <v>2183</v>
+        <v>2156</v>
       </c>
       <c r="B626" s="3" t="b">
         <v>1</v>
@@ -20447,7 +20443,7 @@
         <v>1</v>
       </c>
       <c r="E626" s="3" t="s">
-        <v>1687</v>
+        <v>1684</v>
       </c>
       <c r="F626" s="6" t="s">
         <v>834</v>
@@ -20458,7 +20454,7 @@
     </row>
     <row r="627" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A627" s="3" t="s">
-        <v>2184</v>
+        <v>2157</v>
       </c>
       <c r="B627" s="3" t="b">
         <v>1</v>
@@ -20467,7 +20463,7 @@
         <v>1</v>
       </c>
       <c r="E627" s="3" t="s">
-        <v>1688</v>
+        <v>1685</v>
       </c>
       <c r="F627" s="6" t="s">
         <v>835</v>
@@ -20478,7 +20474,7 @@
     </row>
     <row r="628" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A628" s="3" t="s">
-        <v>2185</v>
+        <v>2158</v>
       </c>
       <c r="B628" s="3" t="b">
         <v>1</v>
@@ -20487,13 +20483,13 @@
         <v>1</v>
       </c>
       <c r="E628" s="3" t="s">
-        <v>2186</v>
+        <v>2159</v>
       </c>
       <c r="F628" s="6" t="s">
-        <v>2187</v>
+        <v>2160</v>
       </c>
       <c r="G628" s="3" t="s">
-        <v>2188</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="629" spans="1:7" x14ac:dyDescent="0.25">
@@ -20540,7 +20536,7 @@
     </row>
     <row r="631" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>2273</v>
+        <v>2246</v>
       </c>
       <c r="B631" s="3" t="b">
         <v>1</v>
@@ -20549,18 +20545,18 @@
         <v>1</v>
       </c>
       <c r="E631" t="s">
-        <v>1739</v>
+        <v>1713</v>
       </c>
       <c r="F631" s="6" t="s">
-        <v>2278</v>
+        <v>2251</v>
       </c>
       <c r="G631" t="s">
-        <v>1787</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>2274</v>
+        <v>2247</v>
       </c>
       <c r="B632" s="3" t="b">
         <v>1</v>
@@ -20572,7 +20568,7 @@
         <v>422</v>
       </c>
       <c r="F632" s="6" t="s">
-        <v>1751</v>
+        <v>1725</v>
       </c>
       <c r="G632" t="s">
         <v>1357</v>
@@ -20580,7 +20576,7 @@
     </row>
     <row r="633" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A633" s="3" t="s">
-        <v>2275</v>
+        <v>2248</v>
       </c>
       <c r="B633" s="3" t="b">
         <v>1</v>
@@ -20592,7 +20588,7 @@
         <v>428</v>
       </c>
       <c r="F633" s="6" t="s">
-        <v>2279</v>
+        <v>2252</v>
       </c>
       <c r="G633" t="s">
         <v>1359</v>
@@ -20600,7 +20596,7 @@
     </row>
     <row r="634" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A634" s="3" t="s">
-        <v>2276</v>
+        <v>2249</v>
       </c>
       <c r="B634" s="3" t="b">
         <v>1</v>
@@ -20612,7 +20608,7 @@
         <v>443</v>
       </c>
       <c r="F634" s="6" t="s">
-        <v>1747</v>
+        <v>1721</v>
       </c>
       <c r="G634" t="s">
         <v>1364</v>
@@ -20620,7 +20616,7 @@
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>2277</v>
+        <v>2250</v>
       </c>
       <c r="B635" s="3" t="b">
         <v>1</v>
@@ -20632,7 +20628,7 @@
         <v>434</v>
       </c>
       <c r="F635" s="6" t="s">
-        <v>1750</v>
+        <v>1724</v>
       </c>
       <c r="G635" t="s">
         <v>1361</v>
@@ -20640,7 +20636,7 @@
     </row>
     <row r="636" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>2280</v>
+        <v>2253</v>
       </c>
       <c r="B636" s="3" t="b">
         <v>1</v>
@@ -20649,18 +20645,18 @@
         <v>1</v>
       </c>
       <c r="E636" t="s">
-        <v>2282</v>
+        <v>2255</v>
       </c>
       <c r="F636" s="6" t="s">
-        <v>2284</v>
+        <v>2257</v>
       </c>
       <c r="G636" t="s">
-        <v>2286</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="637" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>2281</v>
+        <v>2254</v>
       </c>
       <c r="B637" s="3" t="b">
         <v>1</v>
@@ -20669,18 +20665,18 @@
         <v>1</v>
       </c>
       <c r="E637" t="s">
-        <v>2283</v>
+        <v>2256</v>
       </c>
       <c r="F637" s="6" t="s">
-        <v>2285</v>
+        <v>2258</v>
       </c>
       <c r="G637" t="s">
-        <v>2287</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="638" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>2288</v>
+        <v>2261</v>
       </c>
       <c r="B638" t="b">
         <v>1</v>
@@ -20689,18 +20685,18 @@
         <v>1</v>
       </c>
       <c r="E638" t="s">
-        <v>2289</v>
+        <v>2262</v>
       </c>
       <c r="F638" s="6" t="s">
-        <v>2290</v>
+        <v>2263</v>
       </c>
       <c r="G638" t="s">
-        <v>2291</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="639" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>2056</v>
+        <v>2029</v>
       </c>
       <c r="B639" t="b">
         <v>1</v>
@@ -20709,18 +20705,18 @@
         <v>1</v>
       </c>
       <c r="E639" t="s">
-        <v>2056</v>
+        <v>2029</v>
       </c>
       <c r="F639" s="6" t="s">
-        <v>2057</v>
+        <v>2030</v>
       </c>
       <c r="G639" s="3" t="s">
-        <v>2058</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="640" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>2301</v>
+        <v>2274</v>
       </c>
       <c r="B640" t="b">
         <v>0</v>
@@ -20729,21 +20725,21 @@
         <v>1</v>
       </c>
       <c r="D640" t="s">
-        <v>2306</v>
+        <v>2279</v>
       </c>
       <c r="E640" t="s">
-        <v>2301</v>
+        <v>2274</v>
       </c>
       <c r="F640" s="6" t="s">
-        <v>2304</v>
+        <v>2277</v>
       </c>
       <c r="G640" t="s">
-        <v>2307</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>2302</v>
+        <v>2275</v>
       </c>
       <c r="B641" t="b">
         <v>0</v>
@@ -20752,21 +20748,21 @@
         <v>1</v>
       </c>
       <c r="D641" t="s">
-        <v>2306</v>
+        <v>2279</v>
       </c>
       <c r="E641" t="s">
-        <v>2303</v>
+        <v>2276</v>
       </c>
       <c r="F641" s="6" t="s">
-        <v>2305</v>
+        <v>2278</v>
       </c>
       <c r="G641" t="s">
-        <v>2308</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="642" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>2314</v>
+        <v>2287</v>
       </c>
       <c r="B642" t="b">
         <v>1</v>
@@ -20775,18 +20771,18 @@
         <v>1</v>
       </c>
       <c r="E642" t="s">
-        <v>2312</v>
+        <v>2285</v>
       </c>
       <c r="F642" s="6" t="s">
-        <v>2316</v>
+        <v>2289</v>
       </c>
       <c r="G642" t="s">
-        <v>2317</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A643" s="3" t="s">
-        <v>2309</v>
+        <v>2282</v>
       </c>
       <c r="B643" t="b">
         <v>1</v>
@@ -20795,18 +20791,18 @@
         <v>1</v>
       </c>
       <c r="E643" t="s">
-        <v>2313</v>
+        <v>2286</v>
       </c>
       <c r="F643" s="6" t="s">
-        <v>2315</v>
+        <v>2288</v>
       </c>
       <c r="G643" t="s">
-        <v>2317</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="644" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A644" s="3" t="s">
-        <v>2310</v>
+        <v>2283</v>
       </c>
       <c r="B644" s="3" t="b">
         <v>1</v>
@@ -20826,7 +20822,7 @@
     </row>
     <row r="645" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A645" s="3" t="s">
-        <v>2311</v>
+        <v>2284</v>
       </c>
       <c r="B645" s="3" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Working on Documents integration tests
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E456A1-8F86-4956-8F88-81E5038532A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5218A6-EA69-4147-AA1F-05452CF84A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22020" yWindow="450" windowWidth="17790" windowHeight="14805" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
+    <workbookView xWindow="32475" yWindow="7950" windowWidth="23265" windowHeight="19890" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$535</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$536</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="2357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2654" uniqueCount="2364">
   <si>
     <t>Key</t>
   </si>
@@ -7071,9 +7071,6 @@
     <t>时间2</t>
   </si>
   <si>
-    <t>Error_TheDateCannotBeInTheFuture</t>
-  </si>
-  <si>
     <t>The date cannot be in the future</t>
   </si>
   <si>
@@ -7105,6 +7102,30 @@
   </si>
   <si>
     <t>يمنع النظام تعديل أي معاملات قبل هذا التاريخ</t>
+  </si>
+  <si>
+    <t>Error_DateCannotBeInTheFuture</t>
+  </si>
+  <si>
+    <t>The date cannot be before the archive date {0}</t>
+  </si>
+  <si>
+    <t>Error_DateCannotBeBeforeArchiveDate0</t>
+  </si>
+  <si>
+    <t>التاريخ لا يمكن أن يكون قبل تاريخ الأرشفة</t>
+  </si>
+  <si>
+    <t>The amount {0} does not match the value {1} even though both are in {2}</t>
+  </si>
+  <si>
+    <t>المبلغ {0} لا يساوي القيمة {1} مع أن العملة هي {2} لكليهما</t>
+  </si>
+  <si>
+    <t>Error_TheAmount0DoesNotMatchTheValue1EvenThoughBothIn2</t>
+  </si>
+  <si>
+    <t>Account_Currency</t>
   </si>
 </sst>
 </file>
@@ -7510,12 +7531,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G660"/>
+  <dimension ref="A1:G663"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A519" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F349" sqref="F349"/>
+      <selection pane="bottomLeft" activeCell="G521" sqref="G521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14777,19 +14798,19 @@
     </row>
     <row r="346" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
+        <v>2350</v>
+      </c>
+      <c r="B346" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C346" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E346" s="3" t="s">
         <v>2351</v>
       </c>
-      <c r="B346" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C346" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E346" s="3" t="s">
-        <v>2352</v>
-      </c>
       <c r="F346" s="6" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="G346" s="3" t="s">
         <v>2245</v>
@@ -14797,36 +14818,36 @@
     </row>
     <row r="347" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
+        <v>2347</v>
+      </c>
+      <c r="B347" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C347" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E347" s="3" t="s">
         <v>2348</v>
       </c>
-      <c r="B347" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C347" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E347" s="3" t="s">
+      <c r="F347" s="6" t="s">
         <v>2349</v>
-      </c>
-      <c r="F347" s="6" t="s">
-        <v>2350</v>
       </c>
     </row>
     <row r="348" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="s">
+        <v>2352</v>
+      </c>
+      <c r="B348" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C348" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E348" s="3" t="s">
         <v>2353</v>
       </c>
-      <c r="B348" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C348" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E348" s="3" t="s">
-        <v>2354</v>
-      </c>
       <c r="F348" s="6" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -18417,9 +18438,9 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="521" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A521" s="3" t="s">
-        <v>1807</v>
+        <v>2363</v>
       </c>
       <c r="B521" s="3" t="b">
         <v>1</v>
@@ -18427,20 +18448,19 @@
       <c r="C521" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D521" s="3"/>
       <c r="E521" s="3" t="s">
-        <v>1810</v>
+        <v>809</v>
       </c>
       <c r="F521" s="6" t="s">
-        <v>1808</v>
+        <v>819</v>
       </c>
       <c r="G521" s="3" t="s">
-        <v>1824</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="522" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A522" s="3" t="s">
-        <v>1812</v>
+        <v>1807</v>
       </c>
       <c r="B522" s="3" t="b">
         <v>1</v>
@@ -18450,18 +18470,18 @@
       </c>
       <c r="D522" s="3"/>
       <c r="E522" s="3" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="F522" s="6" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="G522" s="3" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="523" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A523" s="3" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="B523" s="3" t="b">
         <v>1</v>
@@ -18471,18 +18491,18 @@
       </c>
       <c r="D523" s="3"/>
       <c r="E523" s="3" t="s">
-        <v>1816</v>
+        <v>1811</v>
       </c>
       <c r="F523" s="6" t="s">
-        <v>1819</v>
+        <v>1809</v>
       </c>
       <c r="G523" s="3" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="524" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A524" s="3" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="B524" s="3" t="b">
         <v>1</v>
@@ -18492,18 +18512,18 @@
       </c>
       <c r="D524" s="3"/>
       <c r="E524" s="3" t="s">
-        <v>1820</v>
+        <v>1816</v>
       </c>
       <c r="F524" s="6" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="G524" s="3" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="525" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A525" s="3" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B525" s="3" t="b">
         <v>1</v>
@@ -18513,18 +18533,18 @@
       </c>
       <c r="D525" s="3"/>
       <c r="E525" s="3" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="F525" s="6" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="G525" s="3" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="526" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A526" s="3" t="s">
-        <v>1839</v>
+        <v>1815</v>
       </c>
       <c r="B526" s="3" t="b">
         <v>1</v>
@@ -18534,18 +18554,18 @@
       </c>
       <c r="D526" s="3"/>
       <c r="E526" s="3" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="F526" s="6" t="s">
-        <v>1823</v>
+        <v>1817</v>
       </c>
       <c r="G526" s="3" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="527" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A527" s="3" t="s">
-        <v>1830</v>
+        <v>1839</v>
       </c>
       <c r="B527" s="3" t="b">
         <v>1</v>
@@ -18555,18 +18575,18 @@
       </c>
       <c r="D527" s="3"/>
       <c r="E527" s="3" t="s">
-        <v>648</v>
+        <v>1822</v>
       </c>
       <c r="F527" s="6" t="s">
-        <v>649</v>
+        <v>1823</v>
       </c>
       <c r="G527" s="3" t="s">
-        <v>1436</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="528" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A528" s="3" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="B528" s="3" t="b">
         <v>1</v>
@@ -18576,18 +18596,18 @@
       </c>
       <c r="D528" s="3"/>
       <c r="E528" s="3" t="s">
-        <v>1649</v>
+        <v>648</v>
       </c>
       <c r="F528" s="6" t="s">
-        <v>1146</v>
+        <v>649</v>
       </c>
       <c r="G528" s="3" t="s">
-        <v>1716</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="529" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A529" s="3" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="B529" s="3" t="b">
         <v>1</v>
@@ -18597,18 +18617,18 @@
       </c>
       <c r="D529" s="3"/>
       <c r="E529" s="3" t="s">
-        <v>1834</v>
+        <v>1649</v>
       </c>
       <c r="F529" s="6" t="s">
-        <v>1836</v>
+        <v>1146</v>
       </c>
       <c r="G529" s="3" t="s">
-        <v>1837</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="530" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A530" s="3" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="B530" s="3" t="b">
         <v>1</v>
@@ -18618,58 +18638,59 @@
       </c>
       <c r="D530" s="3"/>
       <c r="E530" s="3" t="s">
+        <v>1834</v>
+      </c>
+      <c r="F530" s="6" t="s">
+        <v>1836</v>
+      </c>
+      <c r="G530" s="3" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="531" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A531" s="3" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B531" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C531" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D531" s="3"/>
+      <c r="E531" s="3" t="s">
         <v>1835</v>
       </c>
-      <c r="F530" s="6" t="s">
+      <c r="F531" s="6" t="s">
         <v>1751</v>
       </c>
-      <c r="G530" s="3" t="s">
+      <c r="G531" s="3" t="s">
         <v>1838</v>
       </c>
     </row>
-    <row r="531" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A531" s="3" t="s">
+    <row r="532" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A532" s="3" t="s">
         <v>1842</v>
       </c>
-      <c r="B531" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C531" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E531" s="3" t="s">
+      <c r="B532" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C532" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E532" s="3" t="s">
         <v>1840</v>
       </c>
-      <c r="F531" s="6" t="s">
+      <c r="F532" s="6" t="s">
         <v>1843</v>
       </c>
-      <c r="G531" s="3" t="s">
+      <c r="G532" s="3" t="s">
         <v>1841</v>
-      </c>
-    </row>
-    <row r="532" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A532" t="s">
-        <v>1844</v>
-      </c>
-      <c r="B532" t="b">
-        <v>1</v>
-      </c>
-      <c r="C532" t="b">
-        <v>1</v>
-      </c>
-      <c r="E532" s="3" t="s">
-        <v>1844</v>
-      </c>
-      <c r="F532" s="6" t="s">
-        <v>1847</v>
-      </c>
-      <c r="G532" t="s">
-        <v>1849</v>
       </c>
     </row>
     <row r="533" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="B533" t="b">
         <v>1</v>
@@ -18678,84 +18699,84 @@
         <v>1</v>
       </c>
       <c r="E533" s="3" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
       <c r="F533" s="6" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="G533" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="534" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B534" t="b">
+        <v>1</v>
+      </c>
+      <c r="C534" t="b">
+        <v>1</v>
+      </c>
+      <c r="E534" s="3" t="s">
+        <v>1846</v>
+      </c>
+      <c r="F534" s="6" t="s">
+        <v>1848</v>
+      </c>
+      <c r="G534" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="535" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
         <v>1851</v>
       </c>
-      <c r="B534" t="b">
-        <v>1</v>
-      </c>
-      <c r="C534" t="b">
-        <v>0</v>
-      </c>
-      <c r="D534" t="s">
+      <c r="B535" t="b">
+        <v>1</v>
+      </c>
+      <c r="C535" t="b">
+        <v>0</v>
+      </c>
+      <c r="D535" t="s">
         <v>1854</v>
       </c>
-      <c r="E534" s="3" t="s">
+      <c r="E535" s="3" t="s">
         <v>1852</v>
       </c>
-      <c r="F534" s="6" t="s">
+      <c r="F535" s="6" t="s">
         <v>1853</v>
       </c>
-      <c r="G534" s="3" t="s">
+      <c r="G535" s="3" t="s">
         <v>1853</v>
       </c>
     </row>
-    <row r="535" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A535" s="3" t="s">
+    <row r="536" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A536" s="3" t="s">
         <v>1851</v>
       </c>
-      <c r="B535" t="b">
-        <v>0</v>
-      </c>
-      <c r="C535" t="b">
-        <v>1</v>
-      </c>
-      <c r="D535" s="3" t="s">
+      <c r="B536" t="b">
+        <v>0</v>
+      </c>
+      <c r="C536" t="b">
+        <v>1</v>
+      </c>
+      <c r="D536" s="3" t="s">
         <v>1854</v>
       </c>
-      <c r="E535" s="3" t="s">
+      <c r="E536" s="3" t="s">
         <v>1855</v>
       </c>
-      <c r="F535" s="6" t="s">
+      <c r="F536" s="6" t="s">
         <v>1856</v>
       </c>
-      <c r="G535" s="3" t="s">
+      <c r="G536" s="3" t="s">
         <v>1856</v>
-      </c>
-    </row>
-    <row r="536" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A536" t="s">
-        <v>1869</v>
-      </c>
-      <c r="B536" t="b">
-        <v>0</v>
-      </c>
-      <c r="C536" t="b">
-        <v>1</v>
-      </c>
-      <c r="E536" t="s">
-        <v>1872</v>
-      </c>
-      <c r="F536" s="6" t="s">
-        <v>1870</v>
-      </c>
-      <c r="G536" s="3" t="s">
-        <v>1871</v>
       </c>
     </row>
     <row r="537" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>1881</v>
+        <v>1869</v>
       </c>
       <c r="B537" t="b">
         <v>0</v>
@@ -18764,78 +18785,78 @@
         <v>1</v>
       </c>
       <c r="E537" t="s">
-        <v>1881</v>
+        <v>1872</v>
       </c>
       <c r="F537" s="6" t="s">
-        <v>1882</v>
+        <v>1870</v>
       </c>
       <c r="G537" s="3" t="s">
-        <v>1883</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="538" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>1873</v>
-      </c>
-      <c r="B538" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C538" s="3" t="b">
+        <v>1881</v>
+      </c>
+      <c r="B538" t="b">
+        <v>0</v>
+      </c>
+      <c r="C538" t="b">
         <v>1</v>
       </c>
       <c r="E538" t="s">
-        <v>1874</v>
+        <v>1881</v>
       </c>
       <c r="F538" s="6" t="s">
-        <v>1876</v>
-      </c>
-      <c r="G538" t="s">
-        <v>1875</v>
+        <v>1882</v>
+      </c>
+      <c r="G538" s="3" t="s">
+        <v>1883</v>
       </c>
     </row>
     <row r="539" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>1877</v>
-      </c>
-      <c r="B539" t="b">
-        <v>0</v>
-      </c>
-      <c r="C539" t="b">
+        <v>1873</v>
+      </c>
+      <c r="B539" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C539" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E539" t="s">
-        <v>1878</v>
+        <v>1874</v>
       </c>
       <c r="F539" s="6" t="s">
-        <v>1879</v>
+        <v>1876</v>
       </c>
       <c r="G539" t="s">
-        <v>1880</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="540" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>1884</v>
-      </c>
-      <c r="B540" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C540" s="3" t="b">
+        <v>1877</v>
+      </c>
+      <c r="B540" t="b">
+        <v>0</v>
+      </c>
+      <c r="C540" t="b">
         <v>1</v>
       </c>
       <c r="E540" t="s">
-        <v>1886</v>
+        <v>1878</v>
       </c>
       <c r="F540" s="6" t="s">
-        <v>1888</v>
+        <v>1879</v>
       </c>
       <c r="G540" t="s">
-        <v>1977</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="B541" s="3" t="b">
         <v>1</v>
@@ -18844,10 +18865,10 @@
         <v>1</v>
       </c>
       <c r="E541" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="F541" s="6" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="G541" t="s">
         <v>1977</v>
@@ -18855,7 +18876,7 @@
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>42</v>
+        <v>1885</v>
       </c>
       <c r="B542" s="3" t="b">
         <v>1</v>
@@ -18864,18 +18885,18 @@
         <v>1</v>
       </c>
       <c r="E542" t="s">
-        <v>42</v>
+        <v>1887</v>
       </c>
       <c r="F542" s="6" t="s">
-        <v>110</v>
+        <v>1889</v>
       </c>
       <c r="G542" t="s">
-        <v>1227</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="543" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>1896</v>
+        <v>42</v>
       </c>
       <c r="B543" s="3" t="b">
         <v>1</v>
@@ -18884,18 +18905,18 @@
         <v>1</v>
       </c>
       <c r="E543" t="s">
-        <v>1804</v>
+        <v>42</v>
       </c>
       <c r="F543" s="6" t="s">
-        <v>1805</v>
+        <v>110</v>
       </c>
       <c r="G543" t="s">
-        <v>1806</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="544" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="B544" s="3" t="b">
         <v>1</v>
@@ -18904,18 +18925,18 @@
         <v>1</v>
       </c>
       <c r="E544" t="s">
-        <v>1899</v>
+        <v>1804</v>
       </c>
       <c r="F544" s="6" t="s">
-        <v>1904</v>
+        <v>1805</v>
       </c>
       <c r="G544" t="s">
-        <v>1978</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="545" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B545" s="3" t="b">
         <v>1</v>
@@ -18924,18 +18945,18 @@
         <v>1</v>
       </c>
       <c r="E545" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="F545" s="6" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="G545" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="546" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>1890</v>
+        <v>1898</v>
       </c>
       <c r="B546" s="3" t="b">
         <v>1</v>
@@ -18944,18 +18965,18 @@
         <v>1</v>
       </c>
       <c r="E546" t="s">
-        <v>1881</v>
+        <v>1900</v>
       </c>
       <c r="F546" s="6" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="G546" t="s">
-        <v>1883</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="547" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B547" s="3" t="b">
         <v>1</v>
@@ -18964,58 +18985,58 @@
         <v>1</v>
       </c>
       <c r="E547" t="s">
-        <v>1901</v>
+        <v>1881</v>
       </c>
       <c r="F547" s="6" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="G547" t="s">
-        <v>1980</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="548" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B548" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C548" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E548" t="s">
+        <v>1901</v>
+      </c>
+      <c r="F548" s="6" t="s">
+        <v>1907</v>
+      </c>
+      <c r="G548" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="549" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
         <v>1892</v>
       </c>
-      <c r="B548" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C548" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E548" t="s">
+      <c r="B549" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C549" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E549" t="s">
         <v>2094</v>
       </c>
-      <c r="F548" s="6" t="s">
+      <c r="F549" s="6" t="s">
         <v>2100</v>
       </c>
-      <c r="G548" t="s">
+      <c r="G549" t="s">
         <v>1981</v>
-      </c>
-    </row>
-    <row r="549" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A549" s="3" t="s">
-        <v>2048</v>
-      </c>
-      <c r="B549" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C549" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E549" s="3" t="s">
-        <v>2095</v>
-      </c>
-      <c r="F549" s="6" t="s">
-        <v>2101</v>
-      </c>
-      <c r="G549" s="3" t="s">
-        <v>2075</v>
       </c>
     </row>
     <row r="550" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A550" s="3" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B550" s="3" t="b">
         <v>1</v>
@@ -19024,78 +19045,78 @@
         <v>1</v>
       </c>
       <c r="E550" s="3" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="F550" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="G550" s="3" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="551" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A551" s="3" t="s">
+        <v>2049</v>
+      </c>
+      <c r="B551" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C551" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E551" s="3" t="s">
+        <v>2096</v>
+      </c>
+      <c r="F551" s="6" t="s">
+        <v>2102</v>
+      </c>
+      <c r="G551" s="3" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A552" s="3" t="s">
         <v>2050</v>
       </c>
-      <c r="B551" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C551" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E551" s="3" t="s">
+      <c r="B552" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C552" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E552" s="3" t="s">
         <v>2097</v>
       </c>
-      <c r="F551" s="6" t="s">
+      <c r="F552" s="6" t="s">
         <v>2103</v>
       </c>
-      <c r="G551" s="3" t="s">
+      <c r="G552" s="3" t="s">
         <v>2077</v>
       </c>
     </row>
-    <row r="552" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A552" t="s">
+    <row r="553" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
         <v>1893</v>
       </c>
-      <c r="B552" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C552" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E552" t="s">
+      <c r="B553" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C553" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E553" t="s">
         <v>2093</v>
       </c>
-      <c r="F552" s="6" t="s">
+      <c r="F553" s="6" t="s">
         <v>2104</v>
       </c>
-      <c r="G552" t="s">
+      <c r="G553" t="s">
         <v>1982</v>
-      </c>
-    </row>
-    <row r="553" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A553" s="3" t="s">
-        <v>2051</v>
-      </c>
-      <c r="B553" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C553" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E553" s="3" t="s">
-        <v>2092</v>
-      </c>
-      <c r="F553" s="6" t="s">
-        <v>2105</v>
-      </c>
-      <c r="G553" s="3" t="s">
-        <v>2078</v>
       </c>
     </row>
     <row r="554" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A554" s="3" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="B554" s="3" t="b">
         <v>1</v>
@@ -19104,78 +19125,78 @@
         <v>1</v>
       </c>
       <c r="E554" s="3" t="s">
-        <v>2091</v>
+        <v>2092</v>
       </c>
       <c r="F554" s="6" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="G554" s="3" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="555" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A555" s="3" t="s">
+        <v>2052</v>
+      </c>
+      <c r="B555" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C555" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E555" s="3" t="s">
+        <v>2091</v>
+      </c>
+      <c r="F555" s="6" t="s">
+        <v>2106</v>
+      </c>
+      <c r="G555" s="3" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A556" s="3" t="s">
         <v>2053</v>
       </c>
-      <c r="B555" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C555" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E555" s="3" t="s">
+      <c r="B556" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C556" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E556" s="3" t="s">
         <v>2090</v>
       </c>
-      <c r="F555" s="6" t="s">
+      <c r="F556" s="6" t="s">
         <v>2107</v>
       </c>
-      <c r="G555" s="3" t="s">
+      <c r="G556" s="3" t="s">
         <v>2080</v>
       </c>
     </row>
-    <row r="556" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A556" t="s">
+    <row r="557" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
         <v>1894</v>
       </c>
-      <c r="B556" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C556" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E556" t="s">
+      <c r="B557" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C557" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E557" t="s">
         <v>1902</v>
       </c>
-      <c r="F556" s="6" t="s">
+      <c r="F557" s="6" t="s">
         <v>1909</v>
       </c>
-      <c r="G556" t="s">
+      <c r="G557" t="s">
         <v>1983</v>
-      </c>
-    </row>
-    <row r="557" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A557" s="3" t="s">
-        <v>2054</v>
-      </c>
-      <c r="B557" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C557" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E557" s="3" t="s">
-        <v>2062</v>
-      </c>
-      <c r="F557" s="6" t="s">
-        <v>2068</v>
-      </c>
-      <c r="G557" s="3" t="s">
-        <v>2081</v>
       </c>
     </row>
     <row r="558" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A558" s="3" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B558" s="3" t="b">
         <v>1</v>
@@ -19184,78 +19205,78 @@
         <v>1</v>
       </c>
       <c r="E558" s="3" t="s">
-        <v>2098</v>
+        <v>2062</v>
       </c>
       <c r="F558" s="6" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="G558" s="3" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="559" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A559" s="3" t="s">
+        <v>2055</v>
+      </c>
+      <c r="B559" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C559" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E559" s="3" t="s">
+        <v>2098</v>
+      </c>
+      <c r="F559" s="6" t="s">
+        <v>2070</v>
+      </c>
+      <c r="G559" s="3" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A560" s="3" t="s">
         <v>2056</v>
       </c>
-      <c r="B559" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C559" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E559" s="3" t="s">
+      <c r="B560" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C560" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E560" s="3" t="s">
         <v>2099</v>
       </c>
-      <c r="F559" s="6" t="s">
+      <c r="F560" s="6" t="s">
         <v>2069</v>
       </c>
-      <c r="G559" s="3" t="s">
+      <c r="G560" s="3" t="s">
         <v>2083</v>
       </c>
     </row>
-    <row r="560" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A560" t="s">
+    <row r="561" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
         <v>1895</v>
       </c>
-      <c r="B560" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C560" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E560" t="s">
+      <c r="B561" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C561" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E561" t="s">
         <v>1903</v>
       </c>
-      <c r="F560" s="6" t="s">
+      <c r="F561" s="6" t="s">
         <v>1908</v>
       </c>
-      <c r="G560" t="s">
+      <c r="G561" t="s">
         <v>1984</v>
-      </c>
-    </row>
-    <row r="561" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A561" s="3" t="s">
-        <v>2057</v>
-      </c>
-      <c r="B561" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C561" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E561" s="3" t="s">
-        <v>2063</v>
-      </c>
-      <c r="F561" s="6" t="s">
-        <v>2071</v>
-      </c>
-      <c r="G561" s="3" t="s">
-        <v>2084</v>
       </c>
     </row>
     <row r="562" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A562" s="3" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="B562" s="3" t="b">
         <v>1</v>
@@ -19264,18 +19285,18 @@
         <v>1</v>
       </c>
       <c r="E562" s="3" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="F562" s="6" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="G562" s="3" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="563" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A563" s="3" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="B563" s="3" t="b">
         <v>1</v>
@@ -19284,18 +19305,18 @@
         <v>1</v>
       </c>
       <c r="E563" s="3" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="F563" s="6" t="s">
-        <v>2089</v>
+        <v>2072</v>
       </c>
       <c r="G563" s="3" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="564" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A564" s="3" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="B564" s="3" t="b">
         <v>1</v>
@@ -19304,18 +19325,18 @@
         <v>1</v>
       </c>
       <c r="E564" s="3" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="F564" s="6" t="s">
-        <v>2073</v>
+        <v>2089</v>
       </c>
       <c r="G564" s="3" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="565" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A565" s="3" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="B565" s="3" t="b">
         <v>1</v>
@@ -19324,58 +19345,58 @@
         <v>1</v>
       </c>
       <c r="E565" s="3" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="F565" s="6" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="G565" s="3" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="566" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A566" s="3" t="s">
+        <v>2061</v>
+      </c>
+      <c r="B566" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C566" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E566" s="3" t="s">
+        <v>2067</v>
+      </c>
+      <c r="F566" s="6" t="s">
+        <v>2074</v>
+      </c>
+      <c r="G566" s="3" t="s">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A567" s="3" t="s">
         <v>2109</v>
       </c>
-      <c r="B566" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C566" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E566" s="3" t="s">
+      <c r="B567" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C567" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E567" s="3" t="s">
         <v>2110</v>
       </c>
-      <c r="F566" s="6" t="s">
+      <c r="F567" s="6" t="s">
         <v>2111</v>
       </c>
-      <c r="G566" s="3" t="s">
+      <c r="G567" s="3" t="s">
         <v>2112</v>
-      </c>
-    </row>
-    <row r="567" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A567" t="s">
-        <v>1910</v>
-      </c>
-      <c r="B567" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C567" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E567" t="s">
-        <v>1923</v>
-      </c>
-      <c r="F567" s="6" t="s">
-        <v>1957</v>
-      </c>
-      <c r="G567" t="s">
-        <v>1985</v>
       </c>
     </row>
     <row r="568" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B568" s="3" t="b">
         <v>1</v>
@@ -19384,18 +19405,18 @@
         <v>1</v>
       </c>
       <c r="E568" t="s">
-        <v>1927</v>
+        <v>1923</v>
       </c>
       <c r="F568" s="6" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="G568" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B569" s="3" t="b">
         <v>1</v>
@@ -19404,18 +19425,18 @@
         <v>1</v>
       </c>
       <c r="E569" t="s">
-        <v>2006</v>
+        <v>1927</v>
       </c>
       <c r="F569" s="6" t="s">
-        <v>2007</v>
+        <v>1958</v>
       </c>
       <c r="G569" t="s">
-        <v>2008</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="570" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>320</v>
+        <v>1912</v>
       </c>
       <c r="B570" s="3" t="b">
         <v>1</v>
@@ -19424,18 +19445,18 @@
         <v>1</v>
       </c>
       <c r="E570" t="s">
-        <v>320</v>
+        <v>2006</v>
       </c>
       <c r="F570" s="6" t="s">
-        <v>319</v>
+        <v>2007</v>
       </c>
       <c r="G570" t="s">
-        <v>1322</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>1913</v>
+        <v>320</v>
       </c>
       <c r="B571" s="3" t="b">
         <v>1</v>
@@ -19444,18 +19465,18 @@
         <v>1</v>
       </c>
       <c r="E571" t="s">
-        <v>1928</v>
+        <v>320</v>
       </c>
       <c r="F571" s="6" t="s">
-        <v>1959</v>
+        <v>319</v>
       </c>
       <c r="G571" t="s">
-        <v>1987</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="572" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B572" s="3" t="b">
         <v>1</v>
@@ -19464,18 +19485,18 @@
         <v>1</v>
       </c>
       <c r="E572" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="F572" s="6" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="G572" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B573" s="3" t="b">
         <v>1</v>
@@ -19484,18 +19505,18 @@
         <v>1</v>
       </c>
       <c r="E573" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="F573" s="6" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="G573" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B574" s="3" t="b">
         <v>1</v>
@@ -19504,18 +19525,18 @@
         <v>1</v>
       </c>
       <c r="E574" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="F574" s="6" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="G574" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="B575" s="3" t="b">
         <v>1</v>
@@ -19524,18 +19545,18 @@
         <v>1</v>
       </c>
       <c r="E575" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="F575" s="6" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="G575" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="576" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B576" s="3" t="b">
         <v>1</v>
@@ -19544,18 +19565,18 @@
         <v>1</v>
       </c>
       <c r="E576" t="s">
-        <v>882</v>
+        <v>1932</v>
       </c>
       <c r="F576" s="6" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="G576" t="s">
-        <v>1539</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="B577" s="3" t="b">
         <v>1</v>
@@ -19564,18 +19585,18 @@
         <v>1</v>
       </c>
       <c r="E577" t="s">
-        <v>1924</v>
+        <v>882</v>
       </c>
       <c r="F577" s="6" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="G577" t="s">
-        <v>2005</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="578" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="B578" s="3" t="b">
         <v>1</v>
@@ -19584,18 +19605,18 @@
         <v>1</v>
       </c>
       <c r="E578" t="s">
-        <v>1933</v>
+        <v>1924</v>
       </c>
       <c r="F578" s="6" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="G578" t="s">
-        <v>1992</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="579" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="B579" s="3" t="b">
         <v>1</v>
@@ -19604,18 +19625,18 @@
         <v>1</v>
       </c>
       <c r="E579" t="s">
-        <v>1925</v>
+        <v>1933</v>
       </c>
       <c r="F579" s="6" t="s">
-        <v>2108</v>
+        <v>1966</v>
       </c>
       <c r="G579" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="580" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="B580" s="3" t="b">
         <v>1</v>
@@ -19624,38 +19645,38 @@
         <v>1</v>
       </c>
       <c r="E580" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="F580" s="6" t="s">
-        <v>1967</v>
+        <v>2108</v>
       </c>
       <c r="G580" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>1938</v>
-      </c>
-      <c r="B581" t="b">
-        <v>1</v>
-      </c>
-      <c r="C581" t="b">
+        <v>1922</v>
+      </c>
+      <c r="B581" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C581" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E581" t="s">
-        <v>0</v>
+        <v>1926</v>
       </c>
       <c r="F581" s="6" t="s">
-        <v>1208</v>
+        <v>1967</v>
       </c>
       <c r="G581" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="582" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1934</v>
+        <v>1938</v>
       </c>
       <c r="B582" t="b">
         <v>1</v>
@@ -19664,18 +19685,18 @@
         <v>1</v>
       </c>
       <c r="E582" t="s">
-        <v>1935</v>
+        <v>0</v>
       </c>
       <c r="F582" s="6" t="s">
-        <v>1968</v>
+        <v>1208</v>
       </c>
       <c r="G582" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="583" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="B583" t="b">
         <v>1</v>
@@ -19684,38 +19705,38 @@
         <v>1</v>
       </c>
       <c r="E583" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="F583" s="6" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="G583" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>1944</v>
-      </c>
-      <c r="B584" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C584" s="3" t="b">
+        <v>1936</v>
+      </c>
+      <c r="B584" t="b">
+        <v>1</v>
+      </c>
+      <c r="C584" t="b">
         <v>1</v>
       </c>
       <c r="E584" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="F584" s="6" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="G584" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="B585" s="3" t="b">
         <v>1</v>
@@ -19724,18 +19745,18 @@
         <v>1</v>
       </c>
       <c r="E585" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="F585" s="6" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="G585" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>1941</v>
+        <v>1945</v>
       </c>
       <c r="B586" s="3" t="b">
         <v>1</v>
@@ -19744,18 +19765,18 @@
         <v>1</v>
       </c>
       <c r="E586" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="F586" s="6" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="G586" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="B587" s="3" t="b">
         <v>1</v>
@@ -19764,18 +19785,18 @@
         <v>1</v>
       </c>
       <c r="E587" t="s">
-        <v>1974</v>
+        <v>1942</v>
       </c>
       <c r="F587" s="6" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="G587" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="588" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
       <c r="B588" s="3" t="b">
         <v>1</v>
@@ -19784,18 +19805,18 @@
         <v>1</v>
       </c>
       <c r="E588" t="s">
-        <v>422</v>
+        <v>1974</v>
       </c>
       <c r="F588" s="6" t="s">
-        <v>421</v>
+        <v>1973</v>
       </c>
       <c r="G588" t="s">
-        <v>1357</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="589" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="B589" s="3" t="b">
         <v>1</v>
@@ -19804,18 +19825,18 @@
         <v>1</v>
       </c>
       <c r="E589" t="s">
-        <v>1858</v>
+        <v>422</v>
       </c>
       <c r="F589" s="6" t="s">
-        <v>1862</v>
+        <v>421</v>
       </c>
       <c r="G589" t="s">
-        <v>1866</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B590" s="3" t="b">
         <v>1</v>
@@ -19824,18 +19845,18 @@
         <v>1</v>
       </c>
       <c r="E590" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="F590" s="6" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="G590" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="591" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B591" s="3" t="b">
         <v>1</v>
@@ -19844,18 +19865,18 @@
         <v>1</v>
       </c>
       <c r="E591" t="s">
-        <v>1860</v>
+        <v>1857</v>
       </c>
       <c r="F591" s="6" t="s">
-        <v>1864</v>
+        <v>1861</v>
       </c>
       <c r="G591" t="s">
-        <v>1868</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="592" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="B592" s="3" t="b">
         <v>1</v>
@@ -19864,18 +19885,18 @@
         <v>1</v>
       </c>
       <c r="E592" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="F592" s="6" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
       <c r="G592" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B593" s="3" t="b">
         <v>1</v>
@@ -19884,18 +19905,18 @@
         <v>1</v>
       </c>
       <c r="E593" t="s">
-        <v>1952</v>
+        <v>1859</v>
       </c>
       <c r="F593" s="6" t="s">
-        <v>1975</v>
+        <v>1863</v>
       </c>
       <c r="G593" t="s">
-        <v>2002</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="594" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="B594" s="3" t="b">
         <v>1</v>
@@ -19904,18 +19925,18 @@
         <v>1</v>
       </c>
       <c r="E594" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="F594" s="6" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="G594" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="595" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="B595" s="3" t="b">
         <v>1</v>
@@ -19924,38 +19945,38 @@
         <v>1</v>
       </c>
       <c r="E595" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="F595" s="6" t="s">
-        <v>1908</v>
+        <v>1976</v>
       </c>
       <c r="G595" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>2006</v>
-      </c>
-      <c r="B596" t="b">
-        <v>0</v>
-      </c>
-      <c r="C596" t="b">
+        <v>1954</v>
+      </c>
+      <c r="B596" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C596" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E596" t="s">
-        <v>2006</v>
+        <v>1956</v>
       </c>
       <c r="F596" s="6" t="s">
-        <v>2007</v>
+        <v>1908</v>
       </c>
       <c r="G596" t="s">
-        <v>2008</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="597" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="B597" t="b">
         <v>0</v>
@@ -19964,138 +19985,138 @@
         <v>1</v>
       </c>
       <c r="E597" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="F597" s="6" t="s">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="G597" t="s">
-        <v>2011</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="598" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>2019</v>
+        <v>2009</v>
       </c>
       <c r="B598" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C598" t="b">
         <v>1</v>
       </c>
       <c r="E598" t="s">
-        <v>2019</v>
+        <v>2009</v>
       </c>
       <c r="F598" s="6" t="s">
-        <v>2022</v>
+        <v>2010</v>
       </c>
       <c r="G598" t="s">
-        <v>2023</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="599" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>2020</v>
-      </c>
-      <c r="B599" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C599" s="3" t="b">
+        <v>2019</v>
+      </c>
+      <c r="B599" t="b">
+        <v>1</v>
+      </c>
+      <c r="C599" t="b">
         <v>1</v>
       </c>
       <c r="E599" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F599" s="6" t="s">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="G599" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="600" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>2031</v>
-      </c>
-      <c r="B600" t="b">
-        <v>0</v>
-      </c>
-      <c r="C600" t="b">
+        <v>2020</v>
+      </c>
+      <c r="B600" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C600" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E600" t="s">
-        <v>2031</v>
+        <v>2020</v>
       </c>
       <c r="F600" s="6" t="s">
-        <v>1963</v>
+        <v>2021</v>
       </c>
       <c r="G600" t="s">
-        <v>2038</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="601" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
+        <v>2031</v>
+      </c>
+      <c r="B601" t="b">
+        <v>0</v>
+      </c>
+      <c r="C601" t="b">
+        <v>1</v>
+      </c>
+      <c r="E601" t="s">
+        <v>2031</v>
+      </c>
+      <c r="F601" s="6" t="s">
+        <v>1963</v>
+      </c>
+      <c r="G601" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="602" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
         <v>2028</v>
       </c>
-      <c r="B601" t="b">
-        <v>1</v>
-      </c>
-      <c r="C601" t="b">
-        <v>1</v>
-      </c>
-      <c r="E601" t="s">
+      <c r="B602" t="b">
+        <v>1</v>
+      </c>
+      <c r="C602" t="b">
+        <v>1</v>
+      </c>
+      <c r="E602" t="s">
         <v>2029</v>
       </c>
-      <c r="F601" s="6" t="s">
+      <c r="F602" s="6" t="s">
         <v>2030</v>
       </c>
-      <c r="G601" t="s">
+      <c r="G602" t="s">
         <v>2039</v>
       </c>
     </row>
-    <row r="602" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A602" s="3" t="s">
+    <row r="603" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A603" s="3" t="s">
         <v>2032</v>
       </c>
-      <c r="B602" t="b">
-        <v>0</v>
-      </c>
-      <c r="C602" t="b">
-        <v>1</v>
-      </c>
-      <c r="E602" t="s">
+      <c r="B603" t="b">
+        <v>0</v>
+      </c>
+      <c r="C603" t="b">
+        <v>1</v>
+      </c>
+      <c r="E603" t="s">
         <v>2033</v>
       </c>
-      <c r="F602" s="6" t="s">
+      <c r="F603" s="6" t="s">
         <v>2034</v>
       </c>
-      <c r="G602" t="s">
+      <c r="G603" t="s">
         <v>2040</v>
-      </c>
-    </row>
-    <row r="603" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A603" t="s">
-        <v>2035</v>
-      </c>
-      <c r="B603" t="b">
-        <v>0</v>
-      </c>
-      <c r="C603" t="b">
-        <v>1</v>
-      </c>
-      <c r="E603" t="s">
-        <v>2036</v>
-      </c>
-      <c r="F603" s="6" t="s">
-        <v>2037</v>
-      </c>
-      <c r="G603" t="s">
-        <v>2041</v>
       </c>
     </row>
     <row r="604" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>2042</v>
+        <v>2035</v>
       </c>
       <c r="B604" t="b">
         <v>0</v>
@@ -20104,18 +20125,18 @@
         <v>1</v>
       </c>
       <c r="E604" t="s">
-        <v>2042</v>
+        <v>2036</v>
       </c>
       <c r="F604" s="6" t="s">
-        <v>2045</v>
+        <v>2037</v>
       </c>
       <c r="G604" t="s">
-        <v>2046</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B605" t="b">
         <v>0</v>
@@ -20124,18 +20145,18 @@
         <v>1</v>
       </c>
       <c r="E605" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="F605" s="6" t="s">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="G605" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="606" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>970</v>
+        <v>2043</v>
       </c>
       <c r="B606" t="b">
         <v>0</v>
@@ -20144,18 +20165,18 @@
         <v>1</v>
       </c>
       <c r="E606" t="s">
-        <v>970</v>
+        <v>2043</v>
       </c>
       <c r="F606" s="6" t="s">
-        <v>1207</v>
+        <v>2044</v>
       </c>
       <c r="G606" t="s">
-        <v>1620</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="607" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>2113</v>
+        <v>970</v>
       </c>
       <c r="B607" t="b">
         <v>0</v>
@@ -20164,18 +20185,18 @@
         <v>1</v>
       </c>
       <c r="E607" t="s">
-        <v>2114</v>
+        <v>970</v>
       </c>
       <c r="F607" s="6" t="s">
-        <v>2115</v>
+        <v>1207</v>
       </c>
       <c r="G607" t="s">
-        <v>2119</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="608" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
       <c r="B608" t="b">
         <v>0</v>
@@ -20184,18 +20205,18 @@
         <v>1</v>
       </c>
       <c r="E608" t="s">
-        <v>2118</v>
+        <v>2114</v>
       </c>
       <c r="F608" s="6" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="G608" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="609" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>2121</v>
+        <v>2116</v>
       </c>
       <c r="B609" t="b">
         <v>0</v>
@@ -20204,78 +20225,78 @@
         <v>1</v>
       </c>
       <c r="E609" t="s">
-        <v>2122</v>
+        <v>2118</v>
       </c>
       <c r="F609" s="6" t="s">
-        <v>2123</v>
+        <v>2117</v>
       </c>
       <c r="G609" t="s">
-        <v>2124</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="610" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>2125</v>
+        <v>2121</v>
       </c>
       <c r="B610" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C610" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E610" t="s">
-        <v>2128</v>
+        <v>2122</v>
       </c>
       <c r="F610" s="6" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
       <c r="G610" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="611" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
+        <v>2125</v>
+      </c>
+      <c r="B611" t="b">
+        <v>1</v>
+      </c>
+      <c r="C611" t="b">
+        <v>0</v>
+      </c>
+      <c r="E611" t="s">
+        <v>2128</v>
+      </c>
+      <c r="F611" s="6" t="s">
+        <v>2126</v>
+      </c>
+      <c r="G611" t="s">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="612" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
         <v>37</v>
       </c>
-      <c r="B611" t="b">
-        <v>1</v>
-      </c>
-      <c r="C611" t="b">
-        <v>1</v>
-      </c>
-      <c r="E611" t="s">
+      <c r="B612" t="b">
+        <v>1</v>
+      </c>
+      <c r="C612" t="b">
+        <v>1</v>
+      </c>
+      <c r="E612" t="s">
         <v>2129</v>
       </c>
-      <c r="F611" s="6" t="s">
+      <c r="F612" s="6" t="s">
         <v>2130</v>
       </c>
-      <c r="G611" t="s">
+      <c r="G612" t="s">
         <v>1226</v>
-      </c>
-    </row>
-    <row r="612" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A612" s="3" t="s">
-        <v>2145</v>
-      </c>
-      <c r="B612" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C612" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E612" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F612" s="6" t="s">
-        <v>2148</v>
-      </c>
-      <c r="G612" s="3" t="s">
-        <v>1736</v>
       </c>
     </row>
     <row r="613" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A613" s="3" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="B613" s="3" t="b">
         <v>1</v>
@@ -20284,58 +20305,58 @@
         <v>1</v>
       </c>
       <c r="E613" s="3" t="s">
-        <v>2147</v>
+        <v>1700</v>
       </c>
       <c r="F613" s="6" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="G613" s="3" t="s">
         <v>1736</v>
       </c>
     </row>
-    <row r="614" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A614" t="s">
+    <row r="614" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A614" s="3" t="s">
+        <v>2146</v>
+      </c>
+      <c r="B614" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C614" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E614" s="3" t="s">
+        <v>2147</v>
+      </c>
+      <c r="F614" s="6" t="s">
+        <v>2149</v>
+      </c>
+      <c r="G614" s="3" t="s">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="615" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
         <v>2139</v>
       </c>
-      <c r="B614" t="b">
-        <v>1</v>
-      </c>
-      <c r="C614" t="b">
-        <v>1</v>
-      </c>
-      <c r="E614" t="s">
+      <c r="B615" t="b">
+        <v>1</v>
+      </c>
+      <c r="C615" t="b">
+        <v>1</v>
+      </c>
+      <c r="E615" t="s">
         <v>2143</v>
       </c>
-      <c r="F614" s="6" t="s">
+      <c r="F615" s="6" t="s">
         <v>2144</v>
       </c>
-      <c r="G614" t="s">
+      <c r="G615" t="s">
         <v>2166</v>
-      </c>
-    </row>
-    <row r="615" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A615" s="3" t="s">
-        <v>2154</v>
-      </c>
-      <c r="B615" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C615" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E615" s="3" t="s">
-        <v>2158</v>
-      </c>
-      <c r="F615" s="6" t="s">
-        <v>2162</v>
-      </c>
-      <c r="G615" s="3" t="s">
-        <v>2167</v>
       </c>
     </row>
     <row r="616" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A616" s="3" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="B616" s="3" t="b">
         <v>1</v>
@@ -20344,18 +20365,18 @@
         <v>1</v>
       </c>
       <c r="E616" s="3" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="F616" s="6" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="G616" s="3" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="617" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A617" s="3" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="B617" s="3" t="b">
         <v>1</v>
@@ -20364,58 +20385,58 @@
         <v>1</v>
       </c>
       <c r="E617" s="3" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="F617" s="6" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="G617" s="3" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="618" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A618" s="3" t="s">
+        <v>2156</v>
+      </c>
+      <c r="B618" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C618" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E618" s="3" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F618" s="6" t="s">
+        <v>2164</v>
+      </c>
+      <c r="G618" s="3" t="s">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="619" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A619" s="3" t="s">
         <v>2157</v>
       </c>
-      <c r="B618" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C618" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E618" s="3" t="s">
+      <c r="B619" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C619" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E619" s="3" t="s">
         <v>2161</v>
       </c>
-      <c r="F618" s="6" t="s">
+      <c r="F619" s="6" t="s">
         <v>2165</v>
       </c>
-      <c r="G618" s="3" t="s">
+      <c r="G619" s="3" t="s">
         <v>2170</v>
-      </c>
-    </row>
-    <row r="619" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A619" t="s">
-        <v>2141</v>
-      </c>
-      <c r="B619" t="b">
-        <v>1</v>
-      </c>
-      <c r="C619" t="b">
-        <v>1</v>
-      </c>
-      <c r="E619" t="s">
-        <v>2142</v>
-      </c>
-      <c r="F619" s="6" t="s">
-        <v>2150</v>
-      </c>
-      <c r="G619" t="s">
-        <v>2171</v>
       </c>
     </row>
     <row r="620" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>2151</v>
+        <v>2141</v>
       </c>
       <c r="B620" t="b">
         <v>1</v>
@@ -20424,58 +20445,58 @@
         <v>1</v>
       </c>
       <c r="E620" t="s">
-        <v>2152</v>
+        <v>2142</v>
       </c>
       <c r="F620" s="6" t="s">
-        <v>2153</v>
+        <v>2150</v>
       </c>
       <c r="G620" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="621" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>2173</v>
+        <v>2151</v>
       </c>
       <c r="B621" t="b">
         <v>1</v>
       </c>
-      <c r="C621" s="3" t="b">
+      <c r="C621" t="b">
         <v>1</v>
       </c>
       <c r="E621" t="s">
-        <v>2176</v>
+        <v>2152</v>
       </c>
       <c r="F621" s="6" t="s">
-        <v>2179</v>
+        <v>2153</v>
       </c>
       <c r="G621" t="s">
-        <v>2182</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="622" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>2174</v>
-      </c>
-      <c r="B622" s="3" t="b">
+        <v>2173</v>
+      </c>
+      <c r="B622" t="b">
         <v>1</v>
       </c>
       <c r="C622" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E622" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="F622" s="6" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="G622" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="623" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="B623" s="3" t="b">
         <v>1</v>
@@ -20484,18 +20505,18 @@
         <v>1</v>
       </c>
       <c r="E623" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="F623" s="6" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="G623" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="624" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>2191</v>
+        <v>2175</v>
       </c>
       <c r="B624" s="3" t="b">
         <v>1</v>
@@ -20504,58 +20525,58 @@
         <v>1</v>
       </c>
       <c r="E624" t="s">
-        <v>2192</v>
+        <v>2178</v>
       </c>
       <c r="F624" s="6" t="s">
-        <v>2193</v>
+        <v>2181</v>
       </c>
       <c r="G624" t="s">
-        <v>2194</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="625" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>2195</v>
-      </c>
-      <c r="B625" t="b">
-        <v>1</v>
-      </c>
-      <c r="C625" t="b">
+        <v>2191</v>
+      </c>
+      <c r="B625" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C625" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E625" t="s">
-        <v>2196</v>
+        <v>2192</v>
       </c>
       <c r="F625" s="6" t="s">
-        <v>2197</v>
+        <v>2193</v>
       </c>
       <c r="G625" t="s">
-        <v>2216</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="626" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>2198</v>
-      </c>
-      <c r="B626" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C626" s="3" t="b">
+        <v>2195</v>
+      </c>
+      <c r="B626" t="b">
+        <v>1</v>
+      </c>
+      <c r="C626" t="b">
         <v>1</v>
       </c>
       <c r="E626" t="s">
-        <v>2204</v>
+        <v>2196</v>
       </c>
       <c r="F626" s="6" t="s">
-        <v>2210</v>
+        <v>2197</v>
       </c>
       <c r="G626" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="627" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="B627" s="3" t="b">
         <v>1</v>
@@ -20564,18 +20585,18 @@
         <v>1</v>
       </c>
       <c r="E627" t="s">
-        <v>2208</v>
+        <v>2204</v>
       </c>
       <c r="F627" s="6" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="G627" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="628" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="B628" s="3" t="b">
         <v>1</v>
@@ -20583,19 +20604,19 @@
       <c r="C628" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E628" s="3" t="s">
-        <v>2205</v>
+      <c r="E628" t="s">
+        <v>2208</v>
       </c>
       <c r="F628" s="6" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="G628" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="629" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="B629" s="3" t="b">
         <v>1</v>
@@ -20604,18 +20625,18 @@
         <v>1</v>
       </c>
       <c r="E629" s="3" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="F629" s="6" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="G629" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="630" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="B630" s="3" t="b">
         <v>1</v>
@@ -20624,59 +20645,58 @@
         <v>1</v>
       </c>
       <c r="E630" s="3" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="F630" s="6" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="G630" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="631" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
+        <v>2202</v>
+      </c>
+      <c r="B631" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C631" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E631" s="3" t="s">
+        <v>2207</v>
+      </c>
+      <c r="F631" s="6" t="s">
+        <v>2214</v>
+      </c>
+      <c r="G631" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="632" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
         <v>2203</v>
       </c>
-      <c r="B631" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C631" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E631" s="3" t="s">
+      <c r="B632" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C632" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E632" s="3" t="s">
         <v>2209</v>
       </c>
-      <c r="F631" s="6" t="s">
+      <c r="F632" s="6" t="s">
         <v>2215</v>
       </c>
-      <c r="G631" t="s">
+      <c r="G632" t="s">
         <v>2222</v>
-      </c>
-    </row>
-    <row r="632" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A632" s="3" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B632" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C632" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D632" s="3"/>
-      <c r="E632" s="3" t="s">
-        <v>1699</v>
-      </c>
-      <c r="F632" s="6" t="s">
-        <v>2027</v>
-      </c>
-      <c r="G632" s="3" t="s">
-        <v>1737</v>
       </c>
     </row>
     <row r="633" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A633" s="3" t="s">
-        <v>2025</v>
+        <v>1699</v>
       </c>
       <c r="B633" s="3" t="b">
         <v>1</v>
@@ -20686,10 +20706,10 @@
       </c>
       <c r="D633" s="3"/>
       <c r="E633" s="3" t="s">
-        <v>2025</v>
+        <v>1699</v>
       </c>
       <c r="F633" s="6" t="s">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="G633" s="3" t="s">
         <v>1737</v>
@@ -20697,7 +20717,7 @@
     </row>
     <row r="634" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A634" s="3" t="s">
-        <v>816</v>
+        <v>2025</v>
       </c>
       <c r="B634" s="3" t="b">
         <v>1</v>
@@ -20707,18 +20727,18 @@
       </c>
       <c r="D634" s="3"/>
       <c r="E634" s="3" t="s">
-        <v>817</v>
+        <v>2025</v>
       </c>
       <c r="F634" s="6" t="s">
-        <v>439</v>
+        <v>2026</v>
       </c>
       <c r="G634" s="3" t="s">
-        <v>1490</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A635" s="3" t="s">
-        <v>829</v>
+        <v>816</v>
       </c>
       <c r="B635" s="3" t="b">
         <v>1</v>
@@ -20728,18 +20748,18 @@
       </c>
       <c r="D635" s="3"/>
       <c r="E635" s="3" t="s">
-        <v>831</v>
+        <v>817</v>
       </c>
       <c r="F635" s="6" t="s">
-        <v>830</v>
+        <v>439</v>
       </c>
       <c r="G635" s="3" t="s">
-        <v>1494</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="636" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A636" s="3" t="s">
-        <v>818</v>
+        <v>829</v>
       </c>
       <c r="B636" s="3" t="b">
         <v>1</v>
@@ -20749,99 +20769,100 @@
       </c>
       <c r="D636" s="3"/>
       <c r="E636" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="F636" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="G636" s="3" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="637" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A637" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="B637" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C637" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D637" s="3"/>
+      <c r="E637" s="3" t="s">
         <v>809</v>
       </c>
-      <c r="F636" s="6" t="s">
+      <c r="F637" s="6" t="s">
         <v>819</v>
       </c>
-      <c r="G636" s="3" t="s">
+      <c r="G637" s="3" t="s">
         <v>1488</v>
-      </c>
-    </row>
-    <row r="637" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A637" s="3" t="s">
-        <v>820</v>
-      </c>
-      <c r="B637" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C637" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E637" s="3" t="s">
-        <v>822</v>
-      </c>
-      <c r="F637" s="6" t="s">
-        <v>821</v>
-      </c>
-      <c r="G637" s="3" t="s">
-        <v>1491</v>
       </c>
     </row>
     <row r="638" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A638" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="B638" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C638" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E638" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="F638" s="6" t="s">
+        <v>821</v>
+      </c>
+      <c r="G638" s="3" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="639" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A639" s="3" t="s">
         <v>2131</v>
       </c>
-      <c r="B638" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C638" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E638" s="3" t="s">
+      <c r="B639" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C639" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E639" s="3" t="s">
         <v>1682</v>
       </c>
-      <c r="F638" s="6" t="s">
+      <c r="F639" s="6" t="s">
         <v>832</v>
       </c>
-      <c r="G638" s="3" t="s">
+      <c r="G639" s="3" t="s">
         <v>1495</v>
       </c>
     </row>
-    <row r="639" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A639" s="3" t="s">
+    <row r="640" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A640" s="3" t="s">
         <v>2132</v>
       </c>
-      <c r="B639" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C639" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D639" s="3"/>
-      <c r="E639" s="3" t="s">
+      <c r="B640" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C640" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D640" s="3"/>
+      <c r="E640" s="3" t="s">
         <v>1683</v>
       </c>
-      <c r="F639" s="6" t="s">
+      <c r="F640" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="G639" s="3" t="s">
+      <c r="G640" s="3" t="s">
         <v>1496</v>
-      </c>
-    </row>
-    <row r="640" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A640" s="3" t="s">
-        <v>2133</v>
-      </c>
-      <c r="B640" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C640" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E640" s="3" t="s">
-        <v>1684</v>
-      </c>
-      <c r="F640" s="6" t="s">
-        <v>834</v>
-      </c>
-      <c r="G640" s="3" t="s">
-        <v>1497</v>
       </c>
     </row>
     <row r="641" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A641" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="B641" s="3" t="b">
         <v>1</v>
@@ -20850,59 +20871,58 @@
         <v>1</v>
       </c>
       <c r="E641" s="3" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="F641" s="6" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="G641" s="3" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="642" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A642" s="3" t="s">
+        <v>2134</v>
+      </c>
+      <c r="B642" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C642" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E642" s="3" t="s">
+        <v>1685</v>
+      </c>
+      <c r="F642" s="6" t="s">
+        <v>835</v>
+      </c>
+      <c r="G642" s="3" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="643" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A643" s="3" t="s">
         <v>2135</v>
       </c>
-      <c r="B642" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C642" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E642" s="3" t="s">
+      <c r="B643" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C643" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E643" s="3" t="s">
         <v>2136</v>
       </c>
-      <c r="F642" s="6" t="s">
+      <c r="F643" s="6" t="s">
         <v>2137</v>
       </c>
-      <c r="G642" s="3" t="s">
+      <c r="G643" s="3" t="s">
         <v>2138</v>
-      </c>
-    </row>
-    <row r="643" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A643" s="3" t="s">
-        <v>826</v>
-      </c>
-      <c r="B643" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C643" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D643" s="3"/>
-      <c r="E643" s="3" t="s">
-        <v>828</v>
-      </c>
-      <c r="F643" s="6" t="s">
-        <v>827</v>
-      </c>
-      <c r="G643" s="3" t="s">
-        <v>1493</v>
       </c>
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A644" s="3" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="B644" s="3" t="b">
         <v>1</v>
@@ -20912,118 +20932,119 @@
       </c>
       <c r="D644" s="3"/>
       <c r="E644" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="F644" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="G644" s="3" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="645" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A645" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="B645" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C645" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D645" s="3"/>
+      <c r="E645" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="F644" s="6" t="s">
+      <c r="F645" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="G644" s="3" t="s">
+      <c r="G645" s="3" t="s">
         <v>1492</v>
-      </c>
-    </row>
-    <row r="645" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A645" t="s">
-        <v>2223</v>
-      </c>
-      <c r="B645" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C645" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E645" t="s">
-        <v>1701</v>
-      </c>
-      <c r="F645" s="6" t="s">
-        <v>2228</v>
-      </c>
-      <c r="G645" t="s">
-        <v>1738</v>
       </c>
     </row>
     <row r="646" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B646" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C646" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E646" t="s">
+        <v>1701</v>
+      </c>
+      <c r="F646" s="6" t="s">
+        <v>2228</v>
+      </c>
+      <c r="G646" t="s">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="647" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A647" t="s">
         <v>2224</v>
       </c>
-      <c r="B646" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C646" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E646" s="3" t="s">
+      <c r="B647" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C647" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E647" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="F646" s="6" t="s">
+      <c r="F647" s="6" t="s">
         <v>1709</v>
       </c>
-      <c r="G646" t="s">
+      <c r="G647" t="s">
         <v>1357</v>
-      </c>
-    </row>
-    <row r="647" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A647" s="3" t="s">
-        <v>2225</v>
-      </c>
-      <c r="B647" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C647" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E647" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="F647" s="6" t="s">
-        <v>2229</v>
-      </c>
-      <c r="G647" t="s">
-        <v>1359</v>
       </c>
     </row>
     <row r="648" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A648" s="3" t="s">
+        <v>2225</v>
+      </c>
+      <c r="B648" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C648" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E648" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="F648" s="6" t="s">
+        <v>2229</v>
+      </c>
+      <c r="G648" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="649" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A649" s="3" t="s">
         <v>2226</v>
       </c>
-      <c r="B648" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C648" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E648" s="3" t="s">
+      <c r="B649" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C649" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E649" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="F648" s="6" t="s">
+      <c r="F649" s="6" t="s">
         <v>1707</v>
       </c>
-      <c r="G648" t="s">
+      <c r="G649" t="s">
         <v>1364</v>
-      </c>
-    </row>
-    <row r="649" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A649" t="s">
-        <v>2227</v>
-      </c>
-      <c r="B649" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C649" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E649" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="F649" s="6" t="s">
-        <v>1708</v>
-      </c>
-      <c r="G649" t="s">
-        <v>1361</v>
       </c>
     </row>
     <row r="650" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>2230</v>
+        <v>2227</v>
       </c>
       <c r="B650" s="3" t="b">
         <v>1</v>
@@ -21031,19 +21052,19 @@
       <c r="C650" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E650" t="s">
-        <v>2232</v>
+      <c r="E650" s="3" t="s">
+        <v>434</v>
       </c>
       <c r="F650" s="6" t="s">
-        <v>2234</v>
+        <v>1708</v>
       </c>
       <c r="G650" t="s">
-        <v>2236</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="651" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="B651" s="3" t="b">
         <v>1</v>
@@ -21052,38 +21073,38 @@
         <v>1</v>
       </c>
       <c r="E651" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="F651" s="6" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="G651" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="652" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>2238</v>
-      </c>
-      <c r="B652" t="b">
-        <v>1</v>
-      </c>
-      <c r="C652" t="b">
+        <v>2231</v>
+      </c>
+      <c r="B652" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C652" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E652" t="s">
-        <v>2239</v>
+        <v>2233</v>
       </c>
       <c r="F652" s="6" t="s">
-        <v>2240</v>
+        <v>2235</v>
       </c>
       <c r="G652" t="s">
-        <v>2241</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>2006</v>
+        <v>2238</v>
       </c>
       <c r="B653" t="b">
         <v>1</v>
@@ -21092,41 +21113,38 @@
         <v>1</v>
       </c>
       <c r="E653" t="s">
-        <v>2006</v>
+        <v>2239</v>
       </c>
       <c r="F653" s="6" t="s">
-        <v>2007</v>
-      </c>
-      <c r="G653" s="3" t="s">
-        <v>2008</v>
+        <v>2240</v>
+      </c>
+      <c r="G653" t="s">
+        <v>2241</v>
       </c>
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>2251</v>
+        <v>2006</v>
       </c>
       <c r="B654" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C654" t="b">
         <v>1</v>
       </c>
-      <c r="D654" t="s">
-        <v>2256</v>
-      </c>
       <c r="E654" t="s">
-        <v>2251</v>
+        <v>2006</v>
       </c>
       <c r="F654" s="6" t="s">
-        <v>2254</v>
-      </c>
-      <c r="G654" t="s">
-        <v>2257</v>
+        <v>2007</v>
+      </c>
+      <c r="G654" s="3" t="s">
+        <v>2008</v>
       </c>
     </row>
     <row r="655" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
       <c r="B655" t="b">
         <v>0</v>
@@ -21138,114 +21156,171 @@
         <v>2256</v>
       </c>
       <c r="E655" t="s">
-        <v>2253</v>
+        <v>2251</v>
       </c>
       <c r="F655" s="6" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="G655" t="s">
-        <v>2258</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B656" t="b">
+        <v>0</v>
+      </c>
+      <c r="C656" t="b">
+        <v>1</v>
+      </c>
+      <c r="D656" t="s">
+        <v>2256</v>
+      </c>
+      <c r="E656" t="s">
+        <v>2253</v>
+      </c>
+      <c r="F656" s="6" t="s">
+        <v>2255</v>
+      </c>
+      <c r="G656" t="s">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="657" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
         <v>2264</v>
       </c>
-      <c r="B656" t="b">
-        <v>1</v>
-      </c>
-      <c r="C656" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E656" t="s">
+      <c r="B657" t="b">
+        <v>1</v>
+      </c>
+      <c r="C657" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E657" t="s">
         <v>2262</v>
       </c>
-      <c r="F656" s="6" t="s">
+      <c r="F657" s="6" t="s">
         <v>2266</v>
-      </c>
-      <c r="G656" t="s">
-        <v>2267</v>
-      </c>
-    </row>
-    <row r="657" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A657" s="3" t="s">
-        <v>2259</v>
-      </c>
-      <c r="B657" t="b">
-        <v>1</v>
-      </c>
-      <c r="C657" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E657" t="s">
-        <v>2263</v>
-      </c>
-      <c r="F657" s="6" t="s">
-        <v>2265</v>
       </c>
       <c r="G657" t="s">
         <v>2267</v>
       </c>
     </row>
-    <row r="658" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658" s="3" t="s">
-        <v>2260</v>
-      </c>
-      <c r="B658" s="3" t="b">
+        <v>2259</v>
+      </c>
+      <c r="B658" t="b">
         <v>1</v>
       </c>
       <c r="C658" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E658" s="3" t="s">
-        <v>326</v>
+      <c r="E658" t="s">
+        <v>2263</v>
       </c>
       <c r="F658" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="G658" s="3" t="s">
-        <v>1324</v>
+        <v>2265</v>
+      </c>
+      <c r="G658" t="s">
+        <v>2267</v>
       </c>
     </row>
     <row r="659" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A659" s="3" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B659" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C659" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E659" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F659" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="G659" s="3" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="660" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A660" s="3" t="s">
         <v>2261</v>
       </c>
-      <c r="B659" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C659" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E659" s="3" t="s">
+      <c r="B660" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C660" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E660" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="F659" s="6" t="s">
+      <c r="F660" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="G659" s="3" t="s">
+      <c r="G660" s="3" t="s">
         <v>1325</v>
       </c>
     </row>
-    <row r="660" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A660" t="s">
+    <row r="661" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A661" t="s">
+        <v>2356</v>
+      </c>
+      <c r="B661" t="b">
+        <v>1</v>
+      </c>
+      <c r="C661" t="b">
+        <v>1</v>
+      </c>
+      <c r="E661" t="s">
         <v>2345</v>
       </c>
-      <c r="B660" t="b">
-        <v>0</v>
-      </c>
-      <c r="C660" t="b">
-        <v>1</v>
-      </c>
-      <c r="E660" t="s">
+      <c r="F661" s="6" t="s">
         <v>2346</v>
       </c>
-      <c r="F660" s="6" t="s">
-        <v>2347</v>
+    </row>
+    <row r="662" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A662" t="s">
+        <v>2358</v>
+      </c>
+      <c r="B662" t="b">
+        <v>1</v>
+      </c>
+      <c r="C662" t="b">
+        <v>0</v>
+      </c>
+      <c r="E662" t="s">
+        <v>2357</v>
+      </c>
+      <c r="F662" s="6" t="s">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="663" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A663" t="s">
+        <v>2362</v>
+      </c>
+      <c r="B663" t="b">
+        <v>1</v>
+      </c>
+      <c r="C663" t="b">
+        <v>0</v>
+      </c>
+      <c r="E663" t="s">
+        <v>2360</v>
+      </c>
+      <c r="F663" s="6" t="s">
+        <v>2361</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G535" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G536" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented rudimentary version of JV
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66914FFA-6E81-4889-A0CC-E6637C24419C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CAC03C-E421-4FDA-9319-09676F66A87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32475" yWindow="7950" windowWidth="23265" windowHeight="19890" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$536</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="2371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="2377">
   <si>
     <t>Key</t>
   </si>
@@ -7125,9 +7126,6 @@
     <t>تلما</t>
   </si>
   <si>
-    <t>Tellma</t>
-  </si>
-  <si>
     <t>IncludeVoid</t>
   </si>
   <si>
@@ -7147,6 +7145,27 @@
   </si>
   <si>
     <t>包括空</t>
+  </si>
+  <si>
+    <t>tellma</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Cr.</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>مدين</t>
+  </si>
+  <si>
+    <t>دائن</t>
   </si>
 </sst>
 </file>
@@ -7552,12 +7571,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G664"/>
+  <dimension ref="A1:G666"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A620" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A635" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F648" sqref="F648"/>
+      <selection pane="bottomLeft" activeCell="E665" sqref="E665:E666"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8005,7 +8024,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>2363</v>
+        <v>2370</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>2362</v>
@@ -21306,7 +21325,7 @@
         <v>2344</v>
       </c>
       <c r="G661" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="662" spans="1:7" x14ac:dyDescent="0.25">
@@ -21326,7 +21345,7 @@
         <v>2357</v>
       </c>
       <c r="G662" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="663" spans="1:7" x14ac:dyDescent="0.25">
@@ -21346,27 +21365,61 @@
         <v>2359</v>
       </c>
       <c r="G663" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="664" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A664" s="3" t="s">
+        <v>2363</v>
+      </c>
+      <c r="B664" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C664" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E664" s="3" t="s">
         <v>2364</v>
       </c>
-      <c r="B664" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C664" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E664" s="3" t="s">
+      <c r="F664" s="6" t="s">
         <v>2365</v>
       </c>
-      <c r="F664" s="6" t="s">
-        <v>2366</v>
-      </c>
       <c r="G664" s="3" t="s">
-        <v>2370</v>
+        <v>2369</v>
+      </c>
+    </row>
+    <row r="665" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A665" t="s">
+        <v>2371</v>
+      </c>
+      <c r="B665" t="b">
+        <v>0</v>
+      </c>
+      <c r="C665" t="b">
+        <v>1</v>
+      </c>
+      <c r="E665" t="s">
+        <v>2374</v>
+      </c>
+      <c r="F665" s="6" t="s">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="666" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A666" t="s">
+        <v>2372</v>
+      </c>
+      <c r="B666" t="b">
+        <v>0</v>
+      </c>
+      <c r="C666" t="b">
+        <v>1</v>
+      </c>
+      <c r="E666" t="s">
+        <v>2373</v>
+      </c>
+      <c r="F666" s="6" t="s">
+        <v>2376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the signatures
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CAC03C-E421-4FDA-9319-09676F66A87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C29AB8-2E09-4A49-A180-CB3A9A90AB99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32475" yWindow="7950" windowWidth="23265" windowHeight="19890" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$536</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7147,9 +7146,6 @@
     <t>包括空</t>
   </si>
   <si>
-    <t>tellma</t>
-  </si>
-  <si>
     <t>Debit</t>
   </si>
   <si>
@@ -7166,6 +7162,9 @@
   </si>
   <si>
     <t>دائن</t>
+  </si>
+  <si>
+    <t>Tellma</t>
   </si>
 </sst>
 </file>
@@ -7574,9 +7573,9 @@
   <dimension ref="A1:G666"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A635" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E665" sqref="E665:E666"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8024,7 +8023,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>2370</v>
+        <v>2376</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>2362</v>
@@ -21390,7 +21389,7 @@
     </row>
     <row r="665" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="B665" t="b">
         <v>0</v>
@@ -21399,27 +21398,27 @@
         <v>1</v>
       </c>
       <c r="E665" t="s">
+        <v>2373</v>
+      </c>
+      <c r="F665" s="6" t="s">
         <v>2374</v>
-      </c>
-      <c r="F665" s="6" t="s">
-        <v>2375</v>
       </c>
     </row>
     <row r="666" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
+        <v>2371</v>
+      </c>
+      <c r="B666" t="b">
+        <v>0</v>
+      </c>
+      <c r="C666" t="b">
+        <v>1</v>
+      </c>
+      <c r="E666" t="s">
         <v>2372</v>
       </c>
-      <c r="B666" t="b">
-        <v>0</v>
-      </c>
-      <c r="C666" t="b">
-        <v>1</v>
-      </c>
-      <c r="E666" t="s">
-        <v>2373</v>
-      </c>
       <c r="F666" s="6" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved the signature display
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCB3025-69E3-450D-9139-FC3EA1326308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A090CC4B-7FBE-4366-8E19-10646E95FA74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="2390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="2394">
   <si>
     <t>Key</t>
   </si>
@@ -7204,6 +7204,18 @@
   </si>
   <si>
     <t>التوقيعات</t>
+  </si>
+  <si>
+    <t>OnBehalfOf</t>
+  </si>
+  <si>
+    <t>A short hand when someone signs on behalf of another</t>
+  </si>
+  <si>
+    <t>ع/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.p. </t>
   </si>
 </sst>
 </file>
@@ -7609,12 +7621,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G670"/>
+  <dimension ref="A1:G671"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A641" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G465" sqref="G465"/>
+      <selection pane="bottomLeft" activeCell="E673" sqref="E673"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21546,6 +21558,26 @@
         <v>2387</v>
       </c>
     </row>
+    <row r="671" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A671" t="s">
+        <v>2390</v>
+      </c>
+      <c r="B671" t="b">
+        <v>0</v>
+      </c>
+      <c r="C671" t="b">
+        <v>1</v>
+      </c>
+      <c r="D671" t="s">
+        <v>2391</v>
+      </c>
+      <c r="E671" t="s">
+        <v>2393</v>
+      </c>
+      <c r="F671" s="6" t="s">
+        <v>2392</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G537" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Removed Operating segment from Docs, Agents, Resources
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC4B52C-4829-40B8-AB66-2FD1E1845BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF3EA9C-DC8F-4AA6-A1AF-755B07C47EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$679</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$677</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="2442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="2434">
   <si>
     <t>Key</t>
   </si>
@@ -6450,12 +6450,6 @@
     <t>IsLeaf</t>
   </si>
   <si>
-    <t>ResponsibilityCenter_IsOperatingSegment</t>
-  </si>
-  <si>
-    <t>Is Operating Segment</t>
-  </si>
-  <si>
     <t>Responsibility Type</t>
   </si>
   <si>
@@ -6477,9 +6471,6 @@
     <t>مراكز مسؤولية</t>
   </si>
   <si>
-    <t>قطاع تشغيل</t>
-  </si>
-  <si>
     <t>ResponsibilityCenter_Manager</t>
   </si>
   <si>
@@ -6540,9 +6531,6 @@
     <t>成本</t>
   </si>
   <si>
-    <t>是一家以经营分部</t>
-  </si>
-  <si>
     <t>经理</t>
   </si>
   <si>
@@ -6612,15 +6600,6 @@
     <t>资源定义</t>
   </si>
   <si>
-    <t>OperatingSegment</t>
-  </si>
-  <si>
-    <t>Operating Segment</t>
-  </si>
-  <si>
-    <t>قطاع التشغيل</t>
-  </si>
-  <si>
     <t>Agent_StartDate</t>
   </si>
   <si>
@@ -6673,9 +6652,6 @@
   </si>
   <si>
     <t>رقم حساب البنك</t>
-  </si>
-  <si>
-    <t>经营分部</t>
   </si>
   <si>
     <t>开始日期</t>
@@ -7765,12 +7741,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G684"/>
+  <dimension ref="A1:G682"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A611" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F681" sqref="F681"/>
+      <selection pane="bottomLeft" activeCell="A634" sqref="A634:XFD634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8218,10 +8194,10 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>2375</v>
+        <v>2367</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>2361</v>
+        <v>2353</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>1627</v>
@@ -10476,7 +10452,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>2182</v>
+        <v>2178</v>
       </c>
       <c r="B129" s="3" t="b">
         <v>1</v>
@@ -10486,13 +10462,13 @@
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3" t="s">
-        <v>2183</v>
+        <v>2179</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>2185</v>
+        <v>2181</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>2184</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -15012,7 +14988,7 @@
     </row>
     <row r="345" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
-        <v>2240</v>
+        <v>2232</v>
       </c>
       <c r="B345" s="3" t="b">
         <v>1</v>
@@ -15021,18 +14997,18 @@
         <v>1</v>
       </c>
       <c r="E345" s="3" t="s">
-        <v>2241</v>
+        <v>2233</v>
       </c>
       <c r="F345" s="6" t="s">
-        <v>2243</v>
+        <v>2235</v>
       </c>
       <c r="G345" s="3" t="s">
-        <v>2242</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="346" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
-        <v>2347</v>
+        <v>2339</v>
       </c>
       <c r="B346" s="3" t="b">
         <v>1</v>
@@ -15041,18 +15017,18 @@
         <v>1</v>
       </c>
       <c r="E346" s="3" t="s">
-        <v>2348</v>
+        <v>2340</v>
       </c>
       <c r="F346" s="6" t="s">
-        <v>2351</v>
+        <v>2343</v>
       </c>
       <c r="G346" s="3" t="s">
-        <v>2242</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="347" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
-        <v>2344</v>
+        <v>2336</v>
       </c>
       <c r="B347" s="3" t="b">
         <v>1</v>
@@ -15061,15 +15037,15 @@
         <v>1</v>
       </c>
       <c r="E347" s="3" t="s">
-        <v>2345</v>
+        <v>2337</v>
       </c>
       <c r="F347" s="6" t="s">
-        <v>2346</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="348" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="s">
-        <v>2349</v>
+        <v>2341</v>
       </c>
       <c r="B348" s="3" t="b">
         <v>1</v>
@@ -15078,10 +15054,10 @@
         <v>1</v>
       </c>
       <c r="E348" s="3" t="s">
-        <v>2350</v>
+        <v>2342</v>
       </c>
       <c r="F348" s="6" t="s">
-        <v>2352</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -16335,7 +16311,7 @@
       </c>
       <c r="D408" s="3"/>
       <c r="E408" s="3" t="s">
-        <v>2239</v>
+        <v>2231</v>
       </c>
       <c r="F408" s="6" t="s">
         <v>1196</v>
@@ -16472,7 +16448,7 @@
     </row>
     <row r="415" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A415" s="3" t="s">
-        <v>2186</v>
+        <v>2182</v>
       </c>
       <c r="B415" s="3" t="b">
         <v>1</v>
@@ -17080,7 +17056,7 @@
     </row>
     <row r="444" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A444" s="3" t="s">
-        <v>2393</v>
+        <v>2385</v>
       </c>
       <c r="B444" s="3" t="b">
         <v>1</v>
@@ -17089,18 +17065,18 @@
         <v>1</v>
       </c>
       <c r="E444" s="3" t="s">
-        <v>2393</v>
+        <v>2385</v>
       </c>
       <c r="F444" s="6" t="s">
-        <v>2395</v>
+        <v>2387</v>
       </c>
       <c r="G444" s="3" t="s">
-        <v>2397</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="445" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A445" s="3" t="s">
-        <v>2394</v>
+        <v>2386</v>
       </c>
       <c r="B445" s="3" t="b">
         <v>1</v>
@@ -17109,13 +17085,13 @@
         <v>1</v>
       </c>
       <c r="E445" s="3" t="s">
-        <v>2394</v>
+        <v>2386</v>
       </c>
       <c r="F445" s="6" t="s">
-        <v>2396</v>
+        <v>2388</v>
       </c>
       <c r="G445" s="3" t="s">
-        <v>2398</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.25">
@@ -17136,7 +17112,7 @@
         <v>1642</v>
       </c>
       <c r="G446" s="3" t="s">
-        <v>2392</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="447" spans="1:7" x14ac:dyDescent="0.25">
@@ -17351,7 +17327,7 @@
     </row>
     <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" s="3" t="s">
-        <v>2277</v>
+        <v>2269</v>
       </c>
       <c r="B457" s="3" t="b">
         <v>1</v>
@@ -17361,10 +17337,10 @@
       </c>
       <c r="D457" s="3"/>
       <c r="E457" s="3" t="s">
-        <v>2278</v>
+        <v>2270</v>
       </c>
       <c r="F457" s="6" t="s">
-        <v>2279</v>
+        <v>2271</v>
       </c>
       <c r="G457" s="3" t="s">
         <v>1721</v>
@@ -17372,7 +17348,7 @@
     </row>
     <row r="458" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">
-        <v>2280</v>
+        <v>2272</v>
       </c>
       <c r="B458" s="3" t="b">
         <v>1</v>
@@ -17381,10 +17357,10 @@
         <v>1</v>
       </c>
       <c r="E458" s="3" t="s">
-        <v>2281</v>
+        <v>2273</v>
       </c>
       <c r="F458" s="6" t="s">
-        <v>2282</v>
+        <v>2274</v>
       </c>
       <c r="G458" s="3" t="s">
         <v>1835</v>
@@ -17560,7 +17536,7 @@
     </row>
     <row r="467" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A467" s="3" t="s">
-        <v>2387</v>
+        <v>2379</v>
       </c>
       <c r="B467" s="3" t="b">
         <v>1</v>
@@ -17572,7 +17548,7 @@
         <v>623</v>
       </c>
       <c r="F467" s="6" t="s">
-        <v>2388</v>
+        <v>2380</v>
       </c>
       <c r="G467" s="3" t="s">
         <v>1426</v>
@@ -17580,7 +17556,7 @@
     </row>
     <row r="468" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A468" s="3" t="s">
-        <v>2399</v>
+        <v>2391</v>
       </c>
       <c r="B468" s="3" t="b">
         <v>1</v>
@@ -17589,10 +17565,10 @@
         <v>1</v>
       </c>
       <c r="E468" s="3" t="s">
-        <v>2405</v>
+        <v>2397</v>
       </c>
       <c r="F468" s="6" t="s">
-        <v>2416</v>
+        <v>2408</v>
       </c>
       <c r="G468" s="3" t="s">
         <v>1219</v>
@@ -17600,7 +17576,7 @@
     </row>
     <row r="469" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A469" s="3" t="s">
-        <v>2401</v>
+        <v>2393</v>
       </c>
       <c r="B469" s="3" t="b">
         <v>1</v>
@@ -17609,18 +17585,18 @@
         <v>1</v>
       </c>
       <c r="E469" s="3" t="s">
+        <v>2398</v>
+      </c>
+      <c r="F469" s="6" t="s">
         <v>2406</v>
       </c>
-      <c r="F469" s="6" t="s">
-        <v>2414</v>
-      </c>
       <c r="G469" s="3" t="s">
-        <v>2417</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="470" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A470" s="3" t="s">
-        <v>2402</v>
+        <v>2394</v>
       </c>
       <c r="B470" s="3" t="b">
         <v>1</v>
@@ -17629,18 +17605,18 @@
         <v>1</v>
       </c>
       <c r="E470" s="3" t="s">
+        <v>2399</v>
+      </c>
+      <c r="F470" s="6" t="s">
         <v>2407</v>
       </c>
-      <c r="F470" s="6" t="s">
-        <v>2415</v>
-      </c>
       <c r="G470" s="3" t="s">
-        <v>2418</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="471" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A471" s="3" t="s">
-        <v>2403</v>
+        <v>2395</v>
       </c>
       <c r="B471" s="3" t="b">
         <v>1</v>
@@ -17649,18 +17625,18 @@
         <v>1</v>
       </c>
       <c r="E471" s="3" t="s">
-        <v>2408</v>
+        <v>2400</v>
       </c>
       <c r="F471" s="6" t="s">
-        <v>2413</v>
+        <v>2405</v>
       </c>
       <c r="G471" s="3" t="s">
-        <v>2419</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="472" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A472" s="3" t="s">
-        <v>2400</v>
+        <v>2392</v>
       </c>
       <c r="B472" s="3" t="b">
         <v>1</v>
@@ -17669,18 +17645,18 @@
         <v>1</v>
       </c>
       <c r="E472" s="3" t="s">
-        <v>2409</v>
+        <v>2401</v>
       </c>
       <c r="F472" s="6" t="s">
+        <v>2404</v>
+      </c>
+      <c r="G472" s="3" t="s">
         <v>2412</v>
-      </c>
-      <c r="G472" s="3" t="s">
-        <v>2420</v>
       </c>
     </row>
     <row r="473" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A473" s="3" t="s">
-        <v>2404</v>
+        <v>2396</v>
       </c>
       <c r="B473" s="3" t="b">
         <v>1</v>
@@ -17689,18 +17665,18 @@
         <v>1</v>
       </c>
       <c r="E473" s="3" t="s">
-        <v>2411</v>
+        <v>2403</v>
       </c>
       <c r="F473" s="6" t="s">
-        <v>2410</v>
+        <v>2402</v>
       </c>
       <c r="G473" s="3" t="s">
-        <v>2421</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="474" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A474" s="3" t="s">
-        <v>2283</v>
+        <v>2275</v>
       </c>
       <c r="B474" s="3" t="b">
         <v>1</v>
@@ -17720,7 +17696,7 @@
     </row>
     <row r="475" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A475" s="3" t="s">
-        <v>2284</v>
+        <v>2276</v>
       </c>
       <c r="B475" s="3" t="b">
         <v>1</v>
@@ -17740,7 +17716,7 @@
     </row>
     <row r="476" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A476" s="3" t="s">
-        <v>2285</v>
+        <v>2277</v>
       </c>
       <c r="B476" s="3" t="b">
         <v>1</v>
@@ -17760,7 +17736,7 @@
     </row>
     <row r="477" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A477" s="3" t="s">
-        <v>2286</v>
+        <v>2278</v>
       </c>
       <c r="B477" s="3" t="b">
         <v>1</v>
@@ -17769,18 +17745,18 @@
         <v>1</v>
       </c>
       <c r="E477" s="3" t="s">
-        <v>2287</v>
+        <v>2279</v>
       </c>
       <c r="F477" s="6" t="s">
-        <v>2288</v>
+        <v>2280</v>
       </c>
       <c r="G477" s="3" t="s">
-        <v>2293</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="478" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A478" s="3" t="s">
-        <v>2265</v>
+        <v>2257</v>
       </c>
       <c r="B478" s="3" t="b">
         <v>1</v>
@@ -17801,7 +17777,7 @@
     </row>
     <row r="479" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
-        <v>2266</v>
+        <v>2258</v>
       </c>
       <c r="B479" s="3" t="b">
         <v>1</v>
@@ -17822,7 +17798,7 @@
     </row>
     <row r="480" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A480" s="3" t="s">
-        <v>2267</v>
+        <v>2259</v>
       </c>
       <c r="B480" s="3" t="b">
         <v>1</v>
@@ -17843,7 +17819,7 @@
     </row>
     <row r="481" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
-        <v>2294</v>
+        <v>2286</v>
       </c>
       <c r="B481" s="3" t="b">
         <v>1</v>
@@ -17852,18 +17828,18 @@
         <v>1</v>
       </c>
       <c r="E481" s="3" t="s">
-        <v>2295</v>
+        <v>2287</v>
       </c>
       <c r="F481" s="6" t="s">
-        <v>2296</v>
+        <v>2288</v>
       </c>
       <c r="G481" s="3" t="s">
-        <v>2297</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="482" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A482" s="3" t="s">
-        <v>2305</v>
+        <v>2297</v>
       </c>
       <c r="B482" s="3" t="b">
         <v>1</v>
@@ -17873,18 +17849,18 @@
       </c>
       <c r="D482" s="3"/>
       <c r="E482" s="3" t="s">
-        <v>2259</v>
+        <v>2251</v>
       </c>
       <c r="F482" s="6" t="s">
-        <v>2306</v>
+        <v>2298</v>
       </c>
       <c r="G482" s="3" t="s">
-        <v>2307</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="483" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A483" s="3" t="s">
-        <v>2268</v>
+        <v>2260</v>
       </c>
       <c r="B483" s="3" t="b">
         <v>1</v>
@@ -17905,7 +17881,7 @@
     </row>
     <row r="484" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A484" s="3" t="s">
-        <v>2269</v>
+        <v>2261</v>
       </c>
       <c r="B484" s="3" t="b">
         <v>1</v>
@@ -17926,7 +17902,7 @@
     </row>
     <row r="485" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A485" s="3" t="s">
-        <v>2298</v>
+        <v>2290</v>
       </c>
       <c r="B485" s="3" t="b">
         <v>1</v>
@@ -17935,18 +17911,18 @@
         <v>1</v>
       </c>
       <c r="E485" s="3" t="s">
-        <v>2299</v>
+        <v>2291</v>
       </c>
       <c r="F485" s="6" t="s">
-        <v>2302</v>
+        <v>2294</v>
       </c>
       <c r="G485" s="3" t="s">
-        <v>2333</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="486" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A486" s="3" t="s">
-        <v>2300</v>
+        <v>2292</v>
       </c>
       <c r="B486" s="3" t="b">
         <v>1</v>
@@ -17955,18 +17931,18 @@
         <v>1</v>
       </c>
       <c r="E486" s="3" t="s">
-        <v>2301</v>
+        <v>2293</v>
       </c>
       <c r="F486" s="6" t="s">
-        <v>2303</v>
+        <v>2295</v>
       </c>
       <c r="G486" s="3" t="s">
-        <v>2334</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="487" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A487" s="3" t="s">
-        <v>2270</v>
+        <v>2262</v>
       </c>
       <c r="B487" s="3" t="b">
         <v>1</v>
@@ -17987,7 +17963,7 @@
     </row>
     <row r="488" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A488" s="3" t="s">
-        <v>2304</v>
+        <v>2296</v>
       </c>
       <c r="B488" s="3" t="b">
         <v>1</v>
@@ -18007,7 +17983,7 @@
     </row>
     <row r="489" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A489" s="3" t="s">
-        <v>2308</v>
+        <v>2300</v>
       </c>
       <c r="B489" s="3" t="b">
         <v>1</v>
@@ -18016,18 +17992,18 @@
         <v>1</v>
       </c>
       <c r="E489" s="3" t="s">
-        <v>2309</v>
+        <v>2301</v>
       </c>
       <c r="F489" s="6" t="s">
-        <v>2310</v>
+        <v>2302</v>
       </c>
       <c r="G489" s="3" t="s">
-        <v>2335</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="490" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
-        <v>2271</v>
+        <v>2263</v>
       </c>
       <c r="B490" s="3" t="b">
         <v>1</v>
@@ -18048,7 +18024,7 @@
     </row>
     <row r="491" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A491" s="3" t="s">
-        <v>2272</v>
+        <v>2264</v>
       </c>
       <c r="B491" s="3" t="b">
         <v>1</v>
@@ -18069,7 +18045,7 @@
     </row>
     <row r="492" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A492" s="3" t="s">
-        <v>2273</v>
+        <v>2265</v>
       </c>
       <c r="B492" s="3" t="b">
         <v>1</v>
@@ -18090,7 +18066,7 @@
     </row>
     <row r="493" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A493" s="3" t="s">
-        <v>2274</v>
+        <v>2266</v>
       </c>
       <c r="B493" s="3" t="b">
         <v>1</v>
@@ -18111,7 +18087,7 @@
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A494" s="3" t="s">
-        <v>2275</v>
+        <v>2267</v>
       </c>
       <c r="B494" s="3" t="b">
         <v>1</v>
@@ -18132,7 +18108,7 @@
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A495" s="3" t="s">
-        <v>2276</v>
+        <v>2268</v>
       </c>
       <c r="B495" s="3" t="b">
         <v>1</v>
@@ -18153,7 +18129,7 @@
     </row>
     <row r="496" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
-        <v>2311</v>
+        <v>2303</v>
       </c>
       <c r="B496" s="3" t="b">
         <v>1</v>
@@ -18165,7 +18141,7 @@
         <v>1693</v>
       </c>
       <c r="F496" s="6" t="s">
-        <v>2325</v>
+        <v>2317</v>
       </c>
       <c r="G496" s="3" t="s">
         <v>1730</v>
@@ -18173,7 +18149,7 @@
     </row>
     <row r="497" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
-        <v>2312</v>
+        <v>2304</v>
       </c>
       <c r="B497" s="3" t="b">
         <v>1</v>
@@ -18185,7 +18161,7 @@
         <v>1694</v>
       </c>
       <c r="F497" s="6" t="s">
-        <v>2326</v>
+        <v>2318</v>
       </c>
       <c r="G497" s="3" t="s">
         <v>1731</v>
@@ -18193,7 +18169,7 @@
     </row>
     <row r="498" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
-        <v>2313</v>
+        <v>2305</v>
       </c>
       <c r="B498" s="3" t="b">
         <v>1</v>
@@ -18202,38 +18178,38 @@
         <v>1</v>
       </c>
       <c r="E498" s="3" t="s">
+        <v>2311</v>
+      </c>
+      <c r="F498" s="6" t="s">
         <v>2319</v>
       </c>
-      <c r="F498" s="6" t="s">
-        <v>2327</v>
-      </c>
       <c r="G498" s="3" t="s">
-        <v>2336</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="499" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B499" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C499" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E499" s="3" t="s">
         <v>2314</v>
       </c>
-      <c r="B499" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C499" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E499" s="3" t="s">
-        <v>2322</v>
-      </c>
       <c r="F499" s="6" t="s">
-        <v>2328</v>
+        <v>2320</v>
       </c>
       <c r="G499" s="3" t="s">
-        <v>2337</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="500" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
-        <v>2315</v>
+        <v>2307</v>
       </c>
       <c r="B500" s="3" t="b">
         <v>1</v>
@@ -18242,18 +18218,18 @@
         <v>1</v>
       </c>
       <c r="E500" s="3" t="s">
-        <v>2320</v>
+        <v>2312</v>
       </c>
       <c r="F500" s="6" t="s">
-        <v>2329</v>
+        <v>2321</v>
       </c>
       <c r="G500" s="3" t="s">
-        <v>2338</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="501" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A501" s="3" t="s">
-        <v>2316</v>
+        <v>2308</v>
       </c>
       <c r="B501" s="3" t="b">
         <v>1</v>
@@ -18262,18 +18238,18 @@
         <v>1</v>
       </c>
       <c r="E501" s="3" t="s">
-        <v>2321</v>
+        <v>2313</v>
       </c>
       <c r="F501" s="6" t="s">
-        <v>2330</v>
+        <v>2322</v>
       </c>
       <c r="G501" s="3" t="s">
-        <v>2339</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="502" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A502" s="3" t="s">
-        <v>2317</v>
+        <v>2309</v>
       </c>
       <c r="B502" s="3" t="b">
         <v>1</v>
@@ -18282,18 +18258,18 @@
         <v>1</v>
       </c>
       <c r="E502" s="3" t="s">
+        <v>2315</v>
+      </c>
+      <c r="F502" s="6" t="s">
         <v>2323</v>
       </c>
-      <c r="F502" s="6" t="s">
-        <v>2331</v>
-      </c>
       <c r="G502" s="3" t="s">
-        <v>2340</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="503" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A503" s="3" t="s">
-        <v>2318</v>
+        <v>2310</v>
       </c>
       <c r="B503" s="3" t="b">
         <v>1</v>
@@ -18302,18 +18278,18 @@
         <v>1</v>
       </c>
       <c r="E503" s="3" t="s">
+        <v>2316</v>
+      </c>
+      <c r="F503" s="6" t="s">
         <v>2324</v>
       </c>
-      <c r="F503" s="6" t="s">
-        <v>2332</v>
-      </c>
       <c r="G503" s="3" t="s">
-        <v>2341</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="504" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A504" s="3" t="s">
-        <v>2289</v>
+        <v>2281</v>
       </c>
       <c r="B504" s="3" t="b">
         <v>1</v>
@@ -18322,13 +18298,13 @@
         <v>1</v>
       </c>
       <c r="E504" s="3" t="s">
-        <v>2290</v>
+        <v>2282</v>
       </c>
       <c r="F504" s="6" t="s">
-        <v>2291</v>
+        <v>2283</v>
       </c>
       <c r="G504" s="3" t="s">
-        <v>2292</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="505" spans="1:7" x14ac:dyDescent="0.25">
@@ -18625,7 +18601,7 @@
     </row>
     <row r="519" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A519" s="3" t="s">
-        <v>2187</v>
+        <v>2183</v>
       </c>
       <c r="B519" s="3" t="b">
         <v>1</v>
@@ -18813,7 +18789,7 @@
     </row>
     <row r="528" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A528" s="3" t="s">
-        <v>2244</v>
+        <v>2236</v>
       </c>
       <c r="B528" s="3" t="b">
         <v>1</v>
@@ -18822,13 +18798,13 @@
         <v>1</v>
       </c>
       <c r="E528" s="3" t="s">
-        <v>2245</v>
+        <v>2237</v>
       </c>
       <c r="F528" s="6" t="s">
-        <v>2246</v>
+        <v>2238</v>
       </c>
       <c r="G528" s="3" t="s">
-        <v>2247</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="529" spans="1:7" x14ac:dyDescent="0.25">
@@ -18854,7 +18830,7 @@
     </row>
     <row r="530" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A530" s="3" t="s">
-        <v>2360</v>
+        <v>2352</v>
       </c>
       <c r="B530" s="3" t="b">
         <v>1</v>
@@ -20710,7 +20686,7 @@
     </row>
     <row r="622" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A622" s="3" t="s">
-        <v>2142</v>
+        <v>2140</v>
       </c>
       <c r="B622" s="3" t="b">
         <v>1</v>
@@ -20722,7 +20698,7 @@
         <v>1698</v>
       </c>
       <c r="F622" s="6" t="s">
-        <v>2145</v>
+        <v>2143</v>
       </c>
       <c r="G622" s="3" t="s">
         <v>1733</v>
@@ -20730,7 +20706,7 @@
     </row>
     <row r="623" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A623" s="3" t="s">
-        <v>2143</v>
+        <v>2141</v>
       </c>
       <c r="B623" s="3" t="b">
         <v>1</v>
@@ -20739,10 +20715,10 @@
         <v>1</v>
       </c>
       <c r="E623" s="3" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F623" s="6" t="s">
         <v>2144</v>
-      </c>
-      <c r="F623" s="6" t="s">
-        <v>2146</v>
       </c>
       <c r="G623" s="3" t="s">
         <v>1733</v>
@@ -20759,18 +20735,18 @@
         <v>1</v>
       </c>
       <c r="E624" t="s">
-        <v>2140</v>
+        <v>2138</v>
       </c>
       <c r="F624" s="6" t="s">
-        <v>2141</v>
+        <v>2139</v>
       </c>
       <c r="G624" t="s">
-        <v>2163</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="625" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A625" s="3" t="s">
-        <v>2151</v>
+        <v>2148</v>
       </c>
       <c r="B625" s="3" t="b">
         <v>1</v>
@@ -20779,18 +20755,18 @@
         <v>1</v>
       </c>
       <c r="E625" s="3" t="s">
-        <v>2155</v>
+        <v>2152</v>
       </c>
       <c r="F625" s="6" t="s">
-        <v>2159</v>
+        <v>2156</v>
       </c>
       <c r="G625" s="3" t="s">
-        <v>2164</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="626" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A626" s="3" t="s">
-        <v>2152</v>
+        <v>2149</v>
       </c>
       <c r="B626" s="3" t="b">
         <v>1</v>
@@ -20799,18 +20775,18 @@
         <v>1</v>
       </c>
       <c r="E626" s="3" t="s">
-        <v>2156</v>
+        <v>2153</v>
       </c>
       <c r="F626" s="6" t="s">
-        <v>2160</v>
+        <v>2157</v>
       </c>
       <c r="G626" s="3" t="s">
-        <v>2165</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="627" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A627" s="3" t="s">
-        <v>2153</v>
+        <v>2150</v>
       </c>
       <c r="B627" s="3" t="b">
         <v>1</v>
@@ -20819,18 +20795,18 @@
         <v>1</v>
       </c>
       <c r="E627" s="3" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="F627" s="6" t="s">
-        <v>2161</v>
+        <v>2158</v>
       </c>
       <c r="G627" s="3" t="s">
-        <v>2166</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="628" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A628" s="3" t="s">
-        <v>2154</v>
+        <v>2151</v>
       </c>
       <c r="B628" s="3" t="b">
         <v>1</v>
@@ -20839,18 +20815,18 @@
         <v>1</v>
       </c>
       <c r="E628" s="3" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="F628" s="6" t="s">
-        <v>2162</v>
+        <v>2159</v>
       </c>
       <c r="G628" s="3" t="s">
-        <v>2167</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="629" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>2138</v>
+        <v>2145</v>
       </c>
       <c r="B629" t="b">
         <v>1</v>
@@ -20859,78 +20835,78 @@
         <v>1</v>
       </c>
       <c r="E629" t="s">
-        <v>2139</v>
+        <v>2146</v>
       </c>
       <c r="F629" s="6" t="s">
         <v>2147</v>
       </c>
       <c r="G629" t="s">
-        <v>2168</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="630" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>2148</v>
+        <v>2166</v>
       </c>
       <c r="B630" t="b">
         <v>1</v>
       </c>
-      <c r="C630" t="b">
+      <c r="C630" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E630" t="s">
-        <v>2149</v>
+        <v>2169</v>
       </c>
       <c r="F630" s="6" t="s">
-        <v>2150</v>
+        <v>2172</v>
       </c>
       <c r="G630" t="s">
-        <v>2169</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="631" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
+        <v>2167</v>
+      </c>
+      <c r="B631" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C631" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E631" t="s">
         <v>2170</v>
       </c>
-      <c r="B631" t="b">
-        <v>1</v>
-      </c>
-      <c r="C631" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E631" t="s">
+      <c r="F631" s="6" t="s">
         <v>2173</v>
       </c>
-      <c r="F631" s="6" t="s">
+      <c r="G631" t="s">
         <v>2176</v>
-      </c>
-      <c r="G631" t="s">
-        <v>2179</v>
       </c>
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B632" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C632" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E632" t="s">
         <v>2171</v>
       </c>
-      <c r="B632" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C632" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E632" t="s">
+      <c r="F632" s="6" t="s">
         <v>2174</v>
       </c>
-      <c r="F632" s="6" t="s">
+      <c r="G632" t="s">
         <v>2177</v>
-      </c>
-      <c r="G632" t="s">
-        <v>2180</v>
       </c>
     </row>
     <row r="633" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>2172</v>
+        <v>2184</v>
       </c>
       <c r="B633" s="3" t="b">
         <v>1</v>
@@ -20939,13 +20915,13 @@
         <v>1</v>
       </c>
       <c r="E633" t="s">
-        <v>2175</v>
+        <v>2185</v>
       </c>
       <c r="F633" s="6" t="s">
-        <v>2178</v>
+        <v>2186</v>
       </c>
       <c r="G633" t="s">
-        <v>2181</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="634" spans="1:7" x14ac:dyDescent="0.25">
@@ -20959,98 +20935,98 @@
         <v>1</v>
       </c>
       <c r="E634" t="s">
-        <v>2189</v>
+        <v>2194</v>
       </c>
       <c r="F634" s="6" t="s">
-        <v>2190</v>
+        <v>2200</v>
       </c>
       <c r="G634" t="s">
-        <v>2191</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>2192</v>
-      </c>
-      <c r="B635" t="b">
-        <v>1</v>
-      </c>
-      <c r="C635" t="b">
+        <v>2189</v>
+      </c>
+      <c r="B635" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C635" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E635" t="s">
-        <v>2193</v>
+        <v>2198</v>
       </c>
       <c r="F635" s="6" t="s">
-        <v>2194</v>
+        <v>2201</v>
       </c>
       <c r="G635" t="s">
-        <v>2213</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="636" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
+        <v>2190</v>
+      </c>
+      <c r="B636" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C636" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E636" s="3" t="s">
         <v>2195</v>
       </c>
-      <c r="B636" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C636" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E636" t="s">
-        <v>2201</v>
-      </c>
       <c r="F636" s="6" t="s">
-        <v>2207</v>
+        <v>2202</v>
       </c>
       <c r="G636" t="s">
-        <v>2214</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="637" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
+        <v>2191</v>
+      </c>
+      <c r="B637" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C637" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E637" s="3" t="s">
         <v>2196</v>
       </c>
-      <c r="B637" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C637" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E637" t="s">
-        <v>2205</v>
-      </c>
       <c r="F637" s="6" t="s">
-        <v>2208</v>
+        <v>2203</v>
       </c>
       <c r="G637" t="s">
-        <v>2215</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="638" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B638" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C638" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E638" s="3" t="s">
         <v>2197</v>
       </c>
-      <c r="B638" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C638" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E638" s="3" t="s">
-        <v>2202</v>
-      </c>
       <c r="F638" s="6" t="s">
-        <v>2209</v>
+        <v>2204</v>
       </c>
       <c r="G638" t="s">
-        <v>2216</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="639" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>2198</v>
+        <v>2193</v>
       </c>
       <c r="B639" s="3" t="b">
         <v>1</v>
@@ -21059,18 +21035,18 @@
         <v>1</v>
       </c>
       <c r="E639" s="3" t="s">
-        <v>2203</v>
+        <v>2199</v>
       </c>
       <c r="F639" s="6" t="s">
-        <v>2210</v>
+        <v>2205</v>
       </c>
       <c r="G639" t="s">
-        <v>2217</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="640" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A640" t="s">
-        <v>2199</v>
+      <c r="A640" s="3" t="s">
+        <v>1697</v>
       </c>
       <c r="B640" s="3" t="b">
         <v>1</v>
@@ -21078,19 +21054,20 @@
       <c r="C640" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D640" s="3"/>
       <c r="E640" s="3" t="s">
-        <v>2204</v>
+        <v>1697</v>
       </c>
       <c r="F640" s="6" t="s">
-        <v>2211</v>
-      </c>
-      <c r="G640" t="s">
-        <v>2218</v>
+        <v>2024</v>
+      </c>
+      <c r="G640" s="3" t="s">
+        <v>1734</v>
       </c>
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A641" t="s">
-        <v>2200</v>
+      <c r="A641" s="3" t="s">
+        <v>2022</v>
       </c>
       <c r="B641" s="3" t="b">
         <v>1</v>
@@ -21098,19 +21075,20 @@
       <c r="C641" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D641" s="3"/>
       <c r="E641" s="3" t="s">
-        <v>2206</v>
+        <v>2022</v>
       </c>
       <c r="F641" s="6" t="s">
-        <v>2212</v>
-      </c>
-      <c r="G641" t="s">
-        <v>2219</v>
+        <v>2023</v>
+      </c>
+      <c r="G641" s="3" t="s">
+        <v>1734</v>
       </c>
     </row>
     <row r="642" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A642" s="3" t="s">
-        <v>1697</v>
+        <v>814</v>
       </c>
       <c r="B642" s="3" t="b">
         <v>1</v>
@@ -21120,18 +21098,18 @@
       </c>
       <c r="D642" s="3"/>
       <c r="E642" s="3" t="s">
-        <v>1697</v>
+        <v>815</v>
       </c>
       <c r="F642" s="6" t="s">
-        <v>2024</v>
+        <v>437</v>
       </c>
       <c r="G642" s="3" t="s">
-        <v>1734</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A643" s="3" t="s">
-        <v>2022</v>
+        <v>827</v>
       </c>
       <c r="B643" s="3" t="b">
         <v>1</v>
@@ -21141,18 +21119,18 @@
       </c>
       <c r="D643" s="3"/>
       <c r="E643" s="3" t="s">
-        <v>2022</v>
+        <v>829</v>
       </c>
       <c r="F643" s="6" t="s">
-        <v>2023</v>
+        <v>828</v>
       </c>
       <c r="G643" s="3" t="s">
-        <v>1734</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A644" s="3" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B644" s="3" t="b">
         <v>1</v>
@@ -21162,18 +21140,18 @@
       </c>
       <c r="D644" s="3"/>
       <c r="E644" s="3" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="F644" s="6" t="s">
-        <v>437</v>
+        <v>817</v>
       </c>
       <c r="G644" s="3" t="s">
-        <v>1488</v>
-      </c>
-    </row>
-    <row r="645" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="645" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A645" s="3" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
       <c r="B645" s="3" t="b">
         <v>1</v>
@@ -21181,20 +21159,19 @@
       <c r="C645" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D645" s="3"/>
       <c r="E645" s="3" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
       <c r="F645" s="6" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
       <c r="G645" s="3" t="s">
-        <v>1492</v>
-      </c>
-    </row>
-    <row r="646" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="646" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A646" s="3" t="s">
-        <v>816</v>
+        <v>2128</v>
       </c>
       <c r="B646" s="3" t="b">
         <v>1</v>
@@ -21202,20 +21179,19 @@
       <c r="C646" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D646" s="3"/>
       <c r="E646" s="3" t="s">
-        <v>807</v>
+        <v>1680</v>
       </c>
       <c r="F646" s="6" t="s">
-        <v>817</v>
+        <v>830</v>
       </c>
       <c r="G646" s="3" t="s">
-        <v>1486</v>
-      </c>
-    </row>
-    <row r="647" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="647" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A647" s="3" t="s">
-        <v>818</v>
+        <v>2129</v>
       </c>
       <c r="B647" s="3" t="b">
         <v>1</v>
@@ -21223,19 +21199,20 @@
       <c r="C647" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D647" s="3"/>
       <c r="E647" s="3" t="s">
-        <v>820</v>
+        <v>1681</v>
       </c>
       <c r="F647" s="6" t="s">
-        <v>819</v>
+        <v>831</v>
       </c>
       <c r="G647" s="3" t="s">
-        <v>1489</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="648" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A648" s="3" t="s">
-        <v>2128</v>
+        <v>2130</v>
       </c>
       <c r="B648" s="3" t="b">
         <v>1</v>
@@ -21244,18 +21221,18 @@
         <v>1</v>
       </c>
       <c r="E648" s="3" t="s">
-        <v>1680</v>
+        <v>1682</v>
       </c>
       <c r="F648" s="6" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="G648" s="3" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="649" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="649" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A649" s="3" t="s">
-        <v>2129</v>
+        <v>2131</v>
       </c>
       <c r="B649" s="3" t="b">
         <v>1</v>
@@ -21263,20 +21240,19 @@
       <c r="C649" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D649" s="3"/>
       <c r="E649" s="3" t="s">
-        <v>1681</v>
+        <v>1683</v>
       </c>
       <c r="F649" s="6" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="G649" s="3" t="s">
-        <v>1494</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="650" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A650" s="3" t="s">
-        <v>2130</v>
+        <v>2132</v>
       </c>
       <c r="B650" s="3" t="b">
         <v>1</v>
@@ -21285,18 +21261,18 @@
         <v>1</v>
       </c>
       <c r="E650" s="3" t="s">
-        <v>1682</v>
+        <v>2133</v>
       </c>
       <c r="F650" s="6" t="s">
-        <v>832</v>
+        <v>2134</v>
       </c>
       <c r="G650" s="3" t="s">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="651" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="651" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A651" s="3" t="s">
-        <v>2131</v>
+        <v>824</v>
       </c>
       <c r="B651" s="3" t="b">
         <v>1</v>
@@ -21304,19 +21280,20 @@
       <c r="C651" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D651" s="3"/>
       <c r="E651" s="3" t="s">
-        <v>1683</v>
+        <v>826</v>
       </c>
       <c r="F651" s="6" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="G651" s="3" t="s">
-        <v>1496</v>
-      </c>
-    </row>
-    <row r="652" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="652" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A652" s="3" t="s">
-        <v>2132</v>
+        <v>821</v>
       </c>
       <c r="B652" s="3" t="b">
         <v>1</v>
@@ -21324,19 +21301,20 @@
       <c r="C652" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D652" s="3"/>
       <c r="E652" s="3" t="s">
-        <v>2133</v>
+        <v>823</v>
       </c>
       <c r="F652" s="6" t="s">
-        <v>2134</v>
+        <v>822</v>
       </c>
       <c r="G652" s="3" t="s">
-        <v>2135</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A653" s="3" t="s">
-        <v>824</v>
+      <c r="A653" t="s">
+        <v>2212</v>
       </c>
       <c r="B653" s="3" t="b">
         <v>1</v>
@@ -21344,20 +21322,19 @@
       <c r="C653" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D653" s="3"/>
-      <c r="E653" s="3" t="s">
-        <v>826</v>
+      <c r="E653" t="s">
+        <v>1699</v>
       </c>
       <c r="F653" s="6" t="s">
-        <v>825</v>
-      </c>
-      <c r="G653" s="3" t="s">
-        <v>1491</v>
+        <v>2217</v>
+      </c>
+      <c r="G653" t="s">
+        <v>1735</v>
       </c>
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A654" s="3" t="s">
-        <v>821</v>
+      <c r="A654" t="s">
+        <v>2213</v>
       </c>
       <c r="B654" s="3" t="b">
         <v>1</v>
@@ -21365,20 +21342,19 @@
       <c r="C654" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D654" s="3"/>
       <c r="E654" s="3" t="s">
-        <v>823</v>
+        <v>420</v>
       </c>
       <c r="F654" s="6" t="s">
-        <v>822</v>
-      </c>
-      <c r="G654" s="3" t="s">
-        <v>1490</v>
+        <v>1707</v>
+      </c>
+      <c r="G654" t="s">
+        <v>1355</v>
       </c>
     </row>
     <row r="655" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A655" t="s">
-        <v>2220</v>
+      <c r="A655" s="3" t="s">
+        <v>2214</v>
       </c>
       <c r="B655" s="3" t="b">
         <v>1</v>
@@ -21386,485 +21362,488 @@
       <c r="C655" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E655" t="s">
-        <v>1699</v>
+      <c r="E655" s="3" t="s">
+        <v>426</v>
       </c>
       <c r="F655" s="6" t="s">
+        <v>2218</v>
+      </c>
+      <c r="G655" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="656" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A656" s="3" t="s">
+        <v>2215</v>
+      </c>
+      <c r="B656" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C656" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E656" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="F656" s="6" t="s">
+        <v>1705</v>
+      </c>
+      <c r="G656" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="657" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B657" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C657" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E657" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F657" s="6" t="s">
+        <v>1706</v>
+      </c>
+      <c r="G657" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="658" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A658" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B658" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C658" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E658" t="s">
+        <v>2221</v>
+      </c>
+      <c r="F658" s="6" t="s">
+        <v>2223</v>
+      </c>
+      <c r="G658" t="s">
         <v>2225</v>
-      </c>
-      <c r="G655" t="s">
-        <v>1735</v>
-      </c>
-    </row>
-    <row r="656" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A656" t="s">
-        <v>2221</v>
-      </c>
-      <c r="B656" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C656" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E656" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="F656" s="6" t="s">
-        <v>1707</v>
-      </c>
-      <c r="G656" t="s">
-        <v>1355</v>
-      </c>
-    </row>
-    <row r="657" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A657" s="3" t="s">
-        <v>2222</v>
-      </c>
-      <c r="B657" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C657" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E657" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="F657" s="6" t="s">
-        <v>2226</v>
-      </c>
-      <c r="G657" t="s">
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="658" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A658" s="3" t="s">
-        <v>2223</v>
-      </c>
-      <c r="B658" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C658" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E658" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="F658" s="6" t="s">
-        <v>1705</v>
-      </c>
-      <c r="G658" t="s">
-        <v>1362</v>
       </c>
     </row>
     <row r="659" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B659" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C659" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E659" t="s">
+        <v>2222</v>
+      </c>
+      <c r="F659" s="6" t="s">
         <v>2224</v>
       </c>
-      <c r="B659" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C659" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E659" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="F659" s="6" t="s">
-        <v>1706</v>
-      </c>
       <c r="G659" t="s">
-        <v>1359</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="660" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
         <v>2227</v>
       </c>
-      <c r="B660" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C660" s="3" t="b">
+      <c r="B660" t="b">
+        <v>1</v>
+      </c>
+      <c r="C660" t="b">
         <v>1</v>
       </c>
       <c r="E660" t="s">
+        <v>2228</v>
+      </c>
+      <c r="F660" s="6" t="s">
         <v>2229</v>
       </c>
-      <c r="F660" s="6" t="s">
-        <v>2231</v>
-      </c>
       <c r="G660" t="s">
-        <v>2233</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="661" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>2228</v>
-      </c>
-      <c r="B661" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C661" s="3" t="b">
+        <v>2003</v>
+      </c>
+      <c r="B661" t="b">
+        <v>1</v>
+      </c>
+      <c r="C661" t="b">
         <v>1</v>
       </c>
       <c r="E661" t="s">
-        <v>2230</v>
+        <v>2003</v>
       </c>
       <c r="F661" s="6" t="s">
-        <v>2232</v>
-      </c>
-      <c r="G661" t="s">
-        <v>2234</v>
+        <v>2004</v>
+      </c>
+      <c r="G661" s="3" t="s">
+        <v>2005</v>
       </c>
     </row>
     <row r="662" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>2235</v>
+        <v>2240</v>
       </c>
       <c r="B662" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C662" t="b">
         <v>1</v>
       </c>
+      <c r="D662" t="s">
+        <v>2245</v>
+      </c>
       <c r="E662" t="s">
-        <v>2236</v>
+        <v>2240</v>
       </c>
       <c r="F662" s="6" t="s">
-        <v>2237</v>
+        <v>2243</v>
       </c>
       <c r="G662" t="s">
-        <v>2238</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="663" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>2003</v>
+        <v>2241</v>
       </c>
       <c r="B663" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C663" t="b">
         <v>1</v>
       </c>
+      <c r="D663" t="s">
+        <v>2245</v>
+      </c>
       <c r="E663" t="s">
-        <v>2003</v>
+        <v>2242</v>
       </c>
       <c r="F663" s="6" t="s">
-        <v>2004</v>
-      </c>
-      <c r="G663" s="3" t="s">
-        <v>2005</v>
+        <v>2244</v>
+      </c>
+      <c r="G663" t="s">
+        <v>2247</v>
       </c>
     </row>
     <row r="664" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
+        <v>2253</v>
+      </c>
+      <c r="B664" t="b">
+        <v>1</v>
+      </c>
+      <c r="C664" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E664" t="s">
+        <v>2251</v>
+      </c>
+      <c r="F664" s="6" t="s">
+        <v>2255</v>
+      </c>
+      <c r="G664" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="665" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A665" s="3" t="s">
         <v>2248</v>
       </c>
-      <c r="B664" t="b">
-        <v>0</v>
-      </c>
-      <c r="C664" t="b">
-        <v>1</v>
-      </c>
-      <c r="D664" t="s">
-        <v>2253</v>
-      </c>
-      <c r="E664" t="s">
-        <v>2248</v>
-      </c>
-      <c r="F664" s="6" t="s">
-        <v>2251</v>
-      </c>
-      <c r="G664" t="s">
+      <c r="B665" t="b">
+        <v>1</v>
+      </c>
+      <c r="C665" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E665" t="s">
+        <v>2252</v>
+      </c>
+      <c r="F665" s="6" t="s">
         <v>2254</v>
       </c>
-    </row>
-    <row r="665" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A665" t="s">
+      <c r="G665" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="666" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A666" s="3" t="s">
         <v>2249</v>
       </c>
-      <c r="B665" t="b">
-        <v>0</v>
-      </c>
-      <c r="C665" t="b">
-        <v>1</v>
-      </c>
-      <c r="D665" t="s">
-        <v>2253</v>
-      </c>
-      <c r="E665" t="s">
+      <c r="B666" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C666" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E666" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="F666" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G666" s="3" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="667" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A667" s="3" t="s">
         <v>2250</v>
       </c>
-      <c r="F665" s="6" t="s">
-        <v>2252</v>
-      </c>
-      <c r="G665" t="s">
-        <v>2255</v>
-      </c>
-    </row>
-    <row r="666" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A666" t="s">
-        <v>2261</v>
-      </c>
-      <c r="B666" t="b">
-        <v>1</v>
-      </c>
-      <c r="C666" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E666" t="s">
-        <v>2259</v>
-      </c>
-      <c r="F666" s="6" t="s">
-        <v>2263</v>
-      </c>
-      <c r="G666" t="s">
-        <v>2264</v>
-      </c>
-    </row>
-    <row r="667" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A667" s="3" t="s">
-        <v>2256</v>
-      </c>
-      <c r="B667" t="b">
+      <c r="B667" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C667" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E667" t="s">
-        <v>2260</v>
+      <c r="E667" s="3" t="s">
+        <v>327</v>
       </c>
       <c r="F667" s="6" t="s">
-        <v>2262</v>
-      </c>
-      <c r="G667" t="s">
-        <v>2264</v>
-      </c>
-    </row>
-    <row r="668" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A668" s="3" t="s">
-        <v>2257</v>
-      </c>
-      <c r="B668" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C668" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E668" s="3" t="s">
-        <v>324</v>
+        <v>326</v>
+      </c>
+      <c r="G667" s="3" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="668" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A668" t="s">
+        <v>2345</v>
+      </c>
+      <c r="B668" t="b">
+        <v>1</v>
+      </c>
+      <c r="C668" t="b">
+        <v>1</v>
+      </c>
+      <c r="E668" t="s">
+        <v>2334</v>
       </c>
       <c r="F668" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="G668" s="3" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="669" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A669" s="3" t="s">
-        <v>2258</v>
-      </c>
-      <c r="B669" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C669" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E669" s="3" t="s">
-        <v>327</v>
+        <v>2335</v>
+      </c>
+      <c r="G668" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="669" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A669" t="s">
+        <v>2347</v>
+      </c>
+      <c r="B669" t="b">
+        <v>1</v>
+      </c>
+      <c r="C669" t="b">
+        <v>0</v>
+      </c>
+      <c r="E669" t="s">
+        <v>2346</v>
       </c>
       <c r="F669" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="G669" s="3" t="s">
-        <v>1323</v>
+        <v>2348</v>
+      </c>
+      <c r="G669" t="s">
+        <v>2358</v>
       </c>
     </row>
     <row r="670" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>2353</v>
+        <v>2351</v>
       </c>
       <c r="B670" t="b">
         <v>1</v>
       </c>
       <c r="C670" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E670" t="s">
-        <v>2342</v>
+        <v>2349</v>
       </c>
       <c r="F670" s="6" t="s">
-        <v>2343</v>
+        <v>2350</v>
       </c>
       <c r="G670" t="s">
-        <v>2365</v>
-      </c>
-    </row>
-    <row r="671" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A671" t="s">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="671" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A671" s="3" t="s">
+        <v>2354</v>
+      </c>
+      <c r="B671" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C671" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E671" s="3" t="s">
         <v>2355</v>
-      </c>
-      <c r="B671" t="b">
-        <v>1</v>
-      </c>
-      <c r="C671" t="b">
-        <v>0</v>
-      </c>
-      <c r="E671" t="s">
-        <v>2354</v>
       </c>
       <c r="F671" s="6" t="s">
         <v>2356</v>
       </c>
-      <c r="G671" t="s">
-        <v>2366</v>
+      <c r="G671" s="3" t="s">
+        <v>2360</v>
       </c>
     </row>
     <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>2359</v>
+        <v>2361</v>
       </c>
       <c r="B672" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C672" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E672" t="s">
-        <v>2357</v>
+        <v>2364</v>
       </c>
       <c r="F672" s="6" t="s">
-        <v>2358</v>
+        <v>2365</v>
       </c>
       <c r="G672" t="s">
-        <v>2367</v>
-      </c>
-    </row>
-    <row r="673" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A673" s="3" t="s">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="673" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A673" t="s">
         <v>2362</v>
       </c>
-      <c r="B673" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C673" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E673" s="3" t="s">
+      <c r="B673" t="b">
+        <v>0</v>
+      </c>
+      <c r="C673" t="b">
+        <v>1</v>
+      </c>
+      <c r="E673" t="s">
         <v>2363</v>
       </c>
       <c r="F673" s="6" t="s">
-        <v>2364</v>
-      </c>
-      <c r="G673" s="3" t="s">
-        <v>2368</v>
+        <v>2366</v>
+      </c>
+      <c r="G673" t="s">
+        <v>2376</v>
       </c>
     </row>
     <row r="674" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="B674" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C674" t="b">
         <v>1</v>
       </c>
       <c r="E674" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="F674" s="6" t="s">
-        <v>2373</v>
+        <v>2374</v>
       </c>
       <c r="G674" t="s">
-        <v>2383</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>2370</v>
-      </c>
-      <c r="B675" t="b">
-        <v>0</v>
-      </c>
-      <c r="C675" t="b">
+        <v>2369</v>
+      </c>
+      <c r="B675" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C675" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E675" t="s">
-        <v>2371</v>
+        <v>497</v>
       </c>
       <c r="F675" s="6" t="s">
-        <v>2374</v>
+        <v>496</v>
       </c>
       <c r="G675" t="s">
-        <v>2384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="676" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>2376</v>
-      </c>
-      <c r="B676" t="b">
-        <v>1</v>
-      </c>
-      <c r="C676" t="b">
+        <v>2370</v>
+      </c>
+      <c r="B676" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C676" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E676" t="s">
-        <v>2379</v>
+        <v>2372</v>
       </c>
       <c r="F676" s="6" t="s">
-        <v>2382</v>
+        <v>2373</v>
       </c>
       <c r="G676" t="s">
-        <v>2385</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>2377</v>
-      </c>
-      <c r="B677" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C677" s="3" t="b">
-        <v>1</v>
+        <v>2381</v>
+      </c>
+      <c r="B677" t="b">
+        <v>0</v>
+      </c>
+      <c r="C677" t="b">
+        <v>1</v>
+      </c>
+      <c r="D677" t="s">
+        <v>2382</v>
       </c>
       <c r="E677" t="s">
-        <v>497</v>
+        <v>2384</v>
       </c>
       <c r="F677" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G677" t="s">
-        <v>1383</v>
+        <v>2383</v>
+      </c>
+      <c r="G677" s="3" t="s">
+        <v>2389</v>
       </c>
     </row>
     <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>2378</v>
-      </c>
-      <c r="B678" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C678" s="3" t="b">
+        <v>2414</v>
+      </c>
+      <c r="B678" t="b">
+        <v>0</v>
+      </c>
+      <c r="C678" t="b">
         <v>1</v>
       </c>
       <c r="E678" t="s">
-        <v>2380</v>
+        <v>2415</v>
       </c>
       <c r="F678" s="6" t="s">
-        <v>2381</v>
+        <v>2430</v>
       </c>
       <c r="G678" t="s">
-        <v>2386</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="679" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>2389</v>
+        <v>2416</v>
       </c>
       <c r="B679" t="b">
         <v>0</v>
@@ -21872,121 +21851,78 @@
       <c r="C679" t="b">
         <v>1</v>
       </c>
-      <c r="D679" t="s">
-        <v>2390</v>
-      </c>
       <c r="E679" t="s">
-        <v>2392</v>
+        <v>2433</v>
       </c>
       <c r="F679" s="6" t="s">
-        <v>2391</v>
-      </c>
-      <c r="G679" s="3" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="680" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A680" t="s">
+        <v>2419</v>
+      </c>
+      <c r="G679" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="680" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A680" s="3" t="s">
         <v>2422</v>
       </c>
-      <c r="B680" t="b">
-        <v>0</v>
-      </c>
-      <c r="C680" t="b">
-        <v>1</v>
-      </c>
-      <c r="E680" t="s">
+      <c r="B680" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C680" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E680" s="3" t="s">
+        <v>2431</v>
+      </c>
+      <c r="F680" s="6" t="s">
         <v>2423</v>
       </c>
-      <c r="F680" s="6" t="s">
-        <v>2438</v>
-      </c>
-      <c r="G680" t="s">
-        <v>2433</v>
+      <c r="G680" s="3" t="s">
+        <v>2427</v>
       </c>
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
+        <v>2417</v>
+      </c>
+      <c r="B681" t="b">
+        <v>0</v>
+      </c>
+      <c r="C681" t="b">
+        <v>1</v>
+      </c>
+      <c r="E681" t="s">
+        <v>2432</v>
+      </c>
+      <c r="F681" s="6" t="s">
+        <v>2418</v>
+      </c>
+      <c r="G681" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="682" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A682" t="s">
+        <v>2421</v>
+      </c>
+      <c r="B682" t="b">
+        <v>0</v>
+      </c>
+      <c r="C682" t="b">
+        <v>1</v>
+      </c>
+      <c r="E682" t="s">
+        <v>2420</v>
+      </c>
+      <c r="F682" s="6" t="s">
         <v>2424</v>
       </c>
-      <c r="B681" t="b">
-        <v>0</v>
-      </c>
-      <c r="C681" t="b">
-        <v>1</v>
-      </c>
-      <c r="E681" t="s">
-        <v>2441</v>
-      </c>
-      <c r="F681" s="6" t="s">
-        <v>2427</v>
-      </c>
-      <c r="G681" t="s">
-        <v>2434</v>
-      </c>
-    </row>
-    <row r="682" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A682" s="3" t="s">
-        <v>2430</v>
-      </c>
-      <c r="B682" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C682" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E682" s="3" t="s">
-        <v>2439</v>
-      </c>
-      <c r="F682" s="6" t="s">
-        <v>2431</v>
-      </c>
-      <c r="G682" s="3" t="s">
-        <v>2435</v>
-      </c>
-    </row>
-    <row r="683" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A683" t="s">
-        <v>2425</v>
-      </c>
-      <c r="B683" t="b">
-        <v>0</v>
-      </c>
-      <c r="C683" t="b">
-        <v>1</v>
-      </c>
-      <c r="E683" t="s">
-        <v>2440</v>
-      </c>
-      <c r="F683" s="6" t="s">
-        <v>2426</v>
-      </c>
-      <c r="G683" t="s">
-        <v>2436</v>
-      </c>
-    </row>
-    <row r="684" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A684" t="s">
+      <c r="G682" t="s">
         <v>2429</v>
       </c>
-      <c r="B684" t="b">
-        <v>0</v>
-      </c>
-      <c r="C684" t="b">
-        <v>1</v>
-      </c>
-      <c r="E684" t="s">
-        <v>2428</v>
-      </c>
-      <c r="F684" s="6" t="s">
-        <v>2432</v>
-      </c>
-      <c r="G684" t="s">
-        <v>2437</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G679" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G677" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Improved the assign layout a bit and renamed some labels
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF3EA9C-DC8F-4AA6-A1AF-755B07C47EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76367166-1ED6-45CE-9796-D8BDF1B5C4F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="2434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="2433">
   <si>
     <t>Key</t>
   </si>
@@ -7305,6 +7305,9 @@
     <t>AssignTo</t>
   </si>
   <si>
+    <t>Assign To</t>
+  </si>
+  <si>
     <t>إرسال إلى</t>
   </si>
   <si>
@@ -7327,12 +7330,6 @@
   </si>
   <si>
     <t>رسالة اختيارية...</t>
-  </si>
-  <si>
-    <t>Re-Assign To</t>
-  </si>
-  <si>
-    <t>Re-Assign</t>
   </si>
   <si>
     <t>is currently assigned this document</t>
@@ -7744,9 +7741,9 @@
   <dimension ref="A1:G682"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A611" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A662" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A634" sqref="A634:XFD634"/>
+      <selection pane="bottomLeft" activeCell="F684" sqref="F684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21835,10 +21832,10 @@
         <v>2415</v>
       </c>
       <c r="F678" s="6" t="s">
-        <v>2430</v>
+        <v>2431</v>
       </c>
       <c r="G678" t="s">
-        <v>2425</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="679" spans="1:7" x14ac:dyDescent="0.25">
@@ -21852,13 +21849,13 @@
         <v>1</v>
       </c>
       <c r="E679" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="F679" s="6" t="s">
         <v>2419</v>
       </c>
       <c r="G679" t="s">
-        <v>2426</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="680" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -21872,13 +21869,13 @@
         <v>1</v>
       </c>
       <c r="E680" s="3" t="s">
-        <v>2431</v>
+        <v>2423</v>
       </c>
       <c r="F680" s="6" t="s">
-        <v>2423</v>
+        <v>2424</v>
       </c>
       <c r="G680" s="3" t="s">
-        <v>2427</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.25">
@@ -21892,13 +21889,13 @@
         <v>1</v>
       </c>
       <c r="E681" t="s">
-        <v>2432</v>
+        <v>2417</v>
       </c>
       <c r="F681" s="6" t="s">
         <v>2418</v>
       </c>
       <c r="G681" t="s">
-        <v>2428</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="682" spans="1:7" x14ac:dyDescent="0.25">
@@ -21915,10 +21912,10 @@
         <v>2420</v>
       </c>
       <c r="F682" s="6" t="s">
-        <v>2424</v>
+        <v>2425</v>
       </c>
       <c r="G682" t="s">
-        <v>2429</v>
+        <v>2430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented rudimentary document signing
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4362EB4B-C3B1-49E5-BD65-49080A2251A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AB418D-4C9A-42FF-AB7A-4ACC83BB00BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="2433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="2433">
   <si>
     <t>Key</t>
   </si>
@@ -7738,12 +7738,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G682"/>
+  <dimension ref="A1:G683"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A662" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A656" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A676" sqref="A676"/>
+      <selection pane="bottomLeft" activeCell="E686" sqref="E686"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21918,6 +21918,23 @@
         <v>2429</v>
       </c>
     </row>
+    <row r="683" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A683" t="s">
+        <v>500</v>
+      </c>
+      <c r="B683" t="b">
+        <v>0</v>
+      </c>
+      <c r="C683" t="b">
+        <v>1</v>
+      </c>
+      <c r="E683" t="s">
+        <v>500</v>
+      </c>
+      <c r="F683" s="6" t="s">
+        <v>499</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G677" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Working on dynamic properties
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00911DC4-5717-47F9-8AB4-D9102B73BB87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6364157-DC39-4502-A8D4-44412DE246AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2818" uniqueCount="2489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="2493">
   <si>
     <t>Key</t>
   </si>
@@ -7501,6 +7501,18 @@
   </si>
   <si>
     <t>是当前</t>
+  </si>
+  <si>
+    <t>Equivalent</t>
+  </si>
+  <si>
+    <t>يقابله</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>المدة</t>
   </si>
 </sst>
 </file>
@@ -7906,12 +7918,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G703"/>
+  <dimension ref="A1:G704"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A483" sqref="A483"/>
+      <selection pane="bottomLeft" activeCell="E492" sqref="E492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18201,10 +18213,10 @@
       </c>
       <c r="D491" s="3"/>
       <c r="E491" s="3" t="s">
-        <v>432</v>
+        <v>2491</v>
       </c>
       <c r="F491" s="6" t="s">
-        <v>1706</v>
+        <v>2492</v>
       </c>
       <c r="G491" s="3" t="s">
         <v>1359</v>
@@ -22504,6 +22516,23 @@
       </c>
       <c r="G703" t="s">
         <v>1384</v>
+      </c>
+    </row>
+    <row r="704" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A704" t="s">
+        <v>2489</v>
+      </c>
+      <c r="B704" t="b">
+        <v>0</v>
+      </c>
+      <c r="C704" t="b">
+        <v>1</v>
+      </c>
+      <c r="E704" t="s">
+        <v>2489</v>
+      </c>
+      <c r="F704" s="6" t="s">
+        <v>2490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgraded the solution to ASP.NET Core 3.1
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C640381D-2F15-446E-B6CB-8877CF9FA38F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E063D078-2080-4EDC-8086-C2E01006D9FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -7929,7 +7929,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A393" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G400" sqref="G400"/>
+      <selection pane="bottomLeft" activeCell="A400" sqref="A400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Renamed function to modifier
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B122220C-7BEE-439E-8535-64BAD96CEF6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEA208A-C8FF-485E-9EC5-88F5ECD21CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2355" windowWidth="16890" windowHeight="11415" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
@@ -7530,27 +7530,6 @@
     <t>إنقطع الاتصال، تجري محاولة الاتصال من جديد...</t>
   </si>
   <si>
-    <t>Function_year</t>
-  </si>
-  <si>
-    <t>Function_quarter</t>
-  </si>
-  <si>
-    <t>Function_month</t>
-  </si>
-  <si>
-    <t>Function_dayofyear</t>
-  </si>
-  <si>
-    <t>Function_day</t>
-  </si>
-  <si>
-    <t>Function_week</t>
-  </si>
-  <si>
-    <t>Function_weekday</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -7614,15 +7593,6 @@
     <t>美分硬币</t>
   </si>
   <si>
-    <t>ReportDefinition_Function</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>الدالة</t>
-  </si>
-  <si>
     <t>功能</t>
   </si>
   <si>
@@ -7735,6 +7705,36 @@
   </si>
   <si>
     <t>4季度</t>
+  </si>
+  <si>
+    <t>Modifier_year</t>
+  </si>
+  <si>
+    <t>Modifier_quarter</t>
+  </si>
+  <si>
+    <t>Modifier_month</t>
+  </si>
+  <si>
+    <t>Modifier_dayofyear</t>
+  </si>
+  <si>
+    <t>Modifier_day</t>
+  </si>
+  <si>
+    <t>Modifier_week</t>
+  </si>
+  <si>
+    <t>Modifier_weekday</t>
+  </si>
+  <si>
+    <t>ReportDefinition_Modifier</t>
+  </si>
+  <si>
+    <t>Modifier</t>
+  </si>
+  <si>
+    <t>المغير</t>
   </si>
 </sst>
 </file>
@@ -8143,9 +8143,9 @@
   <dimension ref="A1:G724"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A632" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A607" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A654" sqref="A654:XFD654"/>
+      <selection pane="bottomLeft" activeCell="F626" sqref="F626"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15460,7 +15460,7 @@
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="s">
-        <v>2548</v>
+        <v>2538</v>
       </c>
       <c r="B349" s="3" t="b">
         <v>0</v>
@@ -15481,7 +15481,7 @@
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>2549</v>
+        <v>2539</v>
       </c>
       <c r="B350" s="3" t="b">
         <v>0</v>
@@ -15502,7 +15502,7 @@
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="B351" s="3" t="b">
         <v>0</v>
@@ -15523,7 +15523,7 @@
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
-        <v>2551</v>
+        <v>2541</v>
       </c>
       <c r="B352" s="3" t="b">
         <v>0</v>
@@ -15544,7 +15544,7 @@
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="s">
-        <v>2552</v>
+        <v>2542</v>
       </c>
       <c r="B353" s="3" t="b">
         <v>0</v>
@@ -15565,7 +15565,7 @@
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
-        <v>2553</v>
+        <v>2543</v>
       </c>
       <c r="B354" s="3" t="b">
         <v>0</v>
@@ -15586,7 +15586,7 @@
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" s="3" t="s">
-        <v>2554</v>
+        <v>2544</v>
       </c>
       <c r="B355" s="3" t="b">
         <v>0</v>
@@ -15616,10 +15616,10 @@
         <v>1</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>2530</v>
+        <v>2520</v>
       </c>
       <c r="F356" s="6" t="s">
-        <v>2537</v>
+        <v>2527</v>
       </c>
       <c r="G356" s="3" t="s">
         <v>1575</v>
@@ -15636,10 +15636,10 @@
         <v>1</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>2531</v>
+        <v>2521</v>
       </c>
       <c r="F357" s="6" t="s">
-        <v>2538</v>
+        <v>2528</v>
       </c>
       <c r="G357" s="3" t="s">
         <v>1576</v>
@@ -15656,10 +15656,10 @@
         <v>1</v>
       </c>
       <c r="E358" s="3" t="s">
-        <v>2532</v>
+        <v>2522</v>
       </c>
       <c r="F358" s="6" t="s">
-        <v>2539</v>
+        <v>2529</v>
       </c>
       <c r="G358" s="3" t="s">
         <v>1577</v>
@@ -15676,10 +15676,10 @@
         <v>1</v>
       </c>
       <c r="E359" s="3" t="s">
-        <v>2533</v>
+        <v>2523</v>
       </c>
       <c r="F359" s="6" t="s">
-        <v>2540</v>
+        <v>2530</v>
       </c>
       <c r="G359" s="3" t="s">
         <v>1578</v>
@@ -15696,10 +15696,10 @@
         <v>1</v>
       </c>
       <c r="E360" s="3" t="s">
-        <v>2534</v>
+        <v>2524</v>
       </c>
       <c r="F360" s="6" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="G360" s="3" t="s">
         <v>1579</v>
@@ -15716,10 +15716,10 @@
         <v>1</v>
       </c>
       <c r="E361" s="3" t="s">
-        <v>2535</v>
+        <v>2525</v>
       </c>
       <c r="F361" s="6" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="G361" s="3" t="s">
         <v>1580</v>
@@ -15736,10 +15736,10 @@
         <v>1</v>
       </c>
       <c r="E362" s="3" t="s">
-        <v>2536</v>
+        <v>2526</v>
       </c>
       <c r="F362" s="6" t="s">
-        <v>2543</v>
+        <v>2533</v>
       </c>
       <c r="G362" s="3" t="s">
         <v>1581</v>
@@ -15999,7 +15999,7 @@
     </row>
     <row r="375" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3" t="s">
-        <v>2546</v>
+        <v>2536</v>
       </c>
       <c r="B375" s="3" t="b">
         <v>1</v>
@@ -16008,18 +16008,18 @@
         <v>1</v>
       </c>
       <c r="E375" s="3" t="s">
-        <v>2555</v>
+        <v>2545</v>
       </c>
       <c r="F375" s="6" t="s">
-        <v>2559</v>
+        <v>2549</v>
       </c>
       <c r="G375" s="3" t="s">
-        <v>2563</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="376" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3" t="s">
-        <v>2544</v>
+        <v>2534</v>
       </c>
       <c r="B376" s="3" t="b">
         <v>1</v>
@@ -16028,18 +16028,18 @@
         <v>1</v>
       </c>
       <c r="E376" s="3" t="s">
-        <v>2556</v>
+        <v>2546</v>
       </c>
       <c r="F376" s="6" t="s">
-        <v>2560</v>
+        <v>2550</v>
       </c>
       <c r="G376" s="3" t="s">
-        <v>2564</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="377" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="s">
-        <v>2545</v>
+        <v>2535</v>
       </c>
       <c r="B377" s="3" t="b">
         <v>1</v>
@@ -16048,18 +16048,18 @@
         <v>1</v>
       </c>
       <c r="E377" s="3" t="s">
-        <v>2557</v>
+        <v>2547</v>
       </c>
       <c r="F377" s="6" t="s">
-        <v>2561</v>
+        <v>2551</v>
       </c>
       <c r="G377" s="3" t="s">
-        <v>2565</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="378" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3" t="s">
-        <v>2547</v>
+        <v>2537</v>
       </c>
       <c r="B378" s="3" t="b">
         <v>1</v>
@@ -16068,13 +16068,13 @@
         <v>1</v>
       </c>
       <c r="E378" s="3" t="s">
-        <v>2558</v>
+        <v>2548</v>
       </c>
       <c r="F378" s="6" t="s">
-        <v>2562</v>
+        <v>2552</v>
       </c>
       <c r="G378" s="3" t="s">
-        <v>2566</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
@@ -21144,7 +21144,7 @@
     </row>
     <row r="625" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A625" s="3" t="s">
-        <v>2526</v>
+        <v>2564</v>
       </c>
       <c r="B625" s="3" t="b">
         <v>1</v>
@@ -21153,13 +21153,13 @@
         <v>1</v>
       </c>
       <c r="E625" s="3" t="s">
-        <v>2527</v>
+        <v>2565</v>
       </c>
       <c r="F625" s="6" t="s">
-        <v>2528</v>
+        <v>2566</v>
       </c>
       <c r="G625" s="3" t="s">
-        <v>2529</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="626" spans="1:7" x14ac:dyDescent="0.25">
@@ -23021,67 +23021,67 @@
     </row>
     <row r="718" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B718" t="b">
+        <v>1</v>
+      </c>
+      <c r="C718" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E718" t="s">
         <v>2498</v>
       </c>
-      <c r="B718" t="b">
-        <v>1</v>
-      </c>
-      <c r="C718" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E718" t="s">
+      <c r="F718" s="6" t="s">
         <v>2505</v>
       </c>
-      <c r="F718" s="6" t="s">
+      <c r="G718" t="s">
         <v>2512</v>
-      </c>
-      <c r="G718" t="s">
-        <v>2519</v>
       </c>
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
+        <v>2558</v>
+      </c>
+      <c r="B719" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C719" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E719" t="s">
         <v>2499</v>
       </c>
-      <c r="B719" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C719" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E719" t="s">
+      <c r="F719" s="6" t="s">
         <v>2506</v>
       </c>
-      <c r="F719" s="6" t="s">
-        <v>2513</v>
-      </c>
       <c r="G719" t="s">
-        <v>2525</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
+        <v>2559</v>
+      </c>
+      <c r="B720" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C720" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E720" t="s">
         <v>2500</v>
       </c>
-      <c r="B720" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C720" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E720" t="s">
+      <c r="F720" s="6" t="s">
         <v>2507</v>
       </c>
-      <c r="F720" s="6" t="s">
-        <v>2514</v>
-      </c>
       <c r="G720" t="s">
-        <v>2520</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>2501</v>
+        <v>2560</v>
       </c>
       <c r="B721" s="3" t="b">
         <v>1</v>
@@ -23090,18 +23090,18 @@
         <v>1</v>
       </c>
       <c r="E721" t="s">
+        <v>2502</v>
+      </c>
+      <c r="F721" s="6" t="s">
         <v>2509</v>
       </c>
-      <c r="F721" s="6" t="s">
-        <v>2516</v>
-      </c>
       <c r="G721" t="s">
-        <v>2521</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>2502</v>
+        <v>2561</v>
       </c>
       <c r="B722" s="3" t="b">
         <v>1</v>
@@ -23110,18 +23110,18 @@
         <v>1</v>
       </c>
       <c r="E722" t="s">
+        <v>2503</v>
+      </c>
+      <c r="F722" s="6" t="s">
         <v>2510</v>
       </c>
-      <c r="F722" s="6" t="s">
-        <v>2517</v>
-      </c>
       <c r="G722" t="s">
-        <v>2522</v>
+        <v>2515</v>
       </c>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>2503</v>
+        <v>2562</v>
       </c>
       <c r="B723" s="3" t="b">
         <v>1</v>
@@ -23130,33 +23130,33 @@
         <v>1</v>
       </c>
       <c r="E723" t="s">
+        <v>2501</v>
+      </c>
+      <c r="F723" s="6" t="s">
         <v>2508</v>
       </c>
-      <c r="F723" s="6" t="s">
-        <v>2515</v>
-      </c>
       <c r="G723" t="s">
-        <v>2523</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
+        <v>2563</v>
+      </c>
+      <c r="B724" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C724" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E724" t="s">
         <v>2504</v>
       </c>
-      <c r="B724" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C724" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E724" t="s">
+      <c r="F724" s="6" t="s">
         <v>2511</v>
       </c>
-      <c r="F724" s="6" t="s">
-        <v>2518</v>
-      </c>
       <c r="G724" t="s">
-        <v>2524</v>
+        <v>2517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the major overhaul
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41612F25-EADB-4A86-8C55-A30C5E7EBE57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1575A31-0DEF-4FE3-B77D-98C47819AB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$728</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$727</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2974" uniqueCount="2626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2974" uniqueCount="2625">
   <si>
     <t>Key</t>
   </si>
@@ -6042,24 +6042,9 @@
     <t>预习</t>
   </si>
   <si>
-    <t>ResourceClassification</t>
-  </si>
-  <si>
-    <t>ResourceClassifications</t>
-  </si>
-  <si>
     <t>Resource Classification</t>
   </si>
   <si>
-    <t>Resource Classifications</t>
-  </si>
-  <si>
-    <t>تصنيف أصل</t>
-  </si>
-  <si>
-    <t>تصنيفات أصول</t>
-  </si>
-  <si>
     <t>资源分类</t>
   </si>
   <si>
@@ -6567,18 +6552,6 @@
     <t>IsAssignable</t>
   </si>
   <si>
-    <t>ResourceClassification_ResourceDefinition</t>
-  </si>
-  <si>
-    <t>Resource Definition</t>
-  </si>
-  <si>
-    <t>تعريف الموارد</t>
-  </si>
-  <si>
-    <t>资源定义</t>
-  </si>
-  <si>
     <t>Agent_StartDate</t>
   </si>
   <si>
@@ -6759,24 +6732,6 @@
     <t>定期</t>
   </si>
   <si>
-    <t>EntryClassifications</t>
-  </si>
-  <si>
-    <t>EntryClassifications_ForCredit</t>
-  </si>
-  <si>
-    <t>EntryClassifications_ForDebit</t>
-  </si>
-  <si>
-    <t>Entry Classification</t>
-  </si>
-  <si>
-    <t>Entry Classifications</t>
-  </si>
-  <si>
-    <t>EntryClassification</t>
-  </si>
-  <si>
     <t>تصنيفات الأسطر</t>
   </si>
   <si>
@@ -6888,9 +6843,6 @@
     <t>Entry_Currency</t>
   </si>
   <si>
-    <t>Entry_EntryClassification</t>
-  </si>
-  <si>
     <t>条目分类</t>
   </si>
   <si>
@@ -7311,9 +7263,6 @@
     <t>Account_Identifier</t>
   </si>
   <si>
-    <t>Account_EntryClassification</t>
-  </si>
-  <si>
     <t>Agent Definition</t>
   </si>
   <si>
@@ -7912,6 +7861,54 @@
   </si>
   <si>
     <t>是系统</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>明确</t>
+  </si>
+  <si>
+    <t>Account_EntryType</t>
+  </si>
+  <si>
+    <t>Entry_EntryType</t>
+  </si>
+  <si>
+    <t>EntryType</t>
+  </si>
+  <si>
+    <t>EntryTypes</t>
+  </si>
+  <si>
+    <t>EntryType_ForCredit</t>
+  </si>
+  <si>
+    <t>EntryType_ForDebit</t>
+  </si>
+  <si>
+    <t>Entry Type</t>
+  </si>
+  <si>
+    <t>Entry Types</t>
+  </si>
+  <si>
+    <t>LegacyType</t>
+  </si>
+  <si>
+    <t>LegacyTypes</t>
+  </si>
+  <si>
+    <t>Legacy Types</t>
+  </si>
+  <si>
+    <t>Legacy Type</t>
+  </si>
+  <si>
+    <t>تصنيف سابق</t>
+  </si>
+  <si>
+    <t>تصنيفات سابقة</t>
   </si>
 </sst>
 </file>
@@ -8311,9 +8308,9 @@
   <dimension ref="A1:G742"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G529" sqref="G529:G534"/>
+      <selection pane="bottomLeft" activeCell="F519" sqref="F519"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8655,10 +8652,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>2119</v>
+        <v>2114</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>2120</v>
+        <v>2115</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>1218</v>
@@ -8760,10 +8757,10 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>2351</v>
+        <v>2335</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>2337</v>
+        <v>2321</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>1621</v>
@@ -9264,10 +9261,10 @@
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>2489</v>
+        <v>2472</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>2490</v>
+        <v>2473</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>1237</v>
@@ -9285,10 +9282,10 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>2492</v>
+        <v>2475</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>2491</v>
+        <v>2474</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>1627</v>
@@ -11018,7 +11015,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
       <c r="B129" s="3" t="b">
         <v>1</v>
@@ -11028,13 +11025,13 @@
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3" t="s">
-        <v>2172</v>
+        <v>2167</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>2174</v>
+        <v>2169</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>2173</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -15554,7 +15551,7 @@
     </row>
     <row r="345" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
-        <v>2225</v>
+        <v>2216</v>
       </c>
       <c r="B345" s="3" t="b">
         <v>1</v>
@@ -15563,18 +15560,18 @@
         <v>1</v>
       </c>
       <c r="E345" s="3" t="s">
-        <v>2226</v>
+        <v>2217</v>
       </c>
       <c r="F345" s="5" t="s">
-        <v>2228</v>
+        <v>2219</v>
       </c>
       <c r="G345" s="3" t="s">
-        <v>2227</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="346" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
-        <v>2323</v>
+        <v>2307</v>
       </c>
       <c r="B346" s="3" t="b">
         <v>1</v>
@@ -15583,18 +15580,18 @@
         <v>1</v>
       </c>
       <c r="E346" s="3" t="s">
-        <v>2324</v>
+        <v>2308</v>
       </c>
       <c r="F346" s="5" t="s">
-        <v>2327</v>
+        <v>2311</v>
       </c>
       <c r="G346" s="3" t="s">
-        <v>2227</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="347" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
-        <v>2320</v>
+        <v>2304</v>
       </c>
       <c r="B347" s="3" t="b">
         <v>1</v>
@@ -15603,15 +15600,15 @@
         <v>1</v>
       </c>
       <c r="E347" s="3" t="s">
-        <v>2321</v>
+        <v>2305</v>
       </c>
       <c r="F347" s="5" t="s">
-        <v>2322</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="348" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="s">
-        <v>2325</v>
+        <v>2309</v>
       </c>
       <c r="B348" s="3" t="b">
         <v>1</v>
@@ -15620,15 +15617,15 @@
         <v>1</v>
       </c>
       <c r="E348" s="3" t="s">
-        <v>2326</v>
+        <v>2310</v>
       </c>
       <c r="F348" s="5" t="s">
-        <v>2328</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="s">
-        <v>2538</v>
+        <v>2521</v>
       </c>
       <c r="B349" s="3" t="b">
         <v>0</v>
@@ -15649,7 +15646,7 @@
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>2539</v>
+        <v>2522</v>
       </c>
       <c r="B350" s="3" t="b">
         <v>0</v>
@@ -15670,7 +15667,7 @@
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
-        <v>2540</v>
+        <v>2523</v>
       </c>
       <c r="B351" s="3" t="b">
         <v>0</v>
@@ -15691,7 +15688,7 @@
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
-        <v>2541</v>
+        <v>2524</v>
       </c>
       <c r="B352" s="3" t="b">
         <v>0</v>
@@ -15712,7 +15709,7 @@
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="s">
-        <v>2542</v>
+        <v>2525</v>
       </c>
       <c r="B353" s="3" t="b">
         <v>0</v>
@@ -15733,7 +15730,7 @@
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
-        <v>2543</v>
+        <v>2526</v>
       </c>
       <c r="B354" s="3" t="b">
         <v>0</v>
@@ -15754,7 +15751,7 @@
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" s="3" t="s">
-        <v>2544</v>
+        <v>2527</v>
       </c>
       <c r="B355" s="3" t="b">
         <v>0</v>
@@ -15784,10 +15781,10 @@
         <v>1</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>2520</v>
+        <v>2503</v>
       </c>
       <c r="F356" s="5" t="s">
-        <v>2527</v>
+        <v>2510</v>
       </c>
       <c r="G356" s="3" t="s">
         <v>1575</v>
@@ -15804,10 +15801,10 @@
         <v>1</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>2521</v>
+        <v>2504</v>
       </c>
       <c r="F357" s="5" t="s">
-        <v>2528</v>
+        <v>2511</v>
       </c>
       <c r="G357" s="3" t="s">
         <v>1576</v>
@@ -15824,10 +15821,10 @@
         <v>1</v>
       </c>
       <c r="E358" s="3" t="s">
-        <v>2522</v>
+        <v>2505</v>
       </c>
       <c r="F358" s="5" t="s">
-        <v>2529</v>
+        <v>2512</v>
       </c>
       <c r="G358" s="3" t="s">
         <v>1577</v>
@@ -15844,10 +15841,10 @@
         <v>1</v>
       </c>
       <c r="E359" s="3" t="s">
-        <v>2523</v>
+        <v>2506</v>
       </c>
       <c r="F359" s="5" t="s">
-        <v>2530</v>
+        <v>2513</v>
       </c>
       <c r="G359" s="3" t="s">
         <v>1578</v>
@@ -15864,10 +15861,10 @@
         <v>1</v>
       </c>
       <c r="E360" s="3" t="s">
-        <v>2524</v>
+        <v>2507</v>
       </c>
       <c r="F360" s="5" t="s">
-        <v>2531</v>
+        <v>2514</v>
       </c>
       <c r="G360" s="3" t="s">
         <v>1579</v>
@@ -15884,10 +15881,10 @@
         <v>1</v>
       </c>
       <c r="E361" s="3" t="s">
-        <v>2525</v>
+        <v>2508</v>
       </c>
       <c r="F361" s="5" t="s">
-        <v>2532</v>
+        <v>2515</v>
       </c>
       <c r="G361" s="3" t="s">
         <v>1580</v>
@@ -15904,10 +15901,10 @@
         <v>1</v>
       </c>
       <c r="E362" s="3" t="s">
-        <v>2526</v>
+        <v>2509</v>
       </c>
       <c r="F362" s="5" t="s">
-        <v>2533</v>
+        <v>2516</v>
       </c>
       <c r="G362" s="3" t="s">
         <v>1581</v>
@@ -16167,27 +16164,27 @@
     </row>
     <row r="375" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3" t="s">
+        <v>2519</v>
+      </c>
+      <c r="B375" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C375" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E375" s="3" t="s">
+        <v>2528</v>
+      </c>
+      <c r="F375" s="5" t="s">
+        <v>2532</v>
+      </c>
+      <c r="G375" s="3" t="s">
         <v>2536</v>
-      </c>
-      <c r="B375" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C375" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E375" s="3" t="s">
-        <v>2545</v>
-      </c>
-      <c r="F375" s="5" t="s">
-        <v>2549</v>
-      </c>
-      <c r="G375" s="3" t="s">
-        <v>2553</v>
       </c>
     </row>
     <row r="376" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3" t="s">
-        <v>2534</v>
+        <v>2517</v>
       </c>
       <c r="B376" s="3" t="b">
         <v>1</v>
@@ -16196,18 +16193,18 @@
         <v>1</v>
       </c>
       <c r="E376" s="3" t="s">
-        <v>2546</v>
+        <v>2529</v>
       </c>
       <c r="F376" s="5" t="s">
-        <v>2550</v>
+        <v>2533</v>
       </c>
       <c r="G376" s="3" t="s">
-        <v>2554</v>
+        <v>2537</v>
       </c>
     </row>
     <row r="377" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="s">
-        <v>2535</v>
+        <v>2518</v>
       </c>
       <c r="B377" s="3" t="b">
         <v>1</v>
@@ -16216,18 +16213,18 @@
         <v>1</v>
       </c>
       <c r="E377" s="3" t="s">
-        <v>2547</v>
+        <v>2530</v>
       </c>
       <c r="F377" s="5" t="s">
-        <v>2551</v>
+        <v>2534</v>
       </c>
       <c r="G377" s="3" t="s">
-        <v>2555</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="378" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3" t="s">
-        <v>2537</v>
+        <v>2520</v>
       </c>
       <c r="B378" s="3" t="b">
         <v>1</v>
@@ -16236,13 +16233,13 @@
         <v>1</v>
       </c>
       <c r="E378" s="3" t="s">
-        <v>2548</v>
+        <v>2531</v>
       </c>
       <c r="F378" s="5" t="s">
-        <v>2552</v>
+        <v>2535</v>
       </c>
       <c r="G378" s="3" t="s">
-        <v>2556</v>
+        <v>2539</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
@@ -16919,7 +16916,7 @@
     </row>
     <row r="411" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
-        <v>2488</v>
+        <v>2471</v>
       </c>
       <c r="B411" s="3" t="b">
         <v>1</v>
@@ -17117,7 +17114,7 @@
       </c>
       <c r="D420" s="3"/>
       <c r="E420" s="3" t="s">
-        <v>2224</v>
+        <v>2215</v>
       </c>
       <c r="F420" s="5" t="s">
         <v>1190</v>
@@ -17254,7 +17251,7 @@
     </row>
     <row r="427" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A427" s="3" t="s">
-        <v>2175</v>
+        <v>2170</v>
       </c>
       <c r="B427" s="3" t="b">
         <v>1</v>
@@ -17862,7 +17859,7 @@
     </row>
     <row r="456" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A456" s="3" t="s">
-        <v>2368</v>
+        <v>2352</v>
       </c>
       <c r="B456" s="3" t="b">
         <v>1</v>
@@ -17871,18 +17868,18 @@
         <v>1</v>
       </c>
       <c r="E456" s="3" t="s">
-        <v>2368</v>
+        <v>2352</v>
       </c>
       <c r="F456" s="5" t="s">
-        <v>2370</v>
+        <v>2354</v>
       </c>
       <c r="G456" s="3" t="s">
-        <v>2372</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="457" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A457" s="3" t="s">
-        <v>2369</v>
+        <v>2353</v>
       </c>
       <c r="B457" s="3" t="b">
         <v>1</v>
@@ -17891,13 +17888,13 @@
         <v>1</v>
       </c>
       <c r="E457" s="3" t="s">
-        <v>2369</v>
+        <v>2353</v>
       </c>
       <c r="F457" s="5" t="s">
-        <v>2371</v>
+        <v>2355</v>
       </c>
       <c r="G457" s="3" t="s">
-        <v>2373</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.25">
@@ -17918,7 +17915,7 @@
         <v>1636</v>
       </c>
       <c r="G458" s="3" t="s">
-        <v>2367</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="459" spans="1:7" x14ac:dyDescent="0.25">
@@ -18133,7 +18130,7 @@
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A469" s="3" t="s">
-        <v>2262</v>
+        <v>2247</v>
       </c>
       <c r="B469" s="3" t="b">
         <v>1</v>
@@ -18143,10 +18140,10 @@
       </c>
       <c r="D469" s="3"/>
       <c r="E469" s="3" t="s">
-        <v>2263</v>
+        <v>2248</v>
       </c>
       <c r="F469" s="5" t="s">
-        <v>2264</v>
+        <v>2249</v>
       </c>
       <c r="G469" s="3" t="s">
         <v>1715</v>
@@ -18154,7 +18151,7 @@
     </row>
     <row r="470" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A470" s="3" t="s">
-        <v>2265</v>
+        <v>2250</v>
       </c>
       <c r="B470" s="3" t="b">
         <v>1</v>
@@ -18163,10 +18160,10 @@
         <v>1</v>
       </c>
       <c r="E470" s="3" t="s">
-        <v>2266</v>
+        <v>2251</v>
       </c>
       <c r="F470" s="5" t="s">
-        <v>2267</v>
+        <v>2252</v>
       </c>
       <c r="G470" s="3" t="s">
         <v>1828</v>
@@ -18342,7 +18339,7 @@
     </row>
     <row r="479" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
-        <v>2362</v>
+        <v>2346</v>
       </c>
       <c r="B479" s="3" t="b">
         <v>1</v>
@@ -18354,7 +18351,7 @@
         <v>619</v>
       </c>
       <c r="F479" s="5" t="s">
-        <v>2363</v>
+        <v>2347</v>
       </c>
       <c r="G479" s="3" t="s">
         <v>1420</v>
@@ -18362,7 +18359,7 @@
     </row>
     <row r="480" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A480" s="3" t="s">
-        <v>2374</v>
+        <v>2358</v>
       </c>
       <c r="B480" s="3" t="b">
         <v>1</v>
@@ -18371,10 +18368,10 @@
         <v>1</v>
       </c>
       <c r="E480" s="3" t="s">
-        <v>2380</v>
+        <v>2364</v>
       </c>
       <c r="F480" s="5" t="s">
-        <v>2391</v>
+        <v>2375</v>
       </c>
       <c r="G480" s="3" t="s">
         <v>1213</v>
@@ -18382,67 +18379,67 @@
     </row>
     <row r="481" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
+        <v>2360</v>
+      </c>
+      <c r="B481" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C481" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E481" s="3" t="s">
+        <v>2365</v>
+      </c>
+      <c r="F481" s="5" t="s">
+        <v>2373</v>
+      </c>
+      <c r="G481" s="3" t="s">
         <v>2376</v>
-      </c>
-      <c r="B481" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C481" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E481" s="3" t="s">
-        <v>2381</v>
-      </c>
-      <c r="F481" s="5" t="s">
-        <v>2389</v>
-      </c>
-      <c r="G481" s="3" t="s">
-        <v>2392</v>
       </c>
     </row>
     <row r="482" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A482" s="3" t="s">
+        <v>2361</v>
+      </c>
+      <c r="B482" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C482" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E482" s="3" t="s">
+        <v>2366</v>
+      </c>
+      <c r="F482" s="5" t="s">
+        <v>2374</v>
+      </c>
+      <c r="G482" s="3" t="s">
         <v>2377</v>
-      </c>
-      <c r="B482" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C482" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E482" s="3" t="s">
-        <v>2382</v>
-      </c>
-      <c r="F482" s="5" t="s">
-        <v>2390</v>
-      </c>
-      <c r="G482" s="3" t="s">
-        <v>2393</v>
       </c>
     </row>
     <row r="483" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A483" s="3" t="s">
+        <v>2362</v>
+      </c>
+      <c r="B483" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C483" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E483" s="3" t="s">
+        <v>2367</v>
+      </c>
+      <c r="F483" s="5" t="s">
+        <v>2372</v>
+      </c>
+      <c r="G483" s="3" t="s">
         <v>2378</v>
-      </c>
-      <c r="B483" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C483" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E483" s="3" t="s">
-        <v>2383</v>
-      </c>
-      <c r="F483" s="5" t="s">
-        <v>2388</v>
-      </c>
-      <c r="G483" s="3" t="s">
-        <v>2394</v>
       </c>
     </row>
     <row r="484" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A484" s="3" t="s">
-        <v>2375</v>
+        <v>2359</v>
       </c>
       <c r="B484" s="3" t="b">
         <v>1</v>
@@ -18451,18 +18448,18 @@
         <v>1</v>
       </c>
       <c r="E484" s="3" t="s">
-        <v>2384</v>
+        <v>2368</v>
       </c>
       <c r="F484" s="5" t="s">
-        <v>2387</v>
+        <v>2371</v>
       </c>
       <c r="G484" s="3" t="s">
-        <v>2395</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="485" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A485" s="3" t="s">
-        <v>2379</v>
+        <v>2363</v>
       </c>
       <c r="B485" s="3" t="b">
         <v>1</v>
@@ -18471,18 +18468,18 @@
         <v>1</v>
       </c>
       <c r="E485" s="3" t="s">
-        <v>2386</v>
+        <v>2370</v>
       </c>
       <c r="F485" s="5" t="s">
-        <v>2385</v>
+        <v>2369</v>
       </c>
       <c r="G485" s="3" t="s">
-        <v>2396</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="486" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A486" s="3" t="s">
-        <v>2268</v>
+        <v>2253</v>
       </c>
       <c r="B486" s="3" t="b">
         <v>1</v>
@@ -18502,7 +18499,7 @@
     </row>
     <row r="487" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A487" s="3" t="s">
-        <v>2269</v>
+        <v>2254</v>
       </c>
       <c r="B487" s="3" t="b">
         <v>1</v>
@@ -18522,7 +18519,7 @@
     </row>
     <row r="488" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A488" s="3" t="s">
-        <v>2270</v>
+        <v>2255</v>
       </c>
       <c r="B488" s="3" t="b">
         <v>1</v>
@@ -18542,7 +18539,7 @@
     </row>
     <row r="489" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A489" s="3" t="s">
-        <v>2271</v>
+        <v>2256</v>
       </c>
       <c r="B489" s="3" t="b">
         <v>1</v>
@@ -18551,18 +18548,18 @@
         <v>1</v>
       </c>
       <c r="E489" s="3" t="s">
-        <v>2272</v>
+        <v>2257</v>
       </c>
       <c r="F489" s="5" t="s">
-        <v>2273</v>
+        <v>2258</v>
       </c>
       <c r="G489" s="3" t="s">
-        <v>2278</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="490" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
-        <v>2250</v>
+        <v>2235</v>
       </c>
       <c r="B490" s="3" t="b">
         <v>1</v>
@@ -18583,7 +18580,7 @@
     </row>
     <row r="491" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A491" s="3" t="s">
-        <v>2251</v>
+        <v>2236</v>
       </c>
       <c r="B491" s="3" t="b">
         <v>1</v>
@@ -18604,7 +18601,7 @@
     </row>
     <row r="492" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A492" s="3" t="s">
-        <v>2252</v>
+        <v>2237</v>
       </c>
       <c r="B492" s="3" t="b">
         <v>1</v>
@@ -18625,7 +18622,7 @@
     </row>
     <row r="493" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A493" s="3" t="s">
-        <v>2279</v>
+        <v>2264</v>
       </c>
       <c r="B493" s="3" t="b">
         <v>1</v>
@@ -18634,18 +18631,18 @@
         <v>1</v>
       </c>
       <c r="E493" s="3" t="s">
-        <v>2280</v>
+        <v>2265</v>
       </c>
       <c r="F493" s="5" t="s">
-        <v>2281</v>
+        <v>2266</v>
       </c>
       <c r="G493" s="3" t="s">
-        <v>2282</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A494" s="3" t="s">
-        <v>2284</v>
+        <v>2612</v>
       </c>
       <c r="B494" s="3" t="b">
         <v>1</v>
@@ -18655,18 +18652,18 @@
       </c>
       <c r="D494" s="3"/>
       <c r="E494" s="3" t="s">
-        <v>2486</v>
+        <v>2469</v>
       </c>
       <c r="F494" s="5" t="s">
-        <v>2487</v>
+        <v>2470</v>
       </c>
       <c r="G494" s="3" t="s">
-        <v>2285</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A495" s="3" t="s">
-        <v>2253</v>
+        <v>2238</v>
       </c>
       <c r="B495" s="3" t="b">
         <v>1</v>
@@ -18687,7 +18684,7 @@
     </row>
     <row r="496" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
-        <v>2254</v>
+        <v>2239</v>
       </c>
       <c r="B496" s="3" t="b">
         <v>1</v>
@@ -18708,7 +18705,7 @@
     </row>
     <row r="497" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
-        <v>2255</v>
+        <v>2240</v>
       </c>
       <c r="B497" s="3" t="b">
         <v>1</v>
@@ -18729,7 +18726,7 @@
     </row>
     <row r="498" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
-        <v>2283</v>
+        <v>2268</v>
       </c>
       <c r="B498" s="3" t="b">
         <v>1</v>
@@ -18749,7 +18746,7 @@
     </row>
     <row r="499" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
-        <v>2286</v>
+        <v>2270</v>
       </c>
       <c r="B499" s="3" t="b">
         <v>1</v>
@@ -18758,18 +18755,18 @@
         <v>1</v>
       </c>
       <c r="E499" s="3" t="s">
-        <v>2287</v>
+        <v>2271</v>
       </c>
       <c r="F499" s="5" t="s">
-        <v>2288</v>
+        <v>2272</v>
       </c>
       <c r="G499" s="3" t="s">
-        <v>2311</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="500" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
-        <v>2256</v>
+        <v>2241</v>
       </c>
       <c r="B500" s="3" t="b">
         <v>1</v>
@@ -18790,7 +18787,7 @@
     </row>
     <row r="501" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A501" s="3" t="s">
-        <v>2257</v>
+        <v>2242</v>
       </c>
       <c r="B501" s="3" t="b">
         <v>1</v>
@@ -18811,7 +18808,7 @@
     </row>
     <row r="502" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A502" s="3" t="s">
-        <v>2258</v>
+        <v>2243</v>
       </c>
       <c r="B502" s="3" t="b">
         <v>1</v>
@@ -18832,7 +18829,7 @@
     </row>
     <row r="503" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A503" s="3" t="s">
-        <v>2259</v>
+        <v>2244</v>
       </c>
       <c r="B503" s="3" t="b">
         <v>1</v>
@@ -18842,10 +18839,10 @@
       </c>
       <c r="D503" s="3"/>
       <c r="E503" s="3" t="s">
-        <v>2484</v>
+        <v>2467</v>
       </c>
       <c r="F503" s="5" t="s">
-        <v>2485</v>
+        <v>2468</v>
       </c>
       <c r="G503" s="3" t="s">
         <v>1353</v>
@@ -18853,7 +18850,7 @@
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A504" s="3" t="s">
-        <v>2260</v>
+        <v>2245</v>
       </c>
       <c r="B504" s="3" t="b">
         <v>1</v>
@@ -18874,7 +18871,7 @@
     </row>
     <row r="505" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A505" s="3" t="s">
-        <v>2261</v>
+        <v>2246</v>
       </c>
       <c r="B505" s="3" t="b">
         <v>1</v>
@@ -18895,7 +18892,7 @@
     </row>
     <row r="506" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A506" s="3" t="s">
-        <v>2289</v>
+        <v>2273</v>
       </c>
       <c r="B506" s="3" t="b">
         <v>1</v>
@@ -18907,7 +18904,7 @@
         <v>1687</v>
       </c>
       <c r="F506" s="5" t="s">
-        <v>2303</v>
+        <v>2287</v>
       </c>
       <c r="G506" s="3" t="s">
         <v>1724</v>
@@ -18915,7 +18912,7 @@
     </row>
     <row r="507" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A507" s="3" t="s">
-        <v>2290</v>
+        <v>2274</v>
       </c>
       <c r="B507" s="3" t="b">
         <v>1</v>
@@ -18927,7 +18924,7 @@
         <v>1688</v>
       </c>
       <c r="F507" s="5" t="s">
-        <v>2304</v>
+        <v>2288</v>
       </c>
       <c r="G507" s="3" t="s">
         <v>1725</v>
@@ -18935,7 +18932,7 @@
     </row>
     <row r="508" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A508" s="3" t="s">
-        <v>2291</v>
+        <v>2275</v>
       </c>
       <c r="B508" s="3" t="b">
         <v>1</v>
@@ -18944,18 +18941,18 @@
         <v>1</v>
       </c>
       <c r="E508" s="3" t="s">
-        <v>2297</v>
+        <v>2281</v>
       </c>
       <c r="F508" s="5" t="s">
-        <v>2305</v>
+        <v>2289</v>
       </c>
       <c r="G508" s="3" t="s">
-        <v>2312</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="509" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A509" s="3" t="s">
-        <v>2292</v>
+        <v>2276</v>
       </c>
       <c r="B509" s="3" t="b">
         <v>1</v>
@@ -18964,18 +18961,18 @@
         <v>1</v>
       </c>
       <c r="E509" s="3" t="s">
-        <v>2300</v>
+        <v>2284</v>
       </c>
       <c r="F509" s="5" t="s">
-        <v>2306</v>
+        <v>2290</v>
       </c>
       <c r="G509" s="3" t="s">
-        <v>2313</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="510" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A510" s="3" t="s">
-        <v>2293</v>
+        <v>2277</v>
       </c>
       <c r="B510" s="3" t="b">
         <v>1</v>
@@ -18984,18 +18981,18 @@
         <v>1</v>
       </c>
       <c r="E510" s="3" t="s">
+        <v>2282</v>
+      </c>
+      <c r="F510" s="5" t="s">
+        <v>2291</v>
+      </c>
+      <c r="G510" s="3" t="s">
         <v>2298</v>
-      </c>
-      <c r="F510" s="5" t="s">
-        <v>2307</v>
-      </c>
-      <c r="G510" s="3" t="s">
-        <v>2314</v>
       </c>
     </row>
     <row r="511" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A511" s="3" t="s">
-        <v>2294</v>
+        <v>2278</v>
       </c>
       <c r="B511" s="3" t="b">
         <v>1</v>
@@ -19004,18 +19001,18 @@
         <v>1</v>
       </c>
       <c r="E511" s="3" t="s">
+        <v>2283</v>
+      </c>
+      <c r="F511" s="5" t="s">
+        <v>2292</v>
+      </c>
+      <c r="G511" s="3" t="s">
         <v>2299</v>
-      </c>
-      <c r="F511" s="5" t="s">
-        <v>2308</v>
-      </c>
-      <c r="G511" s="3" t="s">
-        <v>2315</v>
       </c>
     </row>
     <row r="512" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A512" s="3" t="s">
-        <v>2295</v>
+        <v>2279</v>
       </c>
       <c r="B512" s="3" t="b">
         <v>1</v>
@@ -19024,18 +19021,18 @@
         <v>1</v>
       </c>
       <c r="E512" s="3" t="s">
-        <v>2301</v>
+        <v>2285</v>
       </c>
       <c r="F512" s="5" t="s">
-        <v>2309</v>
+        <v>2293</v>
       </c>
       <c r="G512" s="3" t="s">
-        <v>2316</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="513" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A513" s="3" t="s">
-        <v>2296</v>
+        <v>2280</v>
       </c>
       <c r="B513" s="3" t="b">
         <v>1</v>
@@ -19044,18 +19041,18 @@
         <v>1</v>
       </c>
       <c r="E513" s="3" t="s">
-        <v>2302</v>
+        <v>2286</v>
       </c>
       <c r="F513" s="5" t="s">
-        <v>2310</v>
+        <v>2294</v>
       </c>
       <c r="G513" s="3" t="s">
-        <v>2317</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="514" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A514" s="3" t="s">
-        <v>2274</v>
+        <v>2259</v>
       </c>
       <c r="B514" s="3" t="b">
         <v>1</v>
@@ -19064,13 +19061,13 @@
         <v>1</v>
       </c>
       <c r="E514" s="3" t="s">
-        <v>2275</v>
+        <v>2260</v>
       </c>
       <c r="F514" s="5" t="s">
-        <v>2276</v>
+        <v>2261</v>
       </c>
       <c r="G514" s="3" t="s">
-        <v>2277</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="515" spans="1:7" x14ac:dyDescent="0.25">
@@ -19117,7 +19114,7 @@
     </row>
     <row r="517" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A517" s="3" t="s">
-        <v>2002</v>
+        <v>2619</v>
       </c>
       <c r="B517" s="3" t="b">
         <v>1</v>
@@ -19126,38 +19123,38 @@
         <v>1</v>
       </c>
       <c r="E517" s="3" t="s">
-        <v>2004</v>
+        <v>2622</v>
       </c>
       <c r="F517" s="5" t="s">
-        <v>2006</v>
+        <v>2623</v>
       </c>
       <c r="G517" s="3" t="s">
-        <v>2008</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="518" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A518" s="3" t="s">
+        <v>2620</v>
+      </c>
+      <c r="B518" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C518" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E518" s="3" t="s">
+        <v>2621</v>
+      </c>
+      <c r="F518" s="5" t="s">
+        <v>2624</v>
+      </c>
+      <c r="G518" s="3" t="s">
         <v>2003</v>
-      </c>
-      <c r="B518" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C518" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E518" s="3" t="s">
-        <v>2005</v>
-      </c>
-      <c r="F518" s="5" t="s">
-        <v>2007</v>
-      </c>
-      <c r="G518" s="3" t="s">
-        <v>2008</v>
       </c>
     </row>
     <row r="519" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A519" s="3" t="s">
-        <v>2130</v>
+        <v>2125</v>
       </c>
       <c r="B519" s="3" t="b">
         <v>1</v>
@@ -19367,7 +19364,7 @@
     </row>
     <row r="529" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A529" s="3" t="s">
-        <v>2604</v>
+        <v>2587</v>
       </c>
       <c r="B529" s="3" t="b">
         <v>1</v>
@@ -19376,18 +19373,18 @@
         <v>1</v>
       </c>
       <c r="E529" s="3" t="s">
-        <v>2280</v>
+        <v>2265</v>
       </c>
       <c r="F529" s="5" t="s">
-        <v>2605</v>
+        <v>2588</v>
       </c>
       <c r="G529" s="3" t="s">
-        <v>2481</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="530" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A530" s="3" t="s">
-        <v>2606</v>
+        <v>2589</v>
       </c>
       <c r="B530" s="3" t="b">
         <v>1</v>
@@ -19396,18 +19393,18 @@
         <v>1</v>
       </c>
       <c r="E530" s="3" t="s">
-        <v>2609</v>
+        <v>2592</v>
       </c>
       <c r="F530" s="5" t="s">
-        <v>2620</v>
+        <v>2603</v>
       </c>
       <c r="G530" s="3" t="s">
-        <v>2621</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="531" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A531" s="3" t="s">
-        <v>2607</v>
+        <v>2590</v>
       </c>
       <c r="B531" s="3" t="b">
         <v>1</v>
@@ -19416,18 +19413,18 @@
         <v>1</v>
       </c>
       <c r="E531" s="3" t="s">
-        <v>2611</v>
+        <v>2594</v>
       </c>
       <c r="F531" s="5" t="s">
-        <v>2618</v>
+        <v>2601</v>
       </c>
       <c r="G531" s="3" t="s">
-        <v>2622</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="532" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A532" s="3" t="s">
-        <v>2608</v>
+        <v>2591</v>
       </c>
       <c r="B532" s="3" t="b">
         <v>1</v>
@@ -19436,18 +19433,18 @@
         <v>1</v>
       </c>
       <c r="E532" s="3" t="s">
-        <v>2610</v>
+        <v>2593</v>
       </c>
       <c r="F532" s="5" t="s">
-        <v>2619</v>
+        <v>2602</v>
       </c>
       <c r="G532" s="3" t="s">
-        <v>2623</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="533" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A533" s="3" t="s">
-        <v>2612</v>
+        <v>2595</v>
       </c>
       <c r="B533" s="3" t="b">
         <v>1</v>
@@ -19456,18 +19453,18 @@
         <v>1</v>
       </c>
       <c r="E533" s="3" t="s">
-        <v>2613</v>
+        <v>2596</v>
       </c>
       <c r="F533" s="5" t="s">
-        <v>2614</v>
+        <v>2597</v>
       </c>
       <c r="G533" s="3" t="s">
-        <v>2624</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="534" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A534" s="3" t="s">
-        <v>2615</v>
+        <v>2598</v>
       </c>
       <c r="B534" s="3" t="b">
         <v>1</v>
@@ -19476,18 +19473,18 @@
         <v>1</v>
       </c>
       <c r="E534" s="3" t="s">
-        <v>2616</v>
+        <v>2599</v>
       </c>
       <c r="F534" s="5" t="s">
-        <v>2617</v>
+        <v>2600</v>
       </c>
       <c r="G534" s="3" t="s">
-        <v>2625</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="535" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A535" s="3" t="s">
-        <v>2176</v>
+        <v>2171</v>
       </c>
       <c r="B535" s="3" t="b">
         <v>1</v>
@@ -19675,7 +19672,7 @@
     </row>
     <row r="544" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A544" s="3" t="s">
-        <v>2229</v>
+        <v>2220</v>
       </c>
       <c r="B544" s="3" t="b">
         <v>1</v>
@@ -19684,13 +19681,13 @@
         <v>1</v>
       </c>
       <c r="E544" s="3" t="s">
-        <v>2230</v>
+        <v>2221</v>
       </c>
       <c r="F544" s="5" t="s">
-        <v>2231</v>
+        <v>2222</v>
       </c>
       <c r="G544" s="3" t="s">
-        <v>2232</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="545" spans="1:7" x14ac:dyDescent="0.25">
@@ -19716,7 +19713,7 @@
     </row>
     <row r="546" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A546" s="3" t="s">
-        <v>2336</v>
+        <v>2320</v>
       </c>
       <c r="B546" s="3" t="b">
         <v>1</v>
@@ -19736,7 +19733,7 @@
     </row>
     <row r="547" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A547" s="3" t="s">
-        <v>2417</v>
+        <v>2401</v>
       </c>
       <c r="B547" s="3" t="b">
         <v>1</v>
@@ -19748,7 +19745,7 @@
         <v>1692</v>
       </c>
       <c r="F547" s="5" t="s">
-        <v>2427</v>
+        <v>2410</v>
       </c>
       <c r="G547" s="3" t="s">
         <v>1727</v>
@@ -19756,7 +19753,7 @@
     </row>
     <row r="548" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A548" s="3" t="s">
-        <v>2418</v>
+        <v>2402</v>
       </c>
       <c r="B548" s="3" t="b">
         <v>1</v>
@@ -19765,58 +19762,58 @@
         <v>1</v>
       </c>
       <c r="E548" s="3" t="s">
-        <v>2275</v>
+        <v>2260</v>
       </c>
       <c r="F548" s="5" t="s">
-        <v>2276</v>
+        <v>2261</v>
       </c>
       <c r="G548" s="3" t="s">
-        <v>2277</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="549" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A549" s="3" t="s">
+        <v>2422</v>
+      </c>
+      <c r="B549" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C549" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E549" s="3" t="s">
+        <v>2435</v>
+      </c>
+      <c r="F549" s="5" t="s">
         <v>2439</v>
       </c>
-      <c r="B549" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C549" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E549" s="3" t="s">
-        <v>2452</v>
-      </c>
-      <c r="F549" s="5" t="s">
-        <v>2456</v>
-      </c>
       <c r="G549" s="3" t="s">
-        <v>2468</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="550" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A550" s="3" t="s">
+        <v>2423</v>
+      </c>
+      <c r="B550" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C550" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E550" s="3" t="s">
+        <v>2436</v>
+      </c>
+      <c r="F550" s="5" t="s">
         <v>2440</v>
       </c>
-      <c r="B550" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C550" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E550" s="3" t="s">
-        <v>2453</v>
-      </c>
-      <c r="F550" s="5" t="s">
-        <v>2457</v>
-      </c>
       <c r="G550" s="3" t="s">
-        <v>2469</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="551" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A551" s="3" t="s">
-        <v>2441</v>
+        <v>2424</v>
       </c>
       <c r="B551" s="3" t="b">
         <v>1</v>
@@ -19825,18 +19822,18 @@
         <v>1</v>
       </c>
       <c r="E551" s="3" t="s">
-        <v>2431</v>
+        <v>2414</v>
       </c>
       <c r="F551" s="5" t="s">
-        <v>2466</v>
+        <v>2449</v>
       </c>
       <c r="G551" s="3" t="s">
-        <v>2470</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="552" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A552" s="3" t="s">
-        <v>2442</v>
+        <v>2425</v>
       </c>
       <c r="B552" s="3" t="b">
         <v>1</v>
@@ -19845,18 +19842,18 @@
         <v>1</v>
       </c>
       <c r="E552" s="3" t="s">
-        <v>2432</v>
+        <v>2415</v>
       </c>
       <c r="F552" s="5" t="s">
-        <v>2458</v>
+        <v>2441</v>
       </c>
       <c r="G552" s="3" t="s">
-        <v>2471</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="553" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A553" s="3" t="s">
-        <v>2443</v>
+        <v>2426</v>
       </c>
       <c r="B553" s="3" t="b">
         <v>1</v>
@@ -19865,18 +19862,18 @@
         <v>1</v>
       </c>
       <c r="E553" s="3" t="s">
-        <v>2433</v>
+        <v>2416</v>
       </c>
       <c r="F553" s="5" t="s">
-        <v>2459</v>
+        <v>2442</v>
       </c>
       <c r="G553" s="3" t="s">
-        <v>2472</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="554" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A554" s="3" t="s">
-        <v>2444</v>
+        <v>2427</v>
       </c>
       <c r="B554" s="3" t="b">
         <v>1</v>
@@ -19885,38 +19882,38 @@
         <v>1</v>
       </c>
       <c r="E554" s="3" t="s">
-        <v>2455</v>
+        <v>2438</v>
       </c>
       <c r="F554" s="5" t="s">
-        <v>2460</v>
+        <v>2443</v>
       </c>
       <c r="G554" s="3" t="s">
-        <v>2473</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="555" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A555" s="3" t="s">
+        <v>2428</v>
+      </c>
+      <c r="B555" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C555" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E555" s="3" t="s">
+        <v>2417</v>
+      </c>
+      <c r="F555" s="5" t="s">
         <v>2445</v>
       </c>
-      <c r="B555" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C555" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E555" s="3" t="s">
-        <v>2434</v>
-      </c>
-      <c r="F555" s="5" t="s">
-        <v>2462</v>
-      </c>
       <c r="G555" s="3" t="s">
-        <v>2474</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="556" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A556" s="3" t="s">
-        <v>2446</v>
+        <v>2429</v>
       </c>
       <c r="B556" s="3" t="b">
         <v>1</v>
@@ -19925,18 +19922,18 @@
         <v>1</v>
       </c>
       <c r="E556" s="3" t="s">
-        <v>2454</v>
+        <v>2437</v>
       </c>
       <c r="F556" s="5" t="s">
-        <v>2465</v>
+        <v>2448</v>
       </c>
       <c r="G556" s="3" t="s">
-        <v>2475</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="557" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A557" s="3" t="s">
-        <v>2447</v>
+        <v>2430</v>
       </c>
       <c r="B557" s="3" t="b">
         <v>1</v>
@@ -19945,18 +19942,18 @@
         <v>1</v>
       </c>
       <c r="E557" s="3" t="s">
-        <v>2435</v>
+        <v>2418</v>
       </c>
       <c r="F557" s="5" t="s">
-        <v>2467</v>
+        <v>2450</v>
       </c>
       <c r="G557" s="3" t="s">
-        <v>2476</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="558" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A558" s="3" t="s">
-        <v>2448</v>
+        <v>2431</v>
       </c>
       <c r="B558" s="3" t="b">
         <v>1</v>
@@ -19965,18 +19962,18 @@
         <v>1</v>
       </c>
       <c r="E558" s="3" t="s">
-        <v>2436</v>
+        <v>2419</v>
       </c>
       <c r="F558" s="5" t="s">
-        <v>2463</v>
+        <v>2446</v>
       </c>
       <c r="G558" s="3" t="s">
-        <v>2477</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="559" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A559" s="3" t="s">
-        <v>2449</v>
+        <v>2432</v>
       </c>
       <c r="B559" s="3" t="b">
         <v>1</v>
@@ -19985,18 +19982,18 @@
         <v>1</v>
       </c>
       <c r="E559" s="3" t="s">
-        <v>2437</v>
+        <v>2420</v>
       </c>
       <c r="F559" s="5" t="s">
+        <v>2444</v>
+      </c>
+      <c r="G559" s="3" t="s">
         <v>2461</v>
-      </c>
-      <c r="G559" s="3" t="s">
-        <v>2478</v>
       </c>
     </row>
     <row r="560" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A560" s="3" t="s">
-        <v>2450</v>
+        <v>2433</v>
       </c>
       <c r="B560" s="3" t="b">
         <v>1</v>
@@ -20005,18 +20002,18 @@
         <v>1</v>
       </c>
       <c r="E560" s="3" t="s">
-        <v>2147</v>
+        <v>2142</v>
       </c>
       <c r="F560" s="5" t="s">
+        <v>2146</v>
+      </c>
+      <c r="G560" s="3" t="s">
         <v>2151</v>
-      </c>
-      <c r="G560" s="3" t="s">
-        <v>2156</v>
       </c>
     </row>
     <row r="561" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A561" s="3" t="s">
-        <v>2451</v>
+        <v>2434</v>
       </c>
       <c r="B561" s="3" t="b">
         <v>1</v>
@@ -20025,18 +20022,18 @@
         <v>1</v>
       </c>
       <c r="E561" s="3" t="s">
-        <v>2438</v>
+        <v>2421</v>
       </c>
       <c r="F561" s="5" t="s">
-        <v>2464</v>
+        <v>2447</v>
       </c>
       <c r="G561" s="3" t="s">
-        <v>2479</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="562" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A562" s="3" t="s">
-        <v>2419</v>
+        <v>2403</v>
       </c>
       <c r="B562" s="3" t="b">
         <v>1</v>
@@ -20045,18 +20042,18 @@
         <v>1</v>
       </c>
       <c r="E562" s="3" t="s">
-        <v>2426</v>
+        <v>2409</v>
       </c>
       <c r="F562" s="5" t="s">
-        <v>2428</v>
+        <v>2411</v>
       </c>
       <c r="G562" s="3" t="s">
-        <v>2480</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="563" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A563" s="3" t="s">
-        <v>2420</v>
+        <v>2404</v>
       </c>
       <c r="B563" s="3" t="b">
         <v>1</v>
@@ -20065,18 +20062,18 @@
         <v>1</v>
       </c>
       <c r="E563" s="3" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="F563" s="5" t="s">
-        <v>2429</v>
+        <v>2412</v>
       </c>
       <c r="G563" s="3" t="s">
-        <v>2008</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="564" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A564" s="3" t="s">
-        <v>2421</v>
+        <v>2405</v>
       </c>
       <c r="B564" s="3" t="b">
         <v>1</v>
@@ -20085,18 +20082,18 @@
         <v>1</v>
       </c>
       <c r="E564" s="3" t="s">
-        <v>2280</v>
+        <v>2265</v>
       </c>
       <c r="F564" s="5" t="s">
-        <v>2430</v>
+        <v>2413</v>
       </c>
       <c r="G564" s="3" t="s">
-        <v>2481</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="565" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A565" s="3" t="s">
-        <v>2422</v>
+        <v>2406</v>
       </c>
       <c r="B565" s="3" t="b">
         <v>1</v>
@@ -20116,7 +20113,7 @@
     </row>
     <row r="566" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A566" s="3" t="s">
-        <v>2423</v>
+        <v>2407</v>
       </c>
       <c r="B566" s="3" t="b">
         <v>1</v>
@@ -20136,7 +20133,7 @@
     </row>
     <row r="567" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A567" s="3" t="s">
-        <v>2424</v>
+        <v>2408</v>
       </c>
       <c r="B567" s="3" t="b">
         <v>1</v>
@@ -20145,18 +20142,18 @@
         <v>1</v>
       </c>
       <c r="E567" s="3" t="s">
-        <v>2221</v>
+        <v>2212</v>
       </c>
       <c r="F567" s="5" t="s">
-        <v>2222</v>
+        <v>2213</v>
       </c>
       <c r="G567" s="3" t="s">
-        <v>2223</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="568" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A568" s="3" t="s">
-        <v>2425</v>
+        <v>2611</v>
       </c>
       <c r="B568" s="3" t="b">
         <v>1</v>
@@ -20165,13 +20162,13 @@
         <v>1</v>
       </c>
       <c r="E568" s="3" t="s">
-        <v>2244</v>
+        <v>2617</v>
       </c>
       <c r="F568" s="5" t="s">
-        <v>2248</v>
+        <v>2233</v>
       </c>
       <c r="G568" s="3" t="s">
-        <v>2249</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.25">
@@ -20741,10 +20738,10 @@
         <v>1</v>
       </c>
       <c r="E596" t="s">
-        <v>2084</v>
+        <v>2079</v>
       </c>
       <c r="F596" s="5" t="s">
-        <v>2090</v>
+        <v>2085</v>
       </c>
       <c r="G596" t="s">
         <v>1971</v>
@@ -20752,7 +20749,7 @@
     </row>
     <row r="597" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A597" s="3" t="s">
-        <v>2038</v>
+        <v>2033</v>
       </c>
       <c r="B597" s="3" t="b">
         <v>1</v>
@@ -20761,18 +20758,18 @@
         <v>1</v>
       </c>
       <c r="E597" s="3" t="s">
-        <v>2085</v>
+        <v>2080</v>
       </c>
       <c r="F597" s="5" t="s">
-        <v>2091</v>
+        <v>2086</v>
       </c>
       <c r="G597" s="3" t="s">
-        <v>2065</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="598" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A598" s="3" t="s">
-        <v>2039</v>
+        <v>2034</v>
       </c>
       <c r="B598" s="3" t="b">
         <v>1</v>
@@ -20781,18 +20778,18 @@
         <v>1</v>
       </c>
       <c r="E598" s="3" t="s">
-        <v>2086</v>
+        <v>2081</v>
       </c>
       <c r="F598" s="5" t="s">
-        <v>2092</v>
+        <v>2087</v>
       </c>
       <c r="G598" s="3" t="s">
-        <v>2066</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="599" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A599" s="3" t="s">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="B599" s="3" t="b">
         <v>1</v>
@@ -20801,13 +20798,13 @@
         <v>1</v>
       </c>
       <c r="E599" s="3" t="s">
-        <v>2087</v>
+        <v>2082</v>
       </c>
       <c r="F599" s="5" t="s">
-        <v>2093</v>
+        <v>2088</v>
       </c>
       <c r="G599" s="3" t="s">
-        <v>2067</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="600" spans="1:7" x14ac:dyDescent="0.25">
@@ -20821,10 +20818,10 @@
         <v>1</v>
       </c>
       <c r="E600" t="s">
-        <v>2083</v>
+        <v>2078</v>
       </c>
       <c r="F600" s="5" t="s">
-        <v>2094</v>
+        <v>2089</v>
       </c>
       <c r="G600" t="s">
         <v>1972</v>
@@ -20832,7 +20829,7 @@
     </row>
     <row r="601" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A601" s="3" t="s">
-        <v>2041</v>
+        <v>2036</v>
       </c>
       <c r="B601" s="3" t="b">
         <v>1</v>
@@ -20841,18 +20838,18 @@
         <v>1</v>
       </c>
       <c r="E601" s="3" t="s">
-        <v>2082</v>
+        <v>2077</v>
       </c>
       <c r="F601" s="5" t="s">
-        <v>2095</v>
+        <v>2090</v>
       </c>
       <c r="G601" s="3" t="s">
-        <v>2068</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="602" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A602" s="3" t="s">
-        <v>2042</v>
+        <v>2037</v>
       </c>
       <c r="B602" s="3" t="b">
         <v>1</v>
@@ -20861,18 +20858,18 @@
         <v>1</v>
       </c>
       <c r="E602" s="3" t="s">
-        <v>2081</v>
+        <v>2076</v>
       </c>
       <c r="F602" s="5" t="s">
-        <v>2096</v>
+        <v>2091</v>
       </c>
       <c r="G602" s="3" t="s">
-        <v>2069</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="603" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A603" s="3" t="s">
-        <v>2043</v>
+        <v>2038</v>
       </c>
       <c r="B603" s="3" t="b">
         <v>1</v>
@@ -20881,13 +20878,13 @@
         <v>1</v>
       </c>
       <c r="E603" s="3" t="s">
-        <v>2080</v>
+        <v>2075</v>
       </c>
       <c r="F603" s="5" t="s">
-        <v>2097</v>
+        <v>2092</v>
       </c>
       <c r="G603" s="3" t="s">
-        <v>2070</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="604" spans="1:7" x14ac:dyDescent="0.25">
@@ -20912,7 +20909,7 @@
     </row>
     <row r="605" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A605" s="3" t="s">
-        <v>2044</v>
+        <v>2039</v>
       </c>
       <c r="B605" s="3" t="b">
         <v>1</v>
@@ -20921,18 +20918,18 @@
         <v>1</v>
       </c>
       <c r="E605" s="3" t="s">
-        <v>2052</v>
+        <v>2047</v>
       </c>
       <c r="F605" s="5" t="s">
-        <v>2058</v>
+        <v>2053</v>
       </c>
       <c r="G605" s="3" t="s">
-        <v>2071</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="606" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A606" s="3" t="s">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="B606" s="3" t="b">
         <v>1</v>
@@ -20941,18 +20938,18 @@
         <v>1</v>
       </c>
       <c r="E606" s="3" t="s">
-        <v>2088</v>
+        <v>2083</v>
       </c>
       <c r="F606" s="5" t="s">
-        <v>2060</v>
+        <v>2055</v>
       </c>
       <c r="G606" s="3" t="s">
-        <v>2072</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="607" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A607" s="3" t="s">
-        <v>2046</v>
+        <v>2041</v>
       </c>
       <c r="B607" s="3" t="b">
         <v>1</v>
@@ -20961,13 +20958,13 @@
         <v>1</v>
       </c>
       <c r="E607" s="3" t="s">
-        <v>2089</v>
+        <v>2084</v>
       </c>
       <c r="F607" s="5" t="s">
-        <v>2059</v>
+        <v>2054</v>
       </c>
       <c r="G607" s="3" t="s">
-        <v>2073</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="608" spans="1:7" x14ac:dyDescent="0.25">
@@ -20992,7 +20989,7 @@
     </row>
     <row r="609" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A609" s="3" t="s">
-        <v>2047</v>
+        <v>2042</v>
       </c>
       <c r="B609" s="3" t="b">
         <v>1</v>
@@ -21001,18 +20998,18 @@
         <v>1</v>
       </c>
       <c r="E609" s="3" t="s">
-        <v>2053</v>
+        <v>2048</v>
       </c>
       <c r="F609" s="5" t="s">
-        <v>2061</v>
+        <v>2056</v>
       </c>
       <c r="G609" s="3" t="s">
-        <v>2074</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="610" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A610" s="3" t="s">
-        <v>2048</v>
+        <v>2043</v>
       </c>
       <c r="B610" s="3" t="b">
         <v>1</v>
@@ -21021,18 +21018,18 @@
         <v>1</v>
       </c>
       <c r="E610" s="3" t="s">
-        <v>2054</v>
+        <v>2049</v>
       </c>
       <c r="F610" s="5" t="s">
-        <v>2062</v>
+        <v>2057</v>
       </c>
       <c r="G610" s="3" t="s">
-        <v>2075</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="611" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A611" s="3" t="s">
-        <v>2049</v>
+        <v>2044</v>
       </c>
       <c r="B611" s="3" t="b">
         <v>1</v>
@@ -21041,18 +21038,18 @@
         <v>1</v>
       </c>
       <c r="E611" s="3" t="s">
-        <v>2055</v>
+        <v>2050</v>
       </c>
       <c r="F611" s="5" t="s">
-        <v>2079</v>
+        <v>2074</v>
       </c>
       <c r="G611" s="3" t="s">
-        <v>2076</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="612" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A612" s="3" t="s">
-        <v>2050</v>
+        <v>2045</v>
       </c>
       <c r="B612" s="3" t="b">
         <v>1</v>
@@ -21061,18 +21058,18 @@
         <v>1</v>
       </c>
       <c r="E612" s="3" t="s">
-        <v>2056</v>
+        <v>2051</v>
       </c>
       <c r="F612" s="5" t="s">
-        <v>2063</v>
+        <v>2058</v>
       </c>
       <c r="G612" s="3" t="s">
-        <v>2077</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="613" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A613" s="3" t="s">
-        <v>2051</v>
+        <v>2046</v>
       </c>
       <c r="B613" s="3" t="b">
         <v>1</v>
@@ -21081,18 +21078,18 @@
         <v>1</v>
       </c>
       <c r="E613" s="3" t="s">
-        <v>2057</v>
+        <v>2052</v>
       </c>
       <c r="F613" s="5" t="s">
-        <v>2064</v>
+        <v>2059</v>
       </c>
       <c r="G613" s="3" t="s">
-        <v>2078</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="614" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A614" s="3" t="s">
-        <v>2099</v>
+        <v>2094</v>
       </c>
       <c r="B614" s="3" t="b">
         <v>1</v>
@@ -21101,13 +21098,13 @@
         <v>1</v>
       </c>
       <c r="E614" s="3" t="s">
-        <v>2100</v>
+        <v>2095</v>
       </c>
       <c r="F614" s="5" t="s">
-        <v>2101</v>
+        <v>2096</v>
       </c>
       <c r="G614" s="3" t="s">
-        <v>2102</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="615" spans="1:7" x14ac:dyDescent="0.25">
@@ -21364,7 +21361,7 @@
         <v>1915</v>
       </c>
       <c r="F627" s="5" t="s">
-        <v>2098</v>
+        <v>2093</v>
       </c>
       <c r="G627" t="s">
         <v>1983</v>
@@ -21432,7 +21429,7 @@
     </row>
     <row r="631" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A631" s="3" t="s">
-        <v>2564</v>
+        <v>2547</v>
       </c>
       <c r="B631" s="3" t="b">
         <v>1</v>
@@ -21441,13 +21438,13 @@
         <v>1</v>
       </c>
       <c r="E631" s="3" t="s">
-        <v>2565</v>
+        <v>2548</v>
       </c>
       <c r="F631" s="5" t="s">
-        <v>2566</v>
+        <v>2549</v>
       </c>
       <c r="G631" s="3" t="s">
-        <v>2519</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.25">
@@ -21532,7 +21529,7 @@
     </row>
     <row r="636" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A636" s="3" t="s">
-        <v>2567</v>
+        <v>2550</v>
       </c>
       <c r="B636" s="3" t="b">
         <v>1</v>
@@ -21541,18 +21538,18 @@
         <v>1</v>
       </c>
       <c r="E636" s="3" t="s">
-        <v>2569</v>
+        <v>2552</v>
       </c>
       <c r="F636" s="5" t="s">
-        <v>2570</v>
+        <v>2553</v>
       </c>
       <c r="G636" s="3" t="s">
-        <v>2574</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="637" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A637" s="3" t="s">
-        <v>2595</v>
+        <v>2578</v>
       </c>
       <c r="B637" s="3" t="b">
         <v>1</v>
@@ -21561,18 +21558,18 @@
         <v>1</v>
       </c>
       <c r="E637" s="3" t="s">
-        <v>2599</v>
+        <v>2582</v>
       </c>
       <c r="F637" s="5" t="s">
-        <v>2573</v>
+        <v>2556</v>
       </c>
       <c r="G637" s="3" t="s">
-        <v>2575</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="638" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A638" s="3" t="s">
-        <v>2596</v>
+        <v>2579</v>
       </c>
       <c r="B638" s="3" t="b">
         <v>1</v>
@@ -21581,18 +21578,18 @@
         <v>1</v>
       </c>
       <c r="E638" s="3" t="s">
-        <v>2597</v>
+        <v>2580</v>
       </c>
       <c r="F638" s="5" t="s">
-        <v>2598</v>
+        <v>2581</v>
       </c>
       <c r="G638" s="3" t="s">
-        <v>2576</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="639" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A639" s="3" t="s">
-        <v>2571</v>
+        <v>2554</v>
       </c>
       <c r="B639" s="3" t="b">
         <v>1</v>
@@ -21601,18 +21598,18 @@
         <v>1</v>
       </c>
       <c r="E639" s="3" t="s">
-        <v>2572</v>
+        <v>2555</v>
       </c>
       <c r="F639" s="5" t="s">
         <v>1664</v>
       </c>
       <c r="G639" s="3" t="s">
-        <v>2577</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="640" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A640" s="3" t="s">
-        <v>2594</v>
+        <v>2577</v>
       </c>
       <c r="B640" s="3" t="b">
         <v>1</v>
@@ -21652,7 +21649,7 @@
     </row>
     <row r="642" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A642" s="3" t="s">
-        <v>2568</v>
+        <v>2551</v>
       </c>
       <c r="B642" s="3" t="b">
         <v>1</v>
@@ -21892,7 +21889,7 @@
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="B654" t="b">
         <v>1</v>
@@ -21901,18 +21898,18 @@
         <v>1</v>
       </c>
       <c r="E654" t="s">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="F654" s="5" t="s">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="G654" t="s">
-        <v>2013</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="655" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="B655" s="3" t="b">
         <v>1</v>
@@ -21921,18 +21918,18 @@
         <v>1</v>
       </c>
       <c r="E655" t="s">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="F655" s="5" t="s">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="G655" t="s">
-        <v>2014</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B656" t="b">
         <v>0</v>
@@ -21941,18 +21938,18 @@
         <v>1</v>
       </c>
       <c r="E656" t="s">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="F656" s="5" t="s">
         <v>1953</v>
       </c>
       <c r="G656" t="s">
-        <v>2028</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="657" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B657" t="b">
         <v>1</v>
@@ -21961,18 +21958,18 @@
         <v>1</v>
       </c>
       <c r="E657" t="s">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="F657" s="5" t="s">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="G657" t="s">
-        <v>2029</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658" s="3" t="s">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B658" t="b">
         <v>0</v>
@@ -21981,18 +21978,18 @@
         <v>1</v>
       </c>
       <c r="E658" t="s">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="F658" s="5" t="s">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="G658" t="s">
-        <v>2030</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="659" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="B659" t="b">
         <v>0</v>
@@ -22001,18 +21998,18 @@
         <v>1</v>
       </c>
       <c r="E659" t="s">
+        <v>2021</v>
+      </c>
+      <c r="F659" s="5" t="s">
+        <v>2022</v>
+      </c>
+      <c r="G659" t="s">
         <v>2026</v>
-      </c>
-      <c r="F659" s="5" t="s">
-        <v>2027</v>
-      </c>
-      <c r="G659" t="s">
-        <v>2031</v>
       </c>
     </row>
     <row r="660" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>2032</v>
+        <v>2027</v>
       </c>
       <c r="B660" t="b">
         <v>0</v>
@@ -22021,18 +22018,18 @@
         <v>1</v>
       </c>
       <c r="E660" t="s">
-        <v>2032</v>
+        <v>2027</v>
       </c>
       <c r="F660" s="5" t="s">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="G660" t="s">
-        <v>2036</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="661" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>2033</v>
+        <v>2028</v>
       </c>
       <c r="B661" t="b">
         <v>0</v>
@@ -22041,13 +22038,13 @@
         <v>1</v>
       </c>
       <c r="E661" t="s">
-        <v>2033</v>
+        <v>2028</v>
       </c>
       <c r="F661" s="5" t="s">
-        <v>2034</v>
+        <v>2029</v>
       </c>
       <c r="G661" t="s">
-        <v>2037</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="662" spans="1:7" x14ac:dyDescent="0.25">
@@ -22072,7 +22069,7 @@
     </row>
     <row r="663" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>2103</v>
+        <v>2098</v>
       </c>
       <c r="B663" t="b">
         <v>0</v>
@@ -22081,18 +22078,18 @@
         <v>1</v>
       </c>
       <c r="E663" t="s">
+        <v>2099</v>
+      </c>
+      <c r="F663" s="5" t="s">
+        <v>2100</v>
+      </c>
+      <c r="G663" t="s">
         <v>2104</v>
-      </c>
-      <c r="F663" s="5" t="s">
-        <v>2105</v>
-      </c>
-      <c r="G663" t="s">
-        <v>2109</v>
       </c>
     </row>
     <row r="664" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>2106</v>
+        <v>2101</v>
       </c>
       <c r="B664" t="b">
         <v>0</v>
@@ -22101,18 +22098,18 @@
         <v>1</v>
       </c>
       <c r="E664" t="s">
-        <v>2108</v>
+        <v>2103</v>
       </c>
       <c r="F664" s="5" t="s">
-        <v>2107</v>
+        <v>2102</v>
       </c>
       <c r="G664" t="s">
-        <v>2110</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="665" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>2111</v>
+        <v>2106</v>
       </c>
       <c r="B665" t="b">
         <v>0</v>
@@ -22121,18 +22118,18 @@
         <v>1</v>
       </c>
       <c r="E665" t="s">
-        <v>2112</v>
+        <v>2107</v>
       </c>
       <c r="F665" s="5" t="s">
-        <v>2113</v>
+        <v>2108</v>
       </c>
       <c r="G665" t="s">
-        <v>2114</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="666" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>2115</v>
+        <v>2110</v>
       </c>
       <c r="B666" t="b">
         <v>1</v>
@@ -22141,18 +22138,18 @@
         <v>0</v>
       </c>
       <c r="E666" t="s">
-        <v>2118</v>
+        <v>2113</v>
       </c>
       <c r="F666" s="5" t="s">
-        <v>2116</v>
+        <v>2111</v>
       </c>
       <c r="G666" t="s">
-        <v>2117</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="667" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A667" s="3" t="s">
-        <v>2133</v>
+        <v>2128</v>
       </c>
       <c r="B667" s="3" t="b">
         <v>1</v>
@@ -22164,7 +22161,7 @@
         <v>1692</v>
       </c>
       <c r="F667" s="5" t="s">
-        <v>2136</v>
+        <v>2131</v>
       </c>
       <c r="G667" s="3" t="s">
         <v>1727</v>
@@ -22172,7 +22169,7 @@
     </row>
     <row r="668" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A668" s="3" t="s">
-        <v>2134</v>
+        <v>2129</v>
       </c>
       <c r="B668" s="3" t="b">
         <v>1</v>
@@ -22181,10 +22178,10 @@
         <v>1</v>
       </c>
       <c r="E668" s="3" t="s">
-        <v>2135</v>
+        <v>2130</v>
       </c>
       <c r="F668" s="5" t="s">
-        <v>2137</v>
+        <v>2132</v>
       </c>
       <c r="G668" s="3" t="s">
         <v>1727</v>
@@ -22192,7 +22189,7 @@
     </row>
     <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>2129</v>
+        <v>2124</v>
       </c>
       <c r="B669" t="b">
         <v>1</v>
@@ -22201,18 +22198,18 @@
         <v>1</v>
       </c>
       <c r="E669" t="s">
-        <v>2131</v>
+        <v>2126</v>
       </c>
       <c r="F669" s="5" t="s">
-        <v>2132</v>
+        <v>2127</v>
       </c>
       <c r="G669" t="s">
-        <v>2153</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="670" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A670" s="3" t="s">
-        <v>2141</v>
+        <v>2136</v>
       </c>
       <c r="B670" s="3" t="b">
         <v>1</v>
@@ -22221,18 +22218,18 @@
         <v>1</v>
       </c>
       <c r="E670" s="3" t="s">
-        <v>2145</v>
+        <v>2140</v>
       </c>
       <c r="F670" s="5" t="s">
+        <v>2144</v>
+      </c>
+      <c r="G670" s="3" t="s">
         <v>2149</v>
-      </c>
-      <c r="G670" s="3" t="s">
-        <v>2154</v>
       </c>
     </row>
     <row r="671" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A671" s="3" t="s">
-        <v>2142</v>
+        <v>2137</v>
       </c>
       <c r="B671" s="3" t="b">
         <v>1</v>
@@ -22241,18 +22238,18 @@
         <v>1</v>
       </c>
       <c r="E671" s="3" t="s">
-        <v>2146</v>
+        <v>2141</v>
       </c>
       <c r="F671" s="5" t="s">
+        <v>2145</v>
+      </c>
+      <c r="G671" s="3" t="s">
         <v>2150</v>
-      </c>
-      <c r="G671" s="3" t="s">
-        <v>2155</v>
       </c>
     </row>
     <row r="672" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A672" s="3" t="s">
-        <v>2143</v>
+        <v>2138</v>
       </c>
       <c r="B672" s="3" t="b">
         <v>1</v>
@@ -22261,18 +22258,18 @@
         <v>1</v>
       </c>
       <c r="E672" s="3" t="s">
-        <v>2147</v>
+        <v>2142</v>
       </c>
       <c r="F672" s="5" t="s">
+        <v>2146</v>
+      </c>
+      <c r="G672" s="3" t="s">
         <v>2151</v>
-      </c>
-      <c r="G672" s="3" t="s">
-        <v>2156</v>
       </c>
     </row>
     <row r="673" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A673" s="3" t="s">
-        <v>2144</v>
+        <v>2139</v>
       </c>
       <c r="B673" s="3" t="b">
         <v>1</v>
@@ -22281,18 +22278,18 @@
         <v>1</v>
       </c>
       <c r="E673" s="3" t="s">
-        <v>2148</v>
+        <v>2143</v>
       </c>
       <c r="F673" s="5" t="s">
+        <v>2147</v>
+      </c>
+      <c r="G673" s="3" t="s">
         <v>2152</v>
-      </c>
-      <c r="G673" s="3" t="s">
-        <v>2157</v>
       </c>
     </row>
     <row r="674" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>2138</v>
+        <v>2133</v>
       </c>
       <c r="B674" t="b">
         <v>1</v>
@@ -22301,18 +22298,18 @@
         <v>1</v>
       </c>
       <c r="E674" t="s">
-        <v>2139</v>
+        <v>2134</v>
       </c>
       <c r="F674" s="5" t="s">
-        <v>2140</v>
+        <v>2135</v>
       </c>
       <c r="G674" t="s">
-        <v>2158</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>2159</v>
+        <v>2154</v>
       </c>
       <c r="B675" t="b">
         <v>1</v>
@@ -22321,18 +22318,18 @@
         <v>1</v>
       </c>
       <c r="E675" t="s">
-        <v>2162</v>
+        <v>2157</v>
       </c>
       <c r="F675" s="5" t="s">
-        <v>2165</v>
+        <v>2160</v>
       </c>
       <c r="G675" t="s">
-        <v>2168</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="676" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>2160</v>
+        <v>2155</v>
       </c>
       <c r="B676" s="3" t="b">
         <v>1</v>
@@ -22341,18 +22338,18 @@
         <v>1</v>
       </c>
       <c r="E676" t="s">
-        <v>2163</v>
+        <v>2158</v>
       </c>
       <c r="F676" s="5" t="s">
-        <v>2166</v>
+        <v>2161</v>
       </c>
       <c r="G676" t="s">
-        <v>2169</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>2161</v>
+        <v>2156</v>
       </c>
       <c r="B677" s="3" t="b">
         <v>1</v>
@@ -22361,18 +22358,18 @@
         <v>1</v>
       </c>
       <c r="E677" t="s">
-        <v>2164</v>
+        <v>2159</v>
       </c>
       <c r="F677" s="5" t="s">
-        <v>2167</v>
+        <v>2162</v>
       </c>
       <c r="G677" t="s">
-        <v>2170</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>2177</v>
+        <v>2172</v>
       </c>
       <c r="B678" s="3" t="b">
         <v>1</v>
@@ -22384,15 +22381,15 @@
         <v>2178</v>
       </c>
       <c r="F678" s="5" t="s">
-        <v>2179</v>
+        <v>2184</v>
       </c>
       <c r="G678" t="s">
-        <v>2180</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="679" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>2181</v>
+        <v>2173</v>
       </c>
       <c r="B679" s="3" t="b">
         <v>1</v>
@@ -22401,18 +22398,18 @@
         <v>1</v>
       </c>
       <c r="E679" t="s">
-        <v>2187</v>
+        <v>2182</v>
       </c>
       <c r="F679" s="5" t="s">
-        <v>2193</v>
+        <v>2185</v>
       </c>
       <c r="G679" t="s">
-        <v>2199</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>2182</v>
+        <v>2174</v>
       </c>
       <c r="B680" s="3" t="b">
         <v>1</v>
@@ -22420,19 +22417,19 @@
       <c r="C680" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E680" t="s">
-        <v>2191</v>
+      <c r="E680" s="3" t="s">
+        <v>2179</v>
       </c>
       <c r="F680" s="5" t="s">
-        <v>2194</v>
+        <v>2186</v>
       </c>
       <c r="G680" t="s">
-        <v>2200</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>2183</v>
+        <v>2175</v>
       </c>
       <c r="B681" s="3" t="b">
         <v>1</v>
@@ -22441,18 +22438,18 @@
         <v>1</v>
       </c>
       <c r="E681" s="3" t="s">
-        <v>2188</v>
+        <v>2180</v>
       </c>
       <c r="F681" s="5" t="s">
-        <v>2195</v>
+        <v>2187</v>
       </c>
       <c r="G681" t="s">
-        <v>2201</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="682" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>2184</v>
+        <v>2176</v>
       </c>
       <c r="B682" s="3" t="b">
         <v>1</v>
@@ -22461,18 +22458,18 @@
         <v>1</v>
       </c>
       <c r="E682" s="3" t="s">
-        <v>2189</v>
+        <v>2181</v>
       </c>
       <c r="F682" s="5" t="s">
-        <v>2196</v>
+        <v>2188</v>
       </c>
       <c r="G682" t="s">
-        <v>2202</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="683" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>2185</v>
+        <v>2177</v>
       </c>
       <c r="B683" s="3" t="b">
         <v>1</v>
@@ -22481,18 +22478,18 @@
         <v>1</v>
       </c>
       <c r="E683" s="3" t="s">
-        <v>2190</v>
+        <v>2183</v>
       </c>
       <c r="F683" s="5" t="s">
-        <v>2197</v>
+        <v>2189</v>
       </c>
       <c r="G683" t="s">
-        <v>2203</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="684" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A684" t="s">
-        <v>2186</v>
+      <c r="A684" s="3" t="s">
+        <v>1691</v>
       </c>
       <c r="B684" s="3" t="b">
         <v>1</v>
@@ -22500,19 +22497,20 @@
       <c r="C684" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D684" s="3"/>
       <c r="E684" s="3" t="s">
-        <v>2192</v>
+        <v>1691</v>
       </c>
       <c r="F684" s="5" t="s">
-        <v>2198</v>
-      </c>
-      <c r="G684" t="s">
-        <v>2204</v>
+        <v>2012</v>
+      </c>
+      <c r="G684" s="3" t="s">
+        <v>1728</v>
       </c>
     </row>
     <row r="685" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A685" s="3" t="s">
-        <v>1691</v>
+        <v>2010</v>
       </c>
       <c r="B685" s="3" t="b">
         <v>1</v>
@@ -22522,10 +22520,10 @@
       </c>
       <c r="D685" s="3"/>
       <c r="E685" s="3" t="s">
-        <v>1691</v>
+        <v>2010</v>
       </c>
       <c r="F685" s="5" t="s">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="G685" s="3" t="s">
         <v>1728</v>
@@ -22533,7 +22531,7 @@
     </row>
     <row r="686" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A686" s="3" t="s">
-        <v>2015</v>
+        <v>810</v>
       </c>
       <c r="B686" s="3" t="b">
         <v>1</v>
@@ -22543,18 +22541,18 @@
       </c>
       <c r="D686" s="3"/>
       <c r="E686" s="3" t="s">
-        <v>2015</v>
+        <v>811</v>
       </c>
       <c r="F686" s="5" t="s">
-        <v>2016</v>
+        <v>433</v>
       </c>
       <c r="G686" s="3" t="s">
-        <v>1728</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="687" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A687" s="3" t="s">
-        <v>810</v>
+        <v>823</v>
       </c>
       <c r="B687" s="3" t="b">
         <v>1</v>
@@ -22564,18 +22562,18 @@
       </c>
       <c r="D687" s="3"/>
       <c r="E687" s="3" t="s">
-        <v>811</v>
+        <v>825</v>
       </c>
       <c r="F687" s="5" t="s">
-        <v>433</v>
+        <v>824</v>
       </c>
       <c r="G687" s="3" t="s">
-        <v>1482</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="688" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A688" s="3" t="s">
-        <v>823</v>
+        <v>812</v>
       </c>
       <c r="B688" s="3" t="b">
         <v>1</v>
@@ -22585,18 +22583,18 @@
       </c>
       <c r="D688" s="3"/>
       <c r="E688" s="3" t="s">
-        <v>825</v>
+        <v>803</v>
       </c>
       <c r="F688" s="5" t="s">
-        <v>824</v>
+        <v>813</v>
       </c>
       <c r="G688" s="3" t="s">
-        <v>1486</v>
-      </c>
-    </row>
-    <row r="689" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="689" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A689" s="3" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B689" s="3" t="b">
         <v>1</v>
@@ -22604,20 +22602,19 @@
       <c r="C689" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D689" s="3"/>
       <c r="E689" s="3" t="s">
-        <v>803</v>
+        <v>816</v>
       </c>
       <c r="F689" s="5" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="G689" s="3" t="s">
-        <v>1480</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="690" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A690" s="3" t="s">
-        <v>814</v>
+        <v>2116</v>
       </c>
       <c r="B690" s="3" t="b">
         <v>1</v>
@@ -22626,18 +22623,18 @@
         <v>1</v>
       </c>
       <c r="E690" s="3" t="s">
-        <v>816</v>
+        <v>1674</v>
       </c>
       <c r="F690" s="5" t="s">
-        <v>815</v>
+        <v>826</v>
       </c>
       <c r="G690" s="3" t="s">
-        <v>1483</v>
-      </c>
-    </row>
-    <row r="691" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="691" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A691" s="3" t="s">
-        <v>2121</v>
+        <v>2117</v>
       </c>
       <c r="B691" s="3" t="b">
         <v>1</v>
@@ -22645,19 +22642,20 @@
       <c r="C691" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D691" s="3"/>
       <c r="E691" s="3" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="F691" s="5" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="G691" s="3" t="s">
-        <v>1487</v>
-      </c>
-    </row>
-    <row r="692" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="692" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A692" s="3" t="s">
-        <v>2122</v>
+        <v>2118</v>
       </c>
       <c r="B692" s="3" t="b">
         <v>1</v>
@@ -22665,20 +22663,19 @@
       <c r="C692" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D692" s="3"/>
       <c r="E692" s="3" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="F692" s="5" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="G692" s="3" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="693" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A693" s="3" t="s">
-        <v>2123</v>
+        <v>2119</v>
       </c>
       <c r="B693" s="3" t="b">
         <v>1</v>
@@ -22687,18 +22684,18 @@
         <v>1</v>
       </c>
       <c r="E693" s="3" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="F693" s="5" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="G693" s="3" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="694" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A694" s="3" t="s">
-        <v>2124</v>
+        <v>2120</v>
       </c>
       <c r="B694" s="3" t="b">
         <v>1</v>
@@ -22707,18 +22704,18 @@
         <v>1</v>
       </c>
       <c r="E694" s="3" t="s">
-        <v>1677</v>
+        <v>2121</v>
       </c>
       <c r="F694" s="5" t="s">
-        <v>829</v>
+        <v>2122</v>
       </c>
       <c r="G694" s="3" t="s">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="695" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="695" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A695" s="3" t="s">
-        <v>2125</v>
+        <v>820</v>
       </c>
       <c r="B695" s="3" t="b">
         <v>1</v>
@@ -22726,19 +22723,20 @@
       <c r="C695" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D695" s="3"/>
       <c r="E695" s="3" t="s">
-        <v>2126</v>
+        <v>822</v>
       </c>
       <c r="F695" s="5" t="s">
-        <v>2127</v>
+        <v>821</v>
       </c>
       <c r="G695" s="3" t="s">
-        <v>2128</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="696" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A696" s="3" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="B696" s="3" t="b">
         <v>1</v>
@@ -22748,18 +22746,18 @@
       </c>
       <c r="D696" s="3"/>
       <c r="E696" s="3" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="F696" s="5" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="G696" s="3" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="697" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A697" s="3" t="s">
-        <v>817</v>
+      <c r="A697" t="s">
+        <v>2196</v>
       </c>
       <c r="B697" s="3" t="b">
         <v>1</v>
@@ -22767,20 +22765,19 @@
       <c r="C697" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D697" s="3"/>
-      <c r="E697" s="3" t="s">
-        <v>819</v>
+      <c r="E697" t="s">
+        <v>1693</v>
       </c>
       <c r="F697" s="5" t="s">
-        <v>818</v>
-      </c>
-      <c r="G697" s="3" t="s">
-        <v>1484</v>
+        <v>2201</v>
+      </c>
+      <c r="G697" t="s">
+        <v>1729</v>
       </c>
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>2205</v>
+        <v>2197</v>
       </c>
       <c r="B698" s="3" t="b">
         <v>1</v>
@@ -22788,19 +22785,19 @@
       <c r="C698" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E698" t="s">
-        <v>1693</v>
+      <c r="E698" s="3" t="s">
+        <v>416</v>
       </c>
       <c r="F698" s="5" t="s">
-        <v>2210</v>
+        <v>1701</v>
       </c>
       <c r="G698" t="s">
-        <v>1729</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="699" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A699" t="s">
-        <v>2206</v>
+      <c r="A699" s="3" t="s">
+        <v>2198</v>
       </c>
       <c r="B699" s="3" t="b">
         <v>1</v>
@@ -22809,18 +22806,18 @@
         <v>1</v>
       </c>
       <c r="E699" s="3" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="F699" s="5" t="s">
-        <v>1701</v>
+        <v>2202</v>
       </c>
       <c r="G699" t="s">
-        <v>1349</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="700" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A700" s="3" t="s">
-        <v>2207</v>
+        <v>2199</v>
       </c>
       <c r="B700" s="3" t="b">
         <v>1</v>
@@ -22829,18 +22826,18 @@
         <v>1</v>
       </c>
       <c r="E700" s="3" t="s">
-        <v>422</v>
+        <v>437</v>
       </c>
       <c r="F700" s="5" t="s">
-        <v>2211</v>
+        <v>1699</v>
       </c>
       <c r="G700" t="s">
-        <v>1351</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="701" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A701" s="3" t="s">
-        <v>2208</v>
+      <c r="A701" t="s">
+        <v>2200</v>
       </c>
       <c r="B701" s="3" t="b">
         <v>1</v>
@@ -22849,38 +22846,38 @@
         <v>1</v>
       </c>
       <c r="E701" s="3" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="F701" s="5" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="G701" t="s">
-        <v>1356</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="702" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
+        <v>2203</v>
+      </c>
+      <c r="B702" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C702" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E702" t="s">
+        <v>2205</v>
+      </c>
+      <c r="F702" s="5" t="s">
+        <v>2207</v>
+      </c>
+      <c r="G702" t="s">
         <v>2209</v>
-      </c>
-      <c r="B702" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C702" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E702" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="F702" s="5" t="s">
-        <v>1700</v>
-      </c>
-      <c r="G702" t="s">
-        <v>1353</v>
       </c>
     </row>
     <row r="703" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>2212</v>
+        <v>2204</v>
       </c>
       <c r="B703" s="3" t="b">
         <v>1</v>
@@ -22889,38 +22886,38 @@
         <v>1</v>
       </c>
       <c r="E703" t="s">
-        <v>2214</v>
+        <v>2206</v>
       </c>
       <c r="F703" s="5" t="s">
-        <v>2216</v>
+        <v>2208</v>
       </c>
       <c r="G703" t="s">
-        <v>2218</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="704" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B704" t="b">
+        <v>1</v>
+      </c>
+      <c r="C704" t="b">
+        <v>1</v>
+      </c>
+      <c r="E704" t="s">
+        <v>2212</v>
+      </c>
+      <c r="F704" s="5" t="s">
         <v>2213</v>
       </c>
-      <c r="B704" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C704" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E704" t="s">
-        <v>2215</v>
-      </c>
-      <c r="F704" s="5" t="s">
-        <v>2217</v>
-      </c>
       <c r="G704" t="s">
-        <v>2219</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>2220</v>
+        <v>1996</v>
       </c>
       <c r="B705" t="b">
         <v>1</v>
@@ -22929,38 +22926,41 @@
         <v>1</v>
       </c>
       <c r="E705" t="s">
-        <v>2221</v>
+        <v>1996</v>
       </c>
       <c r="F705" s="5" t="s">
-        <v>2222</v>
-      </c>
-      <c r="G705" t="s">
-        <v>2223</v>
+        <v>1997</v>
+      </c>
+      <c r="G705" s="3" t="s">
+        <v>1998</v>
       </c>
     </row>
     <row r="706" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>1996</v>
+        <v>2224</v>
       </c>
       <c r="B706" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C706" t="b">
         <v>1</v>
       </c>
+      <c r="D706" t="s">
+        <v>2229</v>
+      </c>
       <c r="E706" t="s">
-        <v>1996</v>
+        <v>2224</v>
       </c>
       <c r="F706" s="5" t="s">
-        <v>1997</v>
-      </c>
-      <c r="G706" s="3" t="s">
-        <v>1998</v>
+        <v>2227</v>
+      </c>
+      <c r="G706" t="s">
+        <v>2230</v>
       </c>
     </row>
     <row r="707" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>2233</v>
+        <v>2225</v>
       </c>
       <c r="B707" t="b">
         <v>0</v>
@@ -22969,44 +22969,41 @@
         <v>1</v>
       </c>
       <c r="D707" t="s">
-        <v>2238</v>
+        <v>2229</v>
       </c>
       <c r="E707" t="s">
-        <v>2233</v>
+        <v>2226</v>
       </c>
       <c r="F707" s="5" t="s">
-        <v>2236</v>
+        <v>2228</v>
       </c>
       <c r="G707" t="s">
-        <v>2239</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="708" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
+        <v>2613</v>
+      </c>
+      <c r="B708" t="b">
+        <v>1</v>
+      </c>
+      <c r="C708" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E708" t="s">
+        <v>2617</v>
+      </c>
+      <c r="F708" s="5" t="s">
+        <v>2233</v>
+      </c>
+      <c r="G708" t="s">
         <v>2234</v>
       </c>
-      <c r="B708" t="b">
-        <v>0</v>
-      </c>
-      <c r="C708" t="b">
-        <v>1</v>
-      </c>
-      <c r="D708" t="s">
-        <v>2238</v>
-      </c>
-      <c r="E708" t="s">
-        <v>2235</v>
-      </c>
-      <c r="F708" s="5" t="s">
-        <v>2237</v>
-      </c>
-      <c r="G708" t="s">
-        <v>2240</v>
-      </c>
     </row>
     <row r="709" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A709" t="s">
-        <v>2246</v>
+      <c r="A709" s="3" t="s">
+        <v>2614</v>
       </c>
       <c r="B709" t="b">
         <v>1</v>
@@ -23015,38 +23012,38 @@
         <v>1</v>
       </c>
       <c r="E709" t="s">
-        <v>2244</v>
+        <v>2618</v>
       </c>
       <c r="F709" s="5" t="s">
-        <v>2248</v>
+        <v>2232</v>
       </c>
       <c r="G709" t="s">
-        <v>2249</v>
-      </c>
-    </row>
-    <row r="710" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="710" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A710" s="3" t="s">
-        <v>2241</v>
-      </c>
-      <c r="B710" t="b">
+        <v>2615</v>
+      </c>
+      <c r="B710" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C710" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E710" t="s">
-        <v>2245</v>
+      <c r="E710" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="F710" s="5" t="s">
-        <v>2247</v>
-      </c>
-      <c r="G710" t="s">
-        <v>2249</v>
+        <v>319</v>
+      </c>
+      <c r="G710" s="3" t="s">
+        <v>1316</v>
       </c>
     </row>
     <row r="711" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A711" s="3" t="s">
-        <v>2242</v>
+        <v>2616</v>
       </c>
       <c r="B711" s="3" t="b">
         <v>1</v>
@@ -23055,58 +23052,58 @@
         <v>1</v>
       </c>
       <c r="E711" s="3" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="F711" s="5" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="G711" s="3" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="712" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A712" s="3" t="s">
-        <v>2243</v>
-      </c>
-      <c r="B712" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C712" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E712" s="3" t="s">
-        <v>323</v>
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="712" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A712" t="s">
+        <v>2313</v>
+      </c>
+      <c r="B712" t="b">
+        <v>1</v>
+      </c>
+      <c r="C712" t="b">
+        <v>1</v>
+      </c>
+      <c r="E712" t="s">
+        <v>2302</v>
       </c>
       <c r="F712" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="G712" s="3" t="s">
-        <v>1317</v>
+        <v>2303</v>
+      </c>
+      <c r="G712" t="s">
+        <v>2325</v>
       </c>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>2329</v>
+        <v>2315</v>
       </c>
       <c r="B713" t="b">
         <v>1</v>
       </c>
       <c r="C713" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E713" t="s">
-        <v>2318</v>
+        <v>2314</v>
       </c>
       <c r="F713" s="5" t="s">
-        <v>2319</v>
+        <v>2316</v>
       </c>
       <c r="G713" t="s">
-        <v>2341</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="714" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>2331</v>
+        <v>2319</v>
       </c>
       <c r="B714" t="b">
         <v>1</v>
@@ -23115,58 +23112,58 @@
         <v>0</v>
       </c>
       <c r="E714" t="s">
-        <v>2330</v>
+        <v>2317</v>
       </c>
       <c r="F714" s="5" t="s">
+        <v>2318</v>
+      </c>
+      <c r="G714" t="s">
+        <v>2327</v>
+      </c>
+    </row>
+    <row r="715" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A715" s="3" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B715" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C715" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E715" s="3" t="s">
+        <v>2323</v>
+      </c>
+      <c r="F715" s="5" t="s">
+        <v>2324</v>
+      </c>
+      <c r="G715" s="3" t="s">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="716" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A716" t="s">
+        <v>2329</v>
+      </c>
+      <c r="B716" t="b">
+        <v>0</v>
+      </c>
+      <c r="C716" t="b">
+        <v>1</v>
+      </c>
+      <c r="E716" t="s">
         <v>2332</v>
       </c>
-      <c r="G714" t="s">
+      <c r="F716" s="5" t="s">
+        <v>2333</v>
+      </c>
+      <c r="G716" t="s">
         <v>2342</v>
-      </c>
-    </row>
-    <row r="715" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A715" t="s">
-        <v>2335</v>
-      </c>
-      <c r="B715" t="b">
-        <v>1</v>
-      </c>
-      <c r="C715" t="b">
-        <v>0</v>
-      </c>
-      <c r="E715" t="s">
-        <v>2333</v>
-      </c>
-      <c r="F715" s="5" t="s">
-        <v>2334</v>
-      </c>
-      <c r="G715" t="s">
-        <v>2343</v>
-      </c>
-    </row>
-    <row r="716" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A716" s="3" t="s">
-        <v>2338</v>
-      </c>
-      <c r="B716" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C716" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E716" s="3" t="s">
-        <v>2339</v>
-      </c>
-      <c r="F716" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="G716" s="3" t="s">
-        <v>2344</v>
       </c>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>2345</v>
+        <v>2330</v>
       </c>
       <c r="B717" t="b">
         <v>0</v>
@@ -23175,58 +23172,58 @@
         <v>1</v>
       </c>
       <c r="E717" t="s">
-        <v>2348</v>
+        <v>2331</v>
       </c>
       <c r="F717" s="5" t="s">
-        <v>2349</v>
+        <v>2334</v>
       </c>
       <c r="G717" t="s">
-        <v>2358</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="718" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>2346</v>
+        <v>2336</v>
       </c>
       <c r="B718" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C718" t="b">
         <v>1</v>
       </c>
       <c r="E718" t="s">
-        <v>2347</v>
+        <v>2338</v>
       </c>
       <c r="F718" s="5" t="s">
-        <v>2350</v>
+        <v>2341</v>
       </c>
       <c r="G718" t="s">
-        <v>2359</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>2352</v>
-      </c>
-      <c r="B719" t="b">
-        <v>1</v>
-      </c>
-      <c r="C719" t="b">
+        <v>2337</v>
+      </c>
+      <c r="B719" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C719" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E719" t="s">
-        <v>2354</v>
+        <v>493</v>
       </c>
       <c r="F719" s="5" t="s">
-        <v>2357</v>
+        <v>492</v>
       </c>
       <c r="G719" t="s">
-        <v>2360</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>2353</v>
+        <v>2400</v>
       </c>
       <c r="B720" s="3" t="b">
         <v>1</v>
@@ -23235,38 +23232,41 @@
         <v>1</v>
       </c>
       <c r="E720" t="s">
-        <v>493</v>
+        <v>2339</v>
       </c>
       <c r="F720" s="5" t="s">
-        <v>492</v>
+        <v>2340</v>
       </c>
       <c r="G720" t="s">
-        <v>1377</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>2416</v>
-      </c>
-      <c r="B721" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C721" s="3" t="b">
-        <v>1</v>
+        <v>2348</v>
+      </c>
+      <c r="B721" t="b">
+        <v>0</v>
+      </c>
+      <c r="C721" t="b">
+        <v>1</v>
+      </c>
+      <c r="D721" t="s">
+        <v>2349</v>
       </c>
       <c r="E721" t="s">
-        <v>2355</v>
+        <v>2351</v>
       </c>
       <c r="F721" s="5" t="s">
+        <v>2350</v>
+      </c>
+      <c r="G721" s="3" t="s">
         <v>2356</v>
-      </c>
-      <c r="G721" t="s">
-        <v>2361</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>2364</v>
+        <v>2381</v>
       </c>
       <c r="B722" t="b">
         <v>0</v>
@@ -23274,22 +23274,19 @@
       <c r="C722" t="b">
         <v>1</v>
       </c>
-      <c r="D722" t="s">
-        <v>2365</v>
-      </c>
       <c r="E722" t="s">
-        <v>2367</v>
+        <v>2382</v>
       </c>
       <c r="F722" s="5" t="s">
-        <v>2366</v>
-      </c>
-      <c r="G722" s="3" t="s">
-        <v>2372</v>
+        <v>2398</v>
+      </c>
+      <c r="G722" t="s">
+        <v>2393</v>
       </c>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>2397</v>
+        <v>2383</v>
       </c>
       <c r="B723" t="b">
         <v>0</v>
@@ -23298,58 +23295,58 @@
         <v>1</v>
       </c>
       <c r="E723" t="s">
-        <v>2398</v>
+        <v>2399</v>
       </c>
       <c r="F723" s="5" t="s">
-        <v>2414</v>
+        <v>2386</v>
       </c>
       <c r="G723" t="s">
-        <v>2409</v>
-      </c>
-    </row>
-    <row r="724" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A724" t="s">
-        <v>2399</v>
-      </c>
-      <c r="B724" t="b">
-        <v>0</v>
-      </c>
-      <c r="C724" t="b">
-        <v>1</v>
-      </c>
-      <c r="E724" t="s">
-        <v>2415</v>
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="724" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A724" s="3" t="s">
+        <v>2389</v>
+      </c>
+      <c r="B724" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C724" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E724" s="3" t="s">
+        <v>2390</v>
       </c>
       <c r="F724" s="5" t="s">
-        <v>2402</v>
-      </c>
-      <c r="G724" t="s">
-        <v>2410</v>
-      </c>
-    </row>
-    <row r="725" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A725" s="3" t="s">
-        <v>2405</v>
-      </c>
-      <c r="B725" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C725" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E725" s="3" t="s">
-        <v>2406</v>
+        <v>2391</v>
+      </c>
+      <c r="G724" s="3" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="725" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A725" t="s">
+        <v>2384</v>
+      </c>
+      <c r="B725" t="b">
+        <v>0</v>
+      </c>
+      <c r="C725" t="b">
+        <v>1</v>
+      </c>
+      <c r="E725" t="s">
+        <v>2384</v>
       </c>
       <c r="F725" s="5" t="s">
-        <v>2407</v>
-      </c>
-      <c r="G725" s="3" t="s">
-        <v>2411</v>
+        <v>2385</v>
+      </c>
+      <c r="G725" t="s">
+        <v>2396</v>
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>2400</v>
+        <v>2388</v>
       </c>
       <c r="B726" t="b">
         <v>0</v>
@@ -23358,18 +23355,18 @@
         <v>1</v>
       </c>
       <c r="E726" t="s">
-        <v>2400</v>
+        <v>2387</v>
       </c>
       <c r="F726" s="5" t="s">
-        <v>2401</v>
+        <v>2392</v>
       </c>
       <c r="G726" t="s">
-        <v>2412</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>2404</v>
+        <v>496</v>
       </c>
       <c r="B727" t="b">
         <v>0</v>
@@ -23378,18 +23375,18 @@
         <v>1</v>
       </c>
       <c r="E727" t="s">
-        <v>2403</v>
+        <v>496</v>
       </c>
       <c r="F727" s="5" t="s">
-        <v>2408</v>
+        <v>495</v>
       </c>
       <c r="G727" t="s">
-        <v>2413</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>496</v>
+        <v>2465</v>
       </c>
       <c r="B728" t="b">
         <v>0</v>
@@ -23398,18 +23395,18 @@
         <v>1</v>
       </c>
       <c r="E728" t="s">
-        <v>496</v>
+        <v>2465</v>
       </c>
       <c r="F728" s="5" t="s">
-        <v>495</v>
+        <v>2466</v>
       </c>
       <c r="G728" t="s">
-        <v>1378</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>2482</v>
+        <v>2476</v>
       </c>
       <c r="B729" t="b">
         <v>0</v>
@@ -23418,58 +23415,58 @@
         <v>1</v>
       </c>
       <c r="E729" t="s">
-        <v>2482</v>
+        <v>2477</v>
       </c>
       <c r="F729" s="5" t="s">
-        <v>2483</v>
+        <v>2480</v>
       </c>
       <c r="G729" t="s">
-        <v>2495</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>2493</v>
+        <v>2540</v>
       </c>
       <c r="B730" t="b">
-        <v>0</v>
-      </c>
-      <c r="C730" t="b">
+        <v>1</v>
+      </c>
+      <c r="C730" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E730" t="s">
-        <v>2494</v>
+        <v>2481</v>
       </c>
       <c r="F730" s="5" t="s">
-        <v>2497</v>
+        <v>2488</v>
       </c>
       <c r="G730" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>2557</v>
-      </c>
-      <c r="B731" t="b">
+        <v>2541</v>
+      </c>
+      <c r="B731" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C731" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E731" t="s">
-        <v>2498</v>
+        <v>2482</v>
       </c>
       <c r="F731" s="5" t="s">
-        <v>2505</v>
+        <v>2489</v>
       </c>
       <c r="G731" t="s">
-        <v>2512</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="732" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>2558</v>
+        <v>2542</v>
       </c>
       <c r="B732" s="3" t="b">
         <v>1</v>
@@ -23478,18 +23475,18 @@
         <v>1</v>
       </c>
       <c r="E732" t="s">
-        <v>2499</v>
+        <v>2483</v>
       </c>
       <c r="F732" s="5" t="s">
-        <v>2506</v>
+        <v>2490</v>
       </c>
       <c r="G732" t="s">
-        <v>2518</v>
+        <v>2496</v>
       </c>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>2559</v>
+        <v>2543</v>
       </c>
       <c r="B733" s="3" t="b">
         <v>1</v>
@@ -23498,18 +23495,18 @@
         <v>1</v>
       </c>
       <c r="E733" t="s">
-        <v>2500</v>
+        <v>2485</v>
       </c>
       <c r="F733" s="5" t="s">
-        <v>2507</v>
+        <v>2492</v>
       </c>
       <c r="G733" t="s">
-        <v>2513</v>
+        <v>2497</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>2560</v>
+        <v>2544</v>
       </c>
       <c r="B734" s="3" t="b">
         <v>1</v>
@@ -23518,18 +23515,18 @@
         <v>1</v>
       </c>
       <c r="E734" t="s">
-        <v>2502</v>
+        <v>2486</v>
       </c>
       <c r="F734" s="5" t="s">
-        <v>2509</v>
+        <v>2493</v>
       </c>
       <c r="G734" t="s">
-        <v>2514</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>2561</v>
+        <v>2545</v>
       </c>
       <c r="B735" s="3" t="b">
         <v>1</v>
@@ -23538,18 +23535,18 @@
         <v>1</v>
       </c>
       <c r="E735" t="s">
-        <v>2503</v>
+        <v>2484</v>
       </c>
       <c r="F735" s="5" t="s">
-        <v>2510</v>
+        <v>2491</v>
       </c>
       <c r="G735" t="s">
-        <v>2515</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="736" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>2562</v>
+        <v>2546</v>
       </c>
       <c r="B736" s="3" t="b">
         <v>1</v>
@@ -23558,38 +23555,38 @@
         <v>1</v>
       </c>
       <c r="E736" t="s">
-        <v>2501</v>
+        <v>2487</v>
       </c>
       <c r="F736" s="5" t="s">
-        <v>2508</v>
+        <v>2494</v>
       </c>
       <c r="G736" t="s">
-        <v>2516</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>2563</v>
-      </c>
-      <c r="B737" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C737" s="3" t="b">
+        <v>2562</v>
+      </c>
+      <c r="B737" t="b">
+        <v>1</v>
+      </c>
+      <c r="C737" t="b">
         <v>1</v>
       </c>
       <c r="E737" t="s">
-        <v>2504</v>
+        <v>2564</v>
       </c>
       <c r="F737" s="5" t="s">
-        <v>2511</v>
+        <v>2566</v>
       </c>
       <c r="G737" t="s">
-        <v>2517</v>
+        <v>2568</v>
       </c>
     </row>
     <row r="738" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>2579</v>
+        <v>2563</v>
       </c>
       <c r="B738" t="b">
         <v>1</v>
@@ -23598,18 +23595,18 @@
         <v>1</v>
       </c>
       <c r="E738" t="s">
-        <v>2581</v>
+        <v>2565</v>
       </c>
       <c r="F738" s="5" t="s">
-        <v>2583</v>
+        <v>2567</v>
       </c>
       <c r="G738" t="s">
-        <v>2585</v>
+        <v>2569</v>
       </c>
     </row>
     <row r="739" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>2580</v>
+        <v>2570</v>
       </c>
       <c r="B739" t="b">
         <v>1</v>
@@ -23618,18 +23615,18 @@
         <v>1</v>
       </c>
       <c r="E739" t="s">
-        <v>2582</v>
+        <v>2571</v>
       </c>
       <c r="F739" s="5" t="s">
-        <v>2584</v>
+        <v>2572</v>
       </c>
       <c r="G739" t="s">
-        <v>2586</v>
+        <v>2575</v>
       </c>
     </row>
     <row r="740" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>2587</v>
+        <v>2573</v>
       </c>
       <c r="B740" t="b">
         <v>1</v>
@@ -23638,38 +23635,38 @@
         <v>1</v>
       </c>
       <c r="E740" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
       <c r="F740" s="5" t="s">
-        <v>2589</v>
+        <v>2574</v>
       </c>
       <c r="G740" t="s">
-        <v>2592</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="741" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>2590</v>
+        <v>2583</v>
       </c>
       <c r="B741" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C741" t="b">
         <v>1</v>
       </c>
       <c r="E741" t="s">
-        <v>2603</v>
+        <v>2584</v>
       </c>
       <c r="F741" s="5" t="s">
-        <v>2591</v>
+        <v>2585</v>
       </c>
       <c r="G741" t="s">
-        <v>2593</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="742" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>2600</v>
+        <v>2609</v>
       </c>
       <c r="B742" t="b">
         <v>0</v>
@@ -23678,17 +23675,17 @@
         <v>1</v>
       </c>
       <c r="E742" t="s">
-        <v>2601</v>
+        <v>2609</v>
       </c>
       <c r="F742" s="5" t="s">
-        <v>2602</v>
+        <v>1088</v>
       </c>
       <c r="G742" t="s">
-        <v>2578</v>
+        <v>2610</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G728" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G727" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adjusted the service layer and front end to some design changes
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\BSharp\Translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B991F2-ADF2-4229-9CE3-92DB54DA3522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CF851B-07D3-4EBE-AD6B-AF22C513AF7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2946" uniqueCount="2606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2946" uniqueCount="2604">
   <si>
     <t>Key</t>
   </si>
@@ -6693,12 +6693,6 @@
     <t>进入分类</t>
   </si>
   <si>
-    <t>Line_ExternalReference</t>
-  </si>
-  <si>
-    <t>Line_AdditionalReference</t>
-  </si>
-  <si>
     <t>Entry_Account</t>
   </si>
   <si>
@@ -6756,15 +6750,6 @@
     <t>Line_Resource</t>
   </si>
   <si>
-    <t>Line_Amount</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>المبلغ</t>
-  </si>
-  <si>
     <t>Entry_ContractType</t>
   </si>
   <si>
@@ -7806,18 +7791,6 @@
     <t>高级</t>
   </si>
   <si>
-    <t>Line_NotedAgent</t>
-  </si>
-  <si>
-    <t>Line_NotedAgentName</t>
-  </si>
-  <si>
-    <t>Line_NotedAmount</t>
-  </si>
-  <si>
-    <t>Line_NotedDate</t>
-  </si>
-  <si>
     <t>Noted Agent</t>
   </si>
   <si>
@@ -7852,6 +7825,27 @@
   </si>
   <si>
     <t>مربتط بتاريخ معني</t>
+  </si>
+  <si>
+    <t>Line_MonetaryValue</t>
+  </si>
+  <si>
+    <t>Entry_ExternalReference</t>
+  </si>
+  <si>
+    <t>Entry_AdditionalReference</t>
+  </si>
+  <si>
+    <t>Entry_NotedAgent</t>
+  </si>
+  <si>
+    <t>Entry_NotedAgentName</t>
+  </si>
+  <si>
+    <t>Entry_NotedAmount</t>
+  </si>
+  <si>
+    <t>Entry_NotedDate</t>
   </si>
 </sst>
 </file>
@@ -8251,9 +8245,9 @@
   <dimension ref="A1:G735"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F555" sqref="F555"/>
+      <selection pane="bottomLeft" activeCell="A496" sqref="A496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8700,10 +8694,10 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>2302</v>
+        <v>2297</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>2288</v>
+        <v>2283</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>1620</v>
@@ -9204,10 +9198,10 @@
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>2387</v>
+        <v>2382</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>2388</v>
+        <v>2383</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>1236</v>
@@ -9225,10 +9219,10 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>2390</v>
+        <v>2385</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>2389</v>
+        <v>2384</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>1626</v>
@@ -15514,7 +15508,7 @@
     </row>
     <row r="346" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
-        <v>2274</v>
+        <v>2269</v>
       </c>
       <c r="B346" s="3" t="b">
         <v>1</v>
@@ -15523,10 +15517,10 @@
         <v>1</v>
       </c>
       <c r="E346" s="3" t="s">
-        <v>2275</v>
+        <v>2270</v>
       </c>
       <c r="F346" s="5" t="s">
-        <v>2278</v>
+        <v>2273</v>
       </c>
       <c r="G346" s="3" t="s">
         <v>2206</v>
@@ -15534,7 +15528,7 @@
     </row>
     <row r="347" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
-        <v>2271</v>
+        <v>2266</v>
       </c>
       <c r="B347" s="3" t="b">
         <v>1</v>
@@ -15543,15 +15537,15 @@
         <v>1</v>
       </c>
       <c r="E347" s="3" t="s">
-        <v>2272</v>
+        <v>2267</v>
       </c>
       <c r="F347" s="5" t="s">
-        <v>2273</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="348" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="s">
-        <v>2276</v>
+        <v>2271</v>
       </c>
       <c r="B348" s="3" t="b">
         <v>1</v>
@@ -15560,15 +15554,15 @@
         <v>1</v>
       </c>
       <c r="E348" s="3" t="s">
-        <v>2277</v>
+        <v>2272</v>
       </c>
       <c r="F348" s="5" t="s">
-        <v>2279</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="s">
-        <v>2436</v>
+        <v>2431</v>
       </c>
       <c r="B349" s="3" t="b">
         <v>0</v>
@@ -15589,7 +15583,7 @@
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>2437</v>
+        <v>2432</v>
       </c>
       <c r="B350" s="3" t="b">
         <v>0</v>
@@ -15610,7 +15604,7 @@
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
-        <v>2438</v>
+        <v>2433</v>
       </c>
       <c r="B351" s="3" t="b">
         <v>0</v>
@@ -15631,7 +15625,7 @@
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
-        <v>2439</v>
+        <v>2434</v>
       </c>
       <c r="B352" s="3" t="b">
         <v>0</v>
@@ -15652,7 +15646,7 @@
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="s">
-        <v>2440</v>
+        <v>2435</v>
       </c>
       <c r="B353" s="3" t="b">
         <v>0</v>
@@ -15673,7 +15667,7 @@
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
-        <v>2441</v>
+        <v>2436</v>
       </c>
       <c r="B354" s="3" t="b">
         <v>0</v>
@@ -15694,7 +15688,7 @@
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" s="3" t="s">
-        <v>2442</v>
+        <v>2437</v>
       </c>
       <c r="B355" s="3" t="b">
         <v>0</v>
@@ -15724,10 +15718,10 @@
         <v>1</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>2418</v>
+        <v>2413</v>
       </c>
       <c r="F356" s="5" t="s">
-        <v>2425</v>
+        <v>2420</v>
       </c>
       <c r="G356" s="3" t="s">
         <v>1574</v>
@@ -15744,10 +15738,10 @@
         <v>1</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>2419</v>
+        <v>2414</v>
       </c>
       <c r="F357" s="5" t="s">
-        <v>2426</v>
+        <v>2421</v>
       </c>
       <c r="G357" s="3" t="s">
         <v>1575</v>
@@ -15764,10 +15758,10 @@
         <v>1</v>
       </c>
       <c r="E358" s="3" t="s">
-        <v>2420</v>
+        <v>2415</v>
       </c>
       <c r="F358" s="5" t="s">
-        <v>2427</v>
+        <v>2422</v>
       </c>
       <c r="G358" s="3" t="s">
         <v>1576</v>
@@ -15784,10 +15778,10 @@
         <v>1</v>
       </c>
       <c r="E359" s="3" t="s">
-        <v>2421</v>
+        <v>2416</v>
       </c>
       <c r="F359" s="5" t="s">
-        <v>2428</v>
+        <v>2423</v>
       </c>
       <c r="G359" s="3" t="s">
         <v>1577</v>
@@ -15804,10 +15798,10 @@
         <v>1</v>
       </c>
       <c r="E360" s="3" t="s">
-        <v>2422</v>
+        <v>2417</v>
       </c>
       <c r="F360" s="5" t="s">
-        <v>2429</v>
+        <v>2424</v>
       </c>
       <c r="G360" s="3" t="s">
         <v>1578</v>
@@ -15824,10 +15818,10 @@
         <v>1</v>
       </c>
       <c r="E361" s="3" t="s">
-        <v>2423</v>
+        <v>2418</v>
       </c>
       <c r="F361" s="5" t="s">
-        <v>2430</v>
+        <v>2425</v>
       </c>
       <c r="G361" s="3" t="s">
         <v>1579</v>
@@ -15844,10 +15838,10 @@
         <v>1</v>
       </c>
       <c r="E362" s="3" t="s">
-        <v>2424</v>
+        <v>2419</v>
       </c>
       <c r="F362" s="5" t="s">
-        <v>2431</v>
+        <v>2426</v>
       </c>
       <c r="G362" s="3" t="s">
         <v>1580</v>
@@ -16107,7 +16101,7 @@
     </row>
     <row r="375" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3" t="s">
-        <v>2434</v>
+        <v>2429</v>
       </c>
       <c r="B375" s="3" t="b">
         <v>1</v>
@@ -16116,18 +16110,18 @@
         <v>1</v>
       </c>
       <c r="E375" s="3" t="s">
-        <v>2443</v>
+        <v>2438</v>
       </c>
       <c r="F375" s="5" t="s">
-        <v>2447</v>
+        <v>2442</v>
       </c>
       <c r="G375" s="3" t="s">
-        <v>2451</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="376" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3" t="s">
-        <v>2432</v>
+        <v>2427</v>
       </c>
       <c r="B376" s="3" t="b">
         <v>1</v>
@@ -16136,18 +16130,18 @@
         <v>1</v>
       </c>
       <c r="E376" s="3" t="s">
-        <v>2444</v>
+        <v>2439</v>
       </c>
       <c r="F376" s="5" t="s">
-        <v>2448</v>
+        <v>2443</v>
       </c>
       <c r="G376" s="3" t="s">
-        <v>2452</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="377" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="s">
-        <v>2433</v>
+        <v>2428</v>
       </c>
       <c r="B377" s="3" t="b">
         <v>1</v>
@@ -16156,18 +16150,18 @@
         <v>1</v>
       </c>
       <c r="E377" s="3" t="s">
-        <v>2445</v>
+        <v>2440</v>
       </c>
       <c r="F377" s="5" t="s">
-        <v>2449</v>
+        <v>2444</v>
       </c>
       <c r="G377" s="3" t="s">
-        <v>2453</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="378" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3" t="s">
-        <v>2435</v>
+        <v>2430</v>
       </c>
       <c r="B378" s="3" t="b">
         <v>1</v>
@@ -16176,13 +16170,13 @@
         <v>1</v>
       </c>
       <c r="E378" s="3" t="s">
-        <v>2446</v>
+        <v>2441</v>
       </c>
       <c r="F378" s="5" t="s">
-        <v>2450</v>
+        <v>2445</v>
       </c>
       <c r="G378" s="3" t="s">
-        <v>2454</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
@@ -16859,7 +16853,7 @@
     </row>
     <row r="411" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
-        <v>2386</v>
+        <v>2381</v>
       </c>
       <c r="B411" s="3" t="b">
         <v>1</v>
@@ -17802,7 +17796,7 @@
     </row>
     <row r="456" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A456" s="3" t="s">
-        <v>2319</v>
+        <v>2314</v>
       </c>
       <c r="B456" s="3" t="b">
         <v>1</v>
@@ -17811,18 +17805,18 @@
         <v>1</v>
       </c>
       <c r="E456" s="3" t="s">
-        <v>2319</v>
+        <v>2314</v>
       </c>
       <c r="F456" s="5" t="s">
-        <v>2321</v>
+        <v>2316</v>
       </c>
       <c r="G456" s="3" t="s">
-        <v>2323</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="457" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A457" s="3" t="s">
-        <v>2320</v>
+        <v>2315</v>
       </c>
       <c r="B457" s="3" t="b">
         <v>1</v>
@@ -17831,13 +17825,13 @@
         <v>1</v>
       </c>
       <c r="E457" s="3" t="s">
-        <v>2320</v>
+        <v>2315</v>
       </c>
       <c r="F457" s="5" t="s">
-        <v>2322</v>
+        <v>2317</v>
       </c>
       <c r="G457" s="3" t="s">
-        <v>2324</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.25">
@@ -17858,7 +17852,7 @@
         <v>1635</v>
       </c>
       <c r="G458" s="3" t="s">
-        <v>2318</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="459" spans="1:7" x14ac:dyDescent="0.25">
@@ -18073,7 +18067,7 @@
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A469" s="3" t="s">
-        <v>2231</v>
+        <v>2229</v>
       </c>
       <c r="B469" s="3" t="b">
         <v>1</v>
@@ -18083,10 +18077,10 @@
       </c>
       <c r="D469" s="3"/>
       <c r="E469" s="3" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
       <c r="F469" s="5" t="s">
-        <v>2233</v>
+        <v>2231</v>
       </c>
       <c r="G469" s="3" t="s">
         <v>1712</v>
@@ -18094,19 +18088,19 @@
     </row>
     <row r="470" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A470" s="3" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B470" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C470" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E470" s="3" t="s">
+        <v>2233</v>
+      </c>
+      <c r="F470" s="5" t="s">
         <v>2234</v>
-      </c>
-      <c r="B470" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C470" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E470" s="3" t="s">
-        <v>2235</v>
-      </c>
-      <c r="F470" s="5" t="s">
-        <v>2236</v>
       </c>
       <c r="G470" s="3" t="s">
         <v>1817</v>
@@ -18282,7 +18276,7 @@
     </row>
     <row r="479" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
-        <v>2313</v>
+        <v>2308</v>
       </c>
       <c r="B479" s="3" t="b">
         <v>1</v>
@@ -18294,7 +18288,7 @@
         <v>619</v>
       </c>
       <c r="F479" s="5" t="s">
-        <v>2314</v>
+        <v>2309</v>
       </c>
       <c r="G479" s="3" t="s">
         <v>1419</v>
@@ -18302,7 +18296,7 @@
     </row>
     <row r="480" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A480" s="3" t="s">
-        <v>2325</v>
+        <v>2320</v>
       </c>
       <c r="B480" s="3" t="b">
         <v>1</v>
@@ -18311,10 +18305,10 @@
         <v>1</v>
       </c>
       <c r="E480" s="3" t="s">
-        <v>2331</v>
+        <v>2326</v>
       </c>
       <c r="F480" s="5" t="s">
-        <v>2342</v>
+        <v>2337</v>
       </c>
       <c r="G480" s="3" t="s">
         <v>1212</v>
@@ -18322,67 +18316,67 @@
     </row>
     <row r="481" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B481" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C481" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E481" s="3" t="s">
         <v>2327</v>
       </c>
-      <c r="B481" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C481" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E481" s="3" t="s">
-        <v>2332</v>
-      </c>
       <c r="F481" s="5" t="s">
-        <v>2340</v>
+        <v>2335</v>
       </c>
       <c r="G481" s="3" t="s">
-        <v>2343</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="482" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A482" s="3" t="s">
+        <v>2323</v>
+      </c>
+      <c r="B482" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C482" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E482" s="3" t="s">
         <v>2328</v>
       </c>
-      <c r="B482" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C482" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E482" s="3" t="s">
-        <v>2333</v>
-      </c>
       <c r="F482" s="5" t="s">
-        <v>2341</v>
+        <v>2336</v>
       </c>
       <c r="G482" s="3" t="s">
-        <v>2344</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="483" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A483" s="3" t="s">
+        <v>2324</v>
+      </c>
+      <c r="B483" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C483" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E483" s="3" t="s">
         <v>2329</v>
       </c>
-      <c r="B483" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C483" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E483" s="3" t="s">
+      <c r="F483" s="5" t="s">
         <v>2334</v>
       </c>
-      <c r="F483" s="5" t="s">
-        <v>2339</v>
-      </c>
       <c r="G483" s="3" t="s">
-        <v>2345</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="484" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A484" s="3" t="s">
-        <v>2326</v>
+        <v>2321</v>
       </c>
       <c r="B484" s="3" t="b">
         <v>1</v>
@@ -18391,18 +18385,18 @@
         <v>1</v>
       </c>
       <c r="E484" s="3" t="s">
-        <v>2335</v>
+        <v>2330</v>
       </c>
       <c r="F484" s="5" t="s">
-        <v>2338</v>
+        <v>2333</v>
       </c>
       <c r="G484" s="3" t="s">
-        <v>2346</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="485" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A485" s="3" t="s">
-        <v>2330</v>
+        <v>2325</v>
       </c>
       <c r="B485" s="3" t="b">
         <v>1</v>
@@ -18411,18 +18405,18 @@
         <v>1</v>
       </c>
       <c r="E485" s="3" t="s">
-        <v>2337</v>
+        <v>2332</v>
       </c>
       <c r="F485" s="5" t="s">
-        <v>2336</v>
+        <v>2331</v>
       </c>
       <c r="G485" s="3" t="s">
-        <v>2347</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="486" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A486" s="3" t="s">
-        <v>2237</v>
+        <v>2235</v>
       </c>
       <c r="B486" s="3" t="b">
         <v>1</v>
@@ -18442,7 +18436,7 @@
     </row>
     <row r="487" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A487" s="3" t="s">
-        <v>2238</v>
+        <v>2236</v>
       </c>
       <c r="B487" s="3" t="b">
         <v>1</v>
@@ -18462,7 +18456,7 @@
     </row>
     <row r="488" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A488" s="3" t="s">
-        <v>2239</v>
+        <v>2237</v>
       </c>
       <c r="B488" s="3" t="b">
         <v>1</v>
@@ -18482,7 +18476,7 @@
     </row>
     <row r="489" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A489" s="3" t="s">
-        <v>2240</v>
+        <v>2597</v>
       </c>
       <c r="B489" s="3" t="b">
         <v>1</v>
@@ -18491,18 +18485,18 @@
         <v>1</v>
       </c>
       <c r="E489" s="3" t="s">
-        <v>2241</v>
+        <v>1690</v>
       </c>
       <c r="F489" s="5" t="s">
+        <v>1694</v>
+      </c>
+      <c r="G489" s="3" t="s">
         <v>2242</v>
-      </c>
-      <c r="G489" s="3" t="s">
-        <v>2247</v>
       </c>
     </row>
     <row r="490" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
-        <v>2219</v>
+        <v>2598</v>
       </c>
       <c r="B490" s="3" t="b">
         <v>1</v>
@@ -18514,7 +18508,7 @@
         <v>1686</v>
       </c>
       <c r="F490" s="5" t="s">
-        <v>2258</v>
+        <v>2253</v>
       </c>
       <c r="G490" s="3" t="s">
         <v>1721</v>
@@ -18522,7 +18516,7 @@
     </row>
     <row r="491" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A491" s="3" t="s">
-        <v>2220</v>
+        <v>2599</v>
       </c>
       <c r="B491" s="3" t="b">
         <v>1</v>
@@ -18534,7 +18528,7 @@
         <v>1687</v>
       </c>
       <c r="F491" s="5" t="s">
-        <v>2259</v>
+        <v>2254</v>
       </c>
       <c r="G491" s="3" t="s">
         <v>1722</v>
@@ -18542,7 +18536,7 @@
     </row>
     <row r="492" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A492" s="3" t="s">
-        <v>2590</v>
+        <v>2600</v>
       </c>
       <c r="B492" s="3" t="b">
         <v>1</v>
@@ -18551,18 +18545,18 @@
         <v>1</v>
       </c>
       <c r="E492" s="3" t="s">
-        <v>2594</v>
+        <v>2585</v>
       </c>
       <c r="F492" s="5" t="s">
-        <v>2600</v>
+        <v>2591</v>
       </c>
       <c r="G492" s="3" t="s">
-        <v>2263</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="493" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A493" s="3" t="s">
-        <v>2591</v>
+        <v>2601</v>
       </c>
       <c r="B493" s="3" t="b">
         <v>1</v>
@@ -18571,18 +18565,18 @@
         <v>1</v>
       </c>
       <c r="E493" s="3" t="s">
-        <v>2595</v>
+        <v>2586</v>
       </c>
       <c r="F493" s="5" t="s">
-        <v>2599</v>
+        <v>2590</v>
       </c>
       <c r="G493" s="3" t="s">
-        <v>2264</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="494" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A494" s="3" t="s">
-        <v>2592</v>
+        <v>2602</v>
       </c>
       <c r="B494" s="3" t="b">
         <v>1</v>
@@ -18591,18 +18585,18 @@
         <v>1</v>
       </c>
       <c r="E494" s="3" t="s">
-        <v>2596</v>
+        <v>2587</v>
       </c>
       <c r="F494" s="5" t="s">
-        <v>2598</v>
+        <v>2589</v>
       </c>
       <c r="G494" s="3" t="s">
-        <v>2265</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="495" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A495" s="3" t="s">
-        <v>2593</v>
+        <v>2603</v>
       </c>
       <c r="B495" s="3" t="b">
         <v>1</v>
@@ -18611,18 +18605,18 @@
         <v>1</v>
       </c>
       <c r="E495" s="3" t="s">
-        <v>2597</v>
+        <v>2588</v>
       </c>
       <c r="F495" s="5" t="s">
-        <v>2601</v>
+        <v>2592</v>
       </c>
       <c r="G495" s="3" t="s">
-        <v>2266</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="496" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
-        <v>2221</v>
+        <v>2219</v>
       </c>
       <c r="B496" s="3" t="b">
         <v>1</v>
@@ -18643,7 +18637,7 @@
     </row>
     <row r="497" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="B497" s="3" t="b">
         <v>1</v>
@@ -18653,18 +18647,18 @@
       </c>
       <c r="D497" s="3"/>
       <c r="E497" s="3" t="s">
-        <v>2384</v>
+        <v>2379</v>
       </c>
       <c r="F497" s="5" t="s">
-        <v>2385</v>
+        <v>2380</v>
       </c>
       <c r="G497" s="3" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="498" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
-        <v>2222</v>
+        <v>2220</v>
       </c>
       <c r="B498" s="3" t="b">
         <v>1</v>
@@ -18685,7 +18679,7 @@
     </row>
     <row r="499" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
-        <v>2223</v>
+        <v>2221</v>
       </c>
       <c r="B499" s="3" t="b">
         <v>1</v>
@@ -18706,7 +18700,7 @@
     </row>
     <row r="500" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="B500" s="3" t="b">
         <v>1</v>
@@ -18727,7 +18721,7 @@
     </row>
     <row r="501" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A501" s="3" t="s">
-        <v>2249</v>
+        <v>2244</v>
       </c>
       <c r="B501" s="3" t="b">
         <v>1</v>
@@ -18747,7 +18741,7 @@
     </row>
     <row r="502" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A502" s="3" t="s">
-        <v>2251</v>
+        <v>2246</v>
       </c>
       <c r="B502" s="3" t="b">
         <v>1</v>
@@ -18756,18 +18750,18 @@
         <v>1</v>
       </c>
       <c r="E502" s="3" t="s">
-        <v>2252</v>
+        <v>2247</v>
       </c>
       <c r="F502" s="5" t="s">
-        <v>2253</v>
+        <v>2248</v>
       </c>
       <c r="G502" s="3" t="s">
-        <v>2262</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="503" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A503" s="3" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
       <c r="B503" s="3" t="b">
         <v>1</v>
@@ -18788,7 +18782,7 @@
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A504" s="3" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="B504" s="3" t="b">
         <v>1</v>
@@ -18809,7 +18803,7 @@
     </row>
     <row r="505" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A505" s="3" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
       <c r="B505" s="3" t="b">
         <v>1</v>
@@ -18830,7 +18824,7 @@
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A506" s="3" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="B506" s="3" t="b">
         <v>1</v>
@@ -18840,10 +18834,10 @@
       </c>
       <c r="D506" s="3"/>
       <c r="E506" s="3" t="s">
-        <v>2382</v>
+        <v>2377</v>
       </c>
       <c r="F506" s="5" t="s">
-        <v>2383</v>
+        <v>2378</v>
       </c>
       <c r="G506" s="3" t="s">
         <v>1352</v>
@@ -18851,7 +18845,7 @@
     </row>
     <row r="507" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A507" s="3" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
       <c r="B507" s="3" t="b">
         <v>1</v>
@@ -18872,7 +18866,7 @@
     </row>
     <row r="508" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A508" s="3" t="s">
-        <v>2230</v>
+        <v>2228</v>
       </c>
       <c r="B508" s="3" t="b">
         <v>1</v>
@@ -18893,7 +18887,7 @@
     </row>
     <row r="509" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A509" s="3" t="s">
-        <v>2254</v>
+        <v>2249</v>
       </c>
       <c r="B509" s="3" t="b">
         <v>1</v>
@@ -18902,18 +18896,18 @@
         <v>1</v>
       </c>
       <c r="E509" s="3" t="s">
-        <v>2256</v>
+        <v>2251</v>
       </c>
       <c r="F509" s="5" t="s">
-        <v>2260</v>
+        <v>2255</v>
       </c>
       <c r="G509" s="3" t="s">
-        <v>2267</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="510" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A510" s="3" t="s">
-        <v>2255</v>
+        <v>2250</v>
       </c>
       <c r="B510" s="3" t="b">
         <v>1</v>
@@ -18922,18 +18916,18 @@
         <v>1</v>
       </c>
       <c r="E510" s="3" t="s">
-        <v>2257</v>
+        <v>2252</v>
       </c>
       <c r="F510" s="5" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="G510" s="3" t="s">
-        <v>2268</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="511" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A511" s="3" t="s">
-        <v>2243</v>
+        <v>2238</v>
       </c>
       <c r="B511" s="3" t="b">
         <v>1</v>
@@ -18942,13 +18936,13 @@
         <v>1</v>
       </c>
       <c r="E511" s="3" t="s">
-        <v>2244</v>
+        <v>2239</v>
       </c>
       <c r="F511" s="5" t="s">
-        <v>2245</v>
+        <v>2240</v>
       </c>
       <c r="G511" s="3" t="s">
-        <v>2246</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.25">
@@ -18995,7 +18989,7 @@
     </row>
     <row r="514" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A514" s="3" t="s">
-        <v>2534</v>
+        <v>2529</v>
       </c>
       <c r="B514" s="3" t="b">
         <v>1</v>
@@ -19004,10 +18998,10 @@
         <v>1</v>
       </c>
       <c r="E514" s="3" t="s">
-        <v>2537</v>
+        <v>2532</v>
       </c>
       <c r="F514" s="5" t="s">
-        <v>2545</v>
+        <v>2540</v>
       </c>
       <c r="G514" s="3" t="s">
         <v>1991</v>
@@ -19015,7 +19009,7 @@
     </row>
     <row r="515" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A515" s="3" t="s">
-        <v>2535</v>
+        <v>2530</v>
       </c>
       <c r="B515" s="3" t="b">
         <v>1</v>
@@ -19024,10 +19018,10 @@
         <v>1</v>
       </c>
       <c r="E515" s="3" t="s">
-        <v>2536</v>
+        <v>2531</v>
       </c>
       <c r="F515" s="5" t="s">
-        <v>2546</v>
+        <v>2541</v>
       </c>
       <c r="G515" s="3" t="s">
         <v>1991</v>
@@ -19056,7 +19050,7 @@
     </row>
     <row r="517" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A517" s="3" t="s">
-        <v>2540</v>
+        <v>2535</v>
       </c>
       <c r="B517" s="3" t="b">
         <v>1</v>
@@ -19066,10 +19060,10 @@
       </c>
       <c r="D517" s="3"/>
       <c r="E517" s="3" t="s">
-        <v>2543</v>
+        <v>2538</v>
       </c>
       <c r="F517" s="5" t="s">
-        <v>2538</v>
+        <v>2533</v>
       </c>
       <c r="G517" s="3" t="s">
         <v>1733</v>
@@ -19077,7 +19071,7 @@
     </row>
     <row r="518" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A518" s="3" t="s">
-        <v>2541</v>
+        <v>2536</v>
       </c>
       <c r="B518" s="3" t="b">
         <v>1</v>
@@ -19087,10 +19081,10 @@
       </c>
       <c r="D518" s="3"/>
       <c r="E518" s="3" t="s">
-        <v>2544</v>
+        <v>2539</v>
       </c>
       <c r="F518" s="5" t="s">
-        <v>2539</v>
+        <v>2534</v>
       </c>
       <c r="G518" s="3" t="s">
         <v>1733</v>
@@ -19098,7 +19092,7 @@
     </row>
     <row r="519" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A519" s="3" t="s">
-        <v>2542</v>
+        <v>2537</v>
       </c>
       <c r="B519" s="3" t="b">
         <v>1</v>
@@ -19245,7 +19239,7 @@
     </row>
     <row r="526" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A526" s="3" t="s">
-        <v>2502</v>
+        <v>2497</v>
       </c>
       <c r="B526" s="3" t="b">
         <v>1</v>
@@ -19254,18 +19248,18 @@
         <v>1</v>
       </c>
       <c r="E526" s="3" t="s">
-        <v>2248</v>
+        <v>2243</v>
       </c>
       <c r="F526" s="5" t="s">
-        <v>2503</v>
+        <v>2498</v>
       </c>
       <c r="G526" s="3" t="s">
-        <v>2379</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="527" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A527" s="3" t="s">
-        <v>2504</v>
+        <v>2499</v>
       </c>
       <c r="B527" s="3" t="b">
         <v>1</v>
@@ -19274,18 +19268,18 @@
         <v>1</v>
       </c>
       <c r="E527" s="3" t="s">
-        <v>2507</v>
+        <v>2502</v>
       </c>
       <c r="F527" s="5" t="s">
-        <v>2518</v>
+        <v>2513</v>
       </c>
       <c r="G527" s="3" t="s">
-        <v>2519</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="528" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A528" s="3" t="s">
-        <v>2505</v>
+        <v>2500</v>
       </c>
       <c r="B528" s="3" t="b">
         <v>1</v>
@@ -19294,18 +19288,18 @@
         <v>1</v>
       </c>
       <c r="E528" s="3" t="s">
-        <v>2509</v>
+        <v>2504</v>
       </c>
       <c r="F528" s="5" t="s">
-        <v>2516</v>
+        <v>2511</v>
       </c>
       <c r="G528" s="3" t="s">
-        <v>2520</v>
+        <v>2515</v>
       </c>
     </row>
     <row r="529" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A529" s="3" t="s">
-        <v>2506</v>
+        <v>2501</v>
       </c>
       <c r="B529" s="3" t="b">
         <v>1</v>
@@ -19314,18 +19308,18 @@
         <v>1</v>
       </c>
       <c r="E529" s="3" t="s">
-        <v>2508</v>
+        <v>2503</v>
       </c>
       <c r="F529" s="5" t="s">
-        <v>2517</v>
+        <v>2512</v>
       </c>
       <c r="G529" s="3" t="s">
-        <v>2521</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="530" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A530" s="3" t="s">
-        <v>2510</v>
+        <v>2505</v>
       </c>
       <c r="B530" s="3" t="b">
         <v>1</v>
@@ -19334,18 +19328,18 @@
         <v>1</v>
       </c>
       <c r="E530" s="3" t="s">
-        <v>2511</v>
+        <v>2506</v>
       </c>
       <c r="F530" s="5" t="s">
-        <v>2512</v>
+        <v>2507</v>
       </c>
       <c r="G530" s="3" t="s">
-        <v>2522</v>
+        <v>2517</v>
       </c>
     </row>
     <row r="531" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A531" s="3" t="s">
-        <v>2513</v>
+        <v>2508</v>
       </c>
       <c r="B531" s="3" t="b">
         <v>1</v>
@@ -19354,13 +19348,13 @@
         <v>1</v>
       </c>
       <c r="E531" s="3" t="s">
-        <v>2514</v>
+        <v>2509</v>
       </c>
       <c r="F531" s="5" t="s">
-        <v>2515</v>
+        <v>2510</v>
       </c>
       <c r="G531" s="3" t="s">
-        <v>2523</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="532" spans="1:7" x14ac:dyDescent="0.25">
@@ -19532,7 +19526,7 @@
     </row>
     <row r="540" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A540" s="3" t="s">
-        <v>2549</v>
+        <v>2544</v>
       </c>
       <c r="B540" s="3" t="b">
         <v>1</v>
@@ -19542,10 +19536,10 @@
       </c>
       <c r="D540" s="3"/>
       <c r="E540" s="3" t="s">
-        <v>2543</v>
+        <v>2538</v>
       </c>
       <c r="F540" s="5" t="s">
-        <v>2550</v>
+        <v>2545</v>
       </c>
       <c r="G540" s="3" t="s">
         <v>1481</v>
@@ -19574,7 +19568,7 @@
     </row>
     <row r="542" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A542" s="3" t="s">
-        <v>2287</v>
+        <v>2282</v>
       </c>
       <c r="B542" s="3" t="b">
         <v>1</v>
@@ -19594,7 +19588,7 @@
     </row>
     <row r="543" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A543" s="3" t="s">
-        <v>2368</v>
+        <v>2363</v>
       </c>
       <c r="B543" s="3" t="b">
         <v>1</v>
@@ -19606,7 +19600,7 @@
         <v>1689</v>
       </c>
       <c r="F543" s="5" t="s">
-        <v>2375</v>
+        <v>2370</v>
       </c>
       <c r="G543" s="3" t="s">
         <v>1724</v>
@@ -19614,27 +19608,27 @@
     </row>
     <row r="544" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A544" s="3" t="s">
+        <v>2364</v>
+      </c>
+      <c r="B544" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C544" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E544" s="3" t="s">
         <v>2369</v>
       </c>
-      <c r="B544" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C544" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E544" s="3" t="s">
-        <v>2374</v>
-      </c>
       <c r="F544" s="5" t="s">
-        <v>2376</v>
+        <v>2371</v>
       </c>
       <c r="G544" s="3" t="s">
-        <v>2378</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="545" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A545" s="3" t="s">
-        <v>2551</v>
+        <v>2546</v>
       </c>
       <c r="B545" s="3" t="b">
         <v>1</v>
@@ -19643,18 +19637,18 @@
         <v>1</v>
       </c>
       <c r="E545" s="3" t="s">
-        <v>2537</v>
+        <v>2532</v>
       </c>
       <c r="F545" s="5" t="s">
-        <v>2552</v>
+        <v>2547</v>
       </c>
       <c r="G545" s="3" t="s">
-        <v>2561</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="546" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A546" s="3" t="s">
-        <v>2370</v>
+        <v>2365</v>
       </c>
       <c r="B546" s="3" t="b">
         <v>1</v>
@@ -19663,18 +19657,18 @@
         <v>1</v>
       </c>
       <c r="E546" s="3" t="s">
-        <v>2248</v>
+        <v>2243</v>
       </c>
       <c r="F546" s="5" t="s">
-        <v>2377</v>
+        <v>2372</v>
       </c>
       <c r="G546" s="3" t="s">
-        <v>2379</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="547" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A547" s="3" t="s">
-        <v>2553</v>
+        <v>2548</v>
       </c>
       <c r="B547" s="3" t="b">
         <v>1</v>
@@ -19683,18 +19677,18 @@
         <v>1</v>
       </c>
       <c r="E547" s="3" t="s">
-        <v>2555</v>
+        <v>2550</v>
       </c>
       <c r="F547" s="5" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G547" s="3" t="s">
         <v>2557</v>
-      </c>
-      <c r="G547" s="3" t="s">
-        <v>2562</v>
       </c>
     </row>
     <row r="548" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A548" s="3" t="s">
-        <v>2554</v>
+        <v>2549</v>
       </c>
       <c r="B548" s="3" t="b">
         <v>1</v>
@@ -19703,18 +19697,18 @@
         <v>1</v>
       </c>
       <c r="E548" s="3" t="s">
-        <v>2556</v>
+        <v>2551</v>
       </c>
       <c r="F548" s="5" t="s">
+        <v>2553</v>
+      </c>
+      <c r="G548" s="3" t="s">
         <v>2558</v>
-      </c>
-      <c r="G548" s="3" t="s">
-        <v>2563</v>
       </c>
     </row>
     <row r="549" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A549" s="3" t="s">
-        <v>2564</v>
+        <v>2559</v>
       </c>
       <c r="B549" s="3" t="b">
         <v>1</v>
@@ -19723,18 +19717,18 @@
         <v>1</v>
       </c>
       <c r="E549" s="3" t="s">
-        <v>2570</v>
+        <v>2565</v>
       </c>
       <c r="F549" s="5" t="s">
-        <v>2576</v>
+        <v>2571</v>
       </c>
       <c r="G549" s="3" t="s">
-        <v>2578</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="550" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A550" s="3" t="s">
-        <v>2565</v>
+        <v>2560</v>
       </c>
       <c r="B550" s="3" t="b">
         <v>1</v>
@@ -19743,18 +19737,18 @@
         <v>1</v>
       </c>
       <c r="E550" s="3" t="s">
-        <v>2571</v>
+        <v>2566</v>
       </c>
       <c r="F550" s="5" t="s">
-        <v>2577</v>
+        <v>2572</v>
       </c>
       <c r="G550" s="3" t="s">
-        <v>2579</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="551" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A551" s="3" t="s">
-        <v>2566</v>
+        <v>2561</v>
       </c>
       <c r="B551" s="3" t="b">
         <v>1</v>
@@ -19763,78 +19757,78 @@
         <v>1</v>
       </c>
       <c r="E551" s="3" t="s">
+        <v>2570</v>
+      </c>
+      <c r="F551" s="5" t="s">
+        <v>2593</v>
+      </c>
+      <c r="G551" s="3" t="s">
         <v>2575</v>
-      </c>
-      <c r="F551" s="5" t="s">
-        <v>2602</v>
-      </c>
-      <c r="G551" s="3" t="s">
-        <v>2580</v>
       </c>
     </row>
     <row r="552" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A552" s="3" t="s">
+        <v>2562</v>
+      </c>
+      <c r="B552" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C552" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E552" s="3" t="s">
         <v>2567</v>
       </c>
-      <c r="B552" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C552" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E552" s="3" t="s">
-        <v>2572</v>
-      </c>
       <c r="F552" s="5" t="s">
-        <v>2603</v>
+        <v>2594</v>
       </c>
       <c r="G552" s="3" t="s">
-        <v>2581</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="553" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A553" s="3" t="s">
+        <v>2563</v>
+      </c>
+      <c r="B553" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C553" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E553" s="3" t="s">
         <v>2568</v>
       </c>
-      <c r="B553" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C553" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E553" s="3" t="s">
-        <v>2573</v>
-      </c>
       <c r="F553" s="5" t="s">
-        <v>2604</v>
+        <v>2595</v>
       </c>
       <c r="G553" s="3" t="s">
-        <v>2582</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="554" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A554" s="3" t="s">
+        <v>2564</v>
+      </c>
+      <c r="B554" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C554" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E554" s="3" t="s">
         <v>2569</v>
       </c>
-      <c r="B554" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C554" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E554" s="3" t="s">
-        <v>2574</v>
-      </c>
       <c r="F554" s="5" t="s">
-        <v>2605</v>
+        <v>2596</v>
       </c>
       <c r="G554" s="3" t="s">
-        <v>2583</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="555" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A555" s="3" t="s">
-        <v>2559</v>
+        <v>2554</v>
       </c>
       <c r="B555" s="3" t="b">
         <v>1</v>
@@ -19846,7 +19840,7 @@
         <v>33</v>
       </c>
       <c r="F555" s="5" t="s">
-        <v>2560</v>
+        <v>2555</v>
       </c>
       <c r="G555" s="3" t="s">
         <v>1215</v>
@@ -19854,7 +19848,7 @@
     </row>
     <row r="556" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A556" s="3" t="s">
-        <v>2371</v>
+        <v>2366</v>
       </c>
       <c r="B556" s="3" t="b">
         <v>1</v>
@@ -19874,7 +19868,7 @@
     </row>
     <row r="557" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A557" s="3" t="s">
-        <v>2372</v>
+        <v>2367</v>
       </c>
       <c r="B557" s="3" t="b">
         <v>1</v>
@@ -19894,7 +19888,7 @@
     </row>
     <row r="558" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A558" s="3" t="s">
-        <v>2373</v>
+        <v>2368</v>
       </c>
       <c r="B558" s="3" t="b">
         <v>1</v>
@@ -19914,7 +19908,7 @@
     </row>
     <row r="559" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A559" s="3" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="B559" s="3" t="b">
         <v>1</v>
@@ -19923,7 +19917,7 @@
         <v>1</v>
       </c>
       <c r="E559" s="3" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="F559" s="5" t="s">
         <v>2217</v>
@@ -21190,7 +21184,7 @@
     </row>
     <row r="622" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A622" s="3" t="s">
-        <v>2462</v>
+        <v>2457</v>
       </c>
       <c r="B622" s="3" t="b">
         <v>1</v>
@@ -21199,13 +21193,13 @@
         <v>1</v>
       </c>
       <c r="E622" s="3" t="s">
-        <v>2463</v>
+        <v>2458</v>
       </c>
       <c r="F622" s="5" t="s">
-        <v>2464</v>
+        <v>2459</v>
       </c>
       <c r="G622" s="3" t="s">
-        <v>2417</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="623" spans="1:7" x14ac:dyDescent="0.25">
@@ -21290,7 +21284,7 @@
     </row>
     <row r="627" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A627" s="3" t="s">
-        <v>2465</v>
+        <v>2460</v>
       </c>
       <c r="B627" s="3" t="b">
         <v>1</v>
@@ -21299,18 +21293,18 @@
         <v>1</v>
       </c>
       <c r="E627" s="3" t="s">
+        <v>2462</v>
+      </c>
+      <c r="F627" s="5" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G627" s="3" t="s">
         <v>2467</v>
-      </c>
-      <c r="F627" s="5" t="s">
-        <v>2468</v>
-      </c>
-      <c r="G627" s="3" t="s">
-        <v>2472</v>
       </c>
     </row>
     <row r="628" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A628" s="3" t="s">
-        <v>2493</v>
+        <v>2488</v>
       </c>
       <c r="B628" s="3" t="b">
         <v>1</v>
@@ -21319,18 +21313,18 @@
         <v>1</v>
       </c>
       <c r="E628" s="3" t="s">
-        <v>2497</v>
+        <v>2492</v>
       </c>
       <c r="F628" s="5" t="s">
-        <v>2471</v>
+        <v>2466</v>
       </c>
       <c r="G628" s="3" t="s">
-        <v>2473</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="629" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A629" s="3" t="s">
-        <v>2494</v>
+        <v>2489</v>
       </c>
       <c r="B629" s="3" t="b">
         <v>1</v>
@@ -21339,18 +21333,18 @@
         <v>1</v>
       </c>
       <c r="E629" s="3" t="s">
-        <v>2495</v>
+        <v>2490</v>
       </c>
       <c r="F629" s="5" t="s">
-        <v>2496</v>
+        <v>2491</v>
       </c>
       <c r="G629" s="3" t="s">
-        <v>2474</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="630" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A630" s="3" t="s">
-        <v>2469</v>
+        <v>2464</v>
       </c>
       <c r="B630" s="3" t="b">
         <v>1</v>
@@ -21359,18 +21353,18 @@
         <v>1</v>
       </c>
       <c r="E630" s="3" t="s">
-        <v>2470</v>
+        <v>2465</v>
       </c>
       <c r="F630" s="5" t="s">
         <v>1663</v>
       </c>
       <c r="G630" s="3" t="s">
-        <v>2475</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="631" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A631" s="3" t="s">
-        <v>2492</v>
+        <v>2487</v>
       </c>
       <c r="B631" s="3" t="b">
         <v>1</v>
@@ -21410,7 +21404,7 @@
     </row>
     <row r="633" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A633" s="3" t="s">
-        <v>2466</v>
+        <v>2461</v>
       </c>
       <c r="B633" s="3" t="b">
         <v>1</v>
@@ -22292,7 +22286,7 @@
     </row>
     <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" s="3" t="s">
-        <v>2547</v>
+        <v>2542</v>
       </c>
       <c r="B677" s="3" t="b">
         <v>1</v>
@@ -22305,7 +22299,7 @@
         <v>1751</v>
       </c>
       <c r="F677" s="5" t="s">
-        <v>2548</v>
+        <v>2543</v>
       </c>
       <c r="G677" s="3" t="s">
         <v>1481</v>
@@ -22744,7 +22738,7 @@
     </row>
     <row r="699" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="B699" t="b">
         <v>1</v>
@@ -22753,7 +22747,7 @@
         <v>1</v>
       </c>
       <c r="E699" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="F699" s="5" t="s">
         <v>2217</v>
@@ -22764,7 +22758,7 @@
     </row>
     <row r="700" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A700" s="3" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="B700" t="b">
         <v>1</v>
@@ -22773,7 +22767,7 @@
         <v>1</v>
       </c>
       <c r="E700" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="F700" s="5" t="s">
         <v>2216</v>
@@ -22784,7 +22778,7 @@
     </row>
     <row r="701" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A701" s="3" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="B701" s="3" t="b">
         <v>1</v>
@@ -22804,7 +22798,7 @@
     </row>
     <row r="702" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A702" s="3" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="B702" s="3" t="b">
         <v>1</v>
@@ -22824,7 +22818,7 @@
     </row>
     <row r="703" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>2280</v>
+        <v>2275</v>
       </c>
       <c r="B703" t="b">
         <v>1</v>
@@ -22833,18 +22827,18 @@
         <v>1</v>
       </c>
       <c r="E703" t="s">
-        <v>2269</v>
+        <v>2264</v>
       </c>
       <c r="F703" s="5" t="s">
-        <v>2270</v>
+        <v>2265</v>
       </c>
       <c r="G703" t="s">
-        <v>2292</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="704" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>2282</v>
+        <v>2277</v>
       </c>
       <c r="B704" t="b">
         <v>1</v>
@@ -22853,18 +22847,18 @@
         <v>0</v>
       </c>
       <c r="E704" t="s">
-        <v>2281</v>
+        <v>2276</v>
       </c>
       <c r="F704" s="5" t="s">
-        <v>2283</v>
+        <v>2278</v>
       </c>
       <c r="G704" t="s">
-        <v>2293</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>2286</v>
+        <v>2281</v>
       </c>
       <c r="B705" t="b">
         <v>1</v>
@@ -22873,18 +22867,18 @@
         <v>0</v>
       </c>
       <c r="E705" t="s">
-        <v>2284</v>
+        <v>2279</v>
       </c>
       <c r="F705" s="5" t="s">
-        <v>2285</v>
+        <v>2280</v>
       </c>
       <c r="G705" t="s">
-        <v>2294</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="706" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A706" s="3" t="s">
-        <v>2289</v>
+        <v>2284</v>
       </c>
       <c r="B706" s="3" t="b">
         <v>0</v>
@@ -22893,18 +22887,18 @@
         <v>1</v>
       </c>
       <c r="E706" s="3" t="s">
+        <v>2285</v>
+      </c>
+      <c r="F706" s="5" t="s">
+        <v>2286</v>
+      </c>
+      <c r="G706" s="3" t="s">
         <v>2290</v>
-      </c>
-      <c r="F706" s="5" t="s">
-        <v>2291</v>
-      </c>
-      <c r="G706" s="3" t="s">
-        <v>2295</v>
       </c>
     </row>
     <row r="707" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>2296</v>
+        <v>2291</v>
       </c>
       <c r="B707" t="b">
         <v>0</v>
@@ -22913,18 +22907,18 @@
         <v>1</v>
       </c>
       <c r="E707" t="s">
-        <v>2299</v>
+        <v>2294</v>
       </c>
       <c r="F707" s="5" t="s">
-        <v>2300</v>
+        <v>2295</v>
       </c>
       <c r="G707" t="s">
-        <v>2309</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="708" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="B708" t="b">
         <v>0</v>
@@ -22933,38 +22927,38 @@
         <v>1</v>
       </c>
       <c r="E708" t="s">
-        <v>2298</v>
+        <v>2293</v>
       </c>
       <c r="F708" s="5" t="s">
-        <v>2301</v>
+        <v>2296</v>
       </c>
       <c r="G708" t="s">
-        <v>2310</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="709" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
+        <v>2298</v>
+      </c>
+      <c r="B709" t="b">
+        <v>1</v>
+      </c>
+      <c r="C709" t="b">
+        <v>1</v>
+      </c>
+      <c r="E709" t="s">
+        <v>2300</v>
+      </c>
+      <c r="F709" s="5" t="s">
         <v>2303</v>
       </c>
-      <c r="B709" t="b">
-        <v>1</v>
-      </c>
-      <c r="C709" t="b">
-        <v>1</v>
-      </c>
-      <c r="E709" t="s">
-        <v>2305</v>
-      </c>
-      <c r="F709" s="5" t="s">
-        <v>2308</v>
-      </c>
       <c r="G709" t="s">
-        <v>2311</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="710" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>2304</v>
+        <v>2299</v>
       </c>
       <c r="B710" s="3" t="b">
         <v>1</v>
@@ -22984,7 +22978,7 @@
     </row>
     <row r="711" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>2367</v>
+        <v>2362</v>
       </c>
       <c r="B711" s="3" t="b">
         <v>1</v>
@@ -22993,18 +22987,18 @@
         <v>1</v>
       </c>
       <c r="E711" t="s">
-        <v>2306</v>
+        <v>2301</v>
       </c>
       <c r="F711" s="5" t="s">
+        <v>2302</v>
+      </c>
+      <c r="G711" t="s">
         <v>2307</v>
-      </c>
-      <c r="G711" t="s">
-        <v>2312</v>
       </c>
     </row>
     <row r="712" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>2315</v>
+        <v>2310</v>
       </c>
       <c r="B712" t="b">
         <v>0</v>
@@ -23013,21 +23007,21 @@
         <v>1</v>
       </c>
       <c r="D712" t="s">
-        <v>2316</v>
+        <v>2311</v>
       </c>
       <c r="E712" t="s">
+        <v>2313</v>
+      </c>
+      <c r="F712" s="5" t="s">
+        <v>2312</v>
+      </c>
+      <c r="G712" s="3" t="s">
         <v>2318</v>
-      </c>
-      <c r="F712" s="5" t="s">
-        <v>2317</v>
-      </c>
-      <c r="G712" s="3" t="s">
-        <v>2323</v>
       </c>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>2348</v>
+        <v>2343</v>
       </c>
       <c r="B713" t="b">
         <v>0</v>
@@ -23036,18 +23030,18 @@
         <v>1</v>
       </c>
       <c r="E713" t="s">
-        <v>2349</v>
+        <v>2344</v>
       </c>
       <c r="F713" s="5" t="s">
-        <v>2365</v>
+        <v>2360</v>
       </c>
       <c r="G713" t="s">
-        <v>2360</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="714" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>2350</v>
+        <v>2345</v>
       </c>
       <c r="B714" t="b">
         <v>0</v>
@@ -23056,18 +23050,18 @@
         <v>1</v>
       </c>
       <c r="E714" t="s">
-        <v>2366</v>
+        <v>2361</v>
       </c>
       <c r="F714" s="5" t="s">
-        <v>2353</v>
+        <v>2348</v>
       </c>
       <c r="G714" t="s">
-        <v>2361</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="715" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A715" s="3" t="s">
-        <v>2356</v>
+        <v>2351</v>
       </c>
       <c r="B715" s="3" t="b">
         <v>0</v>
@@ -23076,18 +23070,18 @@
         <v>1</v>
       </c>
       <c r="E715" s="3" t="s">
+        <v>2352</v>
+      </c>
+      <c r="F715" s="5" t="s">
+        <v>2353</v>
+      </c>
+      <c r="G715" s="3" t="s">
         <v>2357</v>
-      </c>
-      <c r="F715" s="5" t="s">
-        <v>2358</v>
-      </c>
-      <c r="G715" s="3" t="s">
-        <v>2362</v>
       </c>
     </row>
     <row r="716" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>2351</v>
+        <v>2346</v>
       </c>
       <c r="B716" t="b">
         <v>0</v>
@@ -23096,18 +23090,18 @@
         <v>1</v>
       </c>
       <c r="E716" t="s">
-        <v>2351</v>
+        <v>2346</v>
       </c>
       <c r="F716" s="5" t="s">
-        <v>2352</v>
+        <v>2347</v>
       </c>
       <c r="G716" t="s">
-        <v>2363</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>2355</v>
+        <v>2350</v>
       </c>
       <c r="B717" t="b">
         <v>0</v>
@@ -23116,13 +23110,13 @@
         <v>1</v>
       </c>
       <c r="E717" t="s">
+        <v>2349</v>
+      </c>
+      <c r="F717" s="5" t="s">
         <v>2354</v>
       </c>
-      <c r="F717" s="5" t="s">
+      <c r="G717" t="s">
         <v>2359</v>
-      </c>
-      <c r="G717" t="s">
-        <v>2364</v>
       </c>
     </row>
     <row r="718" spans="1:7" x14ac:dyDescent="0.25">
@@ -23147,7 +23141,7 @@
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>2380</v>
+        <v>2375</v>
       </c>
       <c r="B719" t="b">
         <v>0</v>
@@ -23156,18 +23150,18 @@
         <v>1</v>
       </c>
       <c r="E719" t="s">
-        <v>2380</v>
+        <v>2375</v>
       </c>
       <c r="F719" s="5" t="s">
-        <v>2381</v>
+        <v>2376</v>
       </c>
       <c r="G719" t="s">
-        <v>2393</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>2391</v>
+        <v>2386</v>
       </c>
       <c r="B720" t="b">
         <v>0</v>
@@ -23176,18 +23170,18 @@
         <v>1</v>
       </c>
       <c r="E720" t="s">
-        <v>2392</v>
+        <v>2387</v>
       </c>
       <c r="F720" s="5" t="s">
-        <v>2395</v>
+        <v>2390</v>
       </c>
       <c r="G720" t="s">
-        <v>2394</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>2455</v>
+        <v>2450</v>
       </c>
       <c r="B721" t="b">
         <v>1</v>
@@ -23196,18 +23190,18 @@
         <v>1</v>
       </c>
       <c r="E721" t="s">
-        <v>2396</v>
+        <v>2391</v>
       </c>
       <c r="F721" s="5" t="s">
-        <v>2403</v>
+        <v>2398</v>
       </c>
       <c r="G721" t="s">
-        <v>2410</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>2456</v>
+        <v>2451</v>
       </c>
       <c r="B722" s="3" t="b">
         <v>1</v>
@@ -23216,18 +23210,18 @@
         <v>1</v>
       </c>
       <c r="E722" t="s">
-        <v>2397</v>
+        <v>2392</v>
       </c>
       <c r="F722" s="5" t="s">
-        <v>2404</v>
+        <v>2399</v>
       </c>
       <c r="G722" t="s">
-        <v>2416</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>2457</v>
+        <v>2452</v>
       </c>
       <c r="B723" s="3" t="b">
         <v>1</v>
@@ -23236,18 +23230,18 @@
         <v>1</v>
       </c>
       <c r="E723" t="s">
-        <v>2398</v>
+        <v>2393</v>
       </c>
       <c r="F723" s="5" t="s">
-        <v>2405</v>
+        <v>2400</v>
       </c>
       <c r="G723" t="s">
-        <v>2411</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>2458</v>
+        <v>2453</v>
       </c>
       <c r="B724" s="3" t="b">
         <v>1</v>
@@ -23256,18 +23250,18 @@
         <v>1</v>
       </c>
       <c r="E724" t="s">
-        <v>2400</v>
+        <v>2395</v>
       </c>
       <c r="F724" s="5" t="s">
+        <v>2402</v>
+      </c>
+      <c r="G724" t="s">
         <v>2407</v>
-      </c>
-      <c r="G724" t="s">
-        <v>2412</v>
       </c>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>2459</v>
+        <v>2454</v>
       </c>
       <c r="B725" s="3" t="b">
         <v>1</v>
@@ -23276,18 +23270,18 @@
         <v>1</v>
       </c>
       <c r="E725" t="s">
-        <v>2401</v>
+        <v>2396</v>
       </c>
       <c r="F725" s="5" t="s">
+        <v>2403</v>
+      </c>
+      <c r="G725" t="s">
         <v>2408</v>
-      </c>
-      <c r="G725" t="s">
-        <v>2413</v>
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>2460</v>
+        <v>2455</v>
       </c>
       <c r="B726" s="3" t="b">
         <v>1</v>
@@ -23296,18 +23290,18 @@
         <v>1</v>
       </c>
       <c r="E726" t="s">
-        <v>2399</v>
+        <v>2394</v>
       </c>
       <c r="F726" s="5" t="s">
-        <v>2406</v>
+        <v>2401</v>
       </c>
       <c r="G726" t="s">
-        <v>2414</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>2461</v>
+        <v>2456</v>
       </c>
       <c r="B727" s="3" t="b">
         <v>1</v>
@@ -23316,18 +23310,18 @@
         <v>1</v>
       </c>
       <c r="E727" t="s">
-        <v>2402</v>
+        <v>2397</v>
       </c>
       <c r="F727" s="5" t="s">
-        <v>2409</v>
+        <v>2404</v>
       </c>
       <c r="G727" t="s">
-        <v>2415</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>2477</v>
+        <v>2472</v>
       </c>
       <c r="B728" t="b">
         <v>1</v>
@@ -23336,18 +23330,18 @@
         <v>1</v>
       </c>
       <c r="E728" t="s">
-        <v>2479</v>
+        <v>2474</v>
       </c>
       <c r="F728" s="5" t="s">
-        <v>2481</v>
+        <v>2476</v>
       </c>
       <c r="G728" t="s">
-        <v>2483</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>2478</v>
+        <v>2473</v>
       </c>
       <c r="B729" t="b">
         <v>1</v>
@@ -23356,38 +23350,38 @@
         <v>1</v>
       </c>
       <c r="E729" t="s">
-        <v>2480</v>
+        <v>2475</v>
       </c>
       <c r="F729" s="5" t="s">
-        <v>2482</v>
+        <v>2477</v>
       </c>
       <c r="G729" t="s">
-        <v>2484</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
+        <v>2480</v>
+      </c>
+      <c r="B730" t="b">
+        <v>1</v>
+      </c>
+      <c r="C730" t="b">
+        <v>1</v>
+      </c>
+      <c r="E730" t="s">
+        <v>2481</v>
+      </c>
+      <c r="F730" s="5" t="s">
+        <v>2482</v>
+      </c>
+      <c r="G730" t="s">
         <v>2485</v>
-      </c>
-      <c r="B730" t="b">
-        <v>1</v>
-      </c>
-      <c r="C730" t="b">
-        <v>1</v>
-      </c>
-      <c r="E730" t="s">
-        <v>2486</v>
-      </c>
-      <c r="F730" s="5" t="s">
-        <v>2487</v>
-      </c>
-      <c r="G730" t="s">
-        <v>2490</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>2488</v>
+        <v>2483</v>
       </c>
       <c r="B731" t="b">
         <v>1</v>
@@ -23396,18 +23390,18 @@
         <v>1</v>
       </c>
       <c r="E731" t="s">
-        <v>2501</v>
+        <v>2496</v>
       </c>
       <c r="F731" s="5" t="s">
-        <v>2489</v>
+        <v>2484</v>
       </c>
       <c r="G731" t="s">
-        <v>2491</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="732" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>2498</v>
+        <v>2493</v>
       </c>
       <c r="B732" t="b">
         <v>0</v>
@@ -23416,18 +23410,18 @@
         <v>1</v>
       </c>
       <c r="E732" t="s">
-        <v>2499</v>
+        <v>2494</v>
       </c>
       <c r="F732" s="5" t="s">
-        <v>2500</v>
+        <v>2495</v>
       </c>
       <c r="G732" t="s">
-        <v>2476</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>2524</v>
+        <v>2519</v>
       </c>
       <c r="B733" t="b">
         <v>0</v>
@@ -23436,18 +23430,18 @@
         <v>1</v>
       </c>
       <c r="E733" t="s">
-        <v>2524</v>
+        <v>2519</v>
       </c>
       <c r="F733" s="5" t="s">
         <v>1087</v>
       </c>
       <c r="G733" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>2584</v>
+        <v>2579</v>
       </c>
       <c r="B734" t="b">
         <v>0</v>
@@ -23456,18 +23450,18 @@
         <v>1</v>
       </c>
       <c r="E734" t="s">
-        <v>2584</v>
+        <v>2579</v>
       </c>
       <c r="F734" s="5" t="s">
-        <v>2585</v>
+        <v>2580</v>
       </c>
       <c r="G734" t="s">
-        <v>2588</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>2586</v>
+        <v>2581</v>
       </c>
       <c r="B735" t="b">
         <v>0</v>
@@ -23476,13 +23470,13 @@
         <v>1</v>
       </c>
       <c r="E735" t="s">
-        <v>2586</v>
+        <v>2581</v>
       </c>
       <c r="F735" s="5" t="s">
-        <v>2587</v>
+        <v>2582</v>
       </c>
       <c r="G735" t="s">
-        <v>2589</v>
+        <v>2584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor touches on the attachments framework
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F41233-6880-4601-9BA6-0BC6A914C84A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772230C6-63FE-410C-890A-489146513BE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="2631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2980" uniqueCount="2634">
   <si>
     <t>Key</t>
   </si>
@@ -7927,6 +7927,15 @@
   </si>
   <si>
     <t>文件扩展名</t>
+  </si>
+  <si>
+    <t>Error_PendingFilesExceedMaximumSizeOf0</t>
+  </si>
+  <si>
+    <t>The combined size of all unsaved attachments exceeds the maximum allowed size of {{size}}, please save the document and then try again</t>
+  </si>
+  <si>
+    <t>مجموع حجم الملفات التي لم تحفظ بعد يتجاوز الحد الأقصى المسموح به: {{size}}، قم بحفظ المستند ثم إعادة المحاولة مرة أخرى</t>
   </si>
 </sst>
 </file>
@@ -8323,12 +8332,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G743"/>
+  <dimension ref="A1:G744"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A714" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G738" sqref="G738"/>
+      <selection pane="bottomLeft" activeCell="F745" sqref="F745"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23718,6 +23727,23 @@
         <v>2625</v>
       </c>
     </row>
+    <row r="744" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A744" t="s">
+        <v>2631</v>
+      </c>
+      <c r="B744" t="b">
+        <v>0</v>
+      </c>
+      <c r="C744" t="b">
+        <v>1</v>
+      </c>
+      <c r="E744" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F744" s="5" t="s">
+        <v>2633</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G734" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Changed ReportDefinition.State to ShowInMainMenu
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772230C6-63FE-410C-890A-489146513BE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987E9ED5-E93D-414A-BCB8-77AD0FC30016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$734</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$735</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2980" uniqueCount="2634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="2643">
   <si>
     <t>Key</t>
   </si>
@@ -7936,6 +7936,33 @@
   </si>
   <si>
     <t>مجموع حجم الملفات التي لم تحفظ بعد يتجاوز الحد الأقصى المسموح به: {{size}}، قم بحفظ المستند ثم إعادة المحاولة مرة أخرى</t>
+  </si>
+  <si>
+    <t>ReportDefinition_ShowInMainMenu</t>
+  </si>
+  <si>
+    <t>Show in Main Menu</t>
+  </si>
+  <si>
+    <t>إظهار في القائمة الرئيسية</t>
+  </si>
+  <si>
+    <t>VisibleInMainMenu</t>
+  </si>
+  <si>
+    <t>NotVisibleInMainMenu</t>
+  </si>
+  <si>
+    <t>ظاهر في القائمة الرئيسية</t>
+  </si>
+  <si>
+    <t>ليس في القائمة الرئيسية</t>
+  </si>
+  <si>
+    <t>In Main Menu</t>
+  </si>
+  <si>
+    <t>Not in Main Menu</t>
   </si>
 </sst>
 </file>
@@ -8332,12 +8359,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G744"/>
+  <dimension ref="A1:G747"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A714" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A724" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F745" sqref="F745"/>
+      <selection pane="bottomLeft" activeCell="E748" sqref="E748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21672,9 +21699,9 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="642" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A642" t="s">
-        <v>1931</v>
+    <row r="642" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A642" s="3" t="s">
+        <v>2634</v>
       </c>
       <c r="B642" s="3" t="b">
         <v>1</v>
@@ -21682,19 +21709,16 @@
       <c r="C642" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E642" t="s">
-        <v>1933</v>
+      <c r="E642" s="3" t="s">
+        <v>2635</v>
       </c>
       <c r="F642" s="5" t="s">
-        <v>1954</v>
-      </c>
-      <c r="G642" t="s">
-        <v>1981</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B643" s="3" t="b">
         <v>1</v>
@@ -21703,38 +21727,38 @@
         <v>1</v>
       </c>
       <c r="E643" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="F643" s="5" t="s">
-        <v>1886</v>
+        <v>1954</v>
       </c>
       <c r="G643" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>1984</v>
-      </c>
-      <c r="B644" t="b">
-        <v>0</v>
-      </c>
-      <c r="C644" t="b">
+        <v>1932</v>
+      </c>
+      <c r="B644" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C644" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E644" t="s">
-        <v>1984</v>
+        <v>1934</v>
       </c>
       <c r="F644" s="5" t="s">
-        <v>1985</v>
+        <v>1886</v>
       </c>
       <c r="G644" t="s">
-        <v>1986</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="645" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="B645" t="b">
         <v>0</v>
@@ -21743,138 +21767,138 @@
         <v>1</v>
       </c>
       <c r="E645" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="F645" s="5" t="s">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="G645" t="s">
-        <v>1989</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="646" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>1991</v>
+        <v>1987</v>
       </c>
       <c r="B646" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C646" t="b">
         <v>1</v>
       </c>
       <c r="E646" t="s">
-        <v>1991</v>
+        <v>1987</v>
       </c>
       <c r="F646" s="5" t="s">
-        <v>1994</v>
+        <v>1988</v>
       </c>
       <c r="G646" t="s">
-        <v>1995</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="647" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>1992</v>
-      </c>
-      <c r="B647" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C647" s="3" t="b">
+        <v>1991</v>
+      </c>
+      <c r="B647" t="b">
+        <v>1</v>
+      </c>
+      <c r="C647" t="b">
         <v>1</v>
       </c>
       <c r="E647" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="F647" s="5" t="s">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="G647" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="648" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>2003</v>
-      </c>
-      <c r="B648" t="b">
-        <v>0</v>
-      </c>
-      <c r="C648" t="b">
+        <v>1992</v>
+      </c>
+      <c r="B648" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C648" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E648" t="s">
-        <v>2003</v>
+        <v>1992</v>
       </c>
       <c r="F648" s="5" t="s">
-        <v>1941</v>
+        <v>1993</v>
       </c>
       <c r="G648" t="s">
-        <v>2010</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="649" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B649" t="b">
+        <v>0</v>
+      </c>
+      <c r="C649" t="b">
+        <v>1</v>
+      </c>
+      <c r="E649" t="s">
+        <v>2003</v>
+      </c>
+      <c r="F649" s="5" t="s">
+        <v>1941</v>
+      </c>
+      <c r="G649" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="650" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A650" t="s">
         <v>2000</v>
       </c>
-      <c r="B649" t="b">
-        <v>1</v>
-      </c>
-      <c r="C649" t="b">
-        <v>1</v>
-      </c>
-      <c r="E649" t="s">
+      <c r="B650" t="b">
+        <v>1</v>
+      </c>
+      <c r="C650" t="b">
+        <v>1</v>
+      </c>
+      <c r="E650" t="s">
         <v>2001</v>
       </c>
-      <c r="F649" s="5" t="s">
+      <c r="F650" s="5" t="s">
         <v>2002</v>
       </c>
-      <c r="G649" t="s">
+      <c r="G650" t="s">
         <v>2011</v>
       </c>
     </row>
-    <row r="650" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A650" s="3" t="s">
+    <row r="651" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A651" s="3" t="s">
         <v>2004</v>
       </c>
-      <c r="B650" t="b">
-        <v>0</v>
-      </c>
-      <c r="C650" t="b">
-        <v>1</v>
-      </c>
-      <c r="E650" t="s">
+      <c r="B651" t="b">
+        <v>0</v>
+      </c>
+      <c r="C651" t="b">
+        <v>1</v>
+      </c>
+      <c r="E651" t="s">
         <v>2005</v>
       </c>
-      <c r="F650" s="5" t="s">
+      <c r="F651" s="5" t="s">
         <v>2006</v>
       </c>
-      <c r="G650" t="s">
+      <c r="G651" t="s">
         <v>2012</v>
-      </c>
-    </row>
-    <row r="651" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A651" t="s">
-        <v>2007</v>
-      </c>
-      <c r="B651" t="b">
-        <v>0</v>
-      </c>
-      <c r="C651" t="b">
-        <v>1</v>
-      </c>
-      <c r="E651" t="s">
-        <v>2008</v>
-      </c>
-      <c r="F651" s="5" t="s">
-        <v>2009</v>
-      </c>
-      <c r="G651" t="s">
-        <v>2013</v>
       </c>
     </row>
     <row r="652" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="B652" t="b">
         <v>0</v>
@@ -21883,18 +21907,18 @@
         <v>1</v>
       </c>
       <c r="E652" t="s">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="F652" s="5" t="s">
-        <v>2017</v>
+        <v>2009</v>
       </c>
       <c r="G652" t="s">
-        <v>2018</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B653" t="b">
         <v>0</v>
@@ -21903,18 +21927,18 @@
         <v>1</v>
       </c>
       <c r="E653" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="F653" s="5" t="s">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="G653" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>962</v>
+        <v>2015</v>
       </c>
       <c r="B654" t="b">
         <v>0</v>
@@ -21923,18 +21947,18 @@
         <v>1</v>
       </c>
       <c r="E654" t="s">
-        <v>962</v>
+        <v>2015</v>
       </c>
       <c r="F654" s="5" t="s">
-        <v>1198</v>
+        <v>2016</v>
       </c>
       <c r="G654" t="s">
-        <v>1611</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="655" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>2085</v>
+        <v>962</v>
       </c>
       <c r="B655" t="b">
         <v>0</v>
@@ -21943,18 +21967,18 @@
         <v>1</v>
       </c>
       <c r="E655" t="s">
-        <v>2086</v>
+        <v>962</v>
       </c>
       <c r="F655" s="5" t="s">
-        <v>2087</v>
+        <v>1198</v>
       </c>
       <c r="G655" t="s">
-        <v>2091</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="B656" t="b">
         <v>0</v>
@@ -21963,18 +21987,18 @@
         <v>1</v>
       </c>
       <c r="E656" t="s">
-        <v>2090</v>
+        <v>2086</v>
       </c>
       <c r="F656" s="5" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="G656" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="657" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>2093</v>
+        <v>2088</v>
       </c>
       <c r="B657" t="b">
         <v>0</v>
@@ -21983,58 +22007,58 @@
         <v>1</v>
       </c>
       <c r="E657" t="s">
-        <v>2094</v>
+        <v>2090</v>
       </c>
       <c r="F657" s="5" t="s">
-        <v>2095</v>
+        <v>2089</v>
       </c>
       <c r="G657" t="s">
-        <v>2096</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B658" t="b">
+        <v>0</v>
+      </c>
+      <c r="C658" t="b">
+        <v>1</v>
+      </c>
+      <c r="E658" t="s">
+        <v>2094</v>
+      </c>
+      <c r="F658" s="5" t="s">
+        <v>2095</v>
+      </c>
+      <c r="G658" t="s">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="659" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A659" t="s">
         <v>2097</v>
       </c>
-      <c r="B658" t="b">
-        <v>1</v>
-      </c>
-      <c r="C658" t="b">
-        <v>0</v>
-      </c>
-      <c r="E658" t="s">
+      <c r="B659" t="b">
+        <v>1</v>
+      </c>
+      <c r="C659" t="b">
+        <v>0</v>
+      </c>
+      <c r="E659" t="s">
         <v>2100</v>
       </c>
-      <c r="F658" s="5" t="s">
+      <c r="F659" s="5" t="s">
         <v>2098</v>
       </c>
-      <c r="G658" t="s">
+      <c r="G659" t="s">
         <v>2099</v>
-      </c>
-    </row>
-    <row r="659" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A659" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="B659" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C659" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E659" s="3" t="s">
-        <v>1689</v>
-      </c>
-      <c r="F659" s="5" t="s">
-        <v>2118</v>
-      </c>
-      <c r="G659" s="3" t="s">
-        <v>1723</v>
       </c>
     </row>
     <row r="660" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A660" s="3" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="B660" s="3" t="b">
         <v>1</v>
@@ -22043,58 +22067,58 @@
         <v>1</v>
       </c>
       <c r="E660" s="3" t="s">
-        <v>2117</v>
+        <v>1689</v>
       </c>
       <c r="F660" s="5" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="G660" s="3" t="s">
         <v>1723</v>
       </c>
     </row>
-    <row r="661" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A661" t="s">
+    <row r="661" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A661" s="3" t="s">
+        <v>2116</v>
+      </c>
+      <c r="B661" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C661" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E661" s="3" t="s">
+        <v>2117</v>
+      </c>
+      <c r="F661" s="5" t="s">
+        <v>2119</v>
+      </c>
+      <c r="G661" s="3" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="662" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A662" t="s">
         <v>2111</v>
       </c>
-      <c r="B661" t="b">
-        <v>1</v>
-      </c>
-      <c r="C661" t="b">
-        <v>1</v>
-      </c>
-      <c r="E661" t="s">
+      <c r="B662" t="b">
+        <v>1</v>
+      </c>
+      <c r="C662" t="b">
+        <v>1</v>
+      </c>
+      <c r="E662" t="s">
         <v>2113</v>
       </c>
-      <c r="F661" s="5" t="s">
+      <c r="F662" s="5" t="s">
         <v>2114</v>
       </c>
-      <c r="G661" t="s">
+      <c r="G662" t="s">
         <v>2135</v>
-      </c>
-    </row>
-    <row r="662" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A662" s="3" t="s">
-        <v>2123</v>
-      </c>
-      <c r="B662" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C662" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E662" s="3" t="s">
-        <v>2127</v>
-      </c>
-      <c r="F662" s="5" t="s">
-        <v>2131</v>
-      </c>
-      <c r="G662" s="3" t="s">
-        <v>2136</v>
       </c>
     </row>
     <row r="663" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A663" s="3" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="B663" s="3" t="b">
         <v>1</v>
@@ -22103,18 +22127,18 @@
         <v>1</v>
       </c>
       <c r="E663" s="3" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="F663" s="5" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="G663" s="3" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="664" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A664" s="3" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="B664" s="3" t="b">
         <v>1</v>
@@ -22123,98 +22147,98 @@
         <v>1</v>
       </c>
       <c r="E664" s="3" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="F664" s="5" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="G664" s="3" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="665" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A665" s="3" t="s">
+        <v>2125</v>
+      </c>
+      <c r="B665" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C665" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E665" s="3" t="s">
+        <v>2129</v>
+      </c>
+      <c r="F665" s="5" t="s">
+        <v>2133</v>
+      </c>
+      <c r="G665" s="3" t="s">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="666" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A666" s="3" t="s">
         <v>2126</v>
       </c>
-      <c r="B665" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C665" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E665" s="3" t="s">
+      <c r="B666" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C666" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E666" s="3" t="s">
         <v>2130</v>
       </c>
-      <c r="F665" s="5" t="s">
+      <c r="F666" s="5" t="s">
         <v>2134</v>
       </c>
-      <c r="G665" s="3" t="s">
+      <c r="G666" s="3" t="s">
         <v>2139</v>
-      </c>
-    </row>
-    <row r="666" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A666" t="s">
-        <v>2120</v>
-      </c>
-      <c r="B666" t="b">
-        <v>1</v>
-      </c>
-      <c r="C666" t="b">
-        <v>1</v>
-      </c>
-      <c r="E666" t="s">
-        <v>2121</v>
-      </c>
-      <c r="F666" s="5" t="s">
-        <v>2122</v>
-      </c>
-      <c r="G666" t="s">
-        <v>2140</v>
       </c>
     </row>
     <row r="667" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>2141</v>
+        <v>2120</v>
       </c>
       <c r="B667" t="b">
         <v>1</v>
       </c>
-      <c r="C667" s="3" t="b">
+      <c r="C667" t="b">
         <v>1</v>
       </c>
       <c r="E667" t="s">
-        <v>2144</v>
+        <v>2121</v>
       </c>
       <c r="F667" s="5" t="s">
-        <v>2147</v>
+        <v>2122</v>
       </c>
       <c r="G667" t="s">
-        <v>2150</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="668" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>2142</v>
-      </c>
-      <c r="B668" s="3" t="b">
+        <v>2141</v>
+      </c>
+      <c r="B668" t="b">
         <v>1</v>
       </c>
       <c r="C668" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E668" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="F668" s="5" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="G668" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="B669" s="3" t="b">
         <v>1</v>
@@ -22223,18 +22247,18 @@
         <v>1</v>
       </c>
       <c r="E669" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="F669" s="5" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="G669" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="670" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>2159</v>
+        <v>2143</v>
       </c>
       <c r="B670" s="3" t="b">
         <v>1</v>
@@ -22243,18 +22267,18 @@
         <v>1</v>
       </c>
       <c r="E670" t="s">
-        <v>2165</v>
+        <v>2146</v>
       </c>
       <c r="F670" s="5" t="s">
-        <v>2171</v>
+        <v>2149</v>
       </c>
       <c r="G670" t="s">
-        <v>2177</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="671" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="B671" s="3" t="b">
         <v>1</v>
@@ -22263,18 +22287,18 @@
         <v>1</v>
       </c>
       <c r="E671" t="s">
-        <v>2169</v>
+        <v>2165</v>
       </c>
       <c r="F671" s="5" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="G671" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="B672" s="3" t="b">
         <v>1</v>
@@ -22282,19 +22306,19 @@
       <c r="C672" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E672" s="3" t="s">
-        <v>2166</v>
+      <c r="E672" t="s">
+        <v>2169</v>
       </c>
       <c r="F672" s="5" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="G672" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="673" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="B673" s="3" t="b">
         <v>1</v>
@@ -22303,18 +22327,18 @@
         <v>1</v>
       </c>
       <c r="E673" s="3" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="F673" s="5" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="G673" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="674" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="B674" s="3" t="b">
         <v>1</v>
@@ -22323,59 +22347,58 @@
         <v>1</v>
       </c>
       <c r="E674" s="3" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="F674" s="5" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="G674" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
+        <v>2163</v>
+      </c>
+      <c r="B675" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C675" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E675" s="3" t="s">
+        <v>2168</v>
+      </c>
+      <c r="F675" s="5" t="s">
+        <v>2175</v>
+      </c>
+      <c r="G675" t="s">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="676" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A676" t="s">
         <v>2164</v>
       </c>
-      <c r="B675" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C675" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E675" s="3" t="s">
+      <c r="B676" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C676" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E676" s="3" t="s">
         <v>2170</v>
       </c>
-      <c r="F675" s="5" t="s">
+      <c r="F676" s="5" t="s">
         <v>2176</v>
       </c>
-      <c r="G675" t="s">
+      <c r="G676" t="s">
         <v>2182</v>
-      </c>
-    </row>
-    <row r="676" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A676" s="3" t="s">
-        <v>1688</v>
-      </c>
-      <c r="B676" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C676" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D676" s="3"/>
-      <c r="E676" s="3" t="s">
-        <v>1688</v>
-      </c>
-      <c r="F676" s="5" t="s">
-        <v>1999</v>
-      </c>
-      <c r="G676" s="3" t="s">
-        <v>1724</v>
       </c>
     </row>
     <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" s="3" t="s">
-        <v>1997</v>
+        <v>1688</v>
       </c>
       <c r="B677" s="3" t="b">
         <v>1</v>
@@ -22385,10 +22408,10 @@
       </c>
       <c r="D677" s="3"/>
       <c r="E677" s="3" t="s">
-        <v>1997</v>
+        <v>1688</v>
       </c>
       <c r="F677" s="5" t="s">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="G677" s="3" t="s">
         <v>1724</v>
@@ -22396,7 +22419,7 @@
     </row>
     <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678" s="3" t="s">
-        <v>2541</v>
+        <v>1997</v>
       </c>
       <c r="B678" s="3" t="b">
         <v>1</v>
@@ -22406,18 +22429,18 @@
       </c>
       <c r="D678" s="3"/>
       <c r="E678" s="3" t="s">
-        <v>1750</v>
+        <v>1997</v>
       </c>
       <c r="F678" s="5" t="s">
-        <v>2542</v>
+        <v>1998</v>
       </c>
       <c r="G678" s="3" t="s">
-        <v>1481</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="679" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A679" s="3" t="s">
-        <v>822</v>
+        <v>2541</v>
       </c>
       <c r="B679" s="3" t="b">
         <v>1</v>
@@ -22427,18 +22450,18 @@
       </c>
       <c r="D679" s="3"/>
       <c r="E679" s="3" t="s">
-        <v>824</v>
+        <v>1750</v>
       </c>
       <c r="F679" s="5" t="s">
-        <v>823</v>
+        <v>2542</v>
       </c>
       <c r="G679" s="3" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A680" s="3" t="s">
-        <v>811</v>
+        <v>822</v>
       </c>
       <c r="B680" s="3" t="b">
         <v>1</v>
@@ -22448,99 +22471,100 @@
       </c>
       <c r="D680" s="3"/>
       <c r="E680" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="F680" s="5" t="s">
+        <v>823</v>
+      </c>
+      <c r="G680" s="3" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="681" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A681" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="B681" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C681" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D681" s="3"/>
+      <c r="E681" s="3" t="s">
         <v>803</v>
       </c>
-      <c r="F680" s="5" t="s">
+      <c r="F681" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="G680" s="3" t="s">
+      <c r="G681" s="3" t="s">
         <v>1479</v>
-      </c>
-    </row>
-    <row r="681" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A681" s="3" t="s">
-        <v>813</v>
-      </c>
-      <c r="B681" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C681" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E681" s="3" t="s">
-        <v>815</v>
-      </c>
-      <c r="F681" s="5" t="s">
-        <v>814</v>
-      </c>
-      <c r="G681" s="3" t="s">
-        <v>1482</v>
       </c>
     </row>
     <row r="682" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A682" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="B682" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C682" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E682" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="F682" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="G682" s="3" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="683" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A683" s="3" t="s">
         <v>2103</v>
       </c>
-      <c r="B682" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C682" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E682" s="3" t="s">
+      <c r="B683" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C683" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E683" s="3" t="s">
         <v>1673</v>
       </c>
-      <c r="F682" s="5" t="s">
+      <c r="F683" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="G682" s="3" t="s">
+      <c r="G683" s="3" t="s">
         <v>1486</v>
       </c>
     </row>
-    <row r="683" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A683" s="3" t="s">
+    <row r="684" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A684" s="3" t="s">
         <v>2104</v>
       </c>
-      <c r="B683" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C683" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D683" s="3"/>
-      <c r="E683" s="3" t="s">
+      <c r="B684" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C684" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D684" s="3"/>
+      <c r="E684" s="3" t="s">
         <v>1674</v>
       </c>
-      <c r="F683" s="5" t="s">
+      <c r="F684" s="5" t="s">
         <v>826</v>
       </c>
-      <c r="G683" s="3" t="s">
+      <c r="G684" s="3" t="s">
         <v>1487</v>
-      </c>
-    </row>
-    <row r="684" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A684" s="3" t="s">
-        <v>2105</v>
-      </c>
-      <c r="B684" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C684" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E684" s="3" t="s">
-        <v>1675</v>
-      </c>
-      <c r="F684" s="5" t="s">
-        <v>827</v>
-      </c>
-      <c r="G684" s="3" t="s">
-        <v>1488</v>
       </c>
     </row>
     <row r="685" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A685" s="3" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="B685" s="3" t="b">
         <v>1</v>
@@ -22549,59 +22573,58 @@
         <v>1</v>
       </c>
       <c r="E685" s="3" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="F685" s="5" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G685" s="3" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="686" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A686" s="3" t="s">
+        <v>2106</v>
+      </c>
+      <c r="B686" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C686" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E686" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="F686" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="G686" s="3" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="687" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A687" s="3" t="s">
         <v>2107</v>
       </c>
-      <c r="B686" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C686" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E686" s="3" t="s">
+      <c r="B687" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C687" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E687" s="3" t="s">
         <v>2108</v>
       </c>
-      <c r="F686" s="5" t="s">
+      <c r="F687" s="5" t="s">
         <v>2109</v>
       </c>
-      <c r="G686" s="3" t="s">
+      <c r="G687" s="3" t="s">
         <v>2110</v>
-      </c>
-    </row>
-    <row r="687" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A687" s="3" t="s">
-        <v>819</v>
-      </c>
-      <c r="B687" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C687" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D687" s="3"/>
-      <c r="E687" s="3" t="s">
-        <v>821</v>
-      </c>
-      <c r="F687" s="5" t="s">
-        <v>820</v>
-      </c>
-      <c r="G687" s="3" t="s">
-        <v>1484</v>
       </c>
     </row>
     <row r="688" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A688" s="3" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
       <c r="B688" s="3" t="b">
         <v>1</v>
@@ -22611,118 +22634,119 @@
       </c>
       <c r="D688" s="3"/>
       <c r="E688" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="F688" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="G688" s="3" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="689" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A689" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="B689" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C689" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D689" s="3"/>
+      <c r="E689" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="F688" s="5" t="s">
+      <c r="F689" s="5" t="s">
         <v>817</v>
       </c>
-      <c r="G688" s="3" t="s">
+      <c r="G689" s="3" t="s">
         <v>1483</v>
-      </c>
-    </row>
-    <row r="689" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A689" t="s">
-        <v>2183</v>
-      </c>
-      <c r="B689" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C689" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E689" t="s">
-        <v>1690</v>
-      </c>
-      <c r="F689" s="5" t="s">
-        <v>2188</v>
-      </c>
-      <c r="G689" t="s">
-        <v>1725</v>
       </c>
     </row>
     <row r="690" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
+        <v>2183</v>
+      </c>
+      <c r="B690" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C690" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E690" t="s">
+        <v>1690</v>
+      </c>
+      <c r="F690" s="5" t="s">
+        <v>2188</v>
+      </c>
+      <c r="G690" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="691" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A691" t="s">
         <v>2184</v>
       </c>
-      <c r="B690" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C690" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E690" s="3" t="s">
+      <c r="B691" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C691" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E691" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="F690" s="5" t="s">
+      <c r="F691" s="5" t="s">
         <v>1697</v>
       </c>
-      <c r="G690" t="s">
+      <c r="G691" t="s">
         <v>1348</v>
-      </c>
-    </row>
-    <row r="691" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A691" s="3" t="s">
-        <v>2185</v>
-      </c>
-      <c r="B691" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C691" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E691" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="F691" s="5" t="s">
-        <v>2189</v>
-      </c>
-      <c r="G691" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="692" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A692" s="3" t="s">
+        <v>2185</v>
+      </c>
+      <c r="B692" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C692" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E692" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="F692" s="5" t="s">
+        <v>2189</v>
+      </c>
+      <c r="G692" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="693" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A693" s="3" t="s">
         <v>2186</v>
       </c>
-      <c r="B692" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C692" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E692" s="3" t="s">
+      <c r="B693" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C693" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E693" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="F692" s="5" t="s">
+      <c r="F693" s="5" t="s">
         <v>1695</v>
       </c>
-      <c r="G692" t="s">
+      <c r="G693" t="s">
         <v>1355</v>
-      </c>
-    </row>
-    <row r="693" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A693" t="s">
-        <v>2187</v>
-      </c>
-      <c r="B693" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C693" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E693" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="F693" s="5" t="s">
-        <v>1696</v>
-      </c>
-      <c r="G693" t="s">
-        <v>1352</v>
       </c>
     </row>
     <row r="694" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>2190</v>
+        <v>2187</v>
       </c>
       <c r="B694" s="3" t="b">
         <v>1</v>
@@ -22730,19 +22754,19 @@
       <c r="C694" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E694" t="s">
-        <v>2192</v>
+      <c r="E694" s="3" t="s">
+        <v>428</v>
       </c>
       <c r="F694" s="5" t="s">
-        <v>2194</v>
+        <v>1696</v>
       </c>
       <c r="G694" t="s">
-        <v>2196</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="695" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="B695" s="3" t="b">
         <v>1</v>
@@ -22751,38 +22775,38 @@
         <v>1</v>
       </c>
       <c r="E695" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="F695" s="5" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="G695" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="696" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>2198</v>
-      </c>
-      <c r="B696" t="b">
-        <v>1</v>
-      </c>
-      <c r="C696" t="b">
+        <v>2191</v>
+      </c>
+      <c r="B696" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C696" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E696" t="s">
-        <v>2199</v>
+        <v>2193</v>
       </c>
       <c r="F696" s="5" t="s">
-        <v>2200</v>
+        <v>2195</v>
       </c>
       <c r="G696" t="s">
-        <v>2201</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="697" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1984</v>
+        <v>2198</v>
       </c>
       <c r="B697" t="b">
         <v>1</v>
@@ -22791,41 +22815,38 @@
         <v>1</v>
       </c>
       <c r="E697" t="s">
-        <v>1984</v>
+        <v>2199</v>
       </c>
       <c r="F697" s="5" t="s">
-        <v>1985</v>
-      </c>
-      <c r="G697" s="3" t="s">
-        <v>1986</v>
+        <v>2200</v>
+      </c>
+      <c r="G697" t="s">
+        <v>2201</v>
       </c>
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>2207</v>
+        <v>1984</v>
       </c>
       <c r="B698" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C698" t="b">
         <v>1</v>
       </c>
-      <c r="D698" t="s">
-        <v>2212</v>
-      </c>
       <c r="E698" t="s">
-        <v>2207</v>
+        <v>1984</v>
       </c>
       <c r="F698" s="5" t="s">
-        <v>2210</v>
-      </c>
-      <c r="G698" t="s">
-        <v>2213</v>
+        <v>1985</v>
+      </c>
+      <c r="G698" s="3" t="s">
+        <v>1986</v>
       </c>
     </row>
     <row r="699" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="B699" t="b">
         <v>0</v>
@@ -22837,198 +22858,201 @@
         <v>2212</v>
       </c>
       <c r="E699" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
       <c r="F699" s="5" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="G699" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="700" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B700" t="b">
+        <v>0</v>
+      </c>
+      <c r="C700" t="b">
+        <v>1</v>
+      </c>
+      <c r="D700" t="s">
+        <v>2212</v>
+      </c>
+      <c r="E700" t="s">
+        <v>2209</v>
+      </c>
+      <c r="F700" s="5" t="s">
+        <v>2211</v>
+      </c>
+      <c r="G700" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="701" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
         <v>2522</v>
       </c>
-      <c r="B700" t="b">
-        <v>1</v>
-      </c>
-      <c r="C700" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E700" t="s">
+      <c r="B701" t="b">
+        <v>1</v>
+      </c>
+      <c r="C701" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E701" t="s">
         <v>2526</v>
       </c>
-      <c r="F700" s="5" t="s">
+      <c r="F701" s="5" t="s">
         <v>2216</v>
-      </c>
-      <c r="G700" t="s">
-        <v>2217</v>
-      </c>
-    </row>
-    <row r="701" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A701" s="3" t="s">
-        <v>2523</v>
-      </c>
-      <c r="B701" t="b">
-        <v>1</v>
-      </c>
-      <c r="C701" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E701" t="s">
-        <v>2527</v>
-      </c>
-      <c r="F701" s="5" t="s">
-        <v>2215</v>
       </c>
       <c r="G701" t="s">
         <v>2217</v>
       </c>
     </row>
-    <row r="702" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="702" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A702" s="3" t="s">
-        <v>2524</v>
-      </c>
-      <c r="B702" s="3" t="b">
+        <v>2523</v>
+      </c>
+      <c r="B702" t="b">
         <v>1</v>
       </c>
       <c r="C702" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E702" s="3" t="s">
-        <v>320</v>
+      <c r="E702" t="s">
+        <v>2527</v>
       </c>
       <c r="F702" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="G702" s="3" t="s">
-        <v>1315</v>
+        <v>2215</v>
+      </c>
+      <c r="G702" t="s">
+        <v>2217</v>
       </c>
     </row>
     <row r="703" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A703" s="3" t="s">
+        <v>2524</v>
+      </c>
+      <c r="B703" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C703" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E703" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F703" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G703" s="3" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="704" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A704" s="3" t="s">
         <v>2525</v>
       </c>
-      <c r="B703" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C703" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E703" s="3" t="s">
+      <c r="B704" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C704" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E704" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F703" s="5" t="s">
+      <c r="F704" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="G703" s="3" t="s">
+      <c r="G704" s="3" t="s">
         <v>1316</v>
-      </c>
-    </row>
-    <row r="704" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A704" t="s">
-        <v>2274</v>
-      </c>
-      <c r="B704" t="b">
-        <v>1</v>
-      </c>
-      <c r="C704" t="b">
-        <v>1</v>
-      </c>
-      <c r="E704" t="s">
-        <v>2263</v>
-      </c>
-      <c r="F704" s="5" t="s">
-        <v>2264</v>
-      </c>
-      <c r="G704" t="s">
-        <v>2286</v>
       </c>
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>2276</v>
+        <v>2274</v>
       </c>
       <c r="B705" t="b">
         <v>1</v>
       </c>
       <c r="C705" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E705" t="s">
-        <v>2275</v>
+        <v>2263</v>
       </c>
       <c r="F705" s="5" t="s">
-        <v>2277</v>
+        <v>2264</v>
       </c>
       <c r="G705" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="706" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B706" t="b">
+        <v>1</v>
+      </c>
+      <c r="C706" t="b">
+        <v>0</v>
+      </c>
+      <c r="E706" t="s">
+        <v>2275</v>
+      </c>
+      <c r="F706" s="5" t="s">
+        <v>2277</v>
+      </c>
+      <c r="G706" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="707" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A707" t="s">
         <v>2280</v>
       </c>
-      <c r="B706" t="b">
-        <v>1</v>
-      </c>
-      <c r="C706" t="b">
-        <v>0</v>
-      </c>
-      <c r="E706" t="s">
+      <c r="B707" t="b">
+        <v>1</v>
+      </c>
+      <c r="C707" t="b">
+        <v>0</v>
+      </c>
+      <c r="E707" t="s">
         <v>2278</v>
       </c>
-      <c r="F706" s="5" t="s">
+      <c r="F707" s="5" t="s">
         <v>2279</v>
       </c>
-      <c r="G706" t="s">
+      <c r="G707" t="s">
         <v>2288</v>
       </c>
     </row>
-    <row r="707" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A707" s="3" t="s">
+    <row r="708" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A708" s="3" t="s">
         <v>2283</v>
       </c>
-      <c r="B707" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C707" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E707" s="3" t="s">
+      <c r="B708" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C708" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E708" s="3" t="s">
         <v>2284</v>
       </c>
-      <c r="F707" s="5" t="s">
+      <c r="F708" s="5" t="s">
         <v>2285</v>
       </c>
-      <c r="G707" s="3" t="s">
+      <c r="G708" s="3" t="s">
         <v>2289</v>
-      </c>
-    </row>
-    <row r="708" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A708" t="s">
-        <v>2290</v>
-      </c>
-      <c r="B708" t="b">
-        <v>0</v>
-      </c>
-      <c r="C708" t="b">
-        <v>1</v>
-      </c>
-      <c r="E708" t="s">
-        <v>2293</v>
-      </c>
-      <c r="F708" s="5" t="s">
-        <v>2294</v>
-      </c>
-      <c r="G708" t="s">
-        <v>2303</v>
       </c>
     </row>
     <row r="709" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="B709" t="b">
         <v>0</v>
@@ -23037,58 +23061,58 @@
         <v>1</v>
       </c>
       <c r="E709" t="s">
-        <v>2292</v>
+        <v>2293</v>
       </c>
       <c r="F709" s="5" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="G709" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="710" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>2297</v>
+        <v>2291</v>
       </c>
       <c r="B710" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C710" t="b">
         <v>1</v>
       </c>
       <c r="E710" t="s">
-        <v>2299</v>
+        <v>2292</v>
       </c>
       <c r="F710" s="5" t="s">
-        <v>2302</v>
+        <v>2295</v>
       </c>
       <c r="G710" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="711" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>2298</v>
-      </c>
-      <c r="B711" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C711" s="3" t="b">
+        <v>2297</v>
+      </c>
+      <c r="B711" t="b">
+        <v>1</v>
+      </c>
+      <c r="C711" t="b">
         <v>1</v>
       </c>
       <c r="E711" t="s">
-        <v>493</v>
+        <v>2299</v>
       </c>
       <c r="F711" s="5" t="s">
-        <v>492</v>
+        <v>2302</v>
       </c>
       <c r="G711" t="s">
-        <v>1376</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="712" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>2361</v>
+        <v>2298</v>
       </c>
       <c r="B712" s="3" t="b">
         <v>1</v>
@@ -23097,41 +23121,38 @@
         <v>1</v>
       </c>
       <c r="E712" t="s">
-        <v>2300</v>
+        <v>493</v>
       </c>
       <c r="F712" s="5" t="s">
-        <v>2301</v>
+        <v>492</v>
       </c>
       <c r="G712" t="s">
-        <v>2306</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>2309</v>
-      </c>
-      <c r="B713" t="b">
-        <v>0</v>
-      </c>
-      <c r="C713" t="b">
-        <v>1</v>
-      </c>
-      <c r="D713" t="s">
-        <v>2310</v>
+        <v>2361</v>
+      </c>
+      <c r="B713" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C713" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="E713" t="s">
-        <v>2312</v>
+        <v>2300</v>
       </c>
       <c r="F713" s="5" t="s">
-        <v>2311</v>
-      </c>
-      <c r="G713" s="3" t="s">
-        <v>2317</v>
+        <v>2301</v>
+      </c>
+      <c r="G713" t="s">
+        <v>2306</v>
       </c>
     </row>
     <row r="714" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>2342</v>
+        <v>2309</v>
       </c>
       <c r="B714" t="b">
         <v>0</v>
@@ -23139,79 +23160,82 @@
       <c r="C714" t="b">
         <v>1</v>
       </c>
+      <c r="D714" t="s">
+        <v>2310</v>
+      </c>
       <c r="E714" t="s">
-        <v>2343</v>
+        <v>2312</v>
       </c>
       <c r="F714" s="5" t="s">
-        <v>2359</v>
-      </c>
-      <c r="G714" t="s">
-        <v>2354</v>
+        <v>2311</v>
+      </c>
+      <c r="G714" s="3" t="s">
+        <v>2317</v>
       </c>
     </row>
     <row r="715" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
+        <v>2342</v>
+      </c>
+      <c r="B715" t="b">
+        <v>0</v>
+      </c>
+      <c r="C715" t="b">
+        <v>1</v>
+      </c>
+      <c r="E715" t="s">
+        <v>2343</v>
+      </c>
+      <c r="F715" s="5" t="s">
+        <v>2359</v>
+      </c>
+      <c r="G715" t="s">
+        <v>2354</v>
+      </c>
+    </row>
+    <row r="716" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A716" t="s">
         <v>2344</v>
       </c>
-      <c r="B715" t="b">
-        <v>0</v>
-      </c>
-      <c r="C715" t="b">
-        <v>1</v>
-      </c>
-      <c r="E715" t="s">
+      <c r="B716" t="b">
+        <v>0</v>
+      </c>
+      <c r="C716" t="b">
+        <v>1</v>
+      </c>
+      <c r="E716" t="s">
         <v>2360</v>
       </c>
-      <c r="F715" s="5" t="s">
+      <c r="F716" s="5" t="s">
         <v>2347</v>
       </c>
-      <c r="G715" t="s">
+      <c r="G716" t="s">
         <v>2355</v>
       </c>
     </row>
-    <row r="716" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A716" s="3" t="s">
+    <row r="717" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A717" s="3" t="s">
         <v>2350</v>
       </c>
-      <c r="B716" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C716" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E716" s="3" t="s">
+      <c r="B717" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C717" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E717" s="3" t="s">
         <v>2351</v>
       </c>
-      <c r="F716" s="5" t="s">
+      <c r="F717" s="5" t="s">
         <v>2352</v>
       </c>
-      <c r="G716" s="3" t="s">
+      <c r="G717" s="3" t="s">
         <v>2356</v>
-      </c>
-    </row>
-    <row r="717" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A717" t="s">
-        <v>2345</v>
-      </c>
-      <c r="B717" t="b">
-        <v>0</v>
-      </c>
-      <c r="C717" t="b">
-        <v>1</v>
-      </c>
-      <c r="E717" t="s">
-        <v>2345</v>
-      </c>
-      <c r="F717" s="5" t="s">
-        <v>2346</v>
-      </c>
-      <c r="G717" t="s">
-        <v>2357</v>
       </c>
     </row>
     <row r="718" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>2349</v>
+        <v>2345</v>
       </c>
       <c r="B718" t="b">
         <v>0</v>
@@ -23220,18 +23244,18 @@
         <v>1</v>
       </c>
       <c r="E718" t="s">
-        <v>2348</v>
+        <v>2345</v>
       </c>
       <c r="F718" s="5" t="s">
-        <v>2353</v>
+        <v>2346</v>
       </c>
       <c r="G718" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>496</v>
+        <v>2349</v>
       </c>
       <c r="B719" t="b">
         <v>0</v>
@@ -23240,18 +23264,18 @@
         <v>1</v>
       </c>
       <c r="E719" t="s">
-        <v>496</v>
+        <v>2348</v>
       </c>
       <c r="F719" s="5" t="s">
-        <v>495</v>
+        <v>2353</v>
       </c>
       <c r="G719" t="s">
-        <v>1377</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>2374</v>
+        <v>496</v>
       </c>
       <c r="B720" t="b">
         <v>0</v>
@@ -23260,18 +23284,18 @@
         <v>1</v>
       </c>
       <c r="E720" t="s">
-        <v>2374</v>
+        <v>496</v>
       </c>
       <c r="F720" s="5" t="s">
-        <v>2375</v>
+        <v>495</v>
       </c>
       <c r="G720" t="s">
-        <v>2387</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>2385</v>
+        <v>2374</v>
       </c>
       <c r="B721" t="b">
         <v>0</v>
@@ -23280,58 +23304,58 @@
         <v>1</v>
       </c>
       <c r="E721" t="s">
-        <v>2386</v>
+        <v>2374</v>
       </c>
       <c r="F721" s="5" t="s">
-        <v>2389</v>
+        <v>2375</v>
       </c>
       <c r="G721" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>2449</v>
+        <v>2385</v>
       </c>
       <c r="B722" t="b">
-        <v>1</v>
-      </c>
-      <c r="C722" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C722" t="b">
         <v>1</v>
       </c>
       <c r="E722" t="s">
-        <v>2390</v>
+        <v>2386</v>
       </c>
       <c r="F722" s="5" t="s">
-        <v>2397</v>
+        <v>2389</v>
       </c>
       <c r="G722" t="s">
-        <v>2404</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>2450</v>
-      </c>
-      <c r="B723" s="3" t="b">
+        <v>2449</v>
+      </c>
+      <c r="B723" t="b">
         <v>1</v>
       </c>
       <c r="C723" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E723" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="F723" s="5" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="G723" t="s">
-        <v>2410</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="B724" s="3" t="b">
         <v>1</v>
@@ -23340,18 +23364,18 @@
         <v>1</v>
       </c>
       <c r="E724" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="F724" s="5" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="G724" t="s">
-        <v>2405</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="B725" s="3" t="b">
         <v>1</v>
@@ -23360,18 +23384,18 @@
         <v>1</v>
       </c>
       <c r="E725" t="s">
-        <v>2394</v>
+        <v>2392</v>
       </c>
       <c r="F725" s="5" t="s">
-        <v>2401</v>
+        <v>2399</v>
       </c>
       <c r="G725" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="B726" s="3" t="b">
         <v>1</v>
@@ -23380,18 +23404,18 @@
         <v>1</v>
       </c>
       <c r="E726" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="F726" s="5" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="G726" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="B727" s="3" t="b">
         <v>1</v>
@@ -23400,18 +23424,18 @@
         <v>1</v>
       </c>
       <c r="E727" t="s">
-        <v>2393</v>
+        <v>2395</v>
       </c>
       <c r="F727" s="5" t="s">
-        <v>2400</v>
+        <v>2402</v>
       </c>
       <c r="G727" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="B728" s="3" t="b">
         <v>1</v>
@@ -23420,38 +23444,38 @@
         <v>1</v>
       </c>
       <c r="E728" t="s">
-        <v>2396</v>
+        <v>2393</v>
       </c>
       <c r="F728" s="5" t="s">
-        <v>2403</v>
+        <v>2400</v>
       </c>
       <c r="G728" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>2471</v>
-      </c>
-      <c r="B729" t="b">
-        <v>1</v>
-      </c>
-      <c r="C729" t="b">
+        <v>2455</v>
+      </c>
+      <c r="B729" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C729" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E729" t="s">
-        <v>2473</v>
+        <v>2396</v>
       </c>
       <c r="F729" s="5" t="s">
-        <v>2475</v>
+        <v>2403</v>
       </c>
       <c r="G729" t="s">
-        <v>2477</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="B730" t="b">
         <v>1</v>
@@ -23460,18 +23484,18 @@
         <v>1</v>
       </c>
       <c r="E730" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="F730" s="5" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="G730" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>2479</v>
+        <v>2472</v>
       </c>
       <c r="B731" t="b">
         <v>1</v>
@@ -23480,18 +23504,18 @@
         <v>1</v>
       </c>
       <c r="E731" t="s">
-        <v>2480</v>
+        <v>2474</v>
       </c>
       <c r="F731" s="5" t="s">
-        <v>2481</v>
+        <v>2476</v>
       </c>
       <c r="G731" t="s">
-        <v>2484</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="732" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>2482</v>
+        <v>2479</v>
       </c>
       <c r="B732" t="b">
         <v>1</v>
@@ -23500,38 +23524,38 @@
         <v>1</v>
       </c>
       <c r="E732" t="s">
-        <v>2495</v>
+        <v>2480</v>
       </c>
       <c r="F732" s="5" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="G732" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>2492</v>
+        <v>2482</v>
       </c>
       <c r="B733" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C733" t="b">
         <v>1</v>
       </c>
       <c r="E733" t="s">
-        <v>2493</v>
+        <v>2495</v>
       </c>
       <c r="F733" s="5" t="s">
-        <v>2494</v>
+        <v>2483</v>
       </c>
       <c r="G733" t="s">
-        <v>2470</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>2518</v>
+        <v>2492</v>
       </c>
       <c r="B734" t="b">
         <v>0</v>
@@ -23540,18 +23564,18 @@
         <v>1</v>
       </c>
       <c r="E734" t="s">
-        <v>2518</v>
+        <v>2493</v>
       </c>
       <c r="F734" s="5" t="s">
-        <v>1087</v>
+        <v>2494</v>
       </c>
       <c r="G734" t="s">
-        <v>2519</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>2578</v>
+        <v>2518</v>
       </c>
       <c r="B735" t="b">
         <v>0</v>
@@ -23560,98 +23584,98 @@
         <v>1</v>
       </c>
       <c r="E735" t="s">
-        <v>2578</v>
+        <v>2518</v>
       </c>
       <c r="F735" s="5" t="s">
-        <v>2579</v>
+        <v>1087</v>
       </c>
       <c r="G735" t="s">
-        <v>2582</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="736" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B736" t="b">
+        <v>0</v>
+      </c>
+      <c r="C736" t="b">
+        <v>1</v>
+      </c>
+      <c r="E736" t="s">
+        <v>2578</v>
+      </c>
+      <c r="F736" s="5" t="s">
+        <v>2579</v>
+      </c>
+      <c r="G736" t="s">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="737" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A737" t="s">
         <v>2580</v>
       </c>
-      <c r="B736" t="b">
-        <v>0</v>
-      </c>
-      <c r="C736" t="b">
-        <v>1</v>
-      </c>
-      <c r="E736" t="s">
+      <c r="B737" t="b">
+        <v>0</v>
+      </c>
+      <c r="C737" t="b">
+        <v>1</v>
+      </c>
+      <c r="E737" t="s">
         <v>2580</v>
       </c>
-      <c r="F736" s="5" t="s">
+      <c r="F737" s="5" t="s">
         <v>2581</v>
       </c>
-      <c r="G736" t="s">
+      <c r="G737" t="s">
         <v>2583</v>
       </c>
     </row>
-    <row r="737" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A737" s="3" t="s">
+    <row r="738" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A738" s="3" t="s">
         <v>2603</v>
       </c>
-      <c r="B737" t="b">
-        <v>1</v>
-      </c>
-      <c r="C737" t="b">
-        <v>1</v>
-      </c>
-      <c r="E737" t="s">
+      <c r="B738" t="b">
+        <v>1</v>
+      </c>
+      <c r="C738" t="b">
+        <v>1</v>
+      </c>
+      <c r="E738" t="s">
         <v>2604</v>
       </c>
-      <c r="F737" s="5" t="s">
+      <c r="F738" s="5" t="s">
         <v>1695</v>
       </c>
-      <c r="G737" t="s">
+      <c r="G738" t="s">
         <v>2605</v>
       </c>
     </row>
-    <row r="738" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A738" s="3" t="s">
+    <row r="739" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A739" s="3" t="s">
         <v>2627</v>
       </c>
-      <c r="B738" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C738" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E738" s="3" t="s">
+      <c r="B739" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C739" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E739" s="3" t="s">
         <v>2628</v>
       </c>
-      <c r="F738" s="5" t="s">
+      <c r="F739" s="5" t="s">
         <v>2629</v>
       </c>
-      <c r="G738" s="3" t="s">
+      <c r="G739" s="3" t="s">
         <v>2630</v>
-      </c>
-    </row>
-    <row r="739" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A739" t="s">
-        <v>2606</v>
-      </c>
-      <c r="B739" t="b">
-        <v>1</v>
-      </c>
-      <c r="C739" t="b">
-        <v>0</v>
-      </c>
-      <c r="E739" t="s">
-        <v>2614</v>
-      </c>
-      <c r="F739" s="5" t="s">
-        <v>2615</v>
-      </c>
-      <c r="G739" t="s">
-        <v>2617</v>
       </c>
     </row>
     <row r="740" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
       <c r="B740" t="b">
         <v>1</v>
@@ -23660,92 +23684,146 @@
         <v>0</v>
       </c>
       <c r="E740" t="s">
-        <v>2607</v>
+        <v>2614</v>
       </c>
       <c r="F740" s="5" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="G740" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="741" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>2620</v>
+        <v>2608</v>
       </c>
       <c r="B741" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C741" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E741" t="s">
-        <v>2620</v>
+        <v>2607</v>
       </c>
       <c r="F741" s="5" t="s">
-        <v>2613</v>
+        <v>2616</v>
       </c>
       <c r="G741" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="742" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
+        <v>2620</v>
+      </c>
+      <c r="B742" t="b">
+        <v>0</v>
+      </c>
+      <c r="C742" t="b">
+        <v>1</v>
+      </c>
+      <c r="E742" t="s">
+        <v>2620</v>
+      </c>
+      <c r="F742" s="5" t="s">
+        <v>2613</v>
+      </c>
+      <c r="G742" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="743" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
         <v>2621</v>
       </c>
-      <c r="B742" t="b">
-        <v>0</v>
-      </c>
-      <c r="C742" t="b">
-        <v>1</v>
-      </c>
-      <c r="E742" t="s">
+      <c r="B743" t="b">
+        <v>0</v>
+      </c>
+      <c r="C743" t="b">
+        <v>1</v>
+      </c>
+      <c r="E743" t="s">
         <v>2621</v>
       </c>
-      <c r="F742" s="5" t="s">
+      <c r="F743" s="5" t="s">
         <v>2622</v>
       </c>
     </row>
-    <row r="743" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A743" s="3" t="s">
+    <row r="744" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A744" s="3" t="s">
         <v>2626</v>
       </c>
-      <c r="B743" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C743" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D743" s="3"/>
-      <c r="E743" s="3" t="s">
+      <c r="B744" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C744" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D744" s="3"/>
+      <c r="E744" s="3" t="s">
         <v>2623</v>
       </c>
-      <c r="F743" s="5" t="s">
+      <c r="F744" s="5" t="s">
         <v>2624</v>
       </c>
-      <c r="G743" s="3" t="s">
+      <c r="G744" s="3" t="s">
         <v>2625</v>
       </c>
     </row>
-    <row r="744" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A744" t="s">
+    <row r="745" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A745" t="s">
         <v>2631</v>
       </c>
-      <c r="B744" t="b">
-        <v>0</v>
-      </c>
-      <c r="C744" t="b">
-        <v>1</v>
-      </c>
-      <c r="E744" t="s">
+      <c r="B745" t="b">
+        <v>0</v>
+      </c>
+      <c r="C745" t="b">
+        <v>1</v>
+      </c>
+      <c r="E745" t="s">
         <v>2632</v>
       </c>
-      <c r="F744" s="5" t="s">
+      <c r="F745" s="5" t="s">
         <v>2633</v>
       </c>
     </row>
+    <row r="746" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A746" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B746" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C746" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E746" t="s">
+        <v>2641</v>
+      </c>
+      <c r="F746" s="5" t="s">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="747" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A747" t="s">
+        <v>2638</v>
+      </c>
+      <c r="B747" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C747" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E747" t="s">
+        <v>2642</v>
+      </c>
+      <c r="F747" s="5" t="s">
+        <v>2639</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G734" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G735" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on the report definition API
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987E9ED5-E93D-414A-BCB8-77AD0FC30016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5C46D7-DCC8-4275-989F-06C81BE735A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$735</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$747</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="2643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2997" uniqueCount="2651">
   <si>
     <t>Key</t>
   </si>
@@ -7963,6 +7963,30 @@
   </si>
   <si>
     <t>Not in Main Menu</t>
+  </si>
+  <si>
+    <t>下载</t>
+  </si>
+  <si>
+    <t>所有未保存附件的总大小超过了允许的最大值{{size}}，请保存文档，然后再试一次</t>
+  </si>
+  <si>
+    <t>在主菜单</t>
+  </si>
+  <si>
+    <t>不在主菜单</t>
+  </si>
+  <si>
+    <t>Error_TitleIsRequiredWhenShowInMainMenu</t>
+  </si>
+  <si>
+    <t>Title is required to show the report in the main menu</t>
+  </si>
+  <si>
+    <t>حقل العنوان مطلوب لإظهار التقرير في القائمة الرئيسية</t>
+  </si>
+  <si>
+    <t>标题需要显示在主菜单中的报告</t>
   </si>
 </sst>
 </file>
@@ -8359,12 +8383,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G747"/>
+  <dimension ref="A1:G748"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A724" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E748" sqref="E748"/>
+      <selection pane="bottomLeft" activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23749,6 +23773,9 @@
       <c r="F743" s="5" t="s">
         <v>2622</v>
       </c>
+      <c r="G743" t="s">
+        <v>2643</v>
+      </c>
     </row>
     <row r="744" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A744" s="3" t="s">
@@ -23787,6 +23814,9 @@
       <c r="F745" s="5" t="s">
         <v>2633</v>
       </c>
+      <c r="G745" t="s">
+        <v>2644</v>
+      </c>
     </row>
     <row r="746" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
@@ -23804,6 +23834,9 @@
       <c r="F746" s="5" t="s">
         <v>2640</v>
       </c>
+      <c r="G746" t="s">
+        <v>2645</v>
+      </c>
     </row>
     <row r="747" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
@@ -23821,9 +23854,32 @@
       <c r="F747" s="5" t="s">
         <v>2639</v>
       </c>
+      <c r="G747" t="s">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="748" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A748" t="s">
+        <v>2647</v>
+      </c>
+      <c r="B748" t="b">
+        <v>1</v>
+      </c>
+      <c r="C748" t="b">
+        <v>0</v>
+      </c>
+      <c r="E748" t="s">
+        <v>2648</v>
+      </c>
+      <c r="F748" s="5" t="s">
+        <v>2649</v>
+      </c>
+      <c r="G748" t="s">
+        <v>2650</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G735" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G747" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Document.Assignee to metadata
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582B4A65-5222-4FE0-9763-91DDB0A334EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FB149A-04A2-4612-B65F-86FC924C57D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -6993,9 +6993,6 @@
     <t>文件资料</t>
   </si>
   <si>
-    <t>Document_Assingee</t>
-  </si>
-  <si>
     <t>Document_Comment</t>
   </si>
   <si>
@@ -8110,6 +8107,9 @@
   </si>
   <si>
     <t>Line_Definition</t>
+  </si>
+  <si>
+    <t>Document_Assignee</t>
   </si>
 </sst>
 </file>
@@ -8509,9 +8509,9 @@
   <dimension ref="A1:G761"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A468" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A463" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B493" sqref="B493"/>
+      <selection pane="bottomLeft" activeCell="E486" sqref="E486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9462,10 +9462,10 @@
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
+        <v>2380</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>2381</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>2382</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>1236</v>
@@ -9483,10 +9483,10 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>1626</v>
@@ -15807,7 +15807,7 @@
         <v>2267</v>
       </c>
       <c r="G347" s="3" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="348" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -15827,12 +15827,12 @@
         <v>2273</v>
       </c>
       <c r="G348" s="3" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="B349" s="3" t="b">
         <v>0</v>
@@ -15853,7 +15853,7 @@
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="B350" s="3" t="b">
         <v>0</v>
@@ -15874,7 +15874,7 @@
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="B351" s="3" t="b">
         <v>0</v>
@@ -15895,7 +15895,7 @@
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="B352" s="3" t="b">
         <v>0</v>
@@ -15916,7 +15916,7 @@
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="B353" s="3" t="b">
         <v>0</v>
@@ -15937,7 +15937,7 @@
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="B354" s="3" t="b">
         <v>0</v>
@@ -15958,7 +15958,7 @@
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" s="3" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="B355" s="3" t="b">
         <v>0</v>
@@ -15988,10 +15988,10 @@
         <v>1</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="F356" s="5" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="G356" s="3" t="s">
         <v>1574</v>
@@ -16008,10 +16008,10 @@
         <v>1</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="F357" s="5" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="G357" s="3" t="s">
         <v>1575</v>
@@ -16028,10 +16028,10 @@
         <v>1</v>
       </c>
       <c r="E358" s="3" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="F358" s="5" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="G358" s="3" t="s">
         <v>1576</v>
@@ -16048,10 +16048,10 @@
         <v>1</v>
       </c>
       <c r="E359" s="3" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="F359" s="5" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="G359" s="3" t="s">
         <v>1577</v>
@@ -16068,10 +16068,10 @@
         <v>1</v>
       </c>
       <c r="E360" s="3" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="F360" s="5" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="G360" s="3" t="s">
         <v>1578</v>
@@ -16088,10 +16088,10 @@
         <v>1</v>
       </c>
       <c r="E361" s="3" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="F361" s="5" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="G361" s="3" t="s">
         <v>1579</v>
@@ -16108,10 +16108,10 @@
         <v>1</v>
       </c>
       <c r="E362" s="3" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="F362" s="5" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="G362" s="3" t="s">
         <v>1580</v>
@@ -16371,7 +16371,7 @@
     </row>
     <row r="375" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="B375" s="3" t="b">
         <v>1</v>
@@ -16380,18 +16380,18 @@
         <v>1</v>
       </c>
       <c r="E375" s="3" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="F375" s="5" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="G375" s="3" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="376" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="B376" s="3" t="b">
         <v>1</v>
@@ -16400,18 +16400,18 @@
         <v>1</v>
       </c>
       <c r="E376" s="3" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="F376" s="5" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="G376" s="3" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="377" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="B377" s="3" t="b">
         <v>1</v>
@@ -16420,18 +16420,18 @@
         <v>1</v>
       </c>
       <c r="E377" s="3" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="F377" s="5" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="G377" s="3" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="378" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="B378" s="3" t="b">
         <v>1</v>
@@ -16440,13 +16440,13 @@
         <v>1</v>
       </c>
       <c r="E378" s="3" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="F378" s="5" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="G378" s="3" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
@@ -17123,7 +17123,7 @@
     </row>
     <row r="411" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="B411" s="3" t="b">
         <v>1</v>
@@ -18546,22 +18546,22 @@
     </row>
     <row r="479" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
+        <v>2608</v>
+      </c>
+      <c r="B479" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C479" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E479" s="3" t="s">
         <v>2609</v>
       </c>
-      <c r="B479" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C479" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E479" s="3" t="s">
+      <c r="F479" s="5" t="s">
         <v>2610</v>
       </c>
-      <c r="F479" s="5" t="s">
+      <c r="G479" s="2" t="s">
         <v>2611</v>
-      </c>
-      <c r="G479" s="2" t="s">
-        <v>2612</v>
       </c>
     </row>
     <row r="480" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -18586,7 +18586,7 @@
     </row>
     <row r="481" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
-        <v>2319</v>
+        <v>2691</v>
       </c>
       <c r="B481" s="3" t="b">
         <v>1</v>
@@ -18595,10 +18595,10 @@
         <v>1</v>
       </c>
       <c r="E481" s="3" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="F481" s="5" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="G481" s="3" t="s">
         <v>1212</v>
@@ -18606,7 +18606,7 @@
     </row>
     <row r="482" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A482" s="3" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="B482" s="3" t="b">
         <v>1</v>
@@ -18615,18 +18615,18 @@
         <v>1</v>
       </c>
       <c r="E482" s="3" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="F482" s="5" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="G482" s="3" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="483" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A483" s="3" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="B483" s="3" t="b">
         <v>1</v>
@@ -18635,18 +18635,18 @@
         <v>1</v>
       </c>
       <c r="E483" s="3" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="F483" s="5" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="G483" s="3" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="484" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A484" s="3" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="B484" s="3" t="b">
         <v>1</v>
@@ -18655,18 +18655,18 @@
         <v>1</v>
       </c>
       <c r="E484" s="3" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="F484" s="5" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="G484" s="3" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="485" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A485" s="3" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="B485" s="3" t="b">
         <v>1</v>
@@ -18675,18 +18675,18 @@
         <v>1</v>
       </c>
       <c r="E485" s="3" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="F485" s="5" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="G485" s="3" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="486" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A486" s="3" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="B486" s="3" t="b">
         <v>1</v>
@@ -18695,18 +18695,18 @@
         <v>1</v>
       </c>
       <c r="E486" s="3" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="F486" s="5" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="G486" s="3" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="487" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="B487" s="3" t="b">
         <v>1</v>
@@ -18715,30 +18715,30 @@
         <v>1</v>
       </c>
       <c r="E487" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="F487" s="5" t="s">
-        <v>2688</v>
+        <v>2687</v>
       </c>
       <c r="G487" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B488" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C488" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E488" t="s">
+        <v>2685</v>
+      </c>
+      <c r="F488" s="5" t="s">
         <v>2686</v>
-      </c>
-      <c r="B488" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C488" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E488" t="s">
-        <v>2686</v>
-      </c>
-      <c r="F488" s="5" t="s">
-        <v>2687</v>
       </c>
       <c r="G488" t="s">
         <v>1966</v>
@@ -18746,7 +18746,7 @@
     </row>
     <row r="489" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A489" s="3" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="B489" s="3" t="b">
         <v>1</v>
@@ -18766,7 +18766,7 @@
     </row>
     <row r="490" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="B490" s="3" t="b">
         <v>1</v>
@@ -18778,7 +18778,7 @@
         <v>2313</v>
       </c>
       <c r="F490" s="5" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="G490" s="3" t="s">
         <v>2317</v>
@@ -18846,7 +18846,7 @@
     </row>
     <row r="494" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A494" s="3" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="B494" s="3" t="b">
         <v>1</v>
@@ -18866,47 +18866,47 @@
     </row>
     <row r="495" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A495" s="3" t="s">
+        <v>2650</v>
+      </c>
+      <c r="B495" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C495" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E495" s="3" t="s">
         <v>2651</v>
       </c>
-      <c r="B495" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C495" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E495" s="3" t="s">
+      <c r="F495" s="5" t="s">
         <v>2652</v>
       </c>
-      <c r="F495" s="5" t="s">
-        <v>2653</v>
-      </c>
       <c r="G495" s="3" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="496" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
+        <v>2656</v>
+      </c>
+      <c r="B496" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C496" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E496" s="3" t="s">
         <v>2657</v>
       </c>
-      <c r="B496" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C496" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E496" s="3" t="s">
+      <c r="F496" s="5" t="s">
         <v>2658</v>
       </c>
-      <c r="F496" s="5" t="s">
-        <v>2659</v>
-      </c>
       <c r="G496" s="3" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="497" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
-        <v>2682</v>
+        <v>2681</v>
       </c>
       <c r="B497" s="3" t="b">
         <v>1</v>
@@ -18921,12 +18921,12 @@
         <v>2294</v>
       </c>
       <c r="G497" s="3" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
     </row>
     <row r="498" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
       <c r="B498" s="3" t="b">
         <v>1</v>
@@ -18941,12 +18941,12 @@
         <v>2295</v>
       </c>
       <c r="G498" s="3" t="s">
-        <v>2685</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="499" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="B499" s="3" t="b">
         <v>1</v>
@@ -18966,7 +18966,7 @@
     </row>
     <row r="500" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="B500" s="3" t="b">
         <v>1</v>
@@ -18986,7 +18986,7 @@
     </row>
     <row r="501" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A501" s="3" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="B501" s="3" t="b">
         <v>1</v>
@@ -18995,10 +18995,10 @@
         <v>1</v>
       </c>
       <c r="E501" s="3" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="F501" s="5" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="G501" s="3" t="s">
         <v>2257</v>
@@ -19006,7 +19006,7 @@
     </row>
     <row r="502" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A502" s="3" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="B502" s="3" t="b">
         <v>1</v>
@@ -19015,10 +19015,10 @@
         <v>1</v>
       </c>
       <c r="E502" s="3" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="F502" s="5" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="G502" s="3" t="s">
         <v>2258</v>
@@ -19026,7 +19026,7 @@
     </row>
     <row r="503" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A503" s="3" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="B503" s="3" t="b">
         <v>1</v>
@@ -19035,10 +19035,10 @@
         <v>1</v>
       </c>
       <c r="E503" s="3" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="F503" s="5" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="G503" s="3" t="s">
         <v>2259</v>
@@ -19046,7 +19046,7 @@
     </row>
     <row r="504" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A504" s="3" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="B504" s="3" t="b">
         <v>1</v>
@@ -19055,10 +19055,10 @@
         <v>1</v>
       </c>
       <c r="E504" s="3" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="F504" s="5" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="G504" s="3" t="s">
         <v>2260</v>
@@ -19087,7 +19087,7 @@
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A506" s="3" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="B506" s="3" t="b">
         <v>1</v>
@@ -19097,10 +19097,10 @@
       </c>
       <c r="D506" s="3"/>
       <c r="E506" s="3" t="s">
+        <v>2377</v>
+      </c>
+      <c r="F506" s="5" t="s">
         <v>2378</v>
-      </c>
-      <c r="F506" s="5" t="s">
-        <v>2379</v>
       </c>
       <c r="G506" s="3" t="s">
         <v>2244</v>
@@ -19142,7 +19142,7 @@
         <v>1689</v>
       </c>
       <c r="F508" s="5" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="G508" s="3" t="s">
         <v>1723</v>
@@ -19284,10 +19284,10 @@
       </c>
       <c r="D515" s="3"/>
       <c r="E515" s="3" t="s">
+        <v>2375</v>
+      </c>
+      <c r="F515" s="5" t="s">
         <v>2376</v>
-      </c>
-      <c r="F515" s="5" t="s">
-        <v>2377</v>
       </c>
       <c r="G515" s="3" t="s">
         <v>1352</v>
@@ -19439,7 +19439,7 @@
     </row>
     <row r="523" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A523" s="3" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
       <c r="B523" s="3" t="b">
         <v>1</v>
@@ -19448,10 +19448,10 @@
         <v>1</v>
       </c>
       <c r="E523" s="3" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="F523" s="5" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="G523" s="3" t="s">
         <v>1990</v>
@@ -19459,19 +19459,19 @@
     </row>
     <row r="524" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A524" s="3" t="s">
+        <v>2528</v>
+      </c>
+      <c r="B524" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C524" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E524" s="3" t="s">
         <v>2529</v>
       </c>
-      <c r="B524" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C524" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E524" s="3" t="s">
-        <v>2530</v>
-      </c>
       <c r="F524" s="5" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="G524" s="3" t="s">
         <v>1990</v>
@@ -19500,7 +19500,7 @@
     </row>
     <row r="526" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A526" s="3" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="B526" s="3" t="b">
         <v>1</v>
@@ -19510,10 +19510,10 @@
       </c>
       <c r="D526" s="3"/>
       <c r="E526" s="3" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="F526" s="5" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="G526" s="3" t="s">
         <v>1732</v>
@@ -19521,7 +19521,7 @@
     </row>
     <row r="527" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A527" s="3" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="B527" s="3" t="b">
         <v>1</v>
@@ -19531,10 +19531,10 @@
       </c>
       <c r="D527" s="3"/>
       <c r="E527" s="3" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="F527" s="5" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="G527" s="3" t="s">
         <v>1732</v>
@@ -19542,7 +19542,7 @@
     </row>
     <row r="528" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A528" s="3" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="B528" s="3" t="b">
         <v>1</v>
@@ -19689,7 +19689,7 @@
     </row>
     <row r="535" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A535" s="3" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="B535" s="3" t="b">
         <v>1</v>
@@ -19701,15 +19701,15 @@
         <v>2242</v>
       </c>
       <c r="F535" s="5" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="G535" s="3" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="536" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A536" s="3" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="B536" s="3" t="b">
         <v>1</v>
@@ -19718,18 +19718,18 @@
         <v>1</v>
       </c>
       <c r="E536" s="3" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="F536" s="5" t="s">
+        <v>2511</v>
+      </c>
+      <c r="G536" s="3" t="s">
         <v>2512</v>
-      </c>
-      <c r="G536" s="3" t="s">
-        <v>2513</v>
       </c>
     </row>
     <row r="537" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A537" s="3" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="B537" s="3" t="b">
         <v>1</v>
@@ -19738,18 +19738,18 @@
         <v>1</v>
       </c>
       <c r="E537" s="3" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="F537" s="5" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="G537" s="3" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="538" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A538" s="3" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="B538" s="3" t="b">
         <v>1</v>
@@ -19758,53 +19758,53 @@
         <v>1</v>
       </c>
       <c r="E538" s="3" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="F538" s="5" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="G538" s="3" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="539" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A539" s="3" t="s">
+        <v>2503</v>
+      </c>
+      <c r="B539" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C539" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E539" s="3" t="s">
         <v>2504</v>
       </c>
-      <c r="B539" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C539" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E539" s="3" t="s">
+      <c r="F539" s="5" t="s">
         <v>2505</v>
       </c>
-      <c r="F539" s="5" t="s">
-        <v>2506</v>
-      </c>
       <c r="G539" s="3" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
     </row>
     <row r="540" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A540" s="3" t="s">
+        <v>2506</v>
+      </c>
+      <c r="B540" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C540" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E540" s="3" t="s">
         <v>2507</v>
       </c>
-      <c r="B540" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C540" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E540" s="3" t="s">
+      <c r="F540" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="F540" s="5" t="s">
-        <v>2509</v>
-      </c>
       <c r="G540" s="3" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
@@ -19976,7 +19976,7 @@
     </row>
     <row r="549" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A549" s="3" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="B549" s="3" t="b">
         <v>1</v>
@@ -19986,10 +19986,10 @@
       </c>
       <c r="D549" s="3"/>
       <c r="E549" s="3" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="F549" s="5" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="G549" s="3" t="s">
         <v>1481</v>
@@ -20038,7 +20038,7 @@
     </row>
     <row r="552" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A552" s="3" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="B552" s="3" t="b">
         <v>1</v>
@@ -20050,7 +20050,7 @@
         <v>1689</v>
       </c>
       <c r="F552" s="5" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="G552" s="3" t="s">
         <v>1723</v>
@@ -20058,7 +20058,7 @@
     </row>
     <row r="553" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A553" s="3" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="B553" s="3" t="b">
         <v>1</v>
@@ -20067,38 +20067,38 @@
         <v>1</v>
       </c>
       <c r="E553" s="3" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="F553" s="5" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="G553" s="3" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="554" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A554" s="3" t="s">
+        <v>2544</v>
+      </c>
+      <c r="B554" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C554" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E554" s="3" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F554" s="5" t="s">
         <v>2545</v>
       </c>
-      <c r="B554" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C554" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E554" s="3" t="s">
-        <v>2531</v>
-      </c>
-      <c r="F554" s="5" t="s">
-        <v>2546</v>
-      </c>
       <c r="G554" s="3" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="555" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A555" s="3" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="B555" s="3" t="b">
         <v>1</v>
@@ -20110,15 +20110,15 @@
         <v>2242</v>
       </c>
       <c r="F555" s="5" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="G555" s="3" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="556" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A556" s="3" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="B556" s="3" t="b">
         <v>1</v>
@@ -20127,18 +20127,18 @@
         <v>1</v>
       </c>
       <c r="E556" s="3" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="F556" s="5" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="G556" s="3" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="557" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A557" s="3" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="B557" s="3" t="b">
         <v>1</v>
@@ -20147,18 +20147,18 @@
         <v>1</v>
       </c>
       <c r="E557" s="3" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="F557" s="5" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="G557" s="3" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="558" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A558" s="3" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="B558" s="3" t="b">
         <v>1</v>
@@ -20167,18 +20167,18 @@
         <v>1</v>
       </c>
       <c r="E558" s="3" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="F558" s="5" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="G558" s="3" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
     </row>
     <row r="559" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A559" s="3" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="B559" s="3" t="b">
         <v>1</v>
@@ -20187,18 +20187,18 @@
         <v>1</v>
       </c>
       <c r="E559" s="3" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="F559" s="5" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="G559" s="3" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="560" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A560" s="3" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="B560" s="3" t="b">
         <v>1</v>
@@ -20207,18 +20207,18 @@
         <v>1</v>
       </c>
       <c r="E560" s="3" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="F560" s="5" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="G560" s="3" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="561" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A561" s="3" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="B561" s="3" t="b">
         <v>1</v>
@@ -20227,18 +20227,18 @@
         <v>1</v>
       </c>
       <c r="E561" s="3" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="F561" s="5" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="G561" s="3" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="562" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A562" s="3" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="B562" s="3" t="b">
         <v>1</v>
@@ -20247,18 +20247,18 @@
         <v>1</v>
       </c>
       <c r="E562" s="3" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="F562" s="5" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="G562" s="3" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
     </row>
     <row r="563" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A563" s="3" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="B563" s="3" t="b">
         <v>1</v>
@@ -20267,18 +20267,18 @@
         <v>1</v>
       </c>
       <c r="E563" s="3" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="F563" s="5" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="G563" s="3" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="564" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A564" s="3" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="B564" s="3" t="b">
         <v>1</v>
@@ -20290,7 +20290,7 @@
         <v>33</v>
       </c>
       <c r="F564" s="5" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="G564" s="3" t="s">
         <v>1215</v>
@@ -20298,7 +20298,7 @@
     </row>
     <row r="565" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A565" s="3" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="B565" s="3" t="b">
         <v>1</v>
@@ -20318,7 +20318,7 @@
     </row>
     <row r="566" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A566" s="3" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="B566" s="3" t="b">
         <v>1</v>
@@ -20338,7 +20338,7 @@
     </row>
     <row r="567" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A567" s="3" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="B567" s="3" t="b">
         <v>1</v>
@@ -20358,7 +20358,7 @@
     </row>
     <row r="568" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A568" s="3" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="B568" s="3" t="b">
         <v>1</v>
@@ -20367,7 +20367,7 @@
         <v>1</v>
       </c>
       <c r="E568" s="3" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="F568" s="5" t="s">
         <v>2216</v>
@@ -21634,22 +21634,22 @@
     </row>
     <row r="631" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A631" s="3" t="s">
+        <v>2455</v>
+      </c>
+      <c r="B631" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C631" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E631" s="3" t="s">
         <v>2456</v>
       </c>
-      <c r="B631" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C631" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E631" s="3" t="s">
+      <c r="F631" s="5" t="s">
         <v>2457</v>
       </c>
-      <c r="F631" s="5" t="s">
-        <v>2458</v>
-      </c>
       <c r="G631" s="3" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.25">
@@ -21734,7 +21734,7 @@
     </row>
     <row r="636" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A636" s="3" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="B636" s="3" t="b">
         <v>1</v>
@@ -21743,18 +21743,18 @@
         <v>1</v>
       </c>
       <c r="E636" s="3" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F636" s="5" t="s">
         <v>2461</v>
       </c>
-      <c r="F636" s="5" t="s">
-        <v>2462</v>
-      </c>
       <c r="G636" s="3" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="637" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A637" s="3" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="B637" s="3" t="b">
         <v>1</v>
@@ -21763,58 +21763,58 @@
         <v>1</v>
       </c>
       <c r="E637" s="3" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="F637" s="5" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="G637" s="3" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="638" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A638" s="3" t="s">
+        <v>2487</v>
+      </c>
+      <c r="B638" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C638" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E638" s="3" t="s">
         <v>2488</v>
       </c>
-      <c r="B638" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C638" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E638" s="3" t="s">
+      <c r="F638" s="5" t="s">
         <v>2489</v>
       </c>
-      <c r="F638" s="5" t="s">
-        <v>2490</v>
-      </c>
       <c r="G638" s="3" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="639" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A639" s="3" t="s">
+        <v>2462</v>
+      </c>
+      <c r="B639" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C639" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E639" s="3" t="s">
         <v>2463</v>
-      </c>
-      <c r="B639" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C639" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E639" s="3" t="s">
-        <v>2464</v>
       </c>
       <c r="F639" s="5" t="s">
         <v>1663</v>
       </c>
       <c r="G639" s="3" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="640" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A640" s="3" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="B640" s="3" t="b">
         <v>1</v>
@@ -21854,7 +21854,7 @@
     </row>
     <row r="642" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A642" s="3" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="B642" s="3" t="b">
         <v>1</v>
@@ -22014,22 +22014,22 @@
     </row>
     <row r="650" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A650" s="3" t="s">
+        <v>2633</v>
+      </c>
+      <c r="B650" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C650" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E650" s="3" t="s">
         <v>2634</v>
       </c>
-      <c r="B650" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C650" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E650" s="3" t="s">
+      <c r="F650" s="5" t="s">
         <v>2635</v>
       </c>
-      <c r="F650" s="5" t="s">
-        <v>2636</v>
-      </c>
       <c r="G650" s="3" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="651" spans="1:7" x14ac:dyDescent="0.25">
@@ -22756,7 +22756,7 @@
     </row>
     <row r="687" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A687" s="3" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="B687" s="3" t="b">
         <v>1</v>
@@ -22769,7 +22769,7 @@
         <v>1750</v>
       </c>
       <c r="F687" s="5" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="G687" s="3" t="s">
         <v>1481</v>
@@ -23208,7 +23208,7 @@
     </row>
     <row r="709" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="B709" t="b">
         <v>1</v>
@@ -23217,7 +23217,7 @@
         <v>1</v>
       </c>
       <c r="E709" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="F709" s="5" t="s">
         <v>2216</v>
@@ -23228,7 +23228,7 @@
     </row>
     <row r="710" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A710" s="3" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="B710" t="b">
         <v>1</v>
@@ -23237,7 +23237,7 @@
         <v>1</v>
       </c>
       <c r="E710" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
       <c r="F710" s="5" t="s">
         <v>2215</v>
@@ -23248,7 +23248,7 @@
     </row>
     <row r="711" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A711" s="3" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="B711" s="3" t="b">
         <v>1</v>
@@ -23268,7 +23268,7 @@
     </row>
     <row r="712" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A712" s="3" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="B712" s="3" t="b">
         <v>1</v>
@@ -23448,7 +23448,7 @@
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="B721" s="3" t="b">
         <v>1</v>
@@ -23491,27 +23491,27 @@
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
+        <v>2341</v>
+      </c>
+      <c r="B723" t="b">
+        <v>0</v>
+      </c>
+      <c r="C723" t="b">
+        <v>1</v>
+      </c>
+      <c r="E723" t="s">
         <v>2342</v>
       </c>
-      <c r="B723" t="b">
-        <v>0</v>
-      </c>
-      <c r="C723" t="b">
-        <v>1</v>
-      </c>
-      <c r="E723" t="s">
-        <v>2343</v>
-      </c>
       <c r="F723" s="5" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="G723" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="B724" t="b">
         <v>0</v>
@@ -23520,58 +23520,58 @@
         <v>1</v>
       </c>
       <c r="E724" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="F724" s="5" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="G724" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="725" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A725" s="3" t="s">
+        <v>2349</v>
+      </c>
+      <c r="B725" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C725" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E725" s="3" t="s">
         <v>2350</v>
       </c>
-      <c r="B725" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C725" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E725" s="3" t="s">
+      <c r="F725" s="5" t="s">
         <v>2351</v>
       </c>
-      <c r="F725" s="5" t="s">
-        <v>2352</v>
-      </c>
       <c r="G725" s="3" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
+        <v>2344</v>
+      </c>
+      <c r="B726" t="b">
+        <v>0</v>
+      </c>
+      <c r="C726" t="b">
+        <v>1</v>
+      </c>
+      <c r="E726" t="s">
+        <v>2344</v>
+      </c>
+      <c r="F726" s="5" t="s">
         <v>2345</v>
       </c>
-      <c r="B726" t="b">
-        <v>0</v>
-      </c>
-      <c r="C726" t="b">
-        <v>1</v>
-      </c>
-      <c r="E726" t="s">
-        <v>2345</v>
-      </c>
-      <c r="F726" s="5" t="s">
-        <v>2346</v>
-      </c>
       <c r="G726" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="B727" t="b">
         <v>0</v>
@@ -23580,13 +23580,13 @@
         <v>1</v>
       </c>
       <c r="E727" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="F727" s="5" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="G727" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
@@ -23611,47 +23611,47 @@
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
+        <v>2373</v>
+      </c>
+      <c r="B729" t="b">
+        <v>0</v>
+      </c>
+      <c r="C729" t="b">
+        <v>1</v>
+      </c>
+      <c r="E729" t="s">
+        <v>2373</v>
+      </c>
+      <c r="F729" s="5" t="s">
         <v>2374</v>
       </c>
-      <c r="B729" t="b">
-        <v>0</v>
-      </c>
-      <c r="C729" t="b">
-        <v>1</v>
-      </c>
-      <c r="E729" t="s">
-        <v>2374</v>
-      </c>
-      <c r="F729" s="5" t="s">
-        <v>2375</v>
-      </c>
       <c r="G729" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
+        <v>2384</v>
+      </c>
+      <c r="B730" t="b">
+        <v>0</v>
+      </c>
+      <c r="C730" t="b">
+        <v>1</v>
+      </c>
+      <c r="E730" t="s">
         <v>2385</v>
       </c>
-      <c r="B730" t="b">
-        <v>0</v>
-      </c>
-      <c r="C730" t="b">
-        <v>1</v>
-      </c>
-      <c r="E730" t="s">
-        <v>2386</v>
-      </c>
       <c r="F730" s="5" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="G730" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="B731" t="b">
         <v>1</v>
@@ -23660,18 +23660,18 @@
         <v>1</v>
       </c>
       <c r="E731" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="F731" s="5" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="G731" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="732" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="B732" s="3" t="b">
         <v>1</v>
@@ -23680,18 +23680,18 @@
         <v>1</v>
       </c>
       <c r="E732" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="F732" s="5" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="G732" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="B733" s="3" t="b">
         <v>1</v>
@@ -23700,18 +23700,18 @@
         <v>1</v>
       </c>
       <c r="E733" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="F733" s="5" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="G733" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="B734" s="3" t="b">
         <v>1</v>
@@ -23720,18 +23720,18 @@
         <v>1</v>
       </c>
       <c r="E734" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="F734" s="5" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="G734" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="B735" s="3" t="b">
         <v>1</v>
@@ -23740,18 +23740,18 @@
         <v>1</v>
       </c>
       <c r="E735" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="F735" s="5" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="G735" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="736" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="B736" s="3" t="b">
         <v>1</v>
@@ -23760,18 +23760,18 @@
         <v>1</v>
       </c>
       <c r="E736" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="F736" s="5" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="G736" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="B737" s="3" t="b">
         <v>1</v>
@@ -23780,18 +23780,18 @@
         <v>1</v>
       </c>
       <c r="E737" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="F737" s="5" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="G737" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="738" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="B738" t="b">
         <v>1</v>
@@ -23800,18 +23800,18 @@
         <v>1</v>
       </c>
       <c r="E738" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="F738" s="5" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="G738" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="739" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="B739" t="b">
         <v>1</v>
@@ -23820,78 +23820,78 @@
         <v>1</v>
       </c>
       <c r="E739" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="F739" s="5" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="G739" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="740" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
+        <v>2478</v>
+      </c>
+      <c r="B740" t="b">
+        <v>1</v>
+      </c>
+      <c r="C740" t="b">
+        <v>1</v>
+      </c>
+      <c r="E740" t="s">
         <v>2479</v>
       </c>
-      <c r="B740" t="b">
-        <v>1</v>
-      </c>
-      <c r="C740" t="b">
-        <v>1</v>
-      </c>
-      <c r="E740" t="s">
+      <c r="F740" s="5" t="s">
         <v>2480</v>
       </c>
-      <c r="F740" s="5" t="s">
-        <v>2481</v>
-      </c>
       <c r="G740" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
     </row>
     <row r="741" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
+        <v>2481</v>
+      </c>
+      <c r="B741" t="b">
+        <v>1</v>
+      </c>
+      <c r="C741" t="b">
+        <v>1</v>
+      </c>
+      <c r="E741" t="s">
+        <v>2494</v>
+      </c>
+      <c r="F741" s="5" t="s">
         <v>2482</v>
       </c>
-      <c r="B741" t="b">
-        <v>1</v>
-      </c>
-      <c r="C741" t="b">
-        <v>1</v>
-      </c>
-      <c r="E741" t="s">
-        <v>2495</v>
-      </c>
-      <c r="F741" s="5" t="s">
-        <v>2483</v>
-      </c>
       <c r="G741" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="742" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
+        <v>2491</v>
+      </c>
+      <c r="B742" t="b">
+        <v>0</v>
+      </c>
+      <c r="C742" t="b">
+        <v>1</v>
+      </c>
+      <c r="E742" t="s">
         <v>2492</v>
       </c>
-      <c r="B742" t="b">
-        <v>0</v>
-      </c>
-      <c r="C742" t="b">
-        <v>1</v>
-      </c>
-      <c r="E742" t="s">
+      <c r="F742" s="5" t="s">
         <v>2493</v>
       </c>
-      <c r="F742" s="5" t="s">
-        <v>2494</v>
-      </c>
       <c r="G742" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="743" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="B743" t="b">
         <v>0</v>
@@ -23900,98 +23900,98 @@
         <v>1</v>
       </c>
       <c r="E743" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="F743" s="5" t="s">
         <v>1087</v>
       </c>
       <c r="G743" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="744" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
+        <v>2577</v>
+      </c>
+      <c r="B744" t="b">
+        <v>0</v>
+      </c>
+      <c r="C744" t="b">
+        <v>1</v>
+      </c>
+      <c r="E744" t="s">
+        <v>2577</v>
+      </c>
+      <c r="F744" s="5" t="s">
         <v>2578</v>
       </c>
-      <c r="B744" t="b">
-        <v>0</v>
-      </c>
-      <c r="C744" t="b">
-        <v>1</v>
-      </c>
-      <c r="E744" t="s">
-        <v>2578</v>
-      </c>
-      <c r="F744" s="5" t="s">
-        <v>2579</v>
-      </c>
       <c r="G744" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="745" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
+        <v>2579</v>
+      </c>
+      <c r="B745" t="b">
+        <v>0</v>
+      </c>
+      <c r="C745" t="b">
+        <v>1</v>
+      </c>
+      <c r="E745" t="s">
+        <v>2579</v>
+      </c>
+      <c r="F745" s="5" t="s">
         <v>2580</v>
       </c>
-      <c r="B745" t="b">
-        <v>0</v>
-      </c>
-      <c r="C745" t="b">
-        <v>1</v>
-      </c>
-      <c r="E745" t="s">
-        <v>2580</v>
-      </c>
-      <c r="F745" s="5" t="s">
-        <v>2581</v>
-      </c>
       <c r="G745" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="746" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A746" s="3" t="s">
+        <v>2602</v>
+      </c>
+      <c r="B746" t="b">
+        <v>1</v>
+      </c>
+      <c r="C746" t="b">
+        <v>1</v>
+      </c>
+      <c r="E746" t="s">
         <v>2603</v>
-      </c>
-      <c r="B746" t="b">
-        <v>1</v>
-      </c>
-      <c r="C746" t="b">
-        <v>1</v>
-      </c>
-      <c r="E746" t="s">
-        <v>2604</v>
       </c>
       <c r="F746" s="5" t="s">
         <v>1695</v>
       </c>
       <c r="G746" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="747" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A747" s="3" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B747" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C747" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E747" s="3" t="s">
         <v>2627</v>
       </c>
-      <c r="B747" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C747" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E747" s="3" t="s">
+      <c r="F747" s="5" t="s">
         <v>2628</v>
       </c>
-      <c r="F747" s="5" t="s">
+      <c r="G747" s="3" t="s">
         <v>2629</v>
-      </c>
-      <c r="G747" s="3" t="s">
-        <v>2630</v>
       </c>
     </row>
     <row r="748" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="B748" t="b">
         <v>1</v>
@@ -24000,18 +24000,18 @@
         <v>0</v>
       </c>
       <c r="E748" t="s">
+        <v>2613</v>
+      </c>
+      <c r="F748" s="5" t="s">
         <v>2614</v>
       </c>
-      <c r="F748" s="5" t="s">
-        <v>2615</v>
-      </c>
       <c r="G748" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="B749" t="b">
         <v>1</v>
@@ -24020,18 +24020,18 @@
         <v>0</v>
       </c>
       <c r="E749" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="F749" s="5" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="G749" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="750" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="B750" t="b">
         <v>0</v>
@@ -24040,38 +24040,38 @@
         <v>1</v>
       </c>
       <c r="E750" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="F750" s="5" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="G750" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="751" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
+        <v>2620</v>
+      </c>
+      <c r="B751" t="b">
+        <v>0</v>
+      </c>
+      <c r="C751" t="b">
+        <v>1</v>
+      </c>
+      <c r="E751" t="s">
+        <v>2620</v>
+      </c>
+      <c r="F751" s="5" t="s">
         <v>2621</v>
       </c>
-      <c r="B751" t="b">
-        <v>0</v>
-      </c>
-      <c r="C751" t="b">
-        <v>1</v>
-      </c>
-      <c r="E751" t="s">
-        <v>2621</v>
-      </c>
-      <c r="F751" s="5" t="s">
-        <v>2622</v>
-      </c>
       <c r="G751" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="752" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A752" s="3" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="B752" s="3" t="b">
         <v>0</v>
@@ -24081,38 +24081,38 @@
       </c>
       <c r="D752" s="3"/>
       <c r="E752" s="3" t="s">
+        <v>2622</v>
+      </c>
+      <c r="F752" s="5" t="s">
         <v>2623</v>
       </c>
-      <c r="F752" s="5" t="s">
+      <c r="G752" s="3" t="s">
         <v>2624</v>
-      </c>
-      <c r="G752" s="3" t="s">
-        <v>2625</v>
       </c>
     </row>
     <row r="753" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
+        <v>2630</v>
+      </c>
+      <c r="B753" t="b">
+        <v>0</v>
+      </c>
+      <c r="C753" t="b">
+        <v>1</v>
+      </c>
+      <c r="E753" t="s">
         <v>2631</v>
       </c>
-      <c r="B753" t="b">
-        <v>0</v>
-      </c>
-      <c r="C753" t="b">
-        <v>1</v>
-      </c>
-      <c r="E753" t="s">
+      <c r="F753" s="5" t="s">
         <v>2632</v>
       </c>
-      <c r="F753" s="5" t="s">
-        <v>2633</v>
-      </c>
       <c r="G753" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="754" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="B754" s="3" t="b">
         <v>0</v>
@@ -24121,58 +24121,58 @@
         <v>1</v>
       </c>
       <c r="E754" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="F754" s="5" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="G754" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="755" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B755" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C755" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E755" t="s">
+        <v>2641</v>
+      </c>
+      <c r="F755" s="5" t="s">
         <v>2638</v>
       </c>
-      <c r="B755" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C755" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E755" t="s">
-        <v>2642</v>
-      </c>
-      <c r="F755" s="5" t="s">
-        <v>2639</v>
-      </c>
       <c r="G755" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="756" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
+        <v>2646</v>
+      </c>
+      <c r="B756" t="b">
+        <v>1</v>
+      </c>
+      <c r="C756" t="b">
+        <v>0</v>
+      </c>
+      <c r="E756" t="s">
         <v>2647</v>
       </c>
-      <c r="B756" t="b">
-        <v>1</v>
-      </c>
-      <c r="C756" t="b">
-        <v>0</v>
-      </c>
-      <c r="E756" t="s">
+      <c r="F756" s="5" t="s">
         <v>2648</v>
       </c>
-      <c r="F756" s="5" t="s">
+      <c r="G756" t="s">
         <v>2649</v>
-      </c>
-      <c r="G756" t="s">
-        <v>2650</v>
       </c>
     </row>
     <row r="757" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A757" s="3" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
       <c r="B757" s="3" t="b">
         <v>1</v>
@@ -24181,18 +24181,18 @@
         <v>1</v>
       </c>
       <c r="E757" s="3" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
       <c r="F757" s="5" t="s">
-        <v>2678</v>
+        <v>2677</v>
       </c>
       <c r="G757" s="3" t="s">
-        <v>2680</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="758" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A758" s="3" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="B758" s="3" t="b">
         <v>1</v>
@@ -24201,18 +24201,18 @@
         <v>1</v>
       </c>
       <c r="E758" s="3" t="s">
-        <v>2677</v>
+        <v>2676</v>
       </c>
       <c r="F758" s="5" t="s">
-        <v>2679</v>
+        <v>2678</v>
       </c>
       <c r="G758" s="3" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="759" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="B759" s="3" t="b">
         <v>1</v>
@@ -24221,18 +24221,18 @@
         <v>1</v>
       </c>
       <c r="E759" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="F759" s="5" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="G759" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
     </row>
     <row r="760" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
       <c r="B760" s="3" t="b">
         <v>1</v>
@@ -24241,18 +24241,18 @@
         <v>1</v>
       </c>
       <c r="E760" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
       <c r="F760" s="5" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
       <c r="G760" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="761" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
       <c r="B761" s="3" t="b">
         <v>1</v>
@@ -24261,13 +24261,13 @@
         <v>1</v>
       </c>
       <c r="E761" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
       <c r="F761" s="5" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
       <c r="G761" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a few dynamic properties to Resource
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97226450-4947-4ACB-BB07-590C166D633F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1522BD98-EF07-43C5-935C-6E9BEEEC3BB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$766</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$774</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3084" uniqueCount="2728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3116" uniqueCount="2754">
   <si>
     <t>Key</t>
   </si>
@@ -8220,6 +8220,84 @@
   </si>
   <si>
     <t>代数值</t>
+  </si>
+  <si>
+    <t>Resource_ReorderLevel</t>
+  </si>
+  <si>
+    <t>Resource_EconomicOrderQuantity</t>
+  </si>
+  <si>
+    <t>Resource_Decimal1</t>
+  </si>
+  <si>
+    <t>Resource_Int1</t>
+  </si>
+  <si>
+    <t>Resource_Int2</t>
+  </si>
+  <si>
+    <t>Resource_Decimal2</t>
+  </si>
+  <si>
+    <t>Resource_Text1</t>
+  </si>
+  <si>
+    <t>Resource_Text2</t>
+  </si>
+  <si>
+    <t>Decimal Attribute 1</t>
+  </si>
+  <si>
+    <t>Decimal Attribute 2</t>
+  </si>
+  <si>
+    <t>Integer Attribute 1</t>
+  </si>
+  <si>
+    <t>Integer Attribute 2</t>
+  </si>
+  <si>
+    <t>Reorder Level</t>
+  </si>
+  <si>
+    <t>Economic Order Quantity</t>
+  </si>
+  <si>
+    <t>الصفة العددية 1</t>
+  </si>
+  <si>
+    <t>الصفة العددية 2</t>
+  </si>
+  <si>
+    <t>الصفة العشرية 1</t>
+  </si>
+  <si>
+    <t>الصفة العشرية 2</t>
+  </si>
+  <si>
+    <t>حد إعادة الطلب</t>
+  </si>
+  <si>
+    <t>الكمية الاقتصادية</t>
+  </si>
+  <si>
+    <t>订货点水平</t>
+  </si>
+  <si>
+    <t>经济订货量</t>
+  </si>
+  <si>
+    <t>十进制属性1</t>
+  </si>
+  <si>
+    <t>十进制属性2</t>
+  </si>
+  <si>
+    <t>整数属性1</t>
+  </si>
+  <si>
+    <t>整数属性2</t>
   </si>
 </sst>
 </file>
@@ -8616,12 +8694,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G769"/>
+  <dimension ref="A1:G777"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A676" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A691" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E693" sqref="E693"/>
+      <selection pane="bottomLeft" activeCell="G696" sqref="G696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23230,115 +23308,109 @@
         <v>2197</v>
       </c>
     </row>
-    <row r="705" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A705" t="s">
-        <v>2198</v>
-      </c>
-      <c r="B705" t="b">
-        <v>1</v>
-      </c>
-      <c r="C705" t="b">
-        <v>1</v>
-      </c>
-      <c r="E705" t="s">
-        <v>2199</v>
+    <row r="705" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A705" s="3" t="s">
+        <v>2728</v>
+      </c>
+      <c r="B705" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C705" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E705" s="3" t="s">
+        <v>2740</v>
       </c>
       <c r="F705" s="5" t="s">
-        <v>2200</v>
-      </c>
-      <c r="G705" t="s">
-        <v>2201</v>
-      </c>
-    </row>
-    <row r="706" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A706" t="s">
-        <v>2207</v>
-      </c>
-      <c r="B706" t="b">
-        <v>0</v>
-      </c>
-      <c r="C706" t="b">
-        <v>1</v>
-      </c>
-      <c r="D706" t="s">
-        <v>2212</v>
-      </c>
-      <c r="E706" t="s">
-        <v>2207</v>
+        <v>2746</v>
+      </c>
+      <c r="G705" s="3" t="s">
+        <v>2748</v>
+      </c>
+    </row>
+    <row r="706" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A706" s="3" t="s">
+        <v>2729</v>
+      </c>
+      <c r="B706" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C706" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E706" s="3" t="s">
+        <v>2741</v>
       </c>
       <c r="F706" s="5" t="s">
-        <v>2210</v>
-      </c>
-      <c r="G706" t="s">
-        <v>2213</v>
-      </c>
-    </row>
-    <row r="707" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A707" t="s">
-        <v>2208</v>
-      </c>
-      <c r="B707" t="b">
-        <v>0</v>
-      </c>
-      <c r="C707" t="b">
-        <v>1</v>
-      </c>
-      <c r="D707" t="s">
-        <v>2212</v>
-      </c>
-      <c r="E707" t="s">
-        <v>2209</v>
+        <v>2747</v>
+      </c>
+      <c r="G706" s="3" t="s">
+        <v>2749</v>
+      </c>
+    </row>
+    <row r="707" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A707" s="3" t="s">
+        <v>2730</v>
+      </c>
+      <c r="B707" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C707" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E707" s="3" t="s">
+        <v>2736</v>
       </c>
       <c r="F707" s="5" t="s">
-        <v>2211</v>
-      </c>
-      <c r="G707" t="s">
-        <v>2214</v>
-      </c>
-    </row>
-    <row r="708" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A708" t="s">
-        <v>2521</v>
-      </c>
-      <c r="B708" t="b">
+        <v>2744</v>
+      </c>
+      <c r="G707" s="3" t="s">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="708" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A708" s="3" t="s">
+        <v>2733</v>
+      </c>
+      <c r="B708" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C708" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E708" t="s">
-        <v>2525</v>
+      <c r="E708" s="3" t="s">
+        <v>2737</v>
       </c>
       <c r="F708" s="5" t="s">
-        <v>2216</v>
-      </c>
-      <c r="G708" t="s">
-        <v>2217</v>
-      </c>
-    </row>
-    <row r="709" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2745</v>
+      </c>
+      <c r="G708" s="3" t="s">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="709" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A709" s="3" t="s">
-        <v>2522</v>
-      </c>
-      <c r="B709" t="b">
+        <v>2731</v>
+      </c>
+      <c r="B709" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C709" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E709" t="s">
-        <v>2526</v>
+      <c r="E709" s="3" t="s">
+        <v>2738</v>
       </c>
       <c r="F709" s="5" t="s">
-        <v>2215</v>
-      </c>
-      <c r="G709" t="s">
-        <v>2217</v>
+        <v>2742</v>
+      </c>
+      <c r="G709" s="3" t="s">
+        <v>2752</v>
       </c>
     </row>
     <row r="710" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A710" s="3" t="s">
-        <v>2523</v>
+        <v>2732</v>
       </c>
       <c r="B710" s="3" t="b">
         <v>1</v>
@@ -23347,18 +23419,18 @@
         <v>1</v>
       </c>
       <c r="E710" s="3" t="s">
-        <v>320</v>
+        <v>2739</v>
       </c>
       <c r="F710" s="5" t="s">
-        <v>319</v>
+        <v>2743</v>
       </c>
       <c r="G710" s="3" t="s">
-        <v>1315</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="711" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A711" s="3" t="s">
-        <v>2524</v>
+        <v>2734</v>
       </c>
       <c r="B711" s="3" t="b">
         <v>1</v>
@@ -23367,158 +23439,164 @@
         <v>1</v>
       </c>
       <c r="E711" s="3" t="s">
-        <v>323</v>
+        <v>1679</v>
       </c>
       <c r="F711" s="5" t="s">
-        <v>322</v>
+        <v>1681</v>
       </c>
       <c r="G711" s="3" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="712" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A712" t="s">
-        <v>2274</v>
-      </c>
-      <c r="B712" t="b">
-        <v>1</v>
-      </c>
-      <c r="C712" t="b">
-        <v>1</v>
-      </c>
-      <c r="E712" t="s">
-        <v>2263</v>
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="712" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A712" s="3" t="s">
+        <v>2735</v>
+      </c>
+      <c r="B712" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C712" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E712" s="3" t="s">
+        <v>1680</v>
       </c>
       <c r="F712" s="5" t="s">
-        <v>2264</v>
-      </c>
-      <c r="G712" t="s">
-        <v>2286</v>
+        <v>1682</v>
+      </c>
+      <c r="G712" s="3" t="s">
+        <v>1718</v>
       </c>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>2276</v>
+        <v>2198</v>
       </c>
       <c r="B713" t="b">
         <v>1</v>
       </c>
       <c r="C713" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E713" t="s">
-        <v>2275</v>
+        <v>2199</v>
       </c>
       <c r="F713" s="5" t="s">
-        <v>2277</v>
+        <v>2200</v>
       </c>
       <c r="G713" t="s">
-        <v>2287</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="714" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>2280</v>
+        <v>2207</v>
       </c>
       <c r="B714" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C714" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D714" t="s">
+        <v>2212</v>
       </c>
       <c r="E714" t="s">
-        <v>2278</v>
+        <v>2207</v>
       </c>
       <c r="F714" s="5" t="s">
-        <v>2279</v>
+        <v>2210</v>
       </c>
       <c r="G714" t="s">
-        <v>2288</v>
-      </c>
-    </row>
-    <row r="715" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A715" s="3" t="s">
-        <v>2283</v>
-      </c>
-      <c r="B715" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C715" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E715" s="3" t="s">
-        <v>2284</v>
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="715" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A715" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B715" t="b">
+        <v>0</v>
+      </c>
+      <c r="C715" t="b">
+        <v>1</v>
+      </c>
+      <c r="D715" t="s">
+        <v>2212</v>
+      </c>
+      <c r="E715" t="s">
+        <v>2209</v>
       </c>
       <c r="F715" s="5" t="s">
-        <v>2285</v>
-      </c>
-      <c r="G715" s="3" t="s">
-        <v>2289</v>
+        <v>2211</v>
+      </c>
+      <c r="G715" t="s">
+        <v>2214</v>
       </c>
     </row>
     <row r="716" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>2290</v>
+        <v>2521</v>
       </c>
       <c r="B716" t="b">
-        <v>0</v>
-      </c>
-      <c r="C716" t="b">
+        <v>1</v>
+      </c>
+      <c r="C716" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E716" t="s">
-        <v>2293</v>
+        <v>2525</v>
       </c>
       <c r="F716" s="5" t="s">
-        <v>2294</v>
+        <v>2216</v>
       </c>
       <c r="G716" t="s">
-        <v>2303</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A717" t="s">
-        <v>2291</v>
+      <c r="A717" s="3" t="s">
+        <v>2522</v>
       </c>
       <c r="B717" t="b">
-        <v>0</v>
-      </c>
-      <c r="C717" t="b">
+        <v>1</v>
+      </c>
+      <c r="C717" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E717" t="s">
-        <v>2292</v>
+        <v>2526</v>
       </c>
       <c r="F717" s="5" t="s">
-        <v>2295</v>
+        <v>2215</v>
       </c>
       <c r="G717" t="s">
-        <v>2304</v>
-      </c>
-    </row>
-    <row r="718" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A718" t="s">
-        <v>2297</v>
-      </c>
-      <c r="B718" t="b">
-        <v>1</v>
-      </c>
-      <c r="C718" t="b">
-        <v>1</v>
-      </c>
-      <c r="E718" t="s">
-        <v>2299</v>
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="718" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A718" s="3" t="s">
+        <v>2523</v>
+      </c>
+      <c r="B718" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C718" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E718" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="F718" s="5" t="s">
-        <v>2302</v>
-      </c>
-      <c r="G718" t="s">
-        <v>2305</v>
-      </c>
-    </row>
-    <row r="719" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A719" t="s">
-        <v>2298</v>
+        <v>319</v>
+      </c>
+      <c r="G718" s="3" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="719" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A719" s="3" t="s">
+        <v>2524</v>
       </c>
       <c r="B719" s="3" t="b">
         <v>1</v>
@@ -23526,122 +23604,119 @@
       <c r="C719" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E719" t="s">
-        <v>493</v>
+      <c r="E719" s="3" t="s">
+        <v>323</v>
       </c>
       <c r="F719" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="G719" t="s">
-        <v>1376</v>
+        <v>322</v>
+      </c>
+      <c r="G719" s="3" t="s">
+        <v>1316</v>
       </c>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>2360</v>
-      </c>
-      <c r="B720" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C720" s="3" t="b">
+        <v>2274</v>
+      </c>
+      <c r="B720" t="b">
+        <v>1</v>
+      </c>
+      <c r="C720" t="b">
         <v>1</v>
       </c>
       <c r="E720" t="s">
-        <v>2300</v>
+        <v>2263</v>
       </c>
       <c r="F720" s="5" t="s">
-        <v>2301</v>
+        <v>2264</v>
       </c>
       <c r="G720" t="s">
-        <v>2306</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>2309</v>
+        <v>2276</v>
       </c>
       <c r="B721" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C721" t="b">
-        <v>1</v>
-      </c>
-      <c r="D721" t="s">
-        <v>2310</v>
+        <v>0</v>
       </c>
       <c r="E721" t="s">
-        <v>2312</v>
+        <v>2275</v>
       </c>
       <c r="F721" s="5" t="s">
-        <v>2311</v>
-      </c>
-      <c r="G721" s="3" t="s">
-        <v>2317</v>
+        <v>2277</v>
+      </c>
+      <c r="G721" t="s">
+        <v>2287</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>2341</v>
+        <v>2280</v>
       </c>
       <c r="B722" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C722" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E722" t="s">
-        <v>2342</v>
+        <v>2278</v>
       </c>
       <c r="F722" s="5" t="s">
-        <v>2358</v>
+        <v>2279</v>
       </c>
       <c r="G722" t="s">
-        <v>2353</v>
-      </c>
-    </row>
-    <row r="723" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A723" t="s">
-        <v>2343</v>
-      </c>
-      <c r="B723" t="b">
-        <v>0</v>
-      </c>
-      <c r="C723" t="b">
-        <v>1</v>
-      </c>
-      <c r="E723" t="s">
-        <v>2359</v>
+        <v>2288</v>
+      </c>
+    </row>
+    <row r="723" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A723" s="3" t="s">
+        <v>2283</v>
+      </c>
+      <c r="B723" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C723" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E723" s="3" t="s">
+        <v>2284</v>
       </c>
       <c r="F723" s="5" t="s">
-        <v>2346</v>
-      </c>
-      <c r="G723" t="s">
-        <v>2354</v>
-      </c>
-    </row>
-    <row r="724" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A724" s="3" t="s">
-        <v>2349</v>
-      </c>
-      <c r="B724" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C724" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E724" s="3" t="s">
-        <v>2350</v>
+        <v>2285</v>
+      </c>
+      <c r="G723" s="3" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="724" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A724" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B724" t="b">
+        <v>0</v>
+      </c>
+      <c r="C724" t="b">
+        <v>1</v>
+      </c>
+      <c r="E724" t="s">
+        <v>2293</v>
       </c>
       <c r="F724" s="5" t="s">
-        <v>2351</v>
-      </c>
-      <c r="G724" s="3" t="s">
-        <v>2355</v>
+        <v>2294</v>
+      </c>
+      <c r="G724" t="s">
+        <v>2303</v>
       </c>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>2344</v>
+        <v>2291</v>
       </c>
       <c r="B725" t="b">
         <v>0</v>
@@ -23650,78 +23725,78 @@
         <v>1</v>
       </c>
       <c r="E725" t="s">
-        <v>2344</v>
+        <v>2292</v>
       </c>
       <c r="F725" s="5" t="s">
-        <v>2345</v>
+        <v>2295</v>
       </c>
       <c r="G725" t="s">
-        <v>2356</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>2348</v>
+        <v>2297</v>
       </c>
       <c r="B726" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C726" t="b">
         <v>1</v>
       </c>
       <c r="E726" t="s">
-        <v>2347</v>
+        <v>2299</v>
       </c>
       <c r="F726" s="5" t="s">
-        <v>2352</v>
+        <v>2302</v>
       </c>
       <c r="G726" t="s">
-        <v>2357</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>496</v>
-      </c>
-      <c r="B727" t="b">
-        <v>0</v>
-      </c>
-      <c r="C727" t="b">
+        <v>2298</v>
+      </c>
+      <c r="B727" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C727" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E727" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F727" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G727" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>2373</v>
-      </c>
-      <c r="B728" t="b">
-        <v>0</v>
-      </c>
-      <c r="C728" t="b">
+        <v>2360</v>
+      </c>
+      <c r="B728" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C728" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E728" t="s">
-        <v>2373</v>
+        <v>2300</v>
       </c>
       <c r="F728" s="5" t="s">
-        <v>2374</v>
+        <v>2301</v>
       </c>
       <c r="G728" t="s">
-        <v>2386</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>2384</v>
+        <v>2309</v>
       </c>
       <c r="B729" t="b">
         <v>0</v>
@@ -23729,319 +23804,322 @@
       <c r="C729" t="b">
         <v>1</v>
       </c>
+      <c r="D729" t="s">
+        <v>2310</v>
+      </c>
       <c r="E729" t="s">
-        <v>2385</v>
+        <v>2312</v>
       </c>
       <c r="F729" s="5" t="s">
-        <v>2388</v>
-      </c>
-      <c r="G729" t="s">
-        <v>2387</v>
+        <v>2311</v>
+      </c>
+      <c r="G729" s="3" t="s">
+        <v>2317</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>2448</v>
+        <v>2341</v>
       </c>
       <c r="B730" t="b">
-        <v>1</v>
-      </c>
-      <c r="C730" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C730" t="b">
         <v>1</v>
       </c>
       <c r="E730" t="s">
-        <v>2389</v>
+        <v>2342</v>
       </c>
       <c r="F730" s="5" t="s">
-        <v>2396</v>
+        <v>2358</v>
       </c>
       <c r="G730" t="s">
-        <v>2403</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>2449</v>
-      </c>
-      <c r="B731" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C731" s="3" t="b">
+        <v>2343</v>
+      </c>
+      <c r="B731" t="b">
+        <v>0</v>
+      </c>
+      <c r="C731" t="b">
         <v>1</v>
       </c>
       <c r="E731" t="s">
-        <v>2390</v>
+        <v>2359</v>
       </c>
       <c r="F731" s="5" t="s">
-        <v>2397</v>
+        <v>2346</v>
       </c>
       <c r="G731" t="s">
-        <v>2409</v>
-      </c>
-    </row>
-    <row r="732" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A732" t="s">
-        <v>2450</v>
+        <v>2354</v>
+      </c>
+    </row>
+    <row r="732" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A732" s="3" t="s">
+        <v>2349</v>
       </c>
       <c r="B732" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C732" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E732" t="s">
-        <v>2391</v>
+      <c r="E732" s="3" t="s">
+        <v>2350</v>
       </c>
       <c r="F732" s="5" t="s">
-        <v>2398</v>
-      </c>
-      <c r="G732" t="s">
-        <v>2404</v>
+        <v>2351</v>
+      </c>
+      <c r="G732" s="3" t="s">
+        <v>2355</v>
       </c>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>2451</v>
-      </c>
-      <c r="B733" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C733" s="3" t="b">
+        <v>2344</v>
+      </c>
+      <c r="B733" t="b">
+        <v>0</v>
+      </c>
+      <c r="C733" t="b">
         <v>1</v>
       </c>
       <c r="E733" t="s">
-        <v>2393</v>
+        <v>2344</v>
       </c>
       <c r="F733" s="5" t="s">
-        <v>2400</v>
+        <v>2345</v>
       </c>
       <c r="G733" t="s">
-        <v>2405</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>2452</v>
-      </c>
-      <c r="B734" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C734" s="3" t="b">
+        <v>2348</v>
+      </c>
+      <c r="B734" t="b">
+        <v>0</v>
+      </c>
+      <c r="C734" t="b">
         <v>1</v>
       </c>
       <c r="E734" t="s">
-        <v>2394</v>
+        <v>2347</v>
       </c>
       <c r="F734" s="5" t="s">
-        <v>2401</v>
+        <v>2352</v>
       </c>
       <c r="G734" t="s">
-        <v>2406</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>2453</v>
-      </c>
-      <c r="B735" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C735" s="3" t="b">
+        <v>496</v>
+      </c>
+      <c r="B735" t="b">
+        <v>0</v>
+      </c>
+      <c r="C735" t="b">
         <v>1</v>
       </c>
       <c r="E735" t="s">
-        <v>2392</v>
+        <v>496</v>
       </c>
       <c r="F735" s="5" t="s">
-        <v>2399</v>
+        <v>495</v>
       </c>
       <c r="G735" t="s">
-        <v>2407</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="736" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>2454</v>
-      </c>
-      <c r="B736" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C736" s="3" t="b">
+        <v>2373</v>
+      </c>
+      <c r="B736" t="b">
+        <v>0</v>
+      </c>
+      <c r="C736" t="b">
         <v>1</v>
       </c>
       <c r="E736" t="s">
-        <v>2395</v>
+        <v>2373</v>
       </c>
       <c r="F736" s="5" t="s">
-        <v>2402</v>
+        <v>2374</v>
       </c>
       <c r="G736" t="s">
-        <v>2408</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>2470</v>
+        <v>2384</v>
       </c>
       <c r="B737" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C737" t="b">
         <v>1</v>
       </c>
       <c r="E737" t="s">
-        <v>2472</v>
+        <v>2385</v>
       </c>
       <c r="F737" s="5" t="s">
-        <v>2474</v>
+        <v>2388</v>
       </c>
       <c r="G737" t="s">
-        <v>2476</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="738" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>2471</v>
+        <v>2448</v>
       </c>
       <c r="B738" t="b">
         <v>1</v>
       </c>
-      <c r="C738" t="b">
+      <c r="C738" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E738" t="s">
-        <v>2473</v>
+        <v>2389</v>
       </c>
       <c r="F738" s="5" t="s">
-        <v>2475</v>
+        <v>2396</v>
       </c>
       <c r="G738" t="s">
-        <v>2477</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="739" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>2478</v>
-      </c>
-      <c r="B739" t="b">
-        <v>1</v>
-      </c>
-      <c r="C739" t="b">
+        <v>2449</v>
+      </c>
+      <c r="B739" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C739" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E739" t="s">
-        <v>2479</v>
+        <v>2390</v>
       </c>
       <c r="F739" s="5" t="s">
-        <v>2480</v>
+        <v>2397</v>
       </c>
       <c r="G739" t="s">
-        <v>2483</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="740" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>2481</v>
-      </c>
-      <c r="B740" t="b">
-        <v>1</v>
-      </c>
-      <c r="C740" t="b">
+        <v>2450</v>
+      </c>
+      <c r="B740" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C740" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E740" t="s">
-        <v>2494</v>
+        <v>2391</v>
       </c>
       <c r="F740" s="5" t="s">
-        <v>2482</v>
+        <v>2398</v>
       </c>
       <c r="G740" t="s">
-        <v>2484</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="741" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>2491</v>
-      </c>
-      <c r="B741" t="b">
-        <v>0</v>
-      </c>
-      <c r="C741" t="b">
+        <v>2451</v>
+      </c>
+      <c r="B741" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C741" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E741" t="s">
-        <v>2492</v>
+        <v>2393</v>
       </c>
       <c r="F741" s="5" t="s">
-        <v>2493</v>
+        <v>2400</v>
       </c>
       <c r="G741" t="s">
-        <v>2469</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="742" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>2517</v>
-      </c>
-      <c r="B742" t="b">
-        <v>0</v>
-      </c>
-      <c r="C742" t="b">
+        <v>2452</v>
+      </c>
+      <c r="B742" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C742" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E742" t="s">
-        <v>2517</v>
+        <v>2394</v>
       </c>
       <c r="F742" s="5" t="s">
-        <v>1087</v>
+        <v>2401</v>
       </c>
       <c r="G742" t="s">
-        <v>2518</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="743" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>2577</v>
-      </c>
-      <c r="B743" t="b">
-        <v>0</v>
-      </c>
-      <c r="C743" t="b">
+        <v>2453</v>
+      </c>
+      <c r="B743" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C743" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E743" t="s">
-        <v>2577</v>
+        <v>2392</v>
       </c>
       <c r="F743" s="5" t="s">
-        <v>2578</v>
+        <v>2399</v>
       </c>
       <c r="G743" t="s">
-        <v>2581</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="744" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>2579</v>
-      </c>
-      <c r="B744" t="b">
-        <v>0</v>
-      </c>
-      <c r="C744" t="b">
+        <v>2454</v>
+      </c>
+      <c r="B744" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C744" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E744" t="s">
-        <v>2579</v>
+        <v>2395</v>
       </c>
       <c r="F744" s="5" t="s">
-        <v>2580</v>
+        <v>2402</v>
       </c>
       <c r="G744" t="s">
-        <v>2582</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="745" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A745" s="3" t="s">
-        <v>2602</v>
+      <c r="A745" t="s">
+        <v>2470</v>
       </c>
       <c r="B745" t="b">
         <v>1</v>
@@ -24050,78 +24128,78 @@
         <v>1</v>
       </c>
       <c r="E745" t="s">
-        <v>2603</v>
+        <v>2472</v>
       </c>
       <c r="F745" s="5" t="s">
-        <v>1695</v>
+        <v>2474</v>
       </c>
       <c r="G745" t="s">
-        <v>2604</v>
-      </c>
-    </row>
-    <row r="746" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A746" s="3" t="s">
-        <v>2626</v>
-      </c>
-      <c r="B746" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C746" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E746" s="3" t="s">
-        <v>2627</v>
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="746" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A746" t="s">
+        <v>2471</v>
+      </c>
+      <c r="B746" t="b">
+        <v>1</v>
+      </c>
+      <c r="C746" t="b">
+        <v>1</v>
+      </c>
+      <c r="E746" t="s">
+        <v>2473</v>
       </c>
       <c r="F746" s="5" t="s">
-        <v>2628</v>
-      </c>
-      <c r="G746" s="3" t="s">
-        <v>2629</v>
+        <v>2475</v>
+      </c>
+      <c r="G746" t="s">
+        <v>2477</v>
       </c>
     </row>
     <row r="747" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>2605</v>
+        <v>2478</v>
       </c>
       <c r="B747" t="b">
         <v>1</v>
       </c>
       <c r="C747" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E747" t="s">
-        <v>2613</v>
+        <v>2479</v>
       </c>
       <c r="F747" s="5" t="s">
-        <v>2614</v>
+        <v>2480</v>
       </c>
       <c r="G747" t="s">
-        <v>2616</v>
+        <v>2483</v>
       </c>
     </row>
     <row r="748" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>2607</v>
+        <v>2481</v>
       </c>
       <c r="B748" t="b">
         <v>1</v>
       </c>
       <c r="C748" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E748" t="s">
-        <v>2606</v>
+        <v>2494</v>
       </c>
       <c r="F748" s="5" t="s">
-        <v>2615</v>
+        <v>2482</v>
       </c>
       <c r="G748" t="s">
-        <v>2617</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>2619</v>
+        <v>2491</v>
       </c>
       <c r="B749" t="b">
         <v>0</v>
@@ -24130,18 +24208,18 @@
         <v>1</v>
       </c>
       <c r="E749" t="s">
-        <v>2619</v>
+        <v>2492</v>
       </c>
       <c r="F749" s="5" t="s">
-        <v>2612</v>
+        <v>2493</v>
       </c>
       <c r="G749" t="s">
-        <v>2618</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="750" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>2620</v>
+        <v>2517</v>
       </c>
       <c r="B750" t="b">
         <v>0</v>
@@ -24150,39 +24228,38 @@
         <v>1</v>
       </c>
       <c r="E750" t="s">
-        <v>2620</v>
+        <v>2517</v>
       </c>
       <c r="F750" s="5" t="s">
-        <v>2621</v>
+        <v>1087</v>
       </c>
       <c r="G750" t="s">
-        <v>2642</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="751" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A751" s="3" t="s">
-        <v>2625</v>
-      </c>
-      <c r="B751" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C751" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D751" s="3"/>
-      <c r="E751" s="3" t="s">
-        <v>2622</v>
+      <c r="A751" t="s">
+        <v>2577</v>
+      </c>
+      <c r="B751" t="b">
+        <v>0</v>
+      </c>
+      <c r="C751" t="b">
+        <v>1</v>
+      </c>
+      <c r="E751" t="s">
+        <v>2577</v>
       </c>
       <c r="F751" s="5" t="s">
-        <v>2623</v>
-      </c>
-      <c r="G751" s="3" t="s">
-        <v>2624</v>
+        <v>2578</v>
+      </c>
+      <c r="G751" t="s">
+        <v>2581</v>
       </c>
     </row>
     <row r="752" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>2630</v>
+        <v>2579</v>
       </c>
       <c r="B752" t="b">
         <v>0</v>
@@ -24191,58 +24268,58 @@
         <v>1</v>
       </c>
       <c r="E752" t="s">
-        <v>2631</v>
+        <v>2579</v>
       </c>
       <c r="F752" s="5" t="s">
-        <v>2632</v>
+        <v>2580</v>
       </c>
       <c r="G752" t="s">
-        <v>2643</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="753" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A753" t="s">
-        <v>2636</v>
-      </c>
-      <c r="B753" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C753" s="3" t="b">
+      <c r="A753" s="3" t="s">
+        <v>2602</v>
+      </c>
+      <c r="B753" t="b">
+        <v>1</v>
+      </c>
+      <c r="C753" t="b">
         <v>1</v>
       </c>
       <c r="E753" t="s">
-        <v>2640</v>
+        <v>2603</v>
       </c>
       <c r="F753" s="5" t="s">
-        <v>2639</v>
+        <v>1695</v>
       </c>
       <c r="G753" t="s">
-        <v>2644</v>
-      </c>
-    </row>
-    <row r="754" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A754" t="s">
-        <v>2637</v>
+        <v>2604</v>
+      </c>
+    </row>
+    <row r="754" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A754" s="3" t="s">
+        <v>2626</v>
       </c>
       <c r="B754" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C754" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E754" t="s">
-        <v>2641</v>
+      <c r="E754" s="3" t="s">
+        <v>2627</v>
       </c>
       <c r="F754" s="5" t="s">
-        <v>2638</v>
-      </c>
-      <c r="G754" t="s">
-        <v>2645</v>
+        <v>2628</v>
+      </c>
+      <c r="G754" s="3" t="s">
+        <v>2629</v>
       </c>
     </row>
     <row r="755" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>2646</v>
+        <v>2605</v>
       </c>
       <c r="B755" t="b">
         <v>1</v>
@@ -24251,178 +24328,179 @@
         <v>0</v>
       </c>
       <c r="E755" t="s">
-        <v>2647</v>
+        <v>2613</v>
       </c>
       <c r="F755" s="5" t="s">
-        <v>2648</v>
+        <v>2614</v>
       </c>
       <c r="G755" t="s">
-        <v>2649</v>
-      </c>
-    </row>
-    <row r="756" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A756" s="3" t="s">
-        <v>2673</v>
-      </c>
-      <c r="B756" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C756" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E756" s="3" t="s">
-        <v>2675</v>
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="756" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A756" t="s">
+        <v>2607</v>
+      </c>
+      <c r="B756" t="b">
+        <v>1</v>
+      </c>
+      <c r="C756" t="b">
+        <v>0</v>
+      </c>
+      <c r="E756" t="s">
+        <v>2606</v>
       </c>
       <c r="F756" s="5" t="s">
-        <v>2677</v>
-      </c>
-      <c r="G756" s="3" t="s">
-        <v>2679</v>
-      </c>
-    </row>
-    <row r="757" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A757" s="3" t="s">
-        <v>2674</v>
-      </c>
-      <c r="B757" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C757" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E757" s="3" t="s">
-        <v>2676</v>
+        <v>2615</v>
+      </c>
+      <c r="G756" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="757" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A757" t="s">
+        <v>2619</v>
+      </c>
+      <c r="B757" t="b">
+        <v>0</v>
+      </c>
+      <c r="C757" t="b">
+        <v>1</v>
+      </c>
+      <c r="E757" t="s">
+        <v>2619</v>
       </c>
       <c r="F757" s="5" t="s">
-        <v>2678</v>
-      </c>
-      <c r="G757" s="3" t="s">
-        <v>2680</v>
-      </c>
-    </row>
-    <row r="758" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2612</v>
+      </c>
+      <c r="G757" t="s">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="758" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>2692</v>
-      </c>
-      <c r="B758" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C758" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E758" s="3" t="s">
-        <v>2707</v>
+        <v>2620</v>
+      </c>
+      <c r="B758" t="b">
+        <v>0</v>
+      </c>
+      <c r="C758" t="b">
+        <v>1</v>
+      </c>
+      <c r="E758" t="s">
+        <v>2620</v>
       </c>
       <c r="F758" s="5" t="s">
-        <v>2708</v>
-      </c>
-      <c r="G758" s="3" t="s">
-        <v>2716</v>
-      </c>
-    </row>
-    <row r="759" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A759" t="s">
-        <v>2693</v>
+        <v>2621</v>
+      </c>
+      <c r="G758" t="s">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="759" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A759" s="3" t="s">
+        <v>2625</v>
       </c>
       <c r="B759" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C759" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="D759" s="3"/>
       <c r="E759" s="3" t="s">
-        <v>2706</v>
+        <v>2622</v>
       </c>
       <c r="F759" s="5" t="s">
-        <v>2709</v>
+        <v>2623</v>
       </c>
       <c r="G759" s="3" t="s">
-        <v>2717</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="760" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>2653</v>
-      </c>
-      <c r="B760" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C760" s="3" t="b">
+        <v>2630</v>
+      </c>
+      <c r="B760" t="b">
+        <v>0</v>
+      </c>
+      <c r="C760" t="b">
         <v>1</v>
       </c>
       <c r="E760" t="s">
-        <v>2659</v>
+        <v>2631</v>
       </c>
       <c r="F760" s="5" t="s">
-        <v>2662</v>
+        <v>2632</v>
       </c>
       <c r="G760" t="s">
-        <v>2670</v>
-      </c>
-    </row>
-    <row r="761" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A761" s="3" t="s">
-        <v>2694</v>
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="761" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A761" t="s">
+        <v>2636</v>
       </c>
       <c r="B761" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C761" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E761" s="3" t="s">
-        <v>2705</v>
+      <c r="E761" t="s">
+        <v>2640</v>
       </c>
       <c r="F761" s="5" t="s">
-        <v>2710</v>
-      </c>
-      <c r="G761" s="3" t="s">
-        <v>2718</v>
-      </c>
-    </row>
-    <row r="762" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A762" s="3" t="s">
-        <v>2695</v>
+        <v>2639</v>
+      </c>
+      <c r="G761" t="s">
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="762" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A762" t="s">
+        <v>2637</v>
       </c>
       <c r="B762" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C762" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E762" s="3" t="s">
-        <v>2704</v>
+      <c r="E762" t="s">
+        <v>2641</v>
       </c>
       <c r="F762" s="5" t="s">
-        <v>2711</v>
-      </c>
-      <c r="G762" s="3" t="s">
-        <v>2719</v>
+        <v>2638</v>
+      </c>
+      <c r="G762" t="s">
+        <v>2645</v>
       </c>
     </row>
     <row r="763" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>2655</v>
-      </c>
-      <c r="B763" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C763" s="3" t="b">
-        <v>1</v>
+        <v>2646</v>
+      </c>
+      <c r="B763" t="b">
+        <v>1</v>
+      </c>
+      <c r="C763" t="b">
+        <v>0</v>
       </c>
       <c r="E763" t="s">
-        <v>2660</v>
+        <v>2647</v>
       </c>
       <c r="F763" s="5" t="s">
-        <v>2663</v>
+        <v>2648</v>
       </c>
       <c r="G763" t="s">
-        <v>2671</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="764" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A764" s="3" t="s">
-        <v>2696</v>
+        <v>2673</v>
       </c>
       <c r="B764" s="3" t="b">
         <v>1</v>
@@ -24431,18 +24509,18 @@
         <v>1</v>
       </c>
       <c r="E764" s="3" t="s">
-        <v>2703</v>
+        <v>2675</v>
       </c>
       <c r="F764" s="5" t="s">
-        <v>2712</v>
+        <v>2677</v>
       </c>
       <c r="G764" s="3" t="s">
-        <v>2720</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="765" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A765" s="3" t="s">
-        <v>2697</v>
+        <v>2674</v>
       </c>
       <c r="B765" s="3" t="b">
         <v>1</v>
@@ -24451,18 +24529,18 @@
         <v>1</v>
       </c>
       <c r="E765" s="3" t="s">
-        <v>2702</v>
+        <v>2676</v>
       </c>
       <c r="F765" s="5" t="s">
-        <v>2713</v>
+        <v>2678</v>
       </c>
       <c r="G765" s="3" t="s">
-        <v>2721</v>
-      </c>
-    </row>
-    <row r="766" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="766" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>2654</v>
+        <v>2692</v>
       </c>
       <c r="B766" s="3" t="b">
         <v>1</v>
@@ -24470,19 +24548,19 @@
       <c r="C766" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E766" t="s">
-        <v>2661</v>
+      <c r="E766" s="3" t="s">
+        <v>2707</v>
       </c>
       <c r="F766" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="G766" t="s">
-        <v>2672</v>
+        <v>2708</v>
+      </c>
+      <c r="G766" s="3" t="s">
+        <v>2716</v>
       </c>
     </row>
     <row r="767" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A767" s="3" t="s">
-        <v>2698</v>
+      <c r="A767" t="s">
+        <v>2693</v>
       </c>
       <c r="B767" s="3" t="b">
         <v>1</v>
@@ -24491,57 +24569,217 @@
         <v>1</v>
       </c>
       <c r="E767" s="3" t="s">
-        <v>2701</v>
+        <v>2706</v>
       </c>
       <c r="F767" s="5" t="s">
-        <v>2714</v>
+        <v>2709</v>
       </c>
       <c r="G767" s="3" t="s">
-        <v>2722</v>
+        <v>2717</v>
       </c>
     </row>
     <row r="768" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
+        <v>2653</v>
+      </c>
+      <c r="B768" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C768" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E768" t="s">
+        <v>2659</v>
+      </c>
+      <c r="F768" s="5" t="s">
+        <v>2662</v>
+      </c>
+      <c r="G768" t="s">
+        <v>2670</v>
+      </c>
+    </row>
+    <row r="769" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A769" s="3" t="s">
+        <v>2694</v>
+      </c>
+      <c r="B769" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C769" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E769" s="3" t="s">
+        <v>2705</v>
+      </c>
+      <c r="F769" s="5" t="s">
+        <v>2710</v>
+      </c>
+      <c r="G769" s="3" t="s">
+        <v>2718</v>
+      </c>
+    </row>
+    <row r="770" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A770" s="3" t="s">
+        <v>2695</v>
+      </c>
+      <c r="B770" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C770" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E770" s="3" t="s">
+        <v>2704</v>
+      </c>
+      <c r="F770" s="5" t="s">
+        <v>2711</v>
+      </c>
+      <c r="G770" s="3" t="s">
+        <v>2719</v>
+      </c>
+    </row>
+    <row r="771" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A771" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B771" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C771" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E771" t="s">
+        <v>2660</v>
+      </c>
+      <c r="F771" s="5" t="s">
+        <v>2663</v>
+      </c>
+      <c r="G771" t="s">
+        <v>2671</v>
+      </c>
+    </row>
+    <row r="772" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A772" s="3" t="s">
+        <v>2696</v>
+      </c>
+      <c r="B772" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C772" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E772" s="3" t="s">
+        <v>2703</v>
+      </c>
+      <c r="F772" s="5" t="s">
+        <v>2712</v>
+      </c>
+      <c r="G772" s="3" t="s">
+        <v>2720</v>
+      </c>
+    </row>
+    <row r="773" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A773" s="3" t="s">
+        <v>2697</v>
+      </c>
+      <c r="B773" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C773" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E773" s="3" t="s">
+        <v>2702</v>
+      </c>
+      <c r="F773" s="5" t="s">
+        <v>2713</v>
+      </c>
+      <c r="G773" s="3" t="s">
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="774" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A774" t="s">
+        <v>2654</v>
+      </c>
+      <c r="B774" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C774" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E774" t="s">
+        <v>2661</v>
+      </c>
+      <c r="F774" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="G774" t="s">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="775" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A775" s="3" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B775" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C775" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E775" s="3" t="s">
+        <v>2701</v>
+      </c>
+      <c r="F775" s="5" t="s">
+        <v>2714</v>
+      </c>
+      <c r="G775" s="3" t="s">
+        <v>2722</v>
+      </c>
+    </row>
+    <row r="776" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A776" t="s">
         <v>2699</v>
       </c>
-      <c r="B768" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C768" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E768" t="s">
+      <c r="B776" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C776" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E776" t="s">
         <v>2700</v>
       </c>
-      <c r="F768" s="5" t="s">
+      <c r="F776" s="5" t="s">
         <v>2715</v>
       </c>
-      <c r="G768" t="s">
+      <c r="G776" t="s">
         <v>2723</v>
       </c>
     </row>
-    <row r="769" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A769" t="s">
+    <row r="777" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A777" t="s">
         <v>2724</v>
       </c>
-      <c r="B769" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C769" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E769" t="s">
+      <c r="B777" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C777" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E777" t="s">
         <v>2725</v>
       </c>
-      <c r="F769" s="5" t="s">
+      <c r="F777" s="5" t="s">
         <v>2726</v>
       </c>
-      <c r="G769" t="s">
+      <c r="G777" t="s">
         <v>2727</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G766" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G774" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
removed normalized properties from details entries
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1522BD98-EF07-43C5-935C-6E9BEEEC3BB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFE3C0B-0061-496F-9EF1-E196A004ACCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$774</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$769</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3116" uniqueCount="2754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3092" uniqueCount="2730">
   <si>
     <t>Key</t>
   </si>
@@ -7997,15 +7997,6 @@
     <t>السطر</t>
   </si>
   <si>
-    <t>DetailsEntry_NormalizedCount</t>
-  </si>
-  <si>
-    <t>DetailsEntry_NormalizedVolume</t>
-  </si>
-  <si>
-    <t>DetailsEntry_NormalizedMass</t>
-  </si>
-  <si>
     <t>Entry_Direction</t>
   </si>
   <si>
@@ -8015,24 +8006,6 @@
     <t>الاتجاه</t>
   </si>
   <si>
-    <t>Normalized Count</t>
-  </si>
-  <si>
-    <t>Normalized Mass</t>
-  </si>
-  <si>
-    <t>Normalized Volume</t>
-  </si>
-  <si>
-    <t>العدد المطبع</t>
-  </si>
-  <si>
-    <t>الكتلة المطبعة</t>
-  </si>
-  <si>
-    <t>الحجم المطبع</t>
-  </si>
-  <si>
     <t>存档日期</t>
   </si>
   <si>
@@ -8048,15 +8021,6 @@
     <t>显示在主菜单</t>
   </si>
   <si>
-    <t>标准化的计数</t>
-  </si>
-  <si>
-    <t>规范化质量</t>
-  </si>
-  <si>
-    <t>标准体积</t>
-  </si>
-  <si>
     <t>DetailsEntry</t>
   </si>
   <si>
@@ -8120,42 +8084,24 @@
     <t>DetailsEntry_AlgebraicCount</t>
   </si>
   <si>
-    <t>DetailsEntry_AlgebraicNormalizedCount</t>
-  </si>
-  <si>
     <t>DetailsEntry_AlgebraicMass</t>
   </si>
   <si>
-    <t>DetailsEntry_AlgebraicNormalizedMass</t>
-  </si>
-  <si>
     <t>DetailsEntry_AlgebraicVolume</t>
   </si>
   <si>
-    <t>DetailsEntry_AlgebraicNormalizedVolume</t>
-  </si>
-  <si>
     <t>DetailsEntry_AlgebraicTime</t>
   </si>
   <si>
     <t>Algebraic Time</t>
   </si>
   <si>
-    <t>Algebraic Normalized Volume</t>
-  </si>
-  <si>
     <t>Algebraic Volume</t>
   </si>
   <si>
-    <t>Algebraic Normalized Mass</t>
-  </si>
-  <si>
     <t>Algebraic Mass</t>
   </si>
   <si>
-    <t>Algebraic Normalized Count</t>
-  </si>
-  <si>
     <t>Algebraic Count</t>
   </si>
   <si>
@@ -8168,21 +8114,12 @@
     <t>العدد الجبري</t>
   </si>
   <si>
-    <t>العدد الجبري المطبع</t>
-  </si>
-  <si>
     <t>الكتلة الجبرية</t>
   </si>
   <si>
-    <t>الكتلة الجبرية المطبعة</t>
-  </si>
-  <si>
     <t>الحجم الجبري</t>
   </si>
   <si>
-    <t>الحجم الجبري المطبع</t>
-  </si>
-  <si>
     <t>الزمن الجبري</t>
   </si>
   <si>
@@ -8192,19 +8129,10 @@
     <t>代数计数</t>
   </si>
   <si>
-    <t>代数标准化的计数</t>
-  </si>
-  <si>
     <t>代数质量</t>
   </si>
   <si>
-    <t>代数规范化质量</t>
-  </si>
-  <si>
     <t>代数卷</t>
-  </si>
-  <si>
-    <t>代数标准体积</t>
   </si>
   <si>
     <t>代数时间</t>
@@ -8694,12 +8622,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G777"/>
+  <dimension ref="A1:G771"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A691" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A750" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G696" sqref="G696"/>
+      <selection pane="bottomLeft" activeCell="E779" sqref="E779"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15995,7 +15923,7 @@
         <v>2267</v>
       </c>
       <c r="G347" s="3" t="s">
-        <v>2665</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="348" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -16015,7 +15943,7 @@
         <v>2273</v>
       </c>
       <c r="G348" s="3" t="s">
-        <v>2666</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -18774,7 +18702,7 @@
     </row>
     <row r="481" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
-        <v>2691</v>
+        <v>2679</v>
       </c>
       <c r="B481" s="3" t="b">
         <v>1</v>
@@ -18906,15 +18834,15 @@
         <v>2651</v>
       </c>
       <c r="F487" s="5" t="s">
-        <v>2687</v>
+        <v>2675</v>
       </c>
       <c r="G487" t="s">
-        <v>2667</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>2685</v>
+        <v>2673</v>
       </c>
       <c r="B488" s="3" t="b">
         <v>1</v>
@@ -18923,10 +18851,10 @@
         <v>1</v>
       </c>
       <c r="E488" t="s">
-        <v>2685</v>
+        <v>2673</v>
       </c>
       <c r="F488" s="5" t="s">
-        <v>2686</v>
+        <v>2674</v>
       </c>
       <c r="G488" t="s">
         <v>1966</v>
@@ -18934,7 +18862,7 @@
     </row>
     <row r="489" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A489" s="3" t="s">
-        <v>2690</v>
+        <v>2678</v>
       </c>
       <c r="B489" s="3" t="b">
         <v>1</v>
@@ -18954,7 +18882,7 @@
     </row>
     <row r="490" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
-        <v>2688</v>
+        <v>2676</v>
       </c>
       <c r="B490" s="3" t="b">
         <v>1</v>
@@ -18966,7 +18894,7 @@
         <v>2313</v>
       </c>
       <c r="F490" s="5" t="s">
-        <v>2689</v>
+        <v>2677</v>
       </c>
       <c r="G490" s="3" t="s">
         <v>2317</v>
@@ -19069,12 +18997,12 @@
         <v>2652</v>
       </c>
       <c r="G495" s="3" t="s">
-        <v>2667</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="496" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
-        <v>2656</v>
+        <v>2653</v>
       </c>
       <c r="B496" s="3" t="b">
         <v>1</v>
@@ -19083,18 +19011,18 @@
         <v>1</v>
       </c>
       <c r="E496" s="3" t="s">
-        <v>2657</v>
+        <v>2654</v>
       </c>
       <c r="F496" s="5" t="s">
-        <v>2658</v>
+        <v>2655</v>
       </c>
       <c r="G496" s="3" t="s">
-        <v>2668</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="497" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
-        <v>2681</v>
+        <v>2669</v>
       </c>
       <c r="B497" s="3" t="b">
         <v>1</v>
@@ -19109,12 +19037,12 @@
         <v>2294</v>
       </c>
       <c r="G497" s="3" t="s">
-        <v>2683</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="498" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
-        <v>2682</v>
+        <v>2670</v>
       </c>
       <c r="B498" s="3" t="b">
         <v>1</v>
@@ -19129,7 +19057,7 @@
         <v>2295</v>
       </c>
       <c r="G498" s="3" t="s">
-        <v>2684</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="499" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -22217,7 +22145,7 @@
         <v>2635</v>
       </c>
       <c r="G650" s="3" t="s">
-        <v>2669</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="651" spans="1:7" x14ac:dyDescent="0.25">
@@ -23310,7 +23238,7 @@
     </row>
     <row r="705" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A705" s="3" t="s">
-        <v>2728</v>
+        <v>2704</v>
       </c>
       <c r="B705" s="3" t="b">
         <v>1</v>
@@ -23319,18 +23247,18 @@
         <v>1</v>
       </c>
       <c r="E705" s="3" t="s">
-        <v>2740</v>
+        <v>2716</v>
       </c>
       <c r="F705" s="5" t="s">
-        <v>2746</v>
+        <v>2722</v>
       </c>
       <c r="G705" s="3" t="s">
-        <v>2748</v>
+        <v>2724</v>
       </c>
     </row>
     <row r="706" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A706" s="3" t="s">
-        <v>2729</v>
+        <v>2705</v>
       </c>
       <c r="B706" s="3" t="b">
         <v>1</v>
@@ -23339,18 +23267,18 @@
         <v>1</v>
       </c>
       <c r="E706" s="3" t="s">
-        <v>2741</v>
+        <v>2717</v>
       </c>
       <c r="F706" s="5" t="s">
-        <v>2747</v>
+        <v>2723</v>
       </c>
       <c r="G706" s="3" t="s">
-        <v>2749</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="707" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A707" s="3" t="s">
-        <v>2730</v>
+        <v>2706</v>
       </c>
       <c r="B707" s="3" t="b">
         <v>1</v>
@@ -23359,18 +23287,18 @@
         <v>1</v>
       </c>
       <c r="E707" s="3" t="s">
-        <v>2736</v>
+        <v>2712</v>
       </c>
       <c r="F707" s="5" t="s">
-        <v>2744</v>
+        <v>2720</v>
       </c>
       <c r="G707" s="3" t="s">
-        <v>2750</v>
+        <v>2726</v>
       </c>
     </row>
     <row r="708" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A708" s="3" t="s">
-        <v>2733</v>
+        <v>2709</v>
       </c>
       <c r="B708" s="3" t="b">
         <v>1</v>
@@ -23379,18 +23307,18 @@
         <v>1</v>
       </c>
       <c r="E708" s="3" t="s">
-        <v>2737</v>
+        <v>2713</v>
       </c>
       <c r="F708" s="5" t="s">
-        <v>2745</v>
+        <v>2721</v>
       </c>
       <c r="G708" s="3" t="s">
-        <v>2751</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="709" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A709" s="3" t="s">
-        <v>2731</v>
+        <v>2707</v>
       </c>
       <c r="B709" s="3" t="b">
         <v>1</v>
@@ -23399,18 +23327,18 @@
         <v>1</v>
       </c>
       <c r="E709" s="3" t="s">
-        <v>2738</v>
+        <v>2714</v>
       </c>
       <c r="F709" s="5" t="s">
-        <v>2742</v>
+        <v>2718</v>
       </c>
       <c r="G709" s="3" t="s">
-        <v>2752</v>
+        <v>2728</v>
       </c>
     </row>
     <row r="710" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A710" s="3" t="s">
-        <v>2732</v>
+        <v>2708</v>
       </c>
       <c r="B710" s="3" t="b">
         <v>1</v>
@@ -23419,18 +23347,18 @@
         <v>1</v>
       </c>
       <c r="E710" s="3" t="s">
-        <v>2739</v>
+        <v>2715</v>
       </c>
       <c r="F710" s="5" t="s">
-        <v>2743</v>
+        <v>2719</v>
       </c>
       <c r="G710" s="3" t="s">
-        <v>2753</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="711" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A711" s="3" t="s">
-        <v>2734</v>
+        <v>2710</v>
       </c>
       <c r="B711" s="3" t="b">
         <v>1</v>
@@ -23450,7 +23378,7 @@
     </row>
     <row r="712" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A712" s="3" t="s">
-        <v>2735</v>
+        <v>2711</v>
       </c>
       <c r="B712" s="3" t="b">
         <v>1</v>
@@ -24500,7 +24428,7 @@
     </row>
     <row r="764" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A764" s="3" t="s">
-        <v>2673</v>
+        <v>2661</v>
       </c>
       <c r="B764" s="3" t="b">
         <v>1</v>
@@ -24509,18 +24437,18 @@
         <v>1</v>
       </c>
       <c r="E764" s="3" t="s">
-        <v>2675</v>
+        <v>2663</v>
       </c>
       <c r="F764" s="5" t="s">
-        <v>2677</v>
+        <v>2665</v>
       </c>
       <c r="G764" s="3" t="s">
-        <v>2679</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="765" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A765" s="3" t="s">
-        <v>2674</v>
+        <v>2662</v>
       </c>
       <c r="B765" s="3" t="b">
         <v>1</v>
@@ -24529,18 +24457,18 @@
         <v>1</v>
       </c>
       <c r="E765" s="3" t="s">
-        <v>2676</v>
+        <v>2664</v>
       </c>
       <c r="F765" s="5" t="s">
-        <v>2678</v>
+        <v>2666</v>
       </c>
       <c r="G765" s="3" t="s">
-        <v>2680</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="766" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>2692</v>
+        <v>2680</v>
       </c>
       <c r="B766" s="3" t="b">
         <v>1</v>
@@ -24549,18 +24477,18 @@
         <v>1</v>
       </c>
       <c r="E766" s="3" t="s">
-        <v>2707</v>
+        <v>2689</v>
       </c>
       <c r="F766" s="5" t="s">
-        <v>2708</v>
+        <v>2690</v>
       </c>
       <c r="G766" s="3" t="s">
-        <v>2716</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="767" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>2693</v>
+        <v>2681</v>
       </c>
       <c r="B767" s="3" t="b">
         <v>1</v>
@@ -24569,18 +24497,18 @@
         <v>1</v>
       </c>
       <c r="E767" s="3" t="s">
-        <v>2706</v>
+        <v>2688</v>
       </c>
       <c r="F767" s="5" t="s">
-        <v>2709</v>
+        <v>2691</v>
       </c>
       <c r="G767" s="3" t="s">
-        <v>2717</v>
-      </c>
-    </row>
-    <row r="768" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A768" t="s">
-        <v>2653</v>
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="768" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A768" s="3" t="s">
+        <v>2682</v>
       </c>
       <c r="B768" s="3" t="b">
         <v>1</v>
@@ -24588,59 +24516,59 @@
       <c r="C768" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E768" t="s">
-        <v>2659</v>
+      <c r="E768" s="3" t="s">
+        <v>2687</v>
       </c>
       <c r="F768" s="5" t="s">
-        <v>2662</v>
-      </c>
-      <c r="G768" t="s">
-        <v>2670</v>
+        <v>2692</v>
+      </c>
+      <c r="G768" s="3" t="s">
+        <v>2697</v>
       </c>
     </row>
     <row r="769" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A769" s="3" t="s">
+        <v>2683</v>
+      </c>
+      <c r="B769" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C769" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E769" s="3" t="s">
+        <v>2686</v>
+      </c>
+      <c r="F769" s="5" t="s">
+        <v>2693</v>
+      </c>
+      <c r="G769" s="3" t="s">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="770" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A770" t="s">
+        <v>2684</v>
+      </c>
+      <c r="B770" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C770" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E770" t="s">
+        <v>2685</v>
+      </c>
+      <c r="F770" s="5" t="s">
         <v>2694</v>
       </c>
-      <c r="B769" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C769" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E769" s="3" t="s">
-        <v>2705</v>
-      </c>
-      <c r="F769" s="5" t="s">
-        <v>2710</v>
-      </c>
-      <c r="G769" s="3" t="s">
-        <v>2718</v>
-      </c>
-    </row>
-    <row r="770" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A770" s="3" t="s">
-        <v>2695</v>
-      </c>
-      <c r="B770" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C770" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E770" s="3" t="s">
-        <v>2704</v>
-      </c>
-      <c r="F770" s="5" t="s">
-        <v>2711</v>
-      </c>
-      <c r="G770" s="3" t="s">
-        <v>2719</v>
+      <c r="G770" t="s">
+        <v>2699</v>
       </c>
     </row>
     <row r="771" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>2655</v>
+        <v>2700</v>
       </c>
       <c r="B771" s="3" t="b">
         <v>1</v>
@@ -24649,137 +24577,17 @@
         <v>1</v>
       </c>
       <c r="E771" t="s">
-        <v>2660</v>
+        <v>2701</v>
       </c>
       <c r="F771" s="5" t="s">
-        <v>2663</v>
+        <v>2702</v>
       </c>
       <c r="G771" t="s">
-        <v>2671</v>
-      </c>
-    </row>
-    <row r="772" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A772" s="3" t="s">
-        <v>2696</v>
-      </c>
-      <c r="B772" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C772" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E772" s="3" t="s">
         <v>2703</v>
       </c>
-      <c r="F772" s="5" t="s">
-        <v>2712</v>
-      </c>
-      <c r="G772" s="3" t="s">
-        <v>2720</v>
-      </c>
-    </row>
-    <row r="773" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A773" s="3" t="s">
-        <v>2697</v>
-      </c>
-      <c r="B773" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C773" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E773" s="3" t="s">
-        <v>2702</v>
-      </c>
-      <c r="F773" s="5" t="s">
-        <v>2713</v>
-      </c>
-      <c r="G773" s="3" t="s">
-        <v>2721</v>
-      </c>
-    </row>
-    <row r="774" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A774" t="s">
-        <v>2654</v>
-      </c>
-      <c r="B774" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C774" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E774" t="s">
-        <v>2661</v>
-      </c>
-      <c r="F774" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="G774" t="s">
-        <v>2672</v>
-      </c>
-    </row>
-    <row r="775" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A775" s="3" t="s">
-        <v>2698</v>
-      </c>
-      <c r="B775" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C775" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E775" s="3" t="s">
-        <v>2701</v>
-      </c>
-      <c r="F775" s="5" t="s">
-        <v>2714</v>
-      </c>
-      <c r="G775" s="3" t="s">
-        <v>2722</v>
-      </c>
-    </row>
-    <row r="776" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A776" t="s">
-        <v>2699</v>
-      </c>
-      <c r="B776" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C776" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E776" t="s">
-        <v>2700</v>
-      </c>
-      <c r="F776" s="5" t="s">
-        <v>2715</v>
-      </c>
-      <c r="G776" t="s">
-        <v>2723</v>
-      </c>
-    </row>
-    <row r="777" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A777" t="s">
-        <v>2724</v>
-      </c>
-      <c r="B777" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C777" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E777" t="s">
-        <v>2725</v>
-      </c>
-      <c r="F777" s="5" t="s">
-        <v>2726</v>
-      </c>
-      <c r="G777" t="s">
-        <v>2727</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G774" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G769" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented admin console and identity server users screen
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81094A7E-E655-479D-B231-B4144B5FD058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8956DF06-98C9-41CC-9ACB-4573F61B7C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3100" uniqueCount="2738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3184" uniqueCount="2812">
   <si>
     <t>Key</t>
   </si>
@@ -8250,6 +8250,228 @@
   </si>
   <si>
     <t>单元</t>
+  </si>
+  <si>
+    <t>LoadingAdminConsoleSettings</t>
+  </si>
+  <si>
+    <t>Loading admin console settings</t>
+  </si>
+  <si>
+    <t>جار تحميل إعدادات واجهة المشرف</t>
+  </si>
+  <si>
+    <t>加载管理控制台设置</t>
+  </si>
+  <si>
+    <t>Error_LoadingAdminSettings</t>
+  </si>
+  <si>
+    <t>Error loading admin console settings</t>
+  </si>
+  <si>
+    <t>حدث خطأ أثناء تحميل إعدادات واجهة المشرف</t>
+  </si>
+  <si>
+    <t>错误加载管理控制台设置</t>
+  </si>
+  <si>
+    <t>Error_UnauthorizedForAdmin</t>
+  </si>
+  <si>
+    <t>Your account can longer access the admin console.</t>
+  </si>
+  <si>
+    <t>حسابك على النظام لم يعد متاحا له الدخول إلى واجهة المشرف</t>
+  </si>
+  <si>
+    <t>您的帐户可以再访问管理控制台。</t>
+  </si>
+  <si>
+    <t>User_Permissions</t>
+  </si>
+  <si>
+    <t>AdminUser</t>
+  </si>
+  <si>
+    <t>AdminUsers</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>Admin Users</t>
+  </si>
+  <si>
+    <t>الأذونات</t>
+  </si>
+  <si>
+    <t>حسابات مشرفين</t>
+  </si>
+  <si>
+    <t>حساب مشرف</t>
+  </si>
+  <si>
+    <t>管理员用户</t>
+  </si>
+  <si>
+    <t>AdminConsole</t>
+  </si>
+  <si>
+    <t>Administrator Console</t>
+  </si>
+  <si>
+    <t>واجهة المشرف</t>
+  </si>
+  <si>
+    <t>管理员控制台</t>
+  </si>
+  <si>
+    <t>MyAdminAccount</t>
+  </si>
+  <si>
+    <t>My Admin Account</t>
+  </si>
+  <si>
+    <t>حسابي كمشرف</t>
+  </si>
+  <si>
+    <t>我的管理员帐户</t>
+  </si>
+  <si>
+    <t>IdentityServerUser</t>
+  </si>
+  <si>
+    <t>IdentityServerUsers</t>
+  </si>
+  <si>
+    <t>Identity Server User</t>
+  </si>
+  <si>
+    <t>Identity Server Users</t>
+  </si>
+  <si>
+    <t>Email Confirmed</t>
+  </si>
+  <si>
+    <t>Two Factor Enabled</t>
+  </si>
+  <si>
+    <t>Lockout End</t>
+  </si>
+  <si>
+    <t>مستخدمون من خادم الهويات</t>
+  </si>
+  <si>
+    <t>مستخدم من خادم الهويات</t>
+  </si>
+  <si>
+    <t>عنوان البريد مؤكد</t>
+  </si>
+  <si>
+    <t>نهاية المنع من الدخول</t>
+  </si>
+  <si>
+    <t>电子邮件确认</t>
+  </si>
+  <si>
+    <t>双因素启用</t>
+  </si>
+  <si>
+    <t>锁定结束</t>
+  </si>
+  <si>
+    <t>身份服务器的用户</t>
+  </si>
+  <si>
+    <t>IdentityServerUser_EmailConfirmed</t>
+  </si>
+  <si>
+    <t>IdentityServerUser_TwoFactorEnabled</t>
+  </si>
+  <si>
+    <t>IdentityServerUser_LockoutEnd</t>
+  </si>
+  <si>
+    <t>ResetPassword</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>تغيير كلمة المرور</t>
+  </si>
+  <si>
+    <t>重设密码</t>
+  </si>
+  <si>
+    <t>IdentityServerUser_PasswordSet</t>
+  </si>
+  <si>
+    <t>Password Set</t>
+  </si>
+  <si>
+    <t>Password Is Set</t>
+  </si>
+  <si>
+    <t>كلمة المرور محددة</t>
+  </si>
+  <si>
+    <t>密码设置</t>
+  </si>
+  <si>
+    <t>EmailConfirmed</t>
+  </si>
+  <si>
+    <t>EmailNotConfirmed</t>
+  </si>
+  <si>
+    <t>PasswordIsSet</t>
+  </si>
+  <si>
+    <t>PasswordIsNotSet</t>
+  </si>
+  <si>
+    <t>Email Not Confirmed</t>
+  </si>
+  <si>
+    <t>Password Not Set</t>
+  </si>
+  <si>
+    <t>عنوان البريد غير مؤكد</t>
+  </si>
+  <si>
+    <t>كلمة المرور غير محددة</t>
+  </si>
+  <si>
+    <t>电子邮件未确认</t>
+  </si>
+  <si>
+    <t>密码未设定</t>
+  </si>
+  <si>
+    <t>PasswordWasSuccessfullyReset</t>
+  </si>
+  <si>
+    <t>Password was successfully reset</t>
+  </si>
+  <si>
+    <t>تم حفظ كلمة المرور الجديدة</t>
+  </si>
+  <si>
+    <t>密码被重置成功</t>
+  </si>
+  <si>
+    <t>ShowHidePassword</t>
+  </si>
+  <si>
+    <t>Show/Hide Password</t>
+  </si>
+  <si>
+    <t>إظهار/إخفاء كلمة المرور</t>
+  </si>
+  <si>
+    <t>显示/隐藏密码</t>
   </si>
 </sst>
 </file>
@@ -8646,12 +8868,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G773"/>
+  <dimension ref="A1:G794"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A489" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A772" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E514" sqref="E514"/>
+      <selection pane="bottomLeft" activeCell="G794" sqref="G794"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9535,7 +9757,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
@@ -13882,7 +14104,7 @@
         <v>1</v>
       </c>
       <c r="C249" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D249" s="3"/>
       <c r="E249" s="3" t="s">
@@ -24648,6 +24870,426 @@
       </c>
       <c r="G773" t="s">
         <v>2703</v>
+      </c>
+    </row>
+    <row r="774" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A774" t="s">
+        <v>2738</v>
+      </c>
+      <c r="B774" t="b">
+        <v>0</v>
+      </c>
+      <c r="C774" t="b">
+        <v>1</v>
+      </c>
+      <c r="E774" t="s">
+        <v>2739</v>
+      </c>
+      <c r="F774" s="5" t="s">
+        <v>2740</v>
+      </c>
+      <c r="G774" s="2" t="s">
+        <v>2741</v>
+      </c>
+    </row>
+    <row r="775" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A775" s="3" t="s">
+        <v>2742</v>
+      </c>
+      <c r="B775" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C775" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E775" s="3" t="s">
+        <v>2743</v>
+      </c>
+      <c r="F775" s="5" t="s">
+        <v>2744</v>
+      </c>
+      <c r="G775" s="2" t="s">
+        <v>2745</v>
+      </c>
+    </row>
+    <row r="776" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A776" t="s">
+        <v>2746</v>
+      </c>
+      <c r="B776" t="b">
+        <v>0</v>
+      </c>
+      <c r="C776" t="b">
+        <v>1</v>
+      </c>
+      <c r="E776" s="3" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F776" s="5" t="s">
+        <v>2748</v>
+      </c>
+      <c r="G776" s="2" t="s">
+        <v>2749</v>
+      </c>
+    </row>
+    <row r="777" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A777" s="3" t="s">
+        <v>2751</v>
+      </c>
+      <c r="B777" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C777" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E777" s="3" t="s">
+        <v>2753</v>
+      </c>
+      <c r="F777" s="5" t="s">
+        <v>2757</v>
+      </c>
+      <c r="G777" s="2" t="s">
+        <v>2758</v>
+      </c>
+    </row>
+    <row r="778" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A778" s="3" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B778" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C778" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E778" s="3" t="s">
+        <v>2754</v>
+      </c>
+      <c r="F778" s="5" t="s">
+        <v>2756</v>
+      </c>
+      <c r="G778" s="2" t="s">
+        <v>2758</v>
+      </c>
+    </row>
+    <row r="779" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A779" t="s">
+        <v>2750</v>
+      </c>
+      <c r="B779" t="b">
+        <v>1</v>
+      </c>
+      <c r="C779" t="b">
+        <v>1</v>
+      </c>
+      <c r="E779" t="s">
+        <v>501</v>
+      </c>
+      <c r="F779" s="5" t="s">
+        <v>2755</v>
+      </c>
+      <c r="G779" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="780" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A780" t="s">
+        <v>2759</v>
+      </c>
+      <c r="B780" t="b">
+        <v>0</v>
+      </c>
+      <c r="C780" t="b">
+        <v>1</v>
+      </c>
+      <c r="E780" t="s">
+        <v>2760</v>
+      </c>
+      <c r="F780" s="5" t="s">
+        <v>2761</v>
+      </c>
+      <c r="G780" t="s">
+        <v>2762</v>
+      </c>
+    </row>
+    <row r="781" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A781" t="s">
+        <v>2763</v>
+      </c>
+      <c r="B781" t="b">
+        <v>0</v>
+      </c>
+      <c r="C781" t="b">
+        <v>1</v>
+      </c>
+      <c r="E781" t="s">
+        <v>2764</v>
+      </c>
+      <c r="F781" s="5" t="s">
+        <v>2765</v>
+      </c>
+      <c r="G781" t="s">
+        <v>2766</v>
+      </c>
+    </row>
+    <row r="782" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A782" s="3" t="s">
+        <v>2767</v>
+      </c>
+      <c r="B782" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C782" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E782" s="3" t="s">
+        <v>2769</v>
+      </c>
+      <c r="F782" s="5" t="s">
+        <v>2775</v>
+      </c>
+      <c r="G782" s="3" t="s">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="783" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A783" s="3" t="s">
+        <v>2768</v>
+      </c>
+      <c r="B783" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C783" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E783" s="3" t="s">
+        <v>2770</v>
+      </c>
+      <c r="F783" s="5" t="s">
+        <v>2774</v>
+      </c>
+      <c r="G783" s="3" t="s">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="784" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A784" t="s">
+        <v>2782</v>
+      </c>
+      <c r="B784" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C784" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E784" t="s">
+        <v>2771</v>
+      </c>
+      <c r="F784" s="5" t="s">
+        <v>2776</v>
+      </c>
+      <c r="G784" t="s">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="785" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A785" s="3" t="s">
+        <v>2789</v>
+      </c>
+      <c r="B785" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C785" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E785" s="3" t="s">
+        <v>2791</v>
+      </c>
+      <c r="F785" s="5" t="s">
+        <v>2792</v>
+      </c>
+      <c r="G785" s="3" t="s">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="786" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A786" t="s">
+        <v>2783</v>
+      </c>
+      <c r="B786" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C786" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E786" t="s">
+        <v>2772</v>
+      </c>
+      <c r="F786" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="G786" t="s">
+        <v>2779</v>
+      </c>
+    </row>
+    <row r="787" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A787" t="s">
+        <v>2784</v>
+      </c>
+      <c r="B787" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C787" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E787" t="s">
+        <v>2773</v>
+      </c>
+      <c r="F787" s="5" t="s">
+        <v>2777</v>
+      </c>
+      <c r="G787" t="s">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="788" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A788" t="s">
+        <v>2785</v>
+      </c>
+      <c r="B788" t="b">
+        <v>1</v>
+      </c>
+      <c r="C788" t="b">
+        <v>1</v>
+      </c>
+      <c r="E788" t="s">
+        <v>2786</v>
+      </c>
+      <c r="F788" s="5" t="s">
+        <v>2787</v>
+      </c>
+      <c r="G788" t="s">
+        <v>2788</v>
+      </c>
+    </row>
+    <row r="789" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A789" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B789" t="b">
+        <v>0</v>
+      </c>
+      <c r="C789" t="b">
+        <v>1</v>
+      </c>
+      <c r="E789" t="s">
+        <v>2771</v>
+      </c>
+      <c r="F789" s="5" t="s">
+        <v>2776</v>
+      </c>
+      <c r="G789" t="s">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="790" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A790" t="s">
+        <v>2795</v>
+      </c>
+      <c r="B790" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C790" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E790" t="s">
+        <v>2798</v>
+      </c>
+      <c r="F790" s="5" t="s">
+        <v>2800</v>
+      </c>
+      <c r="G790" t="s">
+        <v>2802</v>
+      </c>
+    </row>
+    <row r="791" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A791" t="s">
+        <v>2796</v>
+      </c>
+      <c r="B791" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C791" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E791" t="s">
+        <v>2790</v>
+      </c>
+      <c r="F791" s="5" t="s">
+        <v>2792</v>
+      </c>
+      <c r="G791" t="s">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="792" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A792" t="s">
+        <v>2797</v>
+      </c>
+      <c r="B792" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C792" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E792" t="s">
+        <v>2799</v>
+      </c>
+      <c r="F792" s="5" t="s">
+        <v>2801</v>
+      </c>
+      <c r="G792" t="s">
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="793" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A793" t="s">
+        <v>2804</v>
+      </c>
+      <c r="B793" t="b">
+        <v>0</v>
+      </c>
+      <c r="C793" t="b">
+        <v>1</v>
+      </c>
+      <c r="E793" t="s">
+        <v>2805</v>
+      </c>
+      <c r="F793" s="5" t="s">
+        <v>2806</v>
+      </c>
+      <c r="G793" t="s">
+        <v>2807</v>
+      </c>
+    </row>
+    <row r="794" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A794" t="s">
+        <v>2808</v>
+      </c>
+      <c r="B794" t="b">
+        <v>0</v>
+      </c>
+      <c r="C794" t="b">
+        <v>1</v>
+      </c>
+      <c r="E794" t="s">
+        <v>2809</v>
+      </c>
+      <c r="F794" s="5" t="s">
+        <v>2810</v>
+      </c>
+      <c r="G794" s="2" t="s">
+        <v>2811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the signatures framework
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C205538-3D81-4EBE-9065-68623033E1F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535EEAD4-0209-43AD-BB81-B37D51B65486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$758</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$756</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3164" uniqueCount="2786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3156" uniqueCount="2784">
   <si>
     <t>Key</t>
   </si>
@@ -7479,12 +7479,6 @@
   </si>
   <si>
     <t>EntryTypes</t>
-  </si>
-  <si>
-    <t>EntryType_ForCredit</t>
-  </si>
-  <si>
-    <t>EntryType_ForDebit</t>
   </si>
   <si>
     <t>Entry Type</t>
@@ -8790,12 +8784,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G789"/>
+  <dimension ref="A1:G787"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A481" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A689" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E496" sqref="E496"/>
+      <selection pane="bottomLeft" activeCell="B707" sqref="B707"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16091,7 +16085,7 @@
         <v>2227</v>
       </c>
       <c r="G347" s="3" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="348" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -16111,7 +16105,7 @@
         <v>2233</v>
       </c>
       <c r="G348" s="3" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -18830,7 +18824,7 @@
     </row>
     <row r="479" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
-        <v>2783</v>
+        <v>2781</v>
       </c>
       <c r="B479" s="3" t="b">
         <v>1</v>
@@ -18850,22 +18844,22 @@
     </row>
     <row r="480" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A480" s="3" t="s">
+        <v>2560</v>
+      </c>
+      <c r="B480" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C480" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E480" s="3" t="s">
+        <v>2561</v>
+      </c>
+      <c r="F480" s="5" t="s">
         <v>2562</v>
       </c>
-      <c r="B480" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C480" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E480" s="3" t="s">
+      <c r="G480" s="2" t="s">
         <v>2563</v>
-      </c>
-      <c r="F480" s="5" t="s">
-        <v>2564</v>
-      </c>
-      <c r="G480" s="2" t="s">
-        <v>2565</v>
       </c>
     </row>
     <row r="481" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -18890,7 +18884,7 @@
     </row>
     <row r="482" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A482" s="3" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
       <c r="B482" s="3" t="b">
         <v>1</v>
@@ -19010,7 +19004,7 @@
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
       <c r="B488" s="3" t="b">
         <v>1</v>
@@ -19019,18 +19013,18 @@
         <v>1</v>
       </c>
       <c r="E488" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
       <c r="F488" s="5" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
       <c r="G488" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="489" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="B489" s="3" t="b">
         <v>1</v>
@@ -19039,10 +19033,10 @@
         <v>1</v>
       </c>
       <c r="E489" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="F489" s="5" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
       <c r="G489" t="s">
         <v>1947</v>
@@ -19050,7 +19044,7 @@
     </row>
     <row r="490" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
       <c r="B490" s="3" t="b">
         <v>1</v>
@@ -19070,7 +19064,7 @@
     </row>
     <row r="491" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A491" s="3" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
       <c r="B491" s="3" t="b">
         <v>1</v>
@@ -19082,7 +19076,7 @@
         <v>2273</v>
       </c>
       <c r="F491" s="5" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
       <c r="G491" s="3" t="s">
         <v>2277</v>
@@ -19150,7 +19144,7 @@
     </row>
     <row r="495" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A495" s="3" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
       <c r="B495" s="3" t="b">
         <v>1</v>
@@ -19170,7 +19164,7 @@
     </row>
     <row r="496" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
-        <v>2784</v>
+        <v>2782</v>
       </c>
       <c r="B496" s="3" t="b">
         <v>1</v>
@@ -19179,18 +19173,18 @@
         <v>1</v>
       </c>
       <c r="E496" s="3" t="s">
+        <v>2684</v>
+      </c>
+      <c r="F496" s="5" t="s">
         <v>2686</v>
       </c>
-      <c r="F496" s="5" t="s">
+      <c r="G496" s="3" t="s">
         <v>2688</v>
-      </c>
-      <c r="G496" s="3" t="s">
-        <v>2690</v>
       </c>
     </row>
     <row r="497" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
-        <v>2785</v>
+        <v>2783</v>
       </c>
       <c r="B497" s="3" t="b">
         <v>1</v>
@@ -19199,58 +19193,58 @@
         <v>1</v>
       </c>
       <c r="E497" s="3" t="s">
+        <v>2685</v>
+      </c>
+      <c r="F497" s="5" t="s">
         <v>2687</v>
       </c>
-      <c r="F497" s="5" t="s">
+      <c r="G497" s="3" t="s">
         <v>2689</v>
-      </c>
-      <c r="G497" s="3" t="s">
-        <v>2691</v>
       </c>
     </row>
     <row r="498" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
+        <v>2602</v>
+      </c>
+      <c r="B498" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C498" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E498" s="3" t="s">
+        <v>2603</v>
+      </c>
+      <c r="F498" s="5" t="s">
         <v>2604</v>
       </c>
-      <c r="B498" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C498" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E498" s="3" t="s">
-        <v>2605</v>
-      </c>
-      <c r="F498" s="5" t="s">
-        <v>2606</v>
-      </c>
       <c r="G498" s="3" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="499" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
+        <v>2605</v>
+      </c>
+      <c r="B499" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C499" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E499" s="3" t="s">
+        <v>2606</v>
+      </c>
+      <c r="F499" s="5" t="s">
         <v>2607</v>
       </c>
-      <c r="B499" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C499" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E499" s="3" t="s">
-        <v>2608</v>
-      </c>
-      <c r="F499" s="5" t="s">
-        <v>2609</v>
-      </c>
       <c r="G499" s="3" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="500" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="B500" s="3" t="b">
         <v>1</v>
@@ -19265,12 +19259,12 @@
         <v>2254</v>
       </c>
       <c r="G500" s="3" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="501" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A501" s="3" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="B501" s="3" t="b">
         <v>1</v>
@@ -19285,12 +19279,12 @@
         <v>2255</v>
       </c>
       <c r="G501" s="3" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="502" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A502" s="3" t="s">
-        <v>2550</v>
+        <v>2548</v>
       </c>
       <c r="B502" s="3" t="b">
         <v>1</v>
@@ -19310,7 +19304,7 @@
     </row>
     <row r="503" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A503" s="3" t="s">
-        <v>2551</v>
+        <v>2549</v>
       </c>
       <c r="B503" s="3" t="b">
         <v>1</v>
@@ -19330,7 +19324,7 @@
     </row>
     <row r="504" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A504" s="3" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="B504" s="3" t="b">
         <v>1</v>
@@ -19339,10 +19333,10 @@
         <v>1</v>
       </c>
       <c r="E504" s="3" t="s">
-        <v>2537</v>
+        <v>2535</v>
       </c>
       <c r="F504" s="5" t="s">
-        <v>2543</v>
+        <v>2541</v>
       </c>
       <c r="G504" s="3" t="s">
         <v>2217</v>
@@ -19350,7 +19344,7 @@
     </row>
     <row r="505" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A505" s="3" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
       <c r="B505" s="3" t="b">
         <v>1</v>
@@ -19359,10 +19353,10 @@
         <v>1</v>
       </c>
       <c r="E505" s="3" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="F505" s="5" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
       <c r="G505" s="3" t="s">
         <v>2218</v>
@@ -19370,7 +19364,7 @@
     </row>
     <row r="506" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A506" s="3" t="s">
-        <v>2554</v>
+        <v>2552</v>
       </c>
       <c r="B506" s="3" t="b">
         <v>1</v>
@@ -19379,10 +19373,10 @@
         <v>1</v>
       </c>
       <c r="E506" s="3" t="s">
+        <v>2537</v>
+      </c>
+      <c r="F506" s="5" t="s">
         <v>2539</v>
-      </c>
-      <c r="F506" s="5" t="s">
-        <v>2541</v>
       </c>
       <c r="G506" s="3" t="s">
         <v>2219</v>
@@ -19390,7 +19384,7 @@
     </row>
     <row r="507" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A507" s="3" t="s">
-        <v>2555</v>
+        <v>2553</v>
       </c>
       <c r="B507" s="3" t="b">
         <v>1</v>
@@ -19399,10 +19393,10 @@
         <v>1</v>
       </c>
       <c r="E507" s="3" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
       <c r="F507" s="5" t="s">
-        <v>2544</v>
+        <v>2542</v>
       </c>
       <c r="G507" s="3" t="s">
         <v>2220</v>
@@ -19576,42 +19570,42 @@
     </row>
     <row r="516" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A516" s="3" t="s">
+        <v>2682</v>
+      </c>
+      <c r="B516" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C516" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E516" s="3" t="s">
         <v>2684</v>
       </c>
-      <c r="B516" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C516" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E516" s="3" t="s">
+      <c r="F516" s="5" t="s">
         <v>2686</v>
       </c>
-      <c r="F516" s="5" t="s">
+      <c r="G516" s="3" t="s">
         <v>2688</v>
-      </c>
-      <c r="G516" s="3" t="s">
-        <v>2690</v>
       </c>
     </row>
     <row r="517" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A517" s="3" t="s">
+        <v>2683</v>
+      </c>
+      <c r="B517" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C517" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E517" s="3" t="s">
         <v>2685</v>
       </c>
-      <c r="B517" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C517" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E517" s="3" t="s">
+      <c r="F517" s="5" t="s">
         <v>2687</v>
       </c>
-      <c r="F517" s="5" t="s">
+      <c r="G517" s="3" t="s">
         <v>2689</v>
-      </c>
-      <c r="G517" s="3" t="s">
-        <v>2691</v>
       </c>
     </row>
     <row r="518" spans="1:7" x14ac:dyDescent="0.25">
@@ -19739,7 +19733,7 @@
     </row>
     <row r="524" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A524" s="3" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
       <c r="B524" s="3" t="b">
         <v>1</v>
@@ -19748,10 +19742,10 @@
         <v>1</v>
       </c>
       <c r="E524" s="3" t="s">
-        <v>2488</v>
+        <v>2486</v>
       </c>
       <c r="F524" s="5" t="s">
-        <v>2496</v>
+        <v>2494</v>
       </c>
       <c r="G524" s="3" t="s">
         <v>1971</v>
@@ -19759,7 +19753,7 @@
     </row>
     <row r="525" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A525" s="3" t="s">
-        <v>2486</v>
+        <v>2484</v>
       </c>
       <c r="B525" s="3" t="b">
         <v>1</v>
@@ -19768,10 +19762,10 @@
         <v>1</v>
       </c>
       <c r="E525" s="3" t="s">
-        <v>2487</v>
+        <v>2485</v>
       </c>
       <c r="F525" s="5" t="s">
-        <v>2497</v>
+        <v>2495</v>
       </c>
       <c r="G525" s="3" t="s">
         <v>1971</v>
@@ -19800,7 +19794,7 @@
     </row>
     <row r="527" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A527" s="3" t="s">
-        <v>2491</v>
+        <v>2489</v>
       </c>
       <c r="B527" s="3" t="b">
         <v>1</v>
@@ -19810,10 +19804,10 @@
       </c>
       <c r="D527" s="3"/>
       <c r="E527" s="3" t="s">
-        <v>2494</v>
+        <v>2492</v>
       </c>
       <c r="F527" s="5" t="s">
-        <v>2489</v>
+        <v>2487</v>
       </c>
       <c r="G527" s="3" t="s">
         <v>1713</v>
@@ -19821,7 +19815,7 @@
     </row>
     <row r="528" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A528" s="3" t="s">
-        <v>2492</v>
+        <v>2490</v>
       </c>
       <c r="B528" s="3" t="b">
         <v>1</v>
@@ -19831,10 +19825,10 @@
       </c>
       <c r="D528" s="3"/>
       <c r="E528" s="3" t="s">
-        <v>2495</v>
+        <v>2493</v>
       </c>
       <c r="F528" s="5" t="s">
-        <v>2490</v>
+        <v>2488</v>
       </c>
       <c r="G528" s="3" t="s">
         <v>1713</v>
@@ -19842,7 +19836,7 @@
     </row>
     <row r="529" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A529" s="3" t="s">
-        <v>2493</v>
+        <v>2491</v>
       </c>
       <c r="B529" s="3" t="b">
         <v>1</v>
@@ -20276,7 +20270,7 @@
     </row>
     <row r="550" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A550" s="3" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
       <c r="B550" s="3" t="b">
         <v>1</v>
@@ -20286,10 +20280,10 @@
       </c>
       <c r="D550" s="3"/>
       <c r="E550" s="3" t="s">
-        <v>2494</v>
+        <v>2492</v>
       </c>
       <c r="F550" s="5" t="s">
-        <v>2501</v>
+        <v>2499</v>
       </c>
       <c r="G550" s="3" t="s">
         <v>1469</v>
@@ -20378,7 +20372,7 @@
     </row>
     <row r="555" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A555" s="3" t="s">
-        <v>2502</v>
+        <v>2500</v>
       </c>
       <c r="B555" s="3" t="b">
         <v>1</v>
@@ -20387,13 +20381,13 @@
         <v>1</v>
       </c>
       <c r="E555" s="3" t="s">
-        <v>2488</v>
+        <v>2486</v>
       </c>
       <c r="F555" s="5" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
       <c r="G555" s="3" t="s">
-        <v>2509</v>
+        <v>2507</v>
       </c>
     </row>
     <row r="556" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -20418,27 +20412,27 @@
     </row>
     <row r="557" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A557" s="3" t="s">
+        <v>2502</v>
+      </c>
+      <c r="B557" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C557" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E557" s="3" t="s">
+        <v>2503</v>
+      </c>
+      <c r="F557" s="5" t="s">
         <v>2504</v>
       </c>
-      <c r="B557" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C557" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E557" s="3" t="s">
-        <v>2505</v>
-      </c>
-      <c r="F557" s="5" t="s">
-        <v>2506</v>
-      </c>
       <c r="G557" s="3" t="s">
-        <v>2510</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="558" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A558" s="3" t="s">
-        <v>2511</v>
+        <v>2509</v>
       </c>
       <c r="B558" s="3" t="b">
         <v>1</v>
@@ -20447,18 +20441,18 @@
         <v>1</v>
       </c>
       <c r="E558" s="3" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
       <c r="F558" s="5" t="s">
+        <v>2521</v>
+      </c>
+      <c r="G558" s="3" t="s">
         <v>2523</v>
-      </c>
-      <c r="G558" s="3" t="s">
-        <v>2525</v>
       </c>
     </row>
     <row r="559" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A559" s="3" t="s">
-        <v>2512</v>
+        <v>2510</v>
       </c>
       <c r="B559" s="3" t="b">
         <v>1</v>
@@ -20467,18 +20461,18 @@
         <v>1</v>
       </c>
       <c r="E559" s="3" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
       <c r="F559" s="5" t="s">
+        <v>2522</v>
+      </c>
+      <c r="G559" s="3" t="s">
         <v>2524</v>
-      </c>
-      <c r="G559" s="3" t="s">
-        <v>2526</v>
       </c>
     </row>
     <row r="560" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A560" s="3" t="s">
-        <v>2513</v>
+        <v>2511</v>
       </c>
       <c r="B560" s="3" t="b">
         <v>1</v>
@@ -20487,18 +20481,18 @@
         <v>1</v>
       </c>
       <c r="E560" s="3" t="s">
-        <v>2522</v>
+        <v>2520</v>
       </c>
       <c r="F560" s="5" t="s">
-        <v>2545</v>
+        <v>2543</v>
       </c>
       <c r="G560" s="3" t="s">
-        <v>2527</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="561" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A561" s="3" t="s">
-        <v>2514</v>
+        <v>2512</v>
       </c>
       <c r="B561" s="3" t="b">
         <v>1</v>
@@ -20507,18 +20501,18 @@
         <v>1</v>
       </c>
       <c r="E561" s="3" t="s">
-        <v>2519</v>
+        <v>2517</v>
       </c>
       <c r="F561" s="5" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
       <c r="G561" s="3" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="562" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A562" s="3" t="s">
-        <v>2515</v>
+        <v>2513</v>
       </c>
       <c r="B562" s="3" t="b">
         <v>1</v>
@@ -20527,18 +20521,18 @@
         <v>1</v>
       </c>
       <c r="E562" s="3" t="s">
-        <v>2520</v>
+        <v>2518</v>
       </c>
       <c r="F562" s="5" t="s">
-        <v>2547</v>
+        <v>2545</v>
       </c>
       <c r="G562" s="3" t="s">
-        <v>2529</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="563" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A563" s="3" t="s">
-        <v>2516</v>
+        <v>2514</v>
       </c>
       <c r="B563" s="3" t="b">
         <v>1</v>
@@ -20547,18 +20541,18 @@
         <v>1</v>
       </c>
       <c r="E563" s="3" t="s">
-        <v>2521</v>
+        <v>2519</v>
       </c>
       <c r="F563" s="5" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="G563" s="3" t="s">
-        <v>2530</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="564" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A564" s="3" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
       <c r="B564" s="3" t="b">
         <v>1</v>
@@ -20570,7 +20564,7 @@
         <v>33</v>
       </c>
       <c r="F564" s="5" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
       <c r="G564" s="3" t="s">
         <v>1203</v>
@@ -20647,7 +20641,7 @@
         <v>1</v>
       </c>
       <c r="E568" s="3" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="F568" s="5" t="s">
         <v>2180</v>
@@ -22294,22 +22288,22 @@
     </row>
     <row r="650" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A650" s="3" t="s">
+        <v>2585</v>
+      </c>
+      <c r="B650" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C650" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E650" s="3" t="s">
+        <v>2586</v>
+      </c>
+      <c r="F650" s="5" t="s">
         <v>2587</v>
       </c>
-      <c r="B650" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C650" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E650" s="3" t="s">
-        <v>2588</v>
-      </c>
-      <c r="F650" s="5" t="s">
-        <v>2589</v>
-      </c>
       <c r="G650" s="3" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="651" spans="1:7" x14ac:dyDescent="0.25">
@@ -22976,7 +22970,7 @@
     </row>
     <row r="684" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A684" s="3" t="s">
-        <v>2498</v>
+        <v>2496</v>
       </c>
       <c r="B684" s="3" t="b">
         <v>1</v>
@@ -22989,7 +22983,7 @@
         <v>1731</v>
       </c>
       <c r="F684" s="5" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
       <c r="G684" s="3" t="s">
         <v>1469</v>
@@ -23179,7 +23173,7 @@
     </row>
     <row r="694" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A694" s="3" t="s">
-        <v>2658</v>
+        <v>2656</v>
       </c>
       <c r="B694" s="3" t="b">
         <v>1</v>
@@ -23188,18 +23182,18 @@
         <v>1</v>
       </c>
       <c r="E694" s="3" t="s">
-        <v>2670</v>
+        <v>2668</v>
       </c>
       <c r="F694" s="5" t="s">
+        <v>2674</v>
+      </c>
+      <c r="G694" s="3" t="s">
         <v>2676</v>
-      </c>
-      <c r="G694" s="3" t="s">
-        <v>2678</v>
       </c>
     </row>
     <row r="695" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A695" s="3" t="s">
-        <v>2659</v>
+        <v>2657</v>
       </c>
       <c r="B695" s="3" t="b">
         <v>1</v>
@@ -23208,18 +23202,18 @@
         <v>1</v>
       </c>
       <c r="E695" s="3" t="s">
-        <v>2671</v>
+        <v>2669</v>
       </c>
       <c r="F695" s="5" t="s">
+        <v>2675</v>
+      </c>
+      <c r="G695" s="3" t="s">
         <v>2677</v>
-      </c>
-      <c r="G695" s="3" t="s">
-        <v>2679</v>
       </c>
     </row>
     <row r="696" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A696" s="3" t="s">
-        <v>2660</v>
+        <v>2658</v>
       </c>
       <c r="B696" s="3" t="b">
         <v>1</v>
@@ -23228,18 +23222,18 @@
         <v>1</v>
       </c>
       <c r="E696" s="3" t="s">
-        <v>2666</v>
+        <v>2664</v>
       </c>
       <c r="F696" s="5" t="s">
-        <v>2674</v>
+        <v>2672</v>
       </c>
       <c r="G696" s="3" t="s">
-        <v>2680</v>
+        <v>2678</v>
       </c>
     </row>
     <row r="697" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A697" s="3" t="s">
-        <v>2663</v>
+        <v>2661</v>
       </c>
       <c r="B697" s="3" t="b">
         <v>1</v>
@@ -23248,18 +23242,18 @@
         <v>1</v>
       </c>
       <c r="E697" s="3" t="s">
-        <v>2667</v>
+        <v>2665</v>
       </c>
       <c r="F697" s="5" t="s">
-        <v>2675</v>
+        <v>2673</v>
       </c>
       <c r="G697" s="3" t="s">
-        <v>2681</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="698" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A698" s="3" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="B698" s="3" t="b">
         <v>1</v>
@@ -23268,18 +23262,18 @@
         <v>1</v>
       </c>
       <c r="E698" s="3" t="s">
-        <v>2668</v>
+        <v>2666</v>
       </c>
       <c r="F698" s="5" t="s">
-        <v>2672</v>
+        <v>2670</v>
       </c>
       <c r="G698" s="3" t="s">
-        <v>2682</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="699" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A699" s="3" t="s">
-        <v>2662</v>
+        <v>2660</v>
       </c>
       <c r="B699" s="3" t="b">
         <v>1</v>
@@ -23288,18 +23282,18 @@
         <v>1</v>
       </c>
       <c r="E699" s="3" t="s">
-        <v>2669</v>
+        <v>2667</v>
       </c>
       <c r="F699" s="5" t="s">
-        <v>2673</v>
+        <v>2671</v>
       </c>
       <c r="G699" s="3" t="s">
-        <v>2683</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="700" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A700" s="3" t="s">
-        <v>2664</v>
+        <v>2662</v>
       </c>
       <c r="B700" s="3" t="b">
         <v>1</v>
@@ -23319,7 +23313,7 @@
     </row>
     <row r="701" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A701" s="3" t="s">
-        <v>2665</v>
+        <v>2663</v>
       </c>
       <c r="B701" s="3" t="b">
         <v>1</v>
@@ -23414,7 +23408,7 @@
         <v>1</v>
       </c>
       <c r="E705" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="F705" s="5" t="s">
         <v>2180</v>
@@ -23434,7 +23428,7 @@
         <v>1</v>
       </c>
       <c r="E706" t="s">
-        <v>2484</v>
+        <v>2482</v>
       </c>
       <c r="F706" s="5" t="s">
         <v>2179</v>
@@ -23443,229 +23437,232 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="707" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A707" s="3" t="s">
-        <v>2481</v>
-      </c>
-      <c r="B707" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C707" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E707" s="3" t="s">
-        <v>320</v>
+    <row r="707" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A707" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B707" t="b">
+        <v>1</v>
+      </c>
+      <c r="C707" t="b">
+        <v>1</v>
+      </c>
+      <c r="E707" t="s">
+        <v>2223</v>
       </c>
       <c r="F707" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="G707" s="3" t="s">
-        <v>1303</v>
-      </c>
-    </row>
-    <row r="708" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A708" s="3" t="s">
-        <v>2482</v>
-      </c>
-      <c r="B708" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C708" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E708" s="3" t="s">
-        <v>323</v>
+        <v>2224</v>
+      </c>
+      <c r="G707" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="708" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B708" t="b">
+        <v>1</v>
+      </c>
+      <c r="C708" t="b">
+        <v>0</v>
+      </c>
+      <c r="E708" t="s">
+        <v>2235</v>
       </c>
       <c r="F708" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="G708" s="3" t="s">
-        <v>1304</v>
+        <v>2237</v>
+      </c>
+      <c r="G708" t="s">
+        <v>2247</v>
       </c>
     </row>
     <row r="709" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>2234</v>
+        <v>2240</v>
       </c>
       <c r="B709" t="b">
         <v>1</v>
       </c>
       <c r="C709" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E709" t="s">
-        <v>2223</v>
+        <v>2238</v>
       </c>
       <c r="F709" s="5" t="s">
-        <v>2224</v>
+        <v>2239</v>
       </c>
       <c r="G709" t="s">
-        <v>2246</v>
-      </c>
-    </row>
-    <row r="710" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A710" t="s">
-        <v>2236</v>
-      </c>
-      <c r="B710" t="b">
-        <v>1</v>
-      </c>
-      <c r="C710" t="b">
-        <v>0</v>
-      </c>
-      <c r="E710" t="s">
-        <v>2235</v>
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="710" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A710" s="3" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B710" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C710" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E710" s="3" t="s">
+        <v>2244</v>
       </c>
       <c r="F710" s="5" t="s">
-        <v>2237</v>
-      </c>
-      <c r="G710" t="s">
-        <v>2247</v>
+        <v>2245</v>
+      </c>
+      <c r="G710" s="3" t="s">
+        <v>2249</v>
       </c>
     </row>
     <row r="711" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>2240</v>
+        <v>2250</v>
       </c>
       <c r="B711" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C711" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E711" t="s">
-        <v>2238</v>
+        <v>2253</v>
       </c>
       <c r="F711" s="5" t="s">
-        <v>2239</v>
+        <v>2254</v>
       </c>
       <c r="G711" t="s">
-        <v>2248</v>
-      </c>
-    </row>
-    <row r="712" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A712" s="3" t="s">
-        <v>2243</v>
-      </c>
-      <c r="B712" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C712" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E712" s="3" t="s">
-        <v>2244</v>
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="712" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A712" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B712" t="b">
+        <v>0</v>
+      </c>
+      <c r="C712" t="b">
+        <v>1</v>
+      </c>
+      <c r="E712" t="s">
+        <v>2252</v>
       </c>
       <c r="F712" s="5" t="s">
-        <v>2245</v>
-      </c>
-      <c r="G712" s="3" t="s">
-        <v>2249</v>
+        <v>2255</v>
+      </c>
+      <c r="G712" t="s">
+        <v>2264</v>
       </c>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>2250</v>
+        <v>2257</v>
       </c>
       <c r="B713" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C713" t="b">
         <v>1</v>
       </c>
       <c r="E713" t="s">
-        <v>2253</v>
+        <v>2259</v>
       </c>
       <c r="F713" s="5" t="s">
-        <v>2254</v>
+        <v>2262</v>
       </c>
       <c r="G713" t="s">
-        <v>2263</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="714" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>2251</v>
-      </c>
-      <c r="B714" t="b">
-        <v>0</v>
-      </c>
-      <c r="C714" t="b">
+        <v>2258</v>
+      </c>
+      <c r="B714" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C714" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E714" t="s">
-        <v>2252</v>
+        <v>493</v>
       </c>
       <c r="F714" s="5" t="s">
-        <v>2255</v>
+        <v>492</v>
       </c>
       <c r="G714" t="s">
-        <v>2264</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="715" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>2257</v>
-      </c>
-      <c r="B715" t="b">
-        <v>1</v>
-      </c>
-      <c r="C715" t="b">
+        <v>2320</v>
+      </c>
+      <c r="B715" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C715" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E715" t="s">
-        <v>2259</v>
+        <v>2260</v>
       </c>
       <c r="F715" s="5" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="G715" t="s">
-        <v>2265</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="716" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>2258</v>
-      </c>
-      <c r="B716" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C716" s="3" t="b">
-        <v>1</v>
+        <v>2269</v>
+      </c>
+      <c r="B716" t="b">
+        <v>0</v>
+      </c>
+      <c r="C716" t="b">
+        <v>1</v>
+      </c>
+      <c r="D716" t="s">
+        <v>2270</v>
       </c>
       <c r="E716" t="s">
-        <v>493</v>
+        <v>2272</v>
       </c>
       <c r="F716" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="G716" t="s">
-        <v>1364</v>
+        <v>2271</v>
+      </c>
+      <c r="G716" s="3" t="s">
+        <v>2277</v>
       </c>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>2320</v>
-      </c>
-      <c r="B717" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C717" s="3" t="b">
+        <v>2301</v>
+      </c>
+      <c r="B717" t="b">
+        <v>0</v>
+      </c>
+      <c r="C717" t="b">
         <v>1</v>
       </c>
       <c r="E717" t="s">
-        <v>2260</v>
+        <v>2302</v>
       </c>
       <c r="F717" s="5" t="s">
-        <v>2261</v>
+        <v>2318</v>
       </c>
       <c r="G717" t="s">
-        <v>2266</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="718" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>2269</v>
+        <v>2303</v>
       </c>
       <c r="B718" t="b">
         <v>0</v>
@@ -23673,42 +23670,39 @@
       <c r="C718" t="b">
         <v>1</v>
       </c>
-      <c r="D718" t="s">
-        <v>2270</v>
-      </c>
       <c r="E718" t="s">
-        <v>2272</v>
+        <v>2319</v>
       </c>
       <c r="F718" s="5" t="s">
-        <v>2271</v>
-      </c>
-      <c r="G718" s="3" t="s">
-        <v>2277</v>
-      </c>
-    </row>
-    <row r="719" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A719" t="s">
-        <v>2301</v>
-      </c>
-      <c r="B719" t="b">
-        <v>0</v>
-      </c>
-      <c r="C719" t="b">
-        <v>1</v>
-      </c>
-      <c r="E719" t="s">
-        <v>2302</v>
+        <v>2306</v>
+      </c>
+      <c r="G718" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="719" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A719" s="3" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B719" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C719" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E719" s="3" t="s">
+        <v>2310</v>
       </c>
       <c r="F719" s="5" t="s">
-        <v>2318</v>
-      </c>
-      <c r="G719" t="s">
-        <v>2313</v>
+        <v>2311</v>
+      </c>
+      <c r="G719" s="3" t="s">
+        <v>2315</v>
       </c>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>2303</v>
+        <v>2304</v>
       </c>
       <c r="B720" t="b">
         <v>0</v>
@@ -23717,38 +23711,38 @@
         <v>1</v>
       </c>
       <c r="E720" t="s">
-        <v>2319</v>
+        <v>2304</v>
       </c>
       <c r="F720" s="5" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="G720" t="s">
-        <v>2314</v>
-      </c>
-    </row>
-    <row r="721" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A721" s="3" t="s">
-        <v>2309</v>
-      </c>
-      <c r="B721" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C721" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E721" s="3" t="s">
-        <v>2310</v>
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="721" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A721" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B721" t="b">
+        <v>0</v>
+      </c>
+      <c r="C721" t="b">
+        <v>1</v>
+      </c>
+      <c r="E721" t="s">
+        <v>2307</v>
       </c>
       <c r="F721" s="5" t="s">
-        <v>2311</v>
-      </c>
-      <c r="G721" s="3" t="s">
-        <v>2315</v>
+        <v>2312</v>
+      </c>
+      <c r="G721" t="s">
+        <v>2317</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>2304</v>
+        <v>496</v>
       </c>
       <c r="B722" t="b">
         <v>0</v>
@@ -23757,18 +23751,18 @@
         <v>1</v>
       </c>
       <c r="E722" t="s">
-        <v>2304</v>
+        <v>496</v>
       </c>
       <c r="F722" s="5" t="s">
-        <v>2305</v>
+        <v>495</v>
       </c>
       <c r="G722" t="s">
-        <v>2316</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>2308</v>
+        <v>2333</v>
       </c>
       <c r="B723" t="b">
         <v>0</v>
@@ -23777,18 +23771,18 @@
         <v>1</v>
       </c>
       <c r="E723" t="s">
-        <v>2307</v>
+        <v>2333</v>
       </c>
       <c r="F723" s="5" t="s">
-        <v>2312</v>
+        <v>2334</v>
       </c>
       <c r="G723" t="s">
-        <v>2317</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>496</v>
+        <v>2342</v>
       </c>
       <c r="B724" t="b">
         <v>0</v>
@@ -23797,78 +23791,78 @@
         <v>1</v>
       </c>
       <c r="E724" t="s">
-        <v>496</v>
+        <v>2343</v>
       </c>
       <c r="F724" s="5" t="s">
-        <v>495</v>
+        <v>2346</v>
       </c>
       <c r="G724" t="s">
-        <v>1365</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>2333</v>
+        <v>2406</v>
       </c>
       <c r="B725" t="b">
-        <v>0</v>
-      </c>
-      <c r="C725" t="b">
+        <v>1</v>
+      </c>
+      <c r="C725" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E725" t="s">
-        <v>2333</v>
+        <v>2347</v>
       </c>
       <c r="F725" s="5" t="s">
-        <v>2334</v>
+        <v>2354</v>
       </c>
       <c r="G725" t="s">
-        <v>2344</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>2342</v>
-      </c>
-      <c r="B726" t="b">
-        <v>0</v>
-      </c>
-      <c r="C726" t="b">
+        <v>2407</v>
+      </c>
+      <c r="B726" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C726" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E726" t="s">
-        <v>2343</v>
+        <v>2348</v>
       </c>
       <c r="F726" s="5" t="s">
-        <v>2346</v>
+        <v>2355</v>
       </c>
       <c r="G726" t="s">
-        <v>2345</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>2406</v>
-      </c>
-      <c r="B727" t="b">
+        <v>2408</v>
+      </c>
+      <c r="B727" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C727" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E727" t="s">
-        <v>2347</v>
+        <v>2349</v>
       </c>
       <c r="F727" s="5" t="s">
-        <v>2354</v>
+        <v>2356</v>
       </c>
       <c r="G727" t="s">
-        <v>2361</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>2407</v>
+        <v>2409</v>
       </c>
       <c r="B728" s="3" t="b">
         <v>1</v>
@@ -23877,18 +23871,18 @@
         <v>1</v>
       </c>
       <c r="E728" t="s">
-        <v>2348</v>
+        <v>2351</v>
       </c>
       <c r="F728" s="5" t="s">
-        <v>2355</v>
+        <v>2358</v>
       </c>
       <c r="G728" t="s">
-        <v>2367</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>2408</v>
+        <v>2410</v>
       </c>
       <c r="B729" s="3" t="b">
         <v>1</v>
@@ -23897,18 +23891,18 @@
         <v>1</v>
       </c>
       <c r="E729" t="s">
-        <v>2349</v>
+        <v>2352</v>
       </c>
       <c r="F729" s="5" t="s">
-        <v>2356</v>
+        <v>2359</v>
       </c>
       <c r="G729" t="s">
-        <v>2362</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>2409</v>
+        <v>2411</v>
       </c>
       <c r="B730" s="3" t="b">
         <v>1</v>
@@ -23917,18 +23911,18 @@
         <v>1</v>
       </c>
       <c r="E730" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="F730" s="5" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="G730" t="s">
-        <v>2363</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>2410</v>
+        <v>2412</v>
       </c>
       <c r="B731" s="3" t="b">
         <v>1</v>
@@ -23937,58 +23931,58 @@
         <v>1</v>
       </c>
       <c r="E731" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="F731" s="5" t="s">
-        <v>2359</v>
+        <v>2360</v>
       </c>
       <c r="G731" t="s">
-        <v>2364</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="732" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>2411</v>
-      </c>
-      <c r="B732" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C732" s="3" t="b">
+        <v>2428</v>
+      </c>
+      <c r="B732" t="b">
+        <v>1</v>
+      </c>
+      <c r="C732" t="b">
         <v>1</v>
       </c>
       <c r="E732" t="s">
-        <v>2350</v>
+        <v>2430</v>
       </c>
       <c r="F732" s="5" t="s">
-        <v>2357</v>
+        <v>2432</v>
       </c>
       <c r="G732" t="s">
-        <v>2365</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>2412</v>
-      </c>
-      <c r="B733" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C733" s="3" t="b">
+        <v>2429</v>
+      </c>
+      <c r="B733" t="b">
+        <v>1</v>
+      </c>
+      <c r="C733" t="b">
         <v>1</v>
       </c>
       <c r="E733" t="s">
-        <v>2353</v>
+        <v>2431</v>
       </c>
       <c r="F733" s="5" t="s">
-        <v>2360</v>
+        <v>2433</v>
       </c>
       <c r="G733" t="s">
-        <v>2366</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>2428</v>
+        <v>2436</v>
       </c>
       <c r="B734" t="b">
         <v>1</v>
@@ -23997,18 +23991,18 @@
         <v>1</v>
       </c>
       <c r="E734" t="s">
-        <v>2430</v>
+        <v>2437</v>
       </c>
       <c r="F734" s="5" t="s">
-        <v>2432</v>
+        <v>2438</v>
       </c>
       <c r="G734" t="s">
-        <v>2434</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>2429</v>
+        <v>2439</v>
       </c>
       <c r="B735" t="b">
         <v>1</v>
@@ -24017,58 +24011,58 @@
         <v>1</v>
       </c>
       <c r="E735" t="s">
-        <v>2431</v>
+        <v>2452</v>
       </c>
       <c r="F735" s="5" t="s">
-        <v>2433</v>
+        <v>2440</v>
       </c>
       <c r="G735" t="s">
-        <v>2435</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="736" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>2436</v>
+        <v>2449</v>
       </c>
       <c r="B736" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C736" t="b">
         <v>1</v>
       </c>
       <c r="E736" t="s">
-        <v>2437</v>
+        <v>2450</v>
       </c>
       <c r="F736" s="5" t="s">
-        <v>2438</v>
+        <v>2451</v>
       </c>
       <c r="G736" t="s">
-        <v>2441</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>2439</v>
+        <v>2475</v>
       </c>
       <c r="B737" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C737" t="b">
         <v>1</v>
       </c>
       <c r="E737" t="s">
-        <v>2452</v>
+        <v>2475</v>
       </c>
       <c r="F737" s="5" t="s">
-        <v>2440</v>
+        <v>1075</v>
       </c>
       <c r="G737" t="s">
-        <v>2442</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="738" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>2449</v>
+        <v>2529</v>
       </c>
       <c r="B738" t="b">
         <v>0</v>
@@ -24077,18 +24071,18 @@
         <v>1</v>
       </c>
       <c r="E738" t="s">
-        <v>2450</v>
+        <v>2529</v>
       </c>
       <c r="F738" s="5" t="s">
-        <v>2451</v>
+        <v>2530</v>
       </c>
       <c r="G738" t="s">
-        <v>2427</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="739" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>2475</v>
+        <v>2531</v>
       </c>
       <c r="B739" t="b">
         <v>0</v>
@@ -24097,110 +24091,110 @@
         <v>1</v>
       </c>
       <c r="E739" t="s">
-        <v>2475</v>
+        <v>2531</v>
       </c>
       <c r="F739" s="5" t="s">
-        <v>1075</v>
+        <v>2532</v>
       </c>
       <c r="G739" t="s">
-        <v>2476</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="740" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A740" t="s">
-        <v>2531</v>
+      <c r="A740" s="3" t="s">
+        <v>2554</v>
       </c>
       <c r="B740" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C740" t="b">
         <v>1</v>
       </c>
       <c r="E740" t="s">
-        <v>2531</v>
+        <v>2555</v>
       </c>
       <c r="F740" s="5" t="s">
-        <v>2532</v>
+        <v>1678</v>
       </c>
       <c r="G740" t="s">
-        <v>2535</v>
-      </c>
-    </row>
-    <row r="741" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A741" t="s">
-        <v>2533</v>
-      </c>
-      <c r="B741" t="b">
-        <v>0</v>
-      </c>
-      <c r="C741" t="b">
-        <v>1</v>
-      </c>
-      <c r="E741" t="s">
-        <v>2533</v>
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="741" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A741" s="3" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B741" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C741" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E741" s="3" t="s">
+        <v>2579</v>
       </c>
       <c r="F741" s="5" t="s">
-        <v>2534</v>
-      </c>
-      <c r="G741" t="s">
-        <v>2536</v>
+        <v>2580</v>
+      </c>
+      <c r="G741" s="3" t="s">
+        <v>2581</v>
       </c>
     </row>
     <row r="742" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A742" s="3" t="s">
-        <v>2556</v>
+      <c r="A742" t="s">
+        <v>2557</v>
       </c>
       <c r="B742" t="b">
         <v>1</v>
       </c>
       <c r="C742" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E742" t="s">
-        <v>2557</v>
+        <v>2565</v>
       </c>
       <c r="F742" s="5" t="s">
-        <v>1678</v>
+        <v>2566</v>
       </c>
       <c r="G742" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="743" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
+        <v>2559</v>
+      </c>
+      <c r="B743" t="b">
+        <v>1</v>
+      </c>
+      <c r="C743" t="b">
+        <v>0</v>
+      </c>
+      <c r="E743" t="s">
         <v>2558</v>
       </c>
-    </row>
-    <row r="743" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A743" s="3" t="s">
-        <v>2580</v>
-      </c>
-      <c r="B743" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C743" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E743" s="3" t="s">
-        <v>2581</v>
-      </c>
       <c r="F743" s="5" t="s">
-        <v>2582</v>
-      </c>
-      <c r="G743" s="3" t="s">
-        <v>2583</v>
+        <v>2567</v>
+      </c>
+      <c r="G743" t="s">
+        <v>2569</v>
       </c>
     </row>
     <row r="744" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>2559</v>
+        <v>2571</v>
       </c>
       <c r="B744" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C744" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E744" t="s">
-        <v>2567</v>
+        <v>2571</v>
       </c>
       <c r="F744" s="5" t="s">
-        <v>2568</v>
+        <v>2564</v>
       </c>
       <c r="G744" t="s">
         <v>2570</v>
@@ -24208,47 +24202,48 @@
     </row>
     <row r="745" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>2561</v>
+        <v>2572</v>
       </c>
       <c r="B745" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C745" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E745" t="s">
-        <v>2560</v>
+        <v>2572</v>
       </c>
       <c r="F745" s="5" t="s">
-        <v>2569</v>
+        <v>2573</v>
       </c>
       <c r="G745" t="s">
-        <v>2571</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="746" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A746" t="s">
-        <v>2573</v>
-      </c>
-      <c r="B746" t="b">
-        <v>0</v>
-      </c>
-      <c r="C746" t="b">
-        <v>1</v>
-      </c>
-      <c r="E746" t="s">
-        <v>2573</v>
+      <c r="A746" s="3" t="s">
+        <v>2577</v>
+      </c>
+      <c r="B746" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C746" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D746" s="3"/>
+      <c r="E746" s="3" t="s">
+        <v>2574</v>
       </c>
       <c r="F746" s="5" t="s">
-        <v>2566</v>
-      </c>
-      <c r="G746" t="s">
-        <v>2572</v>
+        <v>2575</v>
+      </c>
+      <c r="G746" s="3" t="s">
+        <v>2576</v>
       </c>
     </row>
     <row r="747" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>2574</v>
+        <v>2582</v>
       </c>
       <c r="B747" t="b">
         <v>0</v>
@@ -24257,51 +24252,50 @@
         <v>1</v>
       </c>
       <c r="E747" t="s">
-        <v>2574</v>
+        <v>2583</v>
       </c>
       <c r="F747" s="5" t="s">
-        <v>2575</v>
+        <v>2584</v>
       </c>
       <c r="G747" t="s">
+        <v>2595</v>
+      </c>
+    </row>
+    <row r="748" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A748" t="s">
+        <v>2588</v>
+      </c>
+      <c r="B748" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C748" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E748" t="s">
+        <v>2592</v>
+      </c>
+      <c r="F748" s="5" t="s">
+        <v>2591</v>
+      </c>
+      <c r="G748" t="s">
         <v>2596</v>
-      </c>
-    </row>
-    <row r="748" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A748" s="3" t="s">
-        <v>2579</v>
-      </c>
-      <c r="B748" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C748" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D748" s="3"/>
-      <c r="E748" s="3" t="s">
-        <v>2576</v>
-      </c>
-      <c r="F748" s="5" t="s">
-        <v>2577</v>
-      </c>
-      <c r="G748" s="3" t="s">
-        <v>2578</v>
       </c>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>2584</v>
-      </c>
-      <c r="B749" t="b">
-        <v>0</v>
-      </c>
-      <c r="C749" t="b">
+        <v>2589</v>
+      </c>
+      <c r="B749" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C749" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E749" t="s">
-        <v>2585</v>
+        <v>2593</v>
       </c>
       <c r="F749" s="5" t="s">
-        <v>2586</v>
+        <v>2590</v>
       </c>
       <c r="G749" t="s">
         <v>2597</v>
@@ -24309,67 +24303,67 @@
     </row>
     <row r="750" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>2590</v>
-      </c>
-      <c r="B750" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C750" s="3" t="b">
-        <v>1</v>
+        <v>2598</v>
+      </c>
+      <c r="B750" t="b">
+        <v>1</v>
+      </c>
+      <c r="C750" t="b">
+        <v>0</v>
       </c>
       <c r="E750" t="s">
-        <v>2594</v>
+        <v>2599</v>
       </c>
       <c r="F750" s="5" t="s">
-        <v>2593</v>
+        <v>2600</v>
       </c>
       <c r="G750" t="s">
-        <v>2598</v>
-      </c>
-    </row>
-    <row r="751" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A751" t="s">
-        <v>2591</v>
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="751" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A751" s="3" t="s">
+        <v>2613</v>
       </c>
       <c r="B751" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C751" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E751" t="s">
-        <v>2595</v>
+      <c r="E751" s="3" t="s">
+        <v>2615</v>
       </c>
       <c r="F751" s="5" t="s">
-        <v>2592</v>
-      </c>
-      <c r="G751" t="s">
-        <v>2599</v>
-      </c>
-    </row>
-    <row r="752" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A752" t="s">
-        <v>2600</v>
-      </c>
-      <c r="B752" t="b">
-        <v>1</v>
-      </c>
-      <c r="C752" t="b">
-        <v>0</v>
-      </c>
-      <c r="E752" t="s">
-        <v>2601</v>
+        <v>2617</v>
+      </c>
+      <c r="G751" s="3" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="752" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A752" s="3" t="s">
+        <v>2614</v>
+      </c>
+      <c r="B752" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C752" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E752" s="3" t="s">
+        <v>2616</v>
       </c>
       <c r="F752" s="5" t="s">
-        <v>2602</v>
-      </c>
-      <c r="G752" t="s">
-        <v>2603</v>
+        <v>2618</v>
+      </c>
+      <c r="G752" s="3" t="s">
+        <v>2620</v>
       </c>
     </row>
     <row r="753" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A753" s="3" t="s">
-        <v>2615</v>
+      <c r="A753" t="s">
+        <v>2632</v>
       </c>
       <c r="B753" s="3" t="b">
         <v>1</v>
@@ -24378,18 +24372,18 @@
         <v>1</v>
       </c>
       <c r="E753" s="3" t="s">
-        <v>2617</v>
+        <v>2641</v>
       </c>
       <c r="F753" s="5" t="s">
-        <v>2619</v>
+        <v>2642</v>
       </c>
       <c r="G753" s="3" t="s">
-        <v>2621</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="754" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A754" s="3" t="s">
-        <v>2616</v>
+      <c r="A754" t="s">
+        <v>2633</v>
       </c>
       <c r="B754" s="3" t="b">
         <v>1</v>
@@ -24398,17 +24392,17 @@
         <v>1</v>
       </c>
       <c r="E754" s="3" t="s">
-        <v>2618</v>
+        <v>2640</v>
       </c>
       <c r="F754" s="5" t="s">
-        <v>2620</v>
+        <v>2643</v>
       </c>
       <c r="G754" s="3" t="s">
-        <v>2622</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="755" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A755" t="s">
+      <c r="A755" s="3" t="s">
         <v>2634</v>
       </c>
       <c r="B755" s="3" t="b">
@@ -24418,7 +24412,7 @@
         <v>1</v>
       </c>
       <c r="E755" s="3" t="s">
-        <v>2643</v>
+        <v>2639</v>
       </c>
       <c r="F755" s="5" t="s">
         <v>2644</v>
@@ -24428,7 +24422,7 @@
       </c>
     </row>
     <row r="756" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A756" t="s">
+      <c r="A756" s="3" t="s">
         <v>2635</v>
       </c>
       <c r="B756" s="3" t="b">
@@ -24438,7 +24432,7 @@
         <v>1</v>
       </c>
       <c r="E756" s="3" t="s">
-        <v>2642</v>
+        <v>2638</v>
       </c>
       <c r="F756" s="5" t="s">
         <v>2645</v>
@@ -24447,8 +24441,8 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="757" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A757" s="3" t="s">
+    <row r="757" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A757" t="s">
         <v>2636</v>
       </c>
       <c r="B757" s="3" t="b">
@@ -24457,19 +24451,19 @@
       <c r="C757" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E757" s="3" t="s">
-        <v>2641</v>
+      <c r="E757" t="s">
+        <v>2637</v>
       </c>
       <c r="F757" s="5" t="s">
         <v>2646</v>
       </c>
-      <c r="G757" s="3" t="s">
+      <c r="G757" t="s">
         <v>2651</v>
       </c>
     </row>
-    <row r="758" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A758" s="3" t="s">
-        <v>2637</v>
+    <row r="758" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A758" t="s">
+        <v>2652</v>
       </c>
       <c r="B758" s="3" t="b">
         <v>1</v>
@@ -24477,59 +24471,59 @@
       <c r="C758" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E758" s="3" t="s">
-        <v>2640</v>
+      <c r="E758" t="s">
+        <v>2653</v>
       </c>
       <c r="F758" s="5" t="s">
-        <v>2647</v>
-      </c>
-      <c r="G758" s="3" t="s">
-        <v>2652</v>
+        <v>2654</v>
+      </c>
+      <c r="G758" t="s">
+        <v>2655</v>
       </c>
     </row>
     <row r="759" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>2638</v>
-      </c>
-      <c r="B759" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C759" s="3" t="b">
+        <v>2690</v>
+      </c>
+      <c r="B759" t="b">
+        <v>0</v>
+      </c>
+      <c r="C759" t="b">
         <v>1</v>
       </c>
       <c r="E759" t="s">
-        <v>2639</v>
+        <v>2691</v>
       </c>
       <c r="F759" s="5" t="s">
-        <v>2648</v>
-      </c>
-      <c r="G759" t="s">
-        <v>2653</v>
-      </c>
-    </row>
-    <row r="760" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A760" t="s">
-        <v>2654</v>
+        <v>2692</v>
+      </c>
+      <c r="G759" s="2" t="s">
+        <v>2693</v>
+      </c>
+    </row>
+    <row r="760" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A760" s="3" t="s">
+        <v>2694</v>
       </c>
       <c r="B760" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C760" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E760" t="s">
-        <v>2655</v>
+      <c r="E760" s="3" t="s">
+        <v>2695</v>
       </c>
       <c r="F760" s="5" t="s">
-        <v>2656</v>
-      </c>
-      <c r="G760" t="s">
-        <v>2657</v>
+        <v>2696</v>
+      </c>
+      <c r="G760" s="2" t="s">
+        <v>2697</v>
       </c>
     </row>
     <row r="761" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>2692</v>
+        <v>2698</v>
       </c>
       <c r="B761" t="b">
         <v>0</v>
@@ -24537,159 +24531,159 @@
       <c r="C761" t="b">
         <v>1</v>
       </c>
-      <c r="E761" t="s">
-        <v>2693</v>
+      <c r="E761" s="3" t="s">
+        <v>2699</v>
       </c>
       <c r="F761" s="5" t="s">
-        <v>2694</v>
+        <v>2700</v>
       </c>
       <c r="G761" s="2" t="s">
-        <v>2695</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="762" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A762" s="3" t="s">
-        <v>2696</v>
+        <v>2703</v>
       </c>
       <c r="B762" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C762" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E762" s="3" t="s">
-        <v>2697</v>
+        <v>2705</v>
       </c>
       <c r="F762" s="5" t="s">
-        <v>2698</v>
+        <v>2709</v>
       </c>
       <c r="G762" s="2" t="s">
-        <v>2699</v>
-      </c>
-    </row>
-    <row r="763" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A763" t="s">
-        <v>2700</v>
-      </c>
-      <c r="B763" t="b">
-        <v>0</v>
-      </c>
-      <c r="C763" t="b">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="763" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A763" s="3" t="s">
+        <v>2704</v>
+      </c>
+      <c r="B763" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C763" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E763" s="3" t="s">
-        <v>2701</v>
+        <v>2706</v>
       </c>
       <c r="F763" s="5" t="s">
+        <v>2708</v>
+      </c>
+      <c r="G763" s="2" t="s">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="764" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A764" t="s">
         <v>2702</v>
       </c>
-      <c r="G763" s="2" t="s">
-        <v>2703</v>
-      </c>
-    </row>
-    <row r="764" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A764" s="3" t="s">
-        <v>2705</v>
-      </c>
-      <c r="B764" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C764" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E764" s="3" t="s">
+      <c r="B764" t="b">
+        <v>1</v>
+      </c>
+      <c r="C764" t="b">
+        <v>1</v>
+      </c>
+      <c r="E764" t="s">
+        <v>501</v>
+      </c>
+      <c r="F764" s="5" t="s">
         <v>2707</v>
       </c>
-      <c r="F764" s="5" t="s">
+      <c r="G764" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="765" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A765" t="s">
         <v>2711</v>
       </c>
-      <c r="G764" s="2" t="s">
+      <c r="B765" t="b">
+        <v>0</v>
+      </c>
+      <c r="C765" t="b">
+        <v>1</v>
+      </c>
+      <c r="E765" t="s">
         <v>2712</v>
       </c>
-    </row>
-    <row r="765" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A765" s="3" t="s">
-        <v>2706</v>
-      </c>
-      <c r="B765" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C765" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E765" s="3" t="s">
-        <v>2708</v>
-      </c>
       <c r="F765" s="5" t="s">
-        <v>2710</v>
-      </c>
-      <c r="G765" s="2" t="s">
-        <v>2712</v>
+        <v>2713</v>
+      </c>
+      <c r="G765" t="s">
+        <v>2714</v>
       </c>
     </row>
     <row r="766" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>2704</v>
+        <v>2715</v>
       </c>
       <c r="B766" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C766" t="b">
         <v>1</v>
       </c>
       <c r="E766" t="s">
-        <v>501</v>
+        <v>2716</v>
       </c>
       <c r="F766" s="5" t="s">
-        <v>2709</v>
+        <v>2717</v>
       </c>
       <c r="G766" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="767" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A767" t="s">
-        <v>2713</v>
-      </c>
-      <c r="B767" t="b">
-        <v>0</v>
-      </c>
-      <c r="C767" t="b">
-        <v>1</v>
-      </c>
-      <c r="E767" t="s">
-        <v>2714</v>
+        <v>2718</v>
+      </c>
+    </row>
+    <row r="767" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A767" s="3" t="s">
+        <v>2719</v>
+      </c>
+      <c r="B767" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C767" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E767" s="3" t="s">
+        <v>2721</v>
       </c>
       <c r="F767" s="5" t="s">
-        <v>2715</v>
-      </c>
-      <c r="G767" t="s">
-        <v>2716</v>
-      </c>
-    </row>
-    <row r="768" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A768" t="s">
-        <v>2717</v>
-      </c>
-      <c r="B768" t="b">
-        <v>0</v>
-      </c>
-      <c r="C768" t="b">
-        <v>1</v>
-      </c>
-      <c r="E768" t="s">
-        <v>2718</v>
+        <v>2727</v>
+      </c>
+      <c r="G767" s="3" t="s">
+        <v>2733</v>
+      </c>
+    </row>
+    <row r="768" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A768" s="3" t="s">
+        <v>2720</v>
+      </c>
+      <c r="B768" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C768" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E768" s="3" t="s">
+        <v>2722</v>
       </c>
       <c r="F768" s="5" t="s">
-        <v>2719</v>
-      </c>
-      <c r="G768" t="s">
-        <v>2720</v>
-      </c>
-    </row>
-    <row r="769" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A769" s="3" t="s">
-        <v>2721</v>
+        <v>2726</v>
+      </c>
+      <c r="G768" s="3" t="s">
+        <v>2733</v>
+      </c>
+    </row>
+    <row r="769" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A769" t="s">
+        <v>2734</v>
       </c>
       <c r="B769" s="3" t="b">
         <v>1</v>
@@ -24697,19 +24691,19 @@
       <c r="C769" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E769" s="3" t="s">
+      <c r="E769" t="s">
         <v>2723</v>
       </c>
       <c r="F769" s="5" t="s">
-        <v>2729</v>
-      </c>
-      <c r="G769" s="3" t="s">
-        <v>2735</v>
+        <v>2728</v>
+      </c>
+      <c r="G769" t="s">
+        <v>2730</v>
       </c>
     </row>
     <row r="770" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A770" s="3" t="s">
-        <v>2722</v>
+        <v>2741</v>
       </c>
       <c r="B770" s="3" t="b">
         <v>1</v>
@@ -24718,133 +24712,133 @@
         <v>1</v>
       </c>
       <c r="E770" s="3" t="s">
-        <v>2724</v>
+        <v>2743</v>
       </c>
       <c r="F770" s="5" t="s">
-        <v>2728</v>
+        <v>2744</v>
       </c>
       <c r="G770" s="3" t="s">
-        <v>2735</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="771" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
+        <v>2735</v>
+      </c>
+      <c r="B771" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C771" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E771" t="s">
+        <v>2724</v>
+      </c>
+      <c r="F771" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="G771" t="s">
+        <v>2731</v>
+      </c>
+    </row>
+    <row r="772" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A772" t="s">
         <v>2736</v>
       </c>
-      <c r="B771" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C771" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E771" t="s">
+      <c r="B772" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C772" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E772" t="s">
         <v>2725</v>
       </c>
-      <c r="F771" s="5" t="s">
-        <v>2730</v>
-      </c>
-      <c r="G771" t="s">
+      <c r="F772" s="5" t="s">
+        <v>2729</v>
+      </c>
+      <c r="G772" t="s">
         <v>2732</v>
-      </c>
-    </row>
-    <row r="772" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A772" s="3" t="s">
-        <v>2743</v>
-      </c>
-      <c r="B772" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C772" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E772" s="3" t="s">
-        <v>2745</v>
-      </c>
-      <c r="F772" s="5" t="s">
-        <v>2746</v>
-      </c>
-      <c r="G772" s="3" t="s">
-        <v>2747</v>
       </c>
     </row>
     <row r="773" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
         <v>2737</v>
       </c>
-      <c r="B773" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C773" s="3" t="b">
+      <c r="B773" t="b">
+        <v>1</v>
+      </c>
+      <c r="C773" t="b">
         <v>1</v>
       </c>
       <c r="E773" t="s">
-        <v>2726</v>
+        <v>2738</v>
       </c>
       <c r="F773" s="5" t="s">
-        <v>678</v>
+        <v>2739</v>
       </c>
       <c r="G773" t="s">
-        <v>2733</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="774" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>2738</v>
-      </c>
-      <c r="B774" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C774" s="3" t="b">
+        <v>2746</v>
+      </c>
+      <c r="B774" t="b">
+        <v>0</v>
+      </c>
+      <c r="C774" t="b">
         <v>1</v>
       </c>
       <c r="E774" t="s">
-        <v>2727</v>
+        <v>2723</v>
       </c>
       <c r="F774" s="5" t="s">
-        <v>2731</v>
+        <v>2728</v>
       </c>
       <c r="G774" t="s">
-        <v>2734</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="775" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>2739</v>
-      </c>
-      <c r="B775" t="b">
-        <v>1</v>
-      </c>
-      <c r="C775" t="b">
+        <v>2747</v>
+      </c>
+      <c r="B775" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C775" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E775" t="s">
-        <v>2740</v>
+        <v>2750</v>
       </c>
       <c r="F775" s="5" t="s">
-        <v>2741</v>
+        <v>2752</v>
       </c>
       <c r="G775" t="s">
-        <v>2742</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="776" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
         <v>2748</v>
       </c>
-      <c r="B776" t="b">
-        <v>0</v>
-      </c>
-      <c r="C776" t="b">
+      <c r="B776" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C776" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E776" t="s">
-        <v>2725</v>
+        <v>2742</v>
       </c>
       <c r="F776" s="5" t="s">
-        <v>2730</v>
+        <v>2744</v>
       </c>
       <c r="G776" t="s">
-        <v>2732</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="777" spans="1:7" x14ac:dyDescent="0.25">
@@ -24858,113 +24852,113 @@
         <v>1</v>
       </c>
       <c r="E777" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="F777" s="5" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="G777" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
     </row>
     <row r="778" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>2750</v>
-      </c>
-      <c r="B778" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C778" s="3" t="b">
+        <v>2756</v>
+      </c>
+      <c r="B778" t="b">
+        <v>0</v>
+      </c>
+      <c r="C778" t="b">
         <v>1</v>
       </c>
       <c r="E778" t="s">
-        <v>2744</v>
+        <v>2757</v>
       </c>
       <c r="F778" s="5" t="s">
-        <v>2746</v>
+        <v>2758</v>
       </c>
       <c r="G778" t="s">
-        <v>2747</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="779" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>2751</v>
-      </c>
-      <c r="B779" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C779" s="3" t="b">
+        <v>2760</v>
+      </c>
+      <c r="B779" t="b">
+        <v>0</v>
+      </c>
+      <c r="C779" t="b">
         <v>1</v>
       </c>
       <c r="E779" t="s">
-        <v>2753</v>
+        <v>2761</v>
       </c>
       <c r="F779" s="5" t="s">
-        <v>2755</v>
-      </c>
-      <c r="G779" t="s">
-        <v>2757</v>
+        <v>2762</v>
+      </c>
+      <c r="G779" s="2" t="s">
+        <v>2763</v>
       </c>
     </row>
     <row r="780" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>2758</v>
+        <v>2764</v>
       </c>
       <c r="B780" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C780" t="b">
         <v>1</v>
       </c>
       <c r="E780" t="s">
-        <v>2759</v>
+        <v>2765</v>
       </c>
       <c r="F780" s="5" t="s">
-        <v>2760</v>
+        <v>2766</v>
       </c>
       <c r="G780" t="s">
-        <v>2761</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="781" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>2762</v>
-      </c>
-      <c r="B781" t="b">
-        <v>0</v>
-      </c>
-      <c r="C781" t="b">
+        <v>2767</v>
+      </c>
+      <c r="B781" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C781" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E781" t="s">
-        <v>2763</v>
+        <v>1</v>
       </c>
       <c r="F781" s="5" t="s">
-        <v>2764</v>
-      </c>
-      <c r="G781" s="2" t="s">
-        <v>2765</v>
+        <v>110</v>
+      </c>
+      <c r="G781" t="s">
+        <v>1705</v>
       </c>
     </row>
     <row r="782" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>2766</v>
-      </c>
-      <c r="B782" t="b">
-        <v>1</v>
-      </c>
-      <c r="C782" t="b">
+        <v>2768</v>
+      </c>
+      <c r="B782" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C782" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E782" t="s">
-        <v>2767</v>
+        <v>2685</v>
       </c>
       <c r="F782" s="5" t="s">
-        <v>2768</v>
+        <v>2687</v>
       </c>
       <c r="G782" t="s">
-        <v>2775</v>
+        <v>2689</v>
       </c>
     </row>
     <row r="783" spans="1:7" x14ac:dyDescent="0.25">
@@ -24978,13 +24972,13 @@
         <v>1</v>
       </c>
       <c r="E783" t="s">
-        <v>1</v>
+        <v>2771</v>
       </c>
       <c r="F783" s="5" t="s">
-        <v>110</v>
+        <v>2772</v>
       </c>
       <c r="G783" t="s">
-        <v>1705</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="784" spans="1:7" x14ac:dyDescent="0.25">
@@ -24998,18 +24992,18 @@
         <v>1</v>
       </c>
       <c r="E784" t="s">
-        <v>2687</v>
+        <v>803</v>
       </c>
       <c r="F784" s="5" t="s">
-        <v>2689</v>
+        <v>812</v>
       </c>
       <c r="G784" t="s">
-        <v>2691</v>
-      </c>
-    </row>
-    <row r="785" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A785" t="s">
-        <v>2771</v>
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="785" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A785" s="3" t="s">
+        <v>2776</v>
       </c>
       <c r="B785" s="3" t="b">
         <v>1</v>
@@ -25017,19 +25011,19 @@
       <c r="C785" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E785" t="s">
-        <v>2773</v>
+      <c r="E785" s="3" t="s">
+        <v>377</v>
       </c>
       <c r="F785" s="5" t="s">
-        <v>2774</v>
-      </c>
-      <c r="G785" t="s">
-        <v>2775</v>
+        <v>2779</v>
+      </c>
+      <c r="G785" s="3" t="s">
+        <v>1323</v>
       </c>
     </row>
     <row r="786" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>2772</v>
+        <v>2774</v>
       </c>
       <c r="B786" s="3" t="b">
         <v>1</v>
@@ -25038,77 +25032,37 @@
         <v>1</v>
       </c>
       <c r="E786" t="s">
-        <v>803</v>
+        <v>2685</v>
       </c>
       <c r="F786" s="5" t="s">
-        <v>812</v>
+        <v>2687</v>
       </c>
       <c r="G786" t="s">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="787" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A787" s="3" t="s">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="787" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A787" t="s">
+        <v>2775</v>
+      </c>
+      <c r="B787" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C787" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E787" t="s">
+        <v>2777</v>
+      </c>
+      <c r="F787" s="5" t="s">
         <v>2778</v>
       </c>
-      <c r="B787" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C787" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E787" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F787" s="5" t="s">
-        <v>2781</v>
-      </c>
-      <c r="G787" s="3" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="788" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A788" t="s">
-        <v>2776</v>
-      </c>
-      <c r="B788" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C788" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E788" t="s">
-        <v>2687</v>
-      </c>
-      <c r="F788" s="5" t="s">
-        <v>2689</v>
-      </c>
-      <c r="G788" t="s">
-        <v>2691</v>
-      </c>
-    </row>
-    <row r="789" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A789" t="s">
-        <v>2777</v>
-      </c>
-      <c r="B789" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C789" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E789" t="s">
-        <v>2779</v>
-      </c>
-      <c r="F789" s="5" t="s">
+      <c r="G787" t="s">
         <v>2780</v>
       </c>
-      <c r="G789" t="s">
-        <v>2782</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G758" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G756" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on signatures framework, implemented other rule types
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7019BEAD-DC0C-4F9D-B044-444318BB24F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11545C4-8EBB-40A0-81E6-F0833B94BE2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3194" uniqueCount="2811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="2818">
   <si>
     <t>Key</t>
   </si>
@@ -8390,60 +8390,15 @@
     <t>RequestedBy</t>
   </si>
   <si>
-    <t>ApprovedBy</t>
-  </si>
-  <si>
     <t>CompletedBy</t>
   </si>
   <si>
     <t>ReviewedBy</t>
   </si>
   <si>
-    <t>الطلب من قبل</t>
-  </si>
-  <si>
     <t>إكمال من قبل</t>
   </si>
   <si>
-    <t>Approve</t>
-  </si>
-  <si>
-    <t>Reject</t>
-  </si>
-  <si>
-    <t>Request</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>طلب</t>
-  </si>
-  <si>
-    <t>إعتماد</t>
-  </si>
-  <si>
-    <t>رفض</t>
-  </si>
-  <si>
-    <t>تعذر الإكمال</t>
-  </si>
-  <si>
-    <t>صحيح</t>
-  </si>
-  <si>
-    <t>غير صحيح</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
     <t>مراجعة من قبل</t>
   </si>
   <si>
@@ -8459,9 +8414,6 @@
     <t>اعتماد من قبل</t>
   </si>
   <si>
-    <t>Requested by</t>
-  </si>
-  <si>
     <t>AreYouSureYouWantToDeleteYourSignature</t>
   </si>
   <si>
@@ -8469,6 +8421,75 @@
   </si>
   <si>
     <t>سيتم حذف توقيعك، هل أنت متأكد؟</t>
+  </si>
+  <si>
+    <t>Stamps</t>
+  </si>
+  <si>
+    <t>الأختام</t>
+  </si>
+  <si>
+    <t>Request by</t>
+  </si>
+  <si>
+    <t>طلب من قبل</t>
+  </si>
+  <si>
+    <t>AuthorizedBy</t>
+  </si>
+  <si>
+    <t>Requester</t>
+  </si>
+  <si>
+    <t>Authorizer</t>
+  </si>
+  <si>
+    <t>Completer</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>المتقدم بالطلب</t>
+  </si>
+  <si>
+    <t>المُكمّل</t>
+  </si>
+  <si>
+    <t>المُعتمِد</t>
+  </si>
+  <si>
+    <t>المُراجِع</t>
+  </si>
+  <si>
+    <t>邮票</t>
+  </si>
+  <si>
+    <t>通过请求</t>
+  </si>
+  <si>
+    <t>通过批准</t>
+  </si>
+  <si>
+    <t>通过完成</t>
+  </si>
+  <si>
+    <t>回顾</t>
+  </si>
+  <si>
+    <t>你确定要删除您的签名？</t>
+  </si>
+  <si>
+    <t>请求者</t>
+  </si>
+  <si>
+    <t>授权</t>
+  </si>
+  <si>
+    <t>完成者</t>
+  </si>
+  <si>
+    <t>评论家</t>
   </si>
 </sst>
 </file>
@@ -8865,12 +8886,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G800"/>
+  <dimension ref="A1:G797"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A766" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A765" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F799" sqref="F799"/>
+      <selection pane="bottomLeft" activeCell="E782" sqref="E782"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25138,44 +25159,53 @@
       <c r="F787" s="5" t="s">
         <v>2267</v>
       </c>
-    </row>
-    <row r="788" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A788" t="s">
-        <v>2783</v>
-      </c>
-      <c r="B788" t="b">
+      <c r="G787" s="3" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="788" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A788" s="3" t="s">
+        <v>2795</v>
+      </c>
+      <c r="B788" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C788" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E788" t="s">
-        <v>2807</v>
+      <c r="E788" s="3" t="s">
+        <v>2795</v>
       </c>
       <c r="F788" s="5" t="s">
-        <v>2787</v>
+        <v>2796</v>
+      </c>
+      <c r="G788" s="3" t="s">
+        <v>2808</v>
       </c>
     </row>
     <row r="789" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>2784</v>
-      </c>
-      <c r="B789" s="3" t="b">
+        <v>2783</v>
+      </c>
+      <c r="B789" t="b">
         <v>0</v>
       </c>
       <c r="C789" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E789" t="s">
-        <v>2804</v>
+        <v>2797</v>
       </c>
       <c r="F789" s="5" t="s">
-        <v>2806</v>
+        <v>2798</v>
+      </c>
+      <c r="G789" t="s">
+        <v>2809</v>
       </c>
     </row>
     <row r="790" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>2785</v>
+        <v>2799</v>
       </c>
       <c r="B790" s="3" t="b">
         <v>0</v>
@@ -25184,66 +25214,78 @@
         <v>1</v>
       </c>
       <c r="E790" t="s">
-        <v>2805</v>
+        <v>2789</v>
       </c>
       <c r="F790" s="5" t="s">
-        <v>2788</v>
+        <v>2791</v>
+      </c>
+      <c r="G790" t="s">
+        <v>2810</v>
       </c>
     </row>
     <row r="791" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
+        <v>2784</v>
+      </c>
+      <c r="B791" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C791" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E791" t="s">
+        <v>2790</v>
+      </c>
+      <c r="F791" s="5" t="s">
         <v>2786</v>
       </c>
-      <c r="B791" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C791" t="b">
-        <v>1</v>
-      </c>
-      <c r="E791" t="s">
-        <v>2803</v>
-      </c>
-      <c r="F791" s="5" t="s">
-        <v>2802</v>
+      <c r="G791" t="s">
+        <v>2811</v>
       </c>
     </row>
     <row r="792" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>2791</v>
-      </c>
-      <c r="B792" t="b">
-        <v>0</v>
-      </c>
-      <c r="C792" s="3" t="b">
+        <v>2785</v>
+      </c>
+      <c r="B792" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C792" t="b">
         <v>1</v>
       </c>
       <c r="E792" t="s">
-        <v>2791</v>
+        <v>2788</v>
       </c>
       <c r="F792" s="5" t="s">
-        <v>2795</v>
+        <v>2787</v>
+      </c>
+      <c r="G792" t="s">
+        <v>2812</v>
       </c>
     </row>
     <row r="793" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>1625</v>
-      </c>
-      <c r="B793" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C793" s="3" t="b">
+        <v>2792</v>
+      </c>
+      <c r="B793" t="b">
+        <v>0</v>
+      </c>
+      <c r="C793" t="b">
         <v>1</v>
       </c>
       <c r="E793" t="s">
-        <v>1625</v>
+        <v>2793</v>
       </c>
       <c r="F793" s="5" t="s">
-        <v>56</v>
+        <v>2794</v>
+      </c>
+      <c r="G793" t="s">
+        <v>2813</v>
       </c>
     </row>
     <row r="794" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>2789</v>
+        <v>2800</v>
       </c>
       <c r="B794" s="3" t="b">
         <v>0</v>
@@ -25252,15 +25294,18 @@
         <v>1</v>
       </c>
       <c r="E794" t="s">
-        <v>2789</v>
+        <v>2800</v>
       </c>
       <c r="F794" s="5" t="s">
-        <v>2796</v>
+        <v>2804</v>
+      </c>
+      <c r="G794" t="s">
+        <v>2814</v>
       </c>
     </row>
     <row r="795" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>2790</v>
+        <v>2801</v>
       </c>
       <c r="B795" s="3" t="b">
         <v>0</v>
@@ -25269,15 +25314,18 @@
         <v>1</v>
       </c>
       <c r="E795" t="s">
-        <v>2790</v>
+        <v>2801</v>
       </c>
       <c r="F795" s="5" t="s">
-        <v>2797</v>
+        <v>2806</v>
+      </c>
+      <c r="G795" t="s">
+        <v>2815</v>
       </c>
     </row>
     <row r="796" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>2792</v>
+        <v>2802</v>
       </c>
       <c r="B796" s="3" t="b">
         <v>0</v>
@@ -25285,16 +25333,19 @@
       <c r="C796" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E796" s="3" t="s">
-        <v>2792</v>
+      <c r="E796" t="s">
+        <v>2802</v>
       </c>
       <c r="F796" s="5" t="s">
-        <v>1644</v>
+        <v>2805</v>
+      </c>
+      <c r="G796" t="s">
+        <v>2816</v>
       </c>
     </row>
     <row r="797" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>2793</v>
+        <v>2803</v>
       </c>
       <c r="B797" s="3" t="b">
         <v>0</v>
@@ -25302,62 +25353,14 @@
       <c r="C797" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E797" s="3" t="s">
-        <v>2793</v>
+      <c r="E797" t="s">
+        <v>2803</v>
       </c>
       <c r="F797" s="5" t="s">
-        <v>2798</v>
-      </c>
-    </row>
-    <row r="798" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A798" t="s">
-        <v>2801</v>
-      </c>
-      <c r="B798" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C798" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E798" s="3" t="s">
-        <v>2794</v>
-      </c>
-      <c r="F798" s="5" t="s">
-        <v>2799</v>
-      </c>
-    </row>
-    <row r="799" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A799" t="s">
-        <v>1631</v>
-      </c>
-      <c r="B799" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C799" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E799" s="3" t="s">
-        <v>1631</v>
-      </c>
-      <c r="F799" s="5" t="s">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="800" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A800" t="s">
-        <v>2808</v>
-      </c>
-      <c r="B800" t="b">
-        <v>0</v>
-      </c>
-      <c r="C800" t="b">
-        <v>1</v>
-      </c>
-      <c r="E800" t="s">
-        <v>2809</v>
-      </c>
-      <c r="F800" s="5" t="s">
-        <v>2810</v>
+        <v>2807</v>
+      </c>
+      <c r="G797" t="s">
+        <v>2817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on signatures framework
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11545C4-8EBB-40A0-81E6-F0833B94BE2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B8F588-C5D7-477C-B5F4-48788915626B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$755</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$757</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="2818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3212" uniqueCount="2831">
   <si>
     <t>Key</t>
   </si>
@@ -8396,24 +8396,12 @@
     <t>ReviewedBy</t>
   </si>
   <si>
-    <t>إكمال من قبل</t>
-  </si>
-  <si>
-    <t>مراجعة من قبل</t>
-  </si>
-  <si>
     <t>Review by</t>
   </si>
   <si>
-    <t>Approval by</t>
-  </si>
-  <si>
     <t>Completion by</t>
   </si>
   <si>
-    <t>اعتماد من قبل</t>
-  </si>
-  <si>
     <t>AreYouSureYouWantToDeleteYourSignature</t>
   </si>
   <si>
@@ -8432,9 +8420,6 @@
     <t>Request by</t>
   </si>
   <si>
-    <t>طلب من قبل</t>
-  </si>
-  <si>
     <t>AuthorizedBy</t>
   </si>
   <si>
@@ -8490,6 +8475,60 @@
   </si>
   <si>
     <t>评论家</t>
+  </si>
+  <si>
+    <t>طلب من</t>
+  </si>
+  <si>
+    <t>اعتماد من</t>
+  </si>
+  <si>
+    <t>إكمال من</t>
+  </si>
+  <si>
+    <t>مراجعة من</t>
+  </si>
+  <si>
+    <t>Authorization by</t>
+  </si>
+  <si>
+    <t>AdditionalInformation</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>معلومات إضافية</t>
+  </si>
+  <si>
+    <t>Signature_ReasonDetails</t>
+  </si>
+  <si>
+    <t>Signature_Reason</t>
+  </si>
+  <si>
+    <t>Reason Details</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>تفصيل السبب</t>
+  </si>
+  <si>
+    <t>详细原因</t>
+  </si>
+  <si>
+    <t>原因</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>موافقة</t>
+  </si>
+  <si>
+    <t>附加信息</t>
   </si>
 </sst>
 </file>
@@ -8886,12 +8925,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G797"/>
+  <dimension ref="A1:G801"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A765" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A778" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E782" sqref="E782"/>
+      <selection pane="bottomLeft" activeCell="G800" sqref="G800:G801"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23699,52 +23738,49 @@
         <v>2266</v>
       </c>
     </row>
-    <row r="715" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A715" t="s">
-        <v>2268</v>
-      </c>
-      <c r="B715" t="b">
-        <v>0</v>
-      </c>
-      <c r="C715" t="b">
-        <v>1</v>
-      </c>
-      <c r="D715" t="s">
-        <v>2269</v>
-      </c>
-      <c r="E715" t="s">
-        <v>2271</v>
+    <row r="715" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A715" s="3" t="s">
+        <v>2821</v>
+      </c>
+      <c r="B715" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C715" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E715" s="3" t="s">
+        <v>2823</v>
       </c>
       <c r="F715" s="5" t="s">
-        <v>2270</v>
+        <v>2825</v>
       </c>
       <c r="G715" s="3" t="s">
-        <v>2276</v>
-      </c>
-    </row>
-    <row r="716" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A716" t="s">
-        <v>2300</v>
-      </c>
-      <c r="B716" t="b">
-        <v>0</v>
-      </c>
-      <c r="C716" t="b">
-        <v>1</v>
-      </c>
-      <c r="E716" t="s">
-        <v>2301</v>
+        <v>2826</v>
+      </c>
+    </row>
+    <row r="716" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A716" s="3" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B716" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C716" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E716" s="3" t="s">
+        <v>2824</v>
       </c>
       <c r="F716" s="5" t="s">
-        <v>2317</v>
-      </c>
-      <c r="G716" t="s">
-        <v>2312</v>
+        <v>2335</v>
+      </c>
+      <c r="G716" s="3" t="s">
+        <v>2827</v>
       </c>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>2302</v>
+        <v>2268</v>
       </c>
       <c r="B717" t="b">
         <v>0</v>
@@ -23752,39 +23788,42 @@
       <c r="C717" t="b">
         <v>1</v>
       </c>
+      <c r="D717" t="s">
+        <v>2269</v>
+      </c>
       <c r="E717" t="s">
-        <v>2318</v>
+        <v>2271</v>
       </c>
       <c r="F717" s="5" t="s">
-        <v>2305</v>
-      </c>
-      <c r="G717" t="s">
-        <v>2313</v>
-      </c>
-    </row>
-    <row r="718" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A718" s="3" t="s">
-        <v>2308</v>
-      </c>
-      <c r="B718" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C718" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E718" s="3" t="s">
-        <v>2309</v>
+        <v>2270</v>
+      </c>
+      <c r="G717" s="3" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="718" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A718" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B718" t="b">
+        <v>0</v>
+      </c>
+      <c r="C718" t="b">
+        <v>1</v>
+      </c>
+      <c r="E718" t="s">
+        <v>2301</v>
       </c>
       <c r="F718" s="5" t="s">
-        <v>2310</v>
-      </c>
-      <c r="G718" s="3" t="s">
-        <v>2314</v>
+        <v>2317</v>
+      </c>
+      <c r="G718" t="s">
+        <v>2312</v>
       </c>
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="B719" t="b">
         <v>0</v>
@@ -23793,38 +23832,38 @@
         <v>1</v>
       </c>
       <c r="E719" t="s">
-        <v>2303</v>
+        <v>2318</v>
       </c>
       <c r="F719" s="5" t="s">
-        <v>2304</v>
+        <v>2305</v>
       </c>
       <c r="G719" t="s">
-        <v>2315</v>
-      </c>
-    </row>
-    <row r="720" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A720" t="s">
-        <v>2307</v>
-      </c>
-      <c r="B720" t="b">
-        <v>0</v>
-      </c>
-      <c r="C720" t="b">
-        <v>1</v>
-      </c>
-      <c r="E720" t="s">
-        <v>2306</v>
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="720" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A720" s="3" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B720" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C720" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E720" s="3" t="s">
+        <v>2309</v>
       </c>
       <c r="F720" s="5" t="s">
-        <v>2311</v>
-      </c>
-      <c r="G720" t="s">
-        <v>2316</v>
+        <v>2310</v>
+      </c>
+      <c r="G720" s="3" t="s">
+        <v>2314</v>
       </c>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>496</v>
+        <v>2303</v>
       </c>
       <c r="B721" t="b">
         <v>0</v>
@@ -23833,18 +23872,18 @@
         <v>1</v>
       </c>
       <c r="E721" t="s">
-        <v>496</v>
+        <v>2303</v>
       </c>
       <c r="F721" s="5" t="s">
-        <v>495</v>
+        <v>2304</v>
       </c>
       <c r="G721" t="s">
-        <v>1365</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>2332</v>
+        <v>2307</v>
       </c>
       <c r="B722" t="b">
         <v>0</v>
@@ -23853,18 +23892,18 @@
         <v>1</v>
       </c>
       <c r="E722" t="s">
-        <v>2332</v>
+        <v>2306</v>
       </c>
       <c r="F722" s="5" t="s">
-        <v>2333</v>
+        <v>2311</v>
       </c>
       <c r="G722" t="s">
-        <v>2343</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>2341</v>
+        <v>496</v>
       </c>
       <c r="B723" t="b">
         <v>0</v>
@@ -23873,78 +23912,78 @@
         <v>1</v>
       </c>
       <c r="E723" t="s">
-        <v>2342</v>
+        <v>496</v>
       </c>
       <c r="F723" s="5" t="s">
-        <v>2345</v>
+        <v>495</v>
       </c>
       <c r="G723" t="s">
-        <v>2344</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>2405</v>
+        <v>2332</v>
       </c>
       <c r="B724" t="b">
-        <v>1</v>
-      </c>
-      <c r="C724" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C724" t="b">
         <v>1</v>
       </c>
       <c r="E724" t="s">
-        <v>2346</v>
+        <v>2332</v>
       </c>
       <c r="F724" s="5" t="s">
-        <v>2353</v>
+        <v>2333</v>
       </c>
       <c r="G724" t="s">
-        <v>2360</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>2406</v>
-      </c>
-      <c r="B725" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C725" s="3" t="b">
+        <v>2341</v>
+      </c>
+      <c r="B725" t="b">
+        <v>0</v>
+      </c>
+      <c r="C725" t="b">
         <v>1</v>
       </c>
       <c r="E725" t="s">
-        <v>2347</v>
+        <v>2342</v>
       </c>
       <c r="F725" s="5" t="s">
-        <v>2354</v>
+        <v>2345</v>
       </c>
       <c r="G725" t="s">
-        <v>2366</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>2407</v>
-      </c>
-      <c r="B726" s="3" t="b">
+        <v>2405</v>
+      </c>
+      <c r="B726" t="b">
         <v>1</v>
       </c>
       <c r="C726" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E726" t="s">
-        <v>2348</v>
+        <v>2346</v>
       </c>
       <c r="F726" s="5" t="s">
-        <v>2355</v>
+        <v>2353</v>
       </c>
       <c r="G726" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>2408</v>
+        <v>2406</v>
       </c>
       <c r="B727" s="3" t="b">
         <v>1</v>
@@ -23953,18 +23992,18 @@
         <v>1</v>
       </c>
       <c r="E727" t="s">
-        <v>2350</v>
+        <v>2347</v>
       </c>
       <c r="F727" s="5" t="s">
-        <v>2357</v>
+        <v>2354</v>
       </c>
       <c r="G727" t="s">
-        <v>2362</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>2409</v>
+        <v>2407</v>
       </c>
       <c r="B728" s="3" t="b">
         <v>1</v>
@@ -23973,18 +24012,18 @@
         <v>1</v>
       </c>
       <c r="E728" t="s">
-        <v>2351</v>
+        <v>2348</v>
       </c>
       <c r="F728" s="5" t="s">
-        <v>2358</v>
+        <v>2355</v>
       </c>
       <c r="G728" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>2410</v>
+        <v>2408</v>
       </c>
       <c r="B729" s="3" t="b">
         <v>1</v>
@@ -23993,18 +24032,18 @@
         <v>1</v>
       </c>
       <c r="E729" t="s">
-        <v>2349</v>
+        <v>2350</v>
       </c>
       <c r="F729" s="5" t="s">
-        <v>2356</v>
+        <v>2357</v>
       </c>
       <c r="G729" t="s">
-        <v>2364</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>2411</v>
+        <v>2409</v>
       </c>
       <c r="B730" s="3" t="b">
         <v>1</v>
@@ -24013,58 +24052,58 @@
         <v>1</v>
       </c>
       <c r="E730" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="F730" s="5" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="G730" t="s">
-        <v>2365</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>2427</v>
-      </c>
-      <c r="B731" t="b">
-        <v>1</v>
-      </c>
-      <c r="C731" t="b">
+        <v>2410</v>
+      </c>
+      <c r="B731" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C731" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E731" t="s">
-        <v>2429</v>
+        <v>2349</v>
       </c>
       <c r="F731" s="5" t="s">
-        <v>2431</v>
+        <v>2356</v>
       </c>
       <c r="G731" t="s">
-        <v>2433</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="732" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>2428</v>
-      </c>
-      <c r="B732" t="b">
-        <v>1</v>
-      </c>
-      <c r="C732" t="b">
+        <v>2411</v>
+      </c>
+      <c r="B732" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C732" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E732" t="s">
-        <v>2430</v>
+        <v>2352</v>
       </c>
       <c r="F732" s="5" t="s">
-        <v>2432</v>
+        <v>2359</v>
       </c>
       <c r="G732" t="s">
-        <v>2434</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>2435</v>
+        <v>2427</v>
       </c>
       <c r="B733" t="b">
         <v>1</v>
@@ -24073,18 +24112,18 @@
         <v>1</v>
       </c>
       <c r="E733" t="s">
-        <v>2436</v>
+        <v>2429</v>
       </c>
       <c r="F733" s="5" t="s">
-        <v>2437</v>
+        <v>2431</v>
       </c>
       <c r="G733" t="s">
-        <v>2440</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>2438</v>
+        <v>2428</v>
       </c>
       <c r="B734" t="b">
         <v>1</v>
@@ -24093,58 +24132,58 @@
         <v>1</v>
       </c>
       <c r="E734" t="s">
-        <v>2451</v>
+        <v>2430</v>
       </c>
       <c r="F734" s="5" t="s">
-        <v>2439</v>
+        <v>2432</v>
       </c>
       <c r="G734" t="s">
-        <v>2441</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>2448</v>
+        <v>2435</v>
       </c>
       <c r="B735" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C735" t="b">
         <v>1</v>
       </c>
       <c r="E735" t="s">
-        <v>2449</v>
+        <v>2436</v>
       </c>
       <c r="F735" s="5" t="s">
-        <v>2450</v>
+        <v>2437</v>
       </c>
       <c r="G735" t="s">
-        <v>2426</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="736" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>2474</v>
+        <v>2438</v>
       </c>
       <c r="B736" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C736" t="b">
         <v>1</v>
       </c>
       <c r="E736" t="s">
-        <v>2474</v>
+        <v>2451</v>
       </c>
       <c r="F736" s="5" t="s">
-        <v>1075</v>
+        <v>2439</v>
       </c>
       <c r="G736" t="s">
-        <v>2475</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>2528</v>
+        <v>2448</v>
       </c>
       <c r="B737" t="b">
         <v>0</v>
@@ -24153,179 +24192,178 @@
         <v>1</v>
       </c>
       <c r="E737" t="s">
-        <v>2528</v>
+        <v>2449</v>
       </c>
       <c r="F737" s="5" t="s">
-        <v>2529</v>
+        <v>2450</v>
       </c>
       <c r="G737" t="s">
-        <v>2532</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="738" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
+        <v>2474</v>
+      </c>
+      <c r="B738" t="b">
+        <v>0</v>
+      </c>
+      <c r="C738" t="b">
+        <v>1</v>
+      </c>
+      <c r="E738" t="s">
+        <v>2474</v>
+      </c>
+      <c r="F738" s="5" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G738" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="739" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A739" t="s">
+        <v>2528</v>
+      </c>
+      <c r="B739" t="b">
+        <v>0</v>
+      </c>
+      <c r="C739" t="b">
+        <v>1</v>
+      </c>
+      <c r="E739" t="s">
+        <v>2528</v>
+      </c>
+      <c r="F739" s="5" t="s">
+        <v>2529</v>
+      </c>
+      <c r="G739" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="740" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A740" t="s">
         <v>2530</v>
       </c>
-      <c r="B738" t="b">
-        <v>0</v>
-      </c>
-      <c r="C738" t="b">
-        <v>1</v>
-      </c>
-      <c r="E738" t="s">
+      <c r="B740" t="b">
+        <v>0</v>
+      </c>
+      <c r="C740" t="b">
+        <v>1</v>
+      </c>
+      <c r="E740" t="s">
         <v>2530</v>
       </c>
-      <c r="F738" s="5" t="s">
+      <c r="F740" s="5" t="s">
         <v>2531</v>
       </c>
-      <c r="G738" t="s">
+      <c r="G740" t="s">
         <v>2533</v>
       </c>
     </row>
-    <row r="739" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A739" s="3" t="s">
+    <row r="741" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A741" s="3" t="s">
         <v>2553</v>
       </c>
-      <c r="B739" t="b">
-        <v>1</v>
-      </c>
-      <c r="C739" t="b">
-        <v>1</v>
-      </c>
-      <c r="E739" t="s">
+      <c r="B741" t="b">
+        <v>1</v>
+      </c>
+      <c r="C741" t="b">
+        <v>1</v>
+      </c>
+      <c r="E741" t="s">
         <v>2554</v>
       </c>
-      <c r="F739" s="5" t="s">
+      <c r="F741" s="5" t="s">
         <v>1678</v>
       </c>
-      <c r="G739" t="s">
+      <c r="G741" t="s">
         <v>2555</v>
       </c>
     </row>
-    <row r="740" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A740" s="3" t="s">
+    <row r="742" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A742" s="3" t="s">
         <v>2577</v>
       </c>
-      <c r="B740" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C740" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E740" s="3" t="s">
+      <c r="B742" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C742" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E742" s="3" t="s">
         <v>2578</v>
       </c>
-      <c r="F740" s="5" t="s">
+      <c r="F742" s="5" t="s">
         <v>2579</v>
       </c>
-      <c r="G740" s="3" t="s">
+      <c r="G742" s="3" t="s">
         <v>2580</v>
-      </c>
-    </row>
-    <row r="741" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A741" t="s">
-        <v>2556</v>
-      </c>
-      <c r="B741" t="b">
-        <v>1</v>
-      </c>
-      <c r="C741" t="b">
-        <v>0</v>
-      </c>
-      <c r="E741" t="s">
-        <v>2564</v>
-      </c>
-      <c r="F741" s="5" t="s">
-        <v>2565</v>
-      </c>
-      <c r="G741" t="s">
-        <v>2567</v>
-      </c>
-    </row>
-    <row r="742" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A742" t="s">
-        <v>2558</v>
-      </c>
-      <c r="B742" t="b">
-        <v>1</v>
-      </c>
-      <c r="C742" t="b">
-        <v>0</v>
-      </c>
-      <c r="E742" t="s">
-        <v>2557</v>
-      </c>
-      <c r="F742" s="5" t="s">
-        <v>2566</v>
-      </c>
-      <c r="G742" t="s">
-        <v>2568</v>
       </c>
     </row>
     <row r="743" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>2570</v>
+        <v>2556</v>
       </c>
       <c r="B743" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C743" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E743" t="s">
-        <v>2570</v>
+        <v>2564</v>
       </c>
       <c r="F743" s="5" t="s">
-        <v>2563</v>
+        <v>2565</v>
       </c>
       <c r="G743" t="s">
-        <v>2569</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="744" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>2571</v>
+        <v>2558</v>
       </c>
       <c r="B744" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C744" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E744" t="s">
-        <v>2571</v>
+        <v>2557</v>
       </c>
       <c r="F744" s="5" t="s">
-        <v>2572</v>
+        <v>2566</v>
       </c>
       <c r="G744" t="s">
-        <v>2593</v>
+        <v>2568</v>
       </c>
     </row>
     <row r="745" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A745" s="3" t="s">
-        <v>2576</v>
-      </c>
-      <c r="B745" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C745" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D745" s="3"/>
-      <c r="E745" s="3" t="s">
-        <v>2573</v>
+      <c r="A745" t="s">
+        <v>2570</v>
+      </c>
+      <c r="B745" t="b">
+        <v>0</v>
+      </c>
+      <c r="C745" t="b">
+        <v>1</v>
+      </c>
+      <c r="E745" t="s">
+        <v>2570</v>
       </c>
       <c r="F745" s="5" t="s">
-        <v>2574</v>
-      </c>
-      <c r="G745" s="3" t="s">
-        <v>2575</v>
+        <v>2563</v>
+      </c>
+      <c r="G745" t="s">
+        <v>2569</v>
       </c>
     </row>
     <row r="746" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>2581</v>
+        <v>2571</v>
       </c>
       <c r="B746" t="b">
         <v>0</v>
@@ -24334,18 +24372,18 @@
         <v>1</v>
       </c>
       <c r="E746" t="s">
-        <v>2582</v>
+        <v>2571</v>
       </c>
       <c r="F746" s="5" t="s">
-        <v>2583</v>
+        <v>2572</v>
       </c>
       <c r="G746" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="747" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A747" t="s">
-        <v>2587</v>
+      <c r="A747" s="3" t="s">
+        <v>2576</v>
       </c>
       <c r="B747" s="3" t="b">
         <v>0</v>
@@ -24353,259 +24391,260 @@
       <c r="C747" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E747" t="s">
-        <v>2591</v>
+      <c r="D747" s="3"/>
+      <c r="E747" s="3" t="s">
+        <v>2573</v>
       </c>
       <c r="F747" s="5" t="s">
-        <v>2590</v>
-      </c>
-      <c r="G747" t="s">
-        <v>2595</v>
+        <v>2574</v>
+      </c>
+      <c r="G747" s="3" t="s">
+        <v>2575</v>
       </c>
     </row>
     <row r="748" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>2588</v>
-      </c>
-      <c r="B748" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C748" s="3" t="b">
+        <v>2581</v>
+      </c>
+      <c r="B748" t="b">
+        <v>0</v>
+      </c>
+      <c r="C748" t="b">
         <v>1</v>
       </c>
       <c r="E748" t="s">
-        <v>2592</v>
+        <v>2582</v>
       </c>
       <c r="F748" s="5" t="s">
-        <v>2589</v>
+        <v>2583</v>
       </c>
       <c r="G748" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
+        <v>2587</v>
+      </c>
+      <c r="B749" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C749" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E749" t="s">
+        <v>2591</v>
+      </c>
+      <c r="F749" s="5" t="s">
+        <v>2590</v>
+      </c>
+      <c r="G749" t="s">
+        <v>2595</v>
+      </c>
+    </row>
+    <row r="750" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A750" t="s">
+        <v>2588</v>
+      </c>
+      <c r="B750" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C750" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E750" t="s">
+        <v>2592</v>
+      </c>
+      <c r="F750" s="5" t="s">
+        <v>2589</v>
+      </c>
+      <c r="G750" t="s">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="751" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A751" t="s">
         <v>2597</v>
       </c>
-      <c r="B749" t="b">
-        <v>1</v>
-      </c>
-      <c r="C749" t="b">
-        <v>0</v>
-      </c>
-      <c r="E749" t="s">
+      <c r="B751" t="b">
+        <v>1</v>
+      </c>
+      <c r="C751" t="b">
+        <v>0</v>
+      </c>
+      <c r="E751" t="s">
         <v>2598</v>
       </c>
-      <c r="F749" s="5" t="s">
+      <c r="F751" s="5" t="s">
         <v>2599</v>
       </c>
-      <c r="G749" t="s">
+      <c r="G751" t="s">
         <v>2600</v>
       </c>
     </row>
-    <row r="750" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A750" s="3" t="s">
+    <row r="752" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A752" s="3" t="s">
         <v>2612</v>
       </c>
-      <c r="B750" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C750" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E750" s="3" t="s">
+      <c r="B752" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C752" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E752" s="3" t="s">
         <v>2614</v>
       </c>
-      <c r="F750" s="5" t="s">
+      <c r="F752" s="5" t="s">
         <v>2616</v>
       </c>
-      <c r="G750" s="3" t="s">
+      <c r="G752" s="3" t="s">
         <v>2618</v>
       </c>
     </row>
-    <row r="751" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A751" s="3" t="s">
+    <row r="753" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A753" s="3" t="s">
         <v>2613</v>
       </c>
-      <c r="B751" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C751" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E751" s="3" t="s">
+      <c r="B753" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C753" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E753" s="3" t="s">
         <v>2615</v>
       </c>
-      <c r="F751" s="5" t="s">
+      <c r="F753" s="5" t="s">
         <v>2617</v>
       </c>
-      <c r="G751" s="3" t="s">
+      <c r="G753" s="3" t="s">
         <v>2619</v>
       </c>
     </row>
-    <row r="752" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A752" t="s">
+    <row r="754" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A754" t="s">
         <v>2631</v>
       </c>
-      <c r="B752" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C752" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E752" s="3" t="s">
+      <c r="B754" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C754" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E754" s="3" t="s">
         <v>2640</v>
       </c>
-      <c r="F752" s="5" t="s">
+      <c r="F754" s="5" t="s">
         <v>2641</v>
       </c>
-      <c r="G752" s="3" t="s">
+      <c r="G754" s="3" t="s">
         <v>2646</v>
       </c>
     </row>
-    <row r="753" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A753" t="s">
+    <row r="755" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A755" t="s">
         <v>2632</v>
       </c>
-      <c r="B753" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C753" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E753" s="3" t="s">
+      <c r="B755" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C755" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E755" s="3" t="s">
         <v>2639</v>
       </c>
-      <c r="F753" s="5" t="s">
+      <c r="F755" s="5" t="s">
         <v>2642</v>
       </c>
-      <c r="G753" s="3" t="s">
+      <c r="G755" s="3" t="s">
         <v>2647</v>
       </c>
     </row>
-    <row r="754" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A754" s="3" t="s">
+    <row r="756" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A756" s="3" t="s">
         <v>2633</v>
       </c>
-      <c r="B754" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C754" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E754" s="3" t="s">
+      <c r="B756" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C756" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E756" s="3" t="s">
         <v>2638</v>
       </c>
-      <c r="F754" s="5" t="s">
+      <c r="F756" s="5" t="s">
         <v>2643</v>
       </c>
-      <c r="G754" s="3" t="s">
+      <c r="G756" s="3" t="s">
         <v>2648</v>
       </c>
     </row>
-    <row r="755" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A755" s="3" t="s">
+    <row r="757" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A757" s="3" t="s">
         <v>2634</v>
       </c>
-      <c r="B755" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C755" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E755" s="3" t="s">
+      <c r="B757" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C757" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E757" s="3" t="s">
         <v>2637</v>
       </c>
-      <c r="F755" s="5" t="s">
+      <c r="F757" s="5" t="s">
         <v>2644</v>
       </c>
-      <c r="G755" s="3" t="s">
+      <c r="G757" s="3" t="s">
         <v>2649</v>
-      </c>
-    </row>
-    <row r="756" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A756" t="s">
-        <v>2635</v>
-      </c>
-      <c r="B756" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C756" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E756" t="s">
-        <v>2636</v>
-      </c>
-      <c r="F756" s="5" t="s">
-        <v>2645</v>
-      </c>
-      <c r="G756" t="s">
-        <v>2650</v>
-      </c>
-    </row>
-    <row r="757" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A757" t="s">
-        <v>2651</v>
-      </c>
-      <c r="B757" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C757" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E757" t="s">
-        <v>2652</v>
-      </c>
-      <c r="F757" s="5" t="s">
-        <v>2653</v>
-      </c>
-      <c r="G757" t="s">
-        <v>2654</v>
       </c>
     </row>
     <row r="758" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>2689</v>
-      </c>
-      <c r="B758" t="b">
-        <v>0</v>
-      </c>
-      <c r="C758" t="b">
+        <v>2635</v>
+      </c>
+      <c r="B758" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C758" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E758" t="s">
-        <v>2690</v>
+        <v>2636</v>
       </c>
       <c r="F758" s="5" t="s">
-        <v>2691</v>
-      </c>
-      <c r="G758" s="2" t="s">
-        <v>2692</v>
-      </c>
-    </row>
-    <row r="759" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A759" s="3" t="s">
-        <v>2693</v>
+        <v>2645</v>
+      </c>
+      <c r="G758" t="s">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="759" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A759" t="s">
+        <v>2651</v>
       </c>
       <c r="B759" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C759" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E759" s="3" t="s">
-        <v>2694</v>
+      <c r="E759" t="s">
+        <v>2652</v>
       </c>
       <c r="F759" s="5" t="s">
-        <v>2695</v>
-      </c>
-      <c r="G759" s="2" t="s">
-        <v>2696</v>
+        <v>2653</v>
+      </c>
+      <c r="G759" t="s">
+        <v>2654</v>
       </c>
     </row>
     <row r="760" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>2697</v>
+        <v>2689</v>
       </c>
       <c r="B760" t="b">
         <v>0</v>
@@ -24613,179 +24652,179 @@
       <c r="C760" t="b">
         <v>1</v>
       </c>
-      <c r="E760" s="3" t="s">
-        <v>2698</v>
+      <c r="E760" t="s">
+        <v>2690</v>
       </c>
       <c r="F760" s="5" t="s">
-        <v>2699</v>
+        <v>2691</v>
       </c>
       <c r="G760" s="2" t="s">
-        <v>2700</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="761" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A761" s="3" t="s">
+        <v>2693</v>
+      </c>
+      <c r="B761" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C761" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E761" s="3" t="s">
+        <v>2694</v>
+      </c>
+      <c r="F761" s="5" t="s">
+        <v>2695</v>
+      </c>
+      <c r="G761" s="2" t="s">
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="762" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A762" t="s">
+        <v>2697</v>
+      </c>
+      <c r="B762" t="b">
+        <v>0</v>
+      </c>
+      <c r="C762" t="b">
+        <v>1</v>
+      </c>
+      <c r="E762" s="3" t="s">
+        <v>2698</v>
+      </c>
+      <c r="F762" s="5" t="s">
+        <v>2699</v>
+      </c>
+      <c r="G762" s="2" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="763" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A763" s="3" t="s">
         <v>2702</v>
       </c>
-      <c r="B761" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C761" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E761" s="3" t="s">
+      <c r="B763" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C763" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E763" s="3" t="s">
         <v>2704</v>
       </c>
-      <c r="F761" s="5" t="s">
+      <c r="F763" s="5" t="s">
         <v>2708</v>
       </c>
-      <c r="G761" s="2" t="s">
+      <c r="G763" s="2" t="s">
         <v>2709</v>
       </c>
     </row>
-    <row r="762" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A762" s="3" t="s">
+    <row r="764" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A764" s="3" t="s">
         <v>2703</v>
       </c>
-      <c r="B762" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C762" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E762" s="3" t="s">
+      <c r="B764" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C764" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E764" s="3" t="s">
         <v>2705</v>
       </c>
-      <c r="F762" s="5" t="s">
+      <c r="F764" s="5" t="s">
         <v>2707</v>
       </c>
-      <c r="G762" s="2" t="s">
+      <c r="G764" s="2" t="s">
         <v>2709</v>
-      </c>
-    </row>
-    <row r="763" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A763" t="s">
-        <v>2701</v>
-      </c>
-      <c r="B763" t="b">
-        <v>1</v>
-      </c>
-      <c r="C763" t="b">
-        <v>1</v>
-      </c>
-      <c r="E763" t="s">
-        <v>501</v>
-      </c>
-      <c r="F763" s="5" t="s">
-        <v>2706</v>
-      </c>
-      <c r="G763" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="764" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A764" t="s">
-        <v>2710</v>
-      </c>
-      <c r="B764" t="b">
-        <v>0</v>
-      </c>
-      <c r="C764" t="b">
-        <v>1</v>
-      </c>
-      <c r="E764" t="s">
-        <v>2711</v>
-      </c>
-      <c r="F764" s="5" t="s">
-        <v>2712</v>
-      </c>
-      <c r="G764" t="s">
-        <v>2713</v>
       </c>
     </row>
     <row r="765" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
+        <v>2701</v>
+      </c>
+      <c r="B765" t="b">
+        <v>1</v>
+      </c>
+      <c r="C765" t="b">
+        <v>1</v>
+      </c>
+      <c r="E765" t="s">
+        <v>501</v>
+      </c>
+      <c r="F765" s="5" t="s">
+        <v>2706</v>
+      </c>
+      <c r="G765" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="766" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A766" t="s">
+        <v>2710</v>
+      </c>
+      <c r="B766" t="b">
+        <v>0</v>
+      </c>
+      <c r="C766" t="b">
+        <v>1</v>
+      </c>
+      <c r="E766" t="s">
+        <v>2711</v>
+      </c>
+      <c r="F766" s="5" t="s">
+        <v>2712</v>
+      </c>
+      <c r="G766" t="s">
+        <v>2713</v>
+      </c>
+    </row>
+    <row r="767" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A767" t="s">
         <v>2714</v>
       </c>
-      <c r="B765" t="b">
-        <v>0</v>
-      </c>
-      <c r="C765" t="b">
-        <v>1</v>
-      </c>
-      <c r="E765" t="s">
+      <c r="B767" t="b">
+        <v>0</v>
+      </c>
+      <c r="C767" t="b">
+        <v>1</v>
+      </c>
+      <c r="E767" t="s">
         <v>2715</v>
       </c>
-      <c r="F765" s="5" t="s">
+      <c r="F767" s="5" t="s">
         <v>2716</v>
       </c>
-      <c r="G765" t="s">
+      <c r="G767" t="s">
         <v>2717</v>
       </c>
     </row>
-    <row r="766" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A766" s="3" t="s">
+    <row r="768" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A768" s="3" t="s">
         <v>2718</v>
       </c>
-      <c r="B766" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C766" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E766" s="3" t="s">
+      <c r="B768" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C768" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E768" s="3" t="s">
         <v>2720</v>
       </c>
-      <c r="F766" s="5" t="s">
+      <c r="F768" s="5" t="s">
         <v>2726</v>
       </c>
-      <c r="G766" s="3" t="s">
+      <c r="G768" s="3" t="s">
         <v>2732</v>
-      </c>
-    </row>
-    <row r="767" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A767" s="3" t="s">
-        <v>2719</v>
-      </c>
-      <c r="B767" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C767" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E767" s="3" t="s">
-        <v>2721</v>
-      </c>
-      <c r="F767" s="5" t="s">
-        <v>2725</v>
-      </c>
-      <c r="G767" s="3" t="s">
-        <v>2732</v>
-      </c>
-    </row>
-    <row r="768" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A768" t="s">
-        <v>2733</v>
-      </c>
-      <c r="B768" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C768" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E768" t="s">
-        <v>2722</v>
-      </c>
-      <c r="F768" s="5" t="s">
-        <v>2727</v>
-      </c>
-      <c r="G768" t="s">
-        <v>2729</v>
       </c>
     </row>
     <row r="769" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A769" s="3" t="s">
-        <v>2740</v>
+        <v>2719</v>
       </c>
       <c r="B769" s="3" t="b">
         <v>1</v>
@@ -24794,18 +24833,18 @@
         <v>1</v>
       </c>
       <c r="E769" s="3" t="s">
-        <v>2742</v>
+        <v>2721</v>
       </c>
       <c r="F769" s="5" t="s">
-        <v>2743</v>
+        <v>2725</v>
       </c>
       <c r="G769" s="3" t="s">
-        <v>2744</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="770" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="B770" s="3" t="b">
         <v>1</v>
@@ -24814,18 +24853,18 @@
         <v>1</v>
       </c>
       <c r="E770" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="F770" s="5" t="s">
-        <v>678</v>
+        <v>2727</v>
       </c>
       <c r="G770" t="s">
-        <v>2730</v>
-      </c>
-    </row>
-    <row r="771" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A771" t="s">
-        <v>2735</v>
+        <v>2729</v>
+      </c>
+    </row>
+    <row r="771" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A771" s="3" t="s">
+        <v>2740</v>
       </c>
       <c r="B771" s="3" t="b">
         <v>1</v>
@@ -24833,99 +24872,99 @@
       <c r="C771" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E771" t="s">
-        <v>2724</v>
+      <c r="E771" s="3" t="s">
+        <v>2742</v>
       </c>
       <c r="F771" s="5" t="s">
-        <v>2728</v>
-      </c>
-      <c r="G771" t="s">
-        <v>2731</v>
+        <v>2743</v>
+      </c>
+      <c r="G771" s="3" t="s">
+        <v>2744</v>
       </c>
     </row>
     <row r="772" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>2736</v>
-      </c>
-      <c r="B772" t="b">
-        <v>1</v>
-      </c>
-      <c r="C772" t="b">
+        <v>2734</v>
+      </c>
+      <c r="B772" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C772" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E772" t="s">
-        <v>2737</v>
+        <v>2723</v>
       </c>
       <c r="F772" s="5" t="s">
-        <v>2738</v>
+        <v>678</v>
       </c>
       <c r="G772" t="s">
-        <v>2739</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="773" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>2745</v>
-      </c>
-      <c r="B773" t="b">
-        <v>0</v>
-      </c>
-      <c r="C773" t="b">
+        <v>2735</v>
+      </c>
+      <c r="B773" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C773" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E773" t="s">
-        <v>2722</v>
+        <v>2724</v>
       </c>
       <c r="F773" s="5" t="s">
-        <v>2727</v>
+        <v>2728</v>
       </c>
       <c r="G773" t="s">
-        <v>2729</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="774" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>2746</v>
-      </c>
-      <c r="B774" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C774" s="3" t="b">
+        <v>2736</v>
+      </c>
+      <c r="B774" t="b">
+        <v>1</v>
+      </c>
+      <c r="C774" t="b">
         <v>1</v>
       </c>
       <c r="E774" t="s">
-        <v>2749</v>
+        <v>2737</v>
       </c>
       <c r="F774" s="5" t="s">
-        <v>2751</v>
+        <v>2738</v>
       </c>
       <c r="G774" t="s">
-        <v>2753</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="775" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>2747</v>
-      </c>
-      <c r="B775" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C775" s="3" t="b">
+        <v>2745</v>
+      </c>
+      <c r="B775" t="b">
+        <v>0</v>
+      </c>
+      <c r="C775" t="b">
         <v>1</v>
       </c>
       <c r="E775" t="s">
-        <v>2741</v>
+        <v>2722</v>
       </c>
       <c r="F775" s="5" t="s">
-        <v>2743</v>
+        <v>2727</v>
       </c>
       <c r="G775" t="s">
-        <v>2744</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="776" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>2748</v>
+        <v>2746</v>
       </c>
       <c r="B776" s="3" t="b">
         <v>0</v>
@@ -24934,118 +24973,118 @@
         <v>1</v>
       </c>
       <c r="E776" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
       <c r="F776" s="5" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="G776" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="777" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>2755</v>
-      </c>
-      <c r="B777" t="b">
-        <v>0</v>
-      </c>
-      <c r="C777" t="b">
+        <v>2747</v>
+      </c>
+      <c r="B777" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C777" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E777" t="s">
-        <v>2756</v>
+        <v>2741</v>
       </c>
       <c r="F777" s="5" t="s">
-        <v>2757</v>
+        <v>2743</v>
       </c>
       <c r="G777" t="s">
-        <v>2758</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="778" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>2759</v>
-      </c>
-      <c r="B778" t="b">
-        <v>0</v>
-      </c>
-      <c r="C778" t="b">
+        <v>2748</v>
+      </c>
+      <c r="B778" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C778" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E778" t="s">
-        <v>2760</v>
+        <v>2750</v>
       </c>
       <c r="F778" s="5" t="s">
-        <v>2761</v>
-      </c>
-      <c r="G778" s="2" t="s">
-        <v>2762</v>
+        <v>2752</v>
+      </c>
+      <c r="G778" t="s">
+        <v>2754</v>
       </c>
     </row>
     <row r="779" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>2763</v>
+        <v>2755</v>
       </c>
       <c r="B779" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C779" t="b">
         <v>1</v>
       </c>
       <c r="E779" t="s">
-        <v>2764</v>
+        <v>2756</v>
       </c>
       <c r="F779" s="5" t="s">
-        <v>2765</v>
+        <v>2757</v>
       </c>
       <c r="G779" t="s">
-        <v>2772</v>
+        <v>2758</v>
       </c>
     </row>
     <row r="780" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>2766</v>
-      </c>
-      <c r="B780" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C780" s="3" t="b">
+        <v>2759</v>
+      </c>
+      <c r="B780" t="b">
+        <v>0</v>
+      </c>
+      <c r="C780" t="b">
         <v>1</v>
       </c>
       <c r="E780" t="s">
-        <v>1</v>
+        <v>2760</v>
       </c>
       <c r="F780" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G780" t="s">
-        <v>1705</v>
+        <v>2761</v>
+      </c>
+      <c r="G780" s="2" t="s">
+        <v>2762</v>
       </c>
     </row>
     <row r="781" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>2767</v>
-      </c>
-      <c r="B781" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C781" s="3" t="b">
+        <v>2763</v>
+      </c>
+      <c r="B781" t="b">
+        <v>1</v>
+      </c>
+      <c r="C781" t="b">
         <v>1</v>
       </c>
       <c r="E781" t="s">
-        <v>2684</v>
+        <v>2764</v>
       </c>
       <c r="F781" s="5" t="s">
-        <v>2686</v>
+        <v>2765</v>
       </c>
       <c r="G781" t="s">
-        <v>2688</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="782" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="B782" s="3" t="b">
         <v>1</v>
@@ -25054,18 +25093,18 @@
         <v>1</v>
       </c>
       <c r="E782" t="s">
-        <v>2770</v>
+        <v>1</v>
       </c>
       <c r="F782" s="5" t="s">
-        <v>2771</v>
+        <v>110</v>
       </c>
       <c r="G782" t="s">
-        <v>2772</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="783" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>2769</v>
+        <v>2767</v>
       </c>
       <c r="B783" s="3" t="b">
         <v>1</v>
@@ -25074,18 +25113,18 @@
         <v>1</v>
       </c>
       <c r="E783" t="s">
-        <v>803</v>
+        <v>2684</v>
       </c>
       <c r="F783" s="5" t="s">
-        <v>812</v>
+        <v>2686</v>
       </c>
       <c r="G783" t="s">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="784" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A784" s="3" t="s">
-        <v>2775</v>
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="784" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A784" t="s">
+        <v>2768</v>
       </c>
       <c r="B784" s="3" t="b">
         <v>1</v>
@@ -25093,119 +25132,119 @@
       <c r="C784" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E784" s="3" t="s">
-        <v>377</v>
+      <c r="E784" t="s">
+        <v>2770</v>
       </c>
       <c r="F784" s="5" t="s">
-        <v>2778</v>
-      </c>
-      <c r="G784" s="3" t="s">
-        <v>1323</v>
+        <v>2771</v>
+      </c>
+      <c r="G784" t="s">
+        <v>2772</v>
       </c>
     </row>
     <row r="785" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
+        <v>2769</v>
+      </c>
+      <c r="B785" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C785" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E785" t="s">
+        <v>803</v>
+      </c>
+      <c r="F785" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="G785" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="786" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A786" s="3" t="s">
+        <v>2775</v>
+      </c>
+      <c r="B786" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C786" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E786" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F786" s="5" t="s">
+        <v>2778</v>
+      </c>
+      <c r="G786" s="3" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="787" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A787" t="s">
         <v>2773</v>
       </c>
-      <c r="B785" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C785" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E785" t="s">
+      <c r="B787" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C787" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E787" t="s">
         <v>2684</v>
       </c>
-      <c r="F785" s="5" t="s">
+      <c r="F787" s="5" t="s">
         <v>2686</v>
       </c>
-      <c r="G785" t="s">
+      <c r="G787" t="s">
         <v>2688</v>
       </c>
     </row>
-    <row r="786" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A786" t="s">
+    <row r="788" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A788" t="s">
         <v>2774</v>
       </c>
-      <c r="B786" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C786" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E786" t="s">
+      <c r="B788" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C788" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E788" t="s">
         <v>2776</v>
       </c>
-      <c r="F786" s="5" t="s">
+      <c r="F788" s="5" t="s">
         <v>2777</v>
       </c>
-      <c r="G786" t="s">
+      <c r="G788" t="s">
         <v>2779</v>
       </c>
     </row>
-    <row r="787" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A787" s="3" t="s">
+    <row r="789" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A789" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="B787" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C787" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E787" s="3" t="s">
+      <c r="B789" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C789" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E789" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="F787" s="5" t="s">
+      <c r="F789" s="5" t="s">
         <v>2267</v>
       </c>
-      <c r="G787" s="3" t="s">
+      <c r="G789" s="3" t="s">
         <v>1407</v>
       </c>
     </row>
-    <row r="788" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A788" s="3" t="s">
-        <v>2795</v>
-      </c>
-      <c r="B788" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C788" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E788" s="3" t="s">
-        <v>2795</v>
-      </c>
-      <c r="F788" s="5" t="s">
-        <v>2796</v>
-      </c>
-      <c r="G788" s="3" t="s">
-        <v>2808</v>
-      </c>
-    </row>
-    <row r="789" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A789" t="s">
-        <v>2783</v>
-      </c>
-      <c r="B789" t="b">
-        <v>0</v>
-      </c>
-      <c r="C789" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E789" t="s">
-        <v>2797</v>
-      </c>
-      <c r="F789" s="5" t="s">
-        <v>2798</v>
-      </c>
-      <c r="G789" t="s">
-        <v>2809</v>
-      </c>
-    </row>
-    <row r="790" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A790" t="s">
-        <v>2799</v>
+    <row r="790" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A790" s="3" t="s">
+        <v>2791</v>
       </c>
       <c r="B790" s="3" t="b">
         <v>0</v>
@@ -25213,119 +25252,119 @@
       <c r="C790" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E790" t="s">
-        <v>2789</v>
+      <c r="E790" s="3" t="s">
+        <v>2791</v>
       </c>
       <c r="F790" s="5" t="s">
-        <v>2791</v>
-      </c>
-      <c r="G790" t="s">
-        <v>2810</v>
+        <v>2792</v>
+      </c>
+      <c r="G790" s="3" t="s">
+        <v>2803</v>
       </c>
     </row>
     <row r="791" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>2784</v>
-      </c>
-      <c r="B791" s="3" t="b">
+        <v>2783</v>
+      </c>
+      <c r="B791" t="b">
         <v>0</v>
       </c>
       <c r="C791" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E791" t="s">
-        <v>2790</v>
+        <v>2793</v>
       </c>
       <c r="F791" s="5" t="s">
-        <v>2786</v>
+        <v>2813</v>
       </c>
       <c r="G791" t="s">
-        <v>2811</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="792" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>2785</v>
+        <v>2794</v>
       </c>
       <c r="B792" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C792" t="b">
+      <c r="C792" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E792" t="s">
-        <v>2788</v>
+        <v>2817</v>
       </c>
       <c r="F792" s="5" t="s">
-        <v>2787</v>
+        <v>2814</v>
       </c>
       <c r="G792" t="s">
-        <v>2812</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="793" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>2792</v>
-      </c>
-      <c r="B793" t="b">
-        <v>0</v>
-      </c>
-      <c r="C793" t="b">
+        <v>2784</v>
+      </c>
+      <c r="B793" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C793" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E793" t="s">
-        <v>2793</v>
+        <v>2787</v>
       </c>
       <c r="F793" s="5" t="s">
-        <v>2794</v>
+        <v>2815</v>
       </c>
       <c r="G793" t="s">
-        <v>2813</v>
+        <v>2806</v>
       </c>
     </row>
     <row r="794" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>2800</v>
+        <v>2785</v>
       </c>
       <c r="B794" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C794" s="3" t="b">
+      <c r="C794" t="b">
         <v>1</v>
       </c>
       <c r="E794" t="s">
-        <v>2800</v>
+        <v>2786</v>
       </c>
       <c r="F794" s="5" t="s">
-        <v>2804</v>
+        <v>2816</v>
       </c>
       <c r="G794" t="s">
-        <v>2814</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="795" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>2801</v>
-      </c>
-      <c r="B795" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C795" s="3" t="b">
+        <v>2788</v>
+      </c>
+      <c r="B795" t="b">
+        <v>0</v>
+      </c>
+      <c r="C795" t="b">
         <v>1</v>
       </c>
       <c r="E795" t="s">
-        <v>2801</v>
+        <v>2789</v>
       </c>
       <c r="F795" s="5" t="s">
-        <v>2806</v>
+        <v>2790</v>
       </c>
       <c r="G795" t="s">
-        <v>2815</v>
+        <v>2808</v>
       </c>
     </row>
     <row r="796" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>2802</v>
+        <v>2795</v>
       </c>
       <c r="B796" s="3" t="b">
         <v>0</v>
@@ -25334,18 +25373,18 @@
         <v>1</v>
       </c>
       <c r="E796" t="s">
-        <v>2802</v>
+        <v>2795</v>
       </c>
       <c r="F796" s="5" t="s">
-        <v>2805</v>
+        <v>2799</v>
       </c>
       <c r="G796" t="s">
-        <v>2816</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="797" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>2803</v>
+        <v>2796</v>
       </c>
       <c r="B797" s="3" t="b">
         <v>0</v>
@@ -25354,17 +25393,97 @@
         <v>1</v>
       </c>
       <c r="E797" t="s">
-        <v>2803</v>
+        <v>2796</v>
       </c>
       <c r="F797" s="5" t="s">
-        <v>2807</v>
+        <v>2801</v>
       </c>
       <c r="G797" t="s">
-        <v>2817</v>
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="798" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A798" t="s">
+        <v>2797</v>
+      </c>
+      <c r="B798" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C798" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E798" t="s">
+        <v>2797</v>
+      </c>
+      <c r="F798" s="5" t="s">
+        <v>2800</v>
+      </c>
+      <c r="G798" t="s">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="799" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A799" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B799" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C799" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E799" t="s">
+        <v>2798</v>
+      </c>
+      <c r="F799" s="5" t="s">
+        <v>2802</v>
+      </c>
+      <c r="G799" t="s">
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="800" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A800" t="s">
+        <v>2818</v>
+      </c>
+      <c r="B800" t="b">
+        <v>0</v>
+      </c>
+      <c r="C800" t="b">
+        <v>1</v>
+      </c>
+      <c r="E800" t="s">
+        <v>2819</v>
+      </c>
+      <c r="F800" s="5" t="s">
+        <v>2820</v>
+      </c>
+      <c r="G800" t="s">
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="801" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A801" t="s">
+        <v>2828</v>
+      </c>
+      <c r="B801" t="b">
+        <v>0</v>
+      </c>
+      <c r="C801" t="b">
+        <v>1</v>
+      </c>
+      <c r="E801" t="s">
+        <v>2828</v>
+      </c>
+      <c r="F801" s="5" t="s">
+        <v>2829</v>
+      </c>
+      <c r="G801" t="s">
+        <v>1432</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G755" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G757" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented the signatures framework
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B8F588-C5D7-477C-B5F4-48788915626B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B9D3BE-32C8-4098-AD78-D76F0D4921F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3212" uniqueCount="2831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="2835">
   <si>
     <t>Key</t>
   </si>
@@ -8529,6 +8529,18 @@
   </si>
   <si>
     <t>附加信息</t>
+  </si>
+  <si>
+    <t>Count0Lines</t>
+  </si>
+  <si>
+    <t>{{0}}线</t>
+  </si>
+  <si>
+    <t>{{0}} line(s)</t>
+  </si>
+  <si>
+    <t>عدد {{0}} أسطر</t>
   </si>
 </sst>
 </file>
@@ -8925,12 +8937,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G801"/>
+  <dimension ref="A1:G802"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A778" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A771" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G800" sqref="G800:G801"/>
+      <selection pane="bottomLeft" activeCell="F806" sqref="F806"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25482,6 +25494,27 @@
         <v>1432</v>
       </c>
     </row>
+    <row r="802" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A802" s="3" t="s">
+        <v>2831</v>
+      </c>
+      <c r="B802" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C802" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D802" s="3"/>
+      <c r="E802" s="3" t="s">
+        <v>2833</v>
+      </c>
+      <c r="F802" s="5" t="s">
+        <v>2834</v>
+      </c>
+      <c r="G802" s="3" t="s">
+        <v>2832</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G757" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Working on smart screens
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1593CAE2-4C6F-4E74-8B97-CD73C566B4B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219E77E8-1079-4BAD-A3C4-D5C17180D60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="2835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232" uniqueCount="2842">
   <si>
     <t>Key</t>
   </si>
@@ -8541,6 +8541,27 @@
   </si>
   <si>
     <t>Are you sure you want to delete {{count}} item(s) with all their descendants? This action is irreversible.</t>
+  </si>
+  <si>
+    <t>DetailsEntry_Count</t>
+  </si>
+  <si>
+    <t>DetailsEntry_Mass</t>
+  </si>
+  <si>
+    <t>DetailsEntry_Volume</t>
+  </si>
+  <si>
+    <t>DetailsEntry_Time</t>
+  </si>
+  <si>
+    <t>العدد</t>
+  </si>
+  <si>
+    <t>الوزن</t>
+  </si>
+  <si>
+    <t>الزمن</t>
   </si>
 </sst>
 </file>
@@ -8937,12 +8958,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G802"/>
+  <dimension ref="A1:G806"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A734" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66:F67"/>
+      <selection pane="bottomLeft" activeCell="F763" sqref="F763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24654,69 +24675,69 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="760" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A760" t="s">
-        <v>2687</v>
-      </c>
-      <c r="B760" t="b">
-        <v>0</v>
-      </c>
-      <c r="C760" t="b">
-        <v>1</v>
-      </c>
-      <c r="E760" t="s">
-        <v>2688</v>
+    <row r="760" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A760" s="3" t="s">
+        <v>2835</v>
+      </c>
+      <c r="B760" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C760" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E760" s="3" t="s">
+        <v>416</v>
       </c>
       <c r="F760" s="5" t="s">
-        <v>2689</v>
-      </c>
-      <c r="G760" s="2" t="s">
-        <v>2690</v>
+        <v>2839</v>
+      </c>
+      <c r="G760" s="3" t="s">
+        <v>1334</v>
       </c>
     </row>
     <row r="761" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A761" s="3" t="s">
-        <v>2691</v>
+        <v>2836</v>
       </c>
       <c r="B761" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C761" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E761" s="3" t="s">
-        <v>2692</v>
+        <v>422</v>
       </c>
       <c r="F761" s="5" t="s">
-        <v>2693</v>
-      </c>
-      <c r="G761" s="2" t="s">
-        <v>2694</v>
-      </c>
-    </row>
-    <row r="762" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A762" t="s">
-        <v>2695</v>
-      </c>
-      <c r="B762" t="b">
-        <v>0</v>
-      </c>
-      <c r="C762" t="b">
+        <v>2840</v>
+      </c>
+      <c r="G761" s="3" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="762" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A762" s="3" t="s">
+        <v>2837</v>
+      </c>
+      <c r="B762" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C762" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E762" s="3" t="s">
-        <v>2696</v>
+        <v>437</v>
       </c>
       <c r="F762" s="5" t="s">
-        <v>2697</v>
-      </c>
-      <c r="G762" s="2" t="s">
-        <v>2698</v>
+        <v>1676</v>
+      </c>
+      <c r="G762" s="3" t="s">
+        <v>1341</v>
       </c>
     </row>
     <row r="763" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A763" s="3" t="s">
-        <v>2700</v>
+        <v>2838</v>
       </c>
       <c r="B763" s="3" t="b">
         <v>1</v>
@@ -24725,58 +24746,58 @@
         <v>1</v>
       </c>
       <c r="E763" s="3" t="s">
-        <v>2702</v>
+        <v>428</v>
       </c>
       <c r="F763" s="5" t="s">
-        <v>2706</v>
-      </c>
-      <c r="G763" s="2" t="s">
-        <v>2707</v>
-      </c>
-    </row>
-    <row r="764" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A764" s="3" t="s">
-        <v>2701</v>
-      </c>
-      <c r="B764" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C764" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E764" s="3" t="s">
-        <v>2703</v>
+        <v>2841</v>
+      </c>
+      <c r="G763" s="3" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="764" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A764" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B764" t="b">
+        <v>0</v>
+      </c>
+      <c r="C764" t="b">
+        <v>1</v>
+      </c>
+      <c r="E764" t="s">
+        <v>2688</v>
       </c>
       <c r="F764" s="5" t="s">
-        <v>2705</v>
+        <v>2689</v>
       </c>
       <c r="G764" s="2" t="s">
-        <v>2707</v>
-      </c>
-    </row>
-    <row r="765" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A765" t="s">
-        <v>2699</v>
-      </c>
-      <c r="B765" t="b">
-        <v>1</v>
-      </c>
-      <c r="C765" t="b">
-        <v>1</v>
-      </c>
-      <c r="E765" t="s">
-        <v>501</v>
+        <v>2690</v>
+      </c>
+    </row>
+    <row r="765" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A765" s="3" t="s">
+        <v>2691</v>
+      </c>
+      <c r="B765" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C765" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E765" s="3" t="s">
+        <v>2692</v>
       </c>
       <c r="F765" s="5" t="s">
-        <v>2704</v>
-      </c>
-      <c r="G765" t="s">
-        <v>1365</v>
+        <v>2693</v>
+      </c>
+      <c r="G765" s="2" t="s">
+        <v>2694</v>
       </c>
     </row>
     <row r="766" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>2708</v>
+        <v>2695</v>
       </c>
       <c r="B766" t="b">
         <v>0</v>
@@ -24784,39 +24805,39 @@
       <c r="C766" t="b">
         <v>1</v>
       </c>
-      <c r="E766" t="s">
-        <v>2709</v>
+      <c r="E766" s="3" t="s">
+        <v>2696</v>
       </c>
       <c r="F766" s="5" t="s">
-        <v>2710</v>
-      </c>
-      <c r="G766" t="s">
-        <v>2711</v>
-      </c>
-    </row>
-    <row r="767" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A767" t="s">
-        <v>2712</v>
-      </c>
-      <c r="B767" t="b">
-        <v>0</v>
-      </c>
-      <c r="C767" t="b">
-        <v>1</v>
-      </c>
-      <c r="E767" t="s">
-        <v>2713</v>
+        <v>2697</v>
+      </c>
+      <c r="G766" s="2" t="s">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="767" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A767" s="3" t="s">
+        <v>2700</v>
+      </c>
+      <c r="B767" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C767" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E767" s="3" t="s">
+        <v>2702</v>
       </c>
       <c r="F767" s="5" t="s">
-        <v>2714</v>
-      </c>
-      <c r="G767" t="s">
-        <v>2715</v>
+        <v>2706</v>
+      </c>
+      <c r="G767" s="2" t="s">
+        <v>2707</v>
       </c>
     </row>
     <row r="768" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A768" s="3" t="s">
-        <v>2716</v>
+        <v>2701</v>
       </c>
       <c r="B768" s="3" t="b">
         <v>1</v>
@@ -24825,78 +24846,78 @@
         <v>1</v>
       </c>
       <c r="E768" s="3" t="s">
-        <v>2718</v>
+        <v>2703</v>
       </c>
       <c r="F768" s="5" t="s">
-        <v>2724</v>
-      </c>
-      <c r="G768" s="3" t="s">
-        <v>2730</v>
-      </c>
-    </row>
-    <row r="769" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A769" s="3" t="s">
-        <v>2717</v>
-      </c>
-      <c r="B769" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C769" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E769" s="3" t="s">
-        <v>2719</v>
+        <v>2705</v>
+      </c>
+      <c r="G768" s="2" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="769" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A769" t="s">
+        <v>2699</v>
+      </c>
+      <c r="B769" t="b">
+        <v>1</v>
+      </c>
+      <c r="C769" t="b">
+        <v>1</v>
+      </c>
+      <c r="E769" t="s">
+        <v>501</v>
       </c>
       <c r="F769" s="5" t="s">
-        <v>2723</v>
-      </c>
-      <c r="G769" s="3" t="s">
-        <v>2730</v>
+        <v>2704</v>
+      </c>
+      <c r="G769" t="s">
+        <v>1365</v>
       </c>
     </row>
     <row r="770" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>2731</v>
-      </c>
-      <c r="B770" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C770" s="3" t="b">
+        <v>2708</v>
+      </c>
+      <c r="B770" t="b">
+        <v>0</v>
+      </c>
+      <c r="C770" t="b">
         <v>1</v>
       </c>
       <c r="E770" t="s">
-        <v>2720</v>
+        <v>2709</v>
       </c>
       <c r="F770" s="5" t="s">
-        <v>2725</v>
+        <v>2710</v>
       </c>
       <c r="G770" t="s">
-        <v>2727</v>
-      </c>
-    </row>
-    <row r="771" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A771" s="3" t="s">
-        <v>2738</v>
-      </c>
-      <c r="B771" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C771" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E771" s="3" t="s">
-        <v>2740</v>
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="771" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A771" t="s">
+        <v>2712</v>
+      </c>
+      <c r="B771" t="b">
+        <v>0</v>
+      </c>
+      <c r="C771" t="b">
+        <v>1</v>
+      </c>
+      <c r="E771" t="s">
+        <v>2713</v>
       </c>
       <c r="F771" s="5" t="s">
-        <v>2741</v>
-      </c>
-      <c r="G771" s="3" t="s">
-        <v>2742</v>
-      </c>
-    </row>
-    <row r="772" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A772" t="s">
-        <v>2732</v>
+        <v>2714</v>
+      </c>
+      <c r="G771" t="s">
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="772" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A772" s="3" t="s">
+        <v>2716</v>
       </c>
       <c r="B772" s="3" t="b">
         <v>1</v>
@@ -24904,19 +24925,19 @@
       <c r="C772" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E772" t="s">
-        <v>2721</v>
+      <c r="E772" s="3" t="s">
+        <v>2718</v>
       </c>
       <c r="F772" s="5" t="s">
-        <v>678</v>
-      </c>
-      <c r="G772" t="s">
-        <v>2728</v>
-      </c>
-    </row>
-    <row r="773" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A773" t="s">
-        <v>2733</v>
+        <v>2724</v>
+      </c>
+      <c r="G772" s="3" t="s">
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="773" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A773" s="3" t="s">
+        <v>2717</v>
       </c>
       <c r="B773" s="3" t="b">
         <v>1</v>
@@ -24924,119 +24945,119 @@
       <c r="C773" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E773" t="s">
-        <v>2722</v>
+      <c r="E773" s="3" t="s">
+        <v>2719</v>
       </c>
       <c r="F773" s="5" t="s">
-        <v>2726</v>
-      </c>
-      <c r="G773" t="s">
-        <v>2729</v>
+        <v>2723</v>
+      </c>
+      <c r="G773" s="3" t="s">
+        <v>2730</v>
       </c>
     </row>
     <row r="774" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>2734</v>
-      </c>
-      <c r="B774" t="b">
-        <v>1</v>
-      </c>
-      <c r="C774" t="b">
+        <v>2731</v>
+      </c>
+      <c r="B774" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C774" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E774" t="s">
-        <v>2735</v>
+        <v>2720</v>
       </c>
       <c r="F774" s="5" t="s">
-        <v>2736</v>
+        <v>2725</v>
       </c>
       <c r="G774" t="s">
-        <v>2737</v>
-      </c>
-    </row>
-    <row r="775" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A775" t="s">
-        <v>2743</v>
-      </c>
-      <c r="B775" t="b">
-        <v>0</v>
-      </c>
-      <c r="C775" t="b">
-        <v>1</v>
-      </c>
-      <c r="E775" t="s">
-        <v>2720</v>
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="775" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A775" s="3" t="s">
+        <v>2738</v>
+      </c>
+      <c r="B775" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C775" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E775" s="3" t="s">
+        <v>2740</v>
       </c>
       <c r="F775" s="5" t="s">
-        <v>2725</v>
-      </c>
-      <c r="G775" t="s">
-        <v>2727</v>
+        <v>2741</v>
+      </c>
+      <c r="G775" s="3" t="s">
+        <v>2742</v>
       </c>
     </row>
     <row r="776" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>2744</v>
+        <v>2732</v>
       </c>
       <c r="B776" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C776" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E776" t="s">
-        <v>2747</v>
+        <v>2721</v>
       </c>
       <c r="F776" s="5" t="s">
-        <v>2749</v>
+        <v>678</v>
       </c>
       <c r="G776" t="s">
-        <v>2751</v>
+        <v>2728</v>
       </c>
     </row>
     <row r="777" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>2745</v>
+        <v>2733</v>
       </c>
       <c r="B777" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C777" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E777" t="s">
-        <v>2739</v>
+        <v>2722</v>
       </c>
       <c r="F777" s="5" t="s">
-        <v>2741</v>
+        <v>2726</v>
       </c>
       <c r="G777" t="s">
-        <v>2742</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="778" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>2746</v>
-      </c>
-      <c r="B778" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C778" s="3" t="b">
+        <v>2734</v>
+      </c>
+      <c r="B778" t="b">
+        <v>1</v>
+      </c>
+      <c r="C778" t="b">
         <v>1</v>
       </c>
       <c r="E778" t="s">
-        <v>2748</v>
+        <v>2735</v>
       </c>
       <c r="F778" s="5" t="s">
-        <v>2750</v>
+        <v>2736</v>
       </c>
       <c r="G778" t="s">
-        <v>2752</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="779" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>2753</v>
+        <v>2743</v>
       </c>
       <c r="B779" t="b">
         <v>0</v>
@@ -25045,138 +25066,138 @@
         <v>1</v>
       </c>
       <c r="E779" t="s">
-        <v>2754</v>
+        <v>2720</v>
       </c>
       <c r="F779" s="5" t="s">
-        <v>2755</v>
+        <v>2725</v>
       </c>
       <c r="G779" t="s">
-        <v>2756</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="780" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>2757</v>
-      </c>
-      <c r="B780" t="b">
-        <v>0</v>
-      </c>
-      <c r="C780" t="b">
+        <v>2744</v>
+      </c>
+      <c r="B780" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C780" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E780" t="s">
-        <v>2758</v>
+        <v>2747</v>
       </c>
       <c r="F780" s="5" t="s">
-        <v>2759</v>
-      </c>
-      <c r="G780" s="2" t="s">
-        <v>2760</v>
+        <v>2749</v>
+      </c>
+      <c r="G780" t="s">
+        <v>2751</v>
       </c>
     </row>
     <row r="781" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>2761</v>
-      </c>
-      <c r="B781" t="b">
-        <v>1</v>
-      </c>
-      <c r="C781" t="b">
+        <v>2745</v>
+      </c>
+      <c r="B781" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C781" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E781" t="s">
-        <v>2762</v>
+        <v>2739</v>
       </c>
       <c r="F781" s="5" t="s">
-        <v>2763</v>
+        <v>2741</v>
       </c>
       <c r="G781" t="s">
-        <v>2770</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="782" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>2764</v>
+        <v>2746</v>
       </c>
       <c r="B782" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C782" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E782" t="s">
-        <v>1</v>
+        <v>2748</v>
       </c>
       <c r="F782" s="5" t="s">
-        <v>110</v>
+        <v>2750</v>
       </c>
       <c r="G782" t="s">
-        <v>1703</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="783" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>2765</v>
-      </c>
-      <c r="B783" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C783" s="3" t="b">
+        <v>2753</v>
+      </c>
+      <c r="B783" t="b">
+        <v>0</v>
+      </c>
+      <c r="C783" t="b">
         <v>1</v>
       </c>
       <c r="E783" t="s">
-        <v>2682</v>
+        <v>2754</v>
       </c>
       <c r="F783" s="5" t="s">
-        <v>2684</v>
+        <v>2755</v>
       </c>
       <c r="G783" t="s">
-        <v>2686</v>
+        <v>2756</v>
       </c>
     </row>
     <row r="784" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>2766</v>
-      </c>
-      <c r="B784" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C784" s="3" t="b">
+        <v>2757</v>
+      </c>
+      <c r="B784" t="b">
+        <v>0</v>
+      </c>
+      <c r="C784" t="b">
         <v>1</v>
       </c>
       <c r="E784" t="s">
-        <v>2768</v>
+        <v>2758</v>
       </c>
       <c r="F784" s="5" t="s">
-        <v>2769</v>
-      </c>
-      <c r="G784" t="s">
-        <v>2770</v>
+        <v>2759</v>
+      </c>
+      <c r="G784" s="2" t="s">
+        <v>2760</v>
       </c>
     </row>
     <row r="785" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>2767</v>
-      </c>
-      <c r="B785" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C785" s="3" t="b">
+        <v>2761</v>
+      </c>
+      <c r="B785" t="b">
+        <v>1</v>
+      </c>
+      <c r="C785" t="b">
         <v>1</v>
       </c>
       <c r="E785" t="s">
-        <v>803</v>
+        <v>2762</v>
       </c>
       <c r="F785" s="5" t="s">
-        <v>812</v>
+        <v>2763</v>
       </c>
       <c r="G785" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="786" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A786" s="3" t="s">
-        <v>2773</v>
+        <v>2770</v>
+      </c>
+    </row>
+    <row r="786" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A786" t="s">
+        <v>2764</v>
       </c>
       <c r="B786" s="3" t="b">
         <v>1</v>
@@ -25184,19 +25205,19 @@
       <c r="C786" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E786" s="3" t="s">
-        <v>377</v>
+      <c r="E786" t="s">
+        <v>1</v>
       </c>
       <c r="F786" s="5" t="s">
-        <v>2776</v>
-      </c>
-      <c r="G786" s="3" t="s">
-        <v>1321</v>
+        <v>110</v>
+      </c>
+      <c r="G786" t="s">
+        <v>1703</v>
       </c>
     </row>
     <row r="787" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>2771</v>
+        <v>2765</v>
       </c>
       <c r="B787" s="3" t="b">
         <v>1</v>
@@ -25216,7 +25237,7 @@
     </row>
     <row r="788" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>2772</v>
+        <v>2766</v>
       </c>
       <c r="B788" s="3" t="b">
         <v>1</v>
@@ -25225,98 +25246,98 @@
         <v>1</v>
       </c>
       <c r="E788" t="s">
-        <v>2774</v>
+        <v>2768</v>
       </c>
       <c r="F788" s="5" t="s">
-        <v>2775</v>
+        <v>2769</v>
       </c>
       <c r="G788" t="s">
-        <v>2777</v>
-      </c>
-    </row>
-    <row r="789" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A789" s="3" t="s">
-        <v>619</v>
+        <v>2770</v>
+      </c>
+    </row>
+    <row r="789" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A789" t="s">
+        <v>2767</v>
       </c>
       <c r="B789" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C789" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E789" s="3" t="s">
-        <v>619</v>
+      <c r="E789" t="s">
+        <v>803</v>
       </c>
       <c r="F789" s="5" t="s">
-        <v>2265</v>
-      </c>
-      <c r="G789" s="3" t="s">
-        <v>1405</v>
+        <v>812</v>
+      </c>
+      <c r="G789" t="s">
+        <v>1465</v>
       </c>
     </row>
     <row r="790" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A790" s="3" t="s">
-        <v>2789</v>
+        <v>2773</v>
       </c>
       <c r="B790" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C790" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E790" s="3" t="s">
-        <v>2789</v>
+        <v>377</v>
       </c>
       <c r="F790" s="5" t="s">
-        <v>2790</v>
+        <v>2776</v>
       </c>
       <c r="G790" s="3" t="s">
-        <v>2801</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="791" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>2781</v>
-      </c>
-      <c r="B791" t="b">
-        <v>0</v>
+        <v>2771</v>
+      </c>
+      <c r="B791" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="C791" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E791" t="s">
-        <v>2791</v>
+        <v>2682</v>
       </c>
       <c r="F791" s="5" t="s">
-        <v>2811</v>
+        <v>2684</v>
       </c>
       <c r="G791" t="s">
-        <v>2802</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="792" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>2792</v>
+        <v>2772</v>
       </c>
       <c r="B792" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C792" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E792" t="s">
-        <v>2815</v>
+        <v>2774</v>
       </c>
       <c r="F792" s="5" t="s">
-        <v>2812</v>
+        <v>2775</v>
       </c>
       <c r="G792" t="s">
-        <v>2803</v>
-      </c>
-    </row>
-    <row r="793" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A793" t="s">
-        <v>2782</v>
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="793" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A793" s="3" t="s">
+        <v>619</v>
       </c>
       <c r="B793" s="3" t="b">
         <v>0</v>
@@ -25324,59 +25345,59 @@
       <c r="C793" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E793" t="s">
-        <v>2785</v>
+      <c r="E793" s="3" t="s">
+        <v>619</v>
       </c>
       <c r="F793" s="5" t="s">
-        <v>2813</v>
-      </c>
-      <c r="G793" t="s">
-        <v>2804</v>
-      </c>
-    </row>
-    <row r="794" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A794" t="s">
-        <v>2783</v>
+        <v>2265</v>
+      </c>
+      <c r="G793" s="3" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="794" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A794" s="3" t="s">
+        <v>2789</v>
       </c>
       <c r="B794" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C794" t="b">
-        <v>1</v>
-      </c>
-      <c r="E794" t="s">
-        <v>2784</v>
+      <c r="C794" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E794" s="3" t="s">
+        <v>2789</v>
       </c>
       <c r="F794" s="5" t="s">
-        <v>2814</v>
-      </c>
-      <c r="G794" t="s">
-        <v>2805</v>
+        <v>2790</v>
+      </c>
+      <c r="G794" s="3" t="s">
+        <v>2801</v>
       </c>
     </row>
     <row r="795" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>2786</v>
+        <v>2781</v>
       </c>
       <c r="B795" t="b">
         <v>0</v>
       </c>
-      <c r="C795" t="b">
+      <c r="C795" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E795" t="s">
-        <v>2787</v>
+        <v>2791</v>
       </c>
       <c r="F795" s="5" t="s">
-        <v>2788</v>
+        <v>2811</v>
       </c>
       <c r="G795" t="s">
-        <v>2806</v>
+        <v>2802</v>
       </c>
     </row>
     <row r="796" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="B796" s="3" t="b">
         <v>0</v>
@@ -25385,18 +25406,18 @@
         <v>1</v>
       </c>
       <c r="E796" t="s">
-        <v>2793</v>
+        <v>2815</v>
       </c>
       <c r="F796" s="5" t="s">
-        <v>2797</v>
+        <v>2812</v>
       </c>
       <c r="G796" t="s">
-        <v>2807</v>
+        <v>2803</v>
       </c>
     </row>
     <row r="797" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>2794</v>
+        <v>2782</v>
       </c>
       <c r="B797" s="3" t="b">
         <v>0</v>
@@ -25405,113 +25426,193 @@
         <v>1</v>
       </c>
       <c r="E797" t="s">
-        <v>2794</v>
+        <v>2785</v>
       </c>
       <c r="F797" s="5" t="s">
-        <v>2799</v>
+        <v>2813</v>
       </c>
       <c r="G797" t="s">
-        <v>2808</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="798" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>2795</v>
+        <v>2783</v>
       </c>
       <c r="B798" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="C798" s="3" t="b">
+      <c r="C798" t="b">
         <v>1</v>
       </c>
       <c r="E798" t="s">
-        <v>2795</v>
+        <v>2784</v>
       </c>
       <c r="F798" s="5" t="s">
-        <v>2798</v>
+        <v>2814</v>
       </c>
       <c r="G798" t="s">
-        <v>2809</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="799" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>2796</v>
-      </c>
-      <c r="B799" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C799" s="3" t="b">
+        <v>2786</v>
+      </c>
+      <c r="B799" t="b">
+        <v>0</v>
+      </c>
+      <c r="C799" t="b">
         <v>1</v>
       </c>
       <c r="E799" t="s">
-        <v>2796</v>
+        <v>2787</v>
       </c>
       <c r="F799" s="5" t="s">
-        <v>2800</v>
+        <v>2788</v>
       </c>
       <c r="G799" t="s">
-        <v>2810</v>
+        <v>2806</v>
       </c>
     </row>
     <row r="800" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>2816</v>
-      </c>
-      <c r="B800" t="b">
-        <v>0</v>
-      </c>
-      <c r="C800" t="b">
+        <v>2793</v>
+      </c>
+      <c r="B800" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C800" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E800" t="s">
-        <v>2817</v>
+        <v>2793</v>
       </c>
       <c r="F800" s="5" t="s">
-        <v>2818</v>
+        <v>2797</v>
       </c>
       <c r="G800" t="s">
-        <v>2828</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="801" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B801" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C801" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E801" t="s">
+        <v>2794</v>
+      </c>
+      <c r="F801" s="5" t="s">
+        <v>2799</v>
+      </c>
+      <c r="G801" t="s">
+        <v>2808</v>
+      </c>
+    </row>
+    <row r="802" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A802" t="s">
+        <v>2795</v>
+      </c>
+      <c r="B802" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C802" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E802" t="s">
+        <v>2795</v>
+      </c>
+      <c r="F802" s="5" t="s">
+        <v>2798</v>
+      </c>
+      <c r="G802" t="s">
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="803" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A803" t="s">
+        <v>2796</v>
+      </c>
+      <c r="B803" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C803" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E803" t="s">
+        <v>2796</v>
+      </c>
+      <c r="F803" s="5" t="s">
+        <v>2800</v>
+      </c>
+      <c r="G803" t="s">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="804" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A804" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B804" t="b">
+        <v>0</v>
+      </c>
+      <c r="C804" t="b">
+        <v>1</v>
+      </c>
+      <c r="E804" t="s">
+        <v>2817</v>
+      </c>
+      <c r="F804" s="5" t="s">
+        <v>2818</v>
+      </c>
+      <c r="G804" t="s">
+        <v>2828</v>
+      </c>
+    </row>
+    <row r="805" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A805" t="s">
         <v>2826</v>
       </c>
-      <c r="B801" t="b">
-        <v>0</v>
-      </c>
-      <c r="C801" t="b">
-        <v>1</v>
-      </c>
-      <c r="E801" t="s">
+      <c r="B805" t="b">
+        <v>0</v>
+      </c>
+      <c r="C805" t="b">
+        <v>1</v>
+      </c>
+      <c r="E805" t="s">
         <v>2826</v>
       </c>
-      <c r="F801" s="5" t="s">
+      <c r="F805" s="5" t="s">
         <v>2827</v>
       </c>
-      <c r="G801" t="s">
+      <c r="G805" t="s">
         <v>1430</v>
       </c>
     </row>
-    <row r="802" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A802" s="3" t="s">
+    <row r="806" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A806" s="3" t="s">
         <v>2829</v>
       </c>
-      <c r="B802" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C802" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D802" s="3"/>
-      <c r="E802" s="3" t="s">
+      <c r="B806" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C806" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D806" s="3"/>
+      <c r="E806" s="3" t="s">
         <v>2831</v>
       </c>
-      <c r="F802" s="5" t="s">
+      <c r="F806" s="5" t="s">
         <v>2832</v>
       </c>
-      <c r="G802" s="3" t="s">
+      <c r="G806" s="3" t="s">
         <v>2830</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More graceful experience when losing access to a company
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5654A7D0-3FBB-42F8-BB1F-547AB46E4A5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133897A2-45E8-4A5C-9BEC-DFF9DEF49CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3272" uniqueCount="2881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3276" uniqueCount="2885">
   <si>
     <t>Key</t>
   </si>
@@ -8679,6 +8679,18 @@
   </si>
   <si>
     <t>不要取消</t>
+  </si>
+  <si>
+    <t>EditDefinition</t>
+  </si>
+  <si>
+    <t>Edit Definition</t>
+  </si>
+  <si>
+    <t>تعديل التعريف</t>
+  </si>
+  <si>
+    <t>编辑定义</t>
   </si>
 </sst>
 </file>
@@ -9075,12 +9087,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G816"/>
+  <dimension ref="A1:G817"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A786" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E815" sqref="E815"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9185,10 +9197,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
@@ -25931,6 +25943,26 @@
       </c>
       <c r="G816" t="s">
         <v>2880</v>
+      </c>
+    </row>
+    <row r="817" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A817" t="s">
+        <v>2881</v>
+      </c>
+      <c r="B817" t="b">
+        <v>0</v>
+      </c>
+      <c r="C817" t="b">
+        <v>1</v>
+      </c>
+      <c r="E817" t="s">
+        <v>2882</v>
+      </c>
+      <c r="F817" s="5" t="s">
+        <v>2883</v>
+      </c>
+      <c r="G817" t="s">
+        <v>2884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new resource properties for PPE
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\source\repos\Tellma\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3A86C9-B6C7-4615-8E03-997DB47B6549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226146FB-E9D6-49E5-AD3C-1C3DC47131AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09F7BBB4-81EA-4503-B8DD-8985A501E98F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Translations" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$756</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Translations!$A$1:$G$762</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3324" uniqueCount="2935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3348" uniqueCount="2958">
   <si>
     <t>Key</t>
   </si>
@@ -8842,6 +8842,75 @@
   </si>
   <si>
     <t>تصنيفات موروثة</t>
+  </si>
+  <si>
+    <t>Resource_CostObject</t>
+  </si>
+  <si>
+    <t>Resource_ExpenseEntryType</t>
+  </si>
+  <si>
+    <t>Resource_ExpenseCenter</t>
+  </si>
+  <si>
+    <t>Resource_InvestmentCenter</t>
+  </si>
+  <si>
+    <t>Resource_ResidualMonetaryValue</t>
+  </si>
+  <si>
+    <t>Resource_ResidualValue</t>
+  </si>
+  <si>
+    <t>Cost Object</t>
+  </si>
+  <si>
+    <t>Expense Center</t>
+  </si>
+  <si>
+    <t>Investment Center</t>
+  </si>
+  <si>
+    <t>Residual Value</t>
+  </si>
+  <si>
+    <t>Residual Monetary Value</t>
+  </si>
+  <si>
+    <t>成本对象</t>
+  </si>
+  <si>
+    <t>费用条目类型</t>
+  </si>
+  <si>
+    <t>费用中心</t>
+  </si>
+  <si>
+    <t>投资中心</t>
+  </si>
+  <si>
+    <t>剩余货币价值</t>
+  </si>
+  <si>
+    <t>剩余价值</t>
+  </si>
+  <si>
+    <t>مركز الاستثمار</t>
+  </si>
+  <si>
+    <t>مركز التكلفة</t>
+  </si>
+  <si>
+    <t>مركز المصروف</t>
+  </si>
+  <si>
+    <t>الغرض</t>
+  </si>
+  <si>
+    <t>قيمة الخردة</t>
+  </si>
+  <si>
+    <t>مبلغ الخردة</t>
   </si>
 </sst>
 </file>
@@ -9238,12 +9307,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FEE134-3B22-427F-8E5A-2A7F994BE2AC}">
-  <dimension ref="A1:G829"/>
+  <dimension ref="A1:G835"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A505" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A683" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F527" sqref="F527"/>
+      <selection pane="bottomLeft" activeCell="F699" sqref="F699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23761,215 +23830,215 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="701" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A701" t="s">
-        <v>2153</v>
-      </c>
-      <c r="B701" t="b">
-        <v>0</v>
-      </c>
-      <c r="C701" t="b">
-        <v>1</v>
-      </c>
-      <c r="D701" t="s">
-        <v>2158</v>
-      </c>
-      <c r="E701" t="s">
-        <v>2153</v>
+    <row r="701" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A701" s="3" t="s">
+        <v>2935</v>
+      </c>
+      <c r="B701" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C701" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E701" s="3" t="s">
+        <v>2941</v>
       </c>
       <c r="F701" s="5" t="s">
-        <v>2156</v>
-      </c>
-      <c r="G701" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="702" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A702" t="s">
-        <v>2154</v>
-      </c>
-      <c r="B702" t="b">
-        <v>0</v>
-      </c>
-      <c r="C702" t="b">
-        <v>1</v>
-      </c>
-      <c r="D702" t="s">
-        <v>2158</v>
-      </c>
-      <c r="E702" t="s">
-        <v>2155</v>
+        <v>2953</v>
+      </c>
+      <c r="G701" s="3" t="s">
+        <v>2946</v>
+      </c>
+    </row>
+    <row r="702" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A702" s="3" t="s">
+        <v>2936</v>
+      </c>
+      <c r="B702" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C702" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E702" s="3" t="s">
+        <v>2307</v>
       </c>
       <c r="F702" s="5" t="s">
-        <v>2157</v>
-      </c>
-      <c r="G702" t="s">
-        <v>2160</v>
-      </c>
-    </row>
-    <row r="703" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A703" t="s">
-        <v>2451</v>
-      </c>
-      <c r="B703" t="b">
+        <v>2955</v>
+      </c>
+      <c r="G702" s="3" t="s">
+        <v>2947</v>
+      </c>
+    </row>
+    <row r="703" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A703" s="3" t="s">
+        <v>2937</v>
+      </c>
+      <c r="B703" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C703" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E703" t="s">
-        <v>2453</v>
+      <c r="E703" s="3" t="s">
+        <v>2942</v>
       </c>
       <c r="F703" s="5" t="s">
-        <v>2162</v>
-      </c>
-      <c r="G703" t="s">
-        <v>2163</v>
-      </c>
-    </row>
-    <row r="704" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2954</v>
+      </c>
+      <c r="G703" s="3" t="s">
+        <v>2948</v>
+      </c>
+    </row>
+    <row r="704" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A704" s="3" t="s">
-        <v>2452</v>
-      </c>
-      <c r="B704" t="b">
+        <v>2938</v>
+      </c>
+      <c r="B704" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C704" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E704" t="s">
-        <v>2454</v>
+      <c r="E704" s="3" t="s">
+        <v>2943</v>
       </c>
       <c r="F704" s="5" t="s">
-        <v>2161</v>
-      </c>
-      <c r="G704" t="s">
-        <v>2163</v>
-      </c>
-    </row>
-    <row r="705" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A705" t="s">
-        <v>2210</v>
-      </c>
-      <c r="B705" t="b">
-        <v>1</v>
-      </c>
-      <c r="C705" t="b">
-        <v>1</v>
-      </c>
-      <c r="E705" t="s">
-        <v>2199</v>
+        <v>2952</v>
+      </c>
+      <c r="G704" s="3" t="s">
+        <v>2949</v>
+      </c>
+    </row>
+    <row r="705" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A705" s="3" t="s">
+        <v>2939</v>
+      </c>
+      <c r="B705" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C705" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E705" s="3" t="s">
+        <v>2945</v>
       </c>
       <c r="F705" s="5" t="s">
-        <v>2200</v>
-      </c>
-      <c r="G705" t="s">
-        <v>2219</v>
-      </c>
-    </row>
-    <row r="706" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A706" t="s">
-        <v>2212</v>
-      </c>
-      <c r="B706" t="b">
-        <v>1</v>
-      </c>
-      <c r="C706" t="b">
-        <v>0</v>
-      </c>
-      <c r="E706" t="s">
-        <v>2211</v>
+        <v>2957</v>
+      </c>
+      <c r="G705" s="3" t="s">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="706" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A706" s="3" t="s">
+        <v>2940</v>
+      </c>
+      <c r="B706" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C706" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E706" s="3" t="s">
+        <v>2944</v>
       </c>
       <c r="F706" s="5" t="s">
-        <v>2213</v>
-      </c>
-      <c r="G706" t="s">
-        <v>2220</v>
+        <v>2956</v>
+      </c>
+      <c r="G706" s="3" t="s">
+        <v>2951</v>
       </c>
     </row>
     <row r="707" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>2216</v>
+        <v>2153</v>
       </c>
       <c r="B707" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C707" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D707" t="s">
+        <v>2158</v>
       </c>
       <c r="E707" t="s">
-        <v>2214</v>
+        <v>2153</v>
       </c>
       <c r="F707" s="5" t="s">
-        <v>2215</v>
+        <v>2156</v>
       </c>
       <c r="G707" t="s">
-        <v>2221</v>
-      </c>
-    </row>
-    <row r="708" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A708" s="3" t="s">
-        <v>2854</v>
-      </c>
-      <c r="B708" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C708" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E708" s="3" t="s">
-        <v>2855</v>
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="708" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
+        <v>2154</v>
+      </c>
+      <c r="B708" t="b">
+        <v>0</v>
+      </c>
+      <c r="C708" t="b">
+        <v>1</v>
+      </c>
+      <c r="D708" t="s">
+        <v>2158</v>
+      </c>
+      <c r="E708" t="s">
+        <v>2155</v>
       </c>
       <c r="F708" s="5" t="s">
-        <v>2856</v>
-      </c>
-      <c r="G708" s="3" t="s">
-        <v>2222</v>
+        <v>2157</v>
+      </c>
+      <c r="G708" t="s">
+        <v>2160</v>
       </c>
     </row>
     <row r="709" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>2223</v>
+        <v>2451</v>
       </c>
       <c r="B709" t="b">
-        <v>0</v>
-      </c>
-      <c r="C709" t="b">
+        <v>1</v>
+      </c>
+      <c r="C709" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E709" t="s">
-        <v>2226</v>
+        <v>2453</v>
       </c>
       <c r="F709" s="5" t="s">
-        <v>2227</v>
+        <v>2162</v>
       </c>
       <c r="G709" t="s">
-        <v>2236</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="710" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A710" t="s">
-        <v>2224</v>
+      <c r="A710" s="3" t="s">
+        <v>2452</v>
       </c>
       <c r="B710" t="b">
-        <v>0</v>
-      </c>
-      <c r="C710" t="b">
+        <v>1</v>
+      </c>
+      <c r="C710" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E710" t="s">
-        <v>2225</v>
+        <v>2454</v>
       </c>
       <c r="F710" s="5" t="s">
-        <v>2228</v>
+        <v>2161</v>
       </c>
       <c r="G710" t="s">
-        <v>2237</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="711" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>2230</v>
+        <v>2210</v>
       </c>
       <c r="B711" t="b">
         <v>1</v>
@@ -23978,98 +24047,98 @@
         <v>1</v>
       </c>
       <c r="E711" t="s">
-        <v>2232</v>
+        <v>2199</v>
       </c>
       <c r="F711" s="5" t="s">
-        <v>2235</v>
+        <v>2200</v>
       </c>
       <c r="G711" t="s">
-        <v>2238</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="712" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>2231</v>
-      </c>
-      <c r="B712" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C712" s="3" t="b">
-        <v>1</v>
+        <v>2212</v>
+      </c>
+      <c r="B712" t="b">
+        <v>1</v>
+      </c>
+      <c r="C712" t="b">
+        <v>0</v>
       </c>
       <c r="E712" t="s">
-        <v>491</v>
+        <v>2211</v>
       </c>
       <c r="F712" s="5" t="s">
-        <v>490</v>
+        <v>2213</v>
       </c>
       <c r="G712" t="s">
-        <v>1357</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>2292</v>
-      </c>
-      <c r="B713" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C713" s="3" t="b">
-        <v>1</v>
+        <v>2216</v>
+      </c>
+      <c r="B713" t="b">
+        <v>1</v>
+      </c>
+      <c r="C713" t="b">
+        <v>0</v>
       </c>
       <c r="E713" t="s">
-        <v>2233</v>
+        <v>2214</v>
       </c>
       <c r="F713" s="5" t="s">
-        <v>2234</v>
+        <v>2215</v>
       </c>
       <c r="G713" t="s">
-        <v>2239</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="714" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A714" s="3" t="s">
-        <v>2778</v>
+        <v>2854</v>
       </c>
       <c r="B714" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C714" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E714" s="3" t="s">
-        <v>2780</v>
+        <v>2855</v>
       </c>
       <c r="F714" s="5" t="s">
-        <v>2782</v>
+        <v>2856</v>
       </c>
       <c r="G714" s="3" t="s">
-        <v>2783</v>
-      </c>
-    </row>
-    <row r="715" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A715" s="3" t="s">
-        <v>2779</v>
-      </c>
-      <c r="B715" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C715" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E715" s="3" t="s">
-        <v>2781</v>
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="715" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A715" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B715" t="b">
+        <v>0</v>
+      </c>
+      <c r="C715" t="b">
+        <v>1</v>
+      </c>
+      <c r="E715" t="s">
+        <v>2226</v>
       </c>
       <c r="F715" s="5" t="s">
-        <v>2308</v>
-      </c>
-      <c r="G715" s="3" t="s">
-        <v>2784</v>
+        <v>2227</v>
+      </c>
+      <c r="G715" t="s">
+        <v>2236</v>
       </c>
     </row>
     <row r="716" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>2241</v>
+        <v>2224</v>
       </c>
       <c r="B716" t="b">
         <v>0</v>
@@ -24077,122 +24146,119 @@
       <c r="C716" t="b">
         <v>1</v>
       </c>
-      <c r="D716" t="s">
-        <v>2242</v>
-      </c>
       <c r="E716" t="s">
-        <v>2244</v>
+        <v>2225</v>
       </c>
       <c r="F716" s="5" t="s">
-        <v>2243</v>
-      </c>
-      <c r="G716" s="3" t="s">
-        <v>2249</v>
+        <v>2228</v>
+      </c>
+      <c r="G716" t="s">
+        <v>2237</v>
       </c>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>2273</v>
+        <v>2230</v>
       </c>
       <c r="B717" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C717" t="b">
         <v>1</v>
       </c>
       <c r="E717" t="s">
-        <v>2274</v>
+        <v>2232</v>
       </c>
       <c r="F717" s="5" t="s">
-        <v>2290</v>
+        <v>2235</v>
       </c>
       <c r="G717" t="s">
-        <v>2285</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="718" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>2275</v>
-      </c>
-      <c r="B718" t="b">
-        <v>0</v>
-      </c>
-      <c r="C718" t="b">
+        <v>2231</v>
+      </c>
+      <c r="B718" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C718" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E718" t="s">
-        <v>2291</v>
+        <v>491</v>
       </c>
       <c r="F718" s="5" t="s">
-        <v>2278</v>
+        <v>490</v>
       </c>
       <c r="G718" t="s">
-        <v>2286</v>
-      </c>
-    </row>
-    <row r="719" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A719" s="3" t="s">
-        <v>2281</v>
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="719" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A719" t="s">
+        <v>2292</v>
       </c>
       <c r="B719" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C719" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E719" s="3" t="s">
-        <v>2282</v>
+      <c r="E719" t="s">
+        <v>2233</v>
       </c>
       <c r="F719" s="5" t="s">
-        <v>2283</v>
-      </c>
-      <c r="G719" s="3" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="720" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A720" t="s">
-        <v>2276</v>
-      </c>
-      <c r="B720" t="b">
-        <v>0</v>
-      </c>
-      <c r="C720" t="b">
-        <v>1</v>
-      </c>
-      <c r="E720" t="s">
-        <v>2276</v>
+        <v>2234</v>
+      </c>
+      <c r="G719" t="s">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="720" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A720" s="3" t="s">
+        <v>2778</v>
+      </c>
+      <c r="B720" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C720" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E720" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="F720" s="5" t="s">
-        <v>2277</v>
-      </c>
-      <c r="G720" t="s">
-        <v>2288</v>
-      </c>
-    </row>
-    <row r="721" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A721" t="s">
-        <v>2280</v>
-      </c>
-      <c r="B721" t="b">
-        <v>0</v>
-      </c>
-      <c r="C721" t="b">
-        <v>1</v>
-      </c>
-      <c r="E721" t="s">
-        <v>2279</v>
+        <v>2782</v>
+      </c>
+      <c r="G720" s="3" t="s">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="721" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A721" s="3" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B721" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C721" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E721" s="3" t="s">
+        <v>2781</v>
       </c>
       <c r="F721" s="5" t="s">
-        <v>2284</v>
-      </c>
-      <c r="G721" t="s">
-        <v>2289</v>
+        <v>2308</v>
+      </c>
+      <c r="G721" s="3" t="s">
+        <v>2784</v>
       </c>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>494</v>
+        <v>2241</v>
       </c>
       <c r="B722" t="b">
         <v>0</v>
@@ -24200,19 +24266,22 @@
       <c r="C722" t="b">
         <v>1</v>
       </c>
+      <c r="D722" t="s">
+        <v>2242</v>
+      </c>
       <c r="E722" t="s">
-        <v>494</v>
+        <v>2244</v>
       </c>
       <c r="F722" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="G722" t="s">
-        <v>1358</v>
+        <v>2243</v>
+      </c>
+      <c r="G722" s="3" t="s">
+        <v>2249</v>
       </c>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>2305</v>
+        <v>2273</v>
       </c>
       <c r="B723" t="b">
         <v>0</v>
@@ -24221,18 +24290,18 @@
         <v>1</v>
       </c>
       <c r="E723" t="s">
-        <v>2305</v>
+        <v>2274</v>
       </c>
       <c r="F723" s="5" t="s">
-        <v>2306</v>
+        <v>2290</v>
       </c>
       <c r="G723" t="s">
-        <v>2316</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>2314</v>
+        <v>2275</v>
       </c>
       <c r="B724" t="b">
         <v>0</v>
@@ -24241,318 +24310,318 @@
         <v>1</v>
       </c>
       <c r="E724" t="s">
-        <v>2315</v>
+        <v>2291</v>
       </c>
       <c r="F724" s="5" t="s">
-        <v>2318</v>
+        <v>2278</v>
       </c>
       <c r="G724" t="s">
-        <v>2317</v>
-      </c>
-    </row>
-    <row r="725" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A725" t="s">
-        <v>2378</v>
-      </c>
-      <c r="B725" t="b">
-        <v>1</v>
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="725" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A725" s="3" t="s">
+        <v>2281</v>
+      </c>
+      <c r="B725" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="C725" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E725" t="s">
-        <v>2319</v>
+      <c r="E725" s="3" t="s">
+        <v>2282</v>
       </c>
       <c r="F725" s="5" t="s">
-        <v>2326</v>
-      </c>
-      <c r="G725" t="s">
-        <v>2333</v>
+        <v>2283</v>
+      </c>
+      <c r="G725" s="3" t="s">
+        <v>2287</v>
       </c>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>2379</v>
-      </c>
-      <c r="B726" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C726" s="3" t="b">
+        <v>2276</v>
+      </c>
+      <c r="B726" t="b">
+        <v>0</v>
+      </c>
+      <c r="C726" t="b">
         <v>1</v>
       </c>
       <c r="E726" t="s">
-        <v>2320</v>
+        <v>2276</v>
       </c>
       <c r="F726" s="5" t="s">
-        <v>2327</v>
+        <v>2277</v>
       </c>
       <c r="G726" t="s">
-        <v>2339</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>2380</v>
-      </c>
-      <c r="B727" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C727" s="3" t="b">
+        <v>2280</v>
+      </c>
+      <c r="B727" t="b">
+        <v>0</v>
+      </c>
+      <c r="C727" t="b">
         <v>1</v>
       </c>
       <c r="E727" t="s">
-        <v>2321</v>
+        <v>2279</v>
       </c>
       <c r="F727" s="5" t="s">
-        <v>2328</v>
+        <v>2284</v>
       </c>
       <c r="G727" t="s">
-        <v>2334</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>2381</v>
-      </c>
-      <c r="B728" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C728" s="3" t="b">
+        <v>494</v>
+      </c>
+      <c r="B728" t="b">
+        <v>0</v>
+      </c>
+      <c r="C728" t="b">
         <v>1</v>
       </c>
       <c r="E728" t="s">
-        <v>2323</v>
+        <v>494</v>
       </c>
       <c r="F728" s="5" t="s">
-        <v>2330</v>
+        <v>493</v>
       </c>
       <c r="G728" t="s">
-        <v>2335</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>2382</v>
-      </c>
-      <c r="B729" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C729" s="3" t="b">
+        <v>2305</v>
+      </c>
+      <c r="B729" t="b">
+        <v>0</v>
+      </c>
+      <c r="C729" t="b">
         <v>1</v>
       </c>
       <c r="E729" t="s">
-        <v>2324</v>
+        <v>2305</v>
       </c>
       <c r="F729" s="5" t="s">
-        <v>2331</v>
+        <v>2306</v>
       </c>
       <c r="G729" t="s">
-        <v>2336</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>2383</v>
-      </c>
-      <c r="B730" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C730" s="3" t="b">
+        <v>2314</v>
+      </c>
+      <c r="B730" t="b">
+        <v>0</v>
+      </c>
+      <c r="C730" t="b">
         <v>1</v>
       </c>
       <c r="E730" t="s">
-        <v>2322</v>
+        <v>2315</v>
       </c>
       <c r="F730" s="5" t="s">
-        <v>2329</v>
+        <v>2318</v>
       </c>
       <c r="G730" t="s">
-        <v>2337</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>2384</v>
-      </c>
-      <c r="B731" s="3" t="b">
+        <v>2378</v>
+      </c>
+      <c r="B731" t="b">
         <v>1</v>
       </c>
       <c r="C731" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E731" t="s">
-        <v>2325</v>
+        <v>2319</v>
       </c>
       <c r="F731" s="5" t="s">
-        <v>2332</v>
+        <v>2326</v>
       </c>
       <c r="G731" t="s">
-        <v>2338</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="732" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>2400</v>
-      </c>
-      <c r="B732" t="b">
-        <v>1</v>
-      </c>
-      <c r="C732" t="b">
+        <v>2379</v>
+      </c>
+      <c r="B732" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C732" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E732" t="s">
-        <v>2402</v>
+        <v>2320</v>
       </c>
       <c r="F732" s="5" t="s">
-        <v>2404</v>
+        <v>2327</v>
       </c>
       <c r="G732" t="s">
-        <v>2406</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>2401</v>
-      </c>
-      <c r="B733" t="b">
-        <v>1</v>
-      </c>
-      <c r="C733" t="b">
+        <v>2380</v>
+      </c>
+      <c r="B733" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C733" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E733" t="s">
-        <v>2403</v>
+        <v>2321</v>
       </c>
       <c r="F733" s="5" t="s">
-        <v>2405</v>
+        <v>2328</v>
       </c>
       <c r="G733" t="s">
-        <v>2407</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>2408</v>
-      </c>
-      <c r="B734" t="b">
-        <v>1</v>
-      </c>
-      <c r="C734" t="b">
+        <v>2381</v>
+      </c>
+      <c r="B734" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C734" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E734" t="s">
-        <v>2409</v>
+        <v>2323</v>
       </c>
       <c r="F734" s="5" t="s">
-        <v>2410</v>
+        <v>2330</v>
       </c>
       <c r="G734" t="s">
-        <v>2413</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>2411</v>
-      </c>
-      <c r="B735" t="b">
-        <v>1</v>
-      </c>
-      <c r="C735" t="b">
+        <v>2382</v>
+      </c>
+      <c r="B735" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C735" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E735" t="s">
-        <v>2424</v>
+        <v>2324</v>
       </c>
       <c r="F735" s="5" t="s">
-        <v>2412</v>
+        <v>2331</v>
       </c>
       <c r="G735" t="s">
-        <v>2414</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="736" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>2421</v>
-      </c>
-      <c r="B736" t="b">
-        <v>0</v>
-      </c>
-      <c r="C736" t="b">
+        <v>2383</v>
+      </c>
+      <c r="B736" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C736" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E736" t="s">
-        <v>2422</v>
+        <v>2322</v>
       </c>
       <c r="F736" s="5" t="s">
-        <v>2423</v>
+        <v>2329</v>
       </c>
       <c r="G736" t="s">
-        <v>2399</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>2447</v>
-      </c>
-      <c r="B737" t="b">
-        <v>0</v>
-      </c>
-      <c r="C737" t="b">
+        <v>2384</v>
+      </c>
+      <c r="B737" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C737" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E737" t="s">
-        <v>2447</v>
+        <v>2325</v>
       </c>
       <c r="F737" s="5" t="s">
-        <v>1069</v>
+        <v>2332</v>
       </c>
       <c r="G737" t="s">
-        <v>2448</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="738" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>2497</v>
+        <v>2400</v>
       </c>
       <c r="B738" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C738" t="b">
         <v>1</v>
       </c>
       <c r="E738" t="s">
-        <v>2497</v>
+        <v>2402</v>
       </c>
       <c r="F738" s="5" t="s">
-        <v>2498</v>
+        <v>2404</v>
       </c>
       <c r="G738" t="s">
-        <v>2501</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="739" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>2499</v>
+        <v>2401</v>
       </c>
       <c r="B739" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C739" t="b">
         <v>1</v>
       </c>
       <c r="E739" t="s">
-        <v>2499</v>
+        <v>2403</v>
       </c>
       <c r="F739" s="5" t="s">
-        <v>2500</v>
+        <v>2405</v>
       </c>
       <c r="G739" t="s">
-        <v>2502</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="740" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A740" s="3" t="s">
-        <v>2522</v>
+      <c r="A740" t="s">
+        <v>2408</v>
       </c>
       <c r="B740" t="b">
         <v>1</v>
@@ -24561,78 +24630,78 @@
         <v>1</v>
       </c>
       <c r="E740" t="s">
-        <v>2523</v>
+        <v>2409</v>
       </c>
       <c r="F740" s="5" t="s">
-        <v>1661</v>
+        <v>2410</v>
       </c>
       <c r="G740" t="s">
-        <v>2524</v>
-      </c>
-    </row>
-    <row r="741" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A741" s="3" t="s">
-        <v>2546</v>
-      </c>
-      <c r="B741" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C741" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E741" s="3" t="s">
-        <v>2547</v>
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="741" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A741" t="s">
+        <v>2411</v>
+      </c>
+      <c r="B741" t="b">
+        <v>1</v>
+      </c>
+      <c r="C741" t="b">
+        <v>1</v>
+      </c>
+      <c r="E741" t="s">
+        <v>2424</v>
       </c>
       <c r="F741" s="5" t="s">
-        <v>2548</v>
-      </c>
-      <c r="G741" s="3" t="s">
-        <v>2549</v>
+        <v>2412</v>
+      </c>
+      <c r="G741" t="s">
+        <v>2414</v>
       </c>
     </row>
     <row r="742" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>2525</v>
+        <v>2421</v>
       </c>
       <c r="B742" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C742" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E742" t="s">
-        <v>2533</v>
+        <v>2422</v>
       </c>
       <c r="F742" s="5" t="s">
-        <v>2534</v>
+        <v>2423</v>
       </c>
       <c r="G742" t="s">
-        <v>2536</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="743" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>2527</v>
+        <v>2447</v>
       </c>
       <c r="B743" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C743" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E743" t="s">
-        <v>2526</v>
+        <v>2447</v>
       </c>
       <c r="F743" s="5" t="s">
-        <v>2535</v>
+        <v>1069</v>
       </c>
       <c r="G743" t="s">
-        <v>2537</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="744" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>2539</v>
+        <v>2497</v>
       </c>
       <c r="B744" t="b">
         <v>0</v>
@@ -24641,18 +24710,18 @@
         <v>1</v>
       </c>
       <c r="E744" t="s">
-        <v>2539</v>
+        <v>2497</v>
       </c>
       <c r="F744" s="5" t="s">
-        <v>2532</v>
+        <v>2498</v>
       </c>
       <c r="G744" t="s">
-        <v>2538</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="745" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>2540</v>
+        <v>2499</v>
       </c>
       <c r="B745" t="b">
         <v>0</v>
@@ -24661,319 +24730,319 @@
         <v>1</v>
       </c>
       <c r="E745" t="s">
-        <v>2540</v>
+        <v>2499</v>
       </c>
       <c r="F745" s="5" t="s">
-        <v>2541</v>
+        <v>2500</v>
       </c>
       <c r="G745" t="s">
-        <v>2562</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="746" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A746" s="3" t="s">
-        <v>2545</v>
-      </c>
-      <c r="B746" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C746" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D746" s="3"/>
-      <c r="E746" s="3" t="s">
-        <v>2542</v>
+        <v>2522</v>
+      </c>
+      <c r="B746" t="b">
+        <v>1</v>
+      </c>
+      <c r="C746" t="b">
+        <v>1</v>
+      </c>
+      <c r="E746" t="s">
+        <v>2523</v>
       </c>
       <c r="F746" s="5" t="s">
-        <v>2543</v>
-      </c>
-      <c r="G746" s="3" t="s">
-        <v>2544</v>
-      </c>
-    </row>
-    <row r="747" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A747" t="s">
-        <v>2550</v>
-      </c>
-      <c r="B747" t="b">
-        <v>0</v>
-      </c>
-      <c r="C747" t="b">
-        <v>1</v>
-      </c>
-      <c r="E747" t="s">
-        <v>2551</v>
+        <v>1661</v>
+      </c>
+      <c r="G746" t="s">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="747" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A747" s="3" t="s">
+        <v>2546</v>
+      </c>
+      <c r="B747" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C747" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E747" s="3" t="s">
+        <v>2547</v>
       </c>
       <c r="F747" s="5" t="s">
-        <v>2552</v>
-      </c>
-      <c r="G747" t="s">
-        <v>2563</v>
+        <v>2548</v>
+      </c>
+      <c r="G747" s="3" t="s">
+        <v>2549</v>
       </c>
     </row>
     <row r="748" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>2556</v>
-      </c>
-      <c r="B748" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C748" s="3" t="b">
-        <v>1</v>
+        <v>2525</v>
+      </c>
+      <c r="B748" t="b">
+        <v>1</v>
+      </c>
+      <c r="C748" t="b">
+        <v>0</v>
       </c>
       <c r="E748" t="s">
-        <v>2560</v>
+        <v>2533</v>
       </c>
       <c r="F748" s="5" t="s">
-        <v>2559</v>
+        <v>2534</v>
       </c>
       <c r="G748" t="s">
-        <v>2564</v>
+        <v>2536</v>
       </c>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>2557</v>
-      </c>
-      <c r="B749" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C749" s="3" t="b">
-        <v>1</v>
+        <v>2527</v>
+      </c>
+      <c r="B749" t="b">
+        <v>1</v>
+      </c>
+      <c r="C749" t="b">
+        <v>0</v>
       </c>
       <c r="E749" t="s">
-        <v>2561</v>
+        <v>2526</v>
       </c>
       <c r="F749" s="5" t="s">
-        <v>2558</v>
+        <v>2535</v>
       </c>
       <c r="G749" t="s">
-        <v>2565</v>
+        <v>2537</v>
       </c>
     </row>
     <row r="750" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
+        <v>2539</v>
+      </c>
+      <c r="B750" t="b">
+        <v>0</v>
+      </c>
+      <c r="C750" t="b">
+        <v>1</v>
+      </c>
+      <c r="E750" t="s">
+        <v>2539</v>
+      </c>
+      <c r="F750" s="5" t="s">
+        <v>2532</v>
+      </c>
+      <c r="G750" t="s">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="751" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A751" t="s">
+        <v>2540</v>
+      </c>
+      <c r="B751" t="b">
+        <v>0</v>
+      </c>
+      <c r="C751" t="b">
+        <v>1</v>
+      </c>
+      <c r="E751" t="s">
+        <v>2540</v>
+      </c>
+      <c r="F751" s="5" t="s">
+        <v>2541</v>
+      </c>
+      <c r="G751" t="s">
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="752" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A752" s="3" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B752" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C752" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D752" s="3"/>
+      <c r="E752" s="3" t="s">
+        <v>2542</v>
+      </c>
+      <c r="F752" s="5" t="s">
+        <v>2543</v>
+      </c>
+      <c r="G752" s="3" t="s">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="753" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A753" t="s">
+        <v>2550</v>
+      </c>
+      <c r="B753" t="b">
+        <v>0</v>
+      </c>
+      <c r="C753" t="b">
+        <v>1</v>
+      </c>
+      <c r="E753" t="s">
+        <v>2551</v>
+      </c>
+      <c r="F753" s="5" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G753" t="s">
+        <v>2563</v>
+      </c>
+    </row>
+    <row r="754" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A754" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B754" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C754" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E754" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F754" s="5" t="s">
+        <v>2559</v>
+      </c>
+      <c r="G754" t="s">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="755" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A755" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B755" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C755" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E755" t="s">
+        <v>2561</v>
+      </c>
+      <c r="F755" s="5" t="s">
+        <v>2558</v>
+      </c>
+      <c r="G755" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="756" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A756" t="s">
         <v>2566</v>
       </c>
-      <c r="B750" t="b">
-        <v>1</v>
-      </c>
-      <c r="C750" t="b">
-        <v>0</v>
-      </c>
-      <c r="E750" t="s">
+      <c r="B756" t="b">
+        <v>1</v>
+      </c>
+      <c r="C756" t="b">
+        <v>0</v>
+      </c>
+      <c r="E756" t="s">
         <v>2567</v>
       </c>
-      <c r="F750" s="5" t="s">
+      <c r="F756" s="5" t="s">
         <v>2568</v>
       </c>
-      <c r="G750" t="s">
+      <c r="G756" t="s">
         <v>2569</v>
       </c>
     </row>
-    <row r="751" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A751" s="3" t="s">
+    <row r="757" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A757" s="3" t="s">
         <v>2581</v>
       </c>
-      <c r="B751" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C751" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E751" s="3" t="s">
+      <c r="B757" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C757" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E757" s="3" t="s">
         <v>2583</v>
       </c>
-      <c r="F751" s="5" t="s">
+      <c r="F757" s="5" t="s">
         <v>2585</v>
       </c>
-      <c r="G751" s="3" t="s">
+      <c r="G757" s="3" t="s">
         <v>2587</v>
       </c>
     </row>
-    <row r="752" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A752" s="3" t="s">
+    <row r="758" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A758" s="3" t="s">
         <v>2582</v>
       </c>
-      <c r="B752" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C752" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E752" s="3" t="s">
+      <c r="B758" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C758" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E758" s="3" t="s">
         <v>2584</v>
       </c>
-      <c r="F752" s="5" t="s">
+      <c r="F758" s="5" t="s">
         <v>2586</v>
       </c>
-      <c r="G752" s="3" t="s">
+      <c r="G758" s="3" t="s">
         <v>2588</v>
       </c>
     </row>
-    <row r="753" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A753" t="s">
+    <row r="759" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A759" t="s">
         <v>2600</v>
       </c>
-      <c r="B753" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C753" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E753" s="3" t="s">
+      <c r="B759" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C759" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E759" s="3" t="s">
         <v>2857</v>
       </c>
-      <c r="F753" s="5" t="s">
+      <c r="F759" s="5" t="s">
         <v>2858</v>
       </c>
-      <c r="G753" s="3" t="s">
+      <c r="G759" s="3" t="s">
         <v>2613</v>
       </c>
     </row>
-    <row r="754" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A754" t="s">
+    <row r="760" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A760" t="s">
         <v>2601</v>
       </c>
-      <c r="B754" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C754" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E754" s="3" t="s">
+      <c r="B760" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C760" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E760" s="3" t="s">
         <v>2608</v>
       </c>
-      <c r="F754" s="5" t="s">
+      <c r="F760" s="5" t="s">
         <v>2609</v>
       </c>
-      <c r="G754" s="3" t="s">
+      <c r="G760" s="3" t="s">
         <v>2614</v>
-      </c>
-    </row>
-    <row r="755" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A755" s="3" t="s">
-        <v>2602</v>
-      </c>
-      <c r="B755" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C755" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E755" s="3" t="s">
-        <v>2607</v>
-      </c>
-      <c r="F755" s="5" t="s">
-        <v>2610</v>
-      </c>
-      <c r="G755" s="3" t="s">
-        <v>2615</v>
-      </c>
-    </row>
-    <row r="756" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A756" s="3" t="s">
-        <v>2603</v>
-      </c>
-      <c r="B756" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C756" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E756" s="3" t="s">
-        <v>2606</v>
-      </c>
-      <c r="F756" s="5" t="s">
-        <v>2611</v>
-      </c>
-      <c r="G756" s="3" t="s">
-        <v>2616</v>
-      </c>
-    </row>
-    <row r="757" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A757" t="s">
-        <v>2604</v>
-      </c>
-      <c r="B757" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C757" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E757" t="s">
-        <v>2605</v>
-      </c>
-      <c r="F757" s="5" t="s">
-        <v>2612</v>
-      </c>
-      <c r="G757" t="s">
-        <v>2617</v>
-      </c>
-    </row>
-    <row r="758" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A758" t="s">
-        <v>2618</v>
-      </c>
-      <c r="B758" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C758" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E758" t="s">
-        <v>2619</v>
-      </c>
-      <c r="F758" s="5" t="s">
-        <v>2620</v>
-      </c>
-      <c r="G758" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="759" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A759" s="3" t="s">
-        <v>2794</v>
-      </c>
-      <c r="B759" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C759" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E759" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="F759" s="5" t="s">
-        <v>2798</v>
-      </c>
-      <c r="G759" s="3" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="760" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A760" s="3" t="s">
-        <v>2795</v>
-      </c>
-      <c r="B760" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C760" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E760" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="F760" s="5" t="s">
-        <v>2799</v>
-      </c>
-      <c r="G760" s="3" t="s">
-        <v>1331</v>
       </c>
     </row>
     <row r="761" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A761" s="3" t="s">
-        <v>2796</v>
+        <v>2602</v>
       </c>
       <c r="B761" s="3" t="b">
         <v>1</v>
@@ -24982,18 +25051,18 @@
         <v>1</v>
       </c>
       <c r="E761" s="3" t="s">
-        <v>437</v>
+        <v>2607</v>
       </c>
       <c r="F761" s="5" t="s">
-        <v>1661</v>
+        <v>2610</v>
       </c>
       <c r="G761" s="3" t="s">
-        <v>1336</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="762" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A762" s="3" t="s">
-        <v>2797</v>
+        <v>2603</v>
       </c>
       <c r="B762" s="3" t="b">
         <v>1</v>
@@ -25002,78 +25071,78 @@
         <v>1</v>
       </c>
       <c r="E762" s="3" t="s">
-        <v>428</v>
+        <v>2606</v>
       </c>
       <c r="F762" s="5" t="s">
-        <v>2800</v>
+        <v>2611</v>
       </c>
       <c r="G762" s="3" t="s">
-        <v>1333</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="763" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>2656</v>
-      </c>
-      <c r="B763" t="b">
-        <v>0</v>
-      </c>
-      <c r="C763" t="b">
+        <v>2604</v>
+      </c>
+      <c r="B763" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C763" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E763" t="s">
-        <v>2657</v>
+        <v>2605</v>
       </c>
       <c r="F763" s="5" t="s">
-        <v>2658</v>
-      </c>
-      <c r="G763" s="2" t="s">
-        <v>2659</v>
-      </c>
-    </row>
-    <row r="764" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A764" s="3" t="s">
-        <v>2660</v>
+        <v>2612</v>
+      </c>
+      <c r="G763" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="764" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A764" t="s">
+        <v>2618</v>
       </c>
       <c r="B764" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C764" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E764" s="3" t="s">
-        <v>2661</v>
+      <c r="E764" t="s">
+        <v>2619</v>
       </c>
       <c r="F764" s="5" t="s">
-        <v>2662</v>
-      </c>
-      <c r="G764" s="2" t="s">
-        <v>2663</v>
-      </c>
-    </row>
-    <row r="765" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A765" t="s">
-        <v>2664</v>
-      </c>
-      <c r="B765" t="b">
-        <v>0</v>
-      </c>
-      <c r="C765" t="b">
+        <v>2620</v>
+      </c>
+      <c r="G764" t="s">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="765" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A765" s="3" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B765" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C765" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E765" s="3" t="s">
-        <v>2665</v>
+        <v>416</v>
       </c>
       <c r="F765" s="5" t="s">
-        <v>2666</v>
-      </c>
-      <c r="G765" s="2" t="s">
-        <v>2667</v>
+        <v>2798</v>
+      </c>
+      <c r="G765" s="3" t="s">
+        <v>1329</v>
       </c>
     </row>
     <row r="766" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A766" s="3" t="s">
-        <v>2669</v>
+        <v>2795</v>
       </c>
       <c r="B766" s="3" t="b">
         <v>1</v>
@@ -25082,18 +25151,18 @@
         <v>1</v>
       </c>
       <c r="E766" s="3" t="s">
-        <v>2671</v>
+        <v>422</v>
       </c>
       <c r="F766" s="5" t="s">
-        <v>2675</v>
-      </c>
-      <c r="G766" s="2" t="s">
-        <v>2676</v>
+        <v>2799</v>
+      </c>
+      <c r="G766" s="3" t="s">
+        <v>1331</v>
       </c>
     </row>
     <row r="767" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A767" s="3" t="s">
-        <v>2670</v>
+        <v>2796</v>
       </c>
       <c r="B767" s="3" t="b">
         <v>1</v>
@@ -25102,38 +25171,38 @@
         <v>1</v>
       </c>
       <c r="E767" s="3" t="s">
-        <v>2672</v>
+        <v>437</v>
       </c>
       <c r="F767" s="5" t="s">
-        <v>2674</v>
-      </c>
-      <c r="G767" s="2" t="s">
-        <v>2676</v>
-      </c>
-    </row>
-    <row r="768" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A768" t="s">
-        <v>2668</v>
-      </c>
-      <c r="B768" t="b">
-        <v>1</v>
-      </c>
-      <c r="C768" t="b">
-        <v>1</v>
-      </c>
-      <c r="E768" t="s">
-        <v>499</v>
+        <v>1661</v>
+      </c>
+      <c r="G767" s="3" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="768" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A768" s="3" t="s">
+        <v>2797</v>
+      </c>
+      <c r="B768" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C768" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E768" s="3" t="s">
+        <v>428</v>
       </c>
       <c r="F768" s="5" t="s">
-        <v>2673</v>
-      </c>
-      <c r="G768" t="s">
-        <v>1360</v>
+        <v>2800</v>
+      </c>
+      <c r="G768" s="3" t="s">
+        <v>1333</v>
       </c>
     </row>
     <row r="769" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
-        <v>2677</v>
+        <v>2656</v>
       </c>
       <c r="B769" t="b">
         <v>0</v>
@@ -25142,58 +25211,58 @@
         <v>1</v>
       </c>
       <c r="E769" t="s">
-        <v>2678</v>
+        <v>2657</v>
       </c>
       <c r="F769" s="5" t="s">
-        <v>2679</v>
-      </c>
-      <c r="G769" t="s">
-        <v>2680</v>
-      </c>
-    </row>
-    <row r="770" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A770" t="s">
-        <v>2681</v>
-      </c>
-      <c r="B770" t="b">
-        <v>0</v>
-      </c>
-      <c r="C770" t="b">
-        <v>1</v>
-      </c>
-      <c r="E770" t="s">
-        <v>2682</v>
+        <v>2658</v>
+      </c>
+      <c r="G769" s="2" t="s">
+        <v>2659</v>
+      </c>
+    </row>
+    <row r="770" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A770" s="3" t="s">
+        <v>2660</v>
+      </c>
+      <c r="B770" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C770" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E770" s="3" t="s">
+        <v>2661</v>
       </c>
       <c r="F770" s="5" t="s">
-        <v>2683</v>
-      </c>
-      <c r="G770" t="s">
-        <v>2684</v>
-      </c>
-    </row>
-    <row r="771" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A771" s="3" t="s">
-        <v>2685</v>
-      </c>
-      <c r="B771" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C771" s="3" t="b">
+        <v>2662</v>
+      </c>
+      <c r="G770" s="2" t="s">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="771" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A771" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B771" t="b">
+        <v>0</v>
+      </c>
+      <c r="C771" t="b">
         <v>1</v>
       </c>
       <c r="E771" s="3" t="s">
-        <v>2687</v>
+        <v>2665</v>
       </c>
       <c r="F771" s="5" t="s">
-        <v>2693</v>
-      </c>
-      <c r="G771" s="3" t="s">
-        <v>2699</v>
+        <v>2666</v>
+      </c>
+      <c r="G771" s="2" t="s">
+        <v>2667</v>
       </c>
     </row>
     <row r="772" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A772" s="3" t="s">
-        <v>2686</v>
+        <v>2669</v>
       </c>
       <c r="B772" s="3" t="b">
         <v>1</v>
@@ -25202,18 +25271,18 @@
         <v>1</v>
       </c>
       <c r="E772" s="3" t="s">
-        <v>2688</v>
+        <v>2671</v>
       </c>
       <c r="F772" s="5" t="s">
-        <v>2692</v>
-      </c>
-      <c r="G772" s="3" t="s">
-        <v>2699</v>
-      </c>
-    </row>
-    <row r="773" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A773" t="s">
-        <v>2700</v>
+        <v>2675</v>
+      </c>
+      <c r="G772" s="2" t="s">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="773" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A773" s="3" t="s">
+        <v>2670</v>
       </c>
       <c r="B773" s="3" t="b">
         <v>1</v>
@@ -25221,359 +25290,359 @@
       <c r="C773" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E773" t="s">
-        <v>2689</v>
+      <c r="E773" s="3" t="s">
+        <v>2672</v>
       </c>
       <c r="F773" s="5" t="s">
-        <v>2694</v>
-      </c>
-      <c r="G773" t="s">
-        <v>2696</v>
-      </c>
-    </row>
-    <row r="774" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A774" s="3" t="s">
-        <v>2707</v>
-      </c>
-      <c r="B774" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C774" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E774" s="3" t="s">
-        <v>2709</v>
+        <v>2674</v>
+      </c>
+      <c r="G773" s="2" t="s">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="774" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A774" t="s">
+        <v>2668</v>
+      </c>
+      <c r="B774" t="b">
+        <v>1</v>
+      </c>
+      <c r="C774" t="b">
+        <v>1</v>
+      </c>
+      <c r="E774" t="s">
+        <v>499</v>
       </c>
       <c r="F774" s="5" t="s">
-        <v>2710</v>
-      </c>
-      <c r="G774" s="3" t="s">
-        <v>2711</v>
+        <v>2673</v>
+      </c>
+      <c r="G774" t="s">
+        <v>1360</v>
       </c>
     </row>
     <row r="775" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>2701</v>
-      </c>
-      <c r="B775" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C775" s="3" t="b">
+        <v>2677</v>
+      </c>
+      <c r="B775" t="b">
+        <v>0</v>
+      </c>
+      <c r="C775" t="b">
         <v>1</v>
       </c>
       <c r="E775" t="s">
-        <v>2690</v>
+        <v>2678</v>
       </c>
       <c r="F775" s="5" t="s">
-        <v>676</v>
+        <v>2679</v>
       </c>
       <c r="G775" t="s">
-        <v>2697</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="776" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>2702</v>
-      </c>
-      <c r="B776" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C776" s="3" t="b">
+        <v>2681</v>
+      </c>
+      <c r="B776" t="b">
+        <v>0</v>
+      </c>
+      <c r="C776" t="b">
         <v>1</v>
       </c>
       <c r="E776" t="s">
-        <v>2691</v>
+        <v>2682</v>
       </c>
       <c r="F776" s="5" t="s">
-        <v>2695</v>
+        <v>2683</v>
       </c>
       <c r="G776" t="s">
-        <v>2698</v>
-      </c>
-    </row>
-    <row r="777" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A777" t="s">
-        <v>2703</v>
-      </c>
-      <c r="B777" t="b">
-        <v>1</v>
-      </c>
-      <c r="C777" t="b">
-        <v>1</v>
-      </c>
-      <c r="E777" t="s">
-        <v>2704</v>
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="777" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A777" s="3" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B777" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C777" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E777" s="3" t="s">
+        <v>2687</v>
       </c>
       <c r="F777" s="5" t="s">
-        <v>2705</v>
-      </c>
-      <c r="G777" t="s">
-        <v>2706</v>
-      </c>
-    </row>
-    <row r="778" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A778" t="s">
-        <v>2712</v>
-      </c>
-      <c r="B778" t="b">
-        <v>0</v>
-      </c>
-      <c r="C778" t="b">
-        <v>1</v>
-      </c>
-      <c r="E778" t="s">
-        <v>2689</v>
+        <v>2693</v>
+      </c>
+      <c r="G777" s="3" t="s">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="778" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A778" s="3" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B778" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C778" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E778" s="3" t="s">
+        <v>2688</v>
       </c>
       <c r="F778" s="5" t="s">
-        <v>2694</v>
-      </c>
-      <c r="G778" t="s">
-        <v>2696</v>
+        <v>2692</v>
+      </c>
+      <c r="G778" s="3" t="s">
+        <v>2699</v>
       </c>
     </row>
     <row r="779" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>2713</v>
+        <v>2700</v>
       </c>
       <c r="B779" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C779" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E779" t="s">
-        <v>2716</v>
+        <v>2689</v>
       </c>
       <c r="F779" s="5" t="s">
-        <v>2718</v>
+        <v>2694</v>
       </c>
       <c r="G779" t="s">
-        <v>2720</v>
-      </c>
-    </row>
-    <row r="780" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A780" t="s">
-        <v>2714</v>
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="780" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A780" s="3" t="s">
+        <v>2707</v>
       </c>
       <c r="B780" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C780" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E780" t="s">
-        <v>2708</v>
+      <c r="E780" s="3" t="s">
+        <v>2709</v>
       </c>
       <c r="F780" s="5" t="s">
         <v>2710</v>
       </c>
-      <c r="G780" t="s">
+      <c r="G780" s="3" t="s">
         <v>2711</v>
       </c>
     </row>
     <row r="781" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>2715</v>
+        <v>2701</v>
       </c>
       <c r="B781" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C781" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E781" t="s">
-        <v>2717</v>
+        <v>2690</v>
       </c>
       <c r="F781" s="5" t="s">
-        <v>2719</v>
+        <v>676</v>
       </c>
       <c r="G781" t="s">
-        <v>2721</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="782" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>2722</v>
-      </c>
-      <c r="B782" t="b">
-        <v>0</v>
-      </c>
-      <c r="C782" t="b">
+        <v>2702</v>
+      </c>
+      <c r="B782" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C782" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E782" t="s">
-        <v>2723</v>
+        <v>2691</v>
       </c>
       <c r="F782" s="5" t="s">
-        <v>2724</v>
+        <v>2695</v>
       </c>
       <c r="G782" t="s">
-        <v>2725</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="783" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>2726</v>
+        <v>2703</v>
       </c>
       <c r="B783" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C783" t="b">
         <v>1</v>
       </c>
       <c r="E783" t="s">
-        <v>2727</v>
+        <v>2704</v>
       </c>
       <c r="F783" s="5" t="s">
-        <v>2728</v>
-      </c>
-      <c r="G783" s="2" t="s">
-        <v>2729</v>
+        <v>2705</v>
+      </c>
+      <c r="G783" t="s">
+        <v>2706</v>
       </c>
     </row>
     <row r="784" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>2730</v>
+        <v>2712</v>
       </c>
       <c r="B784" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C784" t="b">
         <v>1</v>
       </c>
       <c r="E784" t="s">
-        <v>2731</v>
+        <v>2689</v>
       </c>
       <c r="F784" s="5" t="s">
-        <v>2732</v>
+        <v>2694</v>
       </c>
       <c r="G784" t="s">
-        <v>2739</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="785" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>2733</v>
+        <v>2713</v>
       </c>
       <c r="B785" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C785" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E785" t="s">
-        <v>1</v>
+        <v>2716</v>
       </c>
       <c r="F785" s="5" t="s">
-        <v>110</v>
+        <v>2718</v>
       </c>
       <c r="G785" t="s">
-        <v>1688</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="786" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>2734</v>
+        <v>2714</v>
       </c>
       <c r="B786" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C786" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E786" t="s">
-        <v>2651</v>
+        <v>2708</v>
       </c>
       <c r="F786" s="5" t="s">
-        <v>2653</v>
+        <v>2710</v>
       </c>
       <c r="G786" t="s">
-        <v>2655</v>
+        <v>2711</v>
       </c>
     </row>
     <row r="787" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>2735</v>
+        <v>2715</v>
       </c>
       <c r="B787" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C787" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E787" t="s">
-        <v>2737</v>
+        <v>2717</v>
       </c>
       <c r="F787" s="5" t="s">
-        <v>2738</v>
+        <v>2719</v>
       </c>
       <c r="G787" t="s">
-        <v>2739</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="788" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>2736</v>
-      </c>
-      <c r="B788" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C788" s="3" t="b">
+        <v>2722</v>
+      </c>
+      <c r="B788" t="b">
+        <v>0</v>
+      </c>
+      <c r="C788" t="b">
         <v>1</v>
       </c>
       <c r="E788" t="s">
-        <v>801</v>
+        <v>2723</v>
       </c>
       <c r="F788" s="5" t="s">
-        <v>810</v>
+        <v>2724</v>
       </c>
       <c r="G788" t="s">
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="789" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A789" s="3" t="s">
-        <v>2742</v>
-      </c>
-      <c r="B789" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C789" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E789" s="3" t="s">
-        <v>377</v>
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="789" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A789" t="s">
+        <v>2726</v>
+      </c>
+      <c r="B789" t="b">
+        <v>0</v>
+      </c>
+      <c r="C789" t="b">
+        <v>1</v>
+      </c>
+      <c r="E789" t="s">
+        <v>2727</v>
       </c>
       <c r="F789" s="5" t="s">
-        <v>2745</v>
-      </c>
-      <c r="G789" s="3" t="s">
-        <v>1316</v>
+        <v>2728</v>
+      </c>
+      <c r="G789" s="2" t="s">
+        <v>2729</v>
       </c>
     </row>
     <row r="790" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>2740</v>
-      </c>
-      <c r="B790" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C790" s="3" t="b">
+        <v>2730</v>
+      </c>
+      <c r="B790" t="b">
+        <v>1</v>
+      </c>
+      <c r="C790" t="b">
         <v>1</v>
       </c>
       <c r="E790" t="s">
-        <v>2651</v>
+        <v>2731</v>
       </c>
       <c r="F790" s="5" t="s">
-        <v>2653</v>
+        <v>2732</v>
       </c>
       <c r="G790" t="s">
-        <v>2655</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="791" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>2741</v>
+        <v>2733</v>
       </c>
       <c r="B791" s="3" t="b">
         <v>1</v>
@@ -25582,138 +25651,138 @@
         <v>1</v>
       </c>
       <c r="E791" t="s">
-        <v>2743</v>
+        <v>1</v>
       </c>
       <c r="F791" s="5" t="s">
-        <v>2744</v>
+        <v>110</v>
       </c>
       <c r="G791" t="s">
-        <v>2746</v>
-      </c>
-    </row>
-    <row r="792" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A792" s="3" t="s">
-        <v>617</v>
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="792" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A792" t="s">
+        <v>2734</v>
       </c>
       <c r="B792" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C792" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E792" s="3" t="s">
-        <v>617</v>
+      <c r="E792" t="s">
+        <v>2651</v>
       </c>
       <c r="F792" s="5" t="s">
-        <v>2240</v>
-      </c>
-      <c r="G792" s="3" t="s">
-        <v>1400</v>
+        <v>2653</v>
+      </c>
+      <c r="G792" t="s">
+        <v>2655</v>
       </c>
     </row>
     <row r="793" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>2808</v>
-      </c>
-      <c r="B793" t="b">
-        <v>0</v>
+        <v>2735</v>
+      </c>
+      <c r="B793" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="C793" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E793" t="s">
-        <v>2754</v>
+        <v>2737</v>
       </c>
       <c r="F793" s="5" t="s">
-        <v>2771</v>
+        <v>2738</v>
       </c>
       <c r="G793" t="s">
-        <v>2762</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="794" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>2809</v>
+        <v>2736</v>
       </c>
       <c r="B794" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C794" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E794" t="s">
-        <v>2774</v>
+        <v>801</v>
       </c>
       <c r="F794" s="5" t="s">
-        <v>2772</v>
+        <v>810</v>
       </c>
       <c r="G794" t="s">
-        <v>2763</v>
-      </c>
-    </row>
-    <row r="795" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A795" t="s">
-        <v>2810</v>
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="795" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A795" s="3" t="s">
+        <v>2742</v>
       </c>
       <c r="B795" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C795" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E795" t="s">
-        <v>2750</v>
+      <c r="E795" s="3" t="s">
+        <v>377</v>
       </c>
       <c r="F795" s="5" t="s">
-        <v>2773</v>
-      </c>
-      <c r="G795" t="s">
-        <v>2764</v>
+        <v>2745</v>
+      </c>
+      <c r="G795" s="3" t="s">
+        <v>1316</v>
       </c>
     </row>
     <row r="796" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>2811</v>
+        <v>2740</v>
       </c>
       <c r="B796" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C796" t="b">
+        <v>1</v>
+      </c>
+      <c r="C796" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E796" t="s">
-        <v>2824</v>
+        <v>2651</v>
       </c>
       <c r="F796" s="5" t="s">
-        <v>2823</v>
+        <v>2653</v>
       </c>
       <c r="G796" t="s">
-        <v>2765</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="797" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>2751</v>
-      </c>
-      <c r="B797" t="b">
-        <v>0</v>
-      </c>
-      <c r="C797" t="b">
+        <v>2741</v>
+      </c>
+      <c r="B797" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C797" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E797" t="s">
-        <v>2752</v>
+        <v>2743</v>
       </c>
       <c r="F797" s="5" t="s">
-        <v>2753</v>
+        <v>2744</v>
       </c>
       <c r="G797" t="s">
-        <v>2766</v>
-      </c>
-    </row>
-    <row r="798" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A798" t="s">
-        <v>2816</v>
+        <v>2746</v>
+      </c>
+    </row>
+    <row r="798" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A798" s="3" t="s">
+        <v>617</v>
       </c>
       <c r="B798" s="3" t="b">
         <v>0</v>
@@ -25721,39 +25790,39 @@
       <c r="C798" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E798" t="s">
-        <v>2755</v>
+      <c r="E798" s="3" t="s">
+        <v>617</v>
       </c>
       <c r="F798" s="5" t="s">
-        <v>2758</v>
-      </c>
-      <c r="G798" t="s">
-        <v>2767</v>
+        <v>2240</v>
+      </c>
+      <c r="G798" s="3" t="s">
+        <v>1400</v>
       </c>
     </row>
     <row r="799" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>2817</v>
-      </c>
-      <c r="B799" s="3" t="b">
+        <v>2808</v>
+      </c>
+      <c r="B799" t="b">
         <v>0</v>
       </c>
       <c r="C799" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E799" t="s">
-        <v>2756</v>
+        <v>2754</v>
       </c>
       <c r="F799" s="5" t="s">
-        <v>2760</v>
+        <v>2771</v>
       </c>
       <c r="G799" t="s">
-        <v>2768</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="800" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>2818</v>
+        <v>2809</v>
       </c>
       <c r="B800" s="3" t="b">
         <v>0</v>
@@ -25762,18 +25831,18 @@
         <v>1</v>
       </c>
       <c r="E800" t="s">
-        <v>2757</v>
+        <v>2774</v>
       </c>
       <c r="F800" s="5" t="s">
-        <v>2759</v>
+        <v>2772</v>
       </c>
       <c r="G800" t="s">
-        <v>2769</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="801" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>2819</v>
+        <v>2810</v>
       </c>
       <c r="B801" s="3" t="b">
         <v>0</v>
@@ -25782,38 +25851,38 @@
         <v>1</v>
       </c>
       <c r="E801" t="s">
-        <v>2820</v>
+        <v>2750</v>
       </c>
       <c r="F801" s="5" t="s">
-        <v>2761</v>
+        <v>2773</v>
       </c>
       <c r="G801" t="s">
-        <v>2770</v>
+        <v>2764</v>
       </c>
     </row>
     <row r="802" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>2775</v>
-      </c>
-      <c r="B802" t="b">
+        <v>2811</v>
+      </c>
+      <c r="B802" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C802" t="b">
         <v>1</v>
       </c>
       <c r="E802" t="s">
-        <v>2776</v>
+        <v>2824</v>
       </c>
       <c r="F802" s="5" t="s">
-        <v>2777</v>
+        <v>2823</v>
       </c>
       <c r="G802" t="s">
-        <v>2787</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="803" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
-        <v>2785</v>
+        <v>2751</v>
       </c>
       <c r="B803" t="b">
         <v>0</v>
@@ -25822,18 +25891,18 @@
         <v>1</v>
       </c>
       <c r="E803" t="s">
-        <v>2785</v>
+        <v>2752</v>
       </c>
       <c r="F803" s="5" t="s">
-        <v>2786</v>
+        <v>2753</v>
       </c>
       <c r="G803" t="s">
-        <v>1425</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="804" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A804" s="3" t="s">
-        <v>2788</v>
+      <c r="A804" t="s">
+        <v>2816</v>
       </c>
       <c r="B804" s="3" t="b">
         <v>0</v>
@@ -25841,120 +25910,119 @@
       <c r="C804" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D804" s="3"/>
-      <c r="E804" s="3" t="s">
-        <v>2790</v>
+      <c r="E804" t="s">
+        <v>2755</v>
       </c>
       <c r="F804" s="5" t="s">
-        <v>2791</v>
-      </c>
-      <c r="G804" s="3" t="s">
-        <v>2789</v>
+        <v>2758</v>
+      </c>
+      <c r="G804" t="s">
+        <v>2767</v>
       </c>
     </row>
     <row r="805" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
-        <v>2827</v>
-      </c>
-      <c r="B805" t="b">
-        <v>0</v>
-      </c>
-      <c r="C805" t="b">
+        <v>2817</v>
+      </c>
+      <c r="B805" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C805" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E805" t="s">
-        <v>2827</v>
+        <v>2756</v>
       </c>
       <c r="F805" s="5" t="s">
-        <v>397</v>
+        <v>2760</v>
       </c>
       <c r="G805" t="s">
-        <v>2832</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="806" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
-        <v>2828</v>
-      </c>
-      <c r="B806" t="b">
-        <v>0</v>
-      </c>
-      <c r="C806" t="b">
+        <v>2818</v>
+      </c>
+      <c r="B806" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C806" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E806" t="s">
-        <v>2829</v>
+        <v>2757</v>
       </c>
       <c r="F806" s="5" t="s">
-        <v>2831</v>
+        <v>2759</v>
       </c>
       <c r="G806" t="s">
-        <v>2833</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="807" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
-        <v>2830</v>
-      </c>
-      <c r="B807" t="b">
-        <v>0</v>
-      </c>
-      <c r="C807" t="b">
+        <v>2819</v>
+      </c>
+      <c r="B807" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C807" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E807" t="s">
-        <v>2836</v>
+        <v>2820</v>
       </c>
       <c r="F807" s="5" t="s">
-        <v>2835</v>
+        <v>2761</v>
       </c>
       <c r="G807" t="s">
-        <v>2834</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="808" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
-        <v>2848</v>
-      </c>
-      <c r="B808" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C808" s="3" t="b">
+        <v>2775</v>
+      </c>
+      <c r="B808" t="b">
+        <v>0</v>
+      </c>
+      <c r="C808" t="b">
         <v>1</v>
       </c>
       <c r="E808" t="s">
-        <v>2849</v>
+        <v>2776</v>
       </c>
       <c r="F808" s="5" t="s">
-        <v>2850</v>
+        <v>2777</v>
       </c>
       <c r="G808" t="s">
-        <v>2853</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="809" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
-        <v>2859</v>
+        <v>2785</v>
       </c>
       <c r="B809" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C809" t="b">
         <v>1</v>
       </c>
       <c r="E809" t="s">
-        <v>2860</v>
+        <v>2785</v>
       </c>
       <c r="F809" s="5" t="s">
-        <v>2861</v>
+        <v>2786</v>
       </c>
       <c r="G809" t="s">
-        <v>2862</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="810" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A810" t="s">
-        <v>2863</v>
+      <c r="A810" s="3" t="s">
+        <v>2788</v>
       </c>
       <c r="B810" s="3" t="b">
         <v>0</v>
@@ -25962,241 +26030,242 @@
       <c r="C810" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E810" t="s">
-        <v>2863</v>
+      <c r="D810" s="3"/>
+      <c r="E810" s="3" t="s">
+        <v>2790</v>
       </c>
       <c r="F810" s="5" t="s">
-        <v>2870</v>
-      </c>
-      <c r="G810" t="s">
-        <v>2871</v>
+        <v>2791</v>
+      </c>
+      <c r="G810" s="3" t="s">
+        <v>2789</v>
       </c>
     </row>
     <row r="811" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
-        <v>2864</v>
-      </c>
-      <c r="B811" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C811" s="3" t="b">
+        <v>2827</v>
+      </c>
+      <c r="B811" t="b">
+        <v>0</v>
+      </c>
+      <c r="C811" t="b">
         <v>1</v>
       </c>
       <c r="E811" t="s">
-        <v>2866</v>
+        <v>2827</v>
       </c>
       <c r="F811" s="5" t="s">
-        <v>2869</v>
+        <v>397</v>
       </c>
       <c r="G811" t="s">
-        <v>2872</v>
+        <v>2832</v>
       </c>
     </row>
     <row r="812" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
-        <v>2865</v>
-      </c>
-      <c r="B812" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C812" s="3" t="b">
+        <v>2828</v>
+      </c>
+      <c r="B812" t="b">
+        <v>0</v>
+      </c>
+      <c r="C812" t="b">
         <v>1</v>
       </c>
       <c r="E812" t="s">
-        <v>2867</v>
+        <v>2829</v>
       </c>
       <c r="F812" s="5" t="s">
-        <v>2868</v>
+        <v>2831</v>
       </c>
       <c r="G812" t="s">
-        <v>2873</v>
+        <v>2833</v>
       </c>
     </row>
     <row r="813" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
+        <v>2830</v>
+      </c>
+      <c r="B813" t="b">
+        <v>0</v>
+      </c>
+      <c r="C813" t="b">
+        <v>1</v>
+      </c>
+      <c r="E813" t="s">
+        <v>2836</v>
+      </c>
+      <c r="F813" s="5" t="s">
+        <v>2835</v>
+      </c>
+      <c r="G813" t="s">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="814" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A814" t="s">
+        <v>2848</v>
+      </c>
+      <c r="B814" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C814" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E814" t="s">
+        <v>2849</v>
+      </c>
+      <c r="F814" s="5" t="s">
+        <v>2850</v>
+      </c>
+      <c r="G814" t="s">
+        <v>2853</v>
+      </c>
+    </row>
+    <row r="815" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A815" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B815" t="b">
+        <v>1</v>
+      </c>
+      <c r="C815" t="b">
+        <v>1</v>
+      </c>
+      <c r="E815" t="s">
+        <v>2860</v>
+      </c>
+      <c r="F815" s="5" t="s">
+        <v>2861</v>
+      </c>
+      <c r="G815" t="s">
+        <v>2862</v>
+      </c>
+    </row>
+    <row r="816" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A816" t="s">
+        <v>2863</v>
+      </c>
+      <c r="B816" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C816" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E816" t="s">
+        <v>2863</v>
+      </c>
+      <c r="F816" s="5" t="s">
+        <v>2870</v>
+      </c>
+      <c r="G816" t="s">
+        <v>2871</v>
+      </c>
+    </row>
+    <row r="817" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A817" t="s">
+        <v>2864</v>
+      </c>
+      <c r="B817" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C817" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E817" t="s">
+        <v>2866</v>
+      </c>
+      <c r="F817" s="5" t="s">
+        <v>2869</v>
+      </c>
+      <c r="G817" t="s">
+        <v>2872</v>
+      </c>
+    </row>
+    <row r="818" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>2865</v>
+      </c>
+      <c r="B818" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C818" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E818" t="s">
+        <v>2867</v>
+      </c>
+      <c r="F818" s="5" t="s">
+        <v>2868</v>
+      </c>
+      <c r="G818" t="s">
+        <v>2873</v>
+      </c>
+    </row>
+    <row r="819" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A819" t="s">
         <v>2874</v>
       </c>
-      <c r="B813" t="b">
-        <v>0</v>
-      </c>
-      <c r="C813" t="b">
-        <v>1</v>
-      </c>
-      <c r="E813" t="s">
+      <c r="B819" t="b">
+        <v>0</v>
+      </c>
+      <c r="C819" t="b">
+        <v>1</v>
+      </c>
+      <c r="E819" t="s">
         <v>2875</v>
       </c>
-      <c r="F813" s="5" t="s">
+      <c r="F819" s="5" t="s">
         <v>2876</v>
       </c>
-      <c r="G813" t="s">
+      <c r="G819" t="s">
         <v>2877</v>
       </c>
     </row>
-    <row r="814" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A814" s="3" t="s">
+    <row r="820" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A820" s="3" t="s">
         <v>2894</v>
       </c>
-      <c r="B814" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C814" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D814" s="3"/>
-      <c r="E814" s="3" t="s">
+      <c r="B820" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C820" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D820" s="3"/>
+      <c r="E820" s="3" t="s">
         <v>897</v>
       </c>
-      <c r="F814" s="5" t="s">
+      <c r="F820" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="G814" s="2" t="s">
+      <c r="G820" s="2" t="s">
         <v>1539</v>
       </c>
     </row>
-    <row r="815" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A815" s="3" t="s">
+    <row r="821" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A821" s="3" t="s">
         <v>2878</v>
       </c>
-      <c r="B815" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C815" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D815" s="3"/>
-      <c r="E815" s="3" t="s">
+      <c r="B821" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C821" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D821" s="3"/>
+      <c r="E821" s="3" t="s">
         <v>859</v>
       </c>
-      <c r="F815" s="5" t="s">
+      <c r="F821" s="5" t="s">
         <v>2930</v>
       </c>
-      <c r="G815" s="3" t="s">
+      <c r="G821" s="3" t="s">
         <v>1508</v>
-      </c>
-    </row>
-    <row r="816" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A816" s="3" t="s">
-        <v>2881</v>
-      </c>
-      <c r="B816" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C816" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E816" s="3" t="s">
-        <v>2880</v>
-      </c>
-      <c r="F816" s="5" t="s">
-        <v>2912</v>
-      </c>
-      <c r="G816" s="3" t="s">
-        <v>2919</v>
-      </c>
-    </row>
-    <row r="817" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A817" s="3" t="s">
-        <v>2882</v>
-      </c>
-      <c r="B817" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C817" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E817" s="3" t="s">
-        <v>2895</v>
-      </c>
-      <c r="F817" s="5" t="s">
-        <v>2911</v>
-      </c>
-      <c r="G817" s="3" t="s">
-        <v>2920</v>
-      </c>
-    </row>
-    <row r="818" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A818" s="3" t="s">
-        <v>2883</v>
-      </c>
-      <c r="B818" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C818" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E818" s="3" t="s">
-        <v>2897</v>
-      </c>
-      <c r="F818" s="5" t="s">
-        <v>2906</v>
-      </c>
-      <c r="G818" s="3" t="s">
-        <v>2921</v>
-      </c>
-    </row>
-    <row r="819" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A819" s="3" t="s">
-        <v>2884</v>
-      </c>
-      <c r="B819" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C819" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E819" s="3" t="s">
-        <v>2898</v>
-      </c>
-      <c r="F819" s="5" t="s">
-        <v>2907</v>
-      </c>
-      <c r="G819" s="3" t="s">
-        <v>2922</v>
-      </c>
-    </row>
-    <row r="820" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A820" s="3" t="s">
-        <v>2885</v>
-      </c>
-      <c r="B820" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C820" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E820" s="3" t="s">
-        <v>2899</v>
-      </c>
-      <c r="F820" s="5" t="s">
-        <v>2908</v>
-      </c>
-      <c r="G820" s="3" t="s">
-        <v>2923</v>
-      </c>
-    </row>
-    <row r="821" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A821" s="3" t="s">
-        <v>2886</v>
-      </c>
-      <c r="B821" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C821" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E821" s="3" t="s">
-        <v>2900</v>
-      </c>
-      <c r="F821" s="5" t="s">
-        <v>2909</v>
-      </c>
-      <c r="G821" s="3" t="s">
-        <v>2924</v>
       </c>
     </row>
     <row r="822" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A822" s="3" t="s">
-        <v>2887</v>
+        <v>2881</v>
       </c>
       <c r="B822" s="3" t="b">
         <v>1</v>
@@ -26205,18 +26274,18 @@
         <v>1</v>
       </c>
       <c r="E822" s="3" t="s">
-        <v>2896</v>
+        <v>2880</v>
       </c>
       <c r="F822" s="5" t="s">
-        <v>2910</v>
+        <v>2912</v>
       </c>
       <c r="G822" s="3" t="s">
-        <v>2925</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="823" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A823" s="3" t="s">
-        <v>2888</v>
+        <v>2882</v>
       </c>
       <c r="B823" s="3" t="b">
         <v>1</v>
@@ -26225,139 +26294,259 @@
         <v>1</v>
       </c>
       <c r="E823" s="3" t="s">
-        <v>2901</v>
+        <v>2895</v>
       </c>
       <c r="F823" s="5" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
       <c r="G823" s="3" t="s">
-        <v>2100</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="824" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A824" s="3" t="s">
+        <v>2883</v>
+      </c>
+      <c r="B824" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C824" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E824" s="3" t="s">
+        <v>2897</v>
+      </c>
+      <c r="F824" s="5" t="s">
+        <v>2906</v>
+      </c>
+      <c r="G824" s="3" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="825" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A825" s="3" t="s">
+        <v>2884</v>
+      </c>
+      <c r="B825" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C825" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E825" s="3" t="s">
+        <v>2898</v>
+      </c>
+      <c r="F825" s="5" t="s">
+        <v>2907</v>
+      </c>
+      <c r="G825" s="3" t="s">
+        <v>2922</v>
+      </c>
+    </row>
+    <row r="826" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A826" s="3" t="s">
+        <v>2885</v>
+      </c>
+      <c r="B826" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C826" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E826" s="3" t="s">
+        <v>2899</v>
+      </c>
+      <c r="F826" s="5" t="s">
+        <v>2908</v>
+      </c>
+      <c r="G826" s="3" t="s">
+        <v>2923</v>
+      </c>
+    </row>
+    <row r="827" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A827" s="3" t="s">
+        <v>2886</v>
+      </c>
+      <c r="B827" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C827" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E827" s="3" t="s">
+        <v>2900</v>
+      </c>
+      <c r="F827" s="5" t="s">
+        <v>2909</v>
+      </c>
+      <c r="G827" s="3" t="s">
+        <v>2924</v>
+      </c>
+    </row>
+    <row r="828" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A828" s="3" t="s">
+        <v>2887</v>
+      </c>
+      <c r="B828" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C828" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E828" s="3" t="s">
+        <v>2896</v>
+      </c>
+      <c r="F828" s="5" t="s">
+        <v>2910</v>
+      </c>
+      <c r="G828" s="3" t="s">
+        <v>2925</v>
+      </c>
+    </row>
+    <row r="829" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A829" s="3" t="s">
+        <v>2888</v>
+      </c>
+      <c r="B829" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C829" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E829" s="3" t="s">
+        <v>2901</v>
+      </c>
+      <c r="F829" s="5" t="s">
+        <v>2913</v>
+      </c>
+      <c r="G829" s="3" t="s">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="830" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A830" s="3" t="s">
         <v>2889</v>
       </c>
-      <c r="B824" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C824" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E824" s="3" t="s">
+      <c r="B830" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C830" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E830" s="3" t="s">
         <v>2902</v>
       </c>
-      <c r="F824" s="5" t="s">
+      <c r="F830" s="5" t="s">
         <v>2914</v>
       </c>
-      <c r="G824" s="3" t="s">
+      <c r="G830" s="3" t="s">
         <v>2926</v>
       </c>
     </row>
-    <row r="825" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A825" s="3" t="s">
+    <row r="831" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A831" s="3" t="s">
         <v>2879</v>
       </c>
-      <c r="B825" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C825" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D825" s="3"/>
-      <c r="E825" s="3" t="s">
+      <c r="B831" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C831" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D831" s="3"/>
+      <c r="E831" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="F825" s="5" t="s">
+      <c r="F831" s="5" t="s">
         <v>2915</v>
       </c>
-      <c r="G825" s="3" t="s">
+      <c r="G831" s="3" t="s">
         <v>1469</v>
       </c>
     </row>
-    <row r="826" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A826" t="s">
+    <row r="832" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A832" t="s">
         <v>2890</v>
       </c>
-      <c r="B826" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C826" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E826" t="s">
+      <c r="B832" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C832" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E832" t="s">
         <v>2903</v>
       </c>
-      <c r="F826" s="5" t="s">
+      <c r="F832" s="5" t="s">
         <v>2916</v>
       </c>
-      <c r="G826" t="s">
+      <c r="G832" t="s">
         <v>2927</v>
       </c>
     </row>
-    <row r="827" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A827" t="s">
+    <row r="833" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A833" t="s">
         <v>2891</v>
       </c>
-      <c r="B827" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C827" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E827" t="s">
+      <c r="B833" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C833" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E833" t="s">
         <v>2904</v>
       </c>
-      <c r="F827" s="5" t="s">
+      <c r="F833" s="5" t="s">
         <v>2917</v>
       </c>
-      <c r="G827" t="s">
+      <c r="G833" t="s">
         <v>2928</v>
       </c>
     </row>
-    <row r="828" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A828" t="s">
+    <row r="834" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A834" t="s">
         <v>2892</v>
       </c>
-      <c r="B828" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C828" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E828" t="s">
+      <c r="B834" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C834" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E834" t="s">
         <v>2905</v>
       </c>
-      <c r="F828" s="5" t="s">
+      <c r="F834" s="5" t="s">
         <v>2918</v>
       </c>
-      <c r="G828" t="s">
+      <c r="G834" t="s">
         <v>2929</v>
       </c>
     </row>
-    <row r="829" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A829" s="3" t="s">
+    <row r="835" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A835" s="3" t="s">
         <v>2893</v>
       </c>
-      <c r="B829" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C829" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D829" s="3"/>
-      <c r="E829" s="3" t="s">
+      <c r="B835" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C835" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D835" s="3"/>
+      <c r="E835" s="3" t="s">
         <v>945</v>
       </c>
-      <c r="F829" s="5" t="s">
+      <c r="F835" s="5" t="s">
         <v>1178</v>
       </c>
-      <c r="G829" s="3" t="s">
+      <c r="G835" s="3" t="s">
         <v>1587</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G756" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
+  <autoFilter ref="A1:G762" xr:uid="{166F55E6-F4CB-49C4-A0B4-8593C255C448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>